<commit_message>
range & mov effect x 10.
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -6006,102 +6006,6 @@
   <dxfs count="73">
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -6947,6 +6851,90 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7767,6 +7755,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8059,11 +8059,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-545541744"/>
-        <c:axId val="-545546096"/>
+        <c:axId val="-480399776"/>
+        <c:axId val="-480399232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-545541744"/>
+        <c:axId val="-480399776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8106,7 +8106,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-545546096"/>
+        <c:crossAx val="-480399232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8114,7 +8114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-545546096"/>
+        <c:axId val="-480399232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8165,7 +8165,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-545541744"/>
+        <c:crossAx val="-480399776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17858,93 +17858,93 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC311" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC311" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A3:AC311"/>
   <sortState ref="A4:AD311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="69"/>
-    <tableColumn id="2" name="Name" dataDxfId="68"/>
-    <tableColumn id="22" name="Ename" dataDxfId="67"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="66"/>
-    <tableColumn id="3" name="Star" dataDxfId="65"/>
-    <tableColumn id="4" name="Type" dataDxfId="64"/>
-    <tableColumn id="5" name="Attr" dataDxfId="63"/>
-    <tableColumn id="12" name="Cost" dataDxfId="62"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="61"/>
-    <tableColumn id="7" name="DefP" dataDxfId="60"/>
-    <tableColumn id="8" name="MagP" dataDxfId="59"/>
-    <tableColumn id="27" name="LukP" dataDxfId="58"/>
-    <tableColumn id="11" name="SpdP" dataDxfId="57"/>
-    <tableColumn id="24" name="VitP" dataDxfId="56"/>
-    <tableColumn id="26" name="Sum" dataDxfId="55">
+    <tableColumn id="1" name="Id" dataDxfId="68"/>
+    <tableColumn id="2" name="Name" dataDxfId="67"/>
+    <tableColumn id="22" name="Ename" dataDxfId="66"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="65"/>
+    <tableColumn id="3" name="Star" dataDxfId="64"/>
+    <tableColumn id="4" name="Type" dataDxfId="63"/>
+    <tableColumn id="5" name="Attr" dataDxfId="62"/>
+    <tableColumn id="12" name="Cost" dataDxfId="61"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="60"/>
+    <tableColumn id="7" name="DefP" dataDxfId="59"/>
+    <tableColumn id="8" name="MagP" dataDxfId="58"/>
+    <tableColumn id="27" name="LukP" dataDxfId="57"/>
+    <tableColumn id="11" name="SpdP" dataDxfId="56"/>
+    <tableColumn id="24" name="VitP" dataDxfId="55"/>
+    <tableColumn id="26" name="Sum" dataDxfId="54">
       <calculatedColumnFormula>SUM(I4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Modify" dataDxfId="54"/>
-    <tableColumn id="13" name="Range" dataDxfId="53"/>
-    <tableColumn id="14" name="Mov" dataDxfId="52"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="51"/>
-    <tableColumn id="17" name="Cover" dataDxfId="50"/>
-    <tableColumn id="18" name="Skills" dataDxfId="49"/>
-    <tableColumn id="30" name="AttrAtk" dataDxfId="48"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="47"/>
-    <tableColumn id="20" name="Res" dataDxfId="46"/>
-    <tableColumn id="21" name="Icon" dataDxfId="45"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="44"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="43"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="42"/>
-    <tableColumn id="29" name="Remark" dataDxfId="41"/>
+    <tableColumn id="25" name="Modify" dataDxfId="53"/>
+    <tableColumn id="13" name="Range" dataDxfId="52"/>
+    <tableColumn id="14" name="Mov" dataDxfId="51"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="50"/>
+    <tableColumn id="17" name="Cover" dataDxfId="49"/>
+    <tableColumn id="18" name="Skills" dataDxfId="48"/>
+    <tableColumn id="30" name="AttrAtk" dataDxfId="47"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="46"/>
+    <tableColumn id="20" name="Res" dataDxfId="45"/>
+    <tableColumn id="21" name="Icon" dataDxfId="44"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="43"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="42"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="41"/>
+    <tableColumn id="29" name="Remark" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A3:AC9"/>
   <sortState ref="A4:AC9">
     <sortCondition ref="A3:A9"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="37"/>
-    <tableColumn id="2" name="Name" dataDxfId="36"/>
-    <tableColumn id="22" name="Ename" dataDxfId="35"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="34"/>
-    <tableColumn id="3" name="Star" dataDxfId="33"/>
-    <tableColumn id="4" name="Type" dataDxfId="32"/>
-    <tableColumn id="5" name="Attr" dataDxfId="31"/>
-    <tableColumn id="12" name="Cost" dataDxfId="30"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="29"/>
-    <tableColumn id="7" name="DefP" dataDxfId="28"/>
-    <tableColumn id="8" name="MagP" dataDxfId="27"/>
-    <tableColumn id="27" name="LukP" dataDxfId="26"/>
-    <tableColumn id="11" name="SpdP" dataDxfId="25"/>
-    <tableColumn id="24" name="VitP" dataDxfId="24"/>
-    <tableColumn id="26" name="Sum" dataDxfId="23">
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Name" dataDxfId="28"/>
+    <tableColumn id="22" name="Ename" dataDxfId="27"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="26"/>
+    <tableColumn id="3" name="Star" dataDxfId="25"/>
+    <tableColumn id="4" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" name="Attr" dataDxfId="23"/>
+    <tableColumn id="12" name="Cost" dataDxfId="22"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="21"/>
+    <tableColumn id="7" name="DefP" dataDxfId="20"/>
+    <tableColumn id="8" name="MagP" dataDxfId="19"/>
+    <tableColumn id="27" name="LukP" dataDxfId="18"/>
+    <tableColumn id="11" name="SpdP" dataDxfId="17"/>
+    <tableColumn id="24" name="VitP" dataDxfId="16"/>
+    <tableColumn id="26" name="Sum" dataDxfId="15">
       <calculatedColumnFormula>SUM(I4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Modify" dataDxfId="22"/>
-    <tableColumn id="13" name="Range" dataDxfId="21"/>
-    <tableColumn id="14" name="Mov" dataDxfId="20"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="19"/>
-    <tableColumn id="17" name="Cover" dataDxfId="18"/>
-    <tableColumn id="18" name="Skills" dataDxfId="17"/>
-    <tableColumn id="30" name="AttrAtk" dataDxfId="16"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="15"/>
-    <tableColumn id="20" name="Res" dataDxfId="14"/>
-    <tableColumn id="21" name="Icon" dataDxfId="13"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="12"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="11"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="10"/>
-    <tableColumn id="29" name="Remark" dataDxfId="9"/>
+    <tableColumn id="25" name="Modify" dataDxfId="14"/>
+    <tableColumn id="13" name="Range" dataDxfId="13"/>
+    <tableColumn id="14" name="Mov" dataDxfId="12"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="11"/>
+    <tableColumn id="17" name="Cover" dataDxfId="10"/>
+    <tableColumn id="18" name="Skills" dataDxfId="9"/>
+    <tableColumn id="30" name="AttrAtk" dataDxfId="8"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="7"/>
+    <tableColumn id="20" name="Res" dataDxfId="6"/>
+    <tableColumn id="21" name="Icon" dataDxfId="5"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
+    <tableColumn id="29" name="Remark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -18254,7 +18254,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:R3"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18593,10 +18593,10 @@
         <v>-5</v>
       </c>
       <c r="Q4" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R4" s="4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>2</v>
@@ -18681,10 +18681,10 @@
         <v>-5</v>
       </c>
       <c r="Q5" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R5" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>4</v>
@@ -18767,10 +18767,10 @@
         <v>-3</v>
       </c>
       <c r="Q6" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R6" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>6</v>
@@ -18853,10 +18853,10 @@
         <v>-2</v>
       </c>
       <c r="Q7" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R7" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>0</v>
@@ -18939,10 +18939,10 @@
         <v>-1</v>
       </c>
       <c r="Q8" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R8" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>9</v>
@@ -19027,10 +19027,10 @@
         <v>-1</v>
       </c>
       <c r="Q9" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R9" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>11</v>
@@ -19113,10 +19113,10 @@
         <v>-3</v>
       </c>
       <c r="Q10" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R10" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>12</v>
@@ -19199,10 +19199,10 @@
         <v>-3</v>
       </c>
       <c r="Q11" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R11" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>14</v>
@@ -19285,10 +19285,10 @@
         <v>-3</v>
       </c>
       <c r="Q12" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R12" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>16</v>
@@ -19371,10 +19371,10 @@
         <v>-3</v>
       </c>
       <c r="Q13" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R13" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>16</v>
@@ -19457,10 +19457,10 @@
         <v>-5</v>
       </c>
       <c r="Q14" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R14" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>6</v>
@@ -19543,10 +19543,10 @@
         <v>-3</v>
       </c>
       <c r="Q15" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R15" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>19</v>
@@ -19631,10 +19631,10 @@
         <v>-4</v>
       </c>
       <c r="Q16" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R16" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>16</v>
@@ -19719,10 +19719,10 @@
         <v>-3</v>
       </c>
       <c r="Q17" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R17" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S17" s="4" t="s">
         <v>22</v>
@@ -19807,10 +19807,10 @@
         <v>-3</v>
       </c>
       <c r="Q18" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R18" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>16</v>
@@ -19893,10 +19893,10 @@
         <v>-3</v>
       </c>
       <c r="Q19" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R19" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>24</v>
@@ -19979,10 +19979,10 @@
         <v>-3</v>
       </c>
       <c r="Q20" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R20" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S20" s="4" t="s">
         <v>22</v>
@@ -20065,10 +20065,10 @@
         <v>-3</v>
       </c>
       <c r="Q21" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R21" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>12</v>
@@ -20153,10 +20153,10 @@
         <v>-3</v>
       </c>
       <c r="Q22" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R22" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S22" s="4" t="s">
         <v>19</v>
@@ -20239,10 +20239,10 @@
         <v>-5</v>
       </c>
       <c r="Q23" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R23" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S23" s="4" t="s">
         <v>2</v>
@@ -20327,10 +20327,10 @@
         <v>-2</v>
       </c>
       <c r="Q24" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R24" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>0</v>
@@ -20413,10 +20413,10 @@
         <v>-3</v>
       </c>
       <c r="Q25" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R25" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S25" s="4" t="s">
         <v>31</v>
@@ -20499,10 +20499,10 @@
         <v>-3</v>
       </c>
       <c r="Q26" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R26" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>2</v>
@@ -20587,10 +20587,10 @@
         <v>-5</v>
       </c>
       <c r="Q27" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R27" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S27" s="4" t="s">
         <v>16</v>
@@ -20673,10 +20673,10 @@
         <v>-3</v>
       </c>
       <c r="Q28" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R28" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S28" s="4" t="s">
         <v>6</v>
@@ -20759,10 +20759,10 @@
         <v>-3</v>
       </c>
       <c r="Q29" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R29" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S29" s="4" t="s">
         <v>9</v>
@@ -20845,10 +20845,10 @@
         <v>-2</v>
       </c>
       <c r="Q30" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R30" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>12</v>
@@ -20931,10 +20931,10 @@
         <v>-2</v>
       </c>
       <c r="Q31" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R31" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>38</v>
@@ -21017,10 +21017,10 @@
         <v>-3</v>
       </c>
       <c r="Q32" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R32" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>40</v>
@@ -21103,10 +21103,10 @@
         <v>5</v>
       </c>
       <c r="Q33" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R33" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>9</v>
@@ -21189,10 +21189,10 @@
         <v>-9</v>
       </c>
       <c r="Q34" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R34" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>16</v>
@@ -21275,10 +21275,10 @@
         <v>0</v>
       </c>
       <c r="Q35" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R35" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>9</v>
@@ -21361,10 +21361,10 @@
         <v>-2</v>
       </c>
       <c r="Q36" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R36" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>45</v>
@@ -21447,10 +21447,10 @@
         <v>-2</v>
       </c>
       <c r="Q37" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R37" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>38</v>
@@ -21533,10 +21533,10 @@
         <v>-2</v>
       </c>
       <c r="Q38" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R38" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S38" s="4" t="s">
         <v>12</v>
@@ -21621,10 +21621,10 @@
         <v>1</v>
       </c>
       <c r="Q39" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R39" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>12</v>
@@ -21705,10 +21705,10 @@
         <v>0</v>
       </c>
       <c r="Q40" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R40" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>6</v>
@@ -21791,10 +21791,10 @@
         <v>-2</v>
       </c>
       <c r="Q41" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R41" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>51</v>
@@ -21877,10 +21877,10 @@
         <v>1</v>
       </c>
       <c r="Q42" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R42" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>53</v>
@@ -21963,10 +21963,10 @@
         <v>-3</v>
       </c>
       <c r="Q43" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R43" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>4</v>
@@ -22049,10 +22049,10 @@
         <v>-1</v>
       </c>
       <c r="Q44" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R44" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>16</v>
@@ -22135,10 +22135,10 @@
         <v>-3</v>
       </c>
       <c r="Q45" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R45" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S45" s="4" t="s">
         <v>4</v>
@@ -22221,10 +22221,10 @@
         <v>-2</v>
       </c>
       <c r="Q46" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R46" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S46" s="4" t="s">
         <v>2</v>
@@ -22307,10 +22307,10 @@
         <v>-5</v>
       </c>
       <c r="Q47" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R47" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S47" s="4" t="s">
         <v>16</v>
@@ -22393,10 +22393,10 @@
         <v>-3</v>
       </c>
       <c r="Q48" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R48" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S48" s="4" t="s">
         <v>16</v>
@@ -22479,10 +22479,10 @@
         <v>-3</v>
       </c>
       <c r="Q49" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R49" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S49" s="4" t="s">
         <v>19</v>
@@ -22565,10 +22565,10 @@
         <v>-3</v>
       </c>
       <c r="Q50" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R50" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S50" s="4" t="s">
         <v>2</v>
@@ -22651,10 +22651,10 @@
         <v>-3</v>
       </c>
       <c r="Q51" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R51" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S51" s="4" t="s">
         <v>9</v>
@@ -22737,10 +22737,10 @@
         <v>-2</v>
       </c>
       <c r="Q52" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R52" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S52" s="4" t="s">
         <v>9</v>
@@ -22823,10 +22823,10 @@
         <v>-5</v>
       </c>
       <c r="Q53" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R53" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S53" s="4" t="s">
         <v>16</v>
@@ -22909,10 +22909,10 @@
         <v>-2</v>
       </c>
       <c r="Q54" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R54" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S54" s="4" t="s">
         <v>64</v>
@@ -22995,10 +22995,10 @@
         <v>-3</v>
       </c>
       <c r="Q55" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R55" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S55" s="4" t="s">
         <v>65</v>
@@ -23081,10 +23081,10 @@
         <v>-3</v>
       </c>
       <c r="Q56" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R56" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S56" s="4" t="s">
         <v>4</v>
@@ -23167,10 +23167,10 @@
         <v>-3</v>
       </c>
       <c r="Q57" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R57" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S57" s="4" t="s">
         <v>4</v>
@@ -23253,10 +23253,10 @@
         <v>-3</v>
       </c>
       <c r="Q58" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R58" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S58" s="4" t="s">
         <v>4</v>
@@ -23339,10 +23339,10 @@
         <v>3</v>
       </c>
       <c r="Q59" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R59" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S59" s="4" t="s">
         <v>69</v>
@@ -23425,10 +23425,10 @@
         <v>-2</v>
       </c>
       <c r="Q60" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R60" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S60" s="4" t="s">
         <v>9</v>
@@ -23511,10 +23511,10 @@
         <v>-3</v>
       </c>
       <c r="Q61" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R61" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S61" s="4" t="s">
         <v>24</v>
@@ -23597,10 +23597,10 @@
         <v>-4</v>
       </c>
       <c r="Q62" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R62" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S62" s="4" t="s">
         <v>65</v>
@@ -23683,10 +23683,10 @@
         <v>-1</v>
       </c>
       <c r="Q63" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R63" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S63" s="4" t="s">
         <v>38</v>
@@ -23769,10 +23769,10 @@
         <v>-3</v>
       </c>
       <c r="Q64" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R64" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S64" s="4" t="s">
         <v>24</v>
@@ -23853,10 +23853,10 @@
         <v>-2</v>
       </c>
       <c r="Q65" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R65" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S65" s="4" t="s">
         <v>6</v>
@@ -23941,10 +23941,10 @@
         <v>-3</v>
       </c>
       <c r="Q66" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R66" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S66" s="4" t="s">
         <v>2</v>
@@ -24029,10 +24029,10 @@
         <v>0</v>
       </c>
       <c r="Q67" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R67" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S67" s="4" t="s">
         <v>78</v>
@@ -24115,10 +24115,10 @@
         <v>1</v>
       </c>
       <c r="Q68" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R68" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S68" s="4" t="s">
         <v>78</v>
@@ -24203,10 +24203,10 @@
         <v>-2</v>
       </c>
       <c r="Q69" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R69" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S69" s="4" t="s">
         <v>40</v>
@@ -24289,10 +24289,10 @@
         <v>2</v>
       </c>
       <c r="Q70" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R70" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S70" s="4" t="s">
         <v>16</v>
@@ -24375,10 +24375,10 @@
         <v>2</v>
       </c>
       <c r="Q71" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R71" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>2</v>
@@ -24461,10 +24461,10 @@
         <v>3</v>
       </c>
       <c r="Q72" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R72" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S72" s="4" t="s">
         <v>2</v>
@@ -24547,10 +24547,10 @@
         <v>0</v>
       </c>
       <c r="Q73" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R73" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S73" s="4" t="s">
         <v>86</v>
@@ -24633,10 +24633,10 @@
         <v>-7</v>
       </c>
       <c r="Q74" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R74" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S74" s="4" t="s">
         <v>6</v>
@@ -24719,10 +24719,10 @@
         <v>-3</v>
       </c>
       <c r="Q75" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R75" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S75" s="4" t="s">
         <v>89</v>
@@ -24805,10 +24805,10 @@
         <v>2</v>
       </c>
       <c r="Q76" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R76" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>12</v>
@@ -24891,10 +24891,10 @@
         <v>-3</v>
       </c>
       <c r="Q77" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R77" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S77" s="4" t="s">
         <v>92</v>
@@ -24977,10 +24977,10 @@
         <v>0</v>
       </c>
       <c r="Q78" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R78" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S78" s="4" t="s">
         <v>94</v>
@@ -25063,10 +25063,10 @@
         <v>-3</v>
       </c>
       <c r="Q79" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R79" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S79" s="4" t="s">
         <v>4</v>
@@ -25151,10 +25151,10 @@
         <v>-3</v>
       </c>
       <c r="Q80" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R80" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S80" s="4" t="s">
         <v>4</v>
@@ -25239,10 +25239,10 @@
         <v>-3</v>
       </c>
       <c r="Q81" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R81" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S81" s="4" t="s">
         <v>2</v>
@@ -25325,10 +25325,10 @@
         <v>-5</v>
       </c>
       <c r="Q82" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R82" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S82" s="4" t="s">
         <v>2</v>
@@ -25411,10 +25411,10 @@
         <v>-3</v>
       </c>
       <c r="Q83" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R83" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S83" s="4" t="s">
         <v>38</v>
@@ -25497,10 +25497,10 @@
         <v>0</v>
       </c>
       <c r="Q84" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R84" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S84" s="4" t="s">
         <v>100</v>
@@ -25583,10 +25583,10 @@
         <v>-5</v>
       </c>
       <c r="Q85" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R85" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S85" s="4" t="s">
         <v>2</v>
@@ -25669,10 +25669,10 @@
         <v>-2</v>
       </c>
       <c r="Q86" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R86" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S86" s="4" t="s">
         <v>6</v>
@@ -25755,10 +25755,10 @@
         <v>0</v>
       </c>
       <c r="Q87" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R87" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S87" s="4" t="s">
         <v>86</v>
@@ -25841,10 +25841,10 @@
         <v>-3</v>
       </c>
       <c r="Q88" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R88" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S88" s="4" t="s">
         <v>0</v>
@@ -25927,10 +25927,10 @@
         <v>-2</v>
       </c>
       <c r="Q89" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R89" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S89" s="4" t="s">
         <v>105</v>
@@ -26013,10 +26013,10 @@
         <v>-2</v>
       </c>
       <c r="Q90" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R90" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S90" s="4" t="s">
         <v>107</v>
@@ -26099,10 +26099,10 @@
         <v>-2</v>
       </c>
       <c r="Q91" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R91" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S91" s="4" t="s">
         <v>105</v>
@@ -26185,10 +26185,10 @@
         <v>-6</v>
       </c>
       <c r="Q92" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R92" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S92" s="4" t="s">
         <v>16</v>
@@ -26271,10 +26271,10 @@
         <v>-1</v>
       </c>
       <c r="Q93" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R93" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S93" s="4" t="s">
         <v>111</v>
@@ -26357,10 +26357,10 @@
         <v>-3</v>
       </c>
       <c r="Q94" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R94" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S94" s="4" t="s">
         <v>78</v>
@@ -26443,10 +26443,10 @@
         <v>-3</v>
       </c>
       <c r="Q95" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R95" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S95" s="4" t="s">
         <v>107</v>
@@ -26529,10 +26529,10 @@
         <v>-7</v>
       </c>
       <c r="Q96" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R96" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S96" s="4" t="s">
         <v>2</v>
@@ -26615,10 +26615,10 @@
         <v>3</v>
       </c>
       <c r="Q97" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R97" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S97" s="4" t="s">
         <v>22</v>
@@ -26701,10 +26701,10 @@
         <v>-1</v>
       </c>
       <c r="Q98" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R98" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S98" s="4" t="s">
         <v>94</v>
@@ -26787,10 +26787,10 @@
         <v>-3</v>
       </c>
       <c r="Q99" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R99" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S99" s="4" t="s">
         <v>118</v>
@@ -26873,10 +26873,10 @@
         <v>1</v>
       </c>
       <c r="Q100" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R100" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S100" s="4" t="s">
         <v>78</v>
@@ -26961,10 +26961,10 @@
         <v>-3</v>
       </c>
       <c r="Q101" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R101" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S101" s="4" t="s">
         <v>4</v>
@@ -27047,10 +27047,10 @@
         <v>0</v>
       </c>
       <c r="Q102" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R102" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S102" s="4" t="s">
         <v>16</v>
@@ -27133,10 +27133,10 @@
         <v>-3</v>
       </c>
       <c r="Q103" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R103" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S103" s="4" t="s">
         <v>9</v>
@@ -27219,10 +27219,10 @@
         <v>-5</v>
       </c>
       <c r="Q104" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R104" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S104" s="4" t="s">
         <v>4</v>
@@ -27305,10 +27305,10 @@
         <v>-2</v>
       </c>
       <c r="Q105" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R105" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S105" s="4" t="s">
         <v>107</v>
@@ -27391,10 +27391,10 @@
         <v>0</v>
       </c>
       <c r="Q106" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R106" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S106" s="4" t="s">
         <v>9</v>
@@ -27477,10 +27477,10 @@
         <v>-2</v>
       </c>
       <c r="Q107" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R107" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S107" s="4" t="s">
         <v>9</v>
@@ -27563,10 +27563,10 @@
         <v>-3</v>
       </c>
       <c r="Q108" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R108" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S108" s="4" t="s">
         <v>2</v>
@@ -27649,10 +27649,10 @@
         <v>-1</v>
       </c>
       <c r="Q109" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R109" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S109" s="4" t="s">
         <v>128</v>
@@ -27735,10 +27735,10 @@
         <v>-1</v>
       </c>
       <c r="Q110" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R110" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S110" s="4" t="s">
         <v>130</v>
@@ -27821,10 +27821,10 @@
         <v>-3</v>
       </c>
       <c r="Q111" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R111" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S111" s="4" t="s">
         <v>132</v>
@@ -27907,10 +27907,10 @@
         <v>-1</v>
       </c>
       <c r="Q112" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R112" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S112" s="4" t="s">
         <v>118</v>
@@ -27993,10 +27993,10 @@
         <v>-1</v>
       </c>
       <c r="Q113" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R113" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S113" s="4" t="s">
         <v>135</v>
@@ -28079,10 +28079,10 @@
         <v>1</v>
       </c>
       <c r="Q114" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R114" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S114" s="4" t="s">
         <v>89</v>
@@ -28167,10 +28167,10 @@
         <v>1</v>
       </c>
       <c r="Q115" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R115" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S115" s="4" t="s">
         <v>94</v>
@@ -28255,10 +28255,10 @@
         <v>1</v>
       </c>
       <c r="Q116" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R116" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S116" s="4" t="s">
         <v>31</v>
@@ -28343,10 +28343,10 @@
         <v>-2</v>
       </c>
       <c r="Q117" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R117" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S117" s="4" t="s">
         <v>4</v>
@@ -28429,10 +28429,10 @@
         <v>1</v>
       </c>
       <c r="Q118" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R118" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S118" s="4" t="s">
         <v>40</v>
@@ -28517,10 +28517,10 @@
         <v>1</v>
       </c>
       <c r="Q119" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R119" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S119" s="4" t="s">
         <v>100</v>
@@ -28605,10 +28605,10 @@
         <v>1</v>
       </c>
       <c r="Q120" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R120" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S120" s="4" t="s">
         <v>51</v>
@@ -28693,10 +28693,10 @@
         <v>1</v>
       </c>
       <c r="Q121" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R121" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S121" s="4" t="s">
         <v>22</v>
@@ -28781,10 +28781,10 @@
         <v>-3</v>
       </c>
       <c r="Q122" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R122" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S122" s="4" t="s">
         <v>4</v>
@@ -28867,10 +28867,10 @@
         <v>-1</v>
       </c>
       <c r="Q123" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R123" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S123" s="4" t="s">
         <v>4</v>
@@ -28953,10 +28953,10 @@
         <v>-3</v>
       </c>
       <c r="Q124" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R124" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S124" s="4" t="s">
         <v>2</v>
@@ -29039,10 +29039,10 @@
         <v>0</v>
       </c>
       <c r="Q125" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R125" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S125" s="4" t="s">
         <v>2</v>
@@ -29125,10 +29125,10 @@
         <v>-3</v>
       </c>
       <c r="Q126" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R126" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S126" s="4" t="s">
         <v>24</v>
@@ -29211,10 +29211,10 @@
         <v>-1</v>
       </c>
       <c r="Q127" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R127" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S127" s="4" t="s">
         <v>4</v>
@@ -29297,10 +29297,10 @@
         <v>-3</v>
       </c>
       <c r="Q128" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R128" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S128" s="4" t="s">
         <v>4</v>
@@ -29383,10 +29383,10 @@
         <v>-7</v>
       </c>
       <c r="Q129" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R129" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S129" s="4" t="s">
         <v>2</v>
@@ -29469,10 +29469,10 @@
         <v>-2</v>
       </c>
       <c r="Q130" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R130" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S130" s="4" t="s">
         <v>107</v>
@@ -29555,10 +29555,10 @@
         <v>-4</v>
       </c>
       <c r="Q131" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R131" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S131" s="4" t="s">
         <v>6</v>
@@ -29641,10 +29641,10 @@
         <v>-2</v>
       </c>
       <c r="Q132" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R132" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S132" s="4" t="s">
         <v>4</v>
@@ -29727,10 +29727,10 @@
         <v>0</v>
       </c>
       <c r="Q133" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R133" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S133" s="4" t="s">
         <v>107</v>
@@ -29813,10 +29813,10 @@
         <v>-2</v>
       </c>
       <c r="Q134" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R134" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S134" s="4" t="s">
         <v>2</v>
@@ -29899,10 +29899,10 @@
         <v>-3</v>
       </c>
       <c r="Q135" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R135" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S135" s="4" t="s">
         <v>78</v>
@@ -29985,10 +29985,10 @@
         <v>-3</v>
       </c>
       <c r="Q136" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R136" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S136" s="4" t="s">
         <v>107</v>
@@ -30071,10 +30071,10 @@
         <v>-1</v>
       </c>
       <c r="Q137" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R137" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S137" s="4" t="s">
         <v>2</v>
@@ -30157,10 +30157,10 @@
         <v>-1</v>
       </c>
       <c r="Q138" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R138" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S138" s="4" t="s">
         <v>6</v>
@@ -30243,10 +30243,10 @@
         <v>-2</v>
       </c>
       <c r="Q139" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R139" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S139" s="4" t="s">
         <v>107</v>
@@ -30329,10 +30329,10 @@
         <v>-3</v>
       </c>
       <c r="Q140" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R140" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S140" s="4" t="s">
         <v>38</v>
@@ -30415,10 +30415,10 @@
         <v>-2</v>
       </c>
       <c r="Q141" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R141" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S141" s="4" t="s">
         <v>12</v>
@@ -30501,10 +30501,10 @@
         <v>-5</v>
       </c>
       <c r="Q142" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R142" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S142" s="4" t="s">
         <v>40</v>
@@ -30587,10 +30587,10 @@
         <v>-1</v>
       </c>
       <c r="Q143" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R143" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S143" s="4" t="s">
         <v>4</v>
@@ -30673,10 +30673,10 @@
         <v>-3</v>
       </c>
       <c r="Q144" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R144" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S144" s="4" t="s">
         <v>16</v>
@@ -30761,10 +30761,10 @@
         <v>-5</v>
       </c>
       <c r="Q145" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R145" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S145" s="4" t="s">
         <v>0</v>
@@ -30849,10 +30849,10 @@
         <v>-6</v>
       </c>
       <c r="Q146" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R146" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S146" s="4" t="s">
         <v>107</v>
@@ -30935,10 +30935,10 @@
         <v>-3</v>
       </c>
       <c r="Q147" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R147" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S147" s="4" t="s">
         <v>19</v>
@@ -31021,10 +31021,10 @@
         <v>-3</v>
       </c>
       <c r="Q148" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R148" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S148" s="4" t="s">
         <v>166</v>
@@ -31107,10 +31107,10 @@
         <v>-2</v>
       </c>
       <c r="Q149" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R149" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S149" s="4" t="s">
         <v>166</v>
@@ -31193,10 +31193,10 @@
         <v>1</v>
       </c>
       <c r="Q150" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R150" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S150" s="4" t="s">
         <v>4</v>
@@ -31279,10 +31279,10 @@
         <v>-2</v>
       </c>
       <c r="Q151" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R151" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S151" s="4" t="s">
         <v>16</v>
@@ -31365,10 +31365,10 @@
         <v>-4</v>
       </c>
       <c r="Q152" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R152" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S152" s="4" t="s">
         <v>6</v>
@@ -31453,10 +31453,10 @@
         <v>-3</v>
       </c>
       <c r="Q153" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R153" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S153" s="4" t="s">
         <v>2</v>
@@ -31539,10 +31539,10 @@
         <v>-2</v>
       </c>
       <c r="Q154" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R154" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S154" s="4" t="s">
         <v>172</v>
@@ -31625,10 +31625,10 @@
         <v>-2</v>
       </c>
       <c r="Q155" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R155" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S155" s="4" t="s">
         <v>174</v>
@@ -31711,10 +31711,10 @@
         <v>-2</v>
       </c>
       <c r="Q156" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R156" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S156" s="4" t="s">
         <v>4</v>
@@ -31797,10 +31797,10 @@
         <v>-3</v>
       </c>
       <c r="Q157" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R157" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S157" s="4" t="s">
         <v>4</v>
@@ -31885,10 +31885,10 @@
         <v>-5</v>
       </c>
       <c r="Q158" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R158" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S158" s="4" t="s">
         <v>2</v>
@@ -31971,10 +31971,10 @@
         <v>-1</v>
       </c>
       <c r="Q159" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R159" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S159" s="4" t="s">
         <v>2</v>
@@ -32057,10 +32057,10 @@
         <v>-1</v>
       </c>
       <c r="Q160" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R160" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S160" s="4" t="s">
         <v>180</v>
@@ -32143,10 +32143,10 @@
         <v>-4</v>
       </c>
       <c r="Q161" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R161" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S161" s="4" t="s">
         <v>24</v>
@@ -32231,10 +32231,10 @@
         <v>-2</v>
       </c>
       <c r="Q162" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R162" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S162" s="4" t="s">
         <v>107</v>
@@ -32317,10 +32317,10 @@
         <v>-3</v>
       </c>
       <c r="Q163" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R163" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S163" s="4" t="s">
         <v>107</v>
@@ -32403,10 +32403,10 @@
         <v>-3</v>
       </c>
       <c r="Q164" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R164" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S164" s="4" t="s">
         <v>16</v>
@@ -32489,10 +32489,10 @@
         <v>-1</v>
       </c>
       <c r="Q165" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R165" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S165" s="4" t="s">
         <v>38</v>
@@ -32575,10 +32575,10 @@
         <v>-3</v>
       </c>
       <c r="Q166" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R166" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S166" s="4" t="s">
         <v>100</v>
@@ -32661,10 +32661,10 @@
         <v>-2</v>
       </c>
       <c r="Q167" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R167" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S167" s="4" t="s">
         <v>24</v>
@@ -32747,10 +32747,10 @@
         <v>-2</v>
       </c>
       <c r="Q168" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R168" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S168" s="4" t="s">
         <v>16</v>
@@ -32833,10 +32833,10 @@
         <v>0</v>
       </c>
       <c r="Q169" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R169" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S169" s="4" t="s">
         <v>9</v>
@@ -32919,10 +32919,10 @@
         <v>0</v>
       </c>
       <c r="Q170" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R170" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S170" s="4" t="s">
         <v>9</v>
@@ -33005,10 +33005,10 @@
         <v>-2</v>
       </c>
       <c r="Q171" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R171" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S171" s="4" t="s">
         <v>4</v>
@@ -33091,10 +33091,10 @@
         <v>-1</v>
       </c>
       <c r="Q172" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R172" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S172" s="4" t="s">
         <v>4</v>
@@ -33179,10 +33179,10 @@
         <v>-3</v>
       </c>
       <c r="Q173" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R173" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S173" s="4" t="s">
         <v>191</v>
@@ -33265,10 +33265,10 @@
         <v>-2</v>
       </c>
       <c r="Q174" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R174" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S174" s="4" t="s">
         <v>69</v>
@@ -33351,10 +33351,10 @@
         <v>-3</v>
       </c>
       <c r="Q175" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R175" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S175" s="4" t="s">
         <v>2</v>
@@ -33437,10 +33437,10 @@
         <v>-1</v>
       </c>
       <c r="Q176" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R176" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S176" s="4" t="s">
         <v>12</v>
@@ -33523,10 +33523,10 @@
         <v>-3</v>
       </c>
       <c r="Q177" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R177" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S177" s="4" t="s">
         <v>4</v>
@@ -33609,10 +33609,10 @@
         <v>-3</v>
       </c>
       <c r="Q178" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R178" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S178" s="4" t="s">
         <v>4</v>
@@ -33695,10 +33695,10 @@
         <v>-15</v>
       </c>
       <c r="Q179" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R179" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S179" s="4" t="s">
         <v>2</v>
@@ -33781,10 +33781,10 @@
         <v>0</v>
       </c>
       <c r="Q180" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R180" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S180" s="4" t="s">
         <v>65</v>
@@ -33867,10 +33867,10 @@
         <v>-8</v>
       </c>
       <c r="Q181" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R181" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S181" s="7" t="s">
         <v>984</v>
@@ -33955,10 +33955,10 @@
         <v>-3</v>
       </c>
       <c r="Q182" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R182" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S182" s="4" t="s">
         <v>4</v>
@@ -34041,10 +34041,10 @@
         <v>-2</v>
       </c>
       <c r="Q183" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R183" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S183" s="4" t="s">
         <v>16</v>
@@ -34127,10 +34127,10 @@
         <v>-2</v>
       </c>
       <c r="Q184" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R184" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S184" s="4" t="s">
         <v>78</v>
@@ -34213,10 +34213,10 @@
         <v>2</v>
       </c>
       <c r="Q185" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R185" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S185" s="4" t="s">
         <v>12</v>
@@ -34299,10 +34299,10 @@
         <v>0</v>
       </c>
       <c r="Q186" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R186" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S186" s="4" t="s">
         <v>78</v>
@@ -34385,10 +34385,10 @@
         <v>-3</v>
       </c>
       <c r="Q187" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R187" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S187" s="4" t="s">
         <v>6</v>
@@ -34471,10 +34471,10 @@
         <v>-3</v>
       </c>
       <c r="Q188" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R188" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S188" s="4" t="s">
         <v>2</v>
@@ -34557,10 +34557,10 @@
         <v>-2</v>
       </c>
       <c r="Q189" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R189" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S189" s="4" t="s">
         <v>4</v>
@@ -34645,10 +34645,10 @@
         <v>-3</v>
       </c>
       <c r="Q190" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R190" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S190" s="4" t="s">
         <v>2</v>
@@ -34733,10 +34733,10 @@
         <v>-2</v>
       </c>
       <c r="Q191" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R191" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S191" s="4" t="s">
         <v>24</v>
@@ -34819,10 +34819,10 @@
         <v>-1</v>
       </c>
       <c r="Q192" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R192" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S192" s="4" t="s">
         <v>208</v>
@@ -34907,10 +34907,10 @@
         <v>-1</v>
       </c>
       <c r="Q193" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R193" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S193" s="4" t="s">
         <v>2</v>
@@ -34993,10 +34993,10 @@
         <v>-1</v>
       </c>
       <c r="Q194" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R194" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S194" s="4" t="s">
         <v>16</v>
@@ -35079,10 +35079,10 @@
         <v>-1</v>
       </c>
       <c r="Q195" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R195" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S195" s="4" t="s">
         <v>211</v>
@@ -35165,10 +35165,10 @@
         <v>-2</v>
       </c>
       <c r="Q196" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R196" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S196" s="4" t="s">
         <v>4</v>
@@ -35251,10 +35251,10 @@
         <v>-1</v>
       </c>
       <c r="Q197" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R197" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S197" s="4" t="s">
         <v>4</v>
@@ -35337,10 +35337,10 @@
         <v>-3</v>
       </c>
       <c r="Q198" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R198" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S198" s="4" t="s">
         <v>22</v>
@@ -35425,10 +35425,10 @@
         <v>-1</v>
       </c>
       <c r="Q199" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R199" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S199" s="4" t="s">
         <v>2</v>
@@ -35511,10 +35511,10 @@
         <v>-1</v>
       </c>
       <c r="Q200" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R200" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S200" s="4" t="s">
         <v>4</v>
@@ -35597,10 +35597,10 @@
         <v>-1</v>
       </c>
       <c r="Q201" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R201" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S201" s="4" t="s">
         <v>12</v>
@@ -35683,10 +35683,10 @@
         <v>-3</v>
       </c>
       <c r="Q202" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R202" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S202" s="4" t="s">
         <v>219</v>
@@ -35769,10 +35769,10 @@
         <v>-6</v>
       </c>
       <c r="Q203" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R203" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S203" s="4" t="s">
         <v>16</v>
@@ -35855,10 +35855,10 @@
         <v>-2</v>
       </c>
       <c r="Q204" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R204" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S204" s="4" t="s">
         <v>2</v>
@@ -35941,10 +35941,10 @@
         <v>-3</v>
       </c>
       <c r="Q205" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R205" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S205" s="4" t="s">
         <v>223</v>
@@ -36027,10 +36027,10 @@
         <v>-1</v>
       </c>
       <c r="Q206" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R206" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S206" s="4" t="s">
         <v>94</v>
@@ -36113,10 +36113,10 @@
         <v>-2</v>
       </c>
       <c r="Q207" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R207" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S207" s="4" t="s">
         <v>172</v>
@@ -36199,10 +36199,10 @@
         <v>0</v>
       </c>
       <c r="Q208" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R208" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S208" s="4" t="s">
         <v>6</v>
@@ -36285,10 +36285,10 @@
         <v>-2</v>
       </c>
       <c r="Q209" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R209" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S209" s="4" t="s">
         <v>2</v>
@@ -36371,10 +36371,10 @@
         <v>-2</v>
       </c>
       <c r="Q210" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R210" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S210" s="4" t="s">
         <v>172</v>
@@ -36457,10 +36457,10 @@
         <v>-1</v>
       </c>
       <c r="Q211" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R211" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S211" s="4" t="s">
         <v>69</v>
@@ -36543,10 +36543,10 @@
         <v>-1</v>
       </c>
       <c r="Q212" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R212" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S212" s="4" t="s">
         <v>132</v>
@@ -36629,10 +36629,10 @@
         <v>0</v>
       </c>
       <c r="Q213" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R213" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S213" s="4" t="s">
         <v>231</v>
@@ -36715,10 +36715,10 @@
         <v>-3</v>
       </c>
       <c r="Q214" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R214" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S214" s="4" t="s">
         <v>2</v>
@@ -36801,10 +36801,10 @@
         <v>-2</v>
       </c>
       <c r="Q215" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R215" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S215" s="4" t="s">
         <v>191</v>
@@ -36889,10 +36889,10 @@
         <v>-1</v>
       </c>
       <c r="Q216" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R216" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S216" s="4" t="s">
         <v>6</v>
@@ -36975,10 +36975,10 @@
         <v>-2</v>
       </c>
       <c r="Q217" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R217" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S217" s="4" t="s">
         <v>4</v>
@@ -37061,10 +37061,10 @@
         <v>-3</v>
       </c>
       <c r="Q218" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R218" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S218" s="4" t="s">
         <v>4</v>
@@ -37147,10 +37147,10 @@
         <v>-3</v>
       </c>
       <c r="Q219" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R219" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S219" s="4" t="s">
         <v>238</v>
@@ -37235,10 +37235,10 @@
         <v>-1</v>
       </c>
       <c r="Q220" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R220" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S220" s="4" t="s">
         <v>65</v>
@@ -37321,10 +37321,10 @@
         <v>0</v>
       </c>
       <c r="Q221" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R221" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S221" s="4" t="s">
         <v>241</v>
@@ -37407,10 +37407,10 @@
         <v>0</v>
       </c>
       <c r="Q222" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R222" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S222" s="4" t="s">
         <v>6</v>
@@ -37493,10 +37493,10 @@
         <v>3</v>
       </c>
       <c r="Q223" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R223" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S223" s="4" t="s">
         <v>9</v>
@@ -37579,10 +37579,10 @@
         <v>-1</v>
       </c>
       <c r="Q224" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R224" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S224" s="4" t="s">
         <v>107</v>
@@ -37665,10 +37665,10 @@
         <v>-2</v>
       </c>
       <c r="Q225" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R225" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S225" s="4" t="s">
         <v>16</v>
@@ -37751,10 +37751,10 @@
         <v>-1</v>
       </c>
       <c r="Q226" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R226" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S226" s="4" t="s">
         <v>9</v>
@@ -37837,10 +37837,10 @@
         <v>1</v>
       </c>
       <c r="Q227" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R227" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S227" s="4" t="s">
         <v>172</v>
@@ -37923,10 +37923,10 @@
         <v>-2</v>
       </c>
       <c r="Q228" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R228" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S228" s="4" t="s">
         <v>249</v>
@@ -38009,10 +38009,10 @@
         <v>-3</v>
       </c>
       <c r="Q229" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R229" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S229" s="4" t="s">
         <v>24</v>
@@ -38095,10 +38095,10 @@
         <v>0</v>
       </c>
       <c r="Q230" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R230" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S230" s="4" t="s">
         <v>9</v>
@@ -38181,10 +38181,10 @@
         <v>1</v>
       </c>
       <c r="Q231" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R231" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S231" s="4" t="s">
         <v>9</v>
@@ -38267,10 +38267,10 @@
         <v>-2</v>
       </c>
       <c r="Q232" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R232" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S232" s="4" t="s">
         <v>9</v>
@@ -38355,10 +38355,10 @@
         <v>-1</v>
       </c>
       <c r="Q233" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R233" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S233" s="4" t="s">
         <v>255</v>
@@ -38441,10 +38441,10 @@
         <v>-2</v>
       </c>
       <c r="Q234" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R234" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S234" s="4" t="s">
         <v>22</v>
@@ -38527,10 +38527,10 @@
         <v>-2</v>
       </c>
       <c r="Q235" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R235" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S235" s="4" t="s">
         <v>6</v>
@@ -38613,10 +38613,10 @@
         <v>-1</v>
       </c>
       <c r="Q236" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R236" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S236" s="4" t="s">
         <v>12</v>
@@ -38699,10 +38699,10 @@
         <v>3</v>
       </c>
       <c r="Q237" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R237" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S237" s="4" t="s">
         <v>2</v>
@@ -38785,10 +38785,10 @@
         <v>-7</v>
       </c>
       <c r="Q238" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R238" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S238" s="4" t="s">
         <v>4</v>
@@ -38871,10 +38871,10 @@
         <v>-3</v>
       </c>
       <c r="Q239" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R239" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S239" s="4" t="s">
         <v>4</v>
@@ -38957,10 +38957,10 @@
         <v>1</v>
       </c>
       <c r="Q240" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R240" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S240" s="4" t="s">
         <v>2</v>
@@ -39043,10 +39043,10 @@
         <v>-11</v>
       </c>
       <c r="Q241" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R241" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S241" s="4" t="s">
         <v>16</v>
@@ -39129,10 +39129,10 @@
         <v>-1</v>
       </c>
       <c r="Q242" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R242" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S242" s="4" t="s">
         <v>4</v>
@@ -39215,10 +39215,10 @@
         <v>-3</v>
       </c>
       <c r="Q243" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R243" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S243" s="4" t="s">
         <v>223</v>
@@ -39301,10 +39301,10 @@
         <v>-2</v>
       </c>
       <c r="Q244" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R244" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S244" s="4" t="s">
         <v>2</v>
@@ -39387,10 +39387,10 @@
         <v>-2</v>
       </c>
       <c r="Q245" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R245" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S245" s="4" t="s">
         <v>69</v>
@@ -39473,10 +39473,10 @@
         <v>-7</v>
       </c>
       <c r="Q246" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R246" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S246" s="4" t="s">
         <v>255</v>
@@ -39559,10 +39559,10 @@
         <v>1</v>
       </c>
       <c r="Q247" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R247" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S247" s="4" t="s">
         <v>2</v>
@@ -39645,10 +39645,10 @@
         <v>-1</v>
       </c>
       <c r="Q248" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R248" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S248" s="4" t="s">
         <v>19</v>
@@ -39731,10 +39731,10 @@
         <v>1</v>
       </c>
       <c r="Q249" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R249" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S249" s="4" t="s">
         <v>16</v>
@@ -39817,10 +39817,10 @@
         <v>0</v>
       </c>
       <c r="Q250" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R250" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S250" s="4" t="s">
         <v>2</v>
@@ -39903,10 +39903,10 @@
         <v>-3</v>
       </c>
       <c r="Q251" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R251" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S251" s="4" t="s">
         <v>4</v>
@@ -39989,10 +39989,10 @@
         <v>-5</v>
       </c>
       <c r="Q252" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R252" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S252" s="4" t="s">
         <v>135</v>
@@ -40075,10 +40075,10 @@
         <v>2</v>
       </c>
       <c r="Q253" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R253" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S253" s="4" t="s">
         <v>19</v>
@@ -40161,10 +40161,10 @@
         <v>-3</v>
       </c>
       <c r="Q254" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R254" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S254" s="4" t="s">
         <v>211</v>
@@ -40247,10 +40247,10 @@
         <v>1</v>
       </c>
       <c r="Q255" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R255" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S255" s="4" t="s">
         <v>0</v>
@@ -40335,10 +40335,10 @@
         <v>-3</v>
       </c>
       <c r="Q256" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R256" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S256" s="4" t="s">
         <v>4</v>
@@ -40421,10 +40421,10 @@
         <v>-2</v>
       </c>
       <c r="Q257" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R257" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S257" s="4" t="s">
         <v>2</v>
@@ -40507,10 +40507,10 @@
         <v>-3</v>
       </c>
       <c r="Q258" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R258" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S258" s="4" t="s">
         <v>255</v>
@@ -40593,10 +40593,10 @@
         <v>-1</v>
       </c>
       <c r="Q259" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R259" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S259" s="4" t="s">
         <v>4</v>
@@ -40679,10 +40679,10 @@
         <v>-1</v>
       </c>
       <c r="Q260" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R260" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S260" s="4" t="s">
         <v>6</v>
@@ -40765,10 +40765,10 @@
         <v>-2</v>
       </c>
       <c r="Q261" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R261" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S261" s="4" t="s">
         <v>16</v>
@@ -40851,10 +40851,10 @@
         <v>-3</v>
       </c>
       <c r="Q262" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R262" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S262" s="4" t="s">
         <v>4</v>
@@ -40937,10 +40937,10 @@
         <v>-3</v>
       </c>
       <c r="Q263" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R263" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S263" s="4" t="s">
         <v>2</v>
@@ -41025,10 +41025,10 @@
         <v>-3</v>
       </c>
       <c r="Q264" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R264" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S264" s="4" t="s">
         <v>4</v>
@@ -41111,10 +41111,10 @@
         <v>-2</v>
       </c>
       <c r="Q265" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R265" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S265" s="4" t="s">
         <v>2</v>
@@ -41197,10 +41197,10 @@
         <v>-1</v>
       </c>
       <c r="Q266" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R266" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S266" s="4" t="s">
         <v>24</v>
@@ -41283,10 +41283,10 @@
         <v>-3</v>
       </c>
       <c r="Q267" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R267" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S267" s="4" t="s">
         <v>94</v>
@@ -41369,10 +41369,10 @@
         <v>0</v>
       </c>
       <c r="Q268" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R268" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S268" s="4" t="s">
         <v>16</v>
@@ -41455,10 +41455,10 @@
         <v>2</v>
       </c>
       <c r="Q269" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R269" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S269" s="4" t="s">
         <v>9</v>
@@ -41541,10 +41541,10 @@
         <v>-3</v>
       </c>
       <c r="Q270" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R270" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S270" s="4" t="s">
         <v>16</v>
@@ -41627,10 +41627,10 @@
         <v>-3</v>
       </c>
       <c r="Q271" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R271" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S271" s="4" t="s">
         <v>40</v>
@@ -41713,10 +41713,10 @@
         <v>-3</v>
       </c>
       <c r="Q272" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R272" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S272" s="4" t="s">
         <v>31</v>
@@ -41799,10 +41799,10 @@
         <v>-3</v>
       </c>
       <c r="Q273" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R273" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S273" s="4" t="s">
         <v>89</v>
@@ -41885,10 +41885,10 @@
         <v>-3</v>
       </c>
       <c r="Q274" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R274" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S274" s="4" t="s">
         <v>0</v>
@@ -41971,10 +41971,10 @@
         <v>-1</v>
       </c>
       <c r="Q275" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R275" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S275" s="4" t="s">
         <v>281</v>
@@ -42057,10 +42057,10 @@
         <v>-5</v>
       </c>
       <c r="Q276" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R276" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S276" s="4" t="s">
         <v>22</v>
@@ -42143,10 +42143,10 @@
         <v>-2</v>
       </c>
       <c r="Q277" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R277" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S277" s="4" t="s">
         <v>78</v>
@@ -42229,10 +42229,10 @@
         <v>-1</v>
       </c>
       <c r="Q278" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R278" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S278" s="4" t="s">
         <v>4</v>
@@ -42315,10 +42315,10 @@
         <v>-1</v>
       </c>
       <c r="Q279" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R279" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S279" s="4" t="s">
         <v>4</v>
@@ -42401,10 +42401,10 @@
         <v>-3</v>
       </c>
       <c r="Q280" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R280" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S280" s="4" t="s">
         <v>16</v>
@@ -42487,10 +42487,10 @@
         <v>-3</v>
       </c>
       <c r="Q281" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R281" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S281" s="4" t="s">
         <v>9</v>
@@ -42573,10 +42573,10 @@
         <v>-3</v>
       </c>
       <c r="Q282" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R282" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S282" s="4" t="s">
         <v>6</v>
@@ -42659,10 +42659,10 @@
         <v>-3</v>
       </c>
       <c r="Q283" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R283" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S283" s="4" t="s">
         <v>16</v>
@@ -42745,10 +42745,10 @@
         <v>0</v>
       </c>
       <c r="Q284" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R284" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S284" s="4" t="s">
         <v>6</v>
@@ -42831,10 +42831,10 @@
         <v>0</v>
       </c>
       <c r="Q285" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R285" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S285" s="4" t="s">
         <v>16</v>
@@ -42917,10 +42917,10 @@
         <v>-3</v>
       </c>
       <c r="Q286" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R286" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S286" s="4" t="s">
         <v>19</v>
@@ -43005,10 +43005,10 @@
         <v>-2</v>
       </c>
       <c r="Q287" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R287" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S287" s="4" t="s">
         <v>16</v>
@@ -43091,10 +43091,10 @@
         <v>1</v>
       </c>
       <c r="Q288" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R288" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S288" s="4" t="s">
         <v>9</v>
@@ -43177,10 +43177,10 @@
         <v>-2</v>
       </c>
       <c r="Q289" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R289" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S289" s="4" t="s">
         <v>100</v>
@@ -43263,10 +43263,10 @@
         <v>-5</v>
       </c>
       <c r="Q290" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R290" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S290" s="4" t="s">
         <v>16</v>
@@ -43349,10 +43349,10 @@
         <v>1</v>
       </c>
       <c r="Q291" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R291" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S291" s="4" t="s">
         <v>78</v>
@@ -43435,10 +43435,10 @@
         <v>-1</v>
       </c>
       <c r="Q292" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R292" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S292" s="4" t="s">
         <v>22</v>
@@ -43521,10 +43521,10 @@
         <v>-1</v>
       </c>
       <c r="Q293" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R293" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S293" s="4" t="s">
         <v>9</v>
@@ -43607,10 +43607,10 @@
         <v>-2</v>
       </c>
       <c r="Q294" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R294" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S294" s="4" t="s">
         <v>16</v>
@@ -43693,10 +43693,10 @@
         <v>-1</v>
       </c>
       <c r="Q295" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R295" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S295" s="4" t="s">
         <v>1010</v>
@@ -43779,10 +43779,10 @@
         <v>-1</v>
       </c>
       <c r="Q296" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R296" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S296" s="4" t="s">
         <v>2</v>
@@ -43865,10 +43865,10 @@
         <v>-2</v>
       </c>
       <c r="Q297" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R297" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S297" s="4" t="s">
         <v>45</v>
@@ -43951,10 +43951,10 @@
         <v>-2</v>
       </c>
       <c r="Q298" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R298" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S298" s="4" t="s">
         <v>2</v>
@@ -44037,10 +44037,10 @@
         <v>-6</v>
       </c>
       <c r="Q299" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R299" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S299" s="4" t="s">
         <v>22</v>
@@ -44123,10 +44123,10 @@
         <v>-6</v>
       </c>
       <c r="Q300" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R300" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S300" s="4" t="s">
         <v>22</v>
@@ -44209,10 +44209,10 @@
         <v>-2</v>
       </c>
       <c r="Q301" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R301" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S301" s="4" t="s">
         <v>111</v>
@@ -44295,10 +44295,10 @@
         <v>-3</v>
       </c>
       <c r="Q302" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R302" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S302" s="4" t="s">
         <v>211</v>
@@ -44381,10 +44381,10 @@
         <v>-3</v>
       </c>
       <c r="Q303" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R303" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S303" s="4" t="s">
         <v>78</v>
@@ -44467,10 +44467,10 @@
         <v>-9</v>
       </c>
       <c r="Q304" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R304" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S304" s="11" t="s">
         <v>6</v>
@@ -44553,10 +44553,10 @@
         <v>-7</v>
       </c>
       <c r="Q305" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R305" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S305" s="11" t="s">
         <v>6</v>
@@ -44639,10 +44639,10 @@
         <v>-10</v>
       </c>
       <c r="Q306" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R306" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S306" s="11" t="s">
         <v>78</v>
@@ -44725,10 +44725,10 @@
         <v>-2</v>
       </c>
       <c r="Q307" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R307" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S307" s="11" t="s">
         <v>0</v>
@@ -44811,10 +44811,10 @@
         <v>-3</v>
       </c>
       <c r="Q308" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R308" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S308" s="11" t="s">
         <v>6</v>
@@ -44897,10 +44897,10 @@
         <v>-3</v>
       </c>
       <c r="Q309" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R309" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S309" s="11" t="s">
         <v>1035</v>
@@ -44983,10 +44983,10 @@
         <v>-3</v>
       </c>
       <c r="Q310" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R310" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S310" s="11" t="s">
         <v>1040</v>
@@ -45069,10 +45069,10 @@
         <v>-3</v>
       </c>
       <c r="Q311" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R311" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S311" s="11" t="s">
         <v>6</v>
@@ -45119,7 +45119,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:N311">
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -45213,7 +45213,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -45552,10 +45552,10 @@
         <v>-1</v>
       </c>
       <c r="Q4" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R4" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S4" s="11" t="s">
         <v>9</v>
@@ -45638,10 +45638,10 @@
         <v>0</v>
       </c>
       <c r="Q5" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R5" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S5" s="11" t="s">
         <v>6</v>
@@ -45724,10 +45724,10 @@
         <v>-3</v>
       </c>
       <c r="Q6" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R6" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>2</v>
@@ -45808,10 +45808,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R7" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S7" s="11" t="s">
         <v>6</v>
@@ -45894,10 +45894,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R8" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>211</v>
@@ -45980,10 +45980,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R9" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S9" s="11" t="s">
         <v>6</v>
@@ -46030,7 +46030,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K4 L4:N5 J6:N9">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -46048,25 +46048,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I7">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -46084,7 +46084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -46102,7 +46102,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
#1 arrow can rotate now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="1388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="1388">
   <si>
     <t>arrow</t>
   </si>
@@ -4943,10 +4943,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000046;80|55010028;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>英雄</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5060,6 +5056,10 @@
   </si>
   <si>
     <t>Dhit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6050,73 +6050,24 @@
   <dxfs count="77">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6132,9 +6083,36 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="宋体"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -6324,245 +6302,6 @@
         <color theme="1"/>
         <name val="宋体"/>
         <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -7234,6 +6973,255 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -7949,6 +7937,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8241,11 +8241,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-925128960"/>
-        <c:axId val="-925126240"/>
+        <c:axId val="1320121568"/>
+        <c:axId val="1320130272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-925128960"/>
+        <c:axId val="1320121568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8288,7 +8288,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-925126240"/>
+        <c:crossAx val="1320130272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8296,7 +8296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-925126240"/>
+        <c:axId val="1320130272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8347,7 +8347,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-925128960"/>
+        <c:crossAx val="1320121568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18040,99 +18040,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AF311" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AF311" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
   <autoFilter ref="A3:AF311"/>
   <sortState ref="A4:AD311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="Id" dataDxfId="73"/>
-    <tableColumn id="2" name="Name" dataDxfId="72"/>
-    <tableColumn id="22" name="Ename" dataDxfId="71"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="70"/>
-    <tableColumn id="3" name="Star" dataDxfId="69"/>
-    <tableColumn id="4" name="Type" dataDxfId="68"/>
-    <tableColumn id="5" name="Attr" dataDxfId="67"/>
-    <tableColumn id="12" name="Cost" dataDxfId="66"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="65"/>
-    <tableColumn id="24" name="VitP" dataDxfId="64"/>
-    <tableColumn id="26" name="Sum" dataDxfId="63">
+    <tableColumn id="1" name="Id" dataDxfId="72"/>
+    <tableColumn id="2" name="Name" dataDxfId="71"/>
+    <tableColumn id="22" name="Ename" dataDxfId="70"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="69"/>
+    <tableColumn id="3" name="Star" dataDxfId="68"/>
+    <tableColumn id="4" name="Type" dataDxfId="67"/>
+    <tableColumn id="5" name="Attr" dataDxfId="66"/>
+    <tableColumn id="12" name="Cost" dataDxfId="65"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="64"/>
+    <tableColumn id="24" name="VitP" dataDxfId="63"/>
+    <tableColumn id="26" name="Sum" dataDxfId="62">
       <calculatedColumnFormula>SUM(I4:J4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Modify" dataDxfId="62"/>
-    <tableColumn id="9" name="Def" dataDxfId="19"/>
-    <tableColumn id="10" name="Mag" dataDxfId="18"/>
-    <tableColumn id="32" name="Spd" dataDxfId="17"/>
-    <tableColumn id="35" name="Hit" dataDxfId="16"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="15"/>
-    <tableColumn id="34" name="Crt" dataDxfId="14"/>
-    <tableColumn id="33" name="Luk" dataDxfId="13"/>
-    <tableColumn id="13" name="Range" dataDxfId="61"/>
-    <tableColumn id="14" name="Mov" dataDxfId="60"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="59"/>
-    <tableColumn id="17" name="Cover" dataDxfId="58"/>
-    <tableColumn id="18" name="Skills" dataDxfId="57"/>
-    <tableColumn id="30" name="AttrAtk" dataDxfId="56"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="55"/>
-    <tableColumn id="20" name="Res" dataDxfId="54"/>
-    <tableColumn id="21" name="Icon" dataDxfId="53"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="52"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="51"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="50"/>
-    <tableColumn id="29" name="Remark" dataDxfId="49"/>
+    <tableColumn id="25" name="Modify" dataDxfId="61"/>
+    <tableColumn id="9" name="Def" dataDxfId="60"/>
+    <tableColumn id="10" name="Mag" dataDxfId="59"/>
+    <tableColumn id="32" name="Spd" dataDxfId="58"/>
+    <tableColumn id="35" name="Hit" dataDxfId="57"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="56"/>
+    <tableColumn id="34" name="Crt" dataDxfId="55"/>
+    <tableColumn id="33" name="Luk" dataDxfId="54"/>
+    <tableColumn id="13" name="Range" dataDxfId="53"/>
+    <tableColumn id="14" name="Mov" dataDxfId="52"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="51"/>
+    <tableColumn id="17" name="Cover" dataDxfId="50"/>
+    <tableColumn id="18" name="Skills" dataDxfId="49"/>
+    <tableColumn id="30" name="AttrAtk" dataDxfId="48"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="47"/>
+    <tableColumn id="20" name="Res" dataDxfId="46"/>
+    <tableColumn id="21" name="Icon" dataDxfId="45"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="44"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="43"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="42"/>
+    <tableColumn id="29" name="Remark" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A3:AF9" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A3:AF9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A3:AF9"/>
   <sortState ref="A4:AC9">
     <sortCondition ref="A3:A9"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="Id" dataDxfId="45"/>
-    <tableColumn id="2" name="Name" dataDxfId="44"/>
-    <tableColumn id="22" name="Ename" dataDxfId="43"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="42"/>
-    <tableColumn id="3" name="Star" dataDxfId="41"/>
-    <tableColumn id="4" name="Type" dataDxfId="40"/>
-    <tableColumn id="5" name="Attr" dataDxfId="39"/>
-    <tableColumn id="12" name="Cost" dataDxfId="38"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="37"/>
-    <tableColumn id="24" name="VitP" dataDxfId="36"/>
-    <tableColumn id="26" name="Sum" dataDxfId="35">
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Name" dataDxfId="31"/>
+    <tableColumn id="22" name="Ename" dataDxfId="30"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="29"/>
+    <tableColumn id="3" name="Star" dataDxfId="28"/>
+    <tableColumn id="4" name="Type" dataDxfId="27"/>
+    <tableColumn id="5" name="Attr" dataDxfId="26"/>
+    <tableColumn id="12" name="Cost" dataDxfId="25"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="24"/>
+    <tableColumn id="24" name="VitP" dataDxfId="23"/>
+    <tableColumn id="26" name="Sum" dataDxfId="22">
       <calculatedColumnFormula>SUM(I4:J4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Modify" dataDxfId="34"/>
-    <tableColumn id="10" name="Def" dataDxfId="11"/>
-    <tableColumn id="32" name="Mag" dataDxfId="10"/>
-    <tableColumn id="34" name="Spd" dataDxfId="8"/>
-    <tableColumn id="36" name="Hit" dataDxfId="6"/>
-    <tableColumn id="35" name="Dhit" dataDxfId="7"/>
-    <tableColumn id="33" name="Crt" dataDxfId="9"/>
-    <tableColumn id="9" name="Luk" dataDxfId="12"/>
-    <tableColumn id="13" name="Range" dataDxfId="33"/>
-    <tableColumn id="14" name="Mov" dataDxfId="32"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="31"/>
-    <tableColumn id="17" name="Cover" dataDxfId="30"/>
-    <tableColumn id="18" name="Skills" dataDxfId="29"/>
-    <tableColumn id="30" name="AttrAtk" dataDxfId="28"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="27"/>
-    <tableColumn id="20" name="Res" dataDxfId="26"/>
-    <tableColumn id="21" name="Icon" dataDxfId="25"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="24"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="23"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="22"/>
-    <tableColumn id="29" name="Remark" dataDxfId="21"/>
+    <tableColumn id="25" name="Modify" dataDxfId="21"/>
+    <tableColumn id="10" name="Def" dataDxfId="20"/>
+    <tableColumn id="32" name="Mag" dataDxfId="19"/>
+    <tableColumn id="34" name="Spd" dataDxfId="18"/>
+    <tableColumn id="36" name="Hit" dataDxfId="17"/>
+    <tableColumn id="35" name="Dhit" dataDxfId="16"/>
+    <tableColumn id="33" name="Crt" dataDxfId="15"/>
+    <tableColumn id="9" name="Luk" dataDxfId="14"/>
+    <tableColumn id="13" name="Range" dataDxfId="13"/>
+    <tableColumn id="14" name="Mov" dataDxfId="12"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="11"/>
+    <tableColumn id="17" name="Cover" dataDxfId="10"/>
+    <tableColumn id="18" name="Skills" dataDxfId="9"/>
+    <tableColumn id="30" name="AttrAtk" dataDxfId="8"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="7"/>
+    <tableColumn id="20" name="Res" dataDxfId="6"/>
+    <tableColumn id="21" name="Icon" dataDxfId="5"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
+    <tableColumn id="29" name="Remark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -18439,10 +18439,10 @@
   <dimension ref="A1:AF311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18501,31 +18501,31 @@
         <v>976</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="T1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="U1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>1365</v>
       </c>
       <c r="V1" s="17" t="s">
         <v>327</v>
@@ -18599,31 +18599,31 @@
         <v>969</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>300</v>
@@ -18697,31 +18697,31 @@
         <v>977</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="T3" s="6" t="s">
+        <v>1366</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>1367</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>1368</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>310</v>
@@ -18789,7 +18789,7 @@
         <v>-25</v>
       </c>
       <c r="K4" s="15">
-        <f>SUM(I4:J4)</f>
+        <f t="shared" ref="K4:K67" si="0">SUM(I4:J4)</f>
         <v>-20</v>
       </c>
       <c r="L4" s="9">
@@ -18886,7 +18886,7 @@
         <v>13</v>
       </c>
       <c r="K5" s="15">
-        <f>SUM(I5:J5)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="L5" s="9">
@@ -18981,7 +18981,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="15">
-        <f>SUM(I6:J6)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="L6" s="4">
@@ -19076,7 +19076,7 @@
         <v>7</v>
       </c>
       <c r="K7" s="15">
-        <f>SUM(I7:J7)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="L7" s="4">
@@ -19171,7 +19171,7 @@
         <v>30</v>
       </c>
       <c r="K8" s="15">
-        <f>SUM(I8:J8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8" s="4">
@@ -19268,7 +19268,7 @@
         <v>11</v>
       </c>
       <c r="K9" s="15">
-        <f>SUM(I9:J9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9" s="4">
@@ -19363,7 +19363,7 @@
         <v>-5</v>
       </c>
       <c r="K10" s="15">
-        <f>SUM(I10:J10)</f>
+        <f t="shared" si="0"/>
         <v>-14</v>
       </c>
       <c r="L10" s="4">
@@ -19458,7 +19458,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="15">
-        <f>SUM(I11:J11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L11" s="4">
@@ -19553,7 +19553,7 @@
         <v>6</v>
       </c>
       <c r="K12" s="15">
-        <f>SUM(I12:J12)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="L12" s="4">
@@ -19648,7 +19648,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="15">
-        <f>SUM(I13:J13)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L13" s="37">
@@ -19743,7 +19743,7 @@
         <v>-15</v>
       </c>
       <c r="K14" s="15">
-        <f>SUM(I14:J14)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="L14" s="9">
@@ -19838,7 +19838,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="15">
-        <f>SUM(I15:J15)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="L15" s="37">
@@ -19935,7 +19935,7 @@
         <v>9</v>
       </c>
       <c r="K16" s="15">
-        <f>SUM(I16:J16)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L16" s="9">
@@ -20032,7 +20032,7 @@
         <v>12</v>
       </c>
       <c r="K17" s="15">
-        <f>SUM(I17:J17)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="L17" s="4">
@@ -20129,7 +20129,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="15">
-        <f>SUM(I18:J18)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L18" s="4">
@@ -20224,7 +20224,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="15">
-        <f>SUM(I19:J19)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L19" s="4">
@@ -20319,7 +20319,7 @@
         <v>5</v>
       </c>
       <c r="K20" s="15">
-        <f>SUM(I20:J20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L20" s="4">
@@ -20414,7 +20414,7 @@
         <v>13</v>
       </c>
       <c r="K21" s="15">
-        <f>SUM(I21:J21)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="L21" s="4">
@@ -20511,7 +20511,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="15">
-        <f>SUM(I22:J22)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L22" s="4">
@@ -20606,7 +20606,7 @@
         <v>-11</v>
       </c>
       <c r="K23" s="15">
-        <f>SUM(I23:J23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L23" s="9">
@@ -20703,7 +20703,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="15">
-        <f>SUM(I24:J24)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="L24" s="4">
@@ -20798,7 +20798,7 @@
         <v>-10</v>
       </c>
       <c r="K25" s="15">
-        <f>SUM(I25:J25)</f>
+        <f t="shared" si="0"/>
         <v>-14</v>
       </c>
       <c r="L25" s="4">
@@ -20893,7 +20893,7 @@
         <v>-8</v>
       </c>
       <c r="K26" s="15">
-        <f>SUM(I26:J26)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L26" s="4">
@@ -20990,7 +20990,7 @@
         <v>19</v>
       </c>
       <c r="K27" s="15">
-        <f>SUM(I27:J27)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="L27" s="9">
@@ -21085,7 +21085,7 @@
         <v>-17</v>
       </c>
       <c r="K28" s="15">
-        <f>SUM(I28:J28)</f>
+        <f t="shared" si="0"/>
         <v>-21</v>
       </c>
       <c r="L28" s="4">
@@ -21180,7 +21180,7 @@
         <v>19</v>
       </c>
       <c r="K29" s="15">
-        <f>SUM(I29:J29)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L29" s="4">
@@ -21275,7 +21275,7 @@
         <v>13</v>
       </c>
       <c r="K30" s="15">
-        <f>SUM(I30:J30)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L30" s="4">
@@ -21370,7 +21370,7 @@
         <v>-15</v>
       </c>
       <c r="K31" s="15">
-        <f>SUM(I31:J31)</f>
+        <f t="shared" si="0"/>
         <v>-15</v>
       </c>
       <c r="L31" s="4">
@@ -21465,7 +21465,7 @@
         <v>-20</v>
       </c>
       <c r="K32" s="15">
-        <f>SUM(I32:J32)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L32" s="4">
@@ -21560,7 +21560,7 @@
         <v>15</v>
       </c>
       <c r="K33" s="15">
-        <f>SUM(I33:J33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L33" s="9">
@@ -21655,7 +21655,7 @@
         <v>-13</v>
       </c>
       <c r="K34" s="15">
-        <f>SUM(I34:J34)</f>
+        <f t="shared" si="0"/>
         <v>-19</v>
       </c>
       <c r="L34" s="9">
@@ -21750,7 +21750,7 @@
         <v>25</v>
       </c>
       <c r="K35" s="15">
-        <f>SUM(I35:J35)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L35" s="4">
@@ -21845,7 +21845,7 @@
         <v>3</v>
       </c>
       <c r="K36" s="15">
-        <f>SUM(I36:J36)</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="L36" s="4">
@@ -21940,7 +21940,7 @@
         <v>17</v>
       </c>
       <c r="K37" s="15">
-        <f>SUM(I37:J37)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="L37" s="4">
@@ -22035,7 +22035,7 @@
         <v>24</v>
       </c>
       <c r="K38" s="15">
-        <f>SUM(I38:J38)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L38" s="4">
@@ -22132,7 +22132,7 @@
         <v>10</v>
       </c>
       <c r="K39" s="15">
-        <f>SUM(I39:J39)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="L39" s="4">
@@ -22225,7 +22225,7 @@
         <v>9</v>
       </c>
       <c r="K40" s="15">
-        <f>SUM(I40:J40)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="L40" s="4">
@@ -22320,7 +22320,7 @@
         <v>-10</v>
       </c>
       <c r="K41" s="15">
-        <f>SUM(I41:J41)</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="L41" s="4">
@@ -22415,7 +22415,7 @@
         <v>8</v>
       </c>
       <c r="K42" s="15">
-        <f>SUM(I42:J42)</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="L42" s="4">
@@ -22510,7 +22510,7 @@
         <v>15</v>
       </c>
       <c r="K43" s="15">
-        <f>SUM(I43:J43)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="L43" s="4">
@@ -22605,7 +22605,7 @@
         <v>-14</v>
       </c>
       <c r="K44" s="15">
-        <f>SUM(I44:J44)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L44" s="4">
@@ -22700,7 +22700,7 @@
         <v>-12</v>
       </c>
       <c r="K45" s="15">
-        <f>SUM(I45:J45)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="L45" s="4">
@@ -22795,7 +22795,7 @@
         <v>-10</v>
       </c>
       <c r="K46" s="15">
-        <f>SUM(I46:J46)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="L46" s="4">
@@ -22890,7 +22890,7 @@
         <v>10</v>
       </c>
       <c r="K47" s="15">
-        <f>SUM(I47:J47)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="L47" s="9">
@@ -22985,7 +22985,7 @@
         <v>20</v>
       </c>
       <c r="K48" s="15">
-        <f>SUM(I48:J48)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="L48" s="4">
@@ -23080,7 +23080,7 @@
         <v>8</v>
       </c>
       <c r="K49" s="15">
-        <f>SUM(I49:J49)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="L49" s="4">
@@ -23175,7 +23175,7 @@
         <v>3</v>
       </c>
       <c r="K50" s="15">
-        <f>SUM(I50:J50)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="L50" s="4">
@@ -23270,7 +23270,7 @@
         <v>17</v>
       </c>
       <c r="K51" s="15">
-        <f>SUM(I51:J51)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L51" s="4">
@@ -23365,7 +23365,7 @@
         <v>15</v>
       </c>
       <c r="K52" s="15">
-        <f>SUM(I52:J52)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L52" s="4">
@@ -23460,7 +23460,7 @@
         <v>7</v>
       </c>
       <c r="K53" s="15">
-        <f>SUM(I53:J53)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="L53" s="9">
@@ -23555,7 +23555,7 @@
         <v>17</v>
       </c>
       <c r="K54" s="15">
-        <f>SUM(I54:J54)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L54" s="4">
@@ -23650,7 +23650,7 @@
         <v>13</v>
       </c>
       <c r="K55" s="15">
-        <f>SUM(I55:J55)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="L55" s="4">
@@ -23745,7 +23745,7 @@
         <v>-8</v>
       </c>
       <c r="K56" s="15">
-        <f>SUM(I56:J56)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L56" s="4">
@@ -23840,7 +23840,7 @@
         <v>-3</v>
       </c>
       <c r="K57" s="15">
-        <f>SUM(I57:J57)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L57" s="4">
@@ -23935,7 +23935,7 @@
         <v>-10</v>
       </c>
       <c r="K58" s="15">
-        <f>SUM(I58:J58)</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="L58" s="4">
@@ -24030,7 +24030,7 @@
         <v>-5</v>
       </c>
       <c r="K59" s="15">
-        <f>SUM(I59:J59)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="L59" s="4">
@@ -24125,7 +24125,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="15">
-        <f>SUM(I60:J60)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L60" s="4">
@@ -24220,7 +24220,7 @@
         <v>10</v>
       </c>
       <c r="K61" s="15">
-        <f>SUM(I61:J61)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="L61" s="4">
@@ -24315,7 +24315,7 @@
         <v>17</v>
       </c>
       <c r="K62" s="15">
-        <f>SUM(I62:J62)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="L62" s="4">
@@ -24410,7 +24410,7 @@
         <v>12</v>
       </c>
       <c r="K63" s="15">
-        <f>SUM(I63:J63)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="L63" s="4">
@@ -24505,7 +24505,7 @@
         <v>16</v>
       </c>
       <c r="K64" s="15">
-        <f>SUM(I64:J64)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L64" s="4">
@@ -24598,7 +24598,7 @@
         <v>-1</v>
       </c>
       <c r="K65" s="15">
-        <f>SUM(I65:J65)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="L65" s="4">
@@ -24695,7 +24695,7 @@
         <v>5</v>
       </c>
       <c r="K66" s="15">
-        <f>SUM(I66:J66)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L66" s="4">
@@ -24792,7 +24792,7 @@
         <v>14</v>
       </c>
       <c r="K67" s="15">
-        <f>SUM(I67:J67)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="L67" s="4">
@@ -24887,7 +24887,7 @@
         <v>9</v>
       </c>
       <c r="K68" s="15">
-        <f>SUM(I68:J68)</f>
+        <f t="shared" ref="K68:K131" si="1">SUM(I68:J68)</f>
         <v>21</v>
       </c>
       <c r="L68" s="4">
@@ -24984,7 +24984,7 @@
         <v>-10</v>
       </c>
       <c r="K69" s="15">
-        <f>SUM(I69:J69)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L69" s="4">
@@ -25079,7 +25079,7 @@
         <v>18</v>
       </c>
       <c r="K70" s="15">
-        <f>SUM(I70:J70)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="L70" s="4">
@@ -25174,7 +25174,7 @@
         <v>-15</v>
       </c>
       <c r="K71" s="15">
-        <f>SUM(I71:J71)</f>
+        <f t="shared" si="1"/>
         <v>-22</v>
       </c>
       <c r="L71" s="4">
@@ -25269,7 +25269,7 @@
         <v>-10</v>
       </c>
       <c r="K72" s="15">
-        <f>SUM(I72:J72)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L72" s="4">
@@ -25364,7 +25364,7 @@
         <v>18</v>
       </c>
       <c r="K73" s="15">
-        <f>SUM(I73:J73)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="L73" s="4">
@@ -25459,7 +25459,7 @@
         <v>20</v>
       </c>
       <c r="K74" s="15">
-        <f>SUM(I74:J74)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="L74" s="9">
@@ -25554,7 +25554,7 @@
         <v>11</v>
       </c>
       <c r="K75" s="15">
-        <f>SUM(I75:J75)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L75" s="4">
@@ -25649,7 +25649,7 @@
         <v>26</v>
       </c>
       <c r="K76" s="15">
-        <f>SUM(I76:J76)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="L76" s="4">
@@ -25744,7 +25744,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="15">
-        <f>SUM(I77:J77)</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="L77" s="4">
@@ -25839,7 +25839,7 @@
         <v>20</v>
       </c>
       <c r="K78" s="15">
-        <f>SUM(I78:J78)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="L78" s="4">
@@ -25934,7 +25934,7 @@
         <v>-3</v>
       </c>
       <c r="K79" s="15">
-        <f>SUM(I79:J79)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L79" s="4">
@@ -26031,7 +26031,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="15">
-        <f>SUM(I80:J80)</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="L80" s="4">
@@ -26128,7 +26128,7 @@
         <v>14</v>
       </c>
       <c r="K81" s="15">
-        <f>SUM(I81:J81)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="L81" s="4">
@@ -26223,7 +26223,7 @@
         <v>14</v>
       </c>
       <c r="K82" s="15">
-        <f>SUM(I82:J82)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="L82" s="9">
@@ -26318,7 +26318,7 @@
         <v>13</v>
       </c>
       <c r="K83" s="15">
-        <f>SUM(I83:J83)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="L83" s="4">
@@ -26413,7 +26413,7 @@
         <v>-13</v>
       </c>
       <c r="K84" s="15">
-        <f>SUM(I84:J84)</f>
+        <f t="shared" si="1"/>
         <v>-23</v>
       </c>
       <c r="L84" s="4">
@@ -26508,7 +26508,7 @@
         <v>20</v>
       </c>
       <c r="K85" s="15">
-        <f>SUM(I85:J85)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="L85" s="9">
@@ -26603,7 +26603,7 @@
         <v>-19</v>
       </c>
       <c r="K86" s="15">
-        <f>SUM(I86:J86)</f>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="L86" s="4">
@@ -26698,7 +26698,7 @@
         <v>7</v>
       </c>
       <c r="K87" s="15">
-        <f>SUM(I87:J87)</f>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="L87" s="4">
@@ -26793,7 +26793,7 @@
         <v>5</v>
       </c>
       <c r="K88" s="15">
-        <f>SUM(I88:J88)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="L88" s="4">
@@ -26888,7 +26888,7 @@
         <v>18</v>
       </c>
       <c r="K89" s="15">
-        <f>SUM(I89:J89)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="L89" s="4">
@@ -26916,7 +26916,7 @@
         <v>0</v>
       </c>
       <c r="T89" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="U89" s="4">
         <v>10</v>
@@ -26983,7 +26983,7 @@
         <v>-15</v>
       </c>
       <c r="K90" s="15">
-        <f>SUM(I90:J90)</f>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="L90" s="4">
@@ -27078,7 +27078,7 @@
         <v>-19</v>
       </c>
       <c r="K91" s="15">
-        <f>SUM(I91:J91)</f>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="L91" s="4">
@@ -27173,7 +27173,7 @@
         <v>-15</v>
       </c>
       <c r="K92" s="15">
-        <f>SUM(I92:J92)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="L92" s="9">
@@ -27268,7 +27268,7 @@
         <v>-4</v>
       </c>
       <c r="K93" s="15">
-        <f>SUM(I93:J93)</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="L93" s="4">
@@ -27363,7 +27363,7 @@
         <v>14</v>
       </c>
       <c r="K94" s="15">
-        <f>SUM(I94:J94)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="L94" s="4">
@@ -27458,7 +27458,7 @@
         <v>8</v>
       </c>
       <c r="K95" s="15">
-        <f>SUM(I95:J95)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="L95" s="4">
@@ -27553,7 +27553,7 @@
         <v>-10</v>
       </c>
       <c r="K96" s="15">
-        <f>SUM(I96:J96)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="L96" s="4">
@@ -27648,7 +27648,7 @@
         <v>30</v>
       </c>
       <c r="K97" s="15">
-        <f>SUM(I97:J97)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="L97" s="4">
@@ -27743,7 +27743,7 @@
         <v>10</v>
       </c>
       <c r="K98" s="15">
-        <f>SUM(I98:J98)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="L98" s="4">
@@ -27838,7 +27838,7 @@
         <v>0</v>
       </c>
       <c r="K99" s="15">
-        <f>SUM(I99:J99)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="L99" s="4">
@@ -27933,7 +27933,7 @@
         <v>5</v>
       </c>
       <c r="K100" s="15">
-        <f>SUM(I100:J100)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="L100" s="7">
@@ -28030,7 +28030,7 @@
         <v>7</v>
       </c>
       <c r="K101" s="15">
-        <f>SUM(I101:J101)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="L101" s="4">
@@ -28125,7 +28125,7 @@
         <v>5</v>
       </c>
       <c r="K102" s="15">
-        <f>SUM(I102:J102)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L102" s="4">
@@ -28220,7 +28220,7 @@
         <v>25</v>
       </c>
       <c r="K103" s="15">
-        <f>SUM(I103:J103)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L103" s="4">
@@ -28315,7 +28315,7 @@
         <v>22</v>
       </c>
       <c r="K104" s="15">
-        <f>SUM(I104:J104)</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="L104" s="9">
@@ -28410,7 +28410,7 @@
         <v>-29</v>
       </c>
       <c r="K105" s="15">
-        <f>SUM(I105:J105)</f>
+        <f t="shared" si="1"/>
         <v>-23</v>
       </c>
       <c r="L105" s="4">
@@ -28505,7 +28505,7 @@
         <v>15</v>
       </c>
       <c r="K106" s="15">
-        <f>SUM(I106:J106)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L106" s="4">
@@ -28600,7 +28600,7 @@
         <v>21</v>
       </c>
       <c r="K107" s="15">
-        <f>SUM(I107:J107)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L107" s="4">
@@ -28695,7 +28695,7 @@
         <v>10</v>
       </c>
       <c r="K108" s="15">
-        <f>SUM(I108:J108)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="L108" s="4">
@@ -28790,7 +28790,7 @@
         <v>0</v>
       </c>
       <c r="K109" s="15">
-        <f>SUM(I109:J109)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L109" s="4">
@@ -28885,7 +28885,7 @@
         <v>0</v>
       </c>
       <c r="K110" s="15">
-        <f>SUM(I110:J110)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L110" s="4">
@@ -28980,7 +28980,7 @@
         <v>-9</v>
       </c>
       <c r="K111" s="15">
-        <f>SUM(I111:J111)</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="L111" s="4">
@@ -29075,7 +29075,7 @@
         <v>-10</v>
       </c>
       <c r="K112" s="15">
-        <f>SUM(I112:J112)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L112" s="4">
@@ -29170,7 +29170,7 @@
         <v>5</v>
       </c>
       <c r="K113" s="15">
-        <f>SUM(I113:J113)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L113" s="4">
@@ -29265,7 +29265,7 @@
         <v>18</v>
       </c>
       <c r="K114" s="15">
-        <f>SUM(I114:J114)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="L114" s="7">
@@ -29362,7 +29362,7 @@
         <v>9</v>
       </c>
       <c r="K115" s="15">
-        <f>SUM(I115:J115)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="L115" s="7">
@@ -29459,7 +29459,7 @@
         <v>-8</v>
       </c>
       <c r="K116" s="15">
-        <f>SUM(I116:J116)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L116" s="7">
@@ -29556,7 +29556,7 @@
         <v>13</v>
       </c>
       <c r="K117" s="15">
-        <f>SUM(I117:J117)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="L117" s="4">
@@ -29651,7 +29651,7 @@
         <v>5</v>
       </c>
       <c r="K118" s="15">
-        <f>SUM(I118:J118)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="L118" s="7">
@@ -29748,7 +29748,7 @@
         <v>14</v>
       </c>
       <c r="K119" s="15">
-        <f>SUM(I119:J119)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="L119" s="7">
@@ -29845,7 +29845,7 @@
         <v>0</v>
       </c>
       <c r="K120" s="15">
-        <f>SUM(I120:J120)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="L120" s="7">
@@ -29942,7 +29942,7 @@
         <v>11</v>
       </c>
       <c r="K121" s="15">
-        <f>SUM(I121:J121)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="L121" s="7">
@@ -30039,7 +30039,7 @@
         <v>-7</v>
       </c>
       <c r="K122" s="15">
-        <f>SUM(I122:J122)</f>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="L122" s="4">
@@ -30134,7 +30134,7 @@
         <v>-19</v>
       </c>
       <c r="K123" s="15">
-        <f>SUM(I123:J123)</f>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="L123" s="4">
@@ -30229,7 +30229,7 @@
         <v>-9</v>
       </c>
       <c r="K124" s="15">
-        <f>SUM(I124:J124)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L124" s="4">
@@ -30324,7 +30324,7 @@
         <v>-5</v>
       </c>
       <c r="K125" s="15">
-        <f>SUM(I125:J125)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="L125" s="4">
@@ -30419,7 +30419,7 @@
         <v>-25</v>
       </c>
       <c r="K126" s="15">
-        <f>SUM(I126:J126)</f>
+        <f t="shared" si="1"/>
         <v>-38</v>
       </c>
       <c r="L126" s="4">
@@ -30514,7 +30514,7 @@
         <v>19</v>
       </c>
       <c r="K127" s="15">
-        <f>SUM(I127:J127)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="L127" s="4">
@@ -30609,7 +30609,7 @@
         <v>23</v>
       </c>
       <c r="K128" s="15">
-        <f>SUM(I128:J128)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L128" s="4">
@@ -30704,7 +30704,7 @@
         <v>10</v>
       </c>
       <c r="K129" s="15">
-        <f>SUM(I129:J129)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="L129" s="9">
@@ -30799,7 +30799,7 @@
         <v>-15</v>
       </c>
       <c r="K130" s="15">
-        <f>SUM(I130:J130)</f>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="L130" s="4">
@@ -30894,7 +30894,7 @@
         <v>4</v>
       </c>
       <c r="K131" s="15">
-        <f>SUM(I131:J131)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="L131" s="4">
@@ -30989,7 +30989,7 @@
         <v>7</v>
       </c>
       <c r="K132" s="15">
-        <f>SUM(I132:J132)</f>
+        <f t="shared" ref="K132:K195" si="2">SUM(I132:J132)</f>
         <v>23</v>
       </c>
       <c r="L132" s="4">
@@ -31084,7 +31084,7 @@
         <v>15</v>
       </c>
       <c r="K133" s="15">
-        <f>SUM(I133:J133)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L133" s="4">
@@ -31179,7 +31179,7 @@
         <v>0</v>
       </c>
       <c r="K134" s="15">
-        <f>SUM(I134:J134)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="L134" s="4">
@@ -31274,7 +31274,7 @@
         <v>9</v>
       </c>
       <c r="K135" s="15">
-        <f>SUM(I135:J135)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="L135" s="4">
@@ -31369,7 +31369,7 @@
         <v>-8</v>
       </c>
       <c r="K136" s="15">
-        <f>SUM(I136:J136)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="L136" s="4">
@@ -31464,7 +31464,7 @@
         <v>-12</v>
       </c>
       <c r="K137" s="15">
-        <f>SUM(I137:J137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L137" s="4">
@@ -31559,7 +31559,7 @@
         <v>23</v>
       </c>
       <c r="K138" s="15">
-        <f>SUM(I138:J138)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L138" s="4">
@@ -31654,7 +31654,7 @@
         <v>28</v>
       </c>
       <c r="K139" s="15">
-        <f>SUM(I139:J139)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="L139" s="4">
@@ -31749,7 +31749,7 @@
         <v>9</v>
       </c>
       <c r="K140" s="15">
-        <f>SUM(I140:J140)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="L140" s="4">
@@ -31844,7 +31844,7 @@
         <v>-8</v>
       </c>
       <c r="K141" s="15">
-        <f>SUM(I141:J141)</f>
+        <f t="shared" si="2"/>
         <v>-17</v>
       </c>
       <c r="L141" s="4">
@@ -31939,7 +31939,7 @@
         <v>17</v>
       </c>
       <c r="K142" s="15">
-        <f>SUM(I142:J142)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="L142" s="9">
@@ -32034,7 +32034,7 @@
         <v>2</v>
       </c>
       <c r="K143" s="15">
-        <f>SUM(I143:J143)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="L143" s="4">
@@ -32129,7 +32129,7 @@
         <v>10</v>
       </c>
       <c r="K144" s="15">
-        <f>SUM(I144:J144)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="L144" s="4">
@@ -32226,7 +32226,7 @@
         <v>0</v>
       </c>
       <c r="K145" s="15">
-        <f>SUM(I145:J145)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="L145" s="9">
@@ -32323,7 +32323,7 @@
         <v>10</v>
       </c>
       <c r="K146" s="15">
-        <f>SUM(I146:J146)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="L146" s="9">
@@ -32418,7 +32418,7 @@
         <v>7</v>
       </c>
       <c r="K147" s="15">
-        <f>SUM(I147:J147)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="L147" s="4">
@@ -32513,7 +32513,7 @@
         <v>-9</v>
       </c>
       <c r="K148" s="15">
-        <f>SUM(I148:J148)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="L148" s="4">
@@ -32608,7 +32608,7 @@
         <v>0</v>
       </c>
       <c r="K149" s="15">
-        <f>SUM(I149:J149)</f>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="L149" s="4">
@@ -32703,7 +32703,7 @@
         <v>-17</v>
       </c>
       <c r="K150" s="15">
-        <f>SUM(I150:J150)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L150" s="4">
@@ -32798,7 +32798,7 @@
         <v>-23</v>
       </c>
       <c r="K151" s="15">
-        <f>SUM(I151:J151)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="L151" s="4">
@@ -32893,7 +32893,7 @@
         <v>11</v>
       </c>
       <c r="K152" s="15">
-        <f>SUM(I152:J152)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="L152" s="9">
@@ -32990,7 +32990,7 @@
         <v>-9</v>
       </c>
       <c r="K153" s="15">
-        <f>SUM(I153:J153)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L153" s="4">
@@ -33085,7 +33085,7 @@
         <v>17</v>
       </c>
       <c r="K154" s="15">
-        <f>SUM(I154:J154)</f>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="L154" s="4">
@@ -33180,7 +33180,7 @@
         <v>-10</v>
       </c>
       <c r="K155" s="15">
-        <f>SUM(I155:J155)</f>
+        <f t="shared" si="2"/>
         <v>-7</v>
       </c>
       <c r="L155" s="4">
@@ -33275,7 +33275,7 @@
         <v>10</v>
       </c>
       <c r="K156" s="15">
-        <f>SUM(I156:J156)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="L156" s="4">
@@ -33370,7 +33370,7 @@
         <v>2</v>
       </c>
       <c r="K157" s="15">
-        <f>SUM(I157:J157)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L157" s="4">
@@ -33467,7 +33467,7 @@
         <v>-9</v>
       </c>
       <c r="K158" s="15">
-        <f>SUM(I158:J158)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L158" s="9">
@@ -33562,7 +33562,7 @@
         <v>0</v>
       </c>
       <c r="K159" s="15">
-        <f>SUM(I159:J159)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L159" s="4">
@@ -33657,7 +33657,7 @@
         <v>5</v>
       </c>
       <c r="K160" s="15">
-        <f>SUM(I160:J160)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="L160" s="4">
@@ -33752,7 +33752,7 @@
         <v>-11</v>
       </c>
       <c r="K161" s="15">
-        <f>SUM(I161:J161)</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="L161" s="4">
@@ -33849,7 +33849,7 @@
         <v>-13</v>
       </c>
       <c r="K162" s="15">
-        <f>SUM(I162:J162)</f>
+        <f t="shared" si="2"/>
         <v>-7</v>
       </c>
       <c r="L162" s="4">
@@ -33944,7 +33944,7 @@
         <v>0</v>
       </c>
       <c r="K163" s="15">
-        <f>SUM(I163:J163)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L163" s="4">
@@ -34039,7 +34039,7 @@
         <v>19</v>
       </c>
       <c r="K164" s="15">
-        <f>SUM(I164:J164)</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="L164" s="4">
@@ -34134,7 +34134,7 @@
         <v>10</v>
       </c>
       <c r="K165" s="15">
-        <f>SUM(I165:J165)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="L165" s="4">
@@ -34229,7 +34229,7 @@
         <v>9</v>
       </c>
       <c r="K166" s="15">
-        <f>SUM(I166:J166)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="L166" s="4">
@@ -34324,7 +34324,7 @@
         <v>15</v>
       </c>
       <c r="K167" s="15">
-        <f>SUM(I167:J167)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="L167" s="4">
@@ -34419,7 +34419,7 @@
         <v>-24</v>
       </c>
       <c r="K168" s="15">
-        <f>SUM(I168:J168)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="L168" s="4">
@@ -34514,7 +34514,7 @@
         <v>18</v>
       </c>
       <c r="K169" s="15">
-        <f>SUM(I169:J169)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L169" s="4">
@@ -34609,7 +34609,7 @@
         <v>13</v>
       </c>
       <c r="K170" s="15">
-        <f>SUM(I170:J170)</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="L170" s="4">
@@ -34704,7 +34704,7 @@
         <v>4</v>
       </c>
       <c r="K171" s="15">
-        <f>SUM(I171:J171)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="L171" s="4">
@@ -34799,7 +34799,7 @@
         <v>-5</v>
       </c>
       <c r="K172" s="15">
-        <f>SUM(I172:J172)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L172" s="4">
@@ -34896,7 +34896,7 @@
         <v>2</v>
       </c>
       <c r="K173" s="15">
-        <f>SUM(I173:J173)</f>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="L173" s="4">
@@ -34991,7 +34991,7 @@
         <v>12</v>
       </c>
       <c r="K174" s="15">
-        <f>SUM(I174:J174)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L174" s="4">
@@ -35086,7 +35086,7 @@
         <v>15</v>
       </c>
       <c r="K175" s="15">
-        <f>SUM(I175:J175)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L175" s="4">
@@ -35181,7 +35181,7 @@
         <v>18</v>
       </c>
       <c r="K176" s="15">
-        <f>SUM(I176:J176)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L176" s="4">
@@ -35276,7 +35276,7 @@
         <v>-6</v>
       </c>
       <c r="K177" s="15">
-        <f>SUM(I177:J177)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L177" s="4">
@@ -35371,7 +35371,7 @@
         <v>-10</v>
       </c>
       <c r="K178" s="15">
-        <f>SUM(I178:J178)</f>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="L178" s="4">
@@ -35466,7 +35466,7 @@
         <v>11</v>
       </c>
       <c r="K179" s="15">
-        <f>SUM(I179:J179)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="L179" s="9">
@@ -35561,7 +35561,7 @@
         <v>26</v>
       </c>
       <c r="K180" s="15">
-        <f>SUM(I180:J180)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="L180" s="4">
@@ -35656,7 +35656,7 @@
         <v>28</v>
       </c>
       <c r="K181" s="15">
-        <f>SUM(I181:J181)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="L181" s="9">
@@ -35753,7 +35753,7 @@
         <v>15</v>
       </c>
       <c r="K182" s="15">
-        <f>SUM(I182:J182)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="L182" s="4">
@@ -35848,7 +35848,7 @@
         <v>-6</v>
       </c>
       <c r="K183" s="15">
-        <f>SUM(I183:J183)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="L183" s="4">
@@ -35943,7 +35943,7 @@
         <v>0</v>
       </c>
       <c r="K184" s="15">
-        <f>SUM(I184:J184)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="L184" s="4">
@@ -36038,7 +36038,7 @@
         <v>30</v>
       </c>
       <c r="K185" s="15">
-        <f>SUM(I185:J185)</f>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="L185" s="4">
@@ -36133,7 +36133,7 @@
         <v>4</v>
       </c>
       <c r="K186" s="15">
-        <f>SUM(I186:J186)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="L186" s="4">
@@ -36228,7 +36228,7 @@
         <v>21</v>
       </c>
       <c r="K187" s="15">
-        <f>SUM(I187:J187)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="L187" s="4">
@@ -36323,7 +36323,7 @@
         <v>-18</v>
       </c>
       <c r="K188" s="15">
-        <f>SUM(I188:J188)</f>
+        <f t="shared" si="2"/>
         <v>-30</v>
       </c>
       <c r="L188" s="4">
@@ -36418,7 +36418,7 @@
         <v>21</v>
       </c>
       <c r="K189" s="15">
-        <f>SUM(I189:J189)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="L189" s="4">
@@ -36515,7 +36515,7 @@
         <v>18</v>
       </c>
       <c r="K190" s="15">
-        <f>SUM(I190:J190)</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="L190" s="4">
@@ -36612,7 +36612,7 @@
         <v>20</v>
       </c>
       <c r="K191" s="15">
-        <f>SUM(I191:J191)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="L191" s="4">
@@ -36707,7 +36707,7 @@
         <v>-8</v>
       </c>
       <c r="K192" s="15">
-        <f>SUM(I192:J192)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L192" s="4">
@@ -36804,7 +36804,7 @@
         <v>21</v>
       </c>
       <c r="K193" s="15">
-        <f>SUM(I193:J193)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="L193" s="4">
@@ -36899,7 +36899,7 @@
         <v>-10</v>
       </c>
       <c r="K194" s="15">
-        <f>SUM(I194:J194)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="L194" s="4">
@@ -36994,7 +36994,7 @@
         <v>-6</v>
       </c>
       <c r="K195" s="15">
-        <f>SUM(I195:J195)</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="L195" s="4">
@@ -37089,7 +37089,7 @@
         <v>-9</v>
       </c>
       <c r="K196" s="15">
-        <f>SUM(I196:J196)</f>
+        <f t="shared" ref="K196:K259" si="3">SUM(I196:J196)</f>
         <v>-9</v>
       </c>
       <c r="L196" s="4">
@@ -37184,7 +37184,7 @@
         <v>9</v>
       </c>
       <c r="K197" s="15">
-        <f>SUM(I197:J197)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L197" s="4">
@@ -37279,7 +37279,7 @@
         <v>27</v>
       </c>
       <c r="K198" s="15">
-        <f>SUM(I198:J198)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L198" s="4">
@@ -37376,7 +37376,7 @@
         <v>-8</v>
       </c>
       <c r="K199" s="15">
-        <f>SUM(I199:J199)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L199" s="4">
@@ -37471,7 +37471,7 @@
         <v>-20</v>
       </c>
       <c r="K200" s="15">
-        <f>SUM(I200:J200)</f>
+        <f t="shared" si="3"/>
         <v>-27</v>
       </c>
       <c r="L200" s="4">
@@ -37566,7 +37566,7 @@
         <v>14</v>
       </c>
       <c r="K201" s="15">
-        <f>SUM(I201:J201)</f>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
       <c r="L201" s="4">
@@ -37661,7 +37661,7 @@
         <v>19</v>
       </c>
       <c r="K202" s="15">
-        <f>SUM(I202:J202)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L202" s="4">
@@ -37756,7 +37756,7 @@
         <v>-8</v>
       </c>
       <c r="K203" s="15">
-        <f>SUM(I203:J203)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="L203" s="9">
@@ -37851,7 +37851,7 @@
         <v>20</v>
       </c>
       <c r="K204" s="15">
-        <f>SUM(I204:J204)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L204" s="4">
@@ -37946,7 +37946,7 @@
         <v>-5</v>
       </c>
       <c r="K205" s="15">
-        <f>SUM(I205:J205)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L205" s="4">
@@ -38041,7 +38041,7 @@
         <v>19</v>
       </c>
       <c r="K206" s="15">
-        <f>SUM(I206:J206)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="L206" s="4">
@@ -38136,7 +38136,7 @@
         <v>-9</v>
       </c>
       <c r="K207" s="15">
-        <f>SUM(I207:J207)</f>
+        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="L207" s="4">
@@ -38231,7 +38231,7 @@
         <v>16</v>
       </c>
       <c r="K208" s="15">
-        <f>SUM(I208:J208)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L208" s="4">
@@ -38326,7 +38326,7 @@
         <v>9</v>
       </c>
       <c r="K209" s="15">
-        <f>SUM(I209:J209)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L209" s="4">
@@ -38421,7 +38421,7 @@
         <v>-5</v>
       </c>
       <c r="K210" s="15">
-        <f>SUM(I210:J210)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="L210" s="4">
@@ -38516,7 +38516,7 @@
         <v>9</v>
       </c>
       <c r="K211" s="15">
-        <f>SUM(I211:J211)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L211" s="4">
@@ -38611,7 +38611,7 @@
         <v>-13</v>
       </c>
       <c r="K212" s="15">
-        <f>SUM(I212:J212)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L212" s="4">
@@ -38706,7 +38706,7 @@
         <v>-5</v>
       </c>
       <c r="K213" s="15">
-        <f>SUM(I213:J213)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L213" s="4">
@@ -38801,7 +38801,7 @@
         <v>16</v>
       </c>
       <c r="K214" s="15">
-        <f>SUM(I214:J214)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="L214" s="4">
@@ -38896,7 +38896,7 @@
         <v>5</v>
       </c>
       <c r="K215" s="15">
-        <f>SUM(I215:J215)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="L215" s="4">
@@ -38993,7 +38993,7 @@
         <v>-14</v>
       </c>
       <c r="K216" s="15">
-        <f>SUM(I216:J216)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L216" s="4">
@@ -39088,7 +39088,7 @@
         <v>14</v>
       </c>
       <c r="K217" s="15">
-        <f>SUM(I217:J217)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="L217" s="4">
@@ -39183,7 +39183,7 @@
         <v>-5</v>
       </c>
       <c r="K218" s="15">
-        <f>SUM(I218:J218)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L218" s="4">
@@ -39278,7 +39278,7 @@
         <v>0</v>
       </c>
       <c r="K219" s="15">
-        <f>SUM(I219:J219)</f>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="L219" s="4">
@@ -39375,7 +39375,7 @@
         <v>25</v>
       </c>
       <c r="K220" s="15">
-        <f>SUM(I220:J220)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="L220" s="4">
@@ -39470,7 +39470,7 @@
         <v>-8</v>
       </c>
       <c r="K221" s="15">
-        <f>SUM(I221:J221)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L221" s="4">
@@ -39565,7 +39565,7 @@
         <v>21</v>
       </c>
       <c r="K222" s="15">
-        <f>SUM(I222:J222)</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="L222" s="4">
@@ -39660,7 +39660,7 @@
         <v>10</v>
       </c>
       <c r="K223" s="15">
-        <f>SUM(I223:J223)</f>
+        <f t="shared" si="3"/>
         <v>-20</v>
       </c>
       <c r="L223" s="4">
@@ -39755,7 +39755,7 @@
         <v>9</v>
       </c>
       <c r="K224" s="15">
-        <f>SUM(I224:J224)</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="L224" s="4">
@@ -39850,7 +39850,7 @@
         <v>13</v>
       </c>
       <c r="K225" s="15">
-        <f>SUM(I225:J225)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L225" s="4">
@@ -39945,7 +39945,7 @@
         <v>-30</v>
       </c>
       <c r="K226" s="15">
-        <f>SUM(I226:J226)</f>
+        <f t="shared" si="3"/>
         <v>-26</v>
       </c>
       <c r="L226" s="4">
@@ -40040,7 +40040,7 @@
         <v>-13</v>
       </c>
       <c r="K227" s="15">
-        <f>SUM(I227:J227)</f>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="L227" s="4">
@@ -40135,7 +40135,7 @@
         <v>19</v>
       </c>
       <c r="K228" s="15">
-        <f>SUM(I228:J228)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L228" s="4">
@@ -40230,7 +40230,7 @@
         <v>-13</v>
       </c>
       <c r="K229" s="15">
-        <f>SUM(I229:J229)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L229" s="4">
@@ -40325,7 +40325,7 @@
         <v>10</v>
       </c>
       <c r="K230" s="15">
-        <f>SUM(I230:J230)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L230" s="4">
@@ -40420,7 +40420,7 @@
         <v>9</v>
       </c>
       <c r="K231" s="15">
-        <f>SUM(I231:J231)</f>
+        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="L231" s="4">
@@ -40515,7 +40515,7 @@
         <v>18</v>
       </c>
       <c r="K232" s="15">
-        <f>SUM(I232:J232)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="L232" s="4">
@@ -40612,7 +40612,7 @@
         <v>16</v>
       </c>
       <c r="K233" s="15">
-        <f>SUM(I233:J233)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="L233" s="4">
@@ -40707,7 +40707,7 @@
         <v>14</v>
       </c>
       <c r="K234" s="15">
-        <f>SUM(I234:J234)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="L234" s="4">
@@ -40802,7 +40802,7 @@
         <v>13</v>
       </c>
       <c r="K235" s="15">
-        <f>SUM(I235:J235)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="L235" s="4">
@@ -40897,7 +40897,7 @@
         <v>3</v>
       </c>
       <c r="K236" s="15">
-        <f>SUM(I236:J236)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="L236" s="4">
@@ -40992,7 +40992,7 @@
         <v>18</v>
       </c>
       <c r="K237" s="15">
-        <f>SUM(I237:J237)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L237" s="4">
@@ -41087,7 +41087,7 @@
         <v>4</v>
       </c>
       <c r="K238" s="15">
-        <f>SUM(I238:J238)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L238" s="9">
@@ -41182,7 +41182,7 @@
         <v>0</v>
       </c>
       <c r="K239" s="15">
-        <f>SUM(I239:J239)</f>
+        <f t="shared" si="3"/>
         <v>-7</v>
       </c>
       <c r="L239" s="4">
@@ -41277,7 +41277,7 @@
         <v>7</v>
       </c>
       <c r="K240" s="15">
-        <f>SUM(I240:J240)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="L240" s="4">
@@ -41372,7 +41372,7 @@
         <v>-10</v>
       </c>
       <c r="K241" s="15">
-        <f>SUM(I241:J241)</f>
+        <f t="shared" si="3"/>
         <v>-13</v>
       </c>
       <c r="L241" s="9">
@@ -41467,7 +41467,7 @@
         <v>-7</v>
       </c>
       <c r="K242" s="15">
-        <f>SUM(I242:J242)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L242" s="4">
@@ -41562,7 +41562,7 @@
         <v>9</v>
       </c>
       <c r="K243" s="15">
-        <f>SUM(I243:J243)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L243" s="4">
@@ -41657,7 +41657,7 @@
         <v>6</v>
       </c>
       <c r="K244" s="15">
-        <f>SUM(I244:J244)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L244" s="4">
@@ -41752,7 +41752,7 @@
         <v>0</v>
       </c>
       <c r="K245" s="15">
-        <f>SUM(I245:J245)</f>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
       <c r="L245" s="4">
@@ -41847,7 +41847,7 @@
         <v>15</v>
       </c>
       <c r="K246" s="15">
-        <f>SUM(I246:J246)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="L246" s="4">
@@ -41942,7 +41942,7 @@
         <v>10</v>
       </c>
       <c r="K247" s="15">
-        <f>SUM(I247:J247)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L247" s="4">
@@ -42037,7 +42037,7 @@
         <v>5</v>
       </c>
       <c r="K248" s="15">
-        <f>SUM(I248:J248)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L248" s="4">
@@ -42132,7 +42132,7 @@
         <v>7</v>
       </c>
       <c r="K249" s="15">
-        <f>SUM(I249:J249)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="L249" s="4">
@@ -42227,7 +42227,7 @@
         <v>6</v>
       </c>
       <c r="K250" s="15">
-        <f>SUM(I250:J250)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L250" s="4">
@@ -42322,7 +42322,7 @@
         <v>6</v>
       </c>
       <c r="K251" s="15">
-        <f>SUM(I251:J251)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L251" s="4">
@@ -42417,7 +42417,7 @@
         <v>18</v>
       </c>
       <c r="K252" s="15">
-        <f>SUM(I252:J252)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="L252" s="9">
@@ -42512,7 +42512,7 @@
         <v>-9</v>
       </c>
       <c r="K253" s="15">
-        <f>SUM(I253:J253)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L253" s="4">
@@ -42607,7 +42607,7 @@
         <v>7</v>
       </c>
       <c r="K254" s="15">
-        <f>SUM(I254:J254)</f>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="L254" s="4">
@@ -42702,7 +42702,7 @@
         <v>-9</v>
       </c>
       <c r="K255" s="15">
-        <f>SUM(I255:J255)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L255" s="4">
@@ -42799,7 +42799,7 @@
         <v>-20</v>
       </c>
       <c r="K256" s="15">
-        <f>SUM(I256:J256)</f>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
       <c r="L256" s="4">
@@ -42894,7 +42894,7 @@
         <v>10</v>
       </c>
       <c r="K257" s="15">
-        <f>SUM(I257:J257)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="L257" s="4">
@@ -42989,7 +42989,7 @@
         <v>20</v>
       </c>
       <c r="K258" s="15">
-        <f>SUM(I258:J258)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L258" s="4">
@@ -43084,7 +43084,7 @@
         <v>16</v>
       </c>
       <c r="K259" s="15">
-        <f>SUM(I259:J259)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L259" s="4">
@@ -43179,7 +43179,7 @@
         <v>9</v>
       </c>
       <c r="K260" s="15">
-        <f t="shared" ref="K260:K311" si="0">SUM(I260:J260)</f>
+        <f t="shared" ref="K260:K311" si="4">SUM(I260:J260)</f>
         <v>7</v>
       </c>
       <c r="L260" s="4">
@@ -43274,7 +43274,7 @@
         <v>9</v>
       </c>
       <c r="K261" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="L261" s="4">
@@ -43369,7 +43369,7 @@
         <v>-11</v>
       </c>
       <c r="K262" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L262" s="4">
@@ -43464,7 +43464,7 @@
         <v>-7</v>
       </c>
       <c r="K263" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L263" s="4">
@@ -43561,7 +43561,7 @@
         <v>30</v>
       </c>
       <c r="K264" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="L264" s="4">
@@ -43656,7 +43656,7 @@
         <v>14</v>
       </c>
       <c r="K265" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="L265" s="4">
@@ -43751,7 +43751,7 @@
         <v>-25</v>
       </c>
       <c r="K266" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L266" s="4">
@@ -43846,7 +43846,7 @@
         <v>16</v>
       </c>
       <c r="K267" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="L267" s="4">
@@ -43941,7 +43941,7 @@
         <v>-10</v>
       </c>
       <c r="K268" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L268" s="4">
@@ -44036,7 +44036,7 @@
         <v>18</v>
       </c>
       <c r="K269" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L269" s="4">
@@ -44131,7 +44131,7 @@
         <v>14</v>
       </c>
       <c r="K270" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="L270" s="4">
@@ -44226,7 +44226,7 @@
         <v>-4</v>
       </c>
       <c r="K271" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L271" s="4">
@@ -44321,7 +44321,7 @@
         <v>-19</v>
       </c>
       <c r="K272" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-11</v>
       </c>
       <c r="L272" s="4">
@@ -44416,7 +44416,7 @@
         <v>13</v>
       </c>
       <c r="K273" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L273" s="4">
@@ -44511,7 +44511,7 @@
         <v>3</v>
       </c>
       <c r="K274" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L274" s="4">
@@ -44606,7 +44606,7 @@
         <v>2</v>
       </c>
       <c r="K275" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L275" s="4">
@@ -44701,7 +44701,7 @@
         <v>22</v>
       </c>
       <c r="K276" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L276" s="4">
@@ -44796,7 +44796,7 @@
         <v>-4</v>
       </c>
       <c r="K277" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L277" s="4">
@@ -44891,7 +44891,7 @@
         <v>-17</v>
       </c>
       <c r="K278" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-7</v>
       </c>
       <c r="L278" s="4">
@@ -44986,7 +44986,7 @@
         <v>12</v>
       </c>
       <c r="K279" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="L279" s="4">
@@ -45081,7 +45081,7 @@
         <v>14</v>
       </c>
       <c r="K280" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L280" s="4">
@@ -45176,7 +45176,7 @@
         <v>16</v>
       </c>
       <c r="K281" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-10</v>
       </c>
       <c r="L281" s="4">
@@ -45271,7 +45271,7 @@
         <v>23</v>
       </c>
       <c r="K282" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="L282" s="4">
@@ -45366,7 +45366,7 @@
         <v>-8</v>
       </c>
       <c r="K283" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="L283" s="4">
@@ -45461,7 +45461,7 @@
         <v>-10</v>
       </c>
       <c r="K284" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="L284" s="4">
@@ -45556,7 +45556,7 @@
         <v>9</v>
       </c>
       <c r="K285" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="L285" s="4">
@@ -45651,7 +45651,7 @@
         <v>15</v>
       </c>
       <c r="K286" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="L286" s="4">
@@ -45748,7 +45748,7 @@
         <v>0</v>
       </c>
       <c r="K287" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L287" s="4">
@@ -45843,7 +45843,7 @@
         <v>10</v>
       </c>
       <c r="K288" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="L288" s="4">
@@ -45938,7 +45938,7 @@
         <v>27</v>
       </c>
       <c r="K289" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="L289" s="4">
@@ -46033,7 +46033,7 @@
         <v>-10</v>
       </c>
       <c r="K290" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L290" s="4">
@@ -46128,7 +46128,7 @@
         <v>13</v>
       </c>
       <c r="K291" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="L291" s="4">
@@ -46223,7 +46223,7 @@
         <v>9</v>
       </c>
       <c r="K292" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="L292" s="4">
@@ -46318,7 +46318,7 @@
         <v>15</v>
       </c>
       <c r="K293" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L293" s="4">
@@ -46413,7 +46413,7 @@
         <v>-8</v>
       </c>
       <c r="K294" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-14</v>
       </c>
       <c r="L294" s="4">
@@ -46508,7 +46508,7 @@
         <v>13</v>
       </c>
       <c r="K295" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="L295" s="4">
@@ -46603,7 +46603,7 @@
         <v>6</v>
       </c>
       <c r="K296" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L296" s="4">
@@ -46698,7 +46698,7 @@
         <v>-9</v>
       </c>
       <c r="K297" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-19</v>
       </c>
       <c r="L297" s="4">
@@ -46793,7 +46793,7 @@
         <v>0</v>
       </c>
       <c r="K298" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L298" s="4">
@@ -46888,7 +46888,7 @@
         <v>24</v>
       </c>
       <c r="K299" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="L299" s="9">
@@ -46983,7 +46983,7 @@
         <v>16</v>
       </c>
       <c r="K300" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="L300" s="9">
@@ -47078,7 +47078,7 @@
         <v>23</v>
       </c>
       <c r="K301" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="L301" s="4">
@@ -47173,7 +47173,7 @@
         <v>10</v>
       </c>
       <c r="K302" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L302" s="4">
@@ -47268,7 +47268,7 @@
         <v>0</v>
       </c>
       <c r="K303" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-10</v>
       </c>
       <c r="L303" s="11">
@@ -47363,7 +47363,7 @@
         <v>-15</v>
       </c>
       <c r="K304" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-15</v>
       </c>
       <c r="L304" s="10">
@@ -47458,7 +47458,7 @@
         <v>10</v>
       </c>
       <c r="K305" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="L305" s="10">
@@ -47553,7 +47553,7 @@
         <v>-5</v>
       </c>
       <c r="K306" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-15</v>
       </c>
       <c r="L306" s="10">
@@ -47648,7 +47648,7 @@
         <v>14</v>
       </c>
       <c r="K307" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="L307" s="11">
@@ -47743,7 +47743,7 @@
         <v>6</v>
       </c>
       <c r="K308" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="L308" s="11">
@@ -47838,7 +47838,7 @@
         <v>-5</v>
       </c>
       <c r="K309" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L309" s="11">
@@ -47933,7 +47933,7 @@
         <v>-1</v>
       </c>
       <c r="K310" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L310" s="11">
@@ -48028,7 +48028,7 @@
         <v>7</v>
       </c>
       <c r="K311" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="L311" s="11">
@@ -48106,7 +48106,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J311">
-    <cfRule type="cellIs" dxfId="5" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -48200,7 +48200,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -48259,31 +48259,31 @@
         <v>976</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="T1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="U1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>1365</v>
       </c>
       <c r="V1" s="17" t="s">
         <v>327</v>
@@ -48357,31 +48357,31 @@
         <v>969</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>300</v>
@@ -48455,34 +48455,34 @@
         <v>977</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="T3" s="6" t="s">
+        <v>1366</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>1367</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>1368</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>1369</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>311</v>
@@ -48803,13 +48803,13 @@
         <v>51018001</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>1361</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>1362</v>
       </c>
       <c r="E7" s="11">
         <v>1</v>
@@ -48907,7 +48907,7 @@
         <v>871</v>
       </c>
       <c r="E8" s="38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="38">
         <v>8</v>
@@ -48916,7 +48916,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8" s="38">
         <v>0</v>
@@ -48953,18 +48953,16 @@
         <v>0</v>
       </c>
       <c r="T8" s="11">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="U8" s="11">
-        <v>10</v>
-      </c>
-      <c r="V8" s="38" t="s">
-        <v>211</v>
+        <v>15</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>1387</v>
       </c>
       <c r="W8" s="38"/>
-      <c r="X8" s="11" t="s">
-        <v>1358</v>
-      </c>
+      <c r="X8" s="11"/>
       <c r="Y8" s="38" t="s">
         <v>1045</v>
       </c>
@@ -48990,10 +48988,10 @@
     </row>
     <row r="9" spans="1:32" ht="14.25">
       <c r="A9" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>1060</v>
@@ -49098,7 +49096,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J9">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -49116,13 +49114,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I7">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -49140,7 +49138,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -49158,7 +49156,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
close #15 kingtower fight while one arrow tower die
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9682,11 +9682,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1758014640"/>
-        <c:axId val="-1758028784"/>
+        <c:axId val="-304057216"/>
+        <c:axId val="-304048512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1758014640"/>
+        <c:axId val="-304057216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9729,7 +9729,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1758028784"/>
+        <c:crossAx val="-304048512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9737,7 +9737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1758028784"/>
+        <c:axId val="-304048512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9788,7 +9788,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1758014640"/>
+        <c:crossAx val="-304057216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -74339,7 +74339,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -75555,7 +75555,7 @@
         <v>1409</v>
       </c>
       <c r="E8" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8" s="11">
         <v>15</v>
@@ -75571,10 +75571,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
-        <v>-35</v>
+        <v>25</v>
       </c>
       <c r="K8" s="4">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -75602,7 +75602,7 @@
       </c>
       <c r="T8" s="15">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>425</v>
       </c>
       <c r="U8" s="11">
         <v>40</v>
@@ -75714,7 +75714,7 @@
         <v>1410</v>
       </c>
       <c r="E9" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="11">
         <v>2</v>
@@ -75730,10 +75730,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="4">
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="K9" s="4">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -75761,7 +75761,7 @@
       </c>
       <c r="T9" s="15">
         <f t="shared" ref="T9" si="5">SUM(J9:K9)+SUM(M9:S9)*5+4.4*SUM(AP9:AX9)+2.5*SUM(AJ9:AN9)+AI9/100+L9</f>
-        <v>150</v>
+        <v>280</v>
       </c>
       <c r="U9" s="11">
         <v>40</v>

</xml_diff>

<commit_message>
#17 refind checkspecialskill & data for goblin house
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="1429">
   <si>
     <t>arrow</t>
   </si>
@@ -5525,6 +5525,21 @@
   </si>
   <si>
     <t>LifeTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>哥布林巢穴</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goblin Nest</t>
+  </si>
+  <si>
+    <t>召唤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55000300;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6380,7 +6395,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6552,6 +6567,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6597,142 +6615,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="138">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="142">
     <dxf>
       <font>
         <b/>
@@ -6760,33 +6643,6 @@
         <i val="0"/>
         <color rgb="FF00B050"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -7637,6 +7493,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -8207,6 +8090,114 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9018,6 +9009,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -9584,6 +9602,34 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -9881,11 +9927,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="224312400"/>
-        <c:axId val="224312960"/>
+        <c:axId val="278082608"/>
+        <c:axId val="278083168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="224312400"/>
+        <c:axId val="278082608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9928,7 +9974,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224312960"/>
+        <c:crossAx val="278083168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9936,7 +9982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224312960"/>
+        <c:axId val="278083168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9987,7 +10033,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224312400"/>
+        <c:crossAx val="278082608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10694,135 +10740,135 @@
         </row>
         <row r="4">
           <cell r="A4">
-            <v>54999738</v>
+            <v>55000001</v>
           </cell>
           <cell r="Q4">
-            <v>2200</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5">
-            <v>55000001</v>
+            <v>55000002</v>
           </cell>
           <cell r="Q5">
-            <v>200</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>55000002</v>
+            <v>55000003</v>
           </cell>
           <cell r="Q6">
-            <v>80</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>55000003</v>
+            <v>55000004</v>
           </cell>
           <cell r="Q7">
-            <v>120</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8">
-            <v>55000004</v>
+            <v>55000005</v>
           </cell>
           <cell r="Q8">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9">
-            <v>55000005</v>
+            <v>55000006</v>
           </cell>
           <cell r="Q9">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>55000006</v>
+            <v>55000007</v>
           </cell>
           <cell r="Q10">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>55000007</v>
+            <v>55000008</v>
           </cell>
           <cell r="Q11">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>55000008</v>
+            <v>55000009</v>
           </cell>
           <cell r="Q12">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>55000009</v>
+            <v>55000010</v>
           </cell>
           <cell r="Q13">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>55000010</v>
+            <v>55000011</v>
           </cell>
           <cell r="Q14">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>55000011</v>
+            <v>55000012</v>
           </cell>
           <cell r="Q15">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55000012</v>
+            <v>55000013</v>
           </cell>
           <cell r="Q16">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55000013</v>
+            <v>55000014</v>
           </cell>
           <cell r="Q17">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>55000014</v>
+            <v>55000015</v>
           </cell>
           <cell r="Q18">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>55000015</v>
+            <v>55000016</v>
           </cell>
           <cell r="Q19">
-            <v>132</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>55000016</v>
+            <v>55000017</v>
           </cell>
           <cell r="Q20">
             <v>66</v>
@@ -10830,7 +10876,7 @@
         </row>
         <row r="21">
           <cell r="A21">
-            <v>55000017</v>
+            <v>55000018</v>
           </cell>
           <cell r="Q21">
             <v>66</v>
@@ -10838,47 +10884,47 @@
         </row>
         <row r="22">
           <cell r="A22">
-            <v>55000018</v>
+            <v>55000019</v>
           </cell>
           <cell r="Q22">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>55000019</v>
+            <v>55000020</v>
           </cell>
           <cell r="Q23">
-            <v>132</v>
+            <v>160</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>55000020</v>
+            <v>55000021</v>
           </cell>
           <cell r="Q24">
-            <v>160</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>55000021</v>
+            <v>55000029</v>
           </cell>
           <cell r="Q25">
-            <v>0</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>55000029</v>
+            <v>55000030</v>
           </cell>
           <cell r="Q26">
-            <v>300</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>55000030</v>
+            <v>55000031</v>
           </cell>
           <cell r="Q27">
             <v>400</v>
@@ -10886,15 +10932,15 @@
         </row>
         <row r="28">
           <cell r="A28">
-            <v>55000031</v>
+            <v>55000032</v>
           </cell>
           <cell r="Q28">
-            <v>400</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>55000032</v>
+            <v>55000033</v>
           </cell>
           <cell r="Q29">
             <v>600</v>
@@ -10902,127 +10948,127 @@
         </row>
         <row r="30">
           <cell r="A30">
-            <v>55000033</v>
+            <v>55000034</v>
           </cell>
           <cell r="Q30">
-            <v>600</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>55000034</v>
+            <v>55000035</v>
           </cell>
           <cell r="Q31">
-            <v>120</v>
+            <v>800</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>55000035</v>
+            <v>55000036</v>
           </cell>
           <cell r="Q32">
-            <v>800</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>55000036</v>
+            <v>55000037</v>
           </cell>
           <cell r="Q33">
-            <v>100</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>55000037</v>
+            <v>55000038</v>
           </cell>
           <cell r="Q34">
-            <v>500</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>55000038</v>
+            <v>55000039</v>
           </cell>
           <cell r="Q35">
-            <v>1000</v>
+            <v>2000</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>55000039</v>
+            <v>55000040</v>
           </cell>
           <cell r="Q36">
-            <v>2000</v>
+            <v>4000</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>55000040</v>
+            <v>55000041</v>
           </cell>
           <cell r="Q37">
-            <v>4000</v>
+            <v>2000</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55000041</v>
+            <v>55000042</v>
           </cell>
           <cell r="Q38">
-            <v>2000</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55000042</v>
+            <v>55000043</v>
           </cell>
           <cell r="Q39">
-            <v>200</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55000043</v>
+            <v>55000044</v>
           </cell>
           <cell r="Q40">
-            <v>1000</v>
+            <v>2500</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55000044</v>
+            <v>55000045</v>
           </cell>
           <cell r="Q41">
-            <v>2500</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55000045</v>
+            <v>55000046</v>
           </cell>
           <cell r="Q42">
-            <v>200</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55000046</v>
+            <v>55000047</v>
           </cell>
           <cell r="Q43">
-            <v>80</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55000047</v>
+            <v>55000048</v>
           </cell>
           <cell r="Q44">
-            <v>120</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55000048</v>
+            <v>55000049</v>
           </cell>
           <cell r="Q45">
             <v>300</v>
@@ -11030,63 +11076,63 @@
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55000049</v>
+            <v>55000050</v>
           </cell>
           <cell r="Q46">
-            <v>300</v>
+            <v>160</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55000050</v>
+            <v>55000051</v>
           </cell>
           <cell r="Q47">
-            <v>160</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55000051</v>
+            <v>55000061</v>
           </cell>
           <cell r="Q48">
-            <v>500</v>
+            <v>175</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55000061</v>
+            <v>55000062</v>
           </cell>
           <cell r="Q49">
-            <v>175</v>
+            <v>450</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55000062</v>
+            <v>55000063</v>
           </cell>
           <cell r="Q50">
-            <v>450</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55000063</v>
+            <v>55000064</v>
           </cell>
           <cell r="Q51">
-            <v>1000</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55000064</v>
+            <v>55000065</v>
           </cell>
           <cell r="Q52">
-            <v>500</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55000065</v>
+            <v>55000066</v>
           </cell>
           <cell r="Q53">
             <v>100</v>
@@ -11094,7 +11140,7 @@
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55000066</v>
+            <v>55000067</v>
           </cell>
           <cell r="Q54">
             <v>100</v>
@@ -11102,7 +11148,7 @@
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55000067</v>
+            <v>55000068</v>
           </cell>
           <cell r="Q55">
             <v>100</v>
@@ -11110,7 +11156,7 @@
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55000068</v>
+            <v>55000069</v>
           </cell>
           <cell r="Q56">
             <v>100</v>
@@ -11118,7 +11164,7 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55000069</v>
+            <v>55000070</v>
           </cell>
           <cell r="Q57">
             <v>100</v>
@@ -11126,7 +11172,7 @@
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55000070</v>
+            <v>55000071</v>
           </cell>
           <cell r="Q58">
             <v>100</v>
@@ -11134,7 +11180,7 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55000071</v>
+            <v>55000072</v>
           </cell>
           <cell r="Q59">
             <v>100</v>
@@ -11142,63 +11188,63 @@
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55000072</v>
+            <v>55000073</v>
           </cell>
           <cell r="Q60">
-            <v>100</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55000073</v>
+            <v>55000074</v>
           </cell>
           <cell r="Q61">
-            <v>120</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55000074</v>
+            <v>55000075</v>
           </cell>
           <cell r="Q62">
-            <v>100</v>
+            <v>1250</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55000075</v>
+            <v>55000076</v>
           </cell>
           <cell r="Q63">
-            <v>1250</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55000076</v>
+            <v>55000077</v>
           </cell>
           <cell r="Q64">
-            <v>500</v>
+            <v>2600</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55000077</v>
+            <v>55000078</v>
           </cell>
           <cell r="Q65">
-            <v>2600</v>
+            <v>-400</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55000078</v>
+            <v>55000079</v>
           </cell>
           <cell r="Q66">
-            <v>-400</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55000079</v>
+            <v>55000080</v>
           </cell>
           <cell r="Q67">
             <v>200</v>
@@ -11206,79 +11252,79 @@
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55000080</v>
+            <v>55000081</v>
           </cell>
           <cell r="Q68">
-            <v>200</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55000081</v>
+            <v>55000082</v>
           </cell>
           <cell r="Q69">
-            <v>100</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55000082</v>
+            <v>55000083</v>
           </cell>
           <cell r="Q70">
-            <v>600</v>
+            <v>1500</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55000083</v>
+            <v>55000084</v>
           </cell>
           <cell r="Q71">
-            <v>1500</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55000084</v>
+            <v>55000085</v>
           </cell>
           <cell r="Q72">
-            <v>1000</v>
+            <v>250</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55000085</v>
+            <v>55000086</v>
           </cell>
           <cell r="Q73">
-            <v>250</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55000086</v>
+            <v>55000087</v>
           </cell>
           <cell r="Q74">
-            <v>132</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55000087</v>
+            <v>55000088</v>
           </cell>
           <cell r="Q75">
-            <v>600</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55000088</v>
+            <v>55000089</v>
           </cell>
           <cell r="Q76">
-            <v>300</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55000089</v>
+            <v>55000090</v>
           </cell>
           <cell r="Q77">
             <v>600</v>
@@ -11286,303 +11332,303 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55000090</v>
+            <v>55000091</v>
           </cell>
           <cell r="Q78">
-            <v>600</v>
+            <v>-1425</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55000091</v>
+            <v>55000092</v>
           </cell>
           <cell r="Q79">
-            <v>-1425</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55000092</v>
+            <v>55000093</v>
           </cell>
           <cell r="Q80">
-            <v>500</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55000093</v>
+            <v>55000094</v>
           </cell>
           <cell r="Q81">
-            <v>200</v>
+            <v>3000</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55000094</v>
+            <v>55000095</v>
           </cell>
           <cell r="Q82">
-            <v>3000</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55000095</v>
+            <v>55000096</v>
           </cell>
           <cell r="Q83">
-            <v>300</v>
+            <v>280</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55000096</v>
+            <v>55000097</v>
           </cell>
           <cell r="Q84">
-            <v>280</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55000097</v>
+            <v>55000098</v>
           </cell>
           <cell r="Q85">
-            <v>80</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55000098</v>
+            <v>55000099</v>
           </cell>
           <cell r="Q86">
-            <v>400</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55000099</v>
+            <v>55000100</v>
           </cell>
           <cell r="Q87">
-            <v>55</v>
+            <v>555</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55000100</v>
+            <v>55000101</v>
           </cell>
           <cell r="Q88">
-            <v>555</v>
+            <v>180</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55000101</v>
+            <v>55000102</v>
           </cell>
           <cell r="Q89">
-            <v>180</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55000102</v>
+            <v>55000103</v>
           </cell>
           <cell r="Q90">
-            <v>300</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55000103</v>
+            <v>55000104</v>
           </cell>
           <cell r="Q91">
-            <v>1000</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55000104</v>
+            <v>55000105</v>
           </cell>
           <cell r="Q92">
-            <v>132</v>
+            <v>250</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55000105</v>
+            <v>55000106</v>
           </cell>
           <cell r="Q93">
-            <v>250</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55000106</v>
+            <v>55000107</v>
           </cell>
           <cell r="Q94">
-            <v>500</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55000107</v>
+            <v>55000108</v>
           </cell>
           <cell r="Q95">
-            <v>120</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55000108</v>
+            <v>55000109</v>
           </cell>
           <cell r="Q96">
-            <v>80</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55000109</v>
+            <v>55000110</v>
           </cell>
           <cell r="Q97">
-            <v>55</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55000110</v>
+            <v>55000111</v>
           </cell>
           <cell r="Q98">
-            <v>500</v>
+            <v>555</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55000111</v>
+            <v>55000112</v>
           </cell>
           <cell r="Q99">
-            <v>555</v>
+            <v>250</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55000112</v>
+            <v>55000113</v>
           </cell>
           <cell r="Q100">
-            <v>250</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55000113</v>
+            <v>55000114</v>
           </cell>
           <cell r="Q101">
-            <v>111</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55000114</v>
+            <v>55000115</v>
           </cell>
           <cell r="Q102">
-            <v>400</v>
+            <v>2000</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55000115</v>
+            <v>55000116</v>
           </cell>
           <cell r="Q103">
-            <v>2000</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55000116</v>
+            <v>55000117</v>
           </cell>
           <cell r="Q104">
-            <v>300</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55000117</v>
+            <v>55000118</v>
           </cell>
           <cell r="Q105">
-            <v>100</v>
+            <v>83</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55000118</v>
+            <v>55000119</v>
           </cell>
           <cell r="Q106">
-            <v>83</v>
+            <v>700</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55000119</v>
+            <v>55000120</v>
           </cell>
           <cell r="Q107">
-            <v>700</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55000120</v>
+            <v>55000121</v>
           </cell>
           <cell r="Q108">
-            <v>1000</v>
+            <v>333</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55000121</v>
+            <v>55000122</v>
           </cell>
           <cell r="Q109">
-            <v>333</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55000122</v>
+            <v>55000123</v>
           </cell>
           <cell r="Q110">
-            <v>120</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55000123</v>
+            <v>55000124</v>
           </cell>
           <cell r="Q111">
-            <v>200</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55000124</v>
+            <v>55000125</v>
           </cell>
           <cell r="Q112">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55000125</v>
+            <v>55000126</v>
           </cell>
           <cell r="Q113">
-            <v>55</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55000126</v>
+            <v>55000127</v>
           </cell>
           <cell r="Q114">
-            <v>400</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55000127</v>
+            <v>55000128</v>
           </cell>
           <cell r="Q115">
             <v>100</v>
@@ -11590,15 +11636,15 @@
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55000128</v>
+            <v>55000129</v>
           </cell>
           <cell r="Q116">
-            <v>100</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55000129</v>
+            <v>55000130</v>
           </cell>
           <cell r="Q117">
             <v>300</v>
@@ -11606,31 +11652,31 @@
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55000130</v>
+            <v>55000131</v>
           </cell>
           <cell r="Q118">
-            <v>300</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55000131</v>
+            <v>55000132</v>
           </cell>
           <cell r="Q119">
-            <v>500</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55000132</v>
+            <v>55000133</v>
           </cell>
           <cell r="Q120">
-            <v>300</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55000133</v>
+            <v>55000134</v>
           </cell>
           <cell r="Q121">
             <v>500</v>
@@ -11638,47 +11684,47 @@
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55000134</v>
+            <v>55000135</v>
           </cell>
           <cell r="Q122">
-            <v>500</v>
+            <v>-500</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55000135</v>
+            <v>55000136</v>
           </cell>
           <cell r="Q123">
-            <v>-500</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55000136</v>
+            <v>55000137</v>
           </cell>
           <cell r="Q124">
-            <v>600</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55000137</v>
+            <v>55000138</v>
           </cell>
           <cell r="Q125">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55000138</v>
+            <v>55000139</v>
           </cell>
           <cell r="Q126">
-            <v>55</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55000139</v>
+            <v>55000140</v>
           </cell>
           <cell r="Q127">
             <v>111</v>
@@ -11686,7 +11732,7 @@
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55000140</v>
+            <v>55000141</v>
           </cell>
           <cell r="Q128">
             <v>111</v>
@@ -11694,303 +11740,303 @@
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55000141</v>
+            <v>55000142</v>
           </cell>
           <cell r="Q129">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55000142</v>
+            <v>55000143</v>
           </cell>
           <cell r="Q130">
-            <v>55</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55000143</v>
+            <v>55000144</v>
           </cell>
           <cell r="Q131">
-            <v>400</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55000144</v>
+            <v>55000145</v>
           </cell>
           <cell r="Q132">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55000145</v>
+            <v>55000146</v>
           </cell>
           <cell r="Q133">
-            <v>55</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55000146</v>
+            <v>55000147</v>
           </cell>
           <cell r="Q134">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55000147</v>
+            <v>55000148</v>
           </cell>
           <cell r="Q135">
-            <v>55</v>
+            <v>111</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55000148</v>
+            <v>55000149</v>
           </cell>
           <cell r="Q136">
-            <v>111</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55000149</v>
+            <v>55000150</v>
           </cell>
           <cell r="Q137">
-            <v>55</v>
+            <v>75</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55000150</v>
+            <v>55000151</v>
           </cell>
           <cell r="Q138">
-            <v>75</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55000151</v>
+            <v>55000152</v>
           </cell>
           <cell r="Q139">
-            <v>200</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55000152</v>
+            <v>55000153</v>
           </cell>
           <cell r="Q140">
-            <v>300</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55000153</v>
+            <v>55000154</v>
           </cell>
           <cell r="Q141">
-            <v>27</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55000154</v>
+            <v>55000155</v>
           </cell>
           <cell r="Q142">
-            <v>100</v>
+            <v>-120</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55000155</v>
+            <v>55000156</v>
           </cell>
           <cell r="Q143">
-            <v>-120</v>
+            <v>90</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55000156</v>
+            <v>55000157</v>
           </cell>
           <cell r="Q144">
-            <v>90</v>
+            <v>3000</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55000157</v>
+            <v>55000158</v>
           </cell>
           <cell r="Q145">
-            <v>3000</v>
+            <v>700</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55000158</v>
+            <v>55000159</v>
           </cell>
           <cell r="Q146">
-            <v>700</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55000159</v>
+            <v>55000160</v>
           </cell>
           <cell r="Q147">
-            <v>120</v>
+            <v>950</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55000160</v>
+            <v>55000161</v>
           </cell>
           <cell r="Q148">
-            <v>950</v>
+            <v>83</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55000161</v>
+            <v>55000162</v>
           </cell>
           <cell r="Q149">
-            <v>83</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55000162</v>
+            <v>55000163</v>
           </cell>
           <cell r="Q150">
-            <v>100</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55000163</v>
+            <v>55000164</v>
           </cell>
           <cell r="Q151">
-            <v>1000</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55000164</v>
+            <v>55000165</v>
           </cell>
           <cell r="Q152">
-            <v>600</v>
+            <v>266</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55000165</v>
+            <v>55000166</v>
           </cell>
           <cell r="Q153">
-            <v>266</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55000166</v>
+            <v>55000167</v>
           </cell>
           <cell r="Q154">
-            <v>600</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55000167</v>
+            <v>55000168</v>
           </cell>
           <cell r="Q155">
-            <v>1000</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55000168</v>
+            <v>55000169</v>
           </cell>
           <cell r="Q156">
-            <v>200</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55000169</v>
+            <v>55000170</v>
           </cell>
           <cell r="Q157">
-            <v>500</v>
+            <v>112</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55000170</v>
+            <v>55000171</v>
           </cell>
           <cell r="Q158">
-            <v>112</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55000171</v>
+            <v>55000172</v>
           </cell>
           <cell r="Q159">
-            <v>400</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55000172</v>
+            <v>55000173</v>
           </cell>
           <cell r="Q160">
-            <v>200</v>
+            <v>160</v>
           </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55000173</v>
+            <v>55000174</v>
           </cell>
           <cell r="Q161">
-            <v>160</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55000174</v>
+            <v>55000175</v>
           </cell>
           <cell r="Q162">
-            <v>150</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55000175</v>
+            <v>55000176</v>
           </cell>
           <cell r="Q163">
-            <v>132</v>
+            <v>555</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55000176</v>
+            <v>55000177</v>
           </cell>
           <cell r="Q164">
-            <v>555</v>
+            <v>75</v>
           </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55000177</v>
+            <v>55000178</v>
           </cell>
           <cell r="Q165">
-            <v>75</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55000178</v>
+            <v>55000179</v>
           </cell>
           <cell r="Q166">
             <v>500</v>
@@ -11998,215 +12044,215 @@
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55000179</v>
+            <v>55000180</v>
           </cell>
           <cell r="Q167">
-            <v>500</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55000180</v>
+            <v>55000181</v>
           </cell>
           <cell r="Q168">
-            <v>1000</v>
+            <v>4000</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55000181</v>
+            <v>55000182</v>
           </cell>
           <cell r="Q169">
-            <v>4000</v>
+            <v>333</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55000182</v>
+            <v>55000183</v>
           </cell>
           <cell r="Q170">
-            <v>333</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55000183</v>
+            <v>55000184</v>
           </cell>
           <cell r="Q171">
-            <v>300</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55000184</v>
+            <v>55000185</v>
           </cell>
           <cell r="Q172">
-            <v>120</v>
+            <v>360</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55000185</v>
+            <v>55000186</v>
           </cell>
           <cell r="Q173">
-            <v>360</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55000186</v>
+            <v>55000187</v>
           </cell>
           <cell r="Q174">
-            <v>200</v>
+            <v>-1200</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55000187</v>
+            <v>55000188</v>
           </cell>
           <cell r="Q175">
-            <v>-1200</v>
+            <v>-36</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55000188</v>
+            <v>55000189</v>
           </cell>
           <cell r="Q176">
-            <v>-36</v>
+            <v>2000</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55000189</v>
+            <v>55000190</v>
           </cell>
           <cell r="Q177">
-            <v>2000</v>
+            <v>175</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55000190</v>
+            <v>55000191</v>
           </cell>
           <cell r="Q178">
-            <v>175</v>
+            <v>2222</v>
           </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55000191</v>
+            <v>55000192</v>
           </cell>
           <cell r="Q179">
-            <v>2222</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55000192</v>
+            <v>55000193</v>
           </cell>
           <cell r="Q180">
-            <v>200</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55000193</v>
+            <v>55000194</v>
           </cell>
           <cell r="Q181">
-            <v>60</v>
+            <v>166</v>
           </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55000194</v>
+            <v>55000195</v>
           </cell>
           <cell r="Q182">
-            <v>166</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55000195</v>
+            <v>55000196</v>
           </cell>
           <cell r="Q183">
-            <v>100</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55000196</v>
+            <v>55000197</v>
           </cell>
           <cell r="Q184">
-            <v>150</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55000197</v>
+            <v>55000198</v>
           </cell>
           <cell r="Q185">
-            <v>300</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55000198</v>
+            <v>55000199</v>
           </cell>
           <cell r="Q186">
-            <v>200</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55000199</v>
+            <v>55000200</v>
           </cell>
           <cell r="Q187">
-            <v>600</v>
+            <v>1400</v>
           </cell>
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55000200</v>
+            <v>55000201</v>
           </cell>
           <cell r="Q188">
-            <v>1400</v>
+            <v>225</v>
           </cell>
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55000201</v>
+            <v>55000202</v>
           </cell>
           <cell r="Q189">
-            <v>225</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55000202</v>
+            <v>55000203</v>
           </cell>
           <cell r="Q190">
-            <v>1000</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55000203</v>
+            <v>55000204</v>
           </cell>
           <cell r="Q191">
-            <v>500</v>
+            <v>44</v>
           </cell>
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55000204</v>
+            <v>55000205</v>
           </cell>
           <cell r="Q192">
-            <v>44</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55000205</v>
+            <v>55000206</v>
           </cell>
           <cell r="Q193">
             <v>120</v>
@@ -12214,159 +12260,159 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55000206</v>
+            <v>55000207</v>
           </cell>
           <cell r="Q194">
-            <v>120</v>
+            <v>2500</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55000207</v>
+            <v>55000208</v>
           </cell>
           <cell r="Q195">
-            <v>2500</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55000208</v>
+            <v>55000209</v>
           </cell>
           <cell r="Q196">
-            <v>50</v>
+            <v>44</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55000209</v>
+            <v>55000210</v>
           </cell>
           <cell r="Q197">
-            <v>44</v>
+            <v>666</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55000210</v>
+            <v>55000211</v>
           </cell>
           <cell r="Q198">
-            <v>666</v>
+            <v>11</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55000211</v>
+            <v>55000212</v>
           </cell>
           <cell r="Q199">
-            <v>11</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55000212</v>
+            <v>55000213</v>
           </cell>
           <cell r="Q200">
-            <v>300</v>
+            <v>11</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55000213</v>
+            <v>55000214</v>
           </cell>
           <cell r="Q201">
-            <v>11</v>
+            <v>1500</v>
           </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55000214</v>
+            <v>55000215</v>
           </cell>
           <cell r="Q202">
-            <v>1500</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55000215</v>
+            <v>55000216</v>
           </cell>
           <cell r="Q203">
-            <v>400</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="204">
           <cell r="A204">
-            <v>55000216</v>
+            <v>55000217</v>
           </cell>
           <cell r="Q204">
-            <v>500</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="205">
           <cell r="A205">
-            <v>55000217</v>
+            <v>55000218</v>
           </cell>
           <cell r="Q205">
-            <v>200</v>
+            <v>800</v>
           </cell>
         </row>
         <row r="206">
           <cell r="A206">
-            <v>55000218</v>
+            <v>55000219</v>
           </cell>
           <cell r="Q206">
-            <v>800</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>55000219</v>
+            <v>55000220</v>
           </cell>
           <cell r="Q207">
-            <v>200</v>
+            <v>120</v>
           </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>55000220</v>
+            <v>55000221</v>
           </cell>
           <cell r="Q208">
-            <v>120</v>
+            <v>1200</v>
           </cell>
         </row>
         <row r="209">
           <cell r="A209">
-            <v>55000221</v>
+            <v>55000222</v>
           </cell>
           <cell r="Q209">
-            <v>1200</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="210">
           <cell r="A210">
-            <v>55000222</v>
+            <v>55000223</v>
           </cell>
           <cell r="Q210">
-            <v>400</v>
+            <v>66</v>
           </cell>
         </row>
         <row r="211">
           <cell r="A211">
-            <v>55000223</v>
+            <v>55000224</v>
           </cell>
           <cell r="Q211">
-            <v>66</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="212">
           <cell r="A212">
-            <v>55000224</v>
+            <v>55000225</v>
           </cell>
           <cell r="Q212">
-            <v>132</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="213">
           <cell r="A213">
-            <v>55000225</v>
+            <v>55000226</v>
           </cell>
           <cell r="Q213">
             <v>500</v>
@@ -12374,290 +12420,290 @@
         </row>
         <row r="214">
           <cell r="A214">
-            <v>55000226</v>
+            <v>55000227</v>
           </cell>
           <cell r="Q214">
-            <v>500</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="215">
           <cell r="A215">
-            <v>55000227</v>
+            <v>55000228</v>
           </cell>
           <cell r="Q215">
-            <v>300</v>
+            <v>180</v>
           </cell>
         </row>
         <row r="216">
           <cell r="A216">
-            <v>55000228</v>
+            <v>55000229</v>
           </cell>
           <cell r="Q216">
-            <v>180</v>
+            <v>3000</v>
           </cell>
         </row>
         <row r="217">
           <cell r="A217">
-            <v>55000229</v>
+            <v>55000230</v>
           </cell>
           <cell r="Q217">
-            <v>3000</v>
+            <v>-1800</v>
           </cell>
         </row>
         <row r="218">
           <cell r="A218">
-            <v>55000230</v>
+            <v>55000231</v>
           </cell>
           <cell r="Q218">
-            <v>-1800</v>
+            <v>1500</v>
           </cell>
         </row>
         <row r="219">
           <cell r="A219">
-            <v>55000231</v>
+            <v>55000232</v>
           </cell>
           <cell r="Q219">
-            <v>1500</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="220">
           <cell r="A220">
-            <v>55000232</v>
+            <v>55000233</v>
           </cell>
           <cell r="Q220">
-            <v>300</v>
+            <v>-200</v>
           </cell>
         </row>
         <row r="221">
           <cell r="A221">
-            <v>55000233</v>
+            <v>55000234</v>
           </cell>
           <cell r="Q221">
-            <v>-200</v>
+            <v>333</v>
           </cell>
         </row>
         <row r="222">
           <cell r="A222">
-            <v>55000234</v>
+            <v>55000235</v>
           </cell>
           <cell r="Q222">
-            <v>333</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="223">
           <cell r="A223">
-            <v>55000235</v>
+            <v>55000236</v>
           </cell>
           <cell r="Q223">
-            <v>100</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="224">
           <cell r="A224">
-            <v>55000236</v>
+            <v>55000237</v>
           </cell>
           <cell r="Q224">
-            <v>500</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="225">
           <cell r="A225">
-            <v>55000237</v>
+            <v>55000238</v>
           </cell>
           <cell r="Q225">
-            <v>0</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="226">
           <cell r="A226">
-            <v>55000238</v>
+            <v>55000239</v>
           </cell>
           <cell r="Q226">
-            <v>1000</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="227">
           <cell r="A227">
-            <v>55000239</v>
+            <v>55000240</v>
           </cell>
           <cell r="Q227">
-            <v>200</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="228">
           <cell r="A228">
-            <v>55000240</v>
+            <v>55000241</v>
           </cell>
           <cell r="Q228">
-            <v>500</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="229">
           <cell r="A229">
-            <v>55000241</v>
+            <v>55000242</v>
           </cell>
           <cell r="Q229">
-            <v>30</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="230">
           <cell r="A230">
-            <v>55000242</v>
+            <v>55000243</v>
           </cell>
           <cell r="Q230">
-            <v>300</v>
+            <v>222</v>
           </cell>
         </row>
         <row r="231">
           <cell r="A231">
-            <v>55000243</v>
+            <v>55000244</v>
           </cell>
           <cell r="Q231">
-            <v>222</v>
+            <v>280</v>
           </cell>
         </row>
         <row r="232">
           <cell r="A232">
-            <v>55000244</v>
+            <v>55000245</v>
           </cell>
           <cell r="Q232">
-            <v>280</v>
+            <v>450</v>
           </cell>
         </row>
         <row r="233">
           <cell r="A233">
-            <v>55000245</v>
+            <v>55000246</v>
           </cell>
           <cell r="Q233">
-            <v>450</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="234">
           <cell r="A234">
-            <v>55000246</v>
+            <v>55000247</v>
           </cell>
           <cell r="Q234">
-            <v>100</v>
+            <v>132</v>
           </cell>
         </row>
         <row r="235">
           <cell r="A235">
-            <v>55000247</v>
+            <v>55000248</v>
           </cell>
           <cell r="Q235">
-            <v>132</v>
+            <v>800</v>
           </cell>
         </row>
         <row r="236">
           <cell r="A236">
-            <v>55000248</v>
+            <v>55000249</v>
           </cell>
           <cell r="Q236">
-            <v>800</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="237">
           <cell r="A237">
-            <v>55000249</v>
+            <v>55000250</v>
           </cell>
           <cell r="Q237">
-            <v>400</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="238">
           <cell r="A238">
-            <v>55000250</v>
+            <v>55000251</v>
           </cell>
           <cell r="Q238">
-            <v>300</v>
+            <v>250</v>
           </cell>
         </row>
         <row r="239">
           <cell r="A239">
-            <v>55000251</v>
+            <v>55000252</v>
           </cell>
           <cell r="Q239">
-            <v>250</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="240">
           <cell r="A240">
-            <v>55000252</v>
+            <v>55000253</v>
           </cell>
           <cell r="Q240">
-            <v>100</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="241">
           <cell r="A241">
-            <v>55000253</v>
+            <v>55000254</v>
           </cell>
           <cell r="Q241">
-            <v>30</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="242">
           <cell r="A242">
-            <v>55000254</v>
+            <v>55000255</v>
           </cell>
           <cell r="Q242">
-            <v>300</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="243">
           <cell r="A243">
-            <v>55000255</v>
+            <v>55000256</v>
           </cell>
           <cell r="Q243">
-            <v>500</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="244">
           <cell r="A244">
-            <v>55000256</v>
+            <v>55000257</v>
           </cell>
           <cell r="Q244">
-            <v>30</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="245">
           <cell r="A245">
-            <v>55000257</v>
+            <v>55000258</v>
           </cell>
           <cell r="Q245">
-            <v>200</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="246">
           <cell r="A246">
-            <v>55000258</v>
+            <v>55000259</v>
           </cell>
           <cell r="Q246">
-            <v>300</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="247">
           <cell r="A247">
-            <v>55000259</v>
+            <v>55000260</v>
           </cell>
           <cell r="Q247">
-            <v>500</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="248">
           <cell r="A248">
-            <v>55000260</v>
+            <v>55000261</v>
           </cell>
           <cell r="Q248">
-            <v>300</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="249">
           <cell r="A249">
-            <v>55000261</v>
+            <v>55000262</v>
           </cell>
           <cell r="Q249">
-            <v>200</v>
+            <v>2200</v>
           </cell>
         </row>
         <row r="250">
@@ -12950,15 +12996,15 @@
         </row>
         <row r="286">
           <cell r="A286">
-            <v>55000324</v>
+            <v>55000300</v>
           </cell>
           <cell r="Q286">
-            <v>500</v>
+            <v>2500</v>
           </cell>
         </row>
         <row r="287">
           <cell r="A287">
-            <v>55000325</v>
+            <v>55000324</v>
           </cell>
           <cell r="Q287">
             <v>500</v>
@@ -12966,121 +13012,129 @@
         </row>
         <row r="288">
           <cell r="A288">
-            <v>55000326</v>
+            <v>55000325</v>
           </cell>
           <cell r="Q288">
-            <v>1000</v>
+            <v>500</v>
           </cell>
         </row>
         <row r="289">
           <cell r="A289">
-            <v>55000327</v>
+            <v>55000326</v>
           </cell>
           <cell r="Q289">
-            <v>833</v>
+            <v>1000</v>
           </cell>
         </row>
         <row r="290">
           <cell r="A290">
-            <v>55000328</v>
+            <v>55000327</v>
           </cell>
           <cell r="Q290">
-            <v>700</v>
+            <v>833</v>
           </cell>
         </row>
         <row r="291">
           <cell r="A291">
-            <v>55000329</v>
+            <v>55000328</v>
           </cell>
           <cell r="Q291">
-            <v>600</v>
+            <v>700</v>
           </cell>
         </row>
         <row r="292">
           <cell r="A292">
-            <v>55000330</v>
+            <v>55000329</v>
           </cell>
           <cell r="Q292">
-            <v>480</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="293">
           <cell r="A293">
-            <v>55000331</v>
+            <v>55000330</v>
           </cell>
           <cell r="Q293">
-            <v>600</v>
+            <v>480</v>
           </cell>
         </row>
         <row r="294">
           <cell r="A294">
-            <v>55000332</v>
+            <v>55000331</v>
           </cell>
           <cell r="Q294">
-            <v>50</v>
+            <v>600</v>
           </cell>
         </row>
         <row r="295">
           <cell r="A295">
-            <v>55000333</v>
+            <v>55000332</v>
           </cell>
           <cell r="Q295">
-            <v>30</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="296">
           <cell r="A296">
-            <v>55000334</v>
+            <v>55000333</v>
           </cell>
           <cell r="Q296">
-            <v>250</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="297">
           <cell r="A297">
-            <v>55000335</v>
+            <v>55000334</v>
           </cell>
           <cell r="Q297">
-            <v>1500</v>
+            <v>250</v>
           </cell>
         </row>
         <row r="298">
           <cell r="A298">
-            <v>55000340</v>
+            <v>55000335</v>
           </cell>
           <cell r="Q298">
-            <v>200</v>
+            <v>1500</v>
           </cell>
         </row>
         <row r="299">
           <cell r="A299">
-            <v>55000341</v>
+            <v>55000340</v>
           </cell>
           <cell r="Q299">
-            <v>800</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="300">
           <cell r="A300">
-            <v>55000342</v>
+            <v>55000341</v>
           </cell>
           <cell r="Q300">
-            <v>400</v>
+            <v>800</v>
           </cell>
         </row>
         <row r="301">
           <cell r="A301">
+            <v>55000342</v>
+          </cell>
+          <cell r="Q301">
+            <v>400</v>
+          </cell>
+        </row>
+        <row r="302">
+          <cell r="A302">
             <v>55000343</v>
           </cell>
-          <cell r="Q301">
+          <cell r="Q302">
             <v>600</v>
           </cell>
         </row>
-        <row r="302">
-          <cell r="A302" t="str">
+        <row r="303">
+          <cell r="A303" t="str">
             <v>55000060|FightQuick</v>
           </cell>
-          <cell r="Q302">
+          <cell r="Q303">
             <v>100</v>
           </cell>
         </row>
@@ -22118,8 +22172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BF311" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136" tableBorderDxfId="135">
-  <autoFilter ref="A3:BF311"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BF312" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136" tableBorderDxfId="135">
+  <autoFilter ref="A3:BF312"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
@@ -22150,144 +22204,144 @@
     </tableColumn>
     <tableColumn id="13" name="Range" dataDxfId="114"/>
     <tableColumn id="14" name="Mov" dataDxfId="113"/>
-    <tableColumn id="51" name="LifeTime" dataDxfId="14"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="112"/>
-    <tableColumn id="18" name="Skills" dataDxfId="111"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="110"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="109"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="108"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="107"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="106"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="105"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="104"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="103"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="102">
+    <tableColumn id="51" name="LifeTime" dataDxfId="112"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="111"/>
+    <tableColumn id="18" name="Skills" dataDxfId="110"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="109"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="108"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="107"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="106"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="105"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="104"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="103"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="102"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="101">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="101"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="100"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="99"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="98"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="97"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="96">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="100"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="99"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="98"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="97"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="96"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="95">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="95"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="94"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="93"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="92"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="91"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="90"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="89"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="88"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="87"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="86">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="94"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="93"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="92"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="91"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="90"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="89"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="88"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="87"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="86"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="85">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="85"/>
-    <tableColumn id="20" name="Res" dataDxfId="84"/>
-    <tableColumn id="21" name="Icon" dataDxfId="83"/>
-    <tableColumn id="17" name="Cover" dataDxfId="82"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="81"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="80"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="79"/>
-    <tableColumn id="29" name="Remark" dataDxfId="78"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="84"/>
+    <tableColumn id="20" name="Res" dataDxfId="83"/>
+    <tableColumn id="21" name="Icon" dataDxfId="82"/>
+    <tableColumn id="17" name="Cover" dataDxfId="81"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="80"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="79"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="78"/>
+    <tableColumn id="29" name="Remark" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BH11" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BH11" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A3:BH11"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="60">
-    <tableColumn id="1" name="Id" dataDxfId="74"/>
-    <tableColumn id="2" name="Name" dataDxfId="73"/>
-    <tableColumn id="22" name="Ename" dataDxfId="72"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="71"/>
-    <tableColumn id="3" name="Star" dataDxfId="70"/>
-    <tableColumn id="4" name="Type" dataDxfId="69"/>
-    <tableColumn id="5" name="Attr" dataDxfId="68"/>
-    <tableColumn id="58" name="Quality" dataDxfId="67">
+    <tableColumn id="1" name="Id" dataDxfId="64"/>
+    <tableColumn id="2" name="Name" dataDxfId="63"/>
+    <tableColumn id="22" name="Ename" dataDxfId="62"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="61"/>
+    <tableColumn id="3" name="Star" dataDxfId="60"/>
+    <tableColumn id="4" name="Type" dataDxfId="59"/>
+    <tableColumn id="5" name="Attr" dataDxfId="58"/>
+    <tableColumn id="58" name="Quality" dataDxfId="57">
       <calculatedColumnFormula>IF(T4&gt;10,5,IF(T4&gt;5,4,IF(T4&gt;2.5,3,IF(T4&gt;0,2,IF(T4&gt;-2.5,1,IF(T4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="66"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="65"/>
-    <tableColumn id="24" name="VitP" dataDxfId="64"/>
-    <tableColumn id="25" name="Modify" dataDxfId="63"/>
-    <tableColumn id="9" name="Def" dataDxfId="62"/>
-    <tableColumn id="10" name="Mag" dataDxfId="61"/>
-    <tableColumn id="32" name="Spd" dataDxfId="60"/>
-    <tableColumn id="35" name="Hit" dataDxfId="59"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="58"/>
-    <tableColumn id="34" name="Crt" dataDxfId="57"/>
-    <tableColumn id="33" name="Luk" dataDxfId="56"/>
-    <tableColumn id="7" name="Sum" dataDxfId="55">
+    <tableColumn id="12" name="Cost" dataDxfId="56"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="55"/>
+    <tableColumn id="24" name="VitP" dataDxfId="54"/>
+    <tableColumn id="25" name="Modify" dataDxfId="53"/>
+    <tableColumn id="9" name="Def" dataDxfId="52"/>
+    <tableColumn id="10" name="Mag" dataDxfId="51"/>
+    <tableColumn id="32" name="Spd" dataDxfId="50"/>
+    <tableColumn id="35" name="Hit" dataDxfId="49"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="48"/>
+    <tableColumn id="34" name="Crt" dataDxfId="47"/>
+    <tableColumn id="33" name="Luk" dataDxfId="46"/>
+    <tableColumn id="7" name="Sum" dataDxfId="45">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AQ4:AY4)+2.5*SUM(AK4:AO4)+AJ4/100+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="54"/>
-    <tableColumn id="14" name="Mov" dataDxfId="53"/>
-    <tableColumn id="60" name="LifeTime" dataDxfId="0"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="52"/>
-    <tableColumn id="18" name="Skills" dataDxfId="51"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="50"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="49"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="48"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="47"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="46"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="45"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="44"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="43"/>
-    <tableColumn id="50" name="~Skill5" dataDxfId="42"/>
-    <tableColumn id="51" name="~SkillRate5" dataDxfId="41"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="40">
+    <tableColumn id="13" name="Range" dataDxfId="44"/>
+    <tableColumn id="14" name="Mov" dataDxfId="43"/>
+    <tableColumn id="60" name="LifeTime" dataDxfId="42"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="41"/>
+    <tableColumn id="18" name="Skills" dataDxfId="40"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="39"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="38"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="37"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="36"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="35"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="34"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="33"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="32"/>
+    <tableColumn id="50" name="~Skill5" dataDxfId="31"/>
+    <tableColumn id="51" name="~SkillRate5" dataDxfId="30"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="29">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AG4/100)+
 IF(ISBLANK($AH4),0, LOOKUP($AH4,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AI4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="39"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="38"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="37"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="36"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="35"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="34">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="28"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="27"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="26"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="25"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="24"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="23">
       <calculatedColumnFormula>CONCATENATE(AK4,";",AL4,";",AM4,";",AN4,";",AO4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="33"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="32"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="31"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="30"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="29"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="28"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="27"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="26"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="25"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="24">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="22"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="21"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="20"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="19"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="18"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="17"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="16"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="15"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="14"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="13">
       <calculatedColumnFormula>CONCATENATE(AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4,";",AX4,";",AY4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="23"/>
-    <tableColumn id="20" name="Res" dataDxfId="22"/>
-    <tableColumn id="21" name="Icon" dataDxfId="21"/>
-    <tableColumn id="17" name="Cover" dataDxfId="20"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="19"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="18"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="17"/>
-    <tableColumn id="29" name="Remark" dataDxfId="16"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="12"/>
+    <tableColumn id="20" name="Res" dataDxfId="11"/>
+    <tableColumn id="21" name="Icon" dataDxfId="10"/>
+    <tableColumn id="17" name="Cover" dataDxfId="9"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="8"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="7"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="6"/>
+    <tableColumn id="29" name="Remark" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -22591,13 +22645,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF311"/>
+  <dimension ref="A1:BF312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="Z312" sqref="Z312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22607,7 +22661,8 @@
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="6.109375" customWidth="1"/>
     <col min="5" max="9" width="3.33203125" customWidth="1"/>
-    <col min="10" max="11" width="4.109375" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" customWidth="1"/>
     <col min="12" max="19" width="4.77734375" customWidth="1"/>
     <col min="20" max="20" width="4.109375" customWidth="1"/>
     <col min="21" max="23" width="4.77734375" customWidth="1"/>
@@ -67425,7 +67480,7 @@
         <v>1</v>
       </c>
       <c r="H260" s="4">
-        <f t="shared" ref="H260:H311" si="16">IF(T260&gt;10,5,IF(T260&gt;5,4,IF(T260&gt;2.5,3,IF(T260&gt;0,2,IF(T260&gt;-2.5,1,IF(T260&gt;-10,0,6))))))</f>
+        <f t="shared" ref="H260:H312" si="16">IF(T260&gt;10,5,IF(T260&gt;5,4,IF(T260&gt;2.5,3,IF(T260&gt;0,2,IF(T260&gt;-2.5,1,IF(T260&gt;-10,0,6))))))</f>
         <v>4</v>
       </c>
       <c r="I260" s="4">
@@ -67462,7 +67517,7 @@
         <v>0</v>
       </c>
       <c r="T260" s="15">
-        <f t="shared" ref="T260:T311" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AO260:AW260)+2.5*SUM(AI260:AM260)+AH260/100+L260</f>
+        <f t="shared" ref="T260:T312" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AO260:AW260)+2.5*SUM(AI260:AM260)+AH260/100+L260</f>
         <v>9.5</v>
       </c>
       <c r="U260" s="4">
@@ -67550,7 +67605,7 @@
         <v>0</v>
       </c>
       <c r="AX260" s="4" t="str">
-        <f t="shared" ref="AX260:AX311" si="18">CONCATENATE(AO260,";",AP260,";",AQ260,";",AR260,";",AS260,";",AT260,";",AU260,";",AV260,";",AW260)</f>
+        <f t="shared" ref="AX260:AX312" si="18">CONCATENATE(AO260,";",AP260,";",AQ260,";",AR260,";",AS260,";",AT260,";",AU260,";",AV260,";",AW260)</f>
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY260" s="56" t="s">
@@ -67693,7 +67748,7 @@
         <v>0</v>
       </c>
       <c r="AN261" s="4" t="str">
-        <f t="shared" ref="AN261:AN311" si="19">CONCATENATE(AI261,";",AJ261,";",AK261,";",AL261,";",AM261)</f>
+        <f t="shared" ref="AN261:AN312" si="19">CONCATENATE(AI261,";",AJ261,";",AK261,";",AL261,";",AM261)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AO261" s="21">
@@ -75863,7 +75918,7 @@
         <v>0</v>
       </c>
       <c r="BD308" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE308" s="30">
         <v>0.49672129999999998</v>
@@ -76364,10 +76419,180 @@
         <v>1276</v>
       </c>
     </row>
+    <row r="312" spans="1:58">
+      <c r="A312">
+        <v>51000309</v>
+      </c>
+      <c r="B312" s="11" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D312" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="E312" s="11">
+        <v>3</v>
+      </c>
+      <c r="F312" s="11">
+        <v>13</v>
+      </c>
+      <c r="G312" s="11">
+        <v>4</v>
+      </c>
+      <c r="H312" s="24">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="I312" s="11">
+        <v>3</v>
+      </c>
+      <c r="J312" s="11">
+        <v>-100</v>
+      </c>
+      <c r="K312" s="11">
+        <v>20</v>
+      </c>
+      <c r="L312" s="11">
+        <v>-2</v>
+      </c>
+      <c r="M312" s="11">
+        <v>0</v>
+      </c>
+      <c r="N312" s="11">
+        <v>0</v>
+      </c>
+      <c r="O312" s="11">
+        <v>0</v>
+      </c>
+      <c r="P312" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q312" s="11">
+        <v>0</v>
+      </c>
+      <c r="R312" s="11">
+        <v>0</v>
+      </c>
+      <c r="S312" s="11">
+        <v>0</v>
+      </c>
+      <c r="T312" s="24">
+        <f t="shared" si="17"/>
+        <v>-57</v>
+      </c>
+      <c r="U312" s="11">
+        <v>0</v>
+      </c>
+      <c r="V312" s="11">
+        <v>0</v>
+      </c>
+      <c r="W312" s="11">
+        <v>90</v>
+      </c>
+      <c r="X312" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y312" s="11" t="s">
+        <v>1428</v>
+      </c>
+      <c r="Z312" s="21">
+        <v>55000300</v>
+      </c>
+      <c r="AA312" s="21">
+        <v>100</v>
+      </c>
+      <c r="AB312" s="21"/>
+      <c r="AC312" s="21"/>
+      <c r="AD312" s="21"/>
+      <c r="AE312" s="21"/>
+      <c r="AF312" s="21"/>
+      <c r="AG312" s="21"/>
+      <c r="AH312" s="21">
+        <f>IF(ISBLANK($Z312),0, LOOKUP($Z312,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AA312/100)+
+IF(ISBLANK($AB312),0, LOOKUP($AB312,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AC312/100)+
+IF(ISBLANK($AD312),0, LOOKUP($AD312,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AE312/100)+
+IF(ISBLANK($AF312),0, LOOKUP($AF312,[1]Skill!$A:$A,[1]Skill!$Q:$Q)*$AG312/100)</f>
+        <v>2500</v>
+      </c>
+      <c r="AI312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AJ312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AK312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AL312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AM312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN312" s="11" t="str">
+        <f t="shared" si="19"/>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AO312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AP312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AQ312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AR312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AV312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AW312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AX312" s="11" t="str">
+        <f t="shared" si="18"/>
+        <v>0;0;0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AY312" s="57" t="s">
+        <v>1418</v>
+      </c>
+      <c r="AZ312" s="11">
+        <v>6</v>
+      </c>
+      <c r="BA312" s="11">
+        <v>309</v>
+      </c>
+      <c r="BB312" s="11"/>
+      <c r="BC312" s="24">
+        <v>0</v>
+      </c>
+      <c r="BD312" s="11">
+        <v>1</v>
+      </c>
+      <c r="BE312" s="11">
+        <v>0.40819670000000002</v>
+      </c>
+      <c r="BF312" s="11" t="s">
+        <v>1427</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="T4:T311">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="T4:T312">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -76378,17 +76603,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H311">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="H4:H312">
+    <cfRule type="cellIs" dxfId="141" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="138" priority="9" operator="greaterThanOrEqual">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T312">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H312">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -78325,31 +78576,31 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4:K7 K10:K11">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J7">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="9" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78367,13 +78618,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="5" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78391,13 +78642,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
monster life time to set by round
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -220,7 +220,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-主要是建筑类</t>
+主要是建筑类，回合数</t>
         </r>
       </text>
     </comment>
@@ -692,7 +692,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-主要是建筑类</t>
+主要是建筑类，回合数</t>
         </r>
       </text>
     </comment>
@@ -5499,14 +5499,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifeTime</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>哥布林巢穴</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5527,6 +5519,14 @@
   </si>
   <si>
     <t>55000203;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LifeRound</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6606,42 +6606,6 @@
   <dxfs count="140">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -7076,6 +7040,24 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -8825,6 +8807,24 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -9879,11 +9879,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="62134912"/>
-        <c:axId val="62133824"/>
+        <c:axId val="-1104899136"/>
+        <c:axId val="-1104895328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62134912"/>
+        <c:axId val="-1104899136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9926,7 +9926,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62133824"/>
+        <c:crossAx val="-1104895328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9934,7 +9934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62133824"/>
+        <c:axId val="-1104895328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9985,7 +9985,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62134912"/>
+        <c:crossAx val="-1104899136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22125,7 +22125,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BF312" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130" tableBorderDxfId="129">
-  <autoFilter ref="A3:BF312"/>
+  <autoFilter ref="A3:BF312">
+    <filterColumn colId="22">
+      <filters>
+        <filter val="120"/>
+        <filter val="60"/>
+        <filter val="90"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
@@ -22156,7 +22164,7 @@
     </tableColumn>
     <tableColumn id="13" name="Range" dataDxfId="108"/>
     <tableColumn id="14" name="Mov" dataDxfId="107"/>
-    <tableColumn id="51" name="LifeTime" dataDxfId="106"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="106"/>
     <tableColumn id="16" name="Arrow" dataDxfId="105"/>
     <tableColumn id="18" name="Skills" dataDxfId="104"/>
     <tableColumn id="42" name="~Skill1" dataDxfId="103"/>
@@ -22167,130 +22175,130 @@
     <tableColumn id="47" name="~SkillRate3" dataDxfId="98"/>
     <tableColumn id="48" name="~Skill4" dataDxfId="97"/>
     <tableColumn id="49" name="~SkillRate4" dataDxfId="96"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="1">
+    <tableColumn id="54" name="~SkillMark" dataDxfId="95">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="95"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="94"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="93"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="92"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="91"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="90">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="94"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="93"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="92"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="91"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="90"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="89">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="89"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="88"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="87"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="86"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="85"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="84"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="83"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="82"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="81"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="80">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="88"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="87"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="86"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="85"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="84"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="83"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="82"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="81"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="80"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="79">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="79"/>
-    <tableColumn id="20" name="Res" dataDxfId="78"/>
-    <tableColumn id="21" name="Icon" dataDxfId="77"/>
-    <tableColumn id="17" name="Cover" dataDxfId="76"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="75"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="74"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="73"/>
-    <tableColumn id="29" name="Remark" dataDxfId="72"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="78"/>
+    <tableColumn id="20" name="Res" dataDxfId="77"/>
+    <tableColumn id="21" name="Icon" dataDxfId="76"/>
+    <tableColumn id="17" name="Cover" dataDxfId="75"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="74"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="73"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="72"/>
+    <tableColumn id="29" name="Remark" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BF11" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BF11" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="A3:BF11"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="Id" dataDxfId="59"/>
-    <tableColumn id="2" name="Name" dataDxfId="58"/>
-    <tableColumn id="22" name="Ename" dataDxfId="57"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="56"/>
-    <tableColumn id="3" name="Star" dataDxfId="55"/>
-    <tableColumn id="4" name="Type" dataDxfId="54"/>
-    <tableColumn id="5" name="Attr" dataDxfId="53"/>
-    <tableColumn id="58" name="Quality" dataDxfId="52">
+    <tableColumn id="1" name="Id" dataDxfId="58"/>
+    <tableColumn id="2" name="Name" dataDxfId="57"/>
+    <tableColumn id="22" name="Ename" dataDxfId="56"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="55"/>
+    <tableColumn id="3" name="Star" dataDxfId="54"/>
+    <tableColumn id="4" name="Type" dataDxfId="53"/>
+    <tableColumn id="5" name="Attr" dataDxfId="52"/>
+    <tableColumn id="58" name="Quality" dataDxfId="51">
       <calculatedColumnFormula>IF(T4&gt;10,5,IF(T4&gt;5,4,IF(T4&gt;2.5,3,IF(T4&gt;0,2,IF(T4&gt;-2.5,1,IF(T4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="51"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="50"/>
-    <tableColumn id="24" name="VitP" dataDxfId="49"/>
-    <tableColumn id="25" name="Modify" dataDxfId="48"/>
-    <tableColumn id="9" name="Def" dataDxfId="47"/>
-    <tableColumn id="10" name="Mag" dataDxfId="46"/>
-    <tableColumn id="32" name="Spd" dataDxfId="45"/>
-    <tableColumn id="35" name="Hit" dataDxfId="44"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="43"/>
-    <tableColumn id="34" name="Crt" dataDxfId="42"/>
-    <tableColumn id="33" name="Luk" dataDxfId="41"/>
-    <tableColumn id="7" name="Sum" dataDxfId="40">
+    <tableColumn id="12" name="Cost" dataDxfId="50"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="49"/>
+    <tableColumn id="24" name="VitP" dataDxfId="48"/>
+    <tableColumn id="25" name="Modify" dataDxfId="47"/>
+    <tableColumn id="9" name="Def" dataDxfId="46"/>
+    <tableColumn id="10" name="Mag" dataDxfId="45"/>
+    <tableColumn id="32" name="Spd" dataDxfId="44"/>
+    <tableColumn id="35" name="Hit" dataDxfId="43"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="42"/>
+    <tableColumn id="34" name="Crt" dataDxfId="41"/>
+    <tableColumn id="33" name="Luk" dataDxfId="40"/>
+    <tableColumn id="7" name="Sum" dataDxfId="39">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AW4)+2.5*SUM(AI4:AM4)+AH4/100+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="39"/>
-    <tableColumn id="14" name="Mov" dataDxfId="38"/>
-    <tableColumn id="60" name="LifeTime" dataDxfId="37"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="36"/>
-    <tableColumn id="18" name="Skills" dataDxfId="35"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="34"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="33"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="32"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="31"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="30"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="29"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="28"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="27"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="0">
+    <tableColumn id="13" name="Range" dataDxfId="38"/>
+    <tableColumn id="14" name="Mov" dataDxfId="37"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="36"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="35"/>
+    <tableColumn id="18" name="Skills" dataDxfId="34"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="33"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="32"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="31"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="30"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="29"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="28"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="27"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="26"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="26"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="25"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="24"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="23"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="22"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="21">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="20"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="19"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="18"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="17"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="16"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="15"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="14"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="11">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="13"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="12"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
-    <tableColumn id="20" name="Res" dataDxfId="9"/>
-    <tableColumn id="21" name="Icon" dataDxfId="8"/>
-    <tableColumn id="17" name="Cover" dataDxfId="7"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="6"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="5"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="4"/>
-    <tableColumn id="29" name="Remark" dataDxfId="3"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
+    <tableColumn id="20" name="Res" dataDxfId="7"/>
+    <tableColumn id="21" name="Icon" dataDxfId="6"/>
+    <tableColumn id="17" name="Cover" dataDxfId="5"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
+    <tableColumn id="29" name="Remark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -22597,10 +22605,10 @@
   <dimension ref="A1:BF312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AG197" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BF202" sqref="BF202"/>
+      <selection pane="bottomRight" activeCell="W312" sqref="W312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -22876,7 +22884,7 @@
         <v>1141</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1417</v>
+        <v>1423</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -23052,7 +23060,7 @@
         <v>1143</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1418</v>
+        <v>1424</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -23160,7 +23168,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="14.25">
+    <row r="4" spans="1:58" ht="14.25" hidden="1">
       <c r="A4">
         <v>51000001</v>
       </c>
@@ -23324,7 +23332,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="5" spans="1:58" ht="14.25">
+    <row r="5" spans="1:58" ht="14.25" hidden="1">
       <c r="A5">
         <v>51000002</v>
       </c>
@@ -23498,7 +23506,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="6" spans="1:58" ht="14.25">
+    <row r="6" spans="1:58" ht="14.25" hidden="1">
       <c r="A6">
         <v>51000003</v>
       </c>
@@ -23668,7 +23676,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="7" spans="1:58" ht="14.25">
+    <row r="7" spans="1:58" ht="14.25" hidden="1">
       <c r="A7">
         <v>51000004</v>
       </c>
@@ -23908,7 +23916,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="4">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>9</v>
@@ -24002,7 +24010,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="9" spans="1:58" ht="14.25">
+    <row r="9" spans="1:58" ht="14.25" hidden="1">
       <c r="A9">
         <v>51000006</v>
       </c>
@@ -24172,7 +24180,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="10" spans="1:58" ht="14.25">
+    <row r="10" spans="1:58" ht="14.25" hidden="1">
       <c r="A10">
         <v>51000007</v>
       </c>
@@ -24342,7 +24350,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="14.25">
+    <row r="11" spans="1:58" ht="14.25" hidden="1">
       <c r="A11">
         <v>51000008</v>
       </c>
@@ -24512,7 +24520,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="12" spans="1:58" ht="14.25">
+    <row r="12" spans="1:58" ht="14.25" hidden="1">
       <c r="A12">
         <v>51000009</v>
       </c>
@@ -24686,7 +24694,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="13" spans="1:58" ht="14.25">
+    <row r="13" spans="1:58" ht="14.25" hidden="1">
       <c r="A13">
         <v>51000010</v>
       </c>
@@ -24850,7 +24858,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="14" spans="1:58" ht="14.25">
+    <row r="14" spans="1:58" ht="14.25" hidden="1">
       <c r="A14">
         <v>51000011</v>
       </c>
@@ -25028,7 +25036,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="15" spans="1:58" ht="14.25">
+    <row r="15" spans="1:58" ht="14.25" hidden="1">
       <c r="A15">
         <v>51000012</v>
       </c>
@@ -25192,7 +25200,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="16" spans="1:58" ht="14.25">
+    <row r="16" spans="1:58" ht="14.25" hidden="1">
       <c r="A16">
         <v>51000013</v>
       </c>
@@ -25356,7 +25364,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="17" spans="1:58" ht="14.25">
+    <row r="17" spans="1:58" ht="14.25" hidden="1">
       <c r="A17">
         <v>51000014</v>
       </c>
@@ -25520,7 +25528,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="18" spans="1:58" ht="14.25">
+    <row r="18" spans="1:58" ht="14.25" hidden="1">
       <c r="A18">
         <v>51000015</v>
       </c>
@@ -25684,7 +25692,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="19" spans="1:58" ht="14.25">
+    <row r="19" spans="1:58" ht="14.25" hidden="1">
       <c r="A19">
         <v>51000016</v>
       </c>
@@ -25848,7 +25856,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="20" spans="1:58" ht="14.25">
+    <row r="20" spans="1:58" ht="14.25" hidden="1">
       <c r="A20">
         <v>51000017</v>
       </c>
@@ -26012,7 +26020,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="21" spans="1:58" ht="14.25">
+    <row r="21" spans="1:58" ht="14.25" hidden="1">
       <c r="A21">
         <v>51000018</v>
       </c>
@@ -26176,7 +26184,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="22" spans="1:58" ht="14.25">
+    <row r="22" spans="1:58" ht="14.25" hidden="1">
       <c r="A22">
         <v>51000019</v>
       </c>
@@ -26340,7 +26348,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="23" spans="1:58" ht="14.25">
+    <row r="23" spans="1:58" ht="14.25" hidden="1">
       <c r="A23">
         <v>51000020</v>
       </c>
@@ -26504,7 +26512,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="24" spans="1:58" ht="14.25">
+    <row r="24" spans="1:58" ht="14.25" hidden="1">
       <c r="A24">
         <v>51000021</v>
       </c>
@@ -26674,7 +26682,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="25" spans="1:58" ht="14.25">
+    <row r="25" spans="1:58" ht="14.25" hidden="1">
       <c r="A25">
         <v>51000022</v>
       </c>
@@ -26852,7 +26860,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="26" spans="1:58" ht="14.25">
+    <row r="26" spans="1:58" ht="14.25" hidden="1">
       <c r="A26">
         <v>51000023</v>
       </c>
@@ -27016,7 +27024,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="27" spans="1:58" ht="14.25">
+    <row r="27" spans="1:58" ht="14.25" hidden="1">
       <c r="A27">
         <v>51000024</v>
       </c>
@@ -27186,7 +27194,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="28" spans="1:58" ht="14.25">
+    <row r="28" spans="1:58" ht="14.25" hidden="1">
       <c r="A28">
         <v>51000025</v>
       </c>
@@ -27356,7 +27364,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="29" spans="1:58" ht="14.25">
+    <row r="29" spans="1:58" ht="14.25" hidden="1">
       <c r="A29">
         <v>51000026</v>
       </c>
@@ -27526,7 +27534,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="30" spans="1:58" ht="14.25">
+    <row r="30" spans="1:58" ht="14.25" hidden="1">
       <c r="A30">
         <v>51000027</v>
       </c>
@@ -27690,7 +27698,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="31" spans="1:58" ht="14.25">
+    <row r="31" spans="1:58" ht="14.25" hidden="1">
       <c r="A31">
         <v>51000028</v>
       </c>
@@ -27864,7 +27872,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="32" spans="1:58" ht="14.25">
+    <row r="32" spans="1:58" ht="14.25" hidden="1">
       <c r="A32">
         <v>51000029</v>
       </c>
@@ -28042,7 +28050,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="33" spans="1:58" ht="14.25">
+    <row r="33" spans="1:58" ht="14.25" hidden="1">
       <c r="A33">
         <v>51000030</v>
       </c>
@@ -28206,7 +28214,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="34" spans="1:58" ht="14.25">
+    <row r="34" spans="1:58" ht="14.25" hidden="1">
       <c r="A34">
         <v>51000031</v>
       </c>
@@ -28376,7 +28384,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="35" spans="1:58" ht="14.25">
+    <row r="35" spans="1:58" ht="14.25" hidden="1">
       <c r="A35">
         <v>51000032</v>
       </c>
@@ -28546,7 +28554,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="36" spans="1:58" ht="14.25">
+    <row r="36" spans="1:58" ht="14.25" hidden="1">
       <c r="A36">
         <v>51000033</v>
       </c>
@@ -28720,7 +28728,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="37" spans="1:58" ht="14.25">
+    <row r="37" spans="1:58" ht="14.25" hidden="1">
       <c r="A37">
         <v>51000034</v>
       </c>
@@ -28890,7 +28898,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="38" spans="1:58" ht="14.25">
+    <row r="38" spans="1:58" ht="14.25" hidden="1">
       <c r="A38">
         <v>51000035</v>
       </c>
@@ -29054,7 +29062,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="39" spans="1:58" ht="14.25">
+    <row r="39" spans="1:58" ht="14.25" hidden="1">
       <c r="A39">
         <v>51000036</v>
       </c>
@@ -29218,7 +29226,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="40" spans="1:58" ht="14.25">
+    <row r="40" spans="1:58" ht="14.25" hidden="1">
       <c r="A40">
         <v>51000037</v>
       </c>
@@ -29382,7 +29390,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="41" spans="1:58" ht="14.25">
+    <row r="41" spans="1:58" ht="14.25" hidden="1">
       <c r="A41">
         <v>51000038</v>
       </c>
@@ -29552,7 +29560,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="42" spans="1:58" ht="14.25">
+    <row r="42" spans="1:58" ht="14.25" hidden="1">
       <c r="A42">
         <v>51000039</v>
       </c>
@@ -29726,7 +29734,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="43" spans="1:58" ht="14.25">
+    <row r="43" spans="1:58" ht="14.25" hidden="1">
       <c r="A43">
         <v>51000040</v>
       </c>
@@ -29896,7 +29904,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="44" spans="1:58" ht="14.25">
+    <row r="44" spans="1:58" ht="14.25" hidden="1">
       <c r="A44">
         <v>51000041</v>
       </c>
@@ -30070,7 +30078,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="45" spans="1:58" ht="14.25">
+    <row r="45" spans="1:58" ht="14.25" hidden="1">
       <c r="A45">
         <v>51000042</v>
       </c>
@@ -30244,7 +30252,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="46" spans="1:58" ht="14.25">
+    <row r="46" spans="1:58" ht="14.25" hidden="1">
       <c r="A46">
         <v>51000043</v>
       </c>
@@ -30418,7 +30426,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="47" spans="1:58" ht="14.25">
+    <row r="47" spans="1:58" ht="14.25" hidden="1">
       <c r="A47">
         <v>51000044</v>
       </c>
@@ -30588,7 +30596,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="48" spans="1:58" ht="14.25">
+    <row r="48" spans="1:58" ht="14.25" hidden="1">
       <c r="A48">
         <v>51000045</v>
       </c>
@@ -30758,7 +30766,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="49" spans="1:58" ht="14.25">
+    <row r="49" spans="1:58" ht="14.25" hidden="1">
       <c r="A49">
         <v>51000046</v>
       </c>
@@ -30928,7 +30936,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="50" spans="1:58" ht="14.25">
+    <row r="50" spans="1:58" ht="14.25" hidden="1">
       <c r="A50">
         <v>51000047</v>
       </c>
@@ -31102,7 +31110,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="51" spans="1:58" ht="14.25">
+    <row r="51" spans="1:58" ht="14.25" hidden="1">
       <c r="A51">
         <v>51000048</v>
       </c>
@@ -31276,7 +31284,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="52" spans="1:58" ht="14.25">
+    <row r="52" spans="1:58" ht="14.25" hidden="1">
       <c r="A52">
         <v>51000049</v>
       </c>
@@ -31352,7 +31360,7 @@
         <v>9</v>
       </c>
       <c r="Y52" s="4" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="Z52" s="43">
         <v>55000084</v>
@@ -31446,7 +31454,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="53" spans="1:58" ht="14.25">
+    <row r="53" spans="1:58" ht="14.25" hidden="1">
       <c r="A53">
         <v>51000050</v>
       </c>
@@ -31616,7 +31624,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="54" spans="1:58" ht="14.25">
+    <row r="54" spans="1:58" ht="14.25" hidden="1">
       <c r="A54">
         <v>51000051</v>
       </c>
@@ -31786,7 +31794,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="55" spans="1:58" ht="14.25">
+    <row r="55" spans="1:58" ht="14.25" hidden="1">
       <c r="A55">
         <v>51000052</v>
       </c>
@@ -31956,7 +31964,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="56" spans="1:58" ht="14.25">
+    <row r="56" spans="1:58" ht="14.25" hidden="1">
       <c r="A56">
         <v>51000053</v>
       </c>
@@ -32126,7 +32134,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="57" spans="1:58" ht="14.25">
+    <row r="57" spans="1:58" ht="14.25" hidden="1">
       <c r="A57">
         <v>51000054</v>
       </c>
@@ -32300,7 +32308,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="58" spans="1:58" ht="14.25">
+    <row r="58" spans="1:58" ht="14.25" hidden="1">
       <c r="A58">
         <v>51000055</v>
       </c>
@@ -32470,7 +32478,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="59" spans="1:58" ht="14.25">
+    <row r="59" spans="1:58" ht="14.25" hidden="1">
       <c r="A59">
         <v>51000056</v>
       </c>
@@ -32640,7 +32648,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="60" spans="1:58" ht="14.25">
+    <row r="60" spans="1:58" ht="14.25" hidden="1">
       <c r="A60">
         <v>51000057</v>
       </c>
@@ -32810,7 +32818,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="61" spans="1:58" ht="14.25">
+    <row r="61" spans="1:58" ht="14.25" hidden="1">
       <c r="A61">
         <v>51000058</v>
       </c>
@@ -32980,7 +32988,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="62" spans="1:58" ht="14.25">
+    <row r="62" spans="1:58" ht="14.25" hidden="1">
       <c r="A62">
         <v>51000059</v>
       </c>
@@ -33150,7 +33158,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="63" spans="1:58" ht="14.25">
+    <row r="63" spans="1:58" ht="14.25" hidden="1">
       <c r="A63">
         <v>51000060</v>
       </c>
@@ -33320,7 +33328,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="64" spans="1:58" ht="14.25">
+    <row r="64" spans="1:58" ht="14.25" hidden="1">
       <c r="A64">
         <v>51000061</v>
       </c>
@@ -33484,7 +33492,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="65" spans="1:58" ht="14.25">
+    <row r="65" spans="1:58" ht="14.25" hidden="1">
       <c r="A65">
         <v>51000062</v>
       </c>
@@ -33648,7 +33656,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="66" spans="1:58" ht="14.25">
+    <row r="66" spans="1:58" ht="14.25" hidden="1">
       <c r="A66">
         <v>51000063</v>
       </c>
@@ -33812,7 +33820,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="67" spans="1:58" ht="14.25">
+    <row r="67" spans="1:58" ht="14.25" hidden="1">
       <c r="A67">
         <v>51000064</v>
       </c>
@@ -33986,7 +33994,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="68" spans="1:58" ht="14.25">
+    <row r="68" spans="1:58" ht="14.25" hidden="1">
       <c r="A68">
         <v>51000065</v>
       </c>
@@ -34170,7 +34178,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="69" spans="1:58" ht="14.25">
+    <row r="69" spans="1:58" ht="14.25" hidden="1">
       <c r="A69">
         <v>51000066</v>
       </c>
@@ -34348,7 +34356,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="70" spans="1:58" ht="14.25">
+    <row r="70" spans="1:58" ht="14.25" hidden="1">
       <c r="A70">
         <v>51000067</v>
       </c>
@@ -34526,7 +34534,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="71" spans="1:58" ht="14.25">
+    <row r="71" spans="1:58" ht="14.25" hidden="1">
       <c r="A71">
         <v>51000068</v>
       </c>
@@ -34700,7 +34708,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="72" spans="1:58" ht="14.25">
+    <row r="72" spans="1:58" ht="14.25" hidden="1">
       <c r="A72">
         <v>51000069</v>
       </c>
@@ -34874,7 +34882,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="73" spans="1:58" ht="14.25">
+    <row r="73" spans="1:58" ht="14.25" hidden="1">
       <c r="A73">
         <v>51000070</v>
       </c>
@@ -35048,7 +35056,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="74" spans="1:58" ht="14.25">
+    <row r="74" spans="1:58" ht="14.25" hidden="1">
       <c r="A74">
         <v>51000071</v>
       </c>
@@ -35222,7 +35230,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="75" spans="1:58" ht="14.25">
+    <row r="75" spans="1:58" ht="14.25" hidden="1">
       <c r="A75">
         <v>51000072</v>
       </c>
@@ -35396,7 +35404,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="76" spans="1:58" ht="14.25">
+    <row r="76" spans="1:58" ht="14.25" hidden="1">
       <c r="A76">
         <v>51000073</v>
       </c>
@@ -35570,7 +35578,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="77" spans="1:58" ht="14.25">
+    <row r="77" spans="1:58" ht="14.25" hidden="1">
       <c r="A77">
         <v>51000074</v>
       </c>
@@ -35740,7 +35748,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="78" spans="1:58" ht="14.25">
+    <row r="78" spans="1:58" ht="14.25" hidden="1">
       <c r="A78">
         <v>51000075</v>
       </c>
@@ -35914,7 +35922,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="79" spans="1:58" ht="14.25">
+    <row r="79" spans="1:58" ht="14.25" hidden="1">
       <c r="A79">
         <v>51000076</v>
       </c>
@@ -36078,7 +36086,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="80" spans="1:58" ht="14.25">
+    <row r="80" spans="1:58" ht="14.25" hidden="1">
       <c r="A80">
         <v>51000077</v>
       </c>
@@ -36242,7 +36250,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="81" spans="1:58" ht="14.25">
+    <row r="81" spans="1:58" ht="14.25" hidden="1">
       <c r="A81">
         <v>51000078</v>
       </c>
@@ -36416,7 +36424,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="82" spans="1:58" ht="14.25">
+    <row r="82" spans="1:58" ht="14.25" hidden="1">
       <c r="A82">
         <v>51000079</v>
       </c>
@@ -36590,7 +36598,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="83" spans="1:58" ht="14.25">
+    <row r="83" spans="1:58" ht="14.25" hidden="1">
       <c r="A83">
         <v>51000080</v>
       </c>
@@ -36764,7 +36772,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="84" spans="1:58" ht="14.25">
+    <row r="84" spans="1:58" ht="14.25" hidden="1">
       <c r="A84">
         <v>51000081</v>
       </c>
@@ -36934,7 +36942,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="85" spans="1:58" ht="14.25">
+    <row r="85" spans="1:58" ht="14.25" hidden="1">
       <c r="A85">
         <v>51000082</v>
       </c>
@@ -37112,7 +37120,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="86" spans="1:58" ht="14.25">
+    <row r="86" spans="1:58" ht="14.25" hidden="1">
       <c r="A86">
         <v>51000083</v>
       </c>
@@ -37286,7 +37294,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="87" spans="1:58" ht="14.25">
+    <row r="87" spans="1:58" ht="14.25" hidden="1">
       <c r="A87">
         <v>51000084</v>
       </c>
@@ -37460,7 +37468,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="88" spans="1:58" ht="14.25">
+    <row r="88" spans="1:58" ht="14.25" hidden="1">
       <c r="A88">
         <v>51000085</v>
       </c>
@@ -37634,7 +37642,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="89" spans="1:58" ht="14.25">
+    <row r="89" spans="1:58" ht="14.25" hidden="1">
       <c r="A89">
         <v>51000086</v>
       </c>
@@ -37808,7 +37816,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="90" spans="1:58" ht="14.25">
+    <row r="90" spans="1:58" ht="14.25" hidden="1">
       <c r="A90">
         <v>51000087</v>
       </c>
@@ -37982,7 +37990,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="91" spans="1:58" ht="14.25">
+    <row r="91" spans="1:58" ht="14.25" hidden="1">
       <c r="A91">
         <v>51000088</v>
       </c>
@@ -38156,7 +38164,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="92" spans="1:58" ht="14.25">
+    <row r="92" spans="1:58" ht="14.25" hidden="1">
       <c r="A92">
         <v>51000089</v>
       </c>
@@ -38330,7 +38338,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="93" spans="1:58" ht="14.25">
+    <row r="93" spans="1:58" ht="14.25" hidden="1">
       <c r="A93">
         <v>51000090</v>
       </c>
@@ -38504,7 +38512,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="94" spans="1:58" ht="14.25">
+    <row r="94" spans="1:58" ht="14.25" hidden="1">
       <c r="A94">
         <v>51000091</v>
       </c>
@@ -38678,7 +38686,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="95" spans="1:58" ht="14.25">
+    <row r="95" spans="1:58" ht="14.25" hidden="1">
       <c r="A95">
         <v>51000092</v>
       </c>
@@ -38852,7 +38860,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="96" spans="1:58" ht="14.25">
+    <row r="96" spans="1:58" ht="14.25" hidden="1">
       <c r="A96">
         <v>51000093</v>
       </c>
@@ -39026,7 +39034,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="97" spans="1:58" ht="14.25">
+    <row r="97" spans="1:58" ht="14.25" hidden="1">
       <c r="A97">
         <v>51000094</v>
       </c>
@@ -39204,7 +39212,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="98" spans="1:58" ht="14.25">
+    <row r="98" spans="1:58" ht="14.25" hidden="1">
       <c r="A98">
         <v>51000095</v>
       </c>
@@ -39374,7 +39382,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="99" spans="1:58" ht="14.25">
+    <row r="99" spans="1:58" ht="14.25" hidden="1">
       <c r="A99">
         <v>51000096</v>
       </c>
@@ -39548,7 +39556,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="100" spans="1:58" ht="14.25">
+    <row r="100" spans="1:58" ht="14.25" hidden="1">
       <c r="A100">
         <v>51000097</v>
       </c>
@@ -39732,7 +39740,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="101" spans="1:58" ht="14.25">
+    <row r="101" spans="1:58" ht="14.25" hidden="1">
       <c r="A101">
         <v>51000098</v>
       </c>
@@ -39906,7 +39914,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="14.25">
+    <row r="102" spans="1:58" ht="14.25" hidden="1">
       <c r="A102">
         <v>51000099</v>
       </c>
@@ -40084,7 +40092,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="103" spans="1:58" ht="14.25">
+    <row r="103" spans="1:58" ht="14.25" hidden="1">
       <c r="A103">
         <v>51000100</v>
       </c>
@@ -40254,7 +40262,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="14.25">
+    <row r="104" spans="1:58" ht="14.25" hidden="1">
       <c r="A104">
         <v>51000101</v>
       </c>
@@ -40428,7 +40436,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="14.25">
+    <row r="105" spans="1:58" ht="14.25" hidden="1">
       <c r="A105">
         <v>51000102</v>
       </c>
@@ -40602,7 +40610,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="14.25">
+    <row r="106" spans="1:58" ht="14.25" hidden="1">
       <c r="A106">
         <v>51000103</v>
       </c>
@@ -40772,7 +40780,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="107" spans="1:58" ht="14.25">
+    <row r="107" spans="1:58" ht="14.25" hidden="1">
       <c r="A107">
         <v>51000104</v>
       </c>
@@ -40942,7 +40950,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="108" spans="1:58" ht="14.25">
+    <row r="108" spans="1:58" ht="14.25" hidden="1">
       <c r="A108">
         <v>51000105</v>
       </c>
@@ -41120,7 +41128,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="14.25">
+    <row r="109" spans="1:58" ht="14.25" hidden="1">
       <c r="A109">
         <v>51000106</v>
       </c>
@@ -41290,7 +41298,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="110" spans="1:58" ht="14.25">
+    <row r="110" spans="1:58" ht="14.25" hidden="1">
       <c r="A110">
         <v>51000107</v>
       </c>
@@ -41464,7 +41472,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="111" spans="1:58" ht="14.25">
+    <row r="111" spans="1:58" ht="14.25" hidden="1">
       <c r="A111">
         <v>51000108</v>
       </c>
@@ -41634,7 +41642,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="112" spans="1:58" ht="14.25">
+    <row r="112" spans="1:58" ht="14.25" hidden="1">
       <c r="A112">
         <v>51000109</v>
       </c>
@@ -41808,7 +41816,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="113" spans="1:58" ht="14.25">
+    <row r="113" spans="1:58" ht="14.25" hidden="1">
       <c r="A113">
         <v>51000110</v>
       </c>
@@ -41982,7 +41990,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="114" spans="1:58" ht="14.25">
+    <row r="114" spans="1:58" ht="14.25" hidden="1">
       <c r="A114">
         <v>51000111</v>
       </c>
@@ -42166,7 +42174,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="115" spans="1:58" ht="14.25">
+    <row r="115" spans="1:58" ht="14.25" hidden="1">
       <c r="A115">
         <v>51000112</v>
       </c>
@@ -42350,7 +42358,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="116" spans="1:58" ht="14.25">
+    <row r="116" spans="1:58" ht="14.25" hidden="1">
       <c r="A116">
         <v>51000113</v>
       </c>
@@ -42534,7 +42542,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="117" spans="1:58" ht="14.25">
+    <row r="117" spans="1:58" ht="14.25" hidden="1">
       <c r="A117">
         <v>51000114</v>
       </c>
@@ -42708,7 +42716,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="118" spans="1:58" ht="14.25">
+    <row r="118" spans="1:58" ht="14.25" hidden="1">
       <c r="A118">
         <v>51000115</v>
       </c>
@@ -42892,7 +42900,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="119" spans="1:58" ht="14.25">
+    <row r="119" spans="1:58" ht="14.25" hidden="1">
       <c r="A119">
         <v>51000116</v>
       </c>
@@ -43076,7 +43084,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="120" spans="1:58" ht="14.25">
+    <row r="120" spans="1:58" ht="14.25" hidden="1">
       <c r="A120">
         <v>51000117</v>
       </c>
@@ -43260,7 +43268,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="121" spans="1:58" ht="14.25">
+    <row r="121" spans="1:58" ht="14.25" hidden="1">
       <c r="A121">
         <v>51000118</v>
       </c>
@@ -43444,7 +43452,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="122" spans="1:58" ht="14.25">
+    <row r="122" spans="1:58" ht="14.25" hidden="1">
       <c r="A122">
         <v>51000119</v>
       </c>
@@ -43618,7 +43626,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="123" spans="1:58" ht="14.25">
+    <row r="123" spans="1:58" ht="14.25" hidden="1">
       <c r="A123">
         <v>51000120</v>
       </c>
@@ -43796,7 +43804,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="124" spans="1:58" ht="14.25">
+    <row r="124" spans="1:58" ht="14.25" hidden="1">
       <c r="A124">
         <v>51000121</v>
       </c>
@@ -43974,7 +43982,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="125" spans="1:58" ht="14.25">
+    <row r="125" spans="1:58" ht="14.25" hidden="1">
       <c r="A125">
         <v>51000122</v>
       </c>
@@ -44152,7 +44160,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="126" spans="1:58" ht="14.25">
+    <row r="126" spans="1:58" ht="14.25" hidden="1">
       <c r="A126">
         <v>51000123</v>
       </c>
@@ -44322,7 +44330,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="127" spans="1:58" ht="14.25">
+    <row r="127" spans="1:58" ht="14.25" hidden="1">
       <c r="A127">
         <v>51000124</v>
       </c>
@@ -44492,7 +44500,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="128" spans="1:58" ht="14.25">
+    <row r="128" spans="1:58" ht="14.25" hidden="1">
       <c r="A128">
         <v>51000125</v>
       </c>
@@ -44666,7 +44674,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="129" spans="1:58" ht="14.25">
+    <row r="129" spans="1:58" ht="14.25" hidden="1">
       <c r="A129">
         <v>51000126</v>
       </c>
@@ -44840,7 +44848,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="130" spans="1:58" ht="14.25">
+    <row r="130" spans="1:58" ht="14.25" hidden="1">
       <c r="A130">
         <v>51000127</v>
       </c>
@@ -45010,7 +45018,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="131" spans="1:58" ht="14.25">
+    <row r="131" spans="1:58" ht="14.25" hidden="1">
       <c r="A131">
         <v>51000128</v>
       </c>
@@ -45180,7 +45188,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="132" spans="1:58" ht="14.25">
+    <row r="132" spans="1:58" ht="14.25" hidden="1">
       <c r="A132">
         <v>51000129</v>
       </c>
@@ -45354,7 +45362,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="133" spans="1:58" ht="14.25">
+    <row r="133" spans="1:58" ht="14.25" hidden="1">
       <c r="A133">
         <v>51000130</v>
       </c>
@@ -45528,7 +45536,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="134" spans="1:58" ht="14.25">
+    <row r="134" spans="1:58" ht="14.25" hidden="1">
       <c r="A134">
         <v>51000131</v>
       </c>
@@ -45702,7 +45710,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="135" spans="1:58" ht="14.25">
+    <row r="135" spans="1:58" ht="14.25" hidden="1">
       <c r="A135">
         <v>51000132</v>
       </c>
@@ -45876,7 +45884,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="136" spans="1:58" ht="14.25">
+    <row r="136" spans="1:58" ht="14.25" hidden="1">
       <c r="A136">
         <v>51000133</v>
       </c>
@@ -46050,7 +46058,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="137" spans="1:58" ht="14.25">
+    <row r="137" spans="1:58" ht="14.25" hidden="1">
       <c r="A137">
         <v>51000134</v>
       </c>
@@ -46228,7 +46236,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="138" spans="1:58" ht="14.25">
+    <row r="138" spans="1:58" ht="14.25" hidden="1">
       <c r="A138">
         <v>51000135</v>
       </c>
@@ -46402,7 +46410,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="139" spans="1:58" ht="14.25">
+    <row r="139" spans="1:58" ht="14.25" hidden="1">
       <c r="A139">
         <v>51000136</v>
       </c>
@@ -46576,7 +46584,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="140" spans="1:58" ht="14.25">
+    <row r="140" spans="1:58" ht="14.25" hidden="1">
       <c r="A140">
         <v>51000137</v>
       </c>
@@ -46740,7 +46748,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="141" spans="1:58" ht="14.25">
+    <row r="141" spans="1:58" ht="14.25" hidden="1">
       <c r="A141">
         <v>51000138</v>
       </c>
@@ -46914,7 +46922,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="142" spans="1:58" ht="14.25">
+    <row r="142" spans="1:58" ht="14.25" hidden="1">
       <c r="A142">
         <v>51000139</v>
       </c>
@@ -47088,7 +47096,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="143" spans="1:58" ht="14.25">
+    <row r="143" spans="1:58" ht="14.25" hidden="1">
       <c r="A143">
         <v>51000140</v>
       </c>
@@ -47262,7 +47270,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="144" spans="1:58" ht="14.25">
+    <row r="144" spans="1:58" ht="14.25" hidden="1">
       <c r="A144">
         <v>51000141</v>
       </c>
@@ -47432,7 +47440,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="145" spans="1:58" ht="14.25">
+    <row r="145" spans="1:58" ht="14.25" hidden="1">
       <c r="A145">
         <v>51000142</v>
       </c>
@@ -47596,7 +47604,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="146" spans="1:58" ht="14.25">
+    <row r="146" spans="1:58" ht="14.25" hidden="1">
       <c r="A146">
         <v>51000143</v>
       </c>
@@ -47774,7 +47782,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="147" spans="1:58" ht="14.25">
+    <row r="147" spans="1:58" ht="14.25" hidden="1">
       <c r="A147">
         <v>51000144</v>
       </c>
@@ -47948,7 +47956,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="148" spans="1:58" ht="14.25">
+    <row r="148" spans="1:58" ht="14.25" hidden="1">
       <c r="A148">
         <v>51000145</v>
       </c>
@@ -48122,7 +48130,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="149" spans="1:58" ht="14.25">
+    <row r="149" spans="1:58" ht="14.25" hidden="1">
       <c r="A149">
         <v>51000146</v>
       </c>
@@ -48300,7 +48308,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="150" spans="1:58" ht="14.25">
+    <row r="150" spans="1:58" ht="14.25" hidden="1">
       <c r="A150">
         <v>51000147</v>
       </c>
@@ -48478,7 +48486,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="151" spans="1:58" ht="14.25">
+    <row r="151" spans="1:58" ht="14.25" hidden="1">
       <c r="A151">
         <v>51000148</v>
       </c>
@@ -48648,7 +48656,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="152" spans="1:58" ht="14.25">
+    <row r="152" spans="1:58" ht="14.25" hidden="1">
       <c r="A152">
         <v>51000149</v>
       </c>
@@ -48812,7 +48820,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="153" spans="1:58" ht="14.25">
+    <row r="153" spans="1:58" ht="14.25" hidden="1">
       <c r="A153">
         <v>51000150</v>
       </c>
@@ -48982,7 +48990,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="154" spans="1:58" ht="14.25">
+    <row r="154" spans="1:58" ht="14.25" hidden="1">
       <c r="A154">
         <v>51000151</v>
       </c>
@@ -49152,7 +49160,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="155" spans="1:58" ht="14.25">
+    <row r="155" spans="1:58" ht="14.25" hidden="1">
       <c r="A155">
         <v>51000152</v>
       </c>
@@ -49322,7 +49330,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="156" spans="1:58" ht="14.25">
+    <row r="156" spans="1:58" ht="14.25" hidden="1">
       <c r="A156">
         <v>51000153</v>
       </c>
@@ -49492,7 +49500,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="157" spans="1:58" ht="14.25">
+    <row r="157" spans="1:58" ht="14.25" hidden="1">
       <c r="A157">
         <v>51000154</v>
       </c>
@@ -49656,7 +49664,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="158" spans="1:58" ht="14.25">
+    <row r="158" spans="1:58" ht="14.25" hidden="1">
       <c r="A158">
         <v>51000155</v>
       </c>
@@ -49826,7 +49834,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="159" spans="1:58" ht="14.25">
+    <row r="159" spans="1:58" ht="14.25" hidden="1">
       <c r="A159">
         <v>51000156</v>
       </c>
@@ -50000,7 +50008,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="160" spans="1:58" ht="14.25">
+    <row r="160" spans="1:58" ht="14.25" hidden="1">
       <c r="A160">
         <v>51000157</v>
       </c>
@@ -50174,7 +50182,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="161" spans="1:58" ht="14.25">
+    <row r="161" spans="1:58" ht="14.25" hidden="1">
       <c r="A161">
         <v>51000158</v>
       </c>
@@ -50338,7 +50346,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="162" spans="1:58" ht="14.25">
+    <row r="162" spans="1:58" ht="14.25" hidden="1">
       <c r="A162">
         <v>51000159</v>
       </c>
@@ -50508,7 +50516,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="163" spans="1:58" ht="14.25">
+    <row r="163" spans="1:58" ht="14.25" hidden="1">
       <c r="A163">
         <v>51000160</v>
       </c>
@@ -50678,7 +50686,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="164" spans="1:58" ht="14.25">
+    <row r="164" spans="1:58" ht="14.25" hidden="1">
       <c r="A164">
         <v>51000161</v>
       </c>
@@ -50852,7 +50860,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="165" spans="1:58" ht="14.25">
+    <row r="165" spans="1:58" ht="14.25" hidden="1">
       <c r="A165">
         <v>51000162</v>
       </c>
@@ -51030,7 +51038,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="166" spans="1:58" ht="14.25">
+    <row r="166" spans="1:58" ht="14.25" hidden="1">
       <c r="A166">
         <v>51000163</v>
       </c>
@@ -51204,7 +51212,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="167" spans="1:58" ht="14.25">
+    <row r="167" spans="1:58" ht="14.25" hidden="1">
       <c r="A167">
         <v>51000164</v>
       </c>
@@ -51378,7 +51386,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="168" spans="1:58" ht="14.25">
+    <row r="168" spans="1:58" ht="14.25" hidden="1">
       <c r="A168">
         <v>51000165</v>
       </c>
@@ -51556,7 +51564,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="169" spans="1:58" ht="14.25">
+    <row r="169" spans="1:58" ht="14.25" hidden="1">
       <c r="A169">
         <v>51000166</v>
       </c>
@@ -51726,7 +51734,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="170" spans="1:58" ht="14.25">
+    <row r="170" spans="1:58" ht="14.25" hidden="1">
       <c r="A170">
         <v>51000167</v>
       </c>
@@ -51896,7 +51904,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="171" spans="1:58" ht="14.25">
+    <row r="171" spans="1:58" ht="14.25" hidden="1">
       <c r="A171">
         <v>51000168</v>
       </c>
@@ -52078,7 +52086,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="172" spans="1:58" ht="14.25">
+    <row r="172" spans="1:58" ht="14.25" hidden="1">
       <c r="A172">
         <v>51000169</v>
       </c>
@@ -52256,7 +52264,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="173" spans="1:58" ht="14.25">
+    <row r="173" spans="1:58" ht="14.25" hidden="1">
       <c r="A173">
         <v>51000170</v>
       </c>
@@ -52430,7 +52438,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="174" spans="1:58" ht="14.25">
+    <row r="174" spans="1:58" ht="14.25" hidden="1">
       <c r="A174">
         <v>51000171</v>
       </c>
@@ -52600,7 +52608,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="175" spans="1:58" ht="14.25">
+    <row r="175" spans="1:58" ht="14.25" hidden="1">
       <c r="A175">
         <v>51000172</v>
       </c>
@@ -52770,7 +52778,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="176" spans="1:58" ht="14.25">
+    <row r="176" spans="1:58" ht="14.25" hidden="1">
       <c r="A176">
         <v>51000173</v>
       </c>
@@ -52940,7 +52948,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="177" spans="1:58" ht="14.25">
+    <row r="177" spans="1:58" ht="14.25" hidden="1">
       <c r="A177">
         <v>51000174</v>
       </c>
@@ -53114,7 +53122,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="178" spans="1:58" ht="14.25">
+    <row r="178" spans="1:58" ht="14.25" hidden="1">
       <c r="A178">
         <v>51000175</v>
       </c>
@@ -53288,7 +53296,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="179" spans="1:58" ht="14.25">
+    <row r="179" spans="1:58" ht="14.25" hidden="1">
       <c r="A179">
         <v>51000176</v>
       </c>
@@ -53458,7 +53466,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="180" spans="1:58" ht="14.25">
+    <row r="180" spans="1:58" ht="14.25" hidden="1">
       <c r="A180">
         <v>51000177</v>
       </c>
@@ -53640,7 +53648,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="181" spans="1:58" ht="14.25">
+    <row r="181" spans="1:58" ht="14.25" hidden="1">
       <c r="A181">
         <v>51000178</v>
       </c>
@@ -53818,7 +53826,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="182" spans="1:58" ht="14.25">
+    <row r="182" spans="1:58" ht="14.25" hidden="1">
       <c r="A182">
         <v>51000179</v>
       </c>
@@ -53992,7 +54000,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="183" spans="1:58" ht="14.25">
+    <row r="183" spans="1:58" ht="14.25" hidden="1">
       <c r="A183">
         <v>51000180</v>
       </c>
@@ -54166,7 +54174,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="184" spans="1:58" ht="14.25">
+    <row r="184" spans="1:58" ht="14.25" hidden="1">
       <c r="A184">
         <v>51000181</v>
       </c>
@@ -54336,7 +54344,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="185" spans="1:58" ht="14.25">
+    <row r="185" spans="1:58" ht="14.25" hidden="1">
       <c r="A185">
         <v>51000182</v>
       </c>
@@ -54510,7 +54518,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="186" spans="1:58" ht="14.25">
+    <row r="186" spans="1:58" ht="14.25" hidden="1">
       <c r="A186">
         <v>51000183</v>
       </c>
@@ -54684,7 +54692,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="187" spans="1:58" ht="14.25">
+    <row r="187" spans="1:58" ht="14.25" hidden="1">
       <c r="A187">
         <v>51000184</v>
       </c>
@@ -54854,7 +54862,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="188" spans="1:58" ht="14.25">
+    <row r="188" spans="1:58" ht="14.25" hidden="1">
       <c r="A188">
         <v>51000185</v>
       </c>
@@ -55032,7 +55040,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="189" spans="1:58" ht="14.25">
+    <row r="189" spans="1:58" ht="14.25" hidden="1">
       <c r="A189">
         <v>51000186</v>
       </c>
@@ -55202,7 +55210,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="190" spans="1:58" ht="14.25">
+    <row r="190" spans="1:58" ht="14.25" hidden="1">
       <c r="A190">
         <v>51000187</v>
       </c>
@@ -55366,7 +55374,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="191" spans="1:58" ht="14.25">
+    <row r="191" spans="1:58" ht="14.25" hidden="1">
       <c r="A191">
         <v>51000188</v>
       </c>
@@ -55540,7 +55548,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="192" spans="1:58" ht="14.25">
+    <row r="192" spans="1:58" ht="14.25" hidden="1">
       <c r="A192">
         <v>51000189</v>
       </c>
@@ -55718,7 +55726,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="193" spans="1:58" ht="14.25">
+    <row r="193" spans="1:58" ht="14.25" hidden="1">
       <c r="A193">
         <v>51000190</v>
       </c>
@@ -55896,7 +55904,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="194" spans="1:58" ht="14.25">
+    <row r="194" spans="1:58" ht="14.25" hidden="1">
       <c r="A194">
         <v>51000191</v>
       </c>
@@ -56074,7 +56082,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="195" spans="1:58" ht="14.25">
+    <row r="195" spans="1:58" ht="14.25" hidden="1">
       <c r="A195">
         <v>51000192</v>
       </c>
@@ -56256,7 +56264,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="196" spans="1:58" ht="14.25">
+    <row r="196" spans="1:58" ht="14.25" hidden="1">
       <c r="A196">
         <v>51000193</v>
       </c>
@@ -56430,7 +56438,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="197" spans="1:58" ht="14.25">
+    <row r="197" spans="1:58" ht="14.25" hidden="1">
       <c r="A197">
         <v>51000194</v>
       </c>
@@ -56608,7 +56616,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="198" spans="1:58" ht="14.25">
+    <row r="198" spans="1:58" ht="14.25" hidden="1">
       <c r="A198">
         <v>51000195</v>
       </c>
@@ -56786,7 +56794,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="199" spans="1:58" ht="14.25">
+    <row r="199" spans="1:58" ht="14.25" hidden="1">
       <c r="A199">
         <v>51000196</v>
       </c>
@@ -56964,7 +56972,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="200" spans="1:58" ht="14.25">
+    <row r="200" spans="1:58" ht="14.25" hidden="1">
       <c r="A200">
         <v>51000197</v>
       </c>
@@ -57142,7 +57150,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="201" spans="1:58" ht="14.25">
+    <row r="201" spans="1:58" ht="14.25" hidden="1">
       <c r="A201">
         <v>51000198</v>
       </c>
@@ -57382,13 +57390,13 @@
         <v>0</v>
       </c>
       <c r="W202" s="4">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="X202" s="4" t="s">
         <v>1168</v>
       </c>
       <c r="Y202" s="4" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="Z202" s="43">
         <v>55000203</v>
@@ -57480,7 +57488,7 @@
       </c>
       <c r="BF202" s="22"/>
     </row>
-    <row r="203" spans="1:58" ht="14.25">
+    <row r="203" spans="1:58" ht="14.25" hidden="1">
       <c r="A203">
         <v>51000200</v>
       </c>
@@ -57654,7 +57662,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="204" spans="1:58" ht="14.25">
+    <row r="204" spans="1:58" ht="14.25" hidden="1">
       <c r="A204">
         <v>51000201</v>
       </c>
@@ -57828,7 +57836,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="205" spans="1:58" ht="14.25">
+    <row r="205" spans="1:58" ht="14.25" hidden="1">
       <c r="A205">
         <v>51000202</v>
       </c>
@@ -57998,7 +58006,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="206" spans="1:58" ht="14.25">
+    <row r="206" spans="1:58" ht="14.25" hidden="1">
       <c r="A206">
         <v>51000203</v>
       </c>
@@ -58172,7 +58180,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="207" spans="1:58" ht="14.25">
+    <row r="207" spans="1:58" ht="14.25" hidden="1">
       <c r="A207">
         <v>51000204</v>
       </c>
@@ -58342,7 +58350,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="208" spans="1:58" ht="14.25">
+    <row r="208" spans="1:58" ht="14.25" hidden="1">
       <c r="A208">
         <v>51000205</v>
       </c>
@@ -58516,7 +58524,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="209" spans="1:58" ht="14.25">
+    <row r="209" spans="1:58" ht="14.25" hidden="1">
       <c r="A209">
         <v>51000206</v>
       </c>
@@ -58686,7 +58694,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="210" spans="1:58" ht="14.25">
+    <row r="210" spans="1:58" ht="14.25" hidden="1">
       <c r="A210">
         <v>51000207</v>
       </c>
@@ -58860,7 +58868,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="211" spans="1:58" ht="14.25">
+    <row r="211" spans="1:58" ht="14.25" hidden="1">
       <c r="A211">
         <v>51000208</v>
       </c>
@@ -59038,7 +59046,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="212" spans="1:58" ht="14.25">
+    <row r="212" spans="1:58" ht="14.25" hidden="1">
       <c r="A212">
         <v>51000209</v>
       </c>
@@ -59212,7 +59220,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="213" spans="1:58" ht="14.25">
+    <row r="213" spans="1:58" ht="14.25" hidden="1">
       <c r="A213">
         <v>51000210</v>
       </c>
@@ -59390,7 +59398,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="214" spans="1:58" ht="14.25">
+    <row r="214" spans="1:58" ht="14.25" hidden="1">
       <c r="A214">
         <v>51000211</v>
       </c>
@@ -59568,7 +59576,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="215" spans="1:58" ht="14.25">
+    <row r="215" spans="1:58" ht="14.25" hidden="1">
       <c r="A215">
         <v>51000212</v>
       </c>
@@ -59750,7 +59758,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="216" spans="1:58" ht="14.25">
+    <row r="216" spans="1:58" ht="14.25" hidden="1">
       <c r="A216">
         <v>51000213</v>
       </c>
@@ -59920,7 +59928,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="217" spans="1:58" ht="14.25">
+    <row r="217" spans="1:58" ht="14.25" hidden="1">
       <c r="A217">
         <v>51000214</v>
       </c>
@@ -60094,7 +60102,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="218" spans="1:58" ht="14.25">
+    <row r="218" spans="1:58" ht="14.25" hidden="1">
       <c r="A218">
         <v>51000215</v>
       </c>
@@ -60268,7 +60276,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="219" spans="1:58" ht="14.25">
+    <row r="219" spans="1:58" ht="14.25" hidden="1">
       <c r="A219">
         <v>51000216</v>
       </c>
@@ -60442,7 +60450,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="220" spans="1:58" ht="14.25">
+    <row r="220" spans="1:58" ht="14.25" hidden="1">
       <c r="A220">
         <v>51000217</v>
       </c>
@@ -60612,7 +60620,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="221" spans="1:58" ht="14.25">
+    <row r="221" spans="1:58" ht="14.25" hidden="1">
       <c r="A221">
         <v>51000218</v>
       </c>
@@ -60786,7 +60794,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="222" spans="1:58" ht="14.25">
+    <row r="222" spans="1:58" ht="14.25" hidden="1">
       <c r="A222">
         <v>51000219</v>
       </c>
@@ -60956,7 +60964,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="223" spans="1:58" ht="14.25">
+    <row r="223" spans="1:58" ht="14.25" hidden="1">
       <c r="A223">
         <v>51000220</v>
       </c>
@@ -61126,7 +61134,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="224" spans="1:58" ht="14.25">
+    <row r="224" spans="1:58" ht="14.25" hidden="1">
       <c r="A224">
         <v>51000221</v>
       </c>
@@ -61300,7 +61308,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="225" spans="1:58" ht="14.25">
+    <row r="225" spans="1:58" ht="14.25" hidden="1">
       <c r="A225">
         <v>51000222</v>
       </c>
@@ -61474,7 +61482,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="226" spans="1:58" ht="14.25">
+    <row r="226" spans="1:58" ht="14.25" hidden="1">
       <c r="A226">
         <v>51000223</v>
       </c>
@@ -61652,7 +61660,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="227" spans="1:58" ht="14.25">
+    <row r="227" spans="1:58" ht="14.25" hidden="1">
       <c r="A227">
         <v>51000224</v>
       </c>
@@ -61826,7 +61834,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="228" spans="1:58" ht="14.25">
+    <row r="228" spans="1:58" ht="14.25" hidden="1">
       <c r="A228">
         <v>51000225</v>
       </c>
@@ -62000,7 +62008,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="229" spans="1:58" ht="14.25">
+    <row r="229" spans="1:58" ht="14.25" hidden="1">
       <c r="A229">
         <v>51000226</v>
       </c>
@@ -62174,7 +62182,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="230" spans="1:58" ht="14.25">
+    <row r="230" spans="1:58" ht="14.25" hidden="1">
       <c r="A230">
         <v>51000227</v>
       </c>
@@ -62344,7 +62352,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="231" spans="1:58" ht="14.25">
+    <row r="231" spans="1:58" ht="14.25" hidden="1">
       <c r="A231">
         <v>51000228</v>
       </c>
@@ -62514,7 +62522,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="232" spans="1:58" ht="14.25">
+    <row r="232" spans="1:58" ht="14.25" hidden="1">
       <c r="A232">
         <v>51000229</v>
       </c>
@@ -62678,7 +62686,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="233" spans="1:58" ht="14.25">
+    <row r="233" spans="1:58" ht="14.25" hidden="1">
       <c r="A233">
         <v>51000230</v>
       </c>
@@ -62848,7 +62856,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="234" spans="1:58" ht="14.25">
+    <row r="234" spans="1:58" ht="14.25" hidden="1">
       <c r="A234">
         <v>51000231</v>
       </c>
@@ -63022,7 +63030,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="235" spans="1:58" ht="14.25">
+    <row r="235" spans="1:58" ht="14.25" hidden="1">
       <c r="A235">
         <v>51000232</v>
       </c>
@@ -63196,7 +63204,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="236" spans="1:58" ht="14.25">
+    <row r="236" spans="1:58" ht="14.25" hidden="1">
       <c r="A236">
         <v>51000233</v>
       </c>
@@ -63370,7 +63378,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="237" spans="1:58" ht="14.25">
+    <row r="237" spans="1:58" ht="14.25" hidden="1">
       <c r="A237">
         <v>51000234</v>
       </c>
@@ -63552,7 +63560,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="238" spans="1:58" ht="14.25">
+    <row r="238" spans="1:58" ht="14.25" hidden="1">
       <c r="A238">
         <v>51000235</v>
       </c>
@@ -63726,7 +63734,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="239" spans="1:58" ht="14.25">
+    <row r="239" spans="1:58" ht="14.25" hidden="1">
       <c r="A239">
         <v>51000236</v>
       </c>
@@ -63900,7 +63908,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="240" spans="1:58" ht="14.25">
+    <row r="240" spans="1:58" ht="14.25" hidden="1">
       <c r="A240">
         <v>51000237</v>
       </c>
@@ -64074,7 +64082,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="241" spans="1:58" ht="14.25">
+    <row r="241" spans="1:58" ht="14.25" hidden="1">
       <c r="A241">
         <v>51000238</v>
       </c>
@@ -64256,7 +64264,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="242" spans="1:58" ht="14.25">
+    <row r="242" spans="1:58" ht="14.25" hidden="1">
       <c r="A242">
         <v>51000239</v>
       </c>
@@ -64430,7 +64438,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="243" spans="1:58" ht="14.25">
+    <row r="243" spans="1:58" ht="14.25" hidden="1">
       <c r="A243">
         <v>51000240</v>
       </c>
@@ -64608,7 +64616,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="244" spans="1:58" ht="14.25">
+    <row r="244" spans="1:58" ht="14.25" hidden="1">
       <c r="A244">
         <v>51000241</v>
       </c>
@@ -64782,7 +64790,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="245" spans="1:58" ht="14.25">
+    <row r="245" spans="1:58" ht="14.25" hidden="1">
       <c r="A245">
         <v>51000242</v>
       </c>
@@ -64964,7 +64972,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="246" spans="1:58" ht="14.25">
+    <row r="246" spans="1:58" ht="14.25" hidden="1">
       <c r="A246">
         <v>51000243</v>
       </c>
@@ -65134,7 +65142,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="247" spans="1:58" ht="14.25">
+    <row r="247" spans="1:58" ht="14.25" hidden="1">
       <c r="A247">
         <v>51000244</v>
       </c>
@@ -65312,7 +65320,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="248" spans="1:58" ht="14.25">
+    <row r="248" spans="1:58" ht="14.25" hidden="1">
       <c r="A248">
         <v>51000245</v>
       </c>
@@ -65482,7 +65490,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="249" spans="1:58" ht="14.25">
+    <row r="249" spans="1:58" ht="14.25" hidden="1">
       <c r="A249">
         <v>51000246</v>
       </c>
@@ -65656,7 +65664,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="250" spans="1:58" ht="14.25">
+    <row r="250" spans="1:58" ht="14.25" hidden="1">
       <c r="A250">
         <v>51000247</v>
       </c>
@@ -65834,7 +65842,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="251" spans="1:58" ht="14.25">
+    <row r="251" spans="1:58" ht="14.25" hidden="1">
       <c r="A251">
         <v>51000248</v>
       </c>
@@ -66008,7 +66016,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="252" spans="1:58" ht="14.25">
+    <row r="252" spans="1:58" ht="14.25" hidden="1">
       <c r="A252">
         <v>51000249</v>
       </c>
@@ -66186,7 +66194,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="253" spans="1:58" ht="14.25">
+    <row r="253" spans="1:58" ht="14.25" hidden="1">
       <c r="A253">
         <v>51000250</v>
       </c>
@@ -66360,7 +66368,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="254" spans="1:58" ht="14.25">
+    <row r="254" spans="1:58" ht="14.25" hidden="1">
       <c r="A254">
         <v>51000251</v>
       </c>
@@ -66534,7 +66542,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="255" spans="1:58" ht="14.25">
+    <row r="255" spans="1:58" ht="14.25" hidden="1">
       <c r="A255">
         <v>51000252</v>
       </c>
@@ -66708,7 +66716,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="256" spans="1:58" ht="14.25">
+    <row r="256" spans="1:58" ht="14.25" hidden="1">
       <c r="A256">
         <v>51000253</v>
       </c>
@@ -66882,7 +66890,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="257" spans="1:58" ht="14.25">
+    <row r="257" spans="1:58" ht="14.25" hidden="1">
       <c r="A257">
         <v>51000254</v>
       </c>
@@ -67056,7 +67064,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="258" spans="1:58" ht="14.25">
+    <row r="258" spans="1:58" ht="14.25" hidden="1">
       <c r="A258">
         <v>51000255</v>
       </c>
@@ -67230,7 +67238,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="259" spans="1:58" ht="14.25">
+    <row r="259" spans="1:58" ht="14.25" hidden="1">
       <c r="A259">
         <v>51000256</v>
       </c>
@@ -67404,7 +67412,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="260" spans="1:58" ht="14.25">
+    <row r="260" spans="1:58" ht="14.25" hidden="1">
       <c r="A260">
         <v>51000257</v>
       </c>
@@ -67578,7 +67586,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="261" spans="1:58" ht="14.25">
+    <row r="261" spans="1:58" ht="14.25" hidden="1">
       <c r="A261">
         <v>51000258</v>
       </c>
@@ -67752,7 +67760,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="262" spans="1:58" ht="14.25">
+    <row r="262" spans="1:58" ht="14.25" hidden="1">
       <c r="A262">
         <v>51000259</v>
       </c>
@@ -67922,7 +67930,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="263" spans="1:58" ht="14.25">
+    <row r="263" spans="1:58" ht="14.25" hidden="1">
       <c r="A263">
         <v>51000260</v>
       </c>
@@ -68086,7 +68094,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="264" spans="1:58" ht="14.25">
+    <row r="264" spans="1:58" ht="14.25" hidden="1">
       <c r="A264">
         <v>51000261</v>
       </c>
@@ -68260,7 +68268,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="265" spans="1:58" ht="14.25">
+    <row r="265" spans="1:58" ht="14.25" hidden="1">
       <c r="A265">
         <v>51000262</v>
       </c>
@@ -68438,7 +68446,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="266" spans="1:58" ht="14.25">
+    <row r="266" spans="1:58" ht="14.25" hidden="1">
       <c r="A266">
         <v>51000263</v>
       </c>
@@ -68616,7 +68624,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="267" spans="1:58" ht="14.25">
+    <row r="267" spans="1:58" ht="14.25" hidden="1">
       <c r="A267">
         <v>51000264</v>
       </c>
@@ -68794,7 +68802,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="268" spans="1:58" ht="14.25">
+    <row r="268" spans="1:58" ht="14.25" hidden="1">
       <c r="A268">
         <v>51000265</v>
       </c>
@@ -68968,7 +68976,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="269" spans="1:58" ht="14.25">
+    <row r="269" spans="1:58" ht="14.25" hidden="1">
       <c r="A269">
         <v>51000266</v>
       </c>
@@ -69138,7 +69146,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="270" spans="1:58" ht="14.25">
+    <row r="270" spans="1:58" ht="14.25" hidden="1">
       <c r="A270">
         <v>51000267</v>
       </c>
@@ -69312,7 +69320,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="271" spans="1:58" ht="14.25">
+    <row r="271" spans="1:58" ht="14.25" hidden="1">
       <c r="A271">
         <v>51000268</v>
       </c>
@@ -69490,7 +69498,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="272" spans="1:58" ht="14.25">
+    <row r="272" spans="1:58" ht="14.25" hidden="1">
       <c r="A272">
         <v>51000269</v>
       </c>
@@ -69668,7 +69676,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="273" spans="1:58" ht="14.25">
+    <row r="273" spans="1:58" ht="14.25" hidden="1">
       <c r="A273">
         <v>51000270</v>
       </c>
@@ -69846,7 +69854,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="274" spans="1:58" ht="14.25">
+    <row r="274" spans="1:58" ht="14.25" hidden="1">
       <c r="A274">
         <v>51000271</v>
       </c>
@@ -70016,7 +70024,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="275" spans="1:58" ht="14.25">
+    <row r="275" spans="1:58" ht="14.25" hidden="1">
       <c r="A275">
         <v>51000272</v>
       </c>
@@ -70190,7 +70198,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="276" spans="1:58" ht="14.25">
+    <row r="276" spans="1:58" ht="14.25" hidden="1">
       <c r="A276">
         <v>51000273</v>
       </c>
@@ -70362,7 +70370,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="277" spans="1:58" ht="14.25">
+    <row r="277" spans="1:58" ht="14.25" hidden="1">
       <c r="A277">
         <v>51000274</v>
       </c>
@@ -70536,7 +70544,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="278" spans="1:58" ht="14.25">
+    <row r="278" spans="1:58" ht="14.25" hidden="1">
       <c r="A278">
         <v>51000275</v>
       </c>
@@ -70710,7 +70718,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="279" spans="1:58" ht="14.25">
+    <row r="279" spans="1:58" ht="14.25" hidden="1">
       <c r="A279">
         <v>51000276</v>
       </c>
@@ -70880,7 +70888,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="280" spans="1:58" ht="14.25">
+    <row r="280" spans="1:58" ht="14.25" hidden="1">
       <c r="A280">
         <v>51000277</v>
       </c>
@@ -71054,7 +71062,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="281" spans="1:58" ht="14.25">
+    <row r="281" spans="1:58" ht="14.25" hidden="1">
       <c r="A281">
         <v>51000278</v>
       </c>
@@ -71224,7 +71232,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="282" spans="1:58" ht="14.25">
+    <row r="282" spans="1:58" ht="14.25" hidden="1">
       <c r="A282">
         <v>51000279</v>
       </c>
@@ -71394,7 +71402,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="283" spans="1:58" ht="14.25">
+    <row r="283" spans="1:58" ht="14.25" hidden="1">
       <c r="A283">
         <v>51000280</v>
       </c>
@@ -71564,7 +71572,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="284" spans="1:58" ht="14.25">
+    <row r="284" spans="1:58" ht="14.25" hidden="1">
       <c r="A284">
         <v>51000281</v>
       </c>
@@ -71738,7 +71746,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="285" spans="1:58" ht="14.25">
+    <row r="285" spans="1:58" ht="14.25" hidden="1">
       <c r="A285">
         <v>51000282</v>
       </c>
@@ -71912,7 +71920,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="286" spans="1:58" ht="14.25">
+    <row r="286" spans="1:58" ht="14.25" hidden="1">
       <c r="A286">
         <v>51000283</v>
       </c>
@@ -72076,7 +72084,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="287" spans="1:58" ht="14.25">
+    <row r="287" spans="1:58" ht="14.25" hidden="1">
       <c r="A287">
         <v>51000284</v>
       </c>
@@ -72250,7 +72258,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="288" spans="1:58" ht="14.25">
+    <row r="288" spans="1:58" ht="14.25" hidden="1">
       <c r="A288">
         <v>51000285</v>
       </c>
@@ -72424,7 +72432,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="289" spans="1:58" ht="14.25">
+    <row r="289" spans="1:58" ht="14.25" hidden="1">
       <c r="A289">
         <v>51000286</v>
       </c>
@@ -72594,7 +72602,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="290" spans="1:58" ht="14.25">
+    <row r="290" spans="1:58" ht="14.25" hidden="1">
       <c r="A290">
         <v>51000287</v>
       </c>
@@ -72764,7 +72772,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="291" spans="1:58" ht="14.25">
+    <row r="291" spans="1:58" ht="14.25" hidden="1">
       <c r="A291">
         <v>51000288</v>
       </c>
@@ -72938,7 +72946,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="292" spans="1:58" ht="14.25">
+    <row r="292" spans="1:58" ht="14.25" hidden="1">
       <c r="A292">
         <v>51000289</v>
       </c>
@@ -73112,7 +73120,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="293" spans="1:58" ht="14.25">
+    <row r="293" spans="1:58" ht="14.25" hidden="1">
       <c r="A293">
         <v>51000290</v>
       </c>
@@ -73282,7 +73290,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="294" spans="1:58" ht="14.25">
+    <row r="294" spans="1:58" ht="14.25" hidden="1">
       <c r="A294">
         <v>51000291</v>
       </c>
@@ -73460,7 +73468,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="295" spans="1:58" ht="14.25">
+    <row r="295" spans="1:58" ht="14.25" hidden="1">
       <c r="A295">
         <v>51000292</v>
       </c>
@@ -73630,7 +73638,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="296" spans="1:58" ht="14.25">
+    <row r="296" spans="1:58" ht="14.25" hidden="1">
       <c r="A296">
         <v>51000293</v>
       </c>
@@ -73804,7 +73812,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="297" spans="1:58" ht="14.25">
+    <row r="297" spans="1:58" ht="14.25" hidden="1">
       <c r="A297">
         <v>51000294</v>
       </c>
@@ -73982,7 +73990,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="298" spans="1:58" ht="14.25">
+    <row r="298" spans="1:58" ht="14.25" hidden="1">
       <c r="A298">
         <v>51000295</v>
       </c>
@@ -74156,7 +74164,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="299" spans="1:58" ht="14.25">
+    <row r="299" spans="1:58" ht="14.25" hidden="1">
       <c r="A299">
         <v>51000296</v>
       </c>
@@ -74326,7 +74334,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="300" spans="1:58" ht="14.25">
+    <row r="300" spans="1:58" ht="14.25" hidden="1">
       <c r="A300">
         <v>51000297</v>
       </c>
@@ -74496,7 +74504,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="301" spans="1:58" ht="14.25">
+    <row r="301" spans="1:58" ht="14.25" hidden="1">
       <c r="A301">
         <v>51000298</v>
       </c>
@@ -74678,7 +74686,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="302" spans="1:58" ht="14.25">
+    <row r="302" spans="1:58" ht="14.25" hidden="1">
       <c r="A302">
         <v>51000299</v>
       </c>
@@ -74852,7 +74860,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="303" spans="1:58" ht="14.25">
+    <row r="303" spans="1:58" ht="14.25" hidden="1">
       <c r="A303">
         <v>51000300</v>
       </c>
@@ -75026,7 +75034,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="304" spans="1:58" ht="14.25">
+    <row r="304" spans="1:58" ht="14.25" hidden="1">
       <c r="A304">
         <v>51000301</v>
       </c>
@@ -75196,7 +75204,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="305" spans="1:58" ht="14.25">
+    <row r="305" spans="1:58" ht="14.25" hidden="1">
       <c r="A305">
         <v>51000302</v>
       </c>
@@ -75366,7 +75374,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="306" spans="1:58" ht="14.25">
+    <row r="306" spans="1:58" ht="14.25" hidden="1">
       <c r="A306">
         <v>51000303</v>
       </c>
@@ -75540,7 +75548,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="307" spans="1:58" ht="14.25">
+    <row r="307" spans="1:58" ht="14.25" hidden="1">
       <c r="A307">
         <v>51000304</v>
       </c>
@@ -75710,7 +75718,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="308" spans="1:58" ht="14.25">
+    <row r="308" spans="1:58" ht="14.25" hidden="1">
       <c r="A308">
         <v>51000305</v>
       </c>
@@ -75874,7 +75882,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="309" spans="1:58" ht="14.25">
+    <row r="309" spans="1:58" ht="14.25" hidden="1">
       <c r="A309">
         <v>51000306</v>
       </c>
@@ -76038,7 +76046,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="310" spans="1:58" ht="14.25">
+    <row r="310" spans="1:58" ht="14.25" hidden="1">
       <c r="A310">
         <v>51000307</v>
       </c>
@@ -76202,7 +76210,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="311" spans="1:58" ht="14.25">
+    <row r="311" spans="1:58" ht="14.25" hidden="1">
       <c r="A311">
         <v>51000308</v>
       </c>
@@ -76371,10 +76379,10 @@
         <v>51000309</v>
       </c>
       <c r="B312" s="11" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D312" s="8" t="s">
         <v>698</v>
@@ -76436,13 +76444,13 @@
         <v>0</v>
       </c>
       <c r="W312" s="11">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="X312" s="11" t="s">
         <v>9</v>
       </c>
       <c r="Y312" s="11" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="Z312" s="21">
         <v>55000300</v>
@@ -76533,7 +76541,7 @@
         <v>0.40819670000000002</v>
       </c>
       <c r="BF312" s="11" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
   </sheetData>
@@ -76604,10 +76612,10 @@
   <dimension ref="A1:BF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH4" sqref="AH4"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -76882,7 +76890,7 @@
         <v>295</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1417</v>
+        <v>1423</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -77058,7 +77066,7 @@
         <v>1143</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1418</v>
+        <v>1424</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -78481,31 +78489,31 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4:K7 K10:K11">
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="70" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J7">
-    <cfRule type="cellIs" dxfId="69" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="68" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="9" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78523,13 +78531,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="66" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="5" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="65" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78547,13 +78555,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
close #22 FINISH  gardon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="1429">
   <si>
     <t>arrow</t>
   </si>
@@ -5510,10 +5510,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000084;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>55000203;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5543,6 +5539,10 @@
   </si>
   <si>
     <t>55000344;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55000084;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -11219,7 +11219,7 @@
             <v>55000084</v>
           </cell>
           <cell r="V71">
-            <v>10</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="72">
@@ -13083,7 +13083,7 @@
             <v>55000344</v>
           </cell>
           <cell r="V304">
-            <v>5</v>
+            <v>40</v>
           </cell>
         </row>
       </sheetData>
@@ -22593,10 +22593,10 @@
   <dimension ref="A1:BF313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B303" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z313" sqref="Z313"/>
+      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -22872,7 +22872,7 @@
         <v>1141</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -23048,7 +23048,7 @@
         <v>1143</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -27921,7 +27921,7 @@
       </c>
       <c r="T32" s="15">
         <f t="shared" si="1"/>
-        <v>18.399999999999999</v>
+        <v>53.4</v>
       </c>
       <c r="U32" s="4">
         <v>10</v>
@@ -27963,7 +27963,7 @@
 IF(ISBLANK($AB32),0, LOOKUP($AB32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC32/100)+
 IF(ISBLANK($AD32),0, LOOKUP($AD32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE32/100)+
 IF(ISBLANK($AF32),0, LOOKUP($AF32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG32/100)</f>
-        <v>11.4</v>
+        <v>46.4</v>
       </c>
       <c r="AI32" s="21">
         <v>0</v>
@@ -31122,7 +31122,7 @@
       </c>
       <c r="H51" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I51" s="4">
         <v>1</v>
@@ -31159,7 +31159,7 @@
       </c>
       <c r="T51" s="15">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="U51" s="4">
         <v>10</v>
@@ -31197,7 +31197,7 @@
 IF(ISBLANK($AB51),0, LOOKUP($AB51,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC51/100)+
 IF(ISBLANK($AD51),0, LOOKUP($AD51,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE51/100)+
 IF(ISBLANK($AF51),0, LOOKUP($AF51,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG51/100)</f>
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="AI51" s="21">
         <v>0</v>
@@ -31286,7 +31286,7 @@
         <v>722</v>
       </c>
       <c r="E52" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F52" s="4">
         <v>0</v>
@@ -31296,19 +31296,19 @@
       </c>
       <c r="H52" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I52" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J52" s="4">
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="K52" s="4">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="L52" s="4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M52" s="4">
         <v>0</v>
@@ -31333,7 +31333,7 @@
       </c>
       <c r="T52" s="15">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="U52" s="4">
         <v>10</v>
@@ -31348,7 +31348,7 @@
         <v>9</v>
       </c>
       <c r="Y52" s="4" t="s">
-        <v>1420</v>
+        <v>1428</v>
       </c>
       <c r="Z52" s="43">
         <v>55000084</v>
@@ -31367,7 +31367,7 @@
 IF(ISBLANK($AB52),0, LOOKUP($AB52,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC52/100)+
 IF(ISBLANK($AD52),0, LOOKUP($AD52,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE52/100)+
 IF(ISBLANK($AF52),0, LOOKUP($AF52,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG52/100)</f>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="AI52" s="21">
         <v>0</v>
@@ -31438,9 +31438,7 @@
       <c r="BE52" s="30">
         <v>0.2377049</v>
       </c>
-      <c r="BF52" s="22" t="s">
-        <v>1174</v>
-      </c>
+      <c r="BF52" s="22"/>
     </row>
     <row r="53" spans="1:58" ht="14.25">
       <c r="A53">
@@ -36647,7 +36645,7 @@
       </c>
       <c r="T83" s="15">
         <f t="shared" si="5"/>
-        <v>36.32</v>
+        <v>71.319999999999993</v>
       </c>
       <c r="U83" s="4">
         <v>10</v>
@@ -36685,7 +36683,7 @@
 IF(ISBLANK($AB83),0, LOOKUP($AB83,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC83/100)+
 IF(ISBLANK($AD83),0, LOOKUP($AD83,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE83/100)+
 IF(ISBLANK($AF83),0, LOOKUP($AF83,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG83/100)</f>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="AI83" s="21">
         <v>0</v>
@@ -36991,7 +36989,7 @@
       </c>
       <c r="T85" s="15">
         <f t="shared" si="5"/>
-        <v>29.5</v>
+        <v>64.5</v>
       </c>
       <c r="U85" s="4">
         <v>10</v>
@@ -37033,7 +37031,7 @@
 IF(ISBLANK($AB85),0, LOOKUP($AB85,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC85/100)+
 IF(ISBLANK($AD85),0, LOOKUP($AD85,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE85/100)+
 IF(ISBLANK($AF85),0, LOOKUP($AF85,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG85/100)</f>
-        <v>6.5</v>
+        <v>41.5</v>
       </c>
       <c r="AI85" s="21">
         <v>0</v>
@@ -39083,7 +39081,7 @@
       </c>
       <c r="T97" s="15">
         <f t="shared" si="5"/>
-        <v>51.6</v>
+        <v>86.6</v>
       </c>
       <c r="U97" s="4">
         <v>10</v>
@@ -39125,7 +39123,7 @@
 IF(ISBLANK($AB97),0, LOOKUP($AB97,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC97/100)+
 IF(ISBLANK($AD97),0, LOOKUP($AD97,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE97/100)+
 IF(ISBLANK($AF97),0, LOOKUP($AF97,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG97/100)</f>
-        <v>7.6</v>
+        <v>42.6</v>
       </c>
       <c r="AI97" s="21">
         <v>0</v>
@@ -39789,7 +39787,7 @@
       </c>
       <c r="T101" s="15">
         <f t="shared" si="5"/>
-        <v>18.8</v>
+        <v>53.8</v>
       </c>
       <c r="U101" s="4">
         <v>10</v>
@@ -39827,7 +39825,7 @@
 IF(ISBLANK($AB101),0, LOOKUP($AB101,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC101/100)+
 IF(ISBLANK($AD101),0, LOOKUP($AD101,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE101/100)+
 IF(ISBLANK($AF101),0, LOOKUP($AF101,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG101/100)</f>
-        <v>5.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AI101" s="21">
         <v>0</v>
@@ -41691,7 +41689,7 @@
       </c>
       <c r="T112" s="15">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="U112" s="4">
         <v>40</v>
@@ -41729,7 +41727,7 @@
 IF(ISBLANK($AB112),0, LOOKUP($AB112,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC112/100)+
 IF(ISBLANK($AD112),0, LOOKUP($AD112,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE112/100)+
 IF(ISBLANK($AF112),0, LOOKUP($AF112,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG112/100)</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="AI112" s="21">
         <v>0</v>
@@ -41865,7 +41863,7 @@
       </c>
       <c r="T113" s="15">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="U113" s="4">
         <v>35</v>
@@ -41903,7 +41901,7 @@
 IF(ISBLANK($AB113),0, LOOKUP($AB113,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC113/100)+
 IF(ISBLANK($AD113),0, LOOKUP($AD113,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE113/100)+
 IF(ISBLANK($AF113),0, LOOKUP($AF113,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG113/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI113" s="21">
         <v>0</v>
@@ -42591,7 +42589,7 @@
       </c>
       <c r="T117" s="15">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="U117" s="4">
         <v>10</v>
@@ -42629,7 +42627,7 @@
 IF(ISBLANK($AB117),0, LOOKUP($AB117,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC117/100)+
 IF(ISBLANK($AD117),0, LOOKUP($AD117,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE117/100)+
 IF(ISBLANK($AF117),0, LOOKUP($AF117,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG117/100)</f>
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="AI117" s="21">
         <v>0</v>
@@ -43464,7 +43462,7 @@
       </c>
       <c r="H122" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I122" s="4">
         <v>2</v>
@@ -43501,7 +43499,7 @@
       </c>
       <c r="T122" s="15">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>33</v>
       </c>
       <c r="U122" s="4">
         <v>10</v>
@@ -43539,7 +43537,7 @@
 IF(ISBLANK($AB122),0, LOOKUP($AB122,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC122/100)+
 IF(ISBLANK($AD122),0, LOOKUP($AD122,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE122/100)+
 IF(ISBLANK($AF122),0, LOOKUP($AF122,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG122/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI122" s="21">
         <v>0</v>
@@ -43638,7 +43636,7 @@
       </c>
       <c r="H123" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I123" s="4">
         <v>2</v>
@@ -43675,7 +43673,7 @@
       </c>
       <c r="T123" s="15">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>74.5</v>
       </c>
       <c r="U123" s="4">
         <v>10</v>
@@ -43717,7 +43715,7 @@
 IF(ISBLANK($AB123),0, LOOKUP($AB123,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC123/100)+
 IF(ISBLANK($AD123),0, LOOKUP($AD123,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE123/100)+
 IF(ISBLANK($AF123),0, LOOKUP($AF123,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG123/100)</f>
-        <v>11.5</v>
+        <v>81.5</v>
       </c>
       <c r="AI123" s="21">
         <v>0</v>
@@ -43853,7 +43851,7 @@
       </c>
       <c r="T124" s="15">
         <f t="shared" si="5"/>
-        <v>10.8</v>
+        <v>45.8</v>
       </c>
       <c r="U124" s="4">
         <v>10</v>
@@ -43895,7 +43893,7 @@
 IF(ISBLANK($AB124),0, LOOKUP($AB124,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC124/100)+
 IF(ISBLANK($AD124),0, LOOKUP($AD124,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE124/100)+
 IF(ISBLANK($AF124),0, LOOKUP($AF124,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG124/100)</f>
-        <v>5.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AI124" s="21">
         <v>0</v>
@@ -44031,7 +44029,7 @@
       </c>
       <c r="T125" s="15">
         <f t="shared" si="5"/>
-        <v>20.8</v>
+        <v>55.8</v>
       </c>
       <c r="U125" s="4">
         <v>10</v>
@@ -44073,7 +44071,7 @@
 IF(ISBLANK($AB125),0, LOOKUP($AB125,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC125/100)+
 IF(ISBLANK($AD125),0, LOOKUP($AD125,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE125/100)+
 IF(ISBLANK($AF125),0, LOOKUP($AF125,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG125/100)</f>
-        <v>5.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AI125" s="21">
         <v>0</v>
@@ -44512,7 +44510,7 @@
       </c>
       <c r="H128" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I128" s="4">
         <v>1</v>
@@ -44549,7 +44547,7 @@
       </c>
       <c r="T128" s="15">
         <f t="shared" si="5"/>
-        <v>9.75</v>
+        <v>44.75</v>
       </c>
       <c r="U128" s="4">
         <v>10</v>
@@ -44587,7 +44585,7 @@
 IF(ISBLANK($AB128),0, LOOKUP($AB128,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC128/100)+
 IF(ISBLANK($AD128),0, LOOKUP($AD128,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE128/100)+
 IF(ISBLANK($AF128),0, LOOKUP($AF128,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG128/100)</f>
-        <v>5.75</v>
+        <v>40.75</v>
       </c>
       <c r="AI128" s="21">
         <v>0</v>
@@ -45759,7 +45757,7 @@
       </c>
       <c r="T135" s="15">
         <f t="shared" si="9"/>
-        <v>26.92</v>
+        <v>61.92</v>
       </c>
       <c r="U135" s="4">
         <v>10</v>
@@ -45797,7 +45795,7 @@
 IF(ISBLANK($AB135),0, LOOKUP($AB135,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC135/100)+
 IF(ISBLANK($AD135),0, LOOKUP($AD135,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE135/100)+
 IF(ISBLANK($AF135),0, LOOKUP($AF135,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG135/100)</f>
-        <v>6.6</v>
+        <v>41.6</v>
       </c>
       <c r="AI135" s="21">
         <v>0</v>
@@ -46285,7 +46283,7 @@
       </c>
       <c r="T138" s="15">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="U138" s="4">
         <v>10</v>
@@ -46323,7 +46321,7 @@
 IF(ISBLANK($AB138),0, LOOKUP($AB138,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC138/100)+
 IF(ISBLANK($AD138),0, LOOKUP($AD138,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE138/100)+
 IF(ISBLANK($AF138),0, LOOKUP($AF138,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG138/100)</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="AI138" s="21">
         <v>0</v>
@@ -46459,7 +46457,7 @@
       </c>
       <c r="T139" s="15">
         <f t="shared" si="9"/>
-        <v>40.799999999999997</v>
+        <v>75.8</v>
       </c>
       <c r="U139" s="4">
         <v>10</v>
@@ -46497,7 +46495,7 @@
 IF(ISBLANK($AB139),0, LOOKUP($AB139,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC139/100)+
 IF(ISBLANK($AD139),0, LOOKUP($AD139,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE139/100)+
 IF(ISBLANK($AF139),0, LOOKUP($AF139,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG139/100)</f>
-        <v>7.8</v>
+        <v>42.8</v>
       </c>
       <c r="AI139" s="21">
         <v>0</v>
@@ -46971,7 +46969,7 @@
       </c>
       <c r="T142" s="15">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="U142" s="4">
         <v>10</v>
@@ -47009,7 +47007,7 @@
 IF(ISBLANK($AB142),0, LOOKUP($AB142,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC142/100)+
 IF(ISBLANK($AD142),0, LOOKUP($AD142,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE142/100)+
 IF(ISBLANK($AF142),0, LOOKUP($AF142,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG142/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI142" s="21">
         <v>0</v>
@@ -47653,7 +47651,7 @@
       </c>
       <c r="T146" s="15">
         <f t="shared" si="9"/>
-        <v>27.32</v>
+        <v>62.319999999999993</v>
       </c>
       <c r="U146" s="4">
         <v>10</v>
@@ -47695,7 +47693,7 @@
 IF(ISBLANK($AB146),0, LOOKUP($AB146,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC146/100)+
 IF(ISBLANK($AD146),0, LOOKUP($AD146,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE146/100)+
 IF(ISBLANK($AF146),0, LOOKUP($AF146,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG146/100)</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="AI146" s="21">
         <v>0</v>
@@ -48320,7 +48318,7 @@
       </c>
       <c r="H150" s="4">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I150" s="4">
         <v>4</v>
@@ -48357,7 +48355,7 @@
       </c>
       <c r="T150" s="15">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="U150" s="4">
         <v>10</v>
@@ -48399,7 +48397,7 @@
 IF(ISBLANK($AB150),0, LOOKUP($AB150,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC150/100)+
 IF(ISBLANK($AD150),0, LOOKUP($AD150,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE150/100)+
 IF(ISBLANK($AF150),0, LOOKUP($AF150,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG150/100)</f>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="AI150" s="21">
         <v>0</v>
@@ -49883,7 +49881,7 @@
       </c>
       <c r="T159" s="15">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="U159" s="4">
         <v>10</v>
@@ -49921,7 +49919,7 @@
 IF(ISBLANK($AB159),0, LOOKUP($AB159,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC159/100)+
 IF(ISBLANK($AD159),0, LOOKUP($AD159,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE159/100)+
 IF(ISBLANK($AF159),0, LOOKUP($AF159,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG159/100)</f>
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="AI159" s="21">
         <v>0</v>
@@ -51916,7 +51914,7 @@
       </c>
       <c r="H171" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I171" s="4">
         <v>1</v>
@@ -51953,7 +51951,7 @@
       </c>
       <c r="T171" s="15">
         <f t="shared" si="9"/>
-        <v>-4</v>
+        <v>31</v>
       </c>
       <c r="U171" s="4">
         <v>10</v>
@@ -51999,7 +51997,7 @@
 IF(ISBLANK($AB171),0, LOOKUP($AB171,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC171/100)+
 IF(ISBLANK($AD171),0, LOOKUP($AD171,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE171/100)+
 IF(ISBLANK($AF171),0, LOOKUP($AF171,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG171/100)</f>
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="AI171" s="21">
         <v>0</v>
@@ -52135,7 +52133,7 @@
       </c>
       <c r="T172" s="15">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="U172" s="4">
         <v>10</v>
@@ -52177,7 +52175,7 @@
 IF(ISBLANK($AB172),0, LOOKUP($AB172,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC172/100)+
 IF(ISBLANK($AD172),0, LOOKUP($AD172,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE172/100)+
 IF(ISBLANK($AF172),0, LOOKUP($AF172,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG172/100)</f>
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="AI172" s="21">
         <v>0</v>
@@ -53515,7 +53513,7 @@
       </c>
       <c r="T180" s="15">
         <f t="shared" si="9"/>
-        <v>22.2</v>
+        <v>57.2</v>
       </c>
       <c r="U180" s="4">
         <v>10</v>
@@ -53561,7 +53559,7 @@
 IF(ISBLANK($AB180),0, LOOKUP($AB180,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC180/100)+
 IF(ISBLANK($AD180),0, LOOKUP($AD180,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE180/100)+
 IF(ISBLANK($AF180),0, LOOKUP($AF180,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG180/100)</f>
-        <v>8.1999999999999993</v>
+        <v>43.2</v>
       </c>
       <c r="AI180" s="21">
         <v>0</v>
@@ -53875,7 +53873,7 @@
       </c>
       <c r="T182" s="15">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="U182" s="4">
         <v>10</v>
@@ -53913,7 +53911,7 @@
 IF(ISBLANK($AB182),0, LOOKUP($AB182,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC182/100)+
 IF(ISBLANK($AD182),0, LOOKUP($AD182,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE182/100)+
 IF(ISBLANK($AF182),0, LOOKUP($AF182,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG182/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI182" s="21">
         <v>0</v>
@@ -54567,7 +54565,7 @@
       </c>
       <c r="T186" s="15">
         <f t="shared" si="9"/>
-        <v>37.32</v>
+        <v>72.319999999999993</v>
       </c>
       <c r="U186" s="4">
         <v>10</v>
@@ -54605,7 +54603,7 @@
 IF(ISBLANK($AB186),0, LOOKUP($AB186,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC186/100)+
 IF(ISBLANK($AD186),0, LOOKUP($AD186,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE186/100)+
 IF(ISBLANK($AF186),0, LOOKUP($AF186,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG186/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI186" s="21">
         <v>0</v>
@@ -54874,7 +54872,7 @@
       </c>
       <c r="H188" s="4">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I188" s="4">
         <v>5</v>
@@ -54911,7 +54909,7 @@
       </c>
       <c r="T188" s="15">
         <f t="shared" si="9"/>
-        <v>-25.8</v>
+        <v>9.2000000000000028</v>
       </c>
       <c r="U188" s="4">
         <v>10</v>
@@ -54953,7 +54951,7 @@
 IF(ISBLANK($AB188),0, LOOKUP($AB188,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC188/100)+
 IF(ISBLANK($AD188),0, LOOKUP($AD188,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE188/100)+
 IF(ISBLANK($AF188),0, LOOKUP($AF188,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG188/100)</f>
-        <v>7.2</v>
+        <v>42.2</v>
       </c>
       <c r="AI188" s="21">
         <v>0</v>
@@ -56094,7 +56092,7 @@
       </c>
       <c r="H195" s="4">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I195" s="4">
         <v>5</v>
@@ -56131,7 +56129,7 @@
       </c>
       <c r="T195" s="15">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="U195" s="4">
         <v>30</v>
@@ -56177,7 +56175,7 @@
 IF(ISBLANK($AB195),0, LOOKUP($AB195,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC195/100)+
 IF(ISBLANK($AD195),0, LOOKUP($AD195,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE195/100)+
 IF(ISBLANK($AF195),0, LOOKUP($AF195,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG195/100)</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="AI195" s="21">
         <v>0</v>
@@ -57384,7 +57382,7 @@
         <v>1168</v>
       </c>
       <c r="Y202" s="4" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="Z202" s="43">
         <v>55000203</v>
@@ -59447,7 +59445,7 @@
       </c>
       <c r="T214" s="15">
         <f t="shared" si="13"/>
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="U214" s="4">
         <v>10</v>
@@ -59489,7 +59487,7 @@
 IF(ISBLANK($AB214),0, LOOKUP($AB214,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC214/100)+
 IF(ISBLANK($AD214),0, LOOKUP($AD214,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE214/100)+
 IF(ISBLANK($AF214),0, LOOKUP($AF214,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG214/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI214" s="21">
         <v>0</v>
@@ -61494,7 +61492,7 @@
       </c>
       <c r="H226" s="4">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I226" s="4">
         <v>1</v>
@@ -61531,7 +61529,7 @@
       </c>
       <c r="T226" s="15">
         <f t="shared" si="13"/>
-        <v>-22</v>
+        <v>13</v>
       </c>
       <c r="U226" s="4">
         <v>10</v>
@@ -61573,7 +61571,7 @@
 IF(ISBLANK($AB226),0, LOOKUP($AB226,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC226/100)+
 IF(ISBLANK($AD226),0, LOOKUP($AD226,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE226/100)+
 IF(ISBLANK($AF226),0, LOOKUP($AF226,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG226/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI226" s="21">
         <v>0</v>
@@ -63427,7 +63425,7 @@
       </c>
       <c r="T237" s="15">
         <f t="shared" si="13"/>
-        <v>26.5</v>
+        <v>61.5</v>
       </c>
       <c r="U237" s="4">
         <v>10</v>
@@ -63473,7 +63471,7 @@
 IF(ISBLANK($AB237),0, LOOKUP($AB237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC237/100)+
 IF(ISBLANK($AD237),0, LOOKUP($AD237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE237/100)+
 IF(ISBLANK($AF237),0, LOOKUP($AF237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG237/100)</f>
-        <v>13.5</v>
+        <v>48.5</v>
       </c>
       <c r="AI237" s="21">
         <v>0</v>
@@ -63572,7 +63570,7 @@
       </c>
       <c r="H238" s="4">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I238" s="4">
         <v>2</v>
@@ -63609,7 +63607,7 @@
       </c>
       <c r="T238" s="15">
         <f t="shared" si="13"/>
-        <v>7.8000000000000007</v>
+        <v>42.8</v>
       </c>
       <c r="U238" s="4">
         <v>10</v>
@@ -63647,7 +63645,7 @@
 IF(ISBLANK($AB238),0, LOOKUP($AB238,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC238/100)+
 IF(ISBLANK($AD238),0, LOOKUP($AD238,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE238/100)+
 IF(ISBLANK($AF238),0, LOOKUP($AF238,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG238/100)</f>
-        <v>6.8</v>
+        <v>41.8</v>
       </c>
       <c r="AI238" s="21">
         <v>0</v>
@@ -64665,7 +64663,7 @@
       </c>
       <c r="T244" s="15">
         <f t="shared" si="13"/>
-        <v>28.5</v>
+        <v>63.5</v>
       </c>
       <c r="U244" s="4">
         <v>10</v>
@@ -64703,7 +64701,7 @@
 IF(ISBLANK($AB244),0, LOOKUP($AB244,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC244/100)+
 IF(ISBLANK($AD244),0, LOOKUP($AD244,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE244/100)+
 IF(ISBLANK($AF244),0, LOOKUP($AF244,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG244/100)</f>
-        <v>7.5</v>
+        <v>42.5</v>
       </c>
       <c r="AI244" s="21">
         <v>0</v>
@@ -64802,7 +64800,7 @@
       </c>
       <c r="H245" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I245" s="4">
         <v>6</v>
@@ -64839,7 +64837,7 @@
       </c>
       <c r="T245" s="15">
         <f t="shared" si="13"/>
-        <v>-2.5</v>
+        <v>32.5</v>
       </c>
       <c r="U245" s="4">
         <v>10</v>
@@ -64885,7 +64883,7 @@
 IF(ISBLANK($AB245),0, LOOKUP($AB245,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC245/100)+
 IF(ISBLANK($AD245),0, LOOKUP($AD245,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE245/100)+
 IF(ISBLANK($AF245),0, LOOKUP($AF245,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG245/100)</f>
-        <v>7.5</v>
+        <v>42.5</v>
       </c>
       <c r="AI245" s="21">
         <v>0</v>
@@ -65191,7 +65189,7 @@
       </c>
       <c r="T247" s="15">
         <f t="shared" si="13"/>
-        <v>33.700000000000003</v>
+        <v>68.7</v>
       </c>
       <c r="U247" s="4">
         <v>10</v>
@@ -65233,7 +65231,7 @@
 IF(ISBLANK($AB247),0, LOOKUP($AB247,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC247/100)+
 IF(ISBLANK($AD247),0, LOOKUP($AD247,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE247/100)+
 IF(ISBLANK($AF247),0, LOOKUP($AF247,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG247/100)</f>
-        <v>9.6999999999999993</v>
+        <v>44.7</v>
       </c>
       <c r="AI247" s="21">
         <v>0</v>
@@ -66728,7 +66726,7 @@
       </c>
       <c r="H256" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I256" s="4">
         <v>4</v>
@@ -66765,7 +66763,7 @@
       </c>
       <c r="T256" s="15">
         <f t="shared" si="13"/>
-        <v>-5.2</v>
+        <v>29.799999999999997</v>
       </c>
       <c r="U256" s="4">
         <v>10</v>
@@ -66803,7 +66801,7 @@
 IF(ISBLANK($AB256),0, LOOKUP($AB256,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC256/100)+
 IF(ISBLANK($AD256),0, LOOKUP($AD256,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE256/100)+
 IF(ISBLANK($AF256),0, LOOKUP($AF256,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG256/100)</f>
-        <v>6.8</v>
+        <v>41.8</v>
       </c>
       <c r="AI256" s="21">
         <v>0</v>
@@ -68143,7 +68141,7 @@
       </c>
       <c r="T264" s="15">
         <f t="shared" si="17"/>
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="U264" s="4">
         <v>10</v>
@@ -68181,7 +68179,7 @@
 IF(ISBLANK($AB264),0, LOOKUP($AB264,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC264/100)+
 IF(ISBLANK($AD264),0, LOOKUP($AD264,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE264/100)+
 IF(ISBLANK($AF264),0, LOOKUP($AF264,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG264/100)</f>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="AI264" s="21">
         <v>0</v>
@@ -68317,7 +68315,7 @@
       </c>
       <c r="T265" s="15">
         <f t="shared" si="17"/>
-        <v>27.4</v>
+        <v>62.400000000000006</v>
       </c>
       <c r="U265" s="4">
         <v>10</v>
@@ -68359,7 +68357,7 @@
 IF(ISBLANK($AB265),0, LOOKUP($AB265,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC265/100)+
 IF(ISBLANK($AD265),0, LOOKUP($AD265,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE265/100)+
 IF(ISBLANK($AF265),0, LOOKUP($AF265,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG265/100)</f>
-        <v>9.4</v>
+        <v>44.4</v>
       </c>
       <c r="AI265" s="21">
         <v>0</v>
@@ -68851,7 +68849,7 @@
       </c>
       <c r="T268" s="15">
         <f t="shared" si="17"/>
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="U268" s="4">
         <v>10</v>
@@ -68889,7 +68887,7 @@
 IF(ISBLANK($AB268),0, LOOKUP($AB268,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC268/100)+
 IF(ISBLANK($AD268),0, LOOKUP($AD268,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE268/100)+
 IF(ISBLANK($AF268),0, LOOKUP($AF268,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG268/100)</f>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="AI268" s="21">
         <v>0</v>
@@ -72270,7 +72268,7 @@
       </c>
       <c r="H288" s="4">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I288" s="4">
         <v>2</v>
@@ -72307,7 +72305,7 @@
       </c>
       <c r="T288" s="15">
         <f t="shared" si="17"/>
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="U288" s="4">
         <v>10</v>
@@ -72345,7 +72343,7 @@
 IF(ISBLANK($AB288),0, LOOKUP($AB288,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC288/100)+
 IF(ISBLANK($AD288),0, LOOKUP($AD288,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE288/100)+
 IF(ISBLANK($AF288),0, LOOKUP($AF288,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG288/100)</f>
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="AI288" s="21">
         <v>0</v>
@@ -73687,7 +73685,7 @@
       </c>
       <c r="T296" s="15">
         <f t="shared" si="17"/>
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="U296" s="4">
         <v>10</v>
@@ -73725,7 +73723,7 @@
 IF(ISBLANK($AB296),0, LOOKUP($AB296,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC296/100)+
 IF(ISBLANK($AD296),0, LOOKUP($AD296,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE296/100)+
 IF(ISBLANK($AF296),0, LOOKUP($AF296,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG296/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI296" s="21">
         <v>0</v>
@@ -73824,7 +73822,7 @@
       </c>
       <c r="H297" s="4">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I297" s="4">
         <v>3</v>
@@ -73861,7 +73859,7 @@
       </c>
       <c r="T297" s="15">
         <f t="shared" si="17"/>
-        <v>-13.25</v>
+        <v>21.75</v>
       </c>
       <c r="U297" s="4">
         <v>30</v>
@@ -73903,7 +73901,7 @@
 IF(ISBLANK($AB297),0, LOOKUP($AB297,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC297/100)+
 IF(ISBLANK($AD297),0, LOOKUP($AD297,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE297/100)+
 IF(ISBLANK($AF297),0, LOOKUP($AF297,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG297/100)</f>
-        <v>7.75</v>
+        <v>42.75</v>
       </c>
       <c r="AI297" s="21">
         <v>0</v>
@@ -74002,7 +74000,7 @@
       </c>
       <c r="H298" s="4">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I298" s="4">
         <v>1</v>
@@ -74039,7 +74037,7 @@
       </c>
       <c r="T298" s="15">
         <f t="shared" si="17"/>
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="U298" s="4">
         <v>10</v>
@@ -74077,7 +74075,7 @@
 IF(ISBLANK($AB298),0, LOOKUP($AB298,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC298/100)+
 IF(ISBLANK($AD298),0, LOOKUP($AD298,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE298/100)+
 IF(ISBLANK($AF298),0, LOOKUP($AF298,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG298/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI298" s="21">
         <v>0</v>
@@ -74553,7 +74551,7 @@
       </c>
       <c r="T301" s="15">
         <f t="shared" si="17"/>
-        <v>33.700000000000003</v>
+        <v>68.7</v>
       </c>
       <c r="U301" s="4">
         <v>10</v>
@@ -74599,7 +74597,7 @@
 IF(ISBLANK($AB301),0, LOOKUP($AB301,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC301/100)+
 IF(ISBLANK($AD301),0, LOOKUP($AD301,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE301/100)+
 IF(ISBLANK($AF301),0, LOOKUP($AF301,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG301/100)</f>
-        <v>7.7</v>
+        <v>42.7</v>
       </c>
       <c r="AI301" s="21">
         <v>0</v>
@@ -74698,7 +74696,7 @@
       </c>
       <c r="H302" s="4">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I302" s="4">
         <v>3</v>
@@ -74735,7 +74733,7 @@
       </c>
       <c r="T302" s="15">
         <f t="shared" si="17"/>
-        <v>6.5</v>
+        <v>41.5</v>
       </c>
       <c r="U302" s="4">
         <v>30</v>
@@ -74773,7 +74771,7 @@
 IF(ISBLANK($AB302),0, LOOKUP($AB302,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC302/100)+
 IF(ISBLANK($AD302),0, LOOKUP($AD302,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE302/100)+
 IF(ISBLANK($AF302),0, LOOKUP($AF302,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG302/100)</f>
-        <v>9.5</v>
+        <v>44.5</v>
       </c>
       <c r="AI302" s="21">
         <v>0</v>
@@ -74872,7 +74870,7 @@
       </c>
       <c r="H303" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I303" s="11">
         <v>1</v>
@@ -74909,7 +74907,7 @@
       </c>
       <c r="T303" s="24">
         <f t="shared" si="17"/>
-        <v>-6</v>
+        <v>29</v>
       </c>
       <c r="U303" s="4">
         <v>10</v>
@@ -74947,7 +74945,7 @@
 IF(ISBLANK($AB303),0, LOOKUP($AB303,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC303/100)+
 IF(ISBLANK($AD303),0, LOOKUP($AD303,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE303/100)+
 IF(ISBLANK($AF303),0, LOOKUP($AF303,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG303/100)</f>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="AI303" s="21">
         <v>0</v>
@@ -76438,7 +76436,7 @@
         <v>9</v>
       </c>
       <c r="Y312" s="11" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="Z312" s="21">
         <v>55000300</v>
@@ -76537,13 +76535,13 @@
         <v>51000310</v>
       </c>
       <c r="B313" s="11" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C313" s="11" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D313" s="8" t="s">
         <v>1426</v>
-      </c>
-      <c r="C313" s="11" t="s">
-        <v>1425</v>
-      </c>
-      <c r="D313" s="8" t="s">
-        <v>1427</v>
       </c>
       <c r="E313" s="11">
         <v>6</v>
@@ -76556,13 +76554,13 @@
       </c>
       <c r="H313" s="24">
         <f t="shared" ref="H313" si="20">IF(T313&gt;10,5,IF(T313&gt;5,4,IF(T313&gt;2.5,3,IF(T313&gt;0,2,IF(T313&gt;-2.5,1,IF(T313&gt;-10,0,6))))))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I313" s="11">
         <v>6</v>
       </c>
       <c r="J313" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K313" s="11">
         <v>-20</v>
@@ -76577,13 +76575,13 @@
         <v>0</v>
       </c>
       <c r="O313" s="11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P313" s="11">
         <v>0</v>
       </c>
       <c r="Q313" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R313" s="11">
         <v>0</v>
@@ -76593,7 +76591,7 @@
       </c>
       <c r="T313" s="24">
         <f t="shared" ref="T313" si="21">SUM(J313:K313)+SUM(M313:S313)*5+4.4*SUM(AO313:AW313)+2.5*SUM(AI313:AM313)+AH313+L313</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U313" s="11">
         <v>10</v>
@@ -76608,7 +76606,7 @@
         <v>1021</v>
       </c>
       <c r="Y313" s="11" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="Z313" s="21">
         <v>55000344</v>
@@ -76627,7 +76625,7 @@
 IF(ISBLANK($AB313),0, LOOKUP($AB313,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC313/100)+
 IF(ISBLANK($AD313),0, LOOKUP($AD313,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE313/100)+
 IF(ISBLANK($AF313),0, LOOKUP($AF313,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG313/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI313" s="21">
         <v>0</v>
@@ -77020,7 +77018,7 @@
         <v>295</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -77196,7 +77194,7 @@
         <v>1143</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -77328,7 +77326,7 @@
       </c>
       <c r="H4" s="4">
         <f t="shared" ref="H4:H11" si="0">IF(T4&gt;10,5,IF(T4&gt;5,4,IF(T4&gt;2.5,3,IF(T4&gt;0,2,IF(T4&gt;-2.5,1,IF(T4&gt;-10,0,6))))))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="11">
         <v>1</v>
@@ -77365,7 +77363,7 @@
       </c>
       <c r="T4" s="15">
         <f t="shared" ref="T4:T11" si="1">SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AW4)+2.5*SUM(AI4:AM4)+AH4+L4</f>
-        <v>-22</v>
+        <v>13</v>
       </c>
       <c r="U4" s="11">
         <v>10</v>
@@ -77397,7 +77395,7 @@
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG4/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI4" s="21">
         <v>0</v>
@@ -77494,7 +77492,7 @@
       </c>
       <c r="H5" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" s="11">
         <v>2</v>
@@ -77531,7 +77529,7 @@
       </c>
       <c r="T5" s="15">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="U5" s="11">
         <v>10</v>
@@ -77563,7 +77561,7 @@
 IF(ISBLANK($AB5),0, LOOKUP($AB5,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC5/100)+
 IF(ISBLANK($AD5),0, LOOKUP($AD5,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE5/100)+
 IF(ISBLANK($AF5),0, LOOKUP($AF5,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG5/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI5" s="21">
         <v>0</v>

</xml_diff>

<commit_message>
alien skill and data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="1430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="1430">
   <si>
     <t>arrow</t>
   </si>
@@ -5201,10 +5201,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000115;25|55000116;400</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>55000118;100|55000243;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5549,6 +5545,10 @@
   </si>
   <si>
     <t>55000127;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55000116;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -11491,7 +11491,7 @@
             <v>55000116</v>
           </cell>
           <cell r="V103">
-            <v>3</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="104">
@@ -22601,10 +22601,10 @@
   <dimension ref="A1:BF313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A102" sqref="A102"/>
+      <selection pane="bottomRight" activeCell="Y89" sqref="Y89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -22704,7 +22704,7 @@
         <v>1138</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="X1" s="17" t="s">
         <v>323</v>
@@ -22788,7 +22788,7 @@
         <v>1027</v>
       </c>
       <c r="AY1" s="54" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="AZ1" s="17" t="s">
         <v>326</v>
@@ -22880,7 +22880,7 @@
         <v>1139</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -22964,7 +22964,7 @@
         <v>1029</v>
       </c>
       <c r="AY2" s="55" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="AZ2" s="2" t="s">
         <v>295</v>
@@ -23056,7 +23056,7 @@
         <v>1141</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -23140,7 +23140,7 @@
         <v>1028</v>
       </c>
       <c r="AY3" s="14" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="AZ3" s="6" t="s">
         <v>309</v>
@@ -23306,7 +23306,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY4" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ4" s="4">
         <v>6</v>
@@ -23480,7 +23480,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY5" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ5" s="4">
         <v>6</v>
@@ -23650,7 +23650,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY6" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ6" s="4">
         <v>6</v>
@@ -23820,7 +23820,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY7" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ7" s="4">
         <v>6</v>
@@ -23984,7 +23984,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY8" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ8" s="4">
         <v>6</v>
@@ -24082,7 +24082,7 @@
         <v>11</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="Z9" s="43">
         <v>55000067</v>
@@ -24154,7 +24154,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY9" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ9" s="4">
         <v>6</v>
@@ -24324,7 +24324,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY10" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ10" s="4">
         <v>6</v>
@@ -24494,7 +24494,7 @@
         <v>0;0;0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AY11" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ11" s="4">
         <v>6</v>
@@ -24668,7 +24668,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY12" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ12" s="4">
         <v>6</v>
@@ -24832,7 +24832,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY13" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ13" s="4">
         <v>6</v>
@@ -25010,7 +25010,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY14" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ14" s="4">
         <v>6</v>
@@ -25174,7 +25174,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY15" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ15" s="4">
         <v>4</v>
@@ -25338,7 +25338,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY16" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ16" s="4">
         <v>6</v>
@@ -25502,7 +25502,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY17" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ17" s="4">
         <v>6</v>
@@ -25666,7 +25666,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY18" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ18" s="4">
         <v>6</v>
@@ -25830,7 +25830,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY19" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ19" s="4">
         <v>6</v>
@@ -25994,7 +25994,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY20" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ20" s="4">
         <v>6</v>
@@ -26158,7 +26158,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY21" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ21" s="4">
         <v>6</v>
@@ -26322,7 +26322,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY22" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ22" s="4">
         <v>6</v>
@@ -26486,7 +26486,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY23" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ23" s="4">
         <v>6</v>
@@ -26656,7 +26656,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY24" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ24" s="4">
         <v>6</v>
@@ -26834,7 +26834,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY25" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ25" s="4">
         <v>6</v>
@@ -26998,7 +26998,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY26" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ26" s="4">
         <v>6</v>
@@ -27168,7 +27168,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY27" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ27" s="4">
         <v>6</v>
@@ -27338,7 +27338,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY28" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ28" s="4">
         <v>6</v>
@@ -27508,7 +27508,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY29" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ29" s="4">
         <v>6</v>
@@ -27672,7 +27672,7 @@
         <v>0;0;0;0;0.3;0;0;0;0</v>
       </c>
       <c r="AY30" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ30" s="4">
         <v>6</v>
@@ -27846,7 +27846,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY31" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ31" s="4">
         <v>6</v>
@@ -28024,7 +28024,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY32" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ32" s="4">
         <v>6</v>
@@ -28188,7 +28188,7 @@
         <v>0;0.3;0.3;0.3;0;0;0;0.3;0</v>
       </c>
       <c r="AY33" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ33" s="4">
         <v>6</v>
@@ -28358,7 +28358,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY34" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ34" s="4">
         <v>6</v>
@@ -28528,7 +28528,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY35" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ35" s="4">
         <v>6</v>
@@ -28626,7 +28626,7 @@
         <v>1160</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="Z36" s="43">
         <v>55000030</v>
@@ -28702,7 +28702,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY36" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ36" s="4">
         <v>6</v>
@@ -28872,7 +28872,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY37" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ37" s="4">
         <v>6</v>
@@ -29036,7 +29036,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY38" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ38" s="4">
         <v>6</v>
@@ -29200,7 +29200,7 @@
         <v>0;0.3;0;0;0.3;0;0;0;0</v>
       </c>
       <c r="AY39" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ39" s="4">
         <v>6</v>
@@ -29364,7 +29364,7 @@
         <v>0;0.3;0;0.3;0;0.3;0.3;0;0</v>
       </c>
       <c r="AY40" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ40" s="4">
         <v>6</v>
@@ -29462,7 +29462,7 @@
         <v>51</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="Z41" s="43">
         <v>55000071</v>
@@ -29534,7 +29534,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY41" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ41" s="4">
         <v>6</v>
@@ -29632,7 +29632,7 @@
         <v>53</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="Z42" s="43">
         <v>55000034</v>
@@ -29708,7 +29708,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY42" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ42" s="4">
         <v>6</v>
@@ -29878,7 +29878,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY43" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ43" s="4">
         <v>6</v>
@@ -29976,7 +29976,7 @@
         <v>16</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Z44" s="43">
         <v>55000075</v>
@@ -30052,7 +30052,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY44" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ44" s="4">
         <v>6</v>
@@ -30226,7 +30226,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY45" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ45" s="4">
         <v>6</v>
@@ -30324,7 +30324,7 @@
         <v>2</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Z46" s="43">
         <v>55000075</v>
@@ -30400,7 +30400,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY46" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ46" s="4">
         <v>6</v>
@@ -30570,7 +30570,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY47" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ47" s="4">
         <v>6</v>
@@ -30740,7 +30740,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY48" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ48" s="4">
         <v>6</v>
@@ -30910,7 +30910,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY49" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ49" s="4">
         <v>6</v>
@@ -31084,7 +31084,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY50" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ50" s="4">
         <v>4</v>
@@ -31258,7 +31258,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY51" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ51" s="4">
         <v>6</v>
@@ -31356,7 +31356,7 @@
         <v>9</v>
       </c>
       <c r="Y52" s="4" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="Z52" s="43">
         <v>55000084</v>
@@ -31428,7 +31428,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY52" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ52" s="4">
         <v>6</v>
@@ -31596,7 +31596,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY53" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ53" s="4">
         <v>6</v>
@@ -31694,7 +31694,7 @@
         <v>64</v>
       </c>
       <c r="Y54" s="4" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="Z54" s="43">
         <v>55000066</v>
@@ -31766,7 +31766,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY54" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ54" s="4">
         <v>6</v>
@@ -31936,7 +31936,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY55" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ55" s="4">
         <v>6</v>
@@ -32034,7 +32034,7 @@
         <v>4</v>
       </c>
       <c r="Y56" s="4" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="Z56" s="43">
         <v>55000087</v>
@@ -32106,7 +32106,7 @@
         <v>0;0;0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AY56" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ56" s="4">
         <v>6</v>
@@ -32280,7 +32280,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY57" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ57" s="4">
         <v>6</v>
@@ -32450,7 +32450,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY58" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ58" s="4">
         <v>6</v>
@@ -32620,7 +32620,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY59" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ59" s="4">
         <v>6</v>
@@ -32790,7 +32790,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY60" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ60" s="4">
         <v>6</v>
@@ -32960,7 +32960,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY61" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ61" s="4">
         <v>6</v>
@@ -33130,7 +33130,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY62" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ62" s="4">
         <v>6</v>
@@ -33300,7 +33300,7 @@
         <v>0;0;0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AY63" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ63" s="4">
         <v>6</v>
@@ -33464,7 +33464,7 @@
         <v>0;0.3;0.3;0;0.3;0;0;0;0</v>
       </c>
       <c r="AY64" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ64" s="4">
         <v>6</v>
@@ -33628,7 +33628,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY65" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ65" s="4">
         <v>6</v>
@@ -33792,7 +33792,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY66" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ66" s="4">
         <v>6</v>
@@ -33890,7 +33890,7 @@
         <v>78</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="Z67" s="43">
         <v>55000095</v>
@@ -33966,7 +33966,7 @@
         <v>0;0;0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AY67" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ67" s="4">
         <v>5</v>
@@ -34148,7 +34148,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY68" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ68" s="4">
         <v>5</v>
@@ -34328,7 +34328,7 @@
         <v>0;0;0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AY69" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ69" s="4">
         <v>5</v>
@@ -34506,7 +34506,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY70" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ70" s="4">
         <v>5</v>
@@ -34680,7 +34680,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY71" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ71" s="4">
         <v>6</v>
@@ -34854,7 +34854,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY72" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ72" s="4">
         <v>6</v>
@@ -35028,7 +35028,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY73" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ73" s="4">
         <v>6</v>
@@ -35202,7 +35202,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY74" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ74" s="4">
         <v>6</v>
@@ -35300,7 +35300,7 @@
         <v>89</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="Z75" s="43">
         <v>55000004</v>
@@ -35376,7 +35376,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY75" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ75" s="4">
         <v>6</v>
@@ -35550,7 +35550,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY76" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ76" s="4">
         <v>6</v>
@@ -35720,7 +35720,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY77" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ77" s="4">
         <v>6</v>
@@ -35894,7 +35894,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY78" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ78" s="4">
         <v>6</v>
@@ -36058,7 +36058,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY79" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ79" s="4">
         <v>6</v>
@@ -36222,7 +36222,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY80" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ80" s="4">
         <v>6</v>
@@ -36396,7 +36396,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY81" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ81" s="4">
         <v>6</v>
@@ -36570,7 +36570,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY82" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ82" s="4">
         <v>6</v>
@@ -36744,7 +36744,7 @@
         <v>0;0;0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AY83" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ83" s="4">
         <v>6</v>
@@ -36842,7 +36842,7 @@
         <v>100</v>
       </c>
       <c r="Y84" s="4" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="Z84" s="43">
         <v>55000069</v>
@@ -36914,7 +36914,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY84" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ84" s="4">
         <v>6</v>
@@ -37092,7 +37092,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY85" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ85" s="4">
         <v>3</v>
@@ -37266,7 +37266,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY86" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ86" s="4">
         <v>6</v>
@@ -37364,7 +37364,7 @@
         <v>86</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="Z87" s="43">
         <v>55000068</v>
@@ -37440,7 +37440,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY87" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ87" s="4">
         <v>6</v>
@@ -37614,7 +37614,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY88" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ88" s="4">
         <v>6</v>
@@ -37650,7 +37650,7 @@
         <v>880</v>
       </c>
       <c r="E89" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F89" s="4">
         <v>8</v>
@@ -37660,19 +37660,19 @@
       </c>
       <c r="H89" s="4">
         <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I89" s="4">
+        <v>2</v>
+      </c>
+      <c r="J89" s="4">
+        <v>0</v>
+      </c>
+      <c r="K89" s="4">
         <v>5</v>
       </c>
-      <c r="I89" s="4">
-        <v>1</v>
-      </c>
-      <c r="J89" s="4">
-        <v>9</v>
-      </c>
-      <c r="K89" s="4">
-        <v>18</v>
-      </c>
       <c r="L89" s="4">
-        <v>-2</v>
+        <v>-34</v>
       </c>
       <c r="M89" s="4">
         <v>0</v>
@@ -37697,7 +37697,7 @@
       </c>
       <c r="T89" s="15">
         <f t="shared" si="5"/>
-        <v>31.200000000000003</v>
+        <v>1</v>
       </c>
       <c r="U89" s="4">
         <v>10</v>
@@ -37712,20 +37712,16 @@
         <v>105</v>
       </c>
       <c r="Y89" s="4" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Z89" s="43">
-        <v>55000115</v>
+        <v>1429</v>
+      </c>
+      <c r="Z89" s="21">
+        <v>55000116</v>
       </c>
       <c r="AA89" s="21">
-        <v>25</v>
-      </c>
-      <c r="AB89" s="21">
-        <v>55000116</v>
-      </c>
-      <c r="AC89" s="21">
-        <v>40</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="AB89" s="21"/>
+      <c r="AC89" s="21"/>
       <c r="AD89" s="21"/>
       <c r="AE89" s="21"/>
       <c r="AF89" s="21"/>
@@ -37735,7 +37731,7 @@
 IF(ISBLANK($AB89),0, LOOKUP($AB89,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC89/100)+
 IF(ISBLANK($AD89),0, LOOKUP($AD89,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE89/100)+
 IF(ISBLANK($AF89),0, LOOKUP($AF89,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG89/100)</f>
-        <v>6.2</v>
+        <v>30</v>
       </c>
       <c r="AI89" s="21">
         <v>0</v>
@@ -37788,7 +37784,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY89" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ89" s="4">
         <v>6</v>
@@ -37806,9 +37802,7 @@
       <c r="BE89" s="30">
         <v>0.32131150000000003</v>
       </c>
-      <c r="BF89" s="22" t="s">
-        <v>1172</v>
-      </c>
+      <c r="BF89" s="22"/>
     </row>
     <row r="90" spans="1:58" ht="14.25">
       <c r="A90">
@@ -37962,7 +37956,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY90" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ90" s="4">
         <v>6</v>
@@ -38060,7 +38054,7 @@
         <v>105</v>
       </c>
       <c r="Y91" s="4" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="Z91" s="43">
         <v>55000118</v>
@@ -38136,7 +38130,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY91" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ91" s="4">
         <v>6</v>
@@ -38310,7 +38304,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY92" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ92" s="4">
         <v>6</v>
@@ -38484,7 +38478,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY93" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ93" s="4">
         <v>6</v>
@@ -38658,7 +38652,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY94" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ94" s="4">
         <v>5</v>
@@ -38756,7 +38750,7 @@
         <v>107</v>
       </c>
       <c r="Y95" s="4" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="Z95" s="43">
         <v>55000114</v>
@@ -38832,7 +38826,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY95" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ95" s="4">
         <v>6</v>
@@ -39006,7 +39000,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY96" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ96" s="4">
         <v>6</v>
@@ -39104,7 +39098,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="Z97" s="43">
         <v>55000123</v>
@@ -39184,7 +39178,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY97" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ97" s="4">
         <v>3</v>
@@ -39282,7 +39276,7 @@
         <v>94</v>
       </c>
       <c r="Y98" s="4" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="Z98" s="43">
         <v>55000245</v>
@@ -39354,7 +39348,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY98" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ98" s="4">
         <v>6</v>
@@ -39528,7 +39522,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY99" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ99" s="4">
         <v>6</v>
@@ -39710,7 +39704,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY100" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ100" s="4">
         <v>5</v>
@@ -39886,7 +39880,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY101" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ101" s="4">
         <v>6</v>
@@ -39984,7 +39978,7 @@
         <v>16</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="Z102" s="43">
         <v>55000127</v>
@@ -40056,7 +40050,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY102" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ102" s="4">
         <v>4</v>
@@ -40224,7 +40218,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY103" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ103" s="4">
         <v>6</v>
@@ -40398,7 +40392,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY104" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ104" s="4">
         <v>6</v>
@@ -40572,7 +40566,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY105" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ105" s="4">
         <v>6</v>
@@ -40742,7 +40736,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY106" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ106" s="4">
         <v>6</v>
@@ -40912,7 +40906,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY107" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ107" s="4">
         <v>6</v>
@@ -41010,7 +41004,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="Z108" s="43">
         <v>55000017</v>
@@ -41090,7 +41084,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY108" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ108" s="4">
         <v>4</v>
@@ -41188,7 +41182,7 @@
         <v>128</v>
       </c>
       <c r="Y109" s="4" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="Z109" s="43">
         <v>55000135</v>
@@ -41260,7 +41254,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY109" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ109" s="4">
         <v>6</v>
@@ -41358,7 +41352,7 @@
         <v>130</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="Z110" s="43">
         <v>55000135</v>
@@ -41434,7 +41428,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY110" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ110" s="4">
         <v>6</v>
@@ -41532,7 +41526,7 @@
         <v>132</v>
       </c>
       <c r="Y111" s="4" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="Z111" s="43">
         <v>55000038</v>
@@ -41604,7 +41598,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY111" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ111" s="4">
         <v>6</v>
@@ -41702,7 +41696,7 @@
         <v>118</v>
       </c>
       <c r="Y112" s="4" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="Z112" s="43">
         <v>55010003</v>
@@ -41778,7 +41772,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY112" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ112" s="4">
         <v>6</v>
@@ -41952,7 +41946,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY113" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ113" s="4">
         <v>6</v>
@@ -42134,7 +42128,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY114" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ114" s="4">
         <v>3</v>
@@ -42318,7 +42312,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY115" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ115" s="4">
         <v>6</v>
@@ -42502,7 +42496,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY116" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ116" s="4">
         <v>6</v>
@@ -42678,7 +42672,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY117" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ117" s="4">
         <v>6</v>
@@ -42860,7 +42854,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY118" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ118" s="4">
         <v>5</v>
@@ -43044,7 +43038,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY119" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ119" s="4">
         <v>6</v>
@@ -43228,7 +43222,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY120" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ120" s="4">
         <v>5</v>
@@ -43412,7 +43406,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY121" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ121" s="4">
         <v>6</v>
@@ -43588,7 +43582,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY122" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ122" s="4">
         <v>6</v>
@@ -43766,7 +43760,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY123" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ123" s="4">
         <v>6</v>
@@ -43944,7 +43938,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY124" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ124" s="4">
         <v>6</v>
@@ -44122,7 +44116,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY125" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ125" s="4">
         <v>6</v>
@@ -44292,7 +44286,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY126" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ126" s="4">
         <v>6</v>
@@ -44462,7 +44456,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY127" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ127" s="4">
         <v>6</v>
@@ -44636,7 +44630,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY128" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ128" s="4">
         <v>6</v>
@@ -44810,7 +44804,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY129" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ129" s="4">
         <v>3</v>
@@ -44980,7 +44974,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY130" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ130" s="4">
         <v>6</v>
@@ -45150,7 +45144,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY131" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ131" s="4">
         <v>6</v>
@@ -45324,7 +45318,7 @@
         <v>0;0;0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AY132" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ132" s="4">
         <v>6</v>
@@ -45498,7 +45492,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY133" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ133" s="4">
         <v>6</v>
@@ -45672,7 +45666,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY134" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ134" s="4">
         <v>6</v>
@@ -45846,7 +45840,7 @@
         <v>0;0;0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AY135" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ135" s="4">
         <v>6</v>
@@ -46020,7 +46014,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY136" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ136" s="4">
         <v>6</v>
@@ -46198,7 +46192,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY137" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ137" s="4">
         <v>5</v>
@@ -46372,7 +46366,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY138" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ138" s="4">
         <v>6</v>
@@ -46546,7 +46540,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY139" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ139" s="4">
         <v>6</v>
@@ -46710,7 +46704,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY140" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ140" s="4">
         <v>6</v>
@@ -46884,7 +46878,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY141" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ141" s="4">
         <v>6</v>
@@ -46982,7 +46976,7 @@
         <v>40</v>
       </c>
       <c r="Y142" s="4" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="Z142" s="43">
         <v>55000018</v>
@@ -47058,7 +47052,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY142" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ142" s="4">
         <v>6</v>
@@ -47232,7 +47226,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY143" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ143" s="4">
         <v>6</v>
@@ -47402,7 +47396,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY144" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ144" s="4">
         <v>6</v>
@@ -47566,7 +47560,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY145" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ145" s="4">
         <v>6</v>
@@ -47744,7 +47738,7 @@
         <v>0;0;0;0;0.3;0;0;0;0</v>
       </c>
       <c r="AY146" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ146" s="4">
         <v>6</v>
@@ -47918,7 +47912,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY147" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ147" s="4">
         <v>6</v>
@@ -48016,7 +48010,7 @@
         <v>1165</v>
       </c>
       <c r="Y148" s="4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="Z148" s="43">
         <v>55000340</v>
@@ -48092,7 +48086,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY148" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ148" s="4">
         <v>6</v>
@@ -48190,7 +48184,7 @@
         <v>166</v>
       </c>
       <c r="Y149" s="4" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="Z149" s="43">
         <v>55000066</v>
@@ -48270,7 +48264,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY149" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ149" s="4">
         <v>6</v>
@@ -48448,7 +48442,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY150" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ150" s="4">
         <v>6</v>
@@ -48618,7 +48612,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY151" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ151" s="4">
         <v>6</v>
@@ -48782,7 +48776,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY152" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ152" s="4">
         <v>6</v>
@@ -48952,7 +48946,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY153" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ153" s="4">
         <v>6</v>
@@ -49122,7 +49116,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY154" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ154" s="4">
         <v>6</v>
@@ -49220,7 +49214,7 @@
         <v>1169</v>
       </c>
       <c r="Y155" s="4" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="Z155" s="43">
         <v>55000165</v>
@@ -49292,7 +49286,7 @@
         <v>0;0;0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AY155" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ155" s="4">
         <v>6</v>
@@ -49462,7 +49456,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY156" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ156" s="4">
         <v>6</v>
@@ -49626,7 +49620,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY157" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ157" s="4">
         <v>6</v>
@@ -49796,7 +49790,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY158" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ158" s="4">
         <v>6</v>
@@ -49970,7 +49964,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY159" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ159" s="4">
         <v>6</v>
@@ -50068,7 +50062,7 @@
         <v>179</v>
       </c>
       <c r="Y160" s="4" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="Z160" s="43">
         <v>55000048</v>
@@ -50144,7 +50138,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY160" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ160" s="4">
         <v>6</v>
@@ -50308,7 +50302,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY161" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ161" s="4">
         <v>6</v>
@@ -50478,7 +50472,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY162" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ162" s="4">
         <v>6</v>
@@ -50648,7 +50642,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY163" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ163" s="4">
         <v>6</v>
@@ -50822,7 +50816,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY164" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ164" s="4">
         <v>6</v>
@@ -51000,7 +50994,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY165" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ165" s="4">
         <v>6</v>
@@ -51174,7 +51168,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY166" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ166" s="4">
         <v>6</v>
@@ -51348,7 +51342,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY167" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ167" s="4">
         <v>6</v>
@@ -51526,7 +51520,7 @@
         <v>0;0;0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AY168" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ168" s="4">
         <v>5</v>
@@ -51696,7 +51690,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY169" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ169" s="4">
         <v>6</v>
@@ -51866,7 +51860,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY170" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ170" s="4">
         <v>6</v>
@@ -52048,7 +52042,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY171" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ171" s="4">
         <v>6</v>
@@ -52226,7 +52220,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY172" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ172" s="4">
         <v>6</v>
@@ -52324,7 +52318,7 @@
         <v>1163</v>
       </c>
       <c r="Y173" s="4" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="Z173" s="43">
         <v>55000015</v>
@@ -52400,7 +52394,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY173" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ173" s="4">
         <v>6</v>
@@ -52570,7 +52564,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY174" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ174" s="4">
         <v>6</v>
@@ -52740,7 +52734,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY175" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ175" s="4">
         <v>6</v>
@@ -52910,7 +52904,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY176" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ176" s="4">
         <v>6</v>
@@ -53008,7 +53002,7 @@
         <v>4</v>
       </c>
       <c r="Y177" s="4" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="Z177" s="43">
         <v>55000188</v>
@@ -53084,7 +53078,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY177" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ177" s="4">
         <v>6</v>
@@ -53258,7 +53252,7 @@
         <v>0;0;0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AY178" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ178" s="4">
         <v>6</v>
@@ -53428,7 +53422,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY179" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ179" s="4">
         <v>6</v>
@@ -53526,7 +53520,7 @@
         <v>65</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="Z180" s="43">
         <v>55000061</v>
@@ -53610,7 +53604,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY180" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ180" s="4">
         <v>5</v>
@@ -53708,7 +53702,7 @@
         <v>976</v>
       </c>
       <c r="Y181" s="4" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="Z181" s="43">
         <v>55000044</v>
@@ -53788,7 +53782,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY181" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ181" s="4">
         <v>6</v>
@@ -53962,7 +53956,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY182" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ182" s="4">
         <v>6</v>
@@ -54136,7 +54130,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY183" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ183" s="4">
         <v>5</v>
@@ -54306,7 +54300,7 @@
         <v>0;0;0.3;0;0;0;0;0;0</v>
       </c>
       <c r="AY184" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ184" s="4">
         <v>6</v>
@@ -54404,7 +54398,7 @@
         <v>12</v>
       </c>
       <c r="Y185" s="4" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="Z185" s="43">
         <v>55000194</v>
@@ -54480,7 +54474,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY185" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ185" s="4">
         <v>3</v>
@@ -54654,7 +54648,7 @@
         <v>0;0.3;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY186" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ186" s="4">
         <v>6</v>
@@ -54824,7 +54818,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY187" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ187" s="4">
         <v>6</v>
@@ -54922,7 +54916,7 @@
         <v>2</v>
       </c>
       <c r="Y188" s="4" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="Z188" s="43">
         <v>55000196</v>
@@ -55002,7 +54996,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY188" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ188" s="4">
         <v>3</v>
@@ -55172,7 +55166,7 @@
         <v>0;0;0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AY189" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ189" s="4">
         <v>6</v>
@@ -55336,7 +55330,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY190" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ190" s="4">
         <v>6</v>
@@ -55510,7 +55504,7 @@
         <v>0;0;0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AY191" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ191" s="4">
         <v>6</v>
@@ -55608,7 +55602,7 @@
         <v>1164</v>
       </c>
       <c r="Y192" s="4" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="Z192" s="43">
         <v>55000001</v>
@@ -55688,7 +55682,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY192" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ192" s="4">
         <v>6</v>
@@ -55866,7 +55860,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY193" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ193" s="4">
         <v>6</v>
@@ -56044,7 +56038,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY194" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ194" s="4">
         <v>4</v>
@@ -56142,7 +56136,7 @@
         <v>209</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="Z195" s="43">
         <v>55000016</v>
@@ -56226,7 +56220,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY195" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ195" s="4">
         <v>5</v>
@@ -56400,7 +56394,7 @@
         <v>0;0;0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AY196" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ196" s="4">
         <v>5</v>
@@ -56578,7 +56572,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY197" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ197" s="4">
         <v>5</v>
@@ -56756,7 +56750,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY198" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ198" s="4">
         <v>3</v>
@@ -56934,7 +56928,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY199" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ199" s="4">
         <v>6</v>
@@ -57112,7 +57106,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY200" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ200" s="4">
         <v>6</v>
@@ -57282,7 +57276,7 @@
         <v>0;0;0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AY201" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ201" s="4">
         <v>3</v>
@@ -57380,7 +57374,7 @@
         <v>1166</v>
       </c>
       <c r="Y202" s="4" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="Z202" s="43">
         <v>55000203</v>
@@ -57452,7 +57446,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY202" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ202" s="4">
         <v>6</v>
@@ -57624,7 +57618,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY203" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ203" s="4">
         <v>6</v>
@@ -57798,7 +57792,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY204" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ204" s="4">
         <v>6</v>
@@ -57896,7 +57890,7 @@
         <v>1168</v>
       </c>
       <c r="Y205" s="4" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="Z205" s="43">
         <v>55000197</v>
@@ -57968,7 +57962,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY205" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ205" s="4">
         <v>6</v>
@@ -58066,7 +58060,7 @@
         <v>94</v>
       </c>
       <c r="Y206" s="4" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="Z206" s="43">
         <v>55000003</v>
@@ -58142,7 +58136,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY206" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ206" s="4">
         <v>6</v>
@@ -58312,7 +58306,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY207" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ207" s="4">
         <v>6</v>
@@ -58486,7 +58480,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY208" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ208" s="4">
         <v>6</v>
@@ -58584,7 +58578,7 @@
         <v>2</v>
       </c>
       <c r="Y209" s="4" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="Z209" s="43">
         <v>55000120</v>
@@ -58656,7 +58650,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY209" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ209" s="4">
         <v>6</v>
@@ -58830,7 +58824,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY210" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ210" s="4">
         <v>6</v>
@@ -59008,7 +59002,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY211" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ211" s="4">
         <v>6</v>
@@ -59106,7 +59100,7 @@
         <v>132</v>
       </c>
       <c r="Y212" s="4" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="Z212" s="43">
         <v>55000103</v>
@@ -59182,7 +59176,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY212" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ212" s="4">
         <v>6</v>
@@ -59280,7 +59274,7 @@
         <v>228</v>
       </c>
       <c r="Y213" s="4" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="Z213" s="43">
         <v>55000114</v>
@@ -59360,7 +59354,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY213" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ213" s="4">
         <v>6</v>
@@ -59538,7 +59532,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY214" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ214" s="4">
         <v>6</v>
@@ -59636,7 +59630,7 @@
         <v>190</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="Z215" s="43">
         <v>55000102</v>
@@ -59720,7 +59714,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY215" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ215" s="4">
         <v>6</v>
@@ -59890,7 +59884,7 @@
         <v>0;0;0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AY216" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ216" s="4">
         <v>6</v>
@@ -60064,7 +60058,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY217" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ217" s="4">
         <v>6</v>
@@ -60238,7 +60232,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY218" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ218" s="4">
         <v>6</v>
@@ -60336,7 +60330,7 @@
         <v>1167</v>
       </c>
       <c r="Y219" s="4" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="Z219" s="43">
         <v>55000070</v>
@@ -60412,7 +60406,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY219" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ219" s="4">
         <v>6</v>
@@ -60582,7 +60576,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY220" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ220" s="4">
         <v>6</v>
@@ -60756,7 +60750,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY221" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ221" s="4">
         <v>6</v>
@@ -60926,7 +60920,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY222" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ222" s="4">
         <v>6</v>
@@ -61096,7 +61090,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY223" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ223" s="4">
         <v>6</v>
@@ -61270,7 +61264,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY224" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ224" s="4">
         <v>6</v>
@@ -61444,7 +61438,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY225" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ225" s="4">
         <v>6</v>
@@ -61542,7 +61536,7 @@
         <v>9</v>
       </c>
       <c r="Y226" s="4" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="Z226" s="43">
         <v>55000221</v>
@@ -61614,7 +61608,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY226" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ226" s="4">
         <v>6</v>
@@ -61786,7 +61780,7 @@
         <v>0;0;0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AY227" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ227" s="4">
         <v>6</v>
@@ -61884,7 +61878,7 @@
         <v>245</v>
       </c>
       <c r="Y228" s="4" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="Z228" s="43">
         <v>55000160</v>
@@ -61960,7 +61954,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY228" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ228" s="4">
         <v>6</v>
@@ -62134,7 +62128,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY229" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ229" s="4">
         <v>6</v>
@@ -62304,7 +62298,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY230" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ230" s="4">
         <v>6</v>
@@ -62474,7 +62468,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY231" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ231" s="4">
         <v>6</v>
@@ -62638,7 +62632,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY232" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ232" s="4">
         <v>6</v>
@@ -62736,7 +62730,7 @@
         <v>251</v>
       </c>
       <c r="Y233" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="Z233" s="43">
         <v>55000120</v>
@@ -62808,7 +62802,7 @@
         <v>0;0;0.3;0;0;0;0;0;0</v>
       </c>
       <c r="AY233" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ233" s="4">
         <v>6</v>
@@ -62982,7 +62976,7 @@
         <v>0;0;0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AY234" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ234" s="4">
         <v>6</v>
@@ -63156,7 +63150,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY235" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ235" s="4">
         <v>6</v>
@@ -63330,7 +63324,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY236" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ236" s="4">
         <v>6</v>
@@ -63512,7 +63506,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY237" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ237" s="4">
         <v>6</v>
@@ -63686,7 +63680,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY238" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ238" s="4">
         <v>6</v>
@@ -63860,7 +63854,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY239" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ239" s="4">
         <v>6</v>
@@ -64034,7 +64028,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY240" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ240" s="4">
         <v>6</v>
@@ -64216,7 +64210,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY241" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ241" s="4">
         <v>3</v>
@@ -64390,7 +64384,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY242" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ242" s="4">
         <v>6</v>
@@ -64488,7 +64482,7 @@
         <v>220</v>
       </c>
       <c r="Y243" s="4" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="Z243" s="43">
         <v>55000037</v>
@@ -64568,7 +64562,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY243" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ243" s="4">
         <v>6</v>
@@ -64742,7 +64736,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY244" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ244" s="4">
         <v>6</v>
@@ -64924,7 +64918,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY245" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ245" s="4">
         <v>4</v>
@@ -65094,7 +65088,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY246" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ246" s="4">
         <v>4</v>
@@ -65272,7 +65266,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY247" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ247" s="4">
         <v>6</v>
@@ -65442,7 +65436,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY248" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ248" s="4">
         <v>6</v>
@@ -65616,7 +65610,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY249" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ249" s="4">
         <v>6</v>
@@ -65794,7 +65788,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY250" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ250" s="4">
         <v>3</v>
@@ -65968,7 +65962,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY251" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ251" s="4">
         <v>6</v>
@@ -66146,7 +66140,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY252" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ252" s="4">
         <v>6</v>
@@ -66320,7 +66314,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY253" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ253" s="4">
         <v>6</v>
@@ -66418,7 +66412,7 @@
         <v>209</v>
       </c>
       <c r="Y254" s="4" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="Z254" s="43">
         <v>55000340</v>
@@ -66494,7 +66488,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY254" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ254" s="4">
         <v>6</v>
@@ -66592,7 +66586,7 @@
         <v>0</v>
       </c>
       <c r="Y255" s="4" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="Z255" s="43">
         <v>55000181</v>
@@ -66668,7 +66662,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY255" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ255" s="4">
         <v>6</v>
@@ -66842,7 +66836,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY256" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ256" s="4">
         <v>6</v>
@@ -67016,7 +67010,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY257" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ257" s="4">
         <v>6</v>
@@ -67190,7 +67184,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY258" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ258" s="4">
         <v>6</v>
@@ -67364,7 +67358,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY259" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ259" s="4">
         <v>6</v>
@@ -67538,7 +67532,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY260" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ260" s="4">
         <v>6</v>
@@ -67712,7 +67706,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY261" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ261" s="4">
         <v>6</v>
@@ -67882,7 +67876,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY262" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ262" s="4">
         <v>6</v>
@@ -68046,7 +68040,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY263" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ263" s="4">
         <v>6</v>
@@ -68220,7 +68214,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY264" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ264" s="4">
         <v>6</v>
@@ -68398,7 +68392,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY265" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ265" s="4">
         <v>6</v>
@@ -68576,7 +68570,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY266" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ266" s="4">
         <v>6</v>
@@ -68674,7 +68668,7 @@
         <v>94</v>
       </c>
       <c r="Y267" s="4" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="Z267" s="43">
         <v>55000001</v>
@@ -68754,7 +68748,7 @@
         <v>0;0;0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AY267" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ267" s="4">
         <v>6</v>
@@ -68928,7 +68922,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY268" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ268" s="4">
         <v>6</v>
@@ -69098,7 +69092,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY269" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ269" s="4">
         <v>6</v>
@@ -69272,7 +69266,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY270" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ270" s="4">
         <v>6</v>
@@ -69450,7 +69444,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY271" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ271" s="4">
         <v>5</v>
@@ -69628,7 +69622,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY272" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ272" s="4">
         <v>6</v>
@@ -69806,7 +69800,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY273" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ273" s="4">
         <v>3</v>
@@ -69904,7 +69898,7 @@
         <v>0</v>
       </c>
       <c r="Y274" s="4" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="Z274" s="43">
         <v>55000342</v>
@@ -69976,7 +69970,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY274" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ274" s="4">
         <v>6</v>
@@ -70074,7 +70068,7 @@
         <v>277</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="Z275" s="43">
         <v>55000278</v>
@@ -70150,7 +70144,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY275" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ275" s="4">
         <v>6</v>
@@ -70322,7 +70316,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY276" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ276" s="4">
         <v>6</v>
@@ -70496,7 +70490,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY277" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ277" s="4">
         <v>6</v>
@@ -70670,7 +70664,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY278" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ278" s="4">
         <v>6</v>
@@ -70840,7 +70834,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY279" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ279" s="4">
         <v>6</v>
@@ -71014,7 +71008,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY280" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ280" s="4">
         <v>6</v>
@@ -71184,7 +71178,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY281" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ281" s="4">
         <v>6</v>
@@ -71354,7 +71348,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY282" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ282" s="4">
         <v>6</v>
@@ -71524,7 +71518,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY283" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ283" s="4">
         <v>6</v>
@@ -71698,7 +71692,7 @@
         <v>0;0;0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AY284" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ284" s="4">
         <v>6</v>
@@ -71872,7 +71866,7 @@
         <v>0;0;0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AY285" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ285" s="4">
         <v>5</v>
@@ -72036,7 +72030,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY286" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ286" s="4">
         <v>6</v>
@@ -72210,7 +72204,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY287" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ287" s="4">
         <v>6</v>
@@ -72384,7 +72378,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY288" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ288" s="4">
         <v>6</v>
@@ -72482,7 +72476,7 @@
         <v>100</v>
       </c>
       <c r="Y289" s="4" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="Z289" s="43">
         <v>55000293</v>
@@ -72554,7 +72548,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY289" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ289" s="4">
         <v>6</v>
@@ -72724,7 +72718,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY290" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ290" s="4">
         <v>6</v>
@@ -72898,7 +72892,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY291" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ291" s="4">
         <v>6</v>
@@ -73072,7 +73066,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY292" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ292" s="4">
         <v>6</v>
@@ -73242,7 +73236,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY293" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ293" s="4">
         <v>6</v>
@@ -73420,7 +73414,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY294" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ294" s="4">
         <v>6</v>
@@ -73590,7 +73584,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY295" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ295" s="4">
         <v>6</v>
@@ -73764,7 +73758,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY296" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ296" s="4">
         <v>6</v>
@@ -73862,7 +73856,7 @@
         <v>45</v>
       </c>
       <c r="Y297" s="4" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="Z297" s="43">
         <v>55000045</v>
@@ -73942,7 +73936,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY297" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ297" s="4">
         <v>6</v>
@@ -74116,7 +74110,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY298" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ298" s="4">
         <v>6</v>
@@ -74214,7 +74208,7 @@
         <v>22</v>
       </c>
       <c r="Y299" s="4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="Z299" s="43">
         <v>55000047</v>
@@ -74286,7 +74280,7 @@
         <v>0;0;0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AY299" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ299" s="4">
         <v>6</v>
@@ -74384,7 +74378,7 @@
         <v>22</v>
       </c>
       <c r="Y300" s="4" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="Z300" s="43">
         <v>55000107</v>
@@ -74456,7 +74450,7 @@
         <v>0;0.3;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY300" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ300" s="4">
         <v>6</v>
@@ -74638,7 +74632,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY301" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ301" s="4">
         <v>3</v>
@@ -74736,7 +74730,7 @@
         <v>209</v>
       </c>
       <c r="Y302" s="4" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="Z302" s="43">
         <v>55000335</v>
@@ -74812,7 +74806,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY302" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ302" s="4">
         <v>6</v>
@@ -74986,7 +74980,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY303" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ303" s="11">
         <v>6</v>
@@ -75156,7 +75150,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY304" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ304" s="11">
         <v>6</v>
@@ -75326,7 +75320,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY305" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ305" s="11">
         <v>6</v>
@@ -75500,7 +75494,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY306" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ306" s="11">
         <v>6</v>
@@ -75670,7 +75664,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY307" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ307" s="11">
         <v>6</v>
@@ -75834,7 +75828,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY308" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ308" s="11">
         <v>6</v>
@@ -75998,7 +75992,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY309" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ309" s="11">
         <v>6</v>
@@ -76162,7 +76156,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY310" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ310" s="11">
         <v>6</v>
@@ -76326,7 +76320,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY311" s="56" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ311" s="11">
         <v>6</v>
@@ -76353,10 +76347,10 @@
         <v>51000309</v>
       </c>
       <c r="B312" s="11" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C312" s="4" t="s">
         <v>1415</v>
-      </c>
-      <c r="C312" s="4" t="s">
-        <v>1416</v>
       </c>
       <c r="D312" s="8" t="s">
         <v>698</v>
@@ -76424,7 +76418,7 @@
         <v>9</v>
       </c>
       <c r="Y312" s="11" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="Z312" s="21">
         <v>55000300</v>
@@ -76496,7 +76490,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY312" s="57" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ312" s="11">
         <v>6</v>
@@ -76515,7 +76509,7 @@
         <v>0.40819670000000002</v>
       </c>
       <c r="BF312" s="11" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="313" spans="1:58" ht="14.25">
@@ -76523,13 +76517,13 @@
         <v>51000310</v>
       </c>
       <c r="B313" s="11" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C313" s="11" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D313" s="8" t="s">
         <v>1423</v>
-      </c>
-      <c r="C313" s="11" t="s">
-        <v>1422</v>
-      </c>
-      <c r="D313" s="8" t="s">
-        <v>1424</v>
       </c>
       <c r="E313" s="11">
         <v>6</v>
@@ -76594,7 +76588,7 @@
         <v>1021</v>
       </c>
       <c r="Y313" s="11" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="Z313" s="21">
         <v>55000344</v>
@@ -76666,7 +76660,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY313" s="57" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AZ313" s="11">
         <v>6</v>
@@ -76685,7 +76679,7 @@
         <v>0.49672129999999998</v>
       </c>
       <c r="BF313" s="11" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
   </sheetData>
@@ -76835,7 +76829,7 @@
         <v>1138</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="X1" s="17" t="s">
         <v>323</v>
@@ -76919,7 +76913,7 @@
         <v>1027</v>
       </c>
       <c r="AY1" s="54" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="AZ1" s="17" t="s">
         <v>326</v>
@@ -77011,7 +77005,7 @@
         <v>295</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -77095,7 +77089,7 @@
         <v>1029</v>
       </c>
       <c r="AY2" s="55" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="AZ2" s="2" t="s">
         <v>295</v>
@@ -77187,7 +77181,7 @@
         <v>1141</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -77271,7 +77265,7 @@
         <v>1028</v>
       </c>
       <c r="AY3" s="14" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="AZ3" s="6" t="s">
         <v>309</v>
@@ -77437,7 +77431,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY4" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ4" s="11">
         <v>6</v>
@@ -77603,7 +77597,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY5" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ5" s="11">
         <v>6</v>
@@ -77765,7 +77759,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY6" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ6" s="4">
         <v>6</v>
@@ -77927,7 +77921,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY7" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ7" s="11">
         <v>6</v>
@@ -77949,16 +77943,16 @@
     </row>
     <row r="8" spans="1:58" ht="14.25">
       <c r="A8" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="E8" s="11">
         <v>4</v>
@@ -78020,7 +78014,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="Y8" s="22"/>
       <c r="Z8" s="53"/>
@@ -78089,7 +78083,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY8" s="56" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="AZ8" s="11">
         <v>6</v>
@@ -78111,16 +78105,16 @@
     </row>
     <row r="9" spans="1:58" ht="14.25">
       <c r="A9" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="E9" s="11">
         <v>3</v>
@@ -78182,7 +78176,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="11" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="53"/>
@@ -78251,7 +78245,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY9" s="56" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="AZ9" s="11">
         <v>6</v>
@@ -78417,7 +78411,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY10" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ10" s="36">
         <v>6</v>
@@ -78439,7 +78433,7 @@
     </row>
     <row r="11" spans="1:58" ht="14.25">
       <c r="A11" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>1133</v>
@@ -78583,7 +78577,7 @@
         <v>0;0;0;0;0;0;0;0;0</v>
       </c>
       <c r="AY11" s="56" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AZ11" s="11">
         <v>6</v>

</xml_diff>

<commit_message>
#24 finish new card lopsb
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,7 +23,7 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="1430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1436">
   <si>
     <t>arrow</t>
   </si>
@@ -5549,6 +5549,30 @@
   </si>
   <si>
     <t>55000116;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>压制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>洛欧塞布</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loatheb</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55000052;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkfire</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6625,7 +6649,45 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="137">
+  <dxfs count="142">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -9883,11 +9945,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2146182368"/>
-        <c:axId val="2146184000"/>
+        <c:axId val="2119222944"/>
+        <c:axId val="2119223488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2146182368"/>
+        <c:axId val="2119222944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9930,7 +9992,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2146184000"/>
+        <c:crossAx val="2119223488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9938,7 +10000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146184000"/>
+        <c:axId val="2119223488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9989,7 +10051,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2146182368"/>
+        <c:crossAx val="2119222944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11048,47 +11110,47 @@
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55000061</v>
+            <v>55000052</v>
           </cell>
           <cell r="V48">
-            <v>1</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55000062</v>
+            <v>55000061</v>
           </cell>
           <cell r="V49">
-            <v>4</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55000063</v>
+            <v>55000062</v>
           </cell>
           <cell r="V50">
-            <v>10</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55000064</v>
+            <v>55000063</v>
           </cell>
           <cell r="V51">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55000065</v>
+            <v>55000064</v>
           </cell>
           <cell r="V52">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55000066</v>
+            <v>55000065</v>
           </cell>
           <cell r="V53">
             <v>1</v>
@@ -11096,7 +11158,7 @@
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55000067</v>
+            <v>55000066</v>
           </cell>
           <cell r="V54">
             <v>1</v>
@@ -11104,7 +11166,7 @@
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55000068</v>
+            <v>55000067</v>
           </cell>
           <cell r="V55">
             <v>1</v>
@@ -11112,7 +11174,7 @@
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55000069</v>
+            <v>55000068</v>
           </cell>
           <cell r="V56">
             <v>1</v>
@@ -11120,7 +11182,7 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55000070</v>
+            <v>55000069</v>
           </cell>
           <cell r="V57">
             <v>1</v>
@@ -11128,7 +11190,7 @@
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55000071</v>
+            <v>55000070</v>
           </cell>
           <cell r="V58">
             <v>1</v>
@@ -11136,7 +11198,7 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55000072</v>
+            <v>55000071</v>
           </cell>
           <cell r="V59">
             <v>1</v>
@@ -11144,7 +11206,7 @@
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55000073</v>
+            <v>55000072</v>
           </cell>
           <cell r="V60">
             <v>1</v>
@@ -11152,7 +11214,7 @@
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55000074</v>
+            <v>55000073</v>
           </cell>
           <cell r="V61">
             <v>1</v>
@@ -11160,47 +11222,47 @@
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55000075</v>
+            <v>55000074</v>
           </cell>
           <cell r="V62">
-            <v>12</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55000076</v>
+            <v>55000075</v>
           </cell>
           <cell r="V63">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55000077</v>
+            <v>55000076</v>
           </cell>
           <cell r="V64">
-            <v>26</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55000078</v>
+            <v>55000077</v>
           </cell>
           <cell r="V65">
-            <v>-4</v>
+            <v>26</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55000079</v>
+            <v>55000078</v>
           </cell>
           <cell r="V66">
-            <v>2</v>
+            <v>-4</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55000080</v>
+            <v>55000079</v>
           </cell>
           <cell r="V67">
             <v>2</v>
@@ -11208,79 +11270,79 @@
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55000081</v>
+            <v>55000080</v>
           </cell>
           <cell r="V68">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55000082</v>
+            <v>55000081</v>
           </cell>
           <cell r="V69">
-            <v>6</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55000083</v>
+            <v>55000082</v>
           </cell>
           <cell r="V70">
-            <v>15</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55000084</v>
+            <v>55000083</v>
           </cell>
           <cell r="V71">
-            <v>35</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55000085</v>
+            <v>55000084</v>
           </cell>
           <cell r="V72">
-            <v>2</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55000086</v>
+            <v>55000085</v>
           </cell>
           <cell r="V73">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55000087</v>
+            <v>55000086</v>
           </cell>
           <cell r="V74">
-            <v>6</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55000088</v>
+            <v>55000087</v>
           </cell>
           <cell r="V75">
-            <v>3</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55000089</v>
+            <v>55000088</v>
           </cell>
           <cell r="V76">
-            <v>6</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55000090</v>
+            <v>55000089</v>
           </cell>
           <cell r="V77">
             <v>6</v>
@@ -11288,151 +11350,151 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55000091</v>
+            <v>55000090</v>
           </cell>
           <cell r="V78">
-            <v>-15</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55000092</v>
+            <v>55000091</v>
           </cell>
           <cell r="V79">
-            <v>5</v>
+            <v>-15</v>
           </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55000093</v>
+            <v>55000092</v>
           </cell>
           <cell r="V80">
-            <v>2</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55000094</v>
+            <v>55000093</v>
           </cell>
           <cell r="V81">
-            <v>30</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55000095</v>
+            <v>55000094</v>
           </cell>
           <cell r="V82">
-            <v>3</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55000096</v>
+            <v>55000095</v>
           </cell>
           <cell r="V83">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55000097</v>
+            <v>55000096</v>
           </cell>
           <cell r="V84">
-            <v>0</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55000098</v>
+            <v>55000097</v>
           </cell>
           <cell r="V85">
-            <v>4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55000099</v>
+            <v>55000098</v>
           </cell>
           <cell r="V86">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55000100</v>
+            <v>55000099</v>
           </cell>
           <cell r="V87">
-            <v>5</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55000101</v>
+            <v>55000100</v>
           </cell>
           <cell r="V88">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55000102</v>
+            <v>55000101</v>
           </cell>
           <cell r="V89">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55000103</v>
+            <v>55000102</v>
           </cell>
           <cell r="V90">
-            <v>10</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55000104</v>
+            <v>55000103</v>
           </cell>
           <cell r="V91">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55000105</v>
+            <v>55000104</v>
           </cell>
           <cell r="V92">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55000106</v>
+            <v>55000105</v>
           </cell>
           <cell r="V93">
-            <v>5</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55000107</v>
+            <v>55000106</v>
           </cell>
           <cell r="V94">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55000108</v>
+            <v>55000107</v>
           </cell>
           <cell r="V95">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55000109</v>
+            <v>55000108</v>
           </cell>
           <cell r="V96">
             <v>0</v>
@@ -11440,15 +11502,15 @@
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55000110</v>
+            <v>55000109</v>
           </cell>
           <cell r="V97">
-            <v>5</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55000111</v>
+            <v>55000110</v>
           </cell>
           <cell r="V98">
             <v>5</v>
@@ -11456,143 +11518,143 @@
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55000112</v>
+            <v>55000111</v>
           </cell>
           <cell r="V99">
-            <v>2</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55000113</v>
+            <v>55000112</v>
           </cell>
           <cell r="V100">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55000114</v>
+            <v>55000113</v>
           </cell>
           <cell r="V101">
-            <v>4</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55000115</v>
+            <v>55000114</v>
           </cell>
           <cell r="V102">
-            <v>20</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55000116</v>
+            <v>55000115</v>
           </cell>
           <cell r="V103">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55000117</v>
+            <v>55000116</v>
           </cell>
           <cell r="V104">
-            <v>1</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55000118</v>
+            <v>55000117</v>
           </cell>
           <cell r="V105">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55000119</v>
+            <v>55000118</v>
           </cell>
           <cell r="V106">
-            <v>7</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55000120</v>
+            <v>55000119</v>
           </cell>
           <cell r="V107">
-            <v>10</v>
+            <v>7</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55000121</v>
+            <v>55000120</v>
           </cell>
           <cell r="V108">
-            <v>3</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55000122</v>
+            <v>55000121</v>
           </cell>
           <cell r="V109">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55000123</v>
+            <v>55000122</v>
           </cell>
           <cell r="V110">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55000124</v>
+            <v>55000123</v>
           </cell>
           <cell r="V111">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55000125</v>
+            <v>55000124</v>
           </cell>
           <cell r="V112">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55000126</v>
+            <v>55000125</v>
           </cell>
           <cell r="V113">
-            <v>4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55000127</v>
+            <v>55000126</v>
           </cell>
           <cell r="V114">
-            <v>80</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55000129</v>
+            <v>55000127</v>
           </cell>
           <cell r="V115">
-            <v>3</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55000130</v>
+            <v>55000129</v>
           </cell>
           <cell r="V116">
             <v>3</v>
@@ -11600,31 +11662,31 @@
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55000131</v>
+            <v>55000130</v>
           </cell>
           <cell r="V117">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55000132</v>
+            <v>55000131</v>
           </cell>
           <cell r="V118">
-            <v>3</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55000133</v>
+            <v>55000132</v>
           </cell>
           <cell r="V119">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55000134</v>
+            <v>55000133</v>
           </cell>
           <cell r="V120">
             <v>5</v>
@@ -11632,47 +11694,47 @@
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55000135</v>
+            <v>55000134</v>
           </cell>
           <cell r="V121">
-            <v>-5</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55000136</v>
+            <v>55000135</v>
           </cell>
           <cell r="V122">
-            <v>6</v>
+            <v>-5</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55000137</v>
+            <v>55000136</v>
           </cell>
           <cell r="V123">
-            <v>1</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55000138</v>
+            <v>55000137</v>
           </cell>
           <cell r="V124">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55000139</v>
+            <v>55000138</v>
           </cell>
           <cell r="V125">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55000140</v>
+            <v>55000139</v>
           </cell>
           <cell r="V126">
             <v>1</v>
@@ -11680,7 +11742,7 @@
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55000141</v>
+            <v>55000140</v>
           </cell>
           <cell r="V127">
             <v>1</v>
@@ -11688,71 +11750,71 @@
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55000142</v>
+            <v>55000141</v>
           </cell>
           <cell r="V128">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55000143</v>
+            <v>55000142</v>
           </cell>
           <cell r="V129">
-            <v>4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55000144</v>
+            <v>55000143</v>
           </cell>
           <cell r="V130">
-            <v>1</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55000145</v>
+            <v>55000144</v>
           </cell>
           <cell r="V131">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55000146</v>
+            <v>55000145</v>
           </cell>
           <cell r="V132">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55000147</v>
+            <v>55000146</v>
           </cell>
           <cell r="V133">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55000148</v>
+            <v>55000147</v>
           </cell>
           <cell r="V134">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55000149</v>
+            <v>55000148</v>
           </cell>
           <cell r="V135">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55000150</v>
+            <v>55000149</v>
           </cell>
           <cell r="V136">
             <v>0</v>
@@ -11760,191 +11822,191 @@
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55000151</v>
+            <v>55000150</v>
           </cell>
           <cell r="V137">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55000152</v>
+            <v>55000151</v>
           </cell>
           <cell r="V138">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55000153</v>
+            <v>55000152</v>
           </cell>
           <cell r="V139">
-            <v>0</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55000154</v>
+            <v>55000153</v>
           </cell>
           <cell r="V140">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55000155</v>
+            <v>55000154</v>
           </cell>
           <cell r="V141">
-            <v>-2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55000156</v>
+            <v>55000155</v>
           </cell>
           <cell r="V142">
-            <v>0</v>
+            <v>-2</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55000157</v>
+            <v>55000156</v>
           </cell>
           <cell r="V143">
-            <v>30</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55000158</v>
+            <v>55000157</v>
           </cell>
           <cell r="V144">
-            <v>7</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55000159</v>
+            <v>55000158</v>
           </cell>
           <cell r="V145">
-            <v>1</v>
+            <v>7</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55000160</v>
+            <v>55000159</v>
           </cell>
           <cell r="V146">
-            <v>9</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55000161</v>
+            <v>55000160</v>
           </cell>
           <cell r="V147">
-            <v>0</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55000162</v>
+            <v>55000161</v>
           </cell>
           <cell r="V148">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55000163</v>
+            <v>55000162</v>
           </cell>
           <cell r="V149">
-            <v>10</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55000164</v>
+            <v>55000163</v>
           </cell>
           <cell r="V150">
-            <v>6</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55000165</v>
+            <v>55000164</v>
           </cell>
           <cell r="V151">
-            <v>2</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55000166</v>
+            <v>55000165</v>
           </cell>
           <cell r="V152">
-            <v>6</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55000167</v>
+            <v>55000166</v>
           </cell>
           <cell r="V153">
-            <v>10</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55000168</v>
+            <v>55000167</v>
           </cell>
           <cell r="V154">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55000169</v>
+            <v>55000168</v>
           </cell>
           <cell r="V155">
-            <v>5</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55000170</v>
+            <v>55000169</v>
           </cell>
           <cell r="V156">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55000171</v>
+            <v>55000170</v>
           </cell>
           <cell r="V157">
-            <v>4</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55000172</v>
+            <v>55000171</v>
           </cell>
           <cell r="V158">
-            <v>2</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55000173</v>
+            <v>55000172</v>
           </cell>
           <cell r="V159">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55000174</v>
+            <v>55000173</v>
           </cell>
           <cell r="V160">
             <v>1</v>
@@ -11952,7 +12014,7 @@
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55000175</v>
+            <v>55000174</v>
           </cell>
           <cell r="V161">
             <v>1</v>
@@ -11960,31 +12022,31 @@
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55000176</v>
+            <v>55000175</v>
           </cell>
           <cell r="V162">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55000177</v>
+            <v>55000176</v>
           </cell>
           <cell r="V163">
-            <v>0</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55000178</v>
+            <v>55000177</v>
           </cell>
           <cell r="V164">
-            <v>5</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55000179</v>
+            <v>55000178</v>
           </cell>
           <cell r="V165">
             <v>5</v>
@@ -11992,31 +12054,31 @@
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55000180</v>
+            <v>55000179</v>
           </cell>
           <cell r="V166">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55000181</v>
+            <v>55000180</v>
           </cell>
           <cell r="V167">
-            <v>40</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55000182</v>
+            <v>55000181</v>
           </cell>
           <cell r="V168">
-            <v>3</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55000183</v>
+            <v>55000182</v>
           </cell>
           <cell r="V169">
             <v>3</v>
@@ -12024,95 +12086,95 @@
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55000184</v>
+            <v>55000183</v>
           </cell>
           <cell r="V170">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55000185</v>
+            <v>55000184</v>
           </cell>
           <cell r="V171">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55000186</v>
+            <v>55000185</v>
           </cell>
           <cell r="V172">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55000187</v>
+            <v>55000186</v>
           </cell>
           <cell r="V173">
-            <v>-12</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55000188</v>
+            <v>55000187</v>
           </cell>
           <cell r="V174">
-            <v>-1</v>
+            <v>-12</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55000189</v>
+            <v>55000188</v>
           </cell>
           <cell r="V175">
-            <v>20</v>
+            <v>-1</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55000190</v>
+            <v>55000189</v>
           </cell>
           <cell r="V176">
-            <v>1</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55000191</v>
+            <v>55000190</v>
           </cell>
           <cell r="V177">
-            <v>22</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55000192</v>
+            <v>55000191</v>
           </cell>
           <cell r="V178">
-            <v>2</v>
+            <v>22</v>
           </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55000193</v>
+            <v>55000192</v>
           </cell>
           <cell r="V179">
-            <v>0</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55000194</v>
+            <v>55000193</v>
           </cell>
           <cell r="V180">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55000195</v>
+            <v>55000194</v>
           </cell>
           <cell r="V181">
             <v>1</v>
@@ -12120,7 +12182,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55000196</v>
+            <v>55000195</v>
           </cell>
           <cell r="V182">
             <v>1</v>
@@ -12128,79 +12190,79 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55000197</v>
+            <v>55000196</v>
           </cell>
           <cell r="V183">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55000198</v>
+            <v>55000197</v>
           </cell>
           <cell r="V184">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55000199</v>
+            <v>55000198</v>
           </cell>
           <cell r="V185">
-            <v>6</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55000200</v>
+            <v>55000199</v>
           </cell>
           <cell r="V186">
-            <v>14</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55000201</v>
+            <v>55000200</v>
           </cell>
           <cell r="V187">
-            <v>2</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55000202</v>
+            <v>55000201</v>
           </cell>
           <cell r="V188">
-            <v>10</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55000203</v>
+            <v>55000202</v>
           </cell>
           <cell r="V189">
-            <v>100</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55000204</v>
+            <v>55000203</v>
           </cell>
           <cell r="V190">
-            <v>0</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55000205</v>
+            <v>55000204</v>
           </cell>
           <cell r="V191">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55000206</v>
+            <v>55000205</v>
           </cell>
           <cell r="V192">
             <v>1</v>
@@ -12208,23 +12270,23 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55000207</v>
+            <v>55000206</v>
           </cell>
           <cell r="V193">
-            <v>25</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55000208</v>
+            <v>55000207</v>
           </cell>
           <cell r="V194">
-            <v>0</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55000209</v>
+            <v>55000208</v>
           </cell>
           <cell r="V195">
             <v>0</v>
@@ -12232,135 +12294,135 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55000210</v>
+            <v>55000209</v>
           </cell>
           <cell r="V196">
-            <v>6</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55000211</v>
+            <v>55000210</v>
           </cell>
           <cell r="V197">
-            <v>0</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55000212</v>
+            <v>55000211</v>
           </cell>
           <cell r="V198">
-            <v>3</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55000213</v>
+            <v>55000212</v>
           </cell>
           <cell r="V199">
-            <v>0</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55000214</v>
+            <v>55000213</v>
           </cell>
           <cell r="V200">
-            <v>15</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55000215</v>
+            <v>55000214</v>
           </cell>
           <cell r="V201">
-            <v>4</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55000216</v>
+            <v>55000215</v>
           </cell>
           <cell r="V202">
-            <v>5</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55000217</v>
+            <v>55000216</v>
           </cell>
           <cell r="V203">
-            <v>2</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="204">
           <cell r="A204">
-            <v>55000218</v>
+            <v>55000217</v>
           </cell>
           <cell r="V204">
-            <v>8</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="205">
           <cell r="A205">
-            <v>55000219</v>
+            <v>55000218</v>
           </cell>
           <cell r="V205">
-            <v>2</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="206">
           <cell r="A206">
-            <v>55000220</v>
+            <v>55000219</v>
           </cell>
           <cell r="V206">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>55000221</v>
+            <v>55000220</v>
           </cell>
           <cell r="V207">
-            <v>80</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>55000222</v>
+            <v>55000221</v>
           </cell>
           <cell r="V208">
-            <v>4</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="209">
           <cell r="A209">
-            <v>55000223</v>
+            <v>55000222</v>
           </cell>
           <cell r="V209">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="210">
           <cell r="A210">
-            <v>55000224</v>
+            <v>55000223</v>
           </cell>
           <cell r="V210">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="211">
           <cell r="A211">
-            <v>55000225</v>
+            <v>55000224</v>
           </cell>
           <cell r="V211">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="212">
           <cell r="A212">
-            <v>55000226</v>
+            <v>55000225</v>
           </cell>
           <cell r="V212">
             <v>5</v>
@@ -12368,143 +12430,143 @@
         </row>
         <row r="213">
           <cell r="A213">
-            <v>55000227</v>
+            <v>55000226</v>
           </cell>
           <cell r="V213">
-            <v>3</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="214">
           <cell r="A214">
-            <v>55000228</v>
+            <v>55000227</v>
           </cell>
           <cell r="V214">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="215">
           <cell r="A215">
-            <v>55000229</v>
+            <v>55000228</v>
           </cell>
           <cell r="V215">
-            <v>30</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="216">
           <cell r="A216">
-            <v>55000230</v>
+            <v>55000229</v>
           </cell>
           <cell r="V216">
-            <v>-18</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="217">
           <cell r="A217">
-            <v>55000231</v>
+            <v>55000230</v>
           </cell>
           <cell r="V217">
-            <v>15</v>
+            <v>-18</v>
           </cell>
         </row>
         <row r="218">
           <cell r="A218">
-            <v>55000232</v>
+            <v>55000231</v>
           </cell>
           <cell r="V218">
-            <v>3</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="219">
           <cell r="A219">
-            <v>55000233</v>
+            <v>55000232</v>
           </cell>
           <cell r="V219">
-            <v>-2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="220">
           <cell r="A220">
-            <v>55000234</v>
+            <v>55000233</v>
           </cell>
           <cell r="V220">
-            <v>3</v>
+            <v>-2</v>
           </cell>
         </row>
         <row r="221">
           <cell r="A221">
-            <v>55000235</v>
+            <v>55000234</v>
           </cell>
           <cell r="V221">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="222">
           <cell r="A222">
-            <v>55000236</v>
+            <v>55000235</v>
           </cell>
           <cell r="V222">
-            <v>5</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="223">
           <cell r="A223">
-            <v>55000237</v>
+            <v>55000236</v>
           </cell>
           <cell r="V223">
-            <v>0</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="224">
           <cell r="A224">
-            <v>55000238</v>
+            <v>55000237</v>
           </cell>
           <cell r="V224">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="225">
           <cell r="A225">
-            <v>55000239</v>
+            <v>55000238</v>
           </cell>
           <cell r="V225">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="226">
           <cell r="A226">
-            <v>55000240</v>
+            <v>55000239</v>
           </cell>
           <cell r="V226">
-            <v>5</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="227">
           <cell r="A227">
-            <v>55000241</v>
+            <v>55000240</v>
           </cell>
           <cell r="V227">
-            <v>0</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="228">
           <cell r="A228">
-            <v>55000242</v>
+            <v>55000241</v>
           </cell>
           <cell r="V228">
-            <v>3</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="229">
           <cell r="A229">
-            <v>55000243</v>
+            <v>55000242</v>
           </cell>
           <cell r="V229">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="230">
           <cell r="A230">
-            <v>55000244</v>
+            <v>55000243</v>
           </cell>
           <cell r="V230">
             <v>2</v>
@@ -12512,23 +12574,23 @@
         </row>
         <row r="231">
           <cell r="A231">
-            <v>55000245</v>
+            <v>55000244</v>
           </cell>
           <cell r="V231">
-            <v>4</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="232">
           <cell r="A232">
-            <v>55000246</v>
+            <v>55000245</v>
           </cell>
           <cell r="V232">
-            <v>1</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="233">
           <cell r="A233">
-            <v>55000247</v>
+            <v>55000246</v>
           </cell>
           <cell r="V233">
             <v>1</v>
@@ -12536,311 +12598,311 @@
         </row>
         <row r="234">
           <cell r="A234">
-            <v>55000248</v>
+            <v>55000247</v>
           </cell>
           <cell r="V234">
-            <v>8</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="235">
           <cell r="A235">
-            <v>55000249</v>
+            <v>55000248</v>
           </cell>
           <cell r="V235">
-            <v>4</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="236">
           <cell r="A236">
-            <v>55000250</v>
+            <v>55000249</v>
           </cell>
           <cell r="V236">
-            <v>3</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="237">
           <cell r="A237">
-            <v>55000251</v>
+            <v>55000250</v>
           </cell>
           <cell r="V237">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="238">
           <cell r="A238">
-            <v>55000252</v>
+            <v>55000251</v>
           </cell>
           <cell r="V238">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="239">
           <cell r="A239">
-            <v>55000253</v>
+            <v>55000252</v>
           </cell>
           <cell r="V239">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="240">
           <cell r="A240">
-            <v>55000254</v>
+            <v>55000253</v>
           </cell>
           <cell r="V240">
-            <v>3</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="241">
           <cell r="A241">
-            <v>55000255</v>
+            <v>55000254</v>
           </cell>
           <cell r="V241">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="242">
           <cell r="A242">
-            <v>55000256</v>
+            <v>55000255</v>
           </cell>
           <cell r="V242">
-            <v>0</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="243">
           <cell r="A243">
-            <v>55000257</v>
+            <v>55000256</v>
           </cell>
           <cell r="V243">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="244">
           <cell r="A244">
-            <v>55000258</v>
+            <v>55000257</v>
           </cell>
           <cell r="V244">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="245">
           <cell r="A245">
-            <v>55000259</v>
+            <v>55000258</v>
           </cell>
           <cell r="V245">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="246">
           <cell r="A246">
-            <v>55000260</v>
+            <v>55000259</v>
           </cell>
           <cell r="V246">
-            <v>3</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="247">
           <cell r="A247">
-            <v>55000261</v>
+            <v>55000260</v>
           </cell>
           <cell r="V247">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="248">
           <cell r="A248">
-            <v>55000262</v>
+            <v>55000261</v>
           </cell>
           <cell r="V248">
-            <v>22</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="249">
           <cell r="A249">
-            <v>55000263</v>
+            <v>55000262</v>
           </cell>
           <cell r="V249">
-            <v>10</v>
+            <v>22</v>
           </cell>
         </row>
         <row r="250">
           <cell r="A250">
-            <v>55000264</v>
+            <v>55000263</v>
           </cell>
           <cell r="V250">
-            <v>3</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="251">
           <cell r="A251">
-            <v>55000265</v>
+            <v>55000264</v>
           </cell>
           <cell r="V251">
-            <v>10</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="252">
           <cell r="A252">
-            <v>55000266</v>
+            <v>55000265</v>
           </cell>
           <cell r="V252">
-            <v>1</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="253">
           <cell r="A253">
-            <v>55000267</v>
+            <v>55000266</v>
           </cell>
           <cell r="V253">
-            <v>25</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="254">
           <cell r="A254">
-            <v>55000268</v>
+            <v>55000267</v>
           </cell>
           <cell r="V254">
-            <v>2</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="255">
           <cell r="A255">
-            <v>55000269</v>
+            <v>55000268</v>
           </cell>
           <cell r="V255">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="256">
           <cell r="A256">
-            <v>55000270</v>
+            <v>55000269</v>
           </cell>
           <cell r="V256">
-            <v>0</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="257">
           <cell r="A257">
-            <v>55000271</v>
+            <v>55000270</v>
           </cell>
           <cell r="V257">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="258">
           <cell r="A258">
-            <v>55000272</v>
+            <v>55000271</v>
           </cell>
           <cell r="V258">
-            <v>25</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="259">
           <cell r="A259">
-            <v>55000273</v>
+            <v>55000272</v>
           </cell>
           <cell r="V259">
-            <v>4</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="260">
           <cell r="A260">
-            <v>55000274</v>
+            <v>55000273</v>
           </cell>
           <cell r="V260">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="261">
           <cell r="A261">
-            <v>55000275</v>
+            <v>55000274</v>
           </cell>
           <cell r="V261">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="262">
           <cell r="A262">
-            <v>55000276</v>
+            <v>55000275</v>
           </cell>
           <cell r="V262">
-            <v>30</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="263">
           <cell r="A263">
-            <v>55000277</v>
+            <v>55000276</v>
           </cell>
           <cell r="V263">
-            <v>1</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="264">
           <cell r="A264">
-            <v>55000278</v>
+            <v>55000277</v>
           </cell>
           <cell r="V264">
-            <v>9</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="265">
           <cell r="A265">
-            <v>55000279</v>
+            <v>55000278</v>
           </cell>
           <cell r="V265">
-            <v>8</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="266">
           <cell r="A266">
-            <v>55000280</v>
+            <v>55000279</v>
           </cell>
           <cell r="V266">
-            <v>2</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="267">
           <cell r="A267">
-            <v>55000281</v>
+            <v>55000280</v>
           </cell>
           <cell r="V267">
-            <v>15</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="268">
           <cell r="A268">
-            <v>55000282</v>
+            <v>55000281</v>
           </cell>
           <cell r="V268">
-            <v>1</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="269">
           <cell r="A269">
-            <v>55000284</v>
+            <v>55000282</v>
           </cell>
           <cell r="V269">
-            <v>6</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="270">
           <cell r="A270">
-            <v>55000285</v>
+            <v>55000284</v>
           </cell>
           <cell r="V270">
-            <v>4</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="271">
           <cell r="A271">
-            <v>55000286</v>
+            <v>55000285</v>
           </cell>
           <cell r="V271">
-            <v>3</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="272">
           <cell r="A272">
-            <v>55000287</v>
+            <v>55000286</v>
           </cell>
           <cell r="V272">
             <v>3</v>
@@ -12848,87 +12910,87 @@
         </row>
         <row r="273">
           <cell r="A273">
-            <v>55000288</v>
+            <v>55000287</v>
           </cell>
           <cell r="V273">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="274">
           <cell r="A274">
-            <v>55000289</v>
+            <v>55000288</v>
           </cell>
           <cell r="V274">
-            <v>8</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="275">
           <cell r="A275">
-            <v>55000290</v>
+            <v>55000289</v>
           </cell>
           <cell r="V275">
-            <v>6</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="276">
           <cell r="A276">
-            <v>55000291</v>
+            <v>55000290</v>
           </cell>
           <cell r="V276">
-            <v>4</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="277">
           <cell r="A277">
-            <v>55000292</v>
+            <v>55000291</v>
           </cell>
           <cell r="V277">
-            <v>9</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="278">
           <cell r="A278">
-            <v>55000293</v>
+            <v>55000292</v>
           </cell>
           <cell r="V278">
-            <v>1</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="279">
           <cell r="A279">
-            <v>55000294</v>
+            <v>55000293</v>
           </cell>
           <cell r="V279">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="280">
           <cell r="A280">
-            <v>55000295</v>
+            <v>55000294</v>
           </cell>
           <cell r="V280">
-            <v>4</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="281">
           <cell r="A281">
-            <v>55000296</v>
+            <v>55000295</v>
           </cell>
           <cell r="V281">
-            <v>3</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="282">
           <cell r="A282">
-            <v>55000297</v>
+            <v>55000296</v>
           </cell>
           <cell r="V282">
-            <v>2</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="283">
           <cell r="A283">
-            <v>55000298</v>
+            <v>55000297</v>
           </cell>
           <cell r="V283">
             <v>2</v>
@@ -12936,31 +12998,31 @@
         </row>
         <row r="284">
           <cell r="A284">
-            <v>55000299</v>
+            <v>55000298</v>
           </cell>
           <cell r="V284">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="285">
           <cell r="A285">
-            <v>55000300</v>
+            <v>55000299</v>
           </cell>
           <cell r="V285">
-            <v>80</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="286">
           <cell r="A286">
-            <v>55000324</v>
+            <v>55000300</v>
           </cell>
           <cell r="V286">
-            <v>5</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="287">
           <cell r="A287">
-            <v>55000325</v>
+            <v>55000324</v>
           </cell>
           <cell r="V287">
             <v>5</v>
@@ -12968,63 +13030,63 @@
         </row>
         <row r="288">
           <cell r="A288">
-            <v>55000326</v>
+            <v>55000325</v>
           </cell>
           <cell r="V288">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="289">
           <cell r="A289">
-            <v>55000327</v>
+            <v>55000326</v>
           </cell>
           <cell r="V289">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="290">
           <cell r="A290">
-            <v>55000328</v>
+            <v>55000327</v>
           </cell>
           <cell r="V290">
-            <v>7</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="291">
           <cell r="A291">
-            <v>55000329</v>
+            <v>55000328</v>
           </cell>
           <cell r="V291">
-            <v>6</v>
+            <v>7</v>
           </cell>
         </row>
         <row r="292">
           <cell r="A292">
-            <v>55000330</v>
+            <v>55000329</v>
           </cell>
           <cell r="V292">
-            <v>4</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="293">
           <cell r="A293">
-            <v>55000331</v>
+            <v>55000330</v>
           </cell>
           <cell r="V293">
-            <v>6</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="294">
           <cell r="A294">
-            <v>55000332</v>
+            <v>55000331</v>
           </cell>
           <cell r="V294">
-            <v>0</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="295">
           <cell r="A295">
-            <v>55000333</v>
+            <v>55000332</v>
           </cell>
           <cell r="V295">
             <v>0</v>
@@ -13032,65 +13094,73 @@
         </row>
         <row r="296">
           <cell r="A296">
-            <v>55000334</v>
+            <v>55000333</v>
           </cell>
           <cell r="V296">
-            <v>2</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="297">
           <cell r="A297">
-            <v>55000335</v>
+            <v>55000334</v>
           </cell>
           <cell r="V297">
-            <v>15</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="298">
           <cell r="A298">
-            <v>55000340</v>
+            <v>55000335</v>
           </cell>
           <cell r="V298">
-            <v>2</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="299">
           <cell r="A299">
-            <v>55000341</v>
+            <v>55000340</v>
           </cell>
           <cell r="V299">
-            <v>8</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="300">
           <cell r="A300">
-            <v>55000342</v>
+            <v>55000341</v>
           </cell>
           <cell r="V300">
-            <v>4</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="301">
           <cell r="A301">
+            <v>55000342</v>
+          </cell>
+          <cell r="V301">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="302">
+          <cell r="A302">
             <v>55000343</v>
           </cell>
-          <cell r="V301">
+          <cell r="V302">
             <v>6</v>
           </cell>
         </row>
-        <row r="302">
-          <cell r="A302" t="str">
+        <row r="303">
+          <cell r="A303" t="str">
             <v>55000060|FightQuick</v>
           </cell>
-          <cell r="V302">
+          <cell r="V303">
             <v>1</v>
           </cell>
         </row>
-        <row r="303">
-          <cell r="A303">
+        <row r="304">
+          <cell r="A304">
             <v>55000344</v>
           </cell>
-          <cell r="V303">
+          <cell r="V304">
             <v>40</v>
           </cell>
         </row>
@@ -22030,7 +22100,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -22128,173 +22198,173 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BF313" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130" tableBorderDxfId="129">
-  <autoFilter ref="A3:BF313"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BF314" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135" tableBorderDxfId="134">
+  <autoFilter ref="A3:BF314"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="Id" dataDxfId="128"/>
-    <tableColumn id="2" name="Name" dataDxfId="127"/>
-    <tableColumn id="22" name="Ename" dataDxfId="126"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="125"/>
-    <tableColumn id="3" name="Star" dataDxfId="124"/>
-    <tableColumn id="4" name="Type" dataDxfId="123"/>
-    <tableColumn id="5" name="Attr" dataDxfId="122"/>
-    <tableColumn id="58" name="Quality" dataDxfId="121">
+    <tableColumn id="1" name="Id" dataDxfId="133"/>
+    <tableColumn id="2" name="Name" dataDxfId="132"/>
+    <tableColumn id="22" name="Ename" dataDxfId="131"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="130"/>
+    <tableColumn id="3" name="Star" dataDxfId="129"/>
+    <tableColumn id="4" name="Type" dataDxfId="128"/>
+    <tableColumn id="5" name="Attr" dataDxfId="127"/>
+    <tableColumn id="58" name="Quality" dataDxfId="126">
       <calculatedColumnFormula>IF(T4&gt;10,5,IF(T4&gt;5,4,IF(T4&gt;2.5,3,IF(T4&gt;0,2,IF(T4&gt;-2.5,1,IF(T4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="120"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="119"/>
-    <tableColumn id="24" name="VitP" dataDxfId="118"/>
-    <tableColumn id="25" name="Modify" dataDxfId="117"/>
-    <tableColumn id="9" name="Def" dataDxfId="116"/>
-    <tableColumn id="10" name="Mag" dataDxfId="115"/>
-    <tableColumn id="32" name="Spd" dataDxfId="114"/>
-    <tableColumn id="35" name="Hit" dataDxfId="113"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="112"/>
-    <tableColumn id="34" name="Crt" dataDxfId="111"/>
-    <tableColumn id="33" name="Luk" dataDxfId="110"/>
-    <tableColumn id="7" name="Sum" dataDxfId="109">
+    <tableColumn id="12" name="Cost" dataDxfId="125"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="124"/>
+    <tableColumn id="24" name="VitP" dataDxfId="123"/>
+    <tableColumn id="25" name="Modify" dataDxfId="122"/>
+    <tableColumn id="9" name="Def" dataDxfId="121"/>
+    <tableColumn id="10" name="Mag" dataDxfId="120"/>
+    <tableColumn id="32" name="Spd" dataDxfId="119"/>
+    <tableColumn id="35" name="Hit" dataDxfId="118"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="117"/>
+    <tableColumn id="34" name="Crt" dataDxfId="116"/>
+    <tableColumn id="33" name="Luk" dataDxfId="115"/>
+    <tableColumn id="7" name="Sum" dataDxfId="114">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AW4)+2.5*SUM(AI4:AM4)+AH4+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="108"/>
-    <tableColumn id="14" name="Mov" dataDxfId="107"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="106"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="105"/>
-    <tableColumn id="18" name="Skills" dataDxfId="104"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="103"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="102"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="101"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="100"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="99"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="98"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="97"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="96"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="95">
+    <tableColumn id="13" name="Range" dataDxfId="113"/>
+    <tableColumn id="14" name="Mov" dataDxfId="112"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="111"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="110"/>
+    <tableColumn id="18" name="Skills" dataDxfId="109"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="108"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="107"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="106"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="105"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="104"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="103"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="102"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="101"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="100">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="94"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="93"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="92"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="91"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="90"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="89">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="99"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="98"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="97"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="96"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="95"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="94">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="88"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="87"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="86"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="85"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="84"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="83"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="82"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="81"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="80"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="79">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="93"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="92"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="91"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="90"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="89"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="88"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="87"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="86"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="85"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="84">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="78"/>
-    <tableColumn id="20" name="Res" dataDxfId="77"/>
-    <tableColumn id="21" name="Icon" dataDxfId="76"/>
-    <tableColumn id="17" name="Cover" dataDxfId="75"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="74"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="73"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="72"/>
-    <tableColumn id="29" name="Remark" dataDxfId="71"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="83"/>
+    <tableColumn id="20" name="Res" dataDxfId="82"/>
+    <tableColumn id="21" name="Icon" dataDxfId="81"/>
+    <tableColumn id="17" name="Cover" dataDxfId="80"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="79"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="78"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="77"/>
+    <tableColumn id="29" name="Remark" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BF11" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BF11" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A3:BF11"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="Id" dataDxfId="58"/>
-    <tableColumn id="2" name="Name" dataDxfId="57"/>
-    <tableColumn id="22" name="Ename" dataDxfId="56"/>
-    <tableColumn id="23" name="EnameShort" dataDxfId="55"/>
-    <tableColumn id="3" name="Star" dataDxfId="54"/>
-    <tableColumn id="4" name="Type" dataDxfId="53"/>
-    <tableColumn id="5" name="Attr" dataDxfId="52"/>
-    <tableColumn id="58" name="Quality" dataDxfId="51">
+    <tableColumn id="1" name="Id" dataDxfId="63"/>
+    <tableColumn id="2" name="Name" dataDxfId="62"/>
+    <tableColumn id="22" name="Ename" dataDxfId="61"/>
+    <tableColumn id="23" name="EnameShort" dataDxfId="60"/>
+    <tableColumn id="3" name="Star" dataDxfId="59"/>
+    <tableColumn id="4" name="Type" dataDxfId="58"/>
+    <tableColumn id="5" name="Attr" dataDxfId="57"/>
+    <tableColumn id="58" name="Quality" dataDxfId="56">
       <calculatedColumnFormula>IF(T4&gt;10,5,IF(T4&gt;5,4,IF(T4&gt;2.5,3,IF(T4&gt;0,2,IF(T4&gt;-2.5,1,IF(T4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="50"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="49"/>
-    <tableColumn id="24" name="VitP" dataDxfId="48"/>
-    <tableColumn id="25" name="Modify" dataDxfId="47"/>
-    <tableColumn id="9" name="Def" dataDxfId="46"/>
-    <tableColumn id="10" name="Mag" dataDxfId="45"/>
-    <tableColumn id="32" name="Spd" dataDxfId="44"/>
-    <tableColumn id="35" name="Hit" dataDxfId="43"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="42"/>
-    <tableColumn id="34" name="Crt" dataDxfId="41"/>
-    <tableColumn id="33" name="Luk" dataDxfId="40"/>
-    <tableColumn id="7" name="Sum" dataDxfId="39">
+    <tableColumn id="12" name="Cost" dataDxfId="55"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="54"/>
+    <tableColumn id="24" name="VitP" dataDxfId="53"/>
+    <tableColumn id="25" name="Modify" dataDxfId="52"/>
+    <tableColumn id="9" name="Def" dataDxfId="51"/>
+    <tableColumn id="10" name="Mag" dataDxfId="50"/>
+    <tableColumn id="32" name="Spd" dataDxfId="49"/>
+    <tableColumn id="35" name="Hit" dataDxfId="48"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="47"/>
+    <tableColumn id="34" name="Crt" dataDxfId="46"/>
+    <tableColumn id="33" name="Luk" dataDxfId="45"/>
+    <tableColumn id="7" name="Sum" dataDxfId="44">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AW4)+2.5*SUM(AI4:AM4)+AH4+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="38"/>
-    <tableColumn id="14" name="Mov" dataDxfId="37"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="36"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="35"/>
-    <tableColumn id="18" name="Skills" dataDxfId="34"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="33"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="32"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="31"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="30"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="29"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="28"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="27"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="26"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
+    <tableColumn id="13" name="Range" dataDxfId="43"/>
+    <tableColumn id="14" name="Mov" dataDxfId="42"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="41"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="40"/>
+    <tableColumn id="18" name="Skills" dataDxfId="39"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="38"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="37"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="36"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="35"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="34"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="33"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="32"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="31"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="30">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="29"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="28"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="27"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="26"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="25"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
-    <tableColumn id="38" name="~AntiIce" dataDxfId="13"/>
-    <tableColumn id="39" name="~AntiThunder" dataDxfId="12"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="9">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="23"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="22"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="21"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="20"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="19"/>
+    <tableColumn id="38" name="~AntiIce" dataDxfId="18"/>
+    <tableColumn id="39" name="~AntiThunder" dataDxfId="17"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="16"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="15"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="14">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4,";",AV4,";",AW4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
-    <tableColumn id="20" name="Res" dataDxfId="7"/>
-    <tableColumn id="21" name="Icon" dataDxfId="6"/>
-    <tableColumn id="17" name="Cover" dataDxfId="5"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
-    <tableColumn id="29" name="Remark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="13"/>
+    <tableColumn id="20" name="Res" dataDxfId="12"/>
+    <tableColumn id="21" name="Icon" dataDxfId="11"/>
+    <tableColumn id="17" name="Cover" dataDxfId="10"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="9"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="8"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="7"/>
+    <tableColumn id="29" name="Remark" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -22598,13 +22668,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF313"/>
+  <dimension ref="A1:BF314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B299" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I85" sqref="I85"/>
+      <selection pane="bottomRight" activeCell="X314" sqref="X314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -27718,7 +27788,7 @@
       </c>
       <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I31" s="4">
         <v>3</v>
@@ -27755,7 +27825,7 @@
       </c>
       <c r="T31" s="15">
         <f t="shared" si="1"/>
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="U31" s="4">
         <v>10</v>
@@ -27793,7 +27863,7 @@
 IF(ISBLANK($AB31),0, LOOKUP($AB31,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC31/100)+
 IF(ISBLANK($AD31),0, LOOKUP($AD31,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE31/100)+
 IF(ISBLANK($AF31),0, LOOKUP($AF31,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG31/100)</f>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="AI31" s="21">
         <v>0</v>
@@ -27929,7 +27999,7 @@
       </c>
       <c r="T32" s="15">
         <f t="shared" si="1"/>
-        <v>53.4</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="U32" s="4">
         <v>10</v>
@@ -27971,7 +28041,7 @@
 IF(ISBLANK($AB32),0, LOOKUP($AB32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC32/100)+
 IF(ISBLANK($AD32),0, LOOKUP($AD32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE32/100)+
 IF(ISBLANK($AF32),0, LOOKUP($AF32,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG32/100)</f>
-        <v>46.4</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="AI32" s="21">
         <v>0</v>
@@ -34196,7 +34266,7 @@
       </c>
       <c r="H69" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I69" s="4">
         <v>6</v>
@@ -34233,7 +34303,7 @@
       </c>
       <c r="T69" s="15">
         <f t="shared" si="5"/>
-        <v>9.7200000000000006</v>
+        <v>29.72</v>
       </c>
       <c r="U69" s="4">
         <v>10</v>
@@ -34275,7 +34345,7 @@
 IF(ISBLANK($AB69),0, LOOKUP($AB69,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC69/100)+
 IF(ISBLANK($AD69),0, LOOKUP($AD69,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE69/100)+
 IF(ISBLANK($AF69),0, LOOKUP($AF69,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG69/100)</f>
-        <v>6.4</v>
+        <v>26.4</v>
       </c>
       <c r="AI69" s="21">
         <v>0</v>
@@ -34937,7 +35007,7 @@
       </c>
       <c r="T73" s="15">
         <f t="shared" si="5"/>
-        <v>32.5</v>
+        <v>52.5</v>
       </c>
       <c r="U73" s="4">
         <v>40</v>
@@ -34975,7 +35045,7 @@
 IF(ISBLANK($AB73),0, LOOKUP($AB73,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC73/100)+
 IF(ISBLANK($AD73),0, LOOKUP($AD73,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE73/100)+
 IF(ISBLANK($AF73),0, LOOKUP($AF73,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG73/100)</f>
-        <v>5.5</v>
+        <v>25.5</v>
       </c>
       <c r="AI73" s="21">
         <v>0</v>
@@ -56974,7 +57044,7 @@
       </c>
       <c r="H200" s="4">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I200" s="4">
         <v>5</v>
@@ -57011,7 +57081,7 @@
       </c>
       <c r="T200" s="15">
         <f t="shared" si="13"/>
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="U200" s="4">
         <v>10</v>
@@ -57053,7 +57123,7 @@
 IF(ISBLANK($AB200),0, LOOKUP($AB200,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC200/100)+
 IF(ISBLANK($AD200),0, LOOKUP($AD200,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE200/100)+
 IF(ISBLANK($AF200),0, LOOKUP($AF200,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG200/100)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="AI200" s="21">
         <v>0</v>
@@ -59271,7 +59341,7 @@
         <v>0</v>
       </c>
       <c r="X213" s="4" t="s">
-        <v>228</v>
+        <v>1435</v>
       </c>
       <c r="Y213" s="4" t="s">
         <v>1366</v>
@@ -63407,7 +63477,7 @@
       </c>
       <c r="T237" s="15">
         <f t="shared" si="13"/>
-        <v>61.5</v>
+        <v>81.5</v>
       </c>
       <c r="U237" s="4">
         <v>10</v>
@@ -63453,7 +63523,7 @@
 IF(ISBLANK($AB237),0, LOOKUP($AB237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC237/100)+
 IF(ISBLANK($AD237),0, LOOKUP($AD237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE237/100)+
 IF(ISBLANK($AF237),0, LOOKUP($AF237,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG237/100)</f>
-        <v>48.5</v>
+        <v>68.5</v>
       </c>
       <c r="AI237" s="21">
         <v>0</v>
@@ -76682,10 +76752,180 @@
         <v>1426</v>
       </c>
     </row>
+    <row r="314" spans="1:58" ht="14.25">
+      <c r="A314">
+        <v>51000311</v>
+      </c>
+      <c r="B314" s="11" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C314" s="11" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D314" s="8" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E314" s="11">
+        <v>4</v>
+      </c>
+      <c r="F314" s="11">
+        <v>1</v>
+      </c>
+      <c r="G314" s="11">
+        <v>3</v>
+      </c>
+      <c r="H314" s="24">
+        <f t="shared" ref="H314" si="24">IF(T314&gt;10,5,IF(T314&gt;5,4,IF(T314&gt;2.5,3,IF(T314&gt;0,2,IF(T314&gt;-2.5,1,IF(T314&gt;-10,0,6))))))</f>
+        <v>4</v>
+      </c>
+      <c r="I314" s="11">
+        <v>4</v>
+      </c>
+      <c r="J314" s="11">
+        <v>-3</v>
+      </c>
+      <c r="K314" s="11">
+        <v>3</v>
+      </c>
+      <c r="L314" s="11">
+        <v>-17</v>
+      </c>
+      <c r="M314" s="11">
+        <v>0</v>
+      </c>
+      <c r="N314" s="11">
+        <v>0</v>
+      </c>
+      <c r="O314" s="11">
+        <v>0</v>
+      </c>
+      <c r="P314" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q314" s="11">
+        <v>0</v>
+      </c>
+      <c r="R314" s="11">
+        <v>0</v>
+      </c>
+      <c r="S314" s="11">
+        <v>0</v>
+      </c>
+      <c r="T314" s="24">
+        <f t="shared" ref="T314" si="25">SUM(J314:K314)+SUM(M314:S314)*5+4.4*SUM(AO314:AW314)+2.5*SUM(AI314:AM314)+AH314+L314</f>
+        <v>8</v>
+      </c>
+      <c r="U314" s="11">
+        <v>10</v>
+      </c>
+      <c r="V314" s="11">
+        <v>10</v>
+      </c>
+      <c r="W314" s="11">
+        <v>0</v>
+      </c>
+      <c r="X314" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y314" s="11" t="s">
+        <v>1434</v>
+      </c>
+      <c r="Z314" s="21">
+        <v>55000052</v>
+      </c>
+      <c r="AA314" s="21">
+        <v>100</v>
+      </c>
+      <c r="AB314" s="21"/>
+      <c r="AC314" s="21"/>
+      <c r="AD314" s="21"/>
+      <c r="AE314" s="21"/>
+      <c r="AF314" s="21"/>
+      <c r="AG314" s="21"/>
+      <c r="AH314" s="21">
+        <f>IF(ISBLANK($Z314),0, LOOKUP($Z314,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AA314/100)+
+IF(ISBLANK($AB314),0, LOOKUP($AB314,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC314/100)+
+IF(ISBLANK($AD314),0, LOOKUP($AD314,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE314/100)+
+IF(ISBLANK($AF314),0, LOOKUP($AF314,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG314/100)</f>
+        <v>25</v>
+      </c>
+      <c r="AI314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AJ314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AK314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AL314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AM314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN314" s="11" t="str">
+        <f t="shared" ref="AN314" si="26">CONCATENATE(AI314,";",AJ314,";",AK314,";",AL314,";",AM314)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AO314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AP314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AQ314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AR314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AV314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AW314" s="21">
+        <v>0</v>
+      </c>
+      <c r="AX314" s="11" t="str">
+        <f t="shared" ref="AX314" si="27">CONCATENATE(AO314,";",AP314,";",AQ314,";",AR314,";",AS314,";",AT314,";",AU314,";",AV314,";",AW314)</f>
+        <v>0;0;0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AY314" s="57" t="s">
+        <v>1409</v>
+      </c>
+      <c r="AZ314" s="11">
+        <v>6</v>
+      </c>
+      <c r="BA314" s="11">
+        <v>311</v>
+      </c>
+      <c r="BB314" s="11"/>
+      <c r="BC314" s="24">
+        <v>0</v>
+      </c>
+      <c r="BD314" s="11">
+        <v>1</v>
+      </c>
+      <c r="BE314" s="11">
+        <v>0.49672129999999998</v>
+      </c>
+      <c r="BF314" s="11" t="s">
+        <v>1430</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="T4:T313">
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="T4:T314">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -76696,21 +76936,50 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H313">
-    <cfRule type="cellIs" dxfId="136" priority="12" operator="equal">
+  <conditionalFormatting sqref="H4:H314">
+    <cfRule type="cellIs" dxfId="141" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="7" operator="equal">
       <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T314">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H314">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -78600,31 +78869,31 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4:K7 K10:K11">
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="69" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J7">
-    <cfRule type="cellIs" dxfId="68" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="67" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="9" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78642,13 +78911,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="65" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="5" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="64" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -78666,13 +78935,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
close #23 use SpikeManager to manager spike related code
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -13165,10 +13165,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -22671,10 +22671,10 @@
   <dimension ref="A1:BF314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B299" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AG302" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X314" sqref="X314"/>
+      <selection pane="bottomRight" activeCell="BD309" sqref="BD309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -76075,7 +76075,7 @@
         <v>0</v>
       </c>
       <c r="BD309" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE309" s="30">
         <v>0.49672129999999998</v>

</xml_diff>

<commit_message>
close #30 new race totem
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -22557,10 +22557,10 @@
   <dimension ref="A1:BD314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B223" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E227" sqref="E227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -28149,7 +28149,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G35" s="4">
         <v>5</v>
@@ -39431,7 +39431,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G103" s="4">
         <v>0</v>
@@ -40095,7 +40095,7 @@
         <v>2</v>
       </c>
       <c r="F107" s="4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G107" s="4">
         <v>4</v>
@@ -50507,7 +50507,7 @@
         <v>1</v>
       </c>
       <c r="F169" s="4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G169" s="4">
         <v>0</v>
@@ -50671,7 +50671,7 @@
         <v>1</v>
       </c>
       <c r="F170" s="4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G170" s="4">
         <v>2</v>
@@ -60749,7 +60749,7 @@
         <v>1</v>
       </c>
       <c r="F230" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G230" s="4">
         <v>0</v>
@@ -60913,7 +60913,7 @@
         <v>2</v>
       </c>
       <c r="F231" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G231" s="4">
         <v>0</v>
@@ -61077,7 +61077,7 @@
         <v>1</v>
       </c>
       <c r="F232" s="4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G232" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
makeup totem skill #28
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="1434">
   <si>
     <t>arrow</t>
   </si>
@@ -5510,10 +5510,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>压制</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>洛欧塞布</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5535,6 +5531,14 @@
   </si>
   <si>
     <t>AttrDef</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>过牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -11035,7 +11039,7 @@
             <v>55000064</v>
           </cell>
           <cell r="V52">
-            <v>5</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="53">
@@ -11587,7 +11591,7 @@
             <v>55000134</v>
           </cell>
           <cell r="V121">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="122">
@@ -11939,7 +11943,7 @@
             <v>55000178</v>
           </cell>
           <cell r="V165">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="166">
@@ -11947,7 +11951,7 @@
             <v>55000179</v>
           </cell>
           <cell r="V166">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="167">
@@ -12315,7 +12319,7 @@
             <v>55000225</v>
           </cell>
           <cell r="V212">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="213">
@@ -12323,7 +12327,7 @@
             <v>55000226</v>
           </cell>
           <cell r="V213">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="214">
@@ -22557,10 +22561,10 @@
   <dimension ref="A1:BD314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B223" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E227" sqref="E227"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -28146,7 +28150,7 @@
         <v>905</v>
       </c>
       <c r="E35" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35" s="4">
         <v>16</v>
@@ -28156,16 +28160,16 @@
       </c>
       <c r="H35" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I35" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J35" s="4">
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="K35" s="4">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="L35" s="4">
         <v>0</v>
@@ -28193,7 +28197,7 @@
       </c>
       <c r="T35" s="15">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="U35" s="4">
         <v>10</v>
@@ -28227,7 +28231,7 @@
 IF(ISBLANK($AB35),0, LOOKUP($AB35,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC35/100)+
 IF(ISBLANK($AD35),0, LOOKUP($AD35,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE35/100)+
 IF(ISBLANK($AF35),0, LOOKUP($AF35,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG35/100)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AI35" s="21">
         <v>0</v>
@@ -28293,7 +28297,7 @@
         <v>5.0819669999999997E-2</v>
       </c>
       <c r="BD35" s="22" t="s">
-        <v>1172</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="36" spans="1:56" ht="14.25">
@@ -40102,19 +40106,19 @@
       </c>
       <c r="H107" s="4">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I107" s="4">
         <v>2</v>
       </c>
       <c r="J107" s="4">
-        <v>-13</v>
+        <v>-100</v>
       </c>
       <c r="K107" s="4">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="L107" s="4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M107" s="4">
         <v>0</v>
@@ -40139,7 +40143,7 @@
       </c>
       <c r="T107" s="15">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>-5</v>
       </c>
       <c r="U107" s="4">
         <v>10</v>
@@ -40173,7 +40177,7 @@
 IF(ISBLANK($AB107),0, LOOKUP($AB107,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC107/100)+
 IF(ISBLANK($AD107),0, LOOKUP($AD107,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE107/100)+
 IF(ISBLANK($AF107),0, LOOKUP($AF107,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG107/100)</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="AI107" s="21">
         <v>0</v>
@@ -40239,7 +40243,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
       <c r="BD107" s="22" t="s">
-        <v>1172</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="108" spans="1:56" ht="14.25">
@@ -50504,7 +50508,7 @@
         <v>913</v>
       </c>
       <c r="E169" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F169" s="4">
         <v>16</v>
@@ -50514,16 +50518,16 @@
       </c>
       <c r="H169" s="4">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I169" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J169" s="4">
-        <v>-10</v>
+        <v>-100</v>
       </c>
       <c r="K169" s="4">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="L169" s="4">
         <v>0</v>
@@ -50551,7 +50555,7 @@
       </c>
       <c r="T169" s="15">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="U169" s="4">
         <v>10</v>
@@ -50585,7 +50589,7 @@
 IF(ISBLANK($AB169),0, LOOKUP($AB169,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC169/100)+
 IF(ISBLANK($AD169),0, LOOKUP($AD169,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE169/100)+
 IF(ISBLANK($AF169),0, LOOKUP($AF169,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG169/100)</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AI169" s="21">
         <v>0</v>
@@ -50651,7 +50655,7 @@
         <v>5.7377049999999999E-2</v>
       </c>
       <c r="BD169" s="22" t="s">
-        <v>1172</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="170" spans="1:56" ht="14.25">
@@ -50668,7 +50672,7 @@
         <v>797</v>
       </c>
       <c r="E170" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F170" s="4">
         <v>16</v>
@@ -50678,16 +50682,16 @@
       </c>
       <c r="H170" s="4">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I170" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J170" s="4">
-        <v>-14</v>
+        <v>-100</v>
       </c>
       <c r="K170" s="4">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="L170" s="4">
         <v>0</v>
@@ -50715,7 +50719,7 @@
       </c>
       <c r="T170" s="15">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U170" s="4">
         <v>10</v>
@@ -50749,7 +50753,7 @@
 IF(ISBLANK($AB170),0, LOOKUP($AB170,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC170/100)+
 IF(ISBLANK($AD170),0, LOOKUP($AD170,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE170/100)+
 IF(ISBLANK($AF170),0, LOOKUP($AF170,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG170/100)</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AI170" s="21">
         <v>0</v>
@@ -50815,7 +50819,7 @@
         <v>4.0983609999999997E-2</v>
       </c>
       <c r="BD170" s="22" t="s">
-        <v>1172</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="171" spans="1:56" ht="14.25">
@@ -57955,7 +57959,7 @@
         <v>0</v>
       </c>
       <c r="X213" s="4" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="Y213" s="4" t="s">
         <v>1362</v>
@@ -60746,7 +60750,7 @@
         <v>834</v>
       </c>
       <c r="E230" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F230" s="4">
         <v>16</v>
@@ -60756,16 +60760,16 @@
       </c>
       <c r="H230" s="4">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I230" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J230" s="4">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="K230" s="4">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="L230" s="4">
         <v>0</v>
@@ -60793,7 +60797,7 @@
       </c>
       <c r="T230" s="15">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="U230" s="4">
         <v>10</v>
@@ -60827,7 +60831,7 @@
 IF(ISBLANK($AB230),0, LOOKUP($AB230,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC230/100)+
 IF(ISBLANK($AD230),0, LOOKUP($AD230,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE230/100)+
 IF(ISBLANK($AF230),0, LOOKUP($AF230,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG230/100)</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AI230" s="21">
         <v>0</v>
@@ -60893,7 +60897,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
       <c r="BD230" s="22" t="s">
-        <v>1172</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="231" spans="1:56" ht="14.25">
@@ -60910,7 +60914,7 @@
         <v>939</v>
       </c>
       <c r="E231" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F231" s="4">
         <v>16</v>
@@ -60923,16 +60927,16 @@
         <v>1</v>
       </c>
       <c r="I231" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J231" s="4">
-        <v>-15</v>
+        <v>-100</v>
       </c>
       <c r="K231" s="4">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="L231" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M231" s="4">
         <v>0</v>
@@ -60991,7 +60995,7 @@
 IF(ISBLANK($AB231),0, LOOKUP($AB231,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AC231/100)+
 IF(ISBLANK($AD231),0, LOOKUP($AD231,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AE231/100)+
 IF(ISBLANK($AF231),0, LOOKUP($AF231,[1]Skill!$A:$A,[1]Skill!$V:$V)*$AG231/100)</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AI231" s="21">
         <v>0</v>
@@ -61057,7 +61061,7 @@
         <v>5.4098359999999998E-2</v>
       </c>
       <c r="BD231" s="22" t="s">
-        <v>1172</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="232" spans="1:56" ht="14.25">
@@ -61090,13 +61094,13 @@
         <v>1</v>
       </c>
       <c r="J232" s="4">
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="K232" s="4">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="L232" s="4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M232" s="4">
         <v>0</v>
@@ -61121,7 +61125,7 @@
       </c>
       <c r="T232" s="15">
         <f t="shared" si="13"/>
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="U232" s="4">
         <v>10</v>
@@ -74765,13 +74769,13 @@
         <v>51000311</v>
       </c>
       <c r="B314" s="11" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C314" s="11" t="s">
         <v>1427</v>
       </c>
-      <c r="C314" s="11" t="s">
+      <c r="D314" s="8" t="s">
         <v>1428</v>
-      </c>
-      <c r="D314" s="8" t="s">
-        <v>1429</v>
       </c>
       <c r="E314" s="11">
         <v>4</v>
@@ -74836,7 +74840,7 @@
         <v>228</v>
       </c>
       <c r="Y314" s="11" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="Z314" s="21">
         <v>55000052</v>
@@ -74921,7 +74925,7 @@
         <v>0.49672129999999998</v>
       </c>
       <c r="BD314" s="11" t="s">
-        <v>1426</v>
+        <v>1432</v>
       </c>
     </row>
   </sheetData>
@@ -75518,7 +75522,7 @@
         <v>1231</v>
       </c>
       <c r="AV3" s="42" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="AW3" s="14" t="s">
         <v>1404</v>

</xml_diff>

<commit_message>
missile can vary by types , map unit load from file
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,7 +23,7 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="1432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="1433">
   <si>
     <t>arrow</t>
   </si>
@@ -5362,10 +5362,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>51018003|ArrowTowerId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>arrow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5518,6 +5514,14 @@
   </si>
   <si>
     <t>55300007;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018003|ArrowTowerId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9818,11 +9822,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1107170496"/>
-        <c:axId val="-1107169952"/>
+        <c:axId val="570515760"/>
+        <c:axId val="570509232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1107170496"/>
+        <c:axId val="570515760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9865,7 +9869,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1107169952"/>
+        <c:crossAx val="570509232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9873,7 +9877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1107169952"/>
+        <c:axId val="570509232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9924,7 +9928,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1107170496"/>
+        <c:crossAx val="570515760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10728,25 +10732,153 @@
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55900001</v>
+            <v>55500001</v>
           </cell>
           <cell r="V16">
-            <v>35</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55900002</v>
+            <v>55500002</v>
           </cell>
           <cell r="V17">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
+            <v>55500003</v>
+          </cell>
+          <cell r="V18">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>55500004</v>
+          </cell>
+          <cell r="V19">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>55500005</v>
+          </cell>
+          <cell r="V20">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>55500006</v>
+          </cell>
+          <cell r="V21">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>55500007</v>
+          </cell>
+          <cell r="V22">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>55500008</v>
+          </cell>
+          <cell r="V23">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>55500009</v>
+          </cell>
+          <cell r="V24">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>55500010</v>
+          </cell>
+          <cell r="V25">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>55500011</v>
+          </cell>
+          <cell r="V26">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>55500012</v>
+          </cell>
+          <cell r="V27">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>55500013</v>
+          </cell>
+          <cell r="V28">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>55500014</v>
+          </cell>
+          <cell r="V29">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>55500015</v>
+          </cell>
+          <cell r="V30">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>55500016</v>
+          </cell>
+          <cell r="V31">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>55900001</v>
+          </cell>
+          <cell r="V32">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>55900002</v>
+          </cell>
+          <cell r="V33">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
             <v>55900003</v>
           </cell>
-          <cell r="V18">
+          <cell r="V34">
             <v>80</v>
           </cell>
         </row>
@@ -19687,7 +19819,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -20257,7 +20389,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20345,7 +20477,7 @@
         <v>1151</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="T1" s="40" t="s">
         <v>974</v>
@@ -20357,7 +20489,7 @@
         <v>1136</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="X1" s="17" t="s">
         <v>323</v>
@@ -20435,7 +20567,7 @@
         <v>1027</v>
       </c>
       <c r="AW1" s="54" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="AX1" s="17" t="s">
         <v>326</v>
@@ -20527,7 +20659,7 @@
         <v>1137</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -20605,7 +20737,7 @@
         <v>1029</v>
       </c>
       <c r="AW2" s="55" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>295</v>
@@ -20673,7 +20805,7 @@
         <v>1145</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>1148</v>
+        <v>1431</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>1155</v>
@@ -20697,7 +20829,7 @@
         <v>1139</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -20775,7 +20907,7 @@
         <v>1028</v>
       </c>
       <c r="AW3" s="14" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="AX3" s="6" t="s">
         <v>309</v>
@@ -20935,7 +21067,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW4" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX4" s="4">
         <v>6</v>
@@ -21033,7 +21165,7 @@
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="Z5" s="21">
         <v>55100001</v>
@@ -21099,7 +21231,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW5" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX5" s="4">
         <v>6</v>
@@ -21255,7 +21387,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW6" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX6" s="4">
         <v>6</v>
@@ -21411,7 +21543,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW7" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX7" s="4">
         <v>6</v>
@@ -21567,7 +21699,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW8" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX8" s="4">
         <v>6</v>
@@ -21731,7 +21863,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW9" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX9" s="4">
         <v>6</v>
@@ -21895,7 +22027,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW10" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX10" s="4">
         <v>6</v>
@@ -22053,7 +22185,7 @@
         <v>0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AW11" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX11" s="4">
         <v>6</v>
@@ -22219,7 +22351,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW12" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX12" s="4">
         <v>6</v>
@@ -22377,7 +22509,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW13" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX13" s="4">
         <v>6</v>
@@ -22549,7 +22681,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW14" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX14" s="4">
         <v>6</v>
@@ -22707,7 +22839,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW15" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX15" s="4">
         <v>4</v>
@@ -22865,7 +22997,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW16" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX16" s="4">
         <v>6</v>
@@ -23023,7 +23155,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW17" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX17" s="4">
         <v>6</v>
@@ -23181,7 +23313,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW18" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX18" s="4">
         <v>6</v>
@@ -23339,7 +23471,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW19" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX19" s="4">
         <v>6</v>
@@ -23497,7 +23629,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW20" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX20" s="4">
         <v>6</v>
@@ -23655,7 +23787,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW21" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX21" s="4">
         <v>6</v>
@@ -23813,7 +23945,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW22" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX22" s="4">
         <v>6</v>
@@ -23971,7 +24103,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW23" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX23" s="4">
         <v>6</v>
@@ -24135,7 +24267,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW24" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX24" s="4">
         <v>6</v>
@@ -24307,7 +24439,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW25" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX25" s="4">
         <v>6</v>
@@ -24465,7 +24597,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW26" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX26" s="4">
         <v>6</v>
@@ -24629,7 +24761,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW27" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX27" s="4">
         <v>6</v>
@@ -24793,7 +24925,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW28" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX28" s="4">
         <v>6</v>
@@ -24957,7 +25089,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW29" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX29" s="4">
         <v>6</v>
@@ -25115,7 +25247,7 @@
         <v>0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AW30" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX30" s="4">
         <v>6</v>
@@ -25283,7 +25415,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW31" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX31" s="4">
         <v>6</v>
@@ -25455,7 +25587,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW32" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX32" s="4">
         <v>6</v>
@@ -25613,7 +25745,7 @@
         <v>0;0.3;0.3;0.3;0;0.3;0</v>
       </c>
       <c r="AW33" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX33" s="4">
         <v>6</v>
@@ -25777,7 +25909,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW34" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX34" s="4">
         <v>6</v>
@@ -25869,13 +26001,13 @@
         <v>0</v>
       </c>
       <c r="W35" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="Z35" s="43">
         <v>55300001</v>
@@ -25941,7 +26073,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW35" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX35" s="4">
         <v>6</v>
@@ -25960,7 +26092,7 @@
         <v>5.0819669999999997E-2</v>
       </c>
       <c r="BD35" s="22" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="36" spans="1:56" ht="14.25">
@@ -26109,7 +26241,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW36" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX36" s="4">
         <v>6</v>
@@ -26273,7 +26405,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW37" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX37" s="4">
         <v>6</v>
@@ -26431,7 +26563,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW38" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX38" s="4">
         <v>6</v>
@@ -26589,7 +26721,7 @@
         <v>0;0.3;0;0;0.3;0;0</v>
       </c>
       <c r="AW39" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX39" s="4">
         <v>6</v>
@@ -26747,7 +26879,7 @@
         <v>0;0.3;0;0.3;0;0;0</v>
       </c>
       <c r="AW40" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX40" s="4">
         <v>6</v>
@@ -26911,7 +27043,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW41" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX41" s="4">
         <v>6</v>
@@ -27079,7 +27211,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW42" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX42" s="4">
         <v>6</v>
@@ -27243,7 +27375,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW43" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX43" s="4">
         <v>6</v>
@@ -27411,7 +27543,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW44" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX44" s="4">
         <v>6</v>
@@ -27579,7 +27711,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW45" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX45" s="4">
         <v>6</v>
@@ -27747,7 +27879,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW46" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX46" s="4">
         <v>6</v>
@@ -27911,7 +28043,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW47" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX47" s="4">
         <v>6</v>
@@ -28075,7 +28207,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW48" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX48" s="4">
         <v>6</v>
@@ -28239,7 +28371,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW49" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX49" s="4">
         <v>6</v>
@@ -28407,7 +28539,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW50" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX50" s="4">
         <v>4</v>
@@ -28575,7 +28707,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW51" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX51" s="4">
         <v>6</v>
@@ -28673,7 +28805,7 @@
         <v>9</v>
       </c>
       <c r="Y52" s="4" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="Z52" s="43">
         <v>55900001</v>
@@ -28739,7 +28871,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW52" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX52" s="4">
         <v>6</v>
@@ -28901,7 +29033,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW53" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX53" s="4">
         <v>6</v>
@@ -29065,7 +29197,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW54" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX54" s="4">
         <v>6</v>
@@ -29229,7 +29361,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW55" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX55" s="4">
         <v>6</v>
@@ -29393,7 +29525,7 @@
         <v>0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AW56" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX56" s="4">
         <v>6</v>
@@ -29561,7 +29693,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW57" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX57" s="4">
         <v>6</v>
@@ -29725,7 +29857,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW58" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX58" s="4">
         <v>6</v>
@@ -29889,7 +30021,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW59" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX59" s="4">
         <v>6</v>
@@ -30053,7 +30185,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW60" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX60" s="4">
         <v>6</v>
@@ -30217,7 +30349,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW61" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX61" s="4">
         <v>6</v>
@@ -30381,7 +30513,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW62" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX62" s="4">
         <v>6</v>
@@ -30545,7 +30677,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW63" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX63" s="4">
         <v>6</v>
@@ -30703,7 +30835,7 @@
         <v>0;0.3;0.3;0;0.3;0;0</v>
       </c>
       <c r="AW64" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX64" s="4">
         <v>6</v>
@@ -30861,7 +30993,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW65" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX65" s="4">
         <v>6</v>
@@ -31019,7 +31151,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW66" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX66" s="4">
         <v>6</v>
@@ -31187,7 +31319,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW67" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX67" s="4">
         <v>5</v>
@@ -31363,7 +31495,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW68" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX68" s="4">
         <v>5</v>
@@ -31537,7 +31669,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW69" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX69" s="4">
         <v>5</v>
@@ -31709,7 +31841,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW70" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX70" s="4">
         <v>5</v>
@@ -31877,7 +32009,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW71" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX71" s="4">
         <v>6</v>
@@ -32045,7 +32177,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW72" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX72" s="4">
         <v>6</v>
@@ -32213,7 +32345,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW73" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX73" s="4">
         <v>6</v>
@@ -32381,7 +32513,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW74" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX74" s="4">
         <v>6</v>
@@ -32549,7 +32681,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW75" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX75" s="4">
         <v>6</v>
@@ -32717,7 +32849,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW76" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX76" s="4">
         <v>6</v>
@@ -32881,7 +33013,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW77" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX77" s="4">
         <v>6</v>
@@ -33049,7 +33181,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW78" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX78" s="4">
         <v>6</v>
@@ -33207,7 +33339,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW79" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX79" s="4">
         <v>6</v>
@@ -33365,7 +33497,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW80" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX80" s="4">
         <v>6</v>
@@ -33533,7 +33665,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW81" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX81" s="4">
         <v>6</v>
@@ -33701,7 +33833,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW82" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX82" s="4">
         <v>6</v>
@@ -33869,7 +34001,7 @@
         <v>0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AW83" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX83" s="4">
         <v>6</v>
@@ -34033,7 +34165,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW84" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX84" s="4">
         <v>6</v>
@@ -34205,7 +34337,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW85" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX85" s="4">
         <v>3</v>
@@ -34373,7 +34505,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW86" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX86" s="4">
         <v>6</v>
@@ -34541,7 +34673,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW87" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX87" s="4">
         <v>6</v>
@@ -34709,7 +34841,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW88" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX88" s="4">
         <v>6</v>
@@ -34807,7 +34939,7 @@
         <v>105</v>
       </c>
       <c r="Y89" s="4" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="Z89" s="21">
         <v>55900002</v>
@@ -34873,7 +35005,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW89" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX89" s="4">
         <v>6</v>
@@ -35039,7 +35171,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW90" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX90" s="4">
         <v>6</v>
@@ -35207,7 +35339,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW91" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX91" s="4">
         <v>6</v>
@@ -35375,7 +35507,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW92" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX92" s="4">
         <v>6</v>
@@ -35543,7 +35675,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW93" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX93" s="4">
         <v>6</v>
@@ -35711,7 +35843,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW94" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX94" s="4">
         <v>5</v>
@@ -35879,7 +36011,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW95" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX95" s="4">
         <v>6</v>
@@ -36047,7 +36179,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW96" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX96" s="4">
         <v>6</v>
@@ -36219,7 +36351,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW97" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX97" s="4">
         <v>3</v>
@@ -36383,7 +36515,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW98" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX98" s="4">
         <v>6</v>
@@ -36551,7 +36683,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW99" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX99" s="4">
         <v>6</v>
@@ -36727,7 +36859,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW100" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX100" s="4">
         <v>5</v>
@@ -36897,7 +37029,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW101" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX101" s="4">
         <v>6</v>
@@ -36995,7 +37127,7 @@
         <v>16</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="Z102" s="43">
         <v>55900003</v>
@@ -37061,7 +37193,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW102" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX102" s="4">
         <v>4</v>
@@ -37151,7 +37283,7 @@
         <v>0</v>
       </c>
       <c r="W103" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X103" s="4" t="s">
         <v>9</v>
@@ -37223,7 +37355,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW103" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX103" s="4">
         <v>6</v>
@@ -37391,7 +37523,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW104" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX104" s="4">
         <v>6</v>
@@ -37559,7 +37691,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW105" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX105" s="4">
         <v>6</v>
@@ -37723,7 +37855,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW106" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX106" s="4">
         <v>6</v>
@@ -37815,13 +37947,13 @@
         <v>0</v>
       </c>
       <c r="W107" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X107" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y107" s="4" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="Z107" s="43">
         <v>55300007</v>
@@ -37887,7 +38019,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW107" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX107" s="4">
         <v>6</v>
@@ -37906,7 +38038,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
       <c r="BD107" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="108" spans="1:56" ht="14.25">
@@ -38059,7 +38191,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW108" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX108" s="4">
         <v>4</v>
@@ -38223,7 +38355,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW109" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX109" s="4">
         <v>6</v>
@@ -38391,7 +38523,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW110" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX110" s="4">
         <v>6</v>
@@ -38555,7 +38687,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW111" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX111" s="4">
         <v>6</v>
@@ -38723,7 +38855,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW112" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX112" s="4">
         <v>6</v>
@@ -38891,7 +39023,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW113" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX113" s="4">
         <v>6</v>
@@ -39067,7 +39199,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW114" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX114" s="4">
         <v>3</v>
@@ -39245,7 +39377,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW115" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX115" s="4">
         <v>6</v>
@@ -39423,7 +39555,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW116" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX116" s="4">
         <v>6</v>
@@ -39593,7 +39725,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW117" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX117" s="4">
         <v>6</v>
@@ -39769,7 +39901,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW118" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX118" s="4">
         <v>5</v>
@@ -39947,7 +40079,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW119" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX119" s="4">
         <v>6</v>
@@ -40125,7 +40257,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW120" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX120" s="4">
         <v>5</v>
@@ -40303,7 +40435,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW121" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX121" s="4">
         <v>6</v>
@@ -40473,7 +40605,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW122" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX122" s="4">
         <v>6</v>
@@ -40645,7 +40777,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW123" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX123" s="4">
         <v>6</v>
@@ -40817,7 +40949,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW124" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX124" s="4">
         <v>6</v>
@@ -40989,7 +41121,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW125" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX125" s="4">
         <v>6</v>
@@ -41153,7 +41285,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW126" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX126" s="4">
         <v>6</v>
@@ -41317,7 +41449,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW127" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX127" s="4">
         <v>6</v>
@@ -41485,7 +41617,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW128" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX128" s="4">
         <v>6</v>
@@ -41653,7 +41785,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW129" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX129" s="4">
         <v>3</v>
@@ -41817,7 +41949,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW130" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX130" s="4">
         <v>6</v>
@@ -41981,7 +42113,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW131" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX131" s="4">
         <v>6</v>
@@ -42149,7 +42281,7 @@
         <v>0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AW132" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX132" s="4">
         <v>6</v>
@@ -42317,7 +42449,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW133" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX133" s="4">
         <v>6</v>
@@ -42485,7 +42617,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW134" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX134" s="4">
         <v>6</v>
@@ -42653,7 +42785,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW135" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX135" s="4">
         <v>6</v>
@@ -42821,7 +42953,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW136" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX136" s="4">
         <v>6</v>
@@ -42993,7 +43125,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW137" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX137" s="4">
         <v>5</v>
@@ -43161,7 +43293,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW138" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX138" s="4">
         <v>6</v>
@@ -43329,7 +43461,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW139" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX139" s="4">
         <v>6</v>
@@ -43487,7 +43619,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW140" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX140" s="4">
         <v>6</v>
@@ -43655,7 +43787,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW141" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX141" s="4">
         <v>6</v>
@@ -43823,7 +43955,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW142" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX142" s="4">
         <v>6</v>
@@ -43991,7 +44123,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW143" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX143" s="4">
         <v>6</v>
@@ -44155,7 +44287,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW144" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX144" s="4">
         <v>6</v>
@@ -44313,7 +44445,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW145" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX145" s="4">
         <v>6</v>
@@ -44485,7 +44617,7 @@
         <v>0;0;0;0;0.3;0;0</v>
       </c>
       <c r="AW146" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX146" s="4">
         <v>6</v>
@@ -44653,7 +44785,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW147" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX147" s="4">
         <v>6</v>
@@ -44821,7 +44953,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW148" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX148" s="4">
         <v>6</v>
@@ -44993,7 +45125,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW149" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX149" s="4">
         <v>6</v>
@@ -45165,7 +45297,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW150" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX150" s="4">
         <v>6</v>
@@ -45329,7 +45461,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW151" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX151" s="4">
         <v>6</v>
@@ -45487,7 +45619,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW152" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX152" s="4">
         <v>6</v>
@@ -45651,7 +45783,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW153" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX153" s="4">
         <v>6</v>
@@ -45815,7 +45947,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW154" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX154" s="4">
         <v>6</v>
@@ -45979,7 +46111,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW155" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX155" s="4">
         <v>6</v>
@@ -46143,7 +46275,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW156" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX156" s="4">
         <v>6</v>
@@ -46301,7 +46433,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW157" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX157" s="4">
         <v>6</v>
@@ -46465,7 +46597,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW158" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX158" s="4">
         <v>6</v>
@@ -46633,7 +46765,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW159" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX159" s="4">
         <v>6</v>
@@ -46801,7 +46933,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW160" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX160" s="4">
         <v>6</v>
@@ -46959,7 +47091,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW161" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX161" s="4">
         <v>6</v>
@@ -47123,7 +47255,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW162" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX162" s="4">
         <v>6</v>
@@ -47287,7 +47419,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW163" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX163" s="4">
         <v>6</v>
@@ -47455,7 +47587,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW164" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX164" s="4">
         <v>6</v>
@@ -47627,7 +47759,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW165" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX165" s="4">
         <v>6</v>
@@ -47795,7 +47927,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW166" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX166" s="4">
         <v>6</v>
@@ -47963,7 +48095,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW167" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX167" s="4">
         <v>6</v>
@@ -48135,7 +48267,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW168" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX168" s="4">
         <v>5</v>
@@ -48227,13 +48359,13 @@
         <v>0</v>
       </c>
       <c r="W169" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X169" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y169" s="4" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="Z169" s="43">
         <v>55300003</v>
@@ -48299,7 +48431,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW169" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX169" s="4">
         <v>6</v>
@@ -48318,7 +48450,7 @@
         <v>5.7377049999999999E-2</v>
       </c>
       <c r="BD169" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="170" spans="1:56" ht="14.25">
@@ -48391,13 +48523,13 @@
         <v>0</v>
       </c>
       <c r="W170" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X170" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y170" s="4" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="Z170" s="43">
         <v>55300002</v>
@@ -48463,7 +48595,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW170" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX170" s="4">
         <v>6</v>
@@ -48482,7 +48614,7 @@
         <v>4.0983609999999997E-2</v>
       </c>
       <c r="BD170" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="171" spans="1:56" ht="14.25">
@@ -48639,7 +48771,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW171" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX171" s="4">
         <v>6</v>
@@ -48811,7 +48943,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW172" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX172" s="4">
         <v>6</v>
@@ -48979,7 +49111,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW173" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX173" s="4">
         <v>6</v>
@@ -49143,7 +49275,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW174" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX174" s="4">
         <v>6</v>
@@ -49307,7 +49439,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW175" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX175" s="4">
         <v>6</v>
@@ -49471,7 +49603,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW176" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX176" s="4">
         <v>6</v>
@@ -49639,7 +49771,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW177" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX177" s="4">
         <v>6</v>
@@ -49807,7 +49939,7 @@
         <v>0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AW178" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX178" s="4">
         <v>6</v>
@@ -49971,7 +50103,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW179" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX179" s="4">
         <v>6</v>
@@ -50147,7 +50279,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW180" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX180" s="4">
         <v>5</v>
@@ -50319,7 +50451,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW181" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX181" s="4">
         <v>6</v>
@@ -50487,7 +50619,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW182" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX182" s="4">
         <v>6</v>
@@ -50655,7 +50787,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW183" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX183" s="4">
         <v>5</v>
@@ -50819,7 +50951,7 @@
         <v>0;0;0.3;0;0;0;0</v>
       </c>
       <c r="AW184" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX184" s="4">
         <v>6</v>
@@ -50987,7 +51119,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW185" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX185" s="4">
         <v>3</v>
@@ -51155,7 +51287,7 @@
         <v>0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AW186" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX186" s="4">
         <v>6</v>
@@ -51319,7 +51451,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW187" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX187" s="4">
         <v>6</v>
@@ -51491,7 +51623,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW188" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX188" s="4">
         <v>3</v>
@@ -51655,7 +51787,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW189" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX189" s="4">
         <v>6</v>
@@ -51813,7 +51945,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW190" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX190" s="4">
         <v>6</v>
@@ -51981,7 +52113,7 @@
         <v>0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AW191" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX191" s="4">
         <v>6</v>
@@ -52153,7 +52285,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW192" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX192" s="4">
         <v>6</v>
@@ -52325,7 +52457,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW193" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX193" s="4">
         <v>6</v>
@@ -52497,7 +52629,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW194" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX194" s="4">
         <v>4</v>
@@ -52673,7 +52805,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW195" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX195" s="4">
         <v>5</v>
@@ -52841,7 +52973,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW196" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX196" s="4">
         <v>5</v>
@@ -53013,7 +53145,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW197" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX197" s="4">
         <v>5</v>
@@ -53185,7 +53317,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW198" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX198" s="4">
         <v>3</v>
@@ -53357,7 +53489,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW199" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX199" s="4">
         <v>6</v>
@@ -53529,7 +53661,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW200" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX200" s="4">
         <v>6</v>
@@ -53693,7 +53825,7 @@
         <v>0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AW201" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX201" s="4">
         <v>3</v>
@@ -53791,7 +53923,7 @@
         <v>1164</v>
       </c>
       <c r="Y202" s="4" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="Z202" s="43">
         <v>55310001</v>
@@ -53857,7 +53989,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW202" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX202" s="4">
         <v>6</v>
@@ -54023,7 +54155,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW203" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX203" s="4">
         <v>6</v>
@@ -54191,7 +54323,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW204" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX204" s="4">
         <v>6</v>
@@ -54355,7 +54487,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW205" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX205" s="4">
         <v>6</v>
@@ -54453,7 +54585,7 @@
         <v>94</v>
       </c>
       <c r="Y206" s="4" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="Z206" s="43">
         <v>55100001</v>
@@ -54523,7 +54655,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW206" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX206" s="4">
         <v>6</v>
@@ -54687,7 +54819,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW207" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX207" s="4">
         <v>6</v>
@@ -54855,7 +54987,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW208" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX208" s="4">
         <v>6</v>
@@ -55019,7 +55151,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW209" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX209" s="4">
         <v>6</v>
@@ -55187,7 +55319,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW210" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX210" s="4">
         <v>6</v>
@@ -55359,7 +55491,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW211" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX211" s="4">
         <v>6</v>
@@ -55527,7 +55659,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW212" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX212" s="4">
         <v>6</v>
@@ -55622,7 +55754,7 @@
         <v>0</v>
       </c>
       <c r="X213" s="4" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="Y213" s="4" t="s">
         <v>1350</v>
@@ -55699,7 +55831,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW213" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX213" s="4">
         <v>6</v>
@@ -55871,7 +56003,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW214" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX214" s="4">
         <v>6</v>
@@ -56047,7 +56179,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW215" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX215" s="4">
         <v>6</v>
@@ -56211,7 +56343,7 @@
         <v>0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AW216" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX216" s="4">
         <v>6</v>
@@ -56379,7 +56511,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW217" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX217" s="4">
         <v>6</v>
@@ -56547,7 +56679,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW218" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX218" s="4">
         <v>6</v>
@@ -56715,7 +56847,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW219" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX219" s="4">
         <v>6</v>
@@ -56879,7 +57011,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW220" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX220" s="4">
         <v>6</v>
@@ -57047,7 +57179,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW221" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX221" s="4">
         <v>6</v>
@@ -57211,7 +57343,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW222" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX222" s="4">
         <v>6</v>
@@ -57375,7 +57507,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW223" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX223" s="4">
         <v>6</v>
@@ -57543,7 +57675,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW224" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX224" s="4">
         <v>6</v>
@@ -57711,7 +57843,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW225" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX225" s="4">
         <v>6</v>
@@ -57809,7 +57941,7 @@
         <v>9</v>
       </c>
       <c r="Y226" s="4" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="Z226" s="43">
         <v>55400002</v>
@@ -57875,7 +58007,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW226" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX226" s="4">
         <v>6</v>
@@ -58041,7 +58173,7 @@
         <v>0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AW227" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX227" s="4">
         <v>6</v>
@@ -58209,7 +58341,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW228" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX228" s="4">
         <v>6</v>
@@ -58377,7 +58509,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW229" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX229" s="4">
         <v>6</v>
@@ -58469,13 +58601,13 @@
         <v>0</v>
       </c>
       <c r="W230" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X230" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y230" s="4" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="Z230" s="43">
         <v>55300004</v>
@@ -58541,7 +58673,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW230" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX230" s="4">
         <v>6</v>
@@ -58560,7 +58692,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
       <c r="BD230" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="231" spans="1:56" ht="14.25">
@@ -58633,13 +58765,13 @@
         <v>0</v>
       </c>
       <c r="W231" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X231" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Y231" s="4" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="Z231" s="43">
         <v>55300005</v>
@@ -58705,7 +58837,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW231" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX231" s="4">
         <v>6</v>
@@ -58724,7 +58856,7 @@
         <v>5.4098359999999998E-2</v>
       </c>
       <c r="BD231" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="232" spans="1:56" ht="14.25">
@@ -58797,7 +58929,7 @@
         <v>0</v>
       </c>
       <c r="W232" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X232" s="4" t="s">
         <v>9</v>
@@ -58863,7 +58995,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW232" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX232" s="4">
         <v>6</v>
@@ -59027,7 +59159,7 @@
         <v>0;0;0.3;0;0;0;0</v>
       </c>
       <c r="AW233" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX233" s="4">
         <v>6</v>
@@ -59195,7 +59327,7 @@
         <v>0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AW234" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX234" s="4">
         <v>6</v>
@@ -59363,7 +59495,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW235" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX235" s="4">
         <v>6</v>
@@ -59531,7 +59663,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW236" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX236" s="4">
         <v>6</v>
@@ -59629,7 +59761,7 @@
         <v>2</v>
       </c>
       <c r="Y237" s="4" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="Z237" s="43">
         <v>55100001</v>
@@ -59707,7 +59839,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW237" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX237" s="4">
         <v>6</v>
@@ -59875,7 +60007,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW238" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX238" s="4">
         <v>6</v>
@@ -60043,7 +60175,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW239" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX239" s="4">
         <v>6</v>
@@ -60211,7 +60343,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW240" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX240" s="4">
         <v>6</v>
@@ -60387,7 +60519,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW241" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX241" s="4">
         <v>3</v>
@@ -60555,7 +60687,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW242" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX242" s="4">
         <v>6</v>
@@ -60727,7 +60859,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW243" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX243" s="4">
         <v>6</v>
@@ -60895,7 +61027,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW244" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX244" s="4">
         <v>6</v>
@@ -61071,7 +61203,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW245" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX245" s="4">
         <v>4</v>
@@ -61235,7 +61367,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW246" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX246" s="4">
         <v>4</v>
@@ -61407,7 +61539,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW247" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX247" s="4">
         <v>6</v>
@@ -61571,7 +61703,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW248" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX248" s="4">
         <v>6</v>
@@ -61739,7 +61871,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW249" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX249" s="4">
         <v>6</v>
@@ -61911,7 +62043,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW250" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX250" s="4">
         <v>3</v>
@@ -62079,7 +62211,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW251" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX251" s="4">
         <v>6</v>
@@ -62251,7 +62383,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW252" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX252" s="4">
         <v>6</v>
@@ -62419,7 +62551,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW253" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX253" s="4">
         <v>6</v>
@@ -62587,7 +62719,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW254" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX254" s="4">
         <v>6</v>
@@ -62755,7 +62887,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW255" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX255" s="4">
         <v>6</v>
@@ -62923,7 +63055,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW256" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX256" s="4">
         <v>6</v>
@@ -63091,7 +63223,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW257" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX257" s="4">
         <v>6</v>
@@ -63259,7 +63391,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW258" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX258" s="4">
         <v>6</v>
@@ -63427,7 +63559,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW259" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX259" s="4">
         <v>6</v>
@@ -63595,7 +63727,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW260" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX260" s="4">
         <v>6</v>
@@ -63763,7 +63895,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW261" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX261" s="4">
         <v>6</v>
@@ -63927,7 +64059,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW262" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX262" s="4">
         <v>6</v>
@@ -64085,7 +64217,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW263" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX263" s="4">
         <v>6</v>
@@ -64253,7 +64385,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW264" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX264" s="4">
         <v>6</v>
@@ -64425,7 +64557,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW265" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX265" s="4">
         <v>6</v>
@@ -64597,7 +64729,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW266" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX266" s="4">
         <v>6</v>
@@ -64769,7 +64901,7 @@
         <v>0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AW267" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX267" s="4">
         <v>6</v>
@@ -64937,7 +65069,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW268" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX268" s="4">
         <v>6</v>
@@ -65101,7 +65233,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW269" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX269" s="4">
         <v>6</v>
@@ -65269,7 +65401,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW270" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX270" s="4">
         <v>6</v>
@@ -65441,7 +65573,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW271" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX271" s="4">
         <v>5</v>
@@ -65613,7 +65745,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW272" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX272" s="4">
         <v>6</v>
@@ -65785,7 +65917,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW273" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX273" s="4">
         <v>3</v>
@@ -65949,7 +66081,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW274" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX274" s="4">
         <v>6</v>
@@ -66117,7 +66249,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW275" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX275" s="4">
         <v>6</v>
@@ -66283,7 +66415,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW276" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX276" s="4">
         <v>6</v>
@@ -66451,7 +66583,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW277" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX277" s="4">
         <v>6</v>
@@ -66619,7 +66751,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW278" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX278" s="4">
         <v>6</v>
@@ -66783,7 +66915,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW279" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX279" s="4">
         <v>6</v>
@@ -66951,7 +67083,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW280" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX280" s="4">
         <v>6</v>
@@ -67115,7 +67247,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW281" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX281" s="4">
         <v>6</v>
@@ -67279,7 +67411,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW282" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX282" s="4">
         <v>6</v>
@@ -67443,7 +67575,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW283" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX283" s="4">
         <v>6</v>
@@ -67611,7 +67743,7 @@
         <v>0;0;0;0;0;0.3;0</v>
       </c>
       <c r="AW284" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX284" s="4">
         <v>6</v>
@@ -67779,7 +67911,7 @@
         <v>0;0;0;0;0;0;0.3</v>
       </c>
       <c r="AW285" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX285" s="4">
         <v>5</v>
@@ -67937,7 +68069,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW286" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX286" s="4">
         <v>6</v>
@@ -68105,7 +68237,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW287" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX287" s="4">
         <v>6</v>
@@ -68273,7 +68405,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW288" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX288" s="4">
         <v>6</v>
@@ -68437,7 +68569,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW289" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX289" s="4">
         <v>6</v>
@@ -68601,7 +68733,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW290" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX290" s="4">
         <v>6</v>
@@ -68769,7 +68901,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW291" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX291" s="4">
         <v>6</v>
@@ -68937,7 +69069,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW292" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX292" s="4">
         <v>6</v>
@@ -69101,7 +69233,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW293" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX293" s="4">
         <v>6</v>
@@ -69273,7 +69405,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW294" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX294" s="4">
         <v>6</v>
@@ -69437,7 +69569,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW295" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX295" s="4">
         <v>6</v>
@@ -69605,7 +69737,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW296" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX296" s="4">
         <v>6</v>
@@ -69777,7 +69909,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW297" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX297" s="4">
         <v>6</v>
@@ -69945,7 +70077,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW298" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX298" s="4">
         <v>6</v>
@@ -70109,7 +70241,7 @@
         <v>0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AW299" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX299" s="4">
         <v>6</v>
@@ -70273,7 +70405,7 @@
         <v>0;0.3;0;0;0;0;0</v>
       </c>
       <c r="AW300" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX300" s="4">
         <v>6</v>
@@ -70449,7 +70581,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW301" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX301" s="4">
         <v>3</v>
@@ -70617,7 +70749,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW302" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX302" s="4">
         <v>6</v>
@@ -70785,7 +70917,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW303" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX303" s="11">
         <v>6</v>
@@ -70949,7 +71081,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW304" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX304" s="11">
         <v>6</v>
@@ -71113,7 +71245,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW305" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX305" s="11">
         <v>6</v>
@@ -71281,7 +71413,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW306" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX306" s="11">
         <v>6</v>
@@ -71445,7 +71577,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW307" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX307" s="11">
         <v>6</v>
@@ -71603,7 +71735,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW308" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX308" s="11">
         <v>6</v>
@@ -71761,7 +71893,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW309" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX309" s="11">
         <v>6</v>
@@ -71919,7 +72051,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW310" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX310" s="11">
         <v>6</v>
@@ -72077,7 +72209,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW311" s="56" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX311" s="11">
         <v>6</v>
@@ -72104,10 +72236,10 @@
         <v>51000309</v>
       </c>
       <c r="B312" s="11" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C312" s="4" t="s">
         <v>1398</v>
-      </c>
-      <c r="C312" s="4" t="s">
-        <v>1399</v>
       </c>
       <c r="D312" s="8" t="s">
         <v>698</v>
@@ -72175,7 +72307,7 @@
         <v>9</v>
       </c>
       <c r="Y312" s="11" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="Z312" s="21">
         <v>55400001</v>
@@ -72241,7 +72373,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW312" s="57" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX312" s="11">
         <v>6</v>
@@ -72260,7 +72392,7 @@
         <v>0.40819670000000002</v>
       </c>
       <c r="BD312" s="11" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="313" spans="1:56" ht="14.25">
@@ -72268,13 +72400,13 @@
         <v>51000310</v>
       </c>
       <c r="B313" s="11" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C313" s="11" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D313" s="8" t="s">
         <v>1404</v>
-      </c>
-      <c r="C313" s="11" t="s">
-        <v>1403</v>
-      </c>
-      <c r="D313" s="8" t="s">
-        <v>1405</v>
       </c>
       <c r="E313" s="11">
         <v>6</v>
@@ -72339,7 +72471,7 @@
         <v>1021</v>
       </c>
       <c r="Y313" s="11" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="Z313" s="21">
         <v>55200001</v>
@@ -72405,7 +72537,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW313" s="57" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX313" s="11">
         <v>6</v>
@@ -72424,7 +72556,7 @@
         <v>0.49672129999999998</v>
       </c>
       <c r="BD313" s="11" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="314" spans="1:56" ht="14.25">
@@ -72432,13 +72564,13 @@
         <v>51000311</v>
       </c>
       <c r="B314" s="11" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C314" s="11" t="s">
         <v>1407</v>
       </c>
-      <c r="C314" s="11" t="s">
+      <c r="D314" s="8" t="s">
         <v>1408</v>
-      </c>
-      <c r="D314" s="8" t="s">
-        <v>1409</v>
       </c>
       <c r="E314" s="11">
         <v>4</v>
@@ -72503,7 +72635,7 @@
         <v>228</v>
       </c>
       <c r="Y314" s="11" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="Z314" s="21">
         <v>55300006</v>
@@ -72569,7 +72701,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW314" s="57" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AX314" s="11">
         <v>6</v>
@@ -72588,7 +72720,7 @@
         <v>0.49672129999999998</v>
       </c>
       <c r="BD314" s="11" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
   </sheetData>
@@ -72639,15 +72771,15 @@
   <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
     <col min="2" max="2" width="7.25" customWidth="1"/>
     <col min="3" max="3" width="12.875" customWidth="1"/>
     <col min="4" max="4" width="6.125" customWidth="1"/>
@@ -72741,7 +72873,7 @@
         <v>1136</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="X1" s="17" t="s">
         <v>323</v>
@@ -72819,7 +72951,7 @@
         <v>1027</v>
       </c>
       <c r="AW1" s="54" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="AX1" s="17" t="s">
         <v>326</v>
@@ -72911,7 +73043,7 @@
         <v>295</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>296</v>
@@ -72989,7 +73121,7 @@
         <v>1029</v>
       </c>
       <c r="AW2" s="55" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>295</v>
@@ -73081,7 +73213,7 @@
         <v>1139</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>306</v>
@@ -73156,10 +73288,10 @@
         <v>1228</v>
       </c>
       <c r="AV3" s="42" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AW3" s="14" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="AX3" s="6" t="s">
         <v>309</v>
@@ -73319,7 +73451,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW4" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX4" s="11">
         <v>6</v>
@@ -73479,7 +73611,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW5" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX5" s="11">
         <v>6</v>
@@ -73635,7 +73767,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW6" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX6" s="4">
         <v>6</v>
@@ -73672,7 +73804,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="11">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G7" s="11">
         <v>0</v>
@@ -73791,7 +73923,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW7" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX7" s="11">
         <v>6</v>
@@ -73828,7 +73960,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="11">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G8" s="11">
         <v>0</v>
@@ -73884,7 +74016,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="Y8" s="22"/>
       <c r="Z8" s="53"/>
@@ -73947,7 +74079,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW8" s="56" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="AX8" s="11">
         <v>6</v>
@@ -73969,7 +74101,7 @@
     </row>
     <row r="9" spans="1:56" ht="14.25">
       <c r="A9" t="s">
-        <v>1388</v>
+        <v>1432</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>1381</v>
@@ -74040,7 +74172,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="11" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="53"/>
@@ -74103,7 +74235,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW9" s="56" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="AX9" s="11">
         <v>6</v>
@@ -74263,7 +74395,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW10" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX10" s="36">
         <v>6</v>
@@ -74423,7 +74555,7 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AW11" s="56" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AX11" s="11">
         <v>6</v>

</xml_diff>

<commit_message>
#8 fix some monster card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -326,40 +326,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B66" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Real:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>初始卡片</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B79" authorId="1" shapeId="0">
       <text>
         <r>
@@ -429,40 +395,6 @@
       </text>
     </comment>
     <comment ref="B157" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Real:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>初始卡片</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B190" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -701,7 +633,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="1135">
   <si>
     <t>arrow</t>
   </si>
@@ -19372,10 +19304,10 @@
   <dimension ref="A1:BC314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y92" sqref="Y92"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25609,9 +25541,7 @@
       <c r="C40" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D40" s="21" t="s">
-        <v>873</v>
-      </c>
+      <c r="D40" s="21"/>
       <c r="E40" s="4">
         <v>4</v>
       </c>
@@ -25623,19 +25553,19 @@
       </c>
       <c r="H40" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I40" s="4">
         <v>4</v>
       </c>
       <c r="J40" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K40" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L40" s="4">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M40" s="4">
         <v>0</v>
@@ -25660,7 +25590,7 @@
       </c>
       <c r="T40" s="14">
         <f t="shared" si="1"/>
-        <v>25.64</v>
+        <v>7.2800000000000011</v>
       </c>
       <c r="U40" s="4">
         <v>10</v>
@@ -25716,13 +25646,13 @@
         <v>0.3</v>
       </c>
       <c r="AQ40" s="20">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AR40" s="20">
         <v>0.3</v>
       </c>
       <c r="AS40" s="20">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AT40" s="20">
         <v>0</v>
@@ -25732,7 +25662,7 @@
       </c>
       <c r="AV40" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>0;0.3;0;0.3;0;0;0</v>
+        <v>0;0.3;0.3;0.3;0.3;0;0</v>
       </c>
       <c r="AW40" s="52" t="s">
         <v>1091</v>
@@ -29855,16 +29785,16 @@
         <v>-5</v>
       </c>
       <c r="U66" s="4">
+        <v>25</v>
+      </c>
+      <c r="V66" s="4">
         <v>10</v>
       </c>
-      <c r="V66" s="4">
-        <v>20</v>
-      </c>
       <c r="W66" s="4">
         <v>0</v>
       </c>
       <c r="X66" s="4" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="Y66" s="4"/>
       <c r="Z66" s="39"/>
@@ -32004,16 +31934,16 @@
         <v>-4</v>
       </c>
       <c r="U79" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="V79" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="W79" s="4">
         <v>0</v>
       </c>
       <c r="X79" s="4" t="s">
-        <v>4</v>
+        <v>228</v>
       </c>
       <c r="Y79" s="4"/>
       <c r="Z79" s="39"/>
@@ -32159,16 +32089,16 @@
         <v>-4</v>
       </c>
       <c r="U80" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="V80" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="W80" s="4">
         <v>0</v>
       </c>
       <c r="X80" s="4" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="Y80" s="7"/>
       <c r="Z80" s="39"/>
@@ -50274,7 +50204,7 @@
         <v>10</v>
       </c>
       <c r="V190" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="W190" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
monster ai more smart
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -8445,7 +8445,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8508,7 +8507,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8545,9 +8543,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8621,7 +8617,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8710,11 +8705,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="221037264"/>
-        <c:axId val="221037824"/>
+        <c:axId val="638948736"/>
+        <c:axId val="638949296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="221037264"/>
+        <c:axId val="638948736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8757,7 +8752,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221037824"/>
+        <c:crossAx val="638949296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8765,7 +8760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221037824"/>
+        <c:axId val="638949296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8816,7 +8811,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221037264"/>
+        <c:crossAx val="638948736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8830,7 +8825,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18748,7 +18742,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -19312,11 +19306,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B301" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G103" sqref="G103"/>
+      <selection pane="bottomRight" activeCell="A312" sqref="A312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -70735,11 +70729,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -71914,10 +71908,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -71945,10 +71939,10 @@
       </c>
       <c r="T8" s="14">
         <f t="shared" si="1"/>
-        <v>425</v>
+        <v>315</v>
       </c>
       <c r="U8" s="10">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="V8" s="10">
         <v>0</v>
@@ -72067,10 +72061,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="K9" s="4">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -72098,10 +72092,10 @@
       </c>
       <c r="T9" s="14">
         <f t="shared" si="1"/>
-        <v>295</v>
+        <v>180</v>
       </c>
       <c r="U9" s="10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="V9" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
finish skill jianshe and shuangzi
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11736"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -4480,11 +4480,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>55110001;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>55100005;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>55110001;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8712,11 +8712,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1622646176"/>
-        <c:axId val="1622647264"/>
+        <c:axId val="314254432"/>
+        <c:axId val="314254992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1622646176"/>
+        <c:axId val="314254432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8759,7 +8759,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1622647264"/>
+        <c:crossAx val="314254992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8767,7 +8767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1622647264"/>
+        <c:axId val="314254992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8818,7 +8818,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1622646176"/>
+        <c:crossAx val="314254432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9553,7 +9553,7 @@
             <v>55100004</v>
           </cell>
           <cell r="W7">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="8">
@@ -9566,23 +9566,23 @@
         </row>
         <row r="9">
           <cell r="A9">
-            <v>55110001</v>
+            <v>55100006</v>
           </cell>
           <cell r="W9">
-            <v>20</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>55200001</v>
+            <v>55100007</v>
           </cell>
           <cell r="W10">
-            <v>40</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>55200002</v>
+            <v>55100008</v>
           </cell>
           <cell r="W11">
             <v>15</v>
@@ -9590,151 +9590,151 @@
         </row>
         <row r="12">
           <cell r="A12">
-            <v>55300001</v>
+            <v>55100009</v>
           </cell>
           <cell r="W12">
-            <v>40</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>55300002</v>
+            <v>55110001</v>
           </cell>
           <cell r="W13">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>55300003</v>
+            <v>55200001</v>
           </cell>
           <cell r="W14">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>55300004</v>
+            <v>55200002</v>
           </cell>
           <cell r="W15">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55300005</v>
+            <v>55300001</v>
           </cell>
           <cell r="W16">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55300006</v>
+            <v>55300002</v>
           </cell>
           <cell r="W17">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>55300007</v>
+            <v>55300003</v>
           </cell>
           <cell r="W18">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>55310001</v>
+            <v>55300004</v>
           </cell>
           <cell r="W19">
-            <v>100</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>55400001</v>
+            <v>55300005</v>
           </cell>
           <cell r="W20">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>55400002</v>
+            <v>55300006</v>
           </cell>
           <cell r="W21">
-            <v>80</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22">
-            <v>55400003</v>
+            <v>55300007</v>
           </cell>
           <cell r="W22">
-            <v>80</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>55400004</v>
+            <v>55310001</v>
           </cell>
           <cell r="W23">
-            <v>80</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>55400005</v>
+            <v>55400001</v>
           </cell>
           <cell r="W24">
-            <v>70</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>55400006</v>
+            <v>55400002</v>
           </cell>
           <cell r="W25">
-            <v>30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>55500001</v>
+            <v>55400003</v>
           </cell>
           <cell r="W26">
-            <v>5</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>55500002</v>
+            <v>55400004</v>
           </cell>
           <cell r="W27">
-            <v>5</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>55500003</v>
+            <v>55400005</v>
           </cell>
           <cell r="W28">
-            <v>5</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>55500004</v>
+            <v>55400006</v>
           </cell>
           <cell r="W29">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>55500005</v>
+            <v>55500001</v>
           </cell>
           <cell r="W30">
             <v>5</v>
@@ -9742,7 +9742,7 @@
         </row>
         <row r="31">
           <cell r="A31">
-            <v>55500006</v>
+            <v>55500002</v>
           </cell>
           <cell r="W31">
             <v>5</v>
@@ -9750,7 +9750,7 @@
         </row>
         <row r="32">
           <cell r="A32">
-            <v>55500007</v>
+            <v>55500003</v>
           </cell>
           <cell r="W32">
             <v>5</v>
@@ -9758,7 +9758,7 @@
         </row>
         <row r="33">
           <cell r="A33">
-            <v>55500008</v>
+            <v>55500004</v>
           </cell>
           <cell r="W33">
             <v>5</v>
@@ -9766,7 +9766,7 @@
         </row>
         <row r="34">
           <cell r="A34">
-            <v>55500009</v>
+            <v>55500005</v>
           </cell>
           <cell r="W34">
             <v>5</v>
@@ -9774,7 +9774,7 @@
         </row>
         <row r="35">
           <cell r="A35">
-            <v>55500010</v>
+            <v>55500006</v>
           </cell>
           <cell r="W35">
             <v>5</v>
@@ -9782,7 +9782,7 @@
         </row>
         <row r="36">
           <cell r="A36">
-            <v>55500011</v>
+            <v>55500007</v>
           </cell>
           <cell r="W36">
             <v>5</v>
@@ -9790,7 +9790,7 @@
         </row>
         <row r="37">
           <cell r="A37">
-            <v>55500012</v>
+            <v>55500008</v>
           </cell>
           <cell r="W37">
             <v>5</v>
@@ -9798,7 +9798,7 @@
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55500013</v>
+            <v>55500009</v>
           </cell>
           <cell r="W38">
             <v>5</v>
@@ -9806,7 +9806,7 @@
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55500014</v>
+            <v>55500010</v>
           </cell>
           <cell r="W39">
             <v>5</v>
@@ -9814,7 +9814,7 @@
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55500015</v>
+            <v>55500011</v>
           </cell>
           <cell r="W40">
             <v>5</v>
@@ -9822,7 +9822,7 @@
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55500016</v>
+            <v>55500012</v>
           </cell>
           <cell r="W41">
             <v>5</v>
@@ -9830,33 +9830,65 @@
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55600016</v>
+            <v>55500013</v>
           </cell>
           <cell r="W42">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55900001</v>
+            <v>55500014</v>
           </cell>
           <cell r="W43">
-            <v>35</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55900002</v>
+            <v>55500015</v>
           </cell>
           <cell r="W44">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
+            <v>55500016</v>
+          </cell>
+          <cell r="W45">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>55600016</v>
+          </cell>
+          <cell r="W46">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>55900001</v>
+          </cell>
+          <cell r="W47">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>55900002</v>
+          </cell>
+          <cell r="W48">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
             <v>55900003</v>
           </cell>
-          <cell r="W45">
+          <cell r="W49">
             <v>80</v>
           </cell>
         </row>
@@ -19361,43 +19393,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC314"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B88" sqref="B88"/>
+      <selection pane="bottomRight" activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="17.375" customWidth="1"/>
-    <col min="26" max="26" width="8.875" customWidth="1"/>
-    <col min="27" max="27" width="5.5" customWidth="1"/>
-    <col min="28" max="30" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="39" width="4.625" customWidth="1"/>
-    <col min="40" max="40" width="10.125" customWidth="1"/>
-    <col min="41" max="46" width="3.75" customWidth="1"/>
-    <col min="47" max="47" width="4.375" customWidth="1"/>
-    <col min="48" max="48" width="15.75" customWidth="1"/>
-    <col min="49" max="49" width="6.375" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1"/>
+    <col min="27" max="27" width="5.44140625" customWidth="1"/>
+    <col min="28" max="30" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="39" width="4.6640625" customWidth="1"/>
+    <col min="40" max="40" width="10.109375" customWidth="1"/>
+    <col min="41" max="46" width="3.77734375" customWidth="1"/>
+    <col min="47" max="47" width="4.33203125" customWidth="1"/>
+    <col min="48" max="48" width="15.77734375" customWidth="1"/>
+    <col min="49" max="49" width="6.33203125" customWidth="1"/>
     <col min="50" max="50" width="6" customWidth="1"/>
-    <col min="51" max="51" width="4.625" customWidth="1"/>
-    <col min="52" max="52" width="5.75" customWidth="1"/>
-    <col min="53" max="53" width="4.625" customWidth="1"/>
-    <col min="54" max="55" width="4.125" customWidth="1"/>
+    <col min="51" max="51" width="4.6640625" customWidth="1"/>
+    <col min="52" max="52" width="5.77734375" customWidth="1"/>
+    <col min="53" max="53" width="4.6640625" customWidth="1"/>
+    <col min="54" max="55" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="69">
+    <row r="1" spans="1:55" ht="73.2">
       <c r="A1" s="15" t="s">
         <v>311</v>
       </c>
@@ -19974,7 +20006,7 @@
         <v>2</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="Z4" s="39">
         <v>55100005</v>
@@ -34128,7 +34160,7 @@
         <v>16</v>
       </c>
       <c r="Y92" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="Z92" s="39">
         <v>55110001</v>
@@ -53204,7 +53236,7 @@
       </c>
       <c r="H208" s="4">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I208" s="4">
         <v>3</v>
@@ -53241,7 +53273,7 @@
       </c>
       <c r="T208" s="14">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>-10</v>
       </c>
       <c r="U208" s="4">
         <v>10</v>
@@ -53275,7 +53307,7 @@
 IF(ISBLANK($AB208),0, LOOKUP($AB208,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AC208/100)+
 IF(ISBLANK($AD208),0, LOOKUP($AD208,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AE208/100)+
 IF(ISBLANK($AF208),0, LOOKUP($AF208,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AG208/100)</f>
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="AI208" s="20">
         <v>0</v>
@@ -70791,41 +70823,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
-    <col min="10" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="17.375" customWidth="1"/>
-    <col min="26" max="26" width="8.875" customWidth="1"/>
-    <col min="27" max="27" width="5.5" customWidth="1"/>
-    <col min="29" max="29" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="39" width="4.625" customWidth="1"/>
-    <col min="40" max="40" width="10.125" customWidth="1"/>
-    <col min="41" max="47" width="3.75" customWidth="1"/>
-    <col min="48" max="48" width="14.75" customWidth="1"/>
-    <col min="49" max="49" width="5.875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
+    <col min="10" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1"/>
+    <col min="27" max="27" width="5.44140625" customWidth="1"/>
+    <col min="29" max="29" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="39" width="4.6640625" customWidth="1"/>
+    <col min="40" max="40" width="10.109375" customWidth="1"/>
+    <col min="41" max="47" width="3.77734375" customWidth="1"/>
+    <col min="48" max="48" width="14.77734375" customWidth="1"/>
+    <col min="49" max="49" width="5.88671875" customWidth="1"/>
     <col min="50" max="50" width="6" customWidth="1"/>
-    <col min="51" max="51" width="5.625" customWidth="1"/>
-    <col min="52" max="52" width="5.75" customWidth="1"/>
-    <col min="53" max="53" width="4.625" customWidth="1"/>
-    <col min="54" max="55" width="4.125" customWidth="1"/>
+    <col min="51" max="51" width="5.6640625" customWidth="1"/>
+    <col min="52" max="52" width="5.77734375" customWidth="1"/>
+    <col min="53" max="53" width="4.6640625" customWidth="1"/>
+    <col min="54" max="55" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="69">
+    <row r="1" spans="1:55" ht="73.2">
       <c r="A1" s="15" t="s">
         <v>311</v>
       </c>
@@ -72540,10 +72572,10 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.25" customWidth="1"/>
-    <col min="2" max="9" width="7.125" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -72999,9 +73031,9 @@
       <selection activeCell="H292" sqref="H292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="7" width="6.25" customWidth="1"/>
+    <col min="1" max="7" width="6.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -90424,10 +90456,10 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
#10 remove deathhit, mindam, add nodef
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -8447,7 +8447,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8510,7 +8509,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8547,9 +8545,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8623,7 +8619,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8712,11 +8707,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1315654976"/>
-        <c:axId val="-1315647904"/>
+        <c:axId val="-373158512"/>
+        <c:axId val="-373155248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1315654976"/>
+        <c:axId val="-373158512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8759,7 +8754,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1315647904"/>
+        <c:crossAx val="-373155248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8767,7 +8762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1315647904"/>
+        <c:axId val="-373155248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8818,7 +8813,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1315654976"/>
+        <c:crossAx val="-373158512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8832,7 +8827,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9874,7 +9868,7 @@
             <v>55510001</v>
           </cell>
           <cell r="W47">
-            <v>4</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="48">
@@ -9882,7 +9876,7 @@
             <v>55510002</v>
           </cell>
           <cell r="W48">
-            <v>4</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="49">
@@ -9890,7 +9884,7 @@
             <v>55510003</v>
           </cell>
           <cell r="W49">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="50">
@@ -9898,87 +9892,87 @@
             <v>55510004</v>
           </cell>
           <cell r="W50">
-            <v>6</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55510005</v>
+            <v>55510006</v>
           </cell>
           <cell r="W51">
-            <v>9</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55510006</v>
+            <v>55510007</v>
           </cell>
           <cell r="W52">
-            <v>2</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55510007</v>
+            <v>55510009</v>
           </cell>
           <cell r="W53">
-            <v>30</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55510008</v>
+            <v>55510010</v>
           </cell>
           <cell r="W54">
-            <v>3</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55510009</v>
+            <v>55510011</v>
           </cell>
           <cell r="W55">
-            <v>4</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55510010</v>
+            <v>55510012</v>
           </cell>
           <cell r="W56">
-            <v>25</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55510011</v>
+            <v>55510013</v>
           </cell>
           <cell r="W57">
-            <v>3</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55510012</v>
+            <v>55510014</v>
           </cell>
           <cell r="W58">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55510013</v>
+            <v>55510018</v>
           </cell>
           <cell r="W59">
-            <v>40</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55510014</v>
+            <v>55510019</v>
           </cell>
           <cell r="W60">
-            <v>15</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="61">
@@ -9986,7 +9980,7 @@
             <v>55600016</v>
           </cell>
           <cell r="W61">
-            <v>10</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="62">
@@ -10014,11 +10008,11 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19515,10 +19509,10 @@
   <dimension ref="A1:BC314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I78" sqref="I78"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -31953,7 +31947,7 @@
       </c>
       <c r="H78" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I78" s="4">
         <v>6</v>
@@ -31990,7 +31984,7 @@
       </c>
       <c r="T78" s="14">
         <f t="shared" si="5"/>
-        <v>3.6800000000000068</v>
+        <v>293.68</v>
       </c>
       <c r="U78" s="4">
         <v>0</v>
@@ -32028,7 +32022,7 @@
 IF(ISBLANK($AB78),0, LOOKUP($AB78,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AC78/100)+
 IF(ISBLANK($AD78),0, LOOKUP($AD78,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AE78/100)+
 IF(ISBLANK($AF78),0, LOOKUP($AF78,[1]Skill!$A:$A,[1]Skill!$W:$W)*$AG78/100)</f>
-        <v>90</v>
+        <v>380</v>
       </c>
       <c r="AI78" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
close #37 fix sidekick monster test. spell attr load from ispell
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -633,7 +633,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1121">
   <si>
     <t>arrow</t>
   </si>
@@ -3987,10 +3987,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55700003;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>成长</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4437,6 +4433,22 @@
   </si>
   <si>
     <t>55900009;100</t>
+  </si>
+  <si>
+    <t>成长，援护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900010;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>援护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55700003;100|55900010;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -8663,11 +8675,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="309408864"/>
-        <c:axId val="309409424"/>
+        <c:axId val="247724080"/>
+        <c:axId val="247724640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="309408864"/>
+        <c:axId val="247724080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8710,7 +8722,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309409424"/>
+        <c:crossAx val="247724640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8718,7 +8730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309409424"/>
+        <c:axId val="247724640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8769,7 +8781,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309408864"/>
+        <c:crossAx val="247724080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19687,10 +19699,10 @@
   <dimension ref="A1:BC314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L282" sqref="L282"/>
+      <selection pane="bottomRight" activeCell="Y163" sqref="Y163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20100,7 +20112,7 @@
         <v>787</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>797</v>
@@ -21080,7 +21092,7 @@
         <v>11</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="Z9" s="39">
         <v>55100011</v>
@@ -21239,7 +21251,7 @@
         <v>12</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="Z10" s="39">
         <v>55900008</v>
@@ -21551,7 +21563,7 @@
         <v>16</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="Z12" s="39">
         <v>55100004</v>
@@ -21871,7 +21883,7 @@
         <v>6</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="Z14" s="39"/>
       <c r="AA14" s="20"/>
@@ -23586,7 +23598,7 @@
         <v>31</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="Z25" s="39"/>
       <c r="AA25" s="20"/>
@@ -24063,7 +24075,7 @@
         <v>6</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="Z28" s="39">
         <v>55900007</v>
@@ -24693,7 +24705,7 @@
         <v>40</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="Z32" s="39"/>
       <c r="AA32" s="20"/>
@@ -25009,7 +25021,7 @@
         <v>16</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="Z34" s="39">
         <v>55900006</v>
@@ -25331,7 +25343,7 @@
         <v>800</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="Z36" s="39"/>
       <c r="AA36" s="20"/>
@@ -25492,7 +25504,7 @@
         <v>38</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Z37" s="39">
         <v>55610003</v>
@@ -26116,7 +26128,7 @@
         <v>51</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="Z41" s="39">
         <v>55100011</v>
@@ -26277,7 +26289,7 @@
         <v>53</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="Z42" s="39">
         <v>55000034</v>
@@ -26440,7 +26452,7 @@
         <v>4</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="Z43" s="39">
         <v>55900004</v>
@@ -26929,7 +26941,7 @@
         <v>2</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="Z46" s="39">
         <v>55510003</v>
@@ -27251,7 +27263,7 @@
         <v>16</v>
       </c>
       <c r="Y48" s="4" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="Z48" s="39">
         <v>55500009</v>
@@ -27573,7 +27585,7 @@
         <v>2</v>
       </c>
       <c r="Y50" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z50" s="39"/>
       <c r="AA50" s="20"/>
@@ -28056,7 +28068,7 @@
         <v>16</v>
       </c>
       <c r="Y53" s="4" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="Z53" s="39">
         <v>55110006</v>
@@ -28217,7 +28229,7 @@
         <v>64</v>
       </c>
       <c r="Y54" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="Z54" s="39">
         <v>55100011</v>
@@ -28861,7 +28873,7 @@
         <v>4</v>
       </c>
       <c r="Y58" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="Z58" s="39">
         <v>55610001</v>
@@ -29340,7 +29352,7 @@
         <v>24</v>
       </c>
       <c r="Y61" s="4" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="Z61" s="39">
         <v>55510007</v>
@@ -29499,7 +29511,7 @@
         <v>65</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="Z62" s="39">
         <v>55510002</v>
@@ -30292,7 +30304,7 @@
         <v>78</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="Z67" s="39">
         <v>55000095</v>
@@ -30453,7 +30465,7 @@
         <v>78</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="Z68" s="39">
         <v>55100011</v>
@@ -30628,7 +30640,7 @@
         <v>40</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="Z69" s="39"/>
       <c r="AA69" s="20"/>
@@ -31109,7 +31121,7 @@
         <v>2</v>
       </c>
       <c r="Y72" s="4" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="Z72" s="39"/>
       <c r="AA72" s="20"/>
@@ -31268,7 +31280,7 @@
         <v>802</v>
       </c>
       <c r="Y73" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="Z73" s="39">
         <v>55510007</v>
@@ -31594,7 +31606,7 @@
         <v>89</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="Z75" s="39">
         <v>55000004</v>
@@ -31922,7 +31934,7 @@
         <v>92</v>
       </c>
       <c r="Y77" s="4" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="Z77" s="39">
         <v>55110007</v>
@@ -32083,7 +32095,7 @@
         <v>970</v>
       </c>
       <c r="Y78" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="Z78" s="39">
         <v>55400004</v>
@@ -32886,7 +32898,7 @@
         <v>38</v>
       </c>
       <c r="Y83" s="4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="Z83" s="39">
         <v>55100010</v>
@@ -33377,7 +33389,7 @@
         <v>6</v>
       </c>
       <c r="Y86" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Z86" s="39"/>
       <c r="AA86" s="20"/>
@@ -33538,7 +33550,7 @@
         <v>86</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="Z87" s="39">
         <v>55100011</v>
@@ -34027,7 +34039,7 @@
         <v>107</v>
       </c>
       <c r="Y90" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="Z90" s="39"/>
       <c r="AA90" s="20"/>
@@ -34983,7 +34995,7 @@
         <v>2</v>
       </c>
       <c r="Y96" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="Z96" s="39"/>
       <c r="AA96" s="20"/>
@@ -35144,7 +35156,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="Z97" s="39">
         <v>55110007</v>
@@ -35472,7 +35484,7 @@
         <v>801</v>
       </c>
       <c r="Y99" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="Z99" s="39">
         <v>55510010</v>
@@ -35633,7 +35645,7 @@
         <v>78</v>
       </c>
       <c r="Y100" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="Z100" s="39"/>
       <c r="AA100" s="20"/>
@@ -36929,7 +36941,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Z108" s="39">
         <v>55000017</v>
@@ -37245,7 +37257,7 @@
         <v>130</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="Z110" s="39">
         <v>55510009</v>
@@ -37714,7 +37726,7 @@
         <v>135</v>
       </c>
       <c r="Y113" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="Z113" s="39">
         <v>55000018</v>
@@ -37875,7 +37887,7 @@
         <v>89</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="Z114" s="39"/>
       <c r="AA114" s="20"/>
@@ -38046,7 +38058,7 @@
         <v>94</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="Z115" s="39"/>
       <c r="AA115" s="20"/>
@@ -38217,7 +38229,7 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="Z116" s="39"/>
       <c r="AA116" s="20"/>
@@ -38388,7 +38400,7 @@
         <v>4</v>
       </c>
       <c r="Y117" s="7" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="Z117" s="39">
         <v>55000143</v>
@@ -38549,7 +38561,7 @@
         <v>40</v>
       </c>
       <c r="Y118" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="Z118" s="39"/>
       <c r="AA118" s="20"/>
@@ -38720,7 +38732,7 @@
         <v>100</v>
       </c>
       <c r="Y119" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="Z119" s="39"/>
       <c r="AA119" s="20"/>
@@ -38891,7 +38903,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="Z120" s="39"/>
       <c r="AA120" s="20"/>
@@ -39062,7 +39074,7 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="Z121" s="39"/>
       <c r="AA121" s="20"/>
@@ -39233,7 +39245,7 @@
         <v>4</v>
       </c>
       <c r="Y122" s="4" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="Z122" s="39">
         <v>55000150</v>
@@ -39394,7 +39406,7 @@
         <v>4</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="Z123" s="39">
         <v>55000227</v>
@@ -41163,7 +41175,7 @@
         <v>2</v>
       </c>
       <c r="Y134" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="Z134" s="39">
         <v>55900008</v>
@@ -41328,7 +41340,7 @@
         <v>78</v>
       </c>
       <c r="Y135" s="7" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="Z135" s="39">
         <v>55000143</v>
@@ -41489,7 +41501,7 @@
         <v>107</v>
       </c>
       <c r="Y136" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="Z136" s="39">
         <v>55110005</v>
@@ -41823,7 +41835,7 @@
         <v>6</v>
       </c>
       <c r="Y138" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="Z138" s="39">
         <v>55000157</v>
@@ -42290,7 +42302,7 @@
         <v>12</v>
       </c>
       <c r="Y141" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="Z141" s="20">
         <v>55610004</v>
@@ -42451,7 +42463,7 @@
         <v>40</v>
       </c>
       <c r="Y142" s="4" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="Z142" s="39">
         <v>55000018</v>
@@ -43093,7 +43105,7 @@
         <v>107</v>
       </c>
       <c r="Y146" s="4" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="Z146" s="39">
         <v>55000101</v>
@@ -43423,7 +43435,7 @@
         <v>805</v>
       </c>
       <c r="Y148" s="4" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="Z148" s="39">
         <v>55100012</v>
@@ -43588,7 +43600,7 @@
         <v>166</v>
       </c>
       <c r="Y149" s="4" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="Z149" s="39">
         <v>55100011</v>
@@ -43757,7 +43769,7 @@
         <v>4</v>
       </c>
       <c r="Y150" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="Z150" s="39">
         <v>55000017</v>
@@ -44709,7 +44721,7 @@
         <v>4</v>
       </c>
       <c r="Y156" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="Z156" s="39"/>
       <c r="AA156" s="20"/>
@@ -45174,7 +45186,7 @@
         <v>2</v>
       </c>
       <c r="Y159" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="Z159" s="39"/>
       <c r="AA159" s="20"/>
@@ -45735,7 +45747,7 @@
         <v>609</v>
       </c>
       <c r="D163" s="21" t="s">
-        <v>979</v>
+        <v>1119</v>
       </c>
       <c r="E163" s="4">
         <v>3</v>
@@ -45760,7 +45772,7 @@
         <v>0</v>
       </c>
       <c r="L163" s="4">
-        <v>-44</v>
+        <v>-19</v>
       </c>
       <c r="M163" s="4">
         <v>0</v>
@@ -45800,10 +45812,10 @@
         <v>107</v>
       </c>
       <c r="Y163" s="4" t="s">
-        <v>980</v>
+        <v>1118</v>
       </c>
       <c r="Z163" s="39">
-        <v>55100006</v>
+        <v>55900010</v>
       </c>
       <c r="AA163" s="20">
         <v>100</v>
@@ -45819,7 +45831,7 @@
 IF(ISBLANK($AB163),0, LOOKUP($AB163,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC163/100)+
 IF(ISBLANK($AD163),0, LOOKUP($AD163,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE163/100)+
 IF(ISBLANK($AF163),0, LOOKUP($AF163,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG163/100)</f>
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="AI163" s="20">
         <v>0</v>
@@ -45959,7 +45971,7 @@
         <v>16</v>
       </c>
       <c r="Y164" s="4" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="Z164" s="39">
         <v>55110005</v>
@@ -46120,7 +46132,7 @@
         <v>38</v>
       </c>
       <c r="Y165" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="Z165" s="39">
         <v>55000145</v>
@@ -46619,7 +46631,7 @@
         <v>16</v>
       </c>
       <c r="Y168" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="Z168" s="39"/>
       <c r="AA168" s="20"/>
@@ -47104,7 +47116,7 @@
         <v>4</v>
       </c>
       <c r="Y171" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="Z171" s="39">
         <v>55100010</v>
@@ -47265,7 +47277,7 @@
         <v>4</v>
       </c>
       <c r="Y172" s="4" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="Z172" s="39">
         <v>55000181</v>
@@ -47530,7 +47542,7 @@
         <v>615</v>
       </c>
       <c r="D174" s="21" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E174" s="4">
         <v>3</v>
@@ -47595,7 +47607,7 @@
         <v>69</v>
       </c>
       <c r="Y174" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="Z174" s="39">
         <v>55700004</v>
@@ -47691,7 +47703,7 @@
         <v>616</v>
       </c>
       <c r="D175" s="21" t="s">
-        <v>996</v>
+        <v>1117</v>
       </c>
       <c r="E175" s="4">
         <v>2</v>
@@ -47716,7 +47728,7 @@
         <v>0</v>
       </c>
       <c r="L175" s="4">
-        <v>-15</v>
+        <v>-35</v>
       </c>
       <c r="M175" s="4">
         <v>0</v>
@@ -47756,7 +47768,7 @@
         <v>2</v>
       </c>
       <c r="Y175" s="4" t="s">
-        <v>995</v>
+        <v>1120</v>
       </c>
       <c r="Z175" s="39">
         <v>55700003</v>
@@ -47764,8 +47776,12 @@
       <c r="AA175" s="20">
         <v>100</v>
       </c>
-      <c r="AB175" s="20"/>
-      <c r="AC175" s="20"/>
+      <c r="AB175" s="20">
+        <v>55900010</v>
+      </c>
+      <c r="AC175" s="20">
+        <v>100</v>
+      </c>
       <c r="AD175" s="20"/>
       <c r="AE175" s="20"/>
       <c r="AF175" s="20"/>
@@ -47775,7 +47791,7 @@
 IF(ISBLANK($AB175),0, LOOKUP($AB175,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC175/100)+
 IF(ISBLANK($AD175),0, LOOKUP($AD175,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE175/100)+
 IF(ISBLANK($AF175),0, LOOKUP($AF175,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG175/100)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AI175" s="20">
         <v>0</v>
@@ -47917,7 +47933,7 @@
         <v>12</v>
       </c>
       <c r="Y176" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Z176" s="39">
         <v>55610003</v>
@@ -48402,7 +48418,7 @@
         <v>2</v>
       </c>
       <c r="Y179" s="4" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="Z179" s="39">
         <v>55110005</v>
@@ -48563,7 +48579,7 @@
         <v>65</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="Z180" s="39">
         <v>55000061</v>
@@ -48901,7 +48917,7 @@
         <v>4</v>
       </c>
       <c r="Y182" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="Z182" s="39">
         <v>55610003</v>
@@ -49557,7 +49573,7 @@
         <v>78</v>
       </c>
       <c r="Y186" s="4" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="Z186" s="39">
         <v>55000125</v>
@@ -49877,7 +49893,7 @@
         <v>2</v>
       </c>
       <c r="Y188" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="Z188" s="39">
         <v>55000196</v>
@@ -50356,7 +50372,7 @@
         <v>24</v>
       </c>
       <c r="Y191" s="4" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="Z191" s="39">
         <v>55900004</v>
@@ -50690,7 +50706,7 @@
         <v>2</v>
       </c>
       <c r="Y193" s="4" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="Z193" s="39">
         <v>55100011</v>
@@ -50859,7 +50875,7 @@
         <v>16</v>
       </c>
       <c r="Y194" s="4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="Z194" s="39"/>
       <c r="AA194" s="20"/>
@@ -51024,7 +51040,7 @@
         <v>209</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="Z195" s="39">
         <v>55000016</v>
@@ -51193,7 +51209,7 @@
         <v>4</v>
       </c>
       <c r="Y196" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Z196" s="20">
         <v>55520003</v>
@@ -51354,7 +51370,7 @@
         <v>4</v>
       </c>
       <c r="Y197" s="4" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="Z197" s="39">
         <v>55000020</v>
@@ -51523,7 +51539,7 @@
         <v>22</v>
       </c>
       <c r="Y198" s="4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="Z198" s="39">
         <v>55100011</v>
@@ -52501,7 +52517,7 @@
         <v>2</v>
       </c>
       <c r="Y204" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="Z204" s="39">
         <v>55000150</v>
@@ -53626,7 +53642,7 @@
         <v>69</v>
       </c>
       <c r="Y211" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="Z211" s="39">
         <v>55000208</v>
@@ -53795,7 +53811,7 @@
         <v>132</v>
       </c>
       <c r="Y212" s="4" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="Z212" s="39"/>
       <c r="AA212" s="20"/>
@@ -53956,7 +53972,7 @@
         <v>944</v>
       </c>
       <c r="Y213" s="4" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="Z213" s="39">
         <v>55000114</v>
@@ -54278,7 +54294,7 @@
         <v>190</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="Z215" s="39">
         <v>55100001</v>
@@ -54761,7 +54777,7 @@
         <v>4</v>
       </c>
       <c r="Y218" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="Z218" s="39">
         <v>55100012</v>
@@ -55415,7 +55431,7 @@
         <v>6</v>
       </c>
       <c r="Y222" s="4" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="Z222" s="39">
         <v>55900005</v>
@@ -55574,7 +55590,7 @@
         <v>9</v>
       </c>
       <c r="Y223" s="4" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="Z223" s="39">
         <v>55100008</v>
@@ -55900,7 +55916,7 @@
         <v>16</v>
       </c>
       <c r="Y225" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="Z225" s="39">
         <v>55000009</v>
@@ -57359,7 +57375,7 @@
         <v>22</v>
       </c>
       <c r="Y234" s="4" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="Z234" s="39"/>
       <c r="AA234" s="20"/>
@@ -57850,7 +57866,7 @@
         <v>2</v>
       </c>
       <c r="Y237" s="4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="Z237" s="39">
         <v>55100001</v>
@@ -58498,7 +58514,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="Z241" s="39">
         <v>55000216</v>
@@ -59162,7 +59178,7 @@
         <v>69</v>
       </c>
       <c r="Y245" s="4" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="Z245" s="39">
         <v>55000131</v>
@@ -59492,7 +59508,7 @@
         <v>2</v>
       </c>
       <c r="Y247" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="Z247" s="39">
         <v>55000258</v>
@@ -59971,7 +59987,7 @@
         <v>2</v>
       </c>
       <c r="Y250" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="Z250" s="39">
         <v>55500008</v>
@@ -60305,7 +60321,7 @@
         <v>135</v>
       </c>
       <c r="Y252" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="Z252" s="39"/>
       <c r="AA252" s="20"/>
@@ -60570,7 +60586,7 @@
         <v>390</v>
       </c>
       <c r="D254" s="21" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E254" s="4">
         <v>3</v>
@@ -60635,7 +60651,7 @@
         <v>209</v>
       </c>
       <c r="Y254" s="4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="Z254" s="20">
         <v>55100013</v>
@@ -60959,7 +60975,7 @@
         <v>4</v>
       </c>
       <c r="Y256" s="4" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="Z256" s="39">
         <v>55110005</v>
@@ -61450,7 +61466,7 @@
         <v>4</v>
       </c>
       <c r="Y259" s="7" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="Z259" s="39">
         <v>55100012</v>
@@ -62259,7 +62275,7 @@
         <v>4</v>
       </c>
       <c r="Y264" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="Z264" s="39">
         <v>55000271</v>
@@ -62418,7 +62434,7 @@
         <v>2</v>
       </c>
       <c r="Y265" s="4" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="Z265" s="39">
         <v>55110007</v>
@@ -62579,7 +62595,7 @@
         <v>24</v>
       </c>
       <c r="Y266" s="4" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="Z266" s="39">
         <v>55000093</v>
@@ -63241,7 +63257,7 @@
         <v>16</v>
       </c>
       <c r="Y270" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Z270" s="39"/>
       <c r="AA270" s="20"/>
@@ -63402,7 +63418,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="Z271" s="39">
         <v>55000019</v>
@@ -63567,7 +63583,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="Z272" s="39">
         <v>55000275</v>
@@ -63736,7 +63752,7 @@
         <v>810</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="Z273" s="39">
         <v>55000136</v>
@@ -64066,7 +64082,7 @@
         <v>277</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="Z275" s="39">
         <v>55000278</v>
@@ -65034,7 +65050,7 @@
         <v>9</v>
       </c>
       <c r="Y281" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="Z281" s="39">
         <v>55900009</v>
@@ -65193,7 +65209,7 @@
         <v>6</v>
       </c>
       <c r="Y282" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="Z282" s="39">
         <v>55900009</v>
@@ -65352,7 +65368,7 @@
         <v>16</v>
       </c>
       <c r="Y283" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="Z283" s="39">
         <v>55900009</v>
@@ -65678,7 +65694,7 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="Z285" s="39">
         <v>55000289</v>
@@ -66811,7 +66827,7 @@
         <v>22</v>
       </c>
       <c r="Y292" s="4" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="Z292" s="39"/>
       <c r="AA292" s="20"/>
@@ -67628,7 +67644,7 @@
         <v>45</v>
       </c>
       <c r="Y297" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="Z297" s="39">
         <v>55000045</v>
@@ -67956,7 +67972,7 @@
         <v>22</v>
       </c>
       <c r="Y299" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="Z299" s="39">
         <v>55610002</v>
@@ -68115,7 +68131,7 @@
         <v>22</v>
       </c>
       <c r="Y300" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="Z300" s="39">
         <v>55610002</v>
@@ -68276,7 +68292,7 @@
         <v>111</v>
       </c>
       <c r="Y301" s="4" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="Z301" s="39">
         <v>55000013</v>
@@ -68445,7 +68461,7 @@
         <v>209</v>
       </c>
       <c r="Y302" s="4" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="Z302" s="39">
         <v>55000335</v>
@@ -68541,7 +68557,7 @@
         <v>701</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E303" s="10">
         <v>2</v>
@@ -68606,7 +68622,7 @@
         <v>78</v>
       </c>
       <c r="Y303" s="10" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="Z303" s="39">
         <v>55100012</v>
@@ -68702,7 +68718,7 @@
         <v>710</v>
       </c>
       <c r="D304" s="21" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E304" s="10">
         <v>2</v>
@@ -68767,7 +68783,7 @@
         <v>6</v>
       </c>
       <c r="Y304" s="10" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="Z304" s="39">
         <v>55100014</v>
@@ -68863,7 +68879,7 @@
         <v>711</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E305" s="10">
         <v>3</v>
@@ -68928,7 +68944,7 @@
         <v>6</v>
       </c>
       <c r="Y305" s="10" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="Z305" s="39">
         <v>55100014</v>
@@ -69024,7 +69040,7 @@
         <v>712</v>
       </c>
       <c r="D306" s="21" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E306" s="10">
         <v>4</v>
@@ -69089,7 +69105,7 @@
         <v>78</v>
       </c>
       <c r="Y306" s="10" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="Z306" s="39">
         <v>55100014</v>

</xml_diff>

<commit_message>
checkburst can kown the damage is melee or range
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -633,7 +633,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="1122">
   <si>
     <t>arrow</t>
   </si>
@@ -8686,11 +8686,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="262736416"/>
-        <c:axId val="262736976"/>
+        <c:axId val="209284528"/>
+        <c:axId val="213450448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="262736416"/>
+        <c:axId val="209284528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8733,7 +8733,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262736976"/>
+        <c:crossAx val="213450448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8741,7 +8741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262736976"/>
+        <c:axId val="213450448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8792,7 +8792,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262736416"/>
+        <c:crossAx val="209284528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19774,10 +19774,10 @@
   <dimension ref="A1:BC314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B298" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L98" sqref="L98"/>
+      <selection pane="bottomRight" activeCell="E306" sqref="E306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -69237,9 +69237,7 @@
       <c r="C307" s="10" t="s">
         <v>716</v>
       </c>
-      <c r="D307" s="21" t="s">
-        <v>806</v>
-      </c>
+      <c r="D307" s="21"/>
       <c r="E307" s="10">
         <v>3</v>
       </c>
@@ -69251,19 +69249,19 @@
       </c>
       <c r="H307" s="10">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I307" s="10">
         <v>3</v>
       </c>
       <c r="J307" s="10">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K307" s="10">
-        <v>14</v>
+        <v>-20</v>
       </c>
       <c r="L307" s="10">
-        <v>-2</v>
+        <v>-21</v>
       </c>
       <c r="M307" s="4">
         <v>0</v>
@@ -69288,7 +69286,7 @@
       </c>
       <c r="T307" s="23">
         <f t="shared" si="17"/>
-        <v>47</v>
+        <v>-1</v>
       </c>
       <c r="U307" s="4">
         <v>30</v>

</xml_diff>

<commit_message>
#10 move some auro skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -633,7 +633,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="1124">
   <si>
     <t>arrow</t>
   </si>
@@ -3936,9 +3936,6 @@
     <t>55610002;100</t>
   </si>
   <si>
-    <t>55000145;100|55000163;25|55610002;100</t>
-  </si>
-  <si>
     <t>55000009;100|55610002;100</t>
   </si>
   <si>
@@ -4112,9 +4109,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55100011;100|55000095;50|55000097;100|55000219;100</t>
-  </si>
-  <si>
     <t>55100011;100|55000043;15|55000198;100</t>
   </si>
   <si>
@@ -4131,12 +4125,6 @@
   </si>
   <si>
     <t>55000034;20|55100011;100</t>
-  </si>
-  <si>
-    <t>55100012;100|55000161;100</t>
-  </si>
-  <si>
-    <t>55100011;100|55100012;100|55000162;100</t>
   </si>
   <si>
     <t>55100012;100|55000150;100</t>
@@ -4470,6 +4458,25 @@
   <si>
     <t>55110012;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55000145;100|55610002;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55100012;100|55600002;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55100011;100|55600003;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55100011;100|55000095;50|55600004;100|55000219;100</t>
   </si>
 </sst>
 </file>
@@ -5521,7 +5528,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="137">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -10120,212 +10134,212 @@
             <v>55600001</v>
           </cell>
           <cell r="X80">
-            <v>300</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55610001</v>
+            <v>55600002</v>
           </cell>
           <cell r="X81">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55610002</v>
+            <v>55600003</v>
           </cell>
           <cell r="X82">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55610003</v>
+            <v>55600004</v>
           </cell>
           <cell r="X83">
-            <v>5</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55610004</v>
+            <v>55610001</v>
           </cell>
           <cell r="X84">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55700001</v>
+            <v>55610002</v>
           </cell>
           <cell r="X85">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55700002</v>
+            <v>55610003</v>
           </cell>
           <cell r="X86">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55700003</v>
+            <v>55610004</v>
           </cell>
           <cell r="X87">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55700004</v>
+            <v>55700001</v>
           </cell>
           <cell r="X88">
-            <v>9</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55900001</v>
+            <v>55700002</v>
           </cell>
           <cell r="X89">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55900002</v>
+            <v>55700003</v>
           </cell>
           <cell r="X90">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55900003</v>
+            <v>55700004</v>
           </cell>
           <cell r="X91">
-            <v>80</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55900004</v>
+            <v>55900001</v>
           </cell>
           <cell r="X92">
-            <v>-30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55900005</v>
+            <v>55900002</v>
           </cell>
           <cell r="X93">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55900006</v>
+            <v>55900003</v>
           </cell>
           <cell r="X94">
-            <v>35</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55900007</v>
+            <v>55900004</v>
           </cell>
           <cell r="X95">
-            <v>25</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55900008</v>
+            <v>55900005</v>
           </cell>
           <cell r="X96">
-            <v>40</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55900009</v>
+            <v>55900006</v>
           </cell>
           <cell r="X97">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55900010</v>
+            <v>55900007</v>
           </cell>
           <cell r="X98">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55900011</v>
+            <v>55900008</v>
           </cell>
           <cell r="X99">
-            <v>15</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55900012</v>
+            <v>55900009</v>
           </cell>
           <cell r="X100">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55900013</v>
+            <v>55900010</v>
           </cell>
           <cell r="X101">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55900014</v>
+            <v>55900011</v>
           </cell>
           <cell r="X102">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55900015</v>
+            <v>55900012</v>
           </cell>
           <cell r="X103">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55900016</v>
+            <v>55900013</v>
           </cell>
           <cell r="X104">
-            <v>45</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55900017</v>
+            <v>55900014</v>
           </cell>
           <cell r="X105">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55900018</v>
+            <v>55900015</v>
           </cell>
           <cell r="X106">
             <v>30</v>
@@ -10333,9 +10347,33 @@
         </row>
         <row r="107">
           <cell r="A107">
+            <v>55900016</v>
+          </cell>
+          <cell r="X107">
+            <v>45</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>55900017</v>
+          </cell>
+          <cell r="X108">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>55900018</v>
+          </cell>
+          <cell r="X109">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
             <v>55900019</v>
           </cell>
-          <cell r="X107">
+          <cell r="X110">
             <v>80</v>
           </cell>
         </row>
@@ -19373,167 +19411,167 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BC314" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" tableBorderDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BC314" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129" tableBorderDxfId="128">
   <autoFilter ref="A3:BC314"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="55">
-    <tableColumn id="1" name="Id" dataDxfId="126"/>
-    <tableColumn id="2" name="Name" dataDxfId="125"/>
-    <tableColumn id="22" name="Ename" dataDxfId="124"/>
-    <tableColumn id="23" name="Remark" dataDxfId="123"/>
-    <tableColumn id="3" name="Star" dataDxfId="122"/>
-    <tableColumn id="4" name="Type" dataDxfId="121"/>
-    <tableColumn id="5" name="Attr" dataDxfId="120"/>
-    <tableColumn id="58" name="Quality" dataDxfId="119">
+    <tableColumn id="1" name="Id" dataDxfId="127"/>
+    <tableColumn id="2" name="Name" dataDxfId="126"/>
+    <tableColumn id="22" name="Ename" dataDxfId="125"/>
+    <tableColumn id="23" name="Remark" dataDxfId="124"/>
+    <tableColumn id="3" name="Star" dataDxfId="123"/>
+    <tableColumn id="4" name="Type" dataDxfId="122"/>
+    <tableColumn id="5" name="Attr" dataDxfId="121"/>
+    <tableColumn id="58" name="Quality" dataDxfId="120">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="118"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="117"/>
-    <tableColumn id="24" name="VitP" dataDxfId="116"/>
-    <tableColumn id="25" name="Modify" dataDxfId="115"/>
-    <tableColumn id="9" name="Def" dataDxfId="114"/>
-    <tableColumn id="10" name="Mag" dataDxfId="113"/>
-    <tableColumn id="32" name="Spd" dataDxfId="112"/>
-    <tableColumn id="35" name="Hit" dataDxfId="111"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="110"/>
-    <tableColumn id="34" name="Crt" dataDxfId="109"/>
-    <tableColumn id="33" name="Luk" dataDxfId="108"/>
-    <tableColumn id="7" name="Sum" dataDxfId="107">
+    <tableColumn id="12" name="Cost" dataDxfId="119"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="118"/>
+    <tableColumn id="24" name="VitP" dataDxfId="117"/>
+    <tableColumn id="25" name="Modify" dataDxfId="116"/>
+    <tableColumn id="9" name="Def" dataDxfId="115"/>
+    <tableColumn id="10" name="Mag" dataDxfId="114"/>
+    <tableColumn id="32" name="Spd" dataDxfId="113"/>
+    <tableColumn id="35" name="Hit" dataDxfId="112"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="111"/>
+    <tableColumn id="34" name="Crt" dataDxfId="110"/>
+    <tableColumn id="33" name="Luk" dataDxfId="109"/>
+    <tableColumn id="7" name="Sum" dataDxfId="108">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AU4)+2.5*SUM(AI4:AM4)+IF(ISNUMBER(AH4),AH4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="106"/>
-    <tableColumn id="14" name="Mov" dataDxfId="105"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="104"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="103"/>
-    <tableColumn id="18" name="Skills" dataDxfId="102"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="101"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="100"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="99"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="98"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="97"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="96"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="95"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="94"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="93">
+    <tableColumn id="13" name="Range" dataDxfId="107"/>
+    <tableColumn id="14" name="Mov" dataDxfId="106"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="105"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="104"/>
+    <tableColumn id="18" name="Skills" dataDxfId="103"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="102"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="101"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="100"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="99"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="98"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="97"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="96"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="95"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="94">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="92"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="91"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="90"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="89"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="88"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="87">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="93"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="92"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="91"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="90"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="89"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="88">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="86"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="85"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="84"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="83"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="82"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="81"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="80"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="79">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="87"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="86"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="85"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="84"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="83"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="82"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="81"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="80">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="78"/>
-    <tableColumn id="20" name="Res" dataDxfId="77"/>
-    <tableColumn id="21" name="Icon" dataDxfId="76"/>
-    <tableColumn id="17" name="Cover" dataDxfId="75"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="74"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="73"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="72"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="79"/>
+    <tableColumn id="20" name="Res" dataDxfId="78"/>
+    <tableColumn id="21" name="Icon" dataDxfId="77"/>
+    <tableColumn id="17" name="Cover" dataDxfId="76"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="75"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="74"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BC10" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BC10" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A3:BC10"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="55">
-    <tableColumn id="1" name="Id" dataDxfId="55"/>
-    <tableColumn id="2" name="Name" dataDxfId="54"/>
-    <tableColumn id="22" name="Ename" dataDxfId="53"/>
-    <tableColumn id="23" name="Remark" dataDxfId="52"/>
-    <tableColumn id="3" name="Star" dataDxfId="51"/>
-    <tableColumn id="4" name="Type" dataDxfId="50"/>
-    <tableColumn id="5" name="Attr" dataDxfId="49"/>
-    <tableColumn id="58" name="Quality" dataDxfId="48">
+    <tableColumn id="1" name="Id" dataDxfId="56"/>
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="22" name="Ename" dataDxfId="54"/>
+    <tableColumn id="23" name="Remark" dataDxfId="53"/>
+    <tableColumn id="3" name="Star" dataDxfId="52"/>
+    <tableColumn id="4" name="Type" dataDxfId="51"/>
+    <tableColumn id="5" name="Attr" dataDxfId="50"/>
+    <tableColumn id="58" name="Quality" dataDxfId="49">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="47"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="46"/>
-    <tableColumn id="24" name="VitP" dataDxfId="45"/>
-    <tableColumn id="25" name="Modify" dataDxfId="44"/>
-    <tableColumn id="9" name="Def" dataDxfId="43"/>
-    <tableColumn id="10" name="Mag" dataDxfId="42"/>
-    <tableColumn id="32" name="Spd" dataDxfId="41"/>
-    <tableColumn id="35" name="Hit" dataDxfId="40"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="39"/>
-    <tableColumn id="34" name="Crt" dataDxfId="38"/>
-    <tableColumn id="33" name="Luk" dataDxfId="37"/>
-    <tableColumn id="7" name="Sum" dataDxfId="36">
+    <tableColumn id="12" name="Cost" dataDxfId="48"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="47"/>
+    <tableColumn id="24" name="VitP" dataDxfId="46"/>
+    <tableColumn id="25" name="Modify" dataDxfId="45"/>
+    <tableColumn id="9" name="Def" dataDxfId="44"/>
+    <tableColumn id="10" name="Mag" dataDxfId="43"/>
+    <tableColumn id="32" name="Spd" dataDxfId="42"/>
+    <tableColumn id="35" name="Hit" dataDxfId="41"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="40"/>
+    <tableColumn id="34" name="Crt" dataDxfId="39"/>
+    <tableColumn id="33" name="Luk" dataDxfId="38"/>
+    <tableColumn id="7" name="Sum" dataDxfId="37">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AU4)+2.5*SUM(AI4:AM4)+IF(ISNUMBER(AH4),AH4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="35"/>
-    <tableColumn id="14" name="Mov" dataDxfId="34"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="33"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="32"/>
-    <tableColumn id="18" name="Skills" dataDxfId="31"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="30"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="29"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="28"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="27"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="26"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="25"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="24"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="23"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="22">
+    <tableColumn id="13" name="Range" dataDxfId="36"/>
+    <tableColumn id="14" name="Mov" dataDxfId="35"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="34"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="33"/>
+    <tableColumn id="18" name="Skills" dataDxfId="32"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="31"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="30"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="29"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="28"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="27"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="26"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="25"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="24"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="23">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="21"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="20"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="19"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="18"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="17"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="16">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="22"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="21"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="20"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="19"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="18"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="17">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="15"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="14"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="13"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="12"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="11"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="10"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="9"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="8">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="16"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="15"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="14"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="13"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="12"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="7"/>
-    <tableColumn id="20" name="Res" dataDxfId="6"/>
-    <tableColumn id="21" name="Icon" dataDxfId="5"/>
-    <tableColumn id="17" name="Cover" dataDxfId="4"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
+    <tableColumn id="20" name="Res" dataDxfId="7"/>
+    <tableColumn id="21" name="Icon" dataDxfId="6"/>
+    <tableColumn id="17" name="Cover" dataDxfId="5"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -19840,10 +19878,10 @@
   <dimension ref="A1:BC314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P234" sqref="P234"/>
+      <selection pane="bottomRight" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20253,7 +20291,7 @@
         <v>776</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>786</v>
@@ -21168,7 +21206,7 @@
         <v>334</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
@@ -21233,7 +21271,7 @@
         <v>11</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="Z9" s="39">
         <v>55100011</v>
@@ -21396,7 +21434,7 @@
         <v>12</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="Z10" s="39">
         <v>55900008</v>
@@ -21708,7 +21746,7 @@
         <v>16</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="Z12" s="39">
         <v>55100004</v>
@@ -22028,7 +22066,7 @@
         <v>6</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="Z14" s="39"/>
       <c r="AA14" s="20"/>
@@ -23743,7 +23781,7 @@
         <v>31</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Z25" s="39"/>
       <c r="AA25" s="20"/>
@@ -24220,7 +24258,7 @@
         <v>6</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="Z28" s="39">
         <v>55900007</v>
@@ -24850,7 +24888,7 @@
         <v>40</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Z32" s="39"/>
       <c r="AA32" s="20"/>
@@ -25166,7 +25204,7 @@
         <v>16</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Z34" s="39">
         <v>55900006</v>
@@ -25488,7 +25526,7 @@
         <v>789</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="Z36" s="39"/>
       <c r="AA36" s="20"/>
@@ -25649,7 +25687,7 @@
         <v>38</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z37" s="39">
         <v>55610003</v>
@@ -26271,7 +26309,7 @@
         <v>51</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="Z41" s="39">
         <v>55100011</v>
@@ -26432,7 +26470,7 @@
         <v>53</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="Z42" s="39">
         <v>55000034</v>
@@ -26595,7 +26633,7 @@
         <v>4</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="Z43" s="39">
         <v>55900004</v>
@@ -27084,7 +27122,7 @@
         <v>2</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="Z46" s="39">
         <v>55510003</v>
@@ -27406,7 +27444,7 @@
         <v>16</v>
       </c>
       <c r="Y48" s="4" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="Z48" s="39">
         <v>55500009</v>
@@ -27816,7 +27854,7 @@
         <v>345</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="E51" s="4">
         <v>3</v>
@@ -27881,7 +27919,7 @@
         <v>9</v>
       </c>
       <c r="Y51" s="4" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="Z51" s="39">
         <v>55900017</v>
@@ -28199,7 +28237,7 @@
         <v>16</v>
       </c>
       <c r="Y53" s="4" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="Z53" s="39">
         <v>55110006</v>
@@ -28295,7 +28333,7 @@
         <v>534</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="E54" s="4">
         <v>3</v>
@@ -28360,7 +28398,7 @@
         <v>64</v>
       </c>
       <c r="Y54" s="4" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="Z54" s="39">
         <v>55100011</v>
@@ -28684,7 +28722,7 @@
         <v>4</v>
       </c>
       <c r="Y56" s="4" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="Z56" s="39">
         <v>55510003</v>
@@ -29261,7 +29299,7 @@
         <v>537</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="E60" s="4">
         <v>3</v>
@@ -29326,7 +29364,7 @@
         <v>9</v>
       </c>
       <c r="Y60" s="4" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="Z60" s="39">
         <v>55900018</v>
@@ -29485,7 +29523,7 @@
         <v>24</v>
       </c>
       <c r="Y61" s="4" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="Z61" s="39">
         <v>55510007</v>
@@ -29644,7 +29682,7 @@
         <v>65</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="Z62" s="39">
         <v>55510002</v>
@@ -29964,7 +30002,7 @@
         <v>24</v>
       </c>
       <c r="Y64" s="4" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="Z64" s="39">
         <v>55110010</v>
@@ -30441,7 +30479,7 @@
         <v>78</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Z67" s="39">
         <v>55000095</v>
@@ -30602,7 +30640,7 @@
         <v>78</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1026</v>
+        <v>1123</v>
       </c>
       <c r="Z68" s="39">
         <v>55100011</v>
@@ -30617,7 +30655,7 @@
         <v>50</v>
       </c>
       <c r="AD68" s="20">
-        <v>55000097</v>
+        <v>55600004</v>
       </c>
       <c r="AE68" s="20">
         <v>100</v>
@@ -30777,7 +30815,7 @@
         <v>40</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="Z69" s="39"/>
       <c r="AA69" s="20"/>
@@ -31258,7 +31296,7 @@
         <v>2</v>
       </c>
       <c r="Y72" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="Z72" s="39"/>
       <c r="AA72" s="20"/>
@@ -31417,7 +31455,7 @@
         <v>791</v>
       </c>
       <c r="Y73" s="4" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="Z73" s="39">
         <v>55510007</v>
@@ -31743,7 +31781,7 @@
         <v>89</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="Z75" s="39">
         <v>55000004</v>
@@ -32071,7 +32109,7 @@
         <v>92</v>
       </c>
       <c r="Y77" s="4" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="Z77" s="39">
         <v>55110007</v>
@@ -32180,7 +32218,7 @@
       </c>
       <c r="H78" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I78" s="4">
         <v>6</v>
@@ -32217,7 +32255,7 @@
       </c>
       <c r="T78" s="14">
         <f t="shared" si="5"/>
-        <v>293.68</v>
+        <v>1.6800000000000068</v>
       </c>
       <c r="U78" s="4">
         <v>0</v>
@@ -32255,7 +32293,7 @@
 IF(ISBLANK($AB78),0, LOOKUP($AB78,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC78/100)+
 IF(ISBLANK($AD78),0, LOOKUP($AD78,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE78/100)+
 IF(ISBLANK($AF78),0, LOOKUP($AF78,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG78/100)</f>
-        <v>380</v>
+        <v>88</v>
       </c>
       <c r="AI78" s="20">
         <v>0</v>
@@ -33035,7 +33073,7 @@
         <v>38</v>
       </c>
       <c r="Y83" s="4" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="Z83" s="39">
         <v>55100010</v>
@@ -33526,7 +33564,7 @@
         <v>6</v>
       </c>
       <c r="Y86" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="Z86" s="39"/>
       <c r="AA86" s="20"/>
@@ -33687,7 +33725,7 @@
         <v>86</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="Z87" s="39">
         <v>55100011</v>
@@ -33850,7 +33888,7 @@
         <v>0</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="Z88" s="39">
         <v>55200003</v>
@@ -34170,7 +34208,7 @@
         <v>107</v>
       </c>
       <c r="Y90" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="Z90" s="39"/>
       <c r="AA90" s="20"/>
@@ -35126,7 +35164,7 @@
         <v>2</v>
       </c>
       <c r="Y96" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="Z96" s="39"/>
       <c r="AA96" s="20"/>
@@ -35287,7 +35325,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="Z97" s="39">
         <v>55110007</v>
@@ -35615,7 +35653,7 @@
         <v>790</v>
       </c>
       <c r="Y99" s="4" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="Z99" s="39">
         <v>55510010</v>
@@ -35776,7 +35814,7 @@
         <v>78</v>
       </c>
       <c r="Y100" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="Z100" s="39"/>
       <c r="AA100" s="20"/>
@@ -36098,7 +36136,7 @@
         <v>16</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="Z102" s="39">
         <v>55900003</v>
@@ -37076,7 +37114,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="Z108" s="39">
         <v>55000017</v>
@@ -37392,7 +37430,7 @@
         <v>130</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="Z110" s="39">
         <v>55510009</v>
@@ -37861,7 +37899,7 @@
         <v>135</v>
       </c>
       <c r="Y113" s="4" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="Z113" s="39">
         <v>55000018</v>
@@ -38022,7 +38060,7 @@
         <v>89</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Z114" s="39"/>
       <c r="AA114" s="20"/>
@@ -38193,7 +38231,7 @@
         <v>94</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="Z115" s="39"/>
       <c r="AA115" s="20"/>
@@ -38364,7 +38402,7 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="Z116" s="39"/>
       <c r="AA116" s="20"/>
@@ -38533,7 +38571,7 @@
         <v>4</v>
       </c>
       <c r="Y117" s="7" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="Z117" s="39">
         <v>55900016</v>
@@ -38694,7 +38732,7 @@
         <v>40</v>
       </c>
       <c r="Y118" s="4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="Z118" s="39"/>
       <c r="AA118" s="20"/>
@@ -38865,7 +38903,7 @@
         <v>100</v>
       </c>
       <c r="Y119" s="4" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="Z119" s="39"/>
       <c r="AA119" s="20"/>
@@ -39036,7 +39074,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="Z120" s="39"/>
       <c r="AA120" s="20"/>
@@ -39207,7 +39245,7 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="Z121" s="39"/>
       <c r="AA121" s="20"/>
@@ -39378,7 +39416,7 @@
         <v>4</v>
       </c>
       <c r="Y122" s="4" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="Z122" s="39">
         <v>55000150</v>
@@ -39539,7 +39577,7 @@
         <v>4</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="Z123" s="39">
         <v>55000227</v>
@@ -40185,7 +40223,7 @@
         <v>4</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="Z127" s="39">
         <v>55110005</v>
@@ -40281,7 +40319,7 @@
         <v>583</v>
       </c>
       <c r="D128" s="21" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="E128" s="4">
         <v>2</v>
@@ -40346,7 +40384,7 @@
         <v>4</v>
       </c>
       <c r="Y128" s="4" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="Z128" s="39">
         <v>55900019</v>
@@ -40972,7 +41010,7 @@
         <v>4</v>
       </c>
       <c r="Y132" s="4" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="Z132" s="39">
         <v>55510010</v>
@@ -41296,7 +41334,7 @@
         <v>2</v>
       </c>
       <c r="Y134" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="Z134" s="39">
         <v>55900008</v>
@@ -41459,7 +41497,7 @@
         <v>78</v>
       </c>
       <c r="Y135" s="7" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="Z135" s="39">
         <v>55900016</v>
@@ -41620,7 +41658,7 @@
         <v>107</v>
       </c>
       <c r="Y136" s="4" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="Z136" s="39">
         <v>55110005</v>
@@ -41954,7 +41992,7 @@
         <v>6</v>
       </c>
       <c r="Y138" s="4" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="Z138" s="39">
         <v>55000157</v>
@@ -42421,7 +42459,7 @@
         <v>12</v>
       </c>
       <c r="Y141" s="4" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="Z141" s="20">
         <v>55610004</v>
@@ -42582,7 +42620,7 @@
         <v>40</v>
       </c>
       <c r="Y142" s="4" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="Z142" s="39">
         <v>55000018</v>
@@ -43224,7 +43262,7 @@
         <v>107</v>
       </c>
       <c r="Y146" s="4" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="Z146" s="39">
         <v>55000101</v>
@@ -43489,7 +43527,7 @@
         <v>499</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>801</v>
+        <v>1121</v>
       </c>
       <c r="E148" s="4">
         <v>2</v>
@@ -43502,19 +43540,19 @@
       </c>
       <c r="H148" s="4">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I148" s="4">
         <v>2</v>
       </c>
       <c r="J148" s="4">
-        <v>5</v>
+        <v>-10</v>
       </c>
       <c r="K148" s="4">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="L148" s="4">
-        <v>-3</v>
+        <v>-15</v>
       </c>
       <c r="M148" s="4">
         <v>0</v>
@@ -43539,7 +43577,7 @@
       </c>
       <c r="T148" s="14">
         <f t="shared" si="9"/>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="U148" s="4">
         <v>30</v>
@@ -43554,7 +43592,7 @@
         <v>794</v>
       </c>
       <c r="Y148" s="4" t="s">
-        <v>1033</v>
+        <v>1120</v>
       </c>
       <c r="Z148" s="39">
         <v>55100012</v>
@@ -43563,7 +43601,7 @@
         <v>100</v>
       </c>
       <c r="AB148" s="20">
-        <v>55000161</v>
+        <v>55600002</v>
       </c>
       <c r="AC148" s="20">
         <v>100</v>
@@ -43572,12 +43610,12 @@
       <c r="AE148" s="20"/>
       <c r="AF148" s="20"/>
       <c r="AG148" s="20"/>
-      <c r="AH148" s="20" t="e">
+      <c r="AH148" s="20">
         <f>IF(ISBLANK($Z148),0, LOOKUP($Z148,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA148/100)+
 IF(ISBLANK($AB148),0, LOOKUP($AB148,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC148/100)+
 IF(ISBLANK($AD148),0, LOOKUP($AD148,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE148/100)+
 IF(ISBLANK($AF148),0, LOOKUP($AF148,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG148/100)</f>
-        <v>#N/A</v>
+        <v>25</v>
       </c>
       <c r="AI148" s="20">
         <v>0</v>
@@ -43654,7 +43692,7 @@
         <v>371</v>
       </c>
       <c r="D149" s="21" t="s">
-        <v>801</v>
+        <v>1121</v>
       </c>
       <c r="E149" s="4">
         <v>3</v>
@@ -43667,19 +43705,19 @@
       </c>
       <c r="H149" s="4">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I149" s="4">
         <v>3</v>
       </c>
       <c r="J149" s="4">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="K149" s="4">
         <v>0</v>
       </c>
       <c r="L149" s="4">
-        <v>-2</v>
+        <v>-12</v>
       </c>
       <c r="M149" s="4">
         <v>0</v>
@@ -43704,7 +43742,7 @@
       </c>
       <c r="T149" s="14">
         <f t="shared" si="9"/>
-        <v>-12</v>
+        <v>4</v>
       </c>
       <c r="U149" s="4">
         <v>30</v>
@@ -43719,7 +43757,7 @@
         <v>166</v>
       </c>
       <c r="Y149" s="4" t="s">
-        <v>1034</v>
+        <v>1122</v>
       </c>
       <c r="Z149" s="39">
         <v>55100011</v>
@@ -43728,25 +43766,21 @@
         <v>100</v>
       </c>
       <c r="AB149" s="20">
-        <v>55100012</v>
+        <v>55600003</v>
       </c>
       <c r="AC149" s="20">
         <v>100</v>
       </c>
-      <c r="AD149" s="20">
-        <v>55000162</v>
-      </c>
-      <c r="AE149" s="20">
-        <v>100</v>
-      </c>
+      <c r="AD149" s="20"/>
+      <c r="AE149" s="20"/>
       <c r="AF149" s="20"/>
       <c r="AG149" s="20"/>
-      <c r="AH149" s="20" t="e">
+      <c r="AH149" s="20">
         <f>IF(ISBLANK($Z149),0, LOOKUP($Z149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA149/100)+
 IF(ISBLANK($AB149),0, LOOKUP($AB149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC149/100)+
 IF(ISBLANK($AD149),0, LOOKUP($AD149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE149/100)+
 IF(ISBLANK($AF149),0, LOOKUP($AF149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG149/100)</f>
-        <v>#N/A</v>
+        <v>16</v>
       </c>
       <c r="AI149" s="20">
         <v>0</v>
@@ -43888,7 +43922,7 @@
         <v>4</v>
       </c>
       <c r="Y150" s="4" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="Z150" s="39">
         <v>55000017</v>
@@ -44832,7 +44866,7 @@
         <v>4</v>
       </c>
       <c r="Y156" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="Z156" s="39"/>
       <c r="AA156" s="20"/>
@@ -45297,7 +45331,7 @@
         <v>2</v>
       </c>
       <c r="Y159" s="4" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="Z159" s="39"/>
       <c r="AA159" s="20"/>
@@ -45760,7 +45794,7 @@
         <v>107</v>
       </c>
       <c r="Y162" s="4" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="Z162" s="39">
         <v>55110010</v>
@@ -45856,7 +45890,7 @@
         <v>609</v>
       </c>
       <c r="D163" s="21" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="E163" s="4">
         <v>3</v>
@@ -45921,7 +45955,7 @@
         <v>107</v>
       </c>
       <c r="Y163" s="4" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="Z163" s="39">
         <v>55900010</v>
@@ -46080,7 +46114,7 @@
         <v>16</v>
       </c>
       <c r="Y164" s="4" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="Z164" s="39">
         <v>55110005</v>
@@ -46204,7 +46238,7 @@
         <v>-1</v>
       </c>
       <c r="M165" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N165" s="4">
         <v>0</v>
@@ -46226,7 +46260,7 @@
       </c>
       <c r="T165" s="14">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="U165" s="4">
         <v>10</v>
@@ -46241,7 +46275,7 @@
         <v>38</v>
       </c>
       <c r="Y165" s="4" t="s">
-        <v>979</v>
+        <v>1119</v>
       </c>
       <c r="Z165" s="39">
         <v>55000145</v>
@@ -46249,12 +46283,8 @@
       <c r="AA165" s="20">
         <v>100</v>
       </c>
-      <c r="AB165" s="20">
-        <v>55000163</v>
-      </c>
-      <c r="AC165" s="20">
-        <v>25</v>
-      </c>
+      <c r="AB165" s="20"/>
+      <c r="AC165" s="20"/>
       <c r="AD165" s="20">
         <v>55610002</v>
       </c>
@@ -46740,7 +46770,7 @@
         <v>16</v>
       </c>
       <c r="Y168" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="Z168" s="39"/>
       <c r="AA168" s="20"/>
@@ -47386,7 +47416,7 @@
         <v>4</v>
       </c>
       <c r="Y172" s="4" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="Z172" s="39">
         <v>55000181</v>
@@ -47812,7 +47842,7 @@
         <v>616</v>
       </c>
       <c r="D175" s="21" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="E175" s="4">
         <v>2</v>
@@ -47877,7 +47907,7 @@
         <v>2</v>
       </c>
       <c r="Y175" s="4" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="Z175" s="39">
         <v>55700003</v>
@@ -48042,7 +48072,7 @@
         <v>12</v>
       </c>
       <c r="Y176" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z176" s="39">
         <v>55610003</v>
@@ -48527,7 +48557,7 @@
         <v>2</v>
       </c>
       <c r="Y179" s="4" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="Z179" s="39">
         <v>55110005</v>
@@ -48688,7 +48718,7 @@
         <v>65</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="Z180" s="39">
         <v>55000061</v>
@@ -49026,7 +49056,7 @@
         <v>4</v>
       </c>
       <c r="Y182" s="4" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="Z182" s="39">
         <v>55610003</v>
@@ -49682,7 +49712,7 @@
         <v>78</v>
       </c>
       <c r="Y186" s="4" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="Z186" s="39">
         <v>55000125</v>
@@ -50002,7 +50032,7 @@
         <v>2</v>
       </c>
       <c r="Y188" s="4" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="Z188" s="39">
         <v>55000196</v>
@@ -50481,7 +50511,7 @@
         <v>24</v>
       </c>
       <c r="Y191" s="4" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="Z191" s="39">
         <v>55900004</v>
@@ -50815,7 +50845,7 @@
         <v>2</v>
       </c>
       <c r="Y193" s="4" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="Z193" s="39">
         <v>55100011</v>
@@ -50919,7 +50949,7 @@
         <v>631</v>
       </c>
       <c r="D194" s="21" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="E194" s="4">
         <v>5</v>
@@ -50984,7 +51014,7 @@
         <v>16</v>
       </c>
       <c r="Y194" s="4" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="Z194" s="39">
         <v>55900014</v>
@@ -51149,7 +51179,7 @@
         <v>209</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="Z195" s="39">
         <v>55000016</v>
@@ -51318,7 +51348,7 @@
         <v>4</v>
       </c>
       <c r="Y196" s="4" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="Z196" s="20">
         <v>55520003</v>
@@ -51479,7 +51509,7 @@
         <v>4</v>
       </c>
       <c r="Y197" s="4" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="Z197" s="39">
         <v>55000020</v>
@@ -51648,7 +51678,7 @@
         <v>22</v>
       </c>
       <c r="Y198" s="4" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="Z198" s="39">
         <v>55100011</v>
@@ -52459,7 +52489,7 @@
         <v>16</v>
       </c>
       <c r="Y203" s="4" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="Z203" s="39">
         <v>55110011</v>
@@ -52620,7 +52650,7 @@
         <v>2</v>
       </c>
       <c r="Y204" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="Z204" s="39">
         <v>55000150</v>
@@ -53745,7 +53775,7 @@
         <v>69</v>
       </c>
       <c r="Y211" s="4" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="Z211" s="39">
         <v>55000208</v>
@@ -53914,7 +53944,7 @@
         <v>132</v>
       </c>
       <c r="Y212" s="4" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="Z212" s="39"/>
       <c r="AA212" s="20"/>
@@ -54075,7 +54105,7 @@
         <v>924</v>
       </c>
       <c r="Y213" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="Z213" s="39">
         <v>55000114</v>
@@ -54397,7 +54427,7 @@
         <v>190</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="Z215" s="39">
         <v>55100001</v>
@@ -54880,7 +54910,7 @@
         <v>4</v>
       </c>
       <c r="Y218" s="4" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="Z218" s="39">
         <v>55100012</v>
@@ -55371,7 +55401,7 @@
         <v>237</v>
       </c>
       <c r="Y221" s="4" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="Z221" s="39">
         <v>55000215</v>
@@ -55534,7 +55564,7 @@
         <v>6</v>
       </c>
       <c r="Y222" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="Z222" s="39">
         <v>55900005</v>
@@ -55693,7 +55723,7 @@
         <v>9</v>
       </c>
       <c r="Y223" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Z223" s="39">
         <v>55100008</v>
@@ -55854,7 +55884,7 @@
         <v>107</v>
       </c>
       <c r="Y224" s="7" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="Z224" s="39">
         <v>55900016</v>
@@ -56019,7 +56049,7 @@
         <v>16</v>
       </c>
       <c r="Y225" s="4" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="Z225" s="39">
         <v>55000009</v>
@@ -56343,7 +56373,7 @@
         <v>172</v>
       </c>
       <c r="Y227" s="4" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="Z227" s="39">
         <v>55110012</v>
@@ -57470,7 +57500,7 @@
         <v>22</v>
       </c>
       <c r="Y234" s="4" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="Z234" s="39">
         <v>55110009</v>
@@ -57959,7 +57989,7 @@
         <v>2</v>
       </c>
       <c r="Y237" s="4" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="Z237" s="39">
         <v>55100001</v>
@@ -58275,7 +58305,7 @@
         <v>4</v>
       </c>
       <c r="Y239" s="4" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="Z239" s="39">
         <v>55110001</v>
@@ -58605,7 +58635,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="Z241" s="39">
         <v>55100010</v>
@@ -59269,7 +59299,7 @@
         <v>69</v>
       </c>
       <c r="Y245" s="4" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="Z245" s="39">
         <v>55000131</v>
@@ -59438,7 +59468,7 @@
         <v>251</v>
       </c>
       <c r="Y246" s="4" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="Z246" s="39">
         <v>55100010</v>
@@ -59599,7 +59629,7 @@
         <v>2</v>
       </c>
       <c r="Y247" s="4" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="Z247" s="39">
         <v>55000258</v>
@@ -60078,7 +60108,7 @@
         <v>2</v>
       </c>
       <c r="Y250" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="Z250" s="39">
         <v>55500008</v>
@@ -60412,7 +60442,7 @@
         <v>135</v>
       </c>
       <c r="Y252" s="4" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="Z252" s="39"/>
       <c r="AA252" s="20"/>
@@ -60575,7 +60605,7 @@
         <v>19</v>
       </c>
       <c r="Y253" s="4" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="Z253" s="39">
         <v>55900015</v>
@@ -60671,7 +60701,7 @@
         <v>390</v>
       </c>
       <c r="D254" s="21" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="E254" s="4">
         <v>3</v>
@@ -60736,7 +60766,7 @@
         <v>209</v>
       </c>
       <c r="Y254" s="4" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="Z254" s="20">
         <v>55100013</v>
@@ -61060,7 +61090,7 @@
         <v>4</v>
       </c>
       <c r="Y256" s="4" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="Z256" s="39">
         <v>55110005</v>
@@ -61551,7 +61581,7 @@
         <v>4</v>
       </c>
       <c r="Y259" s="7" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="Z259" s="39">
         <v>55100012</v>
@@ -61816,7 +61846,7 @@
         <v>395</v>
       </c>
       <c r="D261" s="21" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="E261" s="4">
         <v>3</v>
@@ -61881,7 +61911,7 @@
         <v>16</v>
       </c>
       <c r="Y261" s="4" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="Z261" s="39">
         <v>55900014</v>
@@ -62356,7 +62386,7 @@
         <v>4</v>
       </c>
       <c r="Y264" s="4" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="Z264" s="39">
         <v>55000271</v>
@@ -62515,7 +62545,7 @@
         <v>2</v>
       </c>
       <c r="Y265" s="4" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="Z265" s="39">
         <v>55110007</v>
@@ -62676,7 +62706,7 @@
         <v>24</v>
       </c>
       <c r="Y266" s="4" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="Z266" s="39">
         <v>55000093</v>
@@ -63338,7 +63368,7 @@
         <v>16</v>
       </c>
       <c r="Y270" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="Z270" s="39"/>
       <c r="AA270" s="20"/>
@@ -63499,7 +63529,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="Z271" s="39">
         <v>55000019</v>
@@ -63664,7 +63694,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="Z272" s="39">
         <v>55000275</v>
@@ -63833,7 +63863,7 @@
         <v>799</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="Z273" s="39">
         <v>55000136</v>
@@ -64002,7 +64032,7 @@
         <v>0</v>
       </c>
       <c r="Y274" s="4" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="Z274" s="39">
         <v>55200003</v>
@@ -64163,7 +64193,7 @@
         <v>277</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="Z275" s="39">
         <v>55000278</v>
@@ -65131,7 +65161,7 @@
         <v>9</v>
       </c>
       <c r="Y281" s="4" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="Z281" s="39">
         <v>55900009</v>
@@ -65290,7 +65320,7 @@
         <v>6</v>
       </c>
       <c r="Y282" s="4" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="Z282" s="39">
         <v>55900009</v>
@@ -65449,7 +65479,7 @@
         <v>16</v>
       </c>
       <c r="Y283" s="4" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="Z283" s="39">
         <v>55900009</v>
@@ -65775,7 +65805,7 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z285" s="39">
         <v>55000289</v>
@@ -66741,7 +66771,7 @@
         <v>78</v>
       </c>
       <c r="Y291" s="4" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="Z291" s="39">
         <v>55510010</v>
@@ -66906,7 +66936,7 @@
         <v>22</v>
       </c>
       <c r="Y292" s="4" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="Z292" s="39"/>
       <c r="AA292" s="20"/>
@@ -67658,7 +67688,7 @@
         <v>409</v>
       </c>
       <c r="D297" s="21" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="E297" s="4">
         <v>3</v>
@@ -67723,7 +67753,7 @@
         <v>45</v>
       </c>
       <c r="Y297" s="4" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="Z297" s="39">
         <v>55900011</v>
@@ -67819,7 +67849,7 @@
         <v>410</v>
       </c>
       <c r="D298" s="21" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="E298" s="4">
         <v>2</v>
@@ -67884,7 +67914,7 @@
         <v>2</v>
       </c>
       <c r="Y298" s="7" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="Z298" s="39">
         <v>55900012</v>
@@ -68363,7 +68393,7 @@
         <v>111</v>
       </c>
       <c r="Y301" s="4" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="Z301" s="39">
         <v>55000013</v>
@@ -68532,7 +68562,7 @@
         <v>209</v>
       </c>
       <c r="Y302" s="4" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="Z302" s="39">
         <v>55000335</v>
@@ -68628,7 +68658,7 @@
         <v>701</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="E303" s="10">
         <v>2</v>
@@ -68693,7 +68723,7 @@
         <v>78</v>
       </c>
       <c r="Y303" s="10" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="Z303" s="39">
         <v>55100012</v>
@@ -68789,7 +68819,7 @@
         <v>710</v>
       </c>
       <c r="D304" s="21" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="E304" s="10">
         <v>2</v>
@@ -68854,7 +68884,7 @@
         <v>6</v>
       </c>
       <c r="Y304" s="10" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="Z304" s="39">
         <v>55100014</v>
@@ -68950,7 +68980,7 @@
         <v>711</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="E305" s="10">
         <v>3</v>
@@ -69015,7 +69045,7 @@
         <v>6</v>
       </c>
       <c r="Y305" s="10" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="Z305" s="39">
         <v>55100014</v>
@@ -69111,7 +69141,7 @@
         <v>712</v>
       </c>
       <c r="D306" s="21" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="E306" s="10">
         <v>4</v>
@@ -69176,7 +69206,7 @@
         <v>78</v>
       </c>
       <c r="Y306" s="10" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="Z306" s="39">
         <v>55100014</v>
@@ -69339,7 +69369,7 @@
         <v>0</v>
       </c>
       <c r="Y307" s="10" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="Z307" s="39">
         <v>55200003</v>
@@ -70542,24 +70572,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H314">
-    <cfRule type="cellIs" dxfId="135" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="136" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D314">
-    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -72188,25 +72218,25 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K9:K10 K4 J5:K6">
-    <cfRule type="cellIs" dxfId="71" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="70" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="69" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="21" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="68" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="20" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -72224,13 +72254,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="67" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="16" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="66" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="15" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -72248,13 +72278,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="64" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -72272,19 +72302,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix some new weapon card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -5497,241 +5497,6 @@
   <dxfs count="138">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -5896,6 +5661,34 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -7082,6 +6875,140 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7231,6 +7158,34 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -8428,6 +8383,51 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -8465,7 +8465,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8528,7 +8527,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8565,9 +8563,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8641,7 +8637,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8730,11 +8725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-695033648"/>
-        <c:axId val="-695032016"/>
+        <c:axId val="1078600864"/>
+        <c:axId val="1078600320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-695033648"/>
+        <c:axId val="1078600864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8777,7 +8772,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-695032016"/>
+        <c:crossAx val="1078600320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8785,7 +8780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-695032016"/>
+        <c:axId val="1078600320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8836,7 +8831,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-695033648"/>
+        <c:crossAx val="1078600864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8850,7 +8845,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19818,175 +19812,169 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BD301" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136" tableBorderDxfId="135">
-  <autoFilter ref="A3:BD301">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="基本"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BD301" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130" tableBorderDxfId="129">
+  <autoFilter ref="A3:BD301"/>
   <sortState ref="A4:BC301">
     <sortCondition ref="A3:A301"/>
   </sortState>
   <tableColumns count="56">
-    <tableColumn id="1" name="Id" dataDxfId="134"/>
-    <tableColumn id="2" name="Name" dataDxfId="133"/>
-    <tableColumn id="22" name="Ename" dataDxfId="132"/>
-    <tableColumn id="23" name="Remark" dataDxfId="131"/>
-    <tableColumn id="3" name="Star" dataDxfId="130"/>
-    <tableColumn id="4" name="Type" dataDxfId="129"/>
-    <tableColumn id="5" name="Attr" dataDxfId="128"/>
-    <tableColumn id="58" name="Quality" dataDxfId="127">
+    <tableColumn id="1" name="Id" dataDxfId="128"/>
+    <tableColumn id="2" name="Name" dataDxfId="127"/>
+    <tableColumn id="22" name="Ename" dataDxfId="126"/>
+    <tableColumn id="23" name="Remark" dataDxfId="125"/>
+    <tableColumn id="3" name="Star" dataDxfId="124"/>
+    <tableColumn id="4" name="Type" dataDxfId="123"/>
+    <tableColumn id="5" name="Attr" dataDxfId="122"/>
+    <tableColumn id="58" name="Quality" dataDxfId="121">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="126"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="125"/>
-    <tableColumn id="24" name="VitP" dataDxfId="124"/>
-    <tableColumn id="25" name="Modify" dataDxfId="123"/>
-    <tableColumn id="9" name="Def" dataDxfId="122"/>
-    <tableColumn id="10" name="Mag" dataDxfId="121"/>
-    <tableColumn id="32" name="Spd" dataDxfId="120"/>
-    <tableColumn id="35" name="Hit" dataDxfId="119"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="118"/>
-    <tableColumn id="34" name="Crt" dataDxfId="117"/>
-    <tableColumn id="33" name="Luk" dataDxfId="116"/>
-    <tableColumn id="7" name="Sum" dataDxfId="115">
+    <tableColumn id="12" name="Cost" dataDxfId="120"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="119"/>
+    <tableColumn id="24" name="VitP" dataDxfId="118"/>
+    <tableColumn id="25" name="Modify" dataDxfId="117"/>
+    <tableColumn id="9" name="Def" dataDxfId="116"/>
+    <tableColumn id="10" name="Mag" dataDxfId="115"/>
+    <tableColumn id="32" name="Spd" dataDxfId="114"/>
+    <tableColumn id="35" name="Hit" dataDxfId="113"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="112"/>
+    <tableColumn id="34" name="Crt" dataDxfId="111"/>
+    <tableColumn id="33" name="Luk" dataDxfId="110"/>
+    <tableColumn id="7" name="Sum" dataDxfId="109">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AU4)+2.5*SUM(AI4:AM4)+IF(ISNUMBER(AH4),AH4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="114"/>
-    <tableColumn id="14" name="Mov" dataDxfId="113"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="112"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="111"/>
-    <tableColumn id="18" name="Skills" dataDxfId="110"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="109"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="108"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="107"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="106"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="105"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="104"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="103"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="102"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="101">
+    <tableColumn id="13" name="Range" dataDxfId="108"/>
+    <tableColumn id="14" name="Mov" dataDxfId="107"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="106"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="105"/>
+    <tableColumn id="18" name="Skills" dataDxfId="104"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="103"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="102"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="101"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="100"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="99"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="98"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="97"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="96"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="95">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="100"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="99"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="98"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="97"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="96"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="95">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="94"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="93"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="92"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="91"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="90"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="89">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="94"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="93"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="92"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="91"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="90"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="89"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="88"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="87">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="88"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="87"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="86"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="85"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="84"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="83"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="82"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="81">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="86"/>
-    <tableColumn id="29" name="JobId" dataDxfId="20"/>
-    <tableColumn id="20" name="Res" dataDxfId="85"/>
-    <tableColumn id="21" name="Icon" dataDxfId="84"/>
-    <tableColumn id="17" name="Cover" dataDxfId="83"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="82"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="81"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="80"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="80"/>
+    <tableColumn id="29" name="JobId" dataDxfId="79"/>
+    <tableColumn id="20" name="Res" dataDxfId="78"/>
+    <tableColumn id="21" name="Icon" dataDxfId="77"/>
+    <tableColumn id="17" name="Cover" dataDxfId="76"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="75"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="74"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BD10" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BD10" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A3:BD10"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="56">
-    <tableColumn id="1" name="Id" dataDxfId="76"/>
-    <tableColumn id="2" name="Name" dataDxfId="75"/>
-    <tableColumn id="22" name="Ename" dataDxfId="74"/>
-    <tableColumn id="23" name="Remark" dataDxfId="73"/>
-    <tableColumn id="3" name="Star" dataDxfId="72"/>
-    <tableColumn id="4" name="Type" dataDxfId="71"/>
-    <tableColumn id="5" name="Attr" dataDxfId="70"/>
-    <tableColumn id="58" name="Quality" dataDxfId="69">
+    <tableColumn id="1" name="Id" dataDxfId="56"/>
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="22" name="Ename" dataDxfId="54"/>
+    <tableColumn id="23" name="Remark" dataDxfId="53"/>
+    <tableColumn id="3" name="Star" dataDxfId="52"/>
+    <tableColumn id="4" name="Type" dataDxfId="51"/>
+    <tableColumn id="5" name="Attr" dataDxfId="50"/>
+    <tableColumn id="58" name="Quality" dataDxfId="49">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="68"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="67"/>
-    <tableColumn id="24" name="VitP" dataDxfId="66"/>
-    <tableColumn id="25" name="Modify" dataDxfId="65"/>
-    <tableColumn id="9" name="Def" dataDxfId="64"/>
-    <tableColumn id="10" name="Mag" dataDxfId="63"/>
-    <tableColumn id="32" name="Spd" dataDxfId="62"/>
-    <tableColumn id="35" name="Hit" dataDxfId="61"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="60"/>
-    <tableColumn id="34" name="Crt" dataDxfId="59"/>
-    <tableColumn id="33" name="Luk" dataDxfId="58"/>
-    <tableColumn id="7" name="Sum" dataDxfId="57">
+    <tableColumn id="12" name="Cost" dataDxfId="48"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="47"/>
+    <tableColumn id="24" name="VitP" dataDxfId="46"/>
+    <tableColumn id="25" name="Modify" dataDxfId="45"/>
+    <tableColumn id="9" name="Def" dataDxfId="44"/>
+    <tableColumn id="10" name="Mag" dataDxfId="43"/>
+    <tableColumn id="32" name="Spd" dataDxfId="42"/>
+    <tableColumn id="35" name="Hit" dataDxfId="41"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="40"/>
+    <tableColumn id="34" name="Crt" dataDxfId="39"/>
+    <tableColumn id="33" name="Luk" dataDxfId="38"/>
+    <tableColumn id="7" name="Sum" dataDxfId="37">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AO4:AU4)+2.5*SUM(AI4:AM4)+IF(ISNUMBER(AH4),AH4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="56"/>
-    <tableColumn id="14" name="Mov" dataDxfId="55"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="54"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="53"/>
-    <tableColumn id="18" name="Skills" dataDxfId="52"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="51"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="50"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="49"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="48"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="47"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="46"/>
-    <tableColumn id="48" name="~Skill4" dataDxfId="45"/>
-    <tableColumn id="49" name="~SkillRate4" dataDxfId="44"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="43">
+    <tableColumn id="13" name="Range" dataDxfId="36"/>
+    <tableColumn id="14" name="Mov" dataDxfId="35"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="34"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="33"/>
+    <tableColumn id="18" name="Skills" dataDxfId="32"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="31"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="30"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="29"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="28"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="27"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="26"/>
+    <tableColumn id="48" name="~Skill4" dataDxfId="25"/>
+    <tableColumn id="49" name="~SkillRate4" dataDxfId="24"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="23">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)+
 IF(ISBLANK($AF4),0, LOOKUP($AF4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="42"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="41"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="40"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="39"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="38"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="37">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="22"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="21"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="20"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="19"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="18"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="17">
       <calculatedColumnFormula>CONCATENATE(AI4,";",AJ4,";",AK4,";",AL4,";",AM4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="36"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="35"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="34"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="33"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="32"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="31"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="30"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="29">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="16"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="15"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="14"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="13"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="12"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE(AO4,";",AP4,";",AQ4,";",AR4,";",AS4,";",AT4,";",AU4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="28"/>
-    <tableColumn id="29" name="JobId" dataDxfId="0"/>
-    <tableColumn id="20" name="Res" dataDxfId="27"/>
-    <tableColumn id="21" name="Icon" dataDxfId="26"/>
-    <tableColumn id="17" name="Cover" dataDxfId="25"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="24"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="23"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="22"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
+    <tableColumn id="29" name="JobId" dataDxfId="7"/>
+    <tableColumn id="20" name="Res" dataDxfId="6"/>
+    <tableColumn id="21" name="Icon" dataDxfId="5"/>
+    <tableColumn id="17" name="Cover" dataDxfId="4"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -20292,11 +20280,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AX1" sqref="AX1:AX3"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20321,7 +20309,7 @@
     <col min="47" max="47" width="4.375" customWidth="1"/>
     <col min="48" max="48" width="15.75" customWidth="1"/>
     <col min="49" max="49" width="6.375" customWidth="1"/>
-    <col min="50" max="50" width="8.5" customWidth="1"/>
+    <col min="50" max="50" width="9.625" customWidth="1"/>
     <col min="51" max="51" width="6" customWidth="1"/>
     <col min="52" max="52" width="4.625" customWidth="1"/>
     <col min="53" max="53" width="5.75" customWidth="1"/>
@@ -20983,7 +20971,7 @@
       <c r="AW4" s="52" t="s">
         <v>843</v>
       </c>
-      <c r="AX4" s="52"/>
+      <c r="AX4" s="14"/>
       <c r="AY4" s="4">
         <v>6</v>
       </c>
@@ -21001,7 +20989,7 @@
         <v>0.104918</v>
       </c>
     </row>
-    <row r="5" spans="1:56" hidden="1">
+    <row r="5" spans="1:56">
       <c r="A5">
         <v>51000002</v>
       </c>
@@ -21161,7 +21149,7 @@
         <v>0.30327870000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:56" hidden="1">
+    <row r="6" spans="1:56">
       <c r="A6">
         <v>51000003</v>
       </c>
@@ -21315,7 +21303,7 @@
         <v>0.52786889999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:56" hidden="1">
+    <row r="7" spans="1:56">
       <c r="A7">
         <v>51000004</v>
       </c>
@@ -21625,7 +21613,7 @@
         <v>0.40819670000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:56" hidden="1">
+    <row r="9" spans="1:56">
       <c r="A9">
         <v>51000006</v>
       </c>
@@ -21791,7 +21779,7 @@
         <v>0.3180328</v>
       </c>
     </row>
-    <row r="10" spans="1:56" hidden="1">
+    <row r="10" spans="1:56">
       <c r="A10">
         <v>51000007</v>
       </c>
@@ -21951,7 +21939,7 @@
         <v>0.20163929999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:56" hidden="1">
+    <row r="11" spans="1:56">
       <c r="A11">
         <v>51000008</v>
       </c>
@@ -22105,7 +22093,7 @@
         <v>0.2377049</v>
       </c>
     </row>
-    <row r="12" spans="1:56" hidden="1">
+    <row r="12" spans="1:56">
       <c r="A12">
         <v>51000009</v>
       </c>
@@ -22425,7 +22413,7 @@
         <v>0.48688520000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:56" hidden="1">
+    <row r="14" spans="1:56">
       <c r="A14">
         <v>51000011</v>
       </c>
@@ -23993,7 +23981,7 @@
         <v>0.26885249999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:56" hidden="1">
+    <row r="24" spans="1:56">
       <c r="A24">
         <v>51000021</v>
       </c>
@@ -24153,7 +24141,7 @@
         <v>0.34754099999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:56" hidden="1">
+    <row r="25" spans="1:56">
       <c r="A25">
         <v>51000022</v>
       </c>
@@ -24471,7 +24459,7 @@
         <v>0.6426229</v>
       </c>
     </row>
-    <row r="27" spans="1:56" hidden="1">
+    <row r="27" spans="1:56">
       <c r="A27">
         <v>51000024</v>
       </c>
@@ -24631,7 +24619,7 @@
         <v>0.58032790000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:56" hidden="1">
+    <row r="28" spans="1:56">
       <c r="A28">
         <v>51000025</v>
       </c>
@@ -24791,7 +24779,7 @@
         <v>0.23278689999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:56" hidden="1">
+    <row r="29" spans="1:56">
       <c r="A29">
         <v>51000026</v>
       </c>
@@ -24951,7 +24939,7 @@
         <v>0.38524589999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:56" hidden="1">
+    <row r="30" spans="1:56">
       <c r="A30">
         <v>51000027</v>
       </c>
@@ -25111,7 +25099,7 @@
         <v>0.58196720000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:56" hidden="1">
+    <row r="31" spans="1:56">
       <c r="A31">
         <v>51000028</v>
       </c>
@@ -25271,7 +25259,7 @@
         <v>0.50819669999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:56" hidden="1">
+    <row r="32" spans="1:56">
       <c r="A32">
         <v>51000029</v>
       </c>
@@ -25425,7 +25413,7 @@
         <v>0.51475409999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:56" hidden="1">
+    <row r="33" spans="1:56">
       <c r="A33">
         <v>51000030</v>
       </c>
@@ -25579,7 +25567,7 @@
         <v>0.43278689999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:56" hidden="1">
+    <row r="34" spans="1:56">
       <c r="A34">
         <v>51000031</v>
       </c>
@@ -25739,7 +25727,7 @@
         <v>0.20163929999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:56" hidden="1">
+    <row r="35" spans="1:56">
       <c r="A35">
         <v>51000032</v>
       </c>
@@ -25901,7 +25889,7 @@
         <v>5.0819669999999997E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:56" hidden="1">
+    <row r="36" spans="1:56">
       <c r="A36">
         <v>51000033</v>
       </c>
@@ -26063,7 +26051,7 @@
         <v>0.36721310000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:56" hidden="1">
+    <row r="37" spans="1:56">
       <c r="A37">
         <v>51000034</v>
       </c>
@@ -26381,7 +26369,7 @@
         <v>0.25901639999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:56" hidden="1">
+    <row r="39" spans="1:56">
       <c r="A39">
         <v>51000036</v>
       </c>
@@ -26535,7 +26523,7 @@
         <v>0.76393440000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:56" hidden="1">
+    <row r="40" spans="1:56">
       <c r="A40">
         <v>51000037</v>
       </c>
@@ -26689,7 +26677,7 @@
         <v>0.79836059999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:56" hidden="1">
+    <row r="41" spans="1:56">
       <c r="A41">
         <v>51000038</v>
       </c>
@@ -26851,7 +26839,7 @@
         <v>0.2377049</v>
       </c>
     </row>
-    <row r="42" spans="1:56" hidden="1">
+    <row r="42" spans="1:56">
       <c r="A42">
         <v>51000039</v>
       </c>
@@ -27017,7 +27005,7 @@
         <v>0.57868850000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:56" hidden="1">
+    <row r="43" spans="1:56">
       <c r="A43">
         <v>51000040</v>
       </c>
@@ -27177,7 +27165,7 @@
         <v>0.13606560000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:56" hidden="1">
+    <row r="44" spans="1:56">
       <c r="A44">
         <v>51000041</v>
       </c>
@@ -27339,7 +27327,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="45" spans="1:56" hidden="1">
+    <row r="45" spans="1:56">
       <c r="A45">
         <v>51000042</v>
       </c>
@@ -27499,7 +27487,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:56" hidden="1">
+    <row r="46" spans="1:56">
       <c r="A46">
         <v>51000043</v>
       </c>
@@ -27663,7 +27651,7 @@
         <v>0.38688529999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:56" hidden="1">
+    <row r="47" spans="1:56">
       <c r="A47">
         <v>51000044</v>
       </c>
@@ -27823,7 +27811,7 @@
         <v>0.5557377</v>
       </c>
     </row>
-    <row r="48" spans="1:56" hidden="1">
+    <row r="48" spans="1:56">
       <c r="A48">
         <v>51000045</v>
       </c>
@@ -27983,7 +27971,7 @@
         <v>0.46721309999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:56" hidden="1">
+    <row r="49" spans="1:56">
       <c r="A49">
         <v>51000046</v>
       </c>
@@ -28145,7 +28133,7 @@
         <v>0.3245902</v>
       </c>
     </row>
-    <row r="50" spans="1:56" hidden="1">
+    <row r="50" spans="1:56">
       <c r="A50">
         <v>51000047</v>
       </c>
@@ -28299,7 +28287,7 @@
         <v>0.8573771</v>
       </c>
     </row>
-    <row r="51" spans="1:56" hidden="1">
+    <row r="51" spans="1:56">
       <c r="A51">
         <v>51000048</v>
       </c>
@@ -28461,7 +28449,7 @@
         <v>0.33606560000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:56" hidden="1">
+    <row r="52" spans="1:56">
       <c r="A52">
         <v>51000049</v>
       </c>
@@ -28621,7 +28609,7 @@
         <v>0.2377049</v>
       </c>
     </row>
-    <row r="53" spans="1:56" hidden="1">
+    <row r="53" spans="1:56">
       <c r="A53">
         <v>51000050</v>
       </c>
@@ -28781,7 +28769,7 @@
         <v>0.39836070000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:56" hidden="1">
+    <row r="54" spans="1:56">
       <c r="A54">
         <v>51000051</v>
       </c>
@@ -28947,7 +28935,7 @@
         <v>0.53442619999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:56" hidden="1">
+    <row r="55" spans="1:56">
       <c r="A55">
         <v>51000052</v>
       </c>
@@ -29109,7 +29097,7 @@
         <v>0.33770489999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:56" hidden="1">
+    <row r="56" spans="1:56">
       <c r="A56">
         <v>51000053</v>
       </c>
@@ -29269,7 +29257,7 @@
         <v>0.5557377</v>
       </c>
     </row>
-    <row r="57" spans="1:56" hidden="1">
+    <row r="57" spans="1:56">
       <c r="A57">
         <v>51000054</v>
       </c>
@@ -29433,7 +29421,7 @@
         <v>0.24918029999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:56" hidden="1">
+    <row r="58" spans="1:56">
       <c r="A58">
         <v>51000055</v>
       </c>
@@ -29593,7 +29581,7 @@
         <v>0.3967213</v>
       </c>
     </row>
-    <row r="59" spans="1:56" hidden="1">
+    <row r="59" spans="1:56">
       <c r="A59">
         <v>51000056</v>
       </c>
@@ -29753,7 +29741,7 @@
         <v>0.70163940000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:56" hidden="1">
+    <row r="60" spans="1:56">
       <c r="A60">
         <v>51000057</v>
       </c>
@@ -29915,7 +29903,7 @@
         <v>0.26065569999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:56" hidden="1">
+    <row r="61" spans="1:56">
       <c r="A61">
         <v>51000058</v>
       </c>
@@ -30075,7 +30063,7 @@
         <v>0.17213120000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:56" hidden="1">
+    <row r="62" spans="1:56">
       <c r="A62">
         <v>51000059</v>
       </c>
@@ -30235,7 +30223,7 @@
         <v>0.13278690000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:56" hidden="1">
+    <row r="63" spans="1:56">
       <c r="A63">
         <v>51000060</v>
       </c>
@@ -30395,7 +30383,7 @@
         <v>0.75737699999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:56" hidden="1">
+    <row r="64" spans="1:56">
       <c r="A64">
         <v>51000061</v>
       </c>
@@ -30711,7 +30699,7 @@
         <v>0.14590159999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:56" hidden="1">
+    <row r="66" spans="1:56">
       <c r="A66">
         <v>51000063</v>
       </c>
@@ -30873,7 +30861,7 @@
         <v>0.15245900000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:56" hidden="1">
+    <row r="67" spans="1:56">
       <c r="A67">
         <v>51000064</v>
       </c>
@@ -31035,7 +31023,7 @@
         <v>0.8180328</v>
       </c>
     </row>
-    <row r="68" spans="1:56" hidden="1">
+    <row r="68" spans="1:56">
       <c r="A68">
         <v>51000065</v>
       </c>
@@ -31207,7 +31195,7 @@
         <v>0.95081970000000005</v>
       </c>
     </row>
-    <row r="69" spans="1:56" hidden="1">
+    <row r="69" spans="1:56">
       <c r="A69">
         <v>51000066</v>
       </c>
@@ -31369,7 +31357,7 @@
         <v>0.84098360000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:56" hidden="1">
+    <row r="70" spans="1:56">
       <c r="A70">
         <v>51000067</v>
       </c>
@@ -31533,7 +31521,7 @@
         <v>0.89508200000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:56" hidden="1">
+    <row r="71" spans="1:56">
       <c r="A71">
         <v>51000068</v>
       </c>
@@ -31687,7 +31675,7 @@
         <v>0.36065570000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:56" hidden="1">
+    <row r="72" spans="1:56">
       <c r="A72">
         <v>51000069</v>
       </c>
@@ -31841,7 +31829,7 @@
         <v>0.72786890000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:56" hidden="1">
+    <row r="73" spans="1:56">
       <c r="A73">
         <v>51000070</v>
       </c>
@@ -32001,7 +31989,7 @@
         <v>0.63278690000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:56" hidden="1">
+    <row r="74" spans="1:56">
       <c r="A74">
         <v>51000071</v>
       </c>
@@ -32161,7 +32149,7 @@
         <v>0.70491800000000004</v>
       </c>
     </row>
-    <row r="75" spans="1:56" hidden="1">
+    <row r="75" spans="1:56">
       <c r="A75">
         <v>51000072</v>
       </c>
@@ -32327,7 +32315,7 @@
         <v>0.31475409999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:56" hidden="1">
+    <row r="76" spans="1:56">
       <c r="A76">
         <v>51000073</v>
       </c>
@@ -32493,7 +32481,7 @@
         <v>0.81147539999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:56" hidden="1">
+    <row r="77" spans="1:56">
       <c r="A77">
         <v>51000074</v>
       </c>
@@ -32653,7 +32641,7 @@
         <v>0.36721310000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:56" hidden="1">
+    <row r="78" spans="1:56">
       <c r="A78">
         <v>51000075</v>
       </c>
@@ -33131,7 +33119,7 @@
         <v>0.1147541</v>
       </c>
     </row>
-    <row r="81" spans="1:56" hidden="1">
+    <row r="81" spans="1:56">
       <c r="A81">
         <v>51000078</v>
       </c>
@@ -33297,7 +33285,7 @@
         <v>0.48196719999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:56" hidden="1">
+    <row r="82" spans="1:56">
       <c r="A82">
         <v>51000079</v>
       </c>
@@ -33461,7 +33449,7 @@
         <v>0.82622949999999995</v>
       </c>
     </row>
-    <row r="83" spans="1:56" hidden="1">
+    <row r="83" spans="1:56">
       <c r="A83">
         <v>51000080</v>
       </c>
@@ -33621,7 +33609,7 @@
         <v>0.71147539999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:56" hidden="1">
+    <row r="84" spans="1:56">
       <c r="A84">
         <v>51000081</v>
       </c>
@@ -33783,7 +33771,7 @@
         <v>0.40819670000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:56" hidden="1">
+    <row r="85" spans="1:56">
       <c r="A85">
         <v>51000082</v>
       </c>
@@ -33945,7 +33933,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:56" hidden="1">
+    <row r="86" spans="1:56">
       <c r="A86">
         <v>51000083</v>
       </c>
@@ -34107,7 +34095,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:56" hidden="1">
+    <row r="87" spans="1:56">
       <c r="A87">
         <v>51000084</v>
       </c>
@@ -34271,7 +34259,7 @@
         <v>0.50819669999999995</v>
       </c>
     </row>
-    <row r="88" spans="1:56" hidden="1">
+    <row r="88" spans="1:56">
       <c r="A88">
         <v>51000085</v>
       </c>
@@ -34431,7 +34419,7 @@
         <v>0.33770489999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:56" hidden="1">
+    <row r="89" spans="1:56">
       <c r="A89">
         <v>51000086</v>
       </c>
@@ -34591,7 +34579,7 @@
         <v>0.32131150000000003</v>
       </c>
     </row>
-    <row r="90" spans="1:56" hidden="1">
+    <row r="90" spans="1:56">
       <c r="A90">
         <v>51000087</v>
       </c>
@@ -34755,7 +34743,7 @@
         <v>0.67213109999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:56" hidden="1">
+    <row r="91" spans="1:56">
       <c r="A91">
         <v>51000088</v>
       </c>
@@ -34917,7 +34905,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="92" spans="1:56" hidden="1">
+    <row r="92" spans="1:56">
       <c r="A92">
         <v>51000089</v>
       </c>
@@ -35077,7 +35065,7 @@
         <v>0.47868850000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:56" hidden="1">
+    <row r="93" spans="1:56">
       <c r="A93">
         <v>51000090</v>
       </c>
@@ -35231,7 +35219,7 @@
         <v>0.3327869</v>
       </c>
     </row>
-    <row r="94" spans="1:56" hidden="1">
+    <row r="94" spans="1:56">
       <c r="A94">
         <v>51000091</v>
       </c>
@@ -35397,7 +35385,7 @@
         <v>0.84262289999999995</v>
       </c>
     </row>
-    <row r="95" spans="1:56" hidden="1">
+    <row r="95" spans="1:56">
       <c r="A95">
         <v>51000092</v>
       </c>
@@ -35551,7 +35539,7 @@
         <v>0.48688520000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:56" hidden="1">
+    <row r="96" spans="1:56">
       <c r="A96">
         <v>51000093</v>
       </c>
@@ -35715,7 +35703,7 @@
         <v>0.66557379999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:56" hidden="1">
+    <row r="97" spans="1:56">
       <c r="A97">
         <v>51000094</v>
       </c>
@@ -35885,7 +35873,7 @@
         <v>0.93114750000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:56" hidden="1">
+    <row r="98" spans="1:56">
       <c r="A98">
         <v>51000095</v>
       </c>
@@ -36047,7 +36035,7 @@
         <v>0.51803279999999996</v>
       </c>
     </row>
-    <row r="99" spans="1:56" hidden="1">
+    <row r="99" spans="1:56">
       <c r="A99">
         <v>51000096</v>
       </c>
@@ -36207,7 +36195,7 @@
         <v>0.36393439999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:56" hidden="1">
+    <row r="100" spans="1:56">
       <c r="A100">
         <v>51000097</v>
       </c>
@@ -36367,7 +36355,7 @@
         <v>0.38196720000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:56" hidden="1">
+    <row r="101" spans="1:56">
       <c r="A101">
         <v>51000098</v>
       </c>
@@ -36521,7 +36509,7 @@
         <v>0.60327869999999995</v>
       </c>
     </row>
-    <row r="102" spans="1:56" hidden="1">
+    <row r="102" spans="1:56">
       <c r="A102">
         <v>51000099</v>
       </c>
@@ -36685,7 +36673,7 @@
         <v>0.75737699999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:56" hidden="1">
+    <row r="103" spans="1:56">
       <c r="A103">
         <v>51000100</v>
       </c>
@@ -36847,7 +36835,7 @@
         <v>0.1032787</v>
       </c>
     </row>
-    <row r="104" spans="1:56" hidden="1">
+    <row r="104" spans="1:56">
       <c r="A104">
         <v>51000101</v>
       </c>
@@ -37013,7 +37001,7 @@
         <v>0.42622949999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:56" hidden="1">
+    <row r="105" spans="1:56">
       <c r="A105">
         <v>51000102</v>
       </c>
@@ -37179,7 +37167,7 @@
         <v>0.2098361</v>
       </c>
     </row>
-    <row r="106" spans="1:56" hidden="1">
+    <row r="106" spans="1:56">
       <c r="A106">
         <v>51000103</v>
       </c>
@@ -37341,7 +37329,7 @@
         <v>4.262295E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:56" hidden="1">
+    <row r="107" spans="1:56">
       <c r="A107">
         <v>51000104</v>
       </c>
@@ -37503,7 +37491,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:56" hidden="1">
+    <row r="108" spans="1:56">
       <c r="A108">
         <v>51000105</v>
       </c>
@@ -37663,7 +37651,7 @@
         <v>0.92622950000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:56" hidden="1">
+    <row r="109" spans="1:56">
       <c r="A109">
         <v>51000106</v>
       </c>
@@ -37817,7 +37805,7 @@
         <v>6.8852460000000004E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:56" hidden="1">
+    <row r="110" spans="1:56">
       <c r="A110">
         <v>51000107</v>
       </c>
@@ -37977,7 +37965,7 @@
         <v>0.24262300000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:56" hidden="1">
+    <row r="111" spans="1:56">
       <c r="A111">
         <v>51000108</v>
       </c>
@@ -38131,7 +38119,7 @@
         <v>0.28360659999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:56" hidden="1">
+    <row r="112" spans="1:56">
       <c r="A112">
         <v>51000109</v>
       </c>
@@ -38285,7 +38273,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:56" hidden="1">
+    <row r="113" spans="1:56">
       <c r="A113">
         <v>51000110</v>
       </c>
@@ -38439,7 +38427,7 @@
         <v>0.51147540000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:56" hidden="1">
+    <row r="114" spans="1:56">
       <c r="A114">
         <v>51000111</v>
       </c>
@@ -38611,7 +38599,7 @@
         <v>0.9442623</v>
       </c>
     </row>
-    <row r="115" spans="1:56" hidden="1">
+    <row r="115" spans="1:56">
       <c r="A115">
         <v>51000112</v>
       </c>
@@ -38783,7 +38771,7 @@
         <v>0.94262299999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:56" hidden="1">
+    <row r="116" spans="1:56">
       <c r="A116">
         <v>51000113</v>
       </c>
@@ -38955,7 +38943,7 @@
         <v>0.92786880000000005</v>
       </c>
     </row>
-    <row r="117" spans="1:56" hidden="1">
+    <row r="117" spans="1:56">
       <c r="A117">
         <v>51000114</v>
       </c>
@@ -39127,7 +39115,7 @@
         <v>0.94918029999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:56" hidden="1">
+    <row r="118" spans="1:56">
       <c r="A118">
         <v>51000115</v>
       </c>
@@ -39299,7 +39287,7 @@
         <v>0.9442623</v>
       </c>
     </row>
-    <row r="119" spans="1:56" hidden="1">
+    <row r="119" spans="1:56">
       <c r="A119">
         <v>51000116</v>
       </c>
@@ -39461,7 +39449,7 @@
         <v>0.19508200000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:56" hidden="1">
+    <row r="120" spans="1:56">
       <c r="A120">
         <v>51000117</v>
       </c>
@@ -39633,7 +39621,7 @@
         <v>0.92786880000000005</v>
       </c>
     </row>
-    <row r="121" spans="1:56" hidden="1">
+    <row r="121" spans="1:56">
       <c r="A121">
         <v>51000118</v>
       </c>
@@ -39805,7 +39793,7 @@
         <v>0.95409829999999995</v>
       </c>
     </row>
-    <row r="122" spans="1:56" hidden="1">
+    <row r="122" spans="1:56">
       <c r="A122">
         <v>51000119</v>
       </c>
@@ -39967,7 +39955,7 @@
         <v>0.24426229999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:56" hidden="1">
+    <row r="123" spans="1:56">
       <c r="A123">
         <v>51000120</v>
       </c>
@@ -40127,7 +40115,7 @@
         <v>0.27213110000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:56" hidden="1">
+    <row r="124" spans="1:56">
       <c r="A124">
         <v>51000121</v>
       </c>
@@ -40289,7 +40277,7 @@
         <v>0.49836069999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:56" hidden="1">
+    <row r="125" spans="1:56">
       <c r="A125">
         <v>51000122</v>
       </c>
@@ -40453,7 +40441,7 @@
         <v>0.73114749999999995</v>
       </c>
     </row>
-    <row r="126" spans="1:56" hidden="1">
+    <row r="126" spans="1:56">
       <c r="A126">
         <v>51000123</v>
       </c>
@@ -40615,7 +40603,7 @@
         <v>9.3442629999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:56" hidden="1">
+    <row r="127" spans="1:56">
       <c r="A127">
         <v>51000124</v>
       </c>
@@ -40775,7 +40763,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="128" spans="1:56" hidden="1">
+    <row r="128" spans="1:56">
       <c r="A128">
         <v>51000125</v>
       </c>
@@ -40937,7 +40925,7 @@
         <v>0.62131150000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:56" hidden="1">
+    <row r="129" spans="1:56">
       <c r="A129">
         <v>51000126</v>
       </c>
@@ -41091,7 +41079,7 @@
         <v>0.85901640000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:56" hidden="1">
+    <row r="130" spans="1:56">
       <c r="A130">
         <v>51000127</v>
       </c>
@@ -41253,7 +41241,7 @@
         <v>0.1114754</v>
       </c>
     </row>
-    <row r="131" spans="1:56" hidden="1">
+    <row r="131" spans="1:56">
       <c r="A131">
         <v>51000128</v>
       </c>
@@ -41407,7 +41395,7 @@
         <v>0.31639339999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:56" hidden="1">
+    <row r="132" spans="1:56">
       <c r="A132">
         <v>51000129</v>
       </c>
@@ -41567,7 +41555,7 @@
         <v>0.76393440000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:56" hidden="1">
+    <row r="133" spans="1:56">
       <c r="A133">
         <v>51000130</v>
       </c>
@@ -41731,7 +41719,7 @@
         <v>0.67213109999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:56" hidden="1">
+    <row r="134" spans="1:56">
       <c r="A134">
         <v>51000131</v>
       </c>
@@ -41895,7 +41883,7 @@
         <v>0.44098359999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:56" hidden="1">
+    <row r="135" spans="1:56">
       <c r="A135">
         <v>51000132</v>
       </c>
@@ -42055,7 +42043,7 @@
         <v>0.43442619999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:56" hidden="1">
+    <row r="136" spans="1:56">
       <c r="A136">
         <v>51000133</v>
       </c>
@@ -42221,7 +42209,7 @@
         <v>0.50819669999999995</v>
       </c>
     </row>
-    <row r="137" spans="1:56" hidden="1">
+    <row r="137" spans="1:56">
       <c r="A137">
         <v>51000134</v>
       </c>
@@ -42385,7 +42373,7 @@
         <v>0.80983609999999995</v>
       </c>
     </row>
-    <row r="138" spans="1:56" hidden="1">
+    <row r="138" spans="1:56">
       <c r="A138">
         <v>51000135</v>
       </c>
@@ -42547,7 +42535,7 @@
         <v>0.25245899999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:56" hidden="1">
+    <row r="139" spans="1:56">
       <c r="A139">
         <v>51000136</v>
       </c>
@@ -42857,7 +42845,7 @@
         <v>0.36393439999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:56" hidden="1">
+    <row r="141" spans="1:56">
       <c r="A141">
         <v>51000138</v>
       </c>
@@ -43017,7 +43005,7 @@
         <v>0.52295080000000005</v>
       </c>
     </row>
-    <row r="142" spans="1:56" hidden="1">
+    <row r="142" spans="1:56">
       <c r="A142">
         <v>51000139</v>
       </c>
@@ -43171,7 +43159,7 @@
         <v>0.3491803</v>
       </c>
     </row>
-    <row r="143" spans="1:56" hidden="1">
+    <row r="143" spans="1:56">
       <c r="A143">
         <v>51000140</v>
       </c>
@@ -43331,7 +43319,7 @@
         <v>0.26065569999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:56" hidden="1">
+    <row r="144" spans="1:56">
       <c r="A144">
         <v>51000141</v>
       </c>
@@ -43647,7 +43635,7 @@
         <v>0.13770489999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:56" hidden="1">
+    <row r="146" spans="1:56">
       <c r="A146">
         <v>51000143</v>
       </c>
@@ -43811,7 +43799,7 @@
         <v>0.75081969999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:56" hidden="1">
+    <row r="147" spans="1:56">
       <c r="A147">
         <v>51000144</v>
       </c>
@@ -43977,7 +43965,7 @@
         <v>0.41639340000000002</v>
       </c>
     </row>
-    <row r="148" spans="1:56" hidden="1">
+    <row r="148" spans="1:56">
       <c r="A148">
         <v>51000145</v>
       </c>
@@ -44143,7 +44131,7 @@
         <v>0.1983607</v>
       </c>
     </row>
-    <row r="149" spans="1:56" hidden="1">
+    <row r="149" spans="1:56">
       <c r="A149">
         <v>51000146</v>
       </c>
@@ -44309,7 +44297,7 @@
         <v>0.52295080000000005</v>
       </c>
     </row>
-    <row r="150" spans="1:56" hidden="1">
+    <row r="150" spans="1:56">
       <c r="A150">
         <v>51000147</v>
       </c>
@@ -44469,7 +44457,7 @@
         <v>0.68852460000000004</v>
       </c>
     </row>
-    <row r="151" spans="1:56" hidden="1">
+    <row r="151" spans="1:56">
       <c r="A151">
         <v>51000148</v>
       </c>
@@ -44779,7 +44767,7 @@
         <v>0.35409829999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:56" hidden="1">
+    <row r="153" spans="1:56">
       <c r="A153">
         <v>51000150</v>
       </c>
@@ -44939,7 +44927,7 @@
         <v>0.32295079999999998</v>
       </c>
     </row>
-    <row r="154" spans="1:56" hidden="1">
+    <row r="154" spans="1:56">
       <c r="A154">
         <v>51000151</v>
       </c>
@@ -45093,7 +45081,7 @@
         <v>0.40819670000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:56" hidden="1">
+    <row r="155" spans="1:56">
       <c r="A155">
         <v>51000152</v>
       </c>
@@ -45255,7 +45243,7 @@
         <v>0.58688530000000005</v>
       </c>
     </row>
-    <row r="156" spans="1:56" hidden="1">
+    <row r="156" spans="1:56">
       <c r="A156">
         <v>51000153</v>
       </c>
@@ -45567,7 +45555,7 @@
         <v>0.12950819999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:56" hidden="1">
+    <row r="158" spans="1:56">
       <c r="A158">
         <v>51000155</v>
       </c>
@@ -45877,7 +45865,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="160" spans="1:56" hidden="1">
+    <row r="160" spans="1:56">
       <c r="A160">
         <v>51000157</v>
       </c>
@@ -46187,7 +46175,7 @@
         <v>0.3098361</v>
       </c>
     </row>
-    <row r="162" spans="1:56" hidden="1">
+    <row r="162" spans="1:56">
       <c r="A162">
         <v>51000159</v>
       </c>
@@ -46347,7 +46335,7 @@
         <v>0.44754100000000002</v>
       </c>
     </row>
-    <row r="163" spans="1:56" hidden="1">
+    <row r="163" spans="1:56">
       <c r="A163">
         <v>51000160</v>
       </c>
@@ -46509,7 +46497,7 @@
         <v>0.45409840000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:56" hidden="1">
+    <row r="164" spans="1:56">
       <c r="A164">
         <v>51000161</v>
       </c>
@@ -46981,7 +46969,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="167" spans="1:56" hidden="1">
+    <row r="167" spans="1:56">
       <c r="A167">
         <v>51000164</v>
       </c>
@@ -47303,7 +47291,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="169" spans="1:56" hidden="1">
+    <row r="169" spans="1:56">
       <c r="A169">
         <v>51000166</v>
       </c>
@@ -47465,7 +47453,7 @@
         <v>5.7377049999999999E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:56" hidden="1">
+    <row r="170" spans="1:56">
       <c r="A170">
         <v>51000167</v>
       </c>
@@ -47627,7 +47615,7 @@
         <v>4.0983609999999997E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:56" hidden="1">
+    <row r="171" spans="1:56">
       <c r="A171">
         <v>51000168</v>
       </c>
@@ -47787,7 +47775,7 @@
         <v>4.590164E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:56" hidden="1">
+    <row r="172" spans="1:56">
       <c r="A172">
         <v>51000169</v>
       </c>
@@ -47953,7 +47941,7 @@
         <v>0.77540980000000004</v>
       </c>
     </row>
-    <row r="173" spans="1:56" hidden="1">
+    <row r="173" spans="1:56">
       <c r="A173">
         <v>51000170</v>
       </c>
@@ -48115,7 +48103,7 @@
         <v>9.0163930000000003E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:56" hidden="1">
+    <row r="174" spans="1:56">
       <c r="A174">
         <v>51000171</v>
       </c>
@@ -48277,7 +48265,7 @@
         <v>0.56721310000000003</v>
       </c>
     </row>
-    <row r="175" spans="1:56" hidden="1">
+    <row r="175" spans="1:56">
       <c r="A175">
         <v>51000172</v>
       </c>
@@ -48443,7 +48431,7 @@
         <v>0.104918</v>
       </c>
     </row>
-    <row r="176" spans="1:56" hidden="1">
+    <row r="176" spans="1:56">
       <c r="A176">
         <v>51000173</v>
       </c>
@@ -48605,7 +48593,7 @@
         <v>0.57213119999999995</v>
       </c>
     </row>
-    <row r="177" spans="1:56" hidden="1">
+    <row r="177" spans="1:56">
       <c r="A177">
         <v>51000174</v>
       </c>
@@ -48767,7 +48755,7 @@
         <v>0.25737710000000003</v>
       </c>
     </row>
-    <row r="178" spans="1:56" hidden="1">
+    <row r="178" spans="1:56">
       <c r="A178">
         <v>51000175</v>
       </c>
@@ -48933,7 +48921,7 @@
         <v>0.64590159999999996</v>
       </c>
     </row>
-    <row r="179" spans="1:56" hidden="1">
+    <row r="179" spans="1:56">
       <c r="A179">
         <v>51000176</v>
       </c>
@@ -49093,7 +49081,7 @@
         <v>0.49508200000000002</v>
       </c>
     </row>
-    <row r="180" spans="1:56" hidden="1">
+    <row r="180" spans="1:56">
       <c r="A180">
         <v>51000177</v>
       </c>
@@ -49257,7 +49245,7 @@
         <v>0.80819669999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:56" hidden="1">
+    <row r="181" spans="1:56">
       <c r="A181">
         <v>51000178</v>
       </c>
@@ -49427,7 +49415,7 @@
         <v>0.91639349999999997</v>
       </c>
     </row>
-    <row r="182" spans="1:56" hidden="1">
+    <row r="182" spans="1:56">
       <c r="A182">
         <v>51000179</v>
       </c>
@@ -49593,7 +49581,7 @@
         <v>0.27377050000000003</v>
       </c>
     </row>
-    <row r="183" spans="1:56" hidden="1">
+    <row r="183" spans="1:56">
       <c r="A183">
         <v>51000180</v>
       </c>
@@ -49759,7 +49747,7 @@
         <v>0.89508200000000004</v>
       </c>
     </row>
-    <row r="184" spans="1:56" hidden="1">
+    <row r="184" spans="1:56">
       <c r="A184">
         <v>51000181</v>
       </c>
@@ -49919,7 +49907,7 @@
         <v>0.65245900000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:56" hidden="1">
+    <row r="185" spans="1:56">
       <c r="A185">
         <v>51000182</v>
       </c>
@@ -50085,7 +50073,7 @@
         <v>0.91639349999999997</v>
       </c>
     </row>
-    <row r="186" spans="1:56" hidden="1">
+    <row r="186" spans="1:56">
       <c r="A186">
         <v>51000183</v>
       </c>
@@ -50247,7 +50235,7 @@
         <v>0.73114749999999995</v>
       </c>
     </row>
-    <row r="187" spans="1:56" hidden="1">
+    <row r="187" spans="1:56">
       <c r="A187">
         <v>51000184</v>
       </c>
@@ -50407,7 +50395,7 @@
         <v>0.37377050000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:56" hidden="1">
+    <row r="188" spans="1:56">
       <c r="A188">
         <v>51000185</v>
       </c>
@@ -50573,7 +50561,7 @@
         <v>0.9442623</v>
       </c>
     </row>
-    <row r="189" spans="1:56" hidden="1">
+    <row r="189" spans="1:56">
       <c r="A189">
         <v>51000186</v>
       </c>
@@ -50889,7 +50877,7 @@
         <v>0.1508197</v>
       </c>
     </row>
-    <row r="191" spans="1:56" hidden="1">
+    <row r="191" spans="1:56">
       <c r="A191">
         <v>51000188</v>
       </c>
@@ -51053,7 +51041,7 @@
         <v>0.85409840000000004</v>
       </c>
     </row>
-    <row r="192" spans="1:56" hidden="1">
+    <row r="192" spans="1:56">
       <c r="A192">
         <v>51000189</v>
       </c>
@@ -51223,7 +51211,7 @@
         <v>0.86229509999999998</v>
       </c>
     </row>
-    <row r="193" spans="1:56" hidden="1">
+    <row r="193" spans="1:56">
       <c r="A193">
         <v>51000190</v>
       </c>
@@ -51389,7 +51377,7 @@
         <v>0.8180328</v>
       </c>
     </row>
-    <row r="194" spans="1:56" hidden="1">
+    <row r="194" spans="1:56">
       <c r="A194">
         <v>51000191</v>
       </c>
@@ -51555,7 +51543,7 @@
         <v>0.89672130000000005</v>
       </c>
     </row>
-    <row r="195" spans="1:56" hidden="1">
+    <row r="195" spans="1:56">
       <c r="A195">
         <v>51000192</v>
       </c>
@@ -51725,7 +51713,7 @@
         <v>0.74262300000000003</v>
       </c>
     </row>
-    <row r="196" spans="1:56" hidden="1">
+    <row r="196" spans="1:56">
       <c r="A196">
         <v>51000193</v>
       </c>
@@ -51891,7 +51879,7 @@
         <v>0.79180329999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:56" hidden="1">
+    <row r="197" spans="1:56">
       <c r="A197">
         <v>51000194</v>
       </c>
@@ -52057,7 +52045,7 @@
         <v>0.8327869</v>
       </c>
     </row>
-    <row r="198" spans="1:56" hidden="1">
+    <row r="198" spans="1:56">
       <c r="A198">
         <v>51000195</v>
       </c>
@@ -52221,7 +52209,7 @@
         <v>0.81967210000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:56" hidden="1">
+    <row r="199" spans="1:56">
       <c r="A199">
         <v>51000196</v>
       </c>
@@ -52391,7 +52379,7 @@
         <v>0.9606557</v>
       </c>
     </row>
-    <row r="200" spans="1:56" hidden="1">
+    <row r="200" spans="1:56">
       <c r="A200">
         <v>51000197</v>
       </c>
@@ -52547,7 +52535,7 @@
         <v>0.82459009999999999</v>
       </c>
     </row>
-    <row r="201" spans="1:56" hidden="1">
+    <row r="201" spans="1:56">
       <c r="A201">
         <v>51000198</v>
       </c>
@@ -52709,7 +52697,7 @@
         <v>0.70327870000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:56" hidden="1">
+    <row r="202" spans="1:56">
       <c r="A202">
         <v>51000199</v>
       </c>
@@ -52869,7 +52857,7 @@
         <v>8.3606559999999996E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:56" hidden="1">
+    <row r="203" spans="1:56">
       <c r="A203">
         <v>51000200</v>
       </c>
@@ -53029,7 +53017,7 @@
         <v>0.38196720000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:56" hidden="1">
+    <row r="204" spans="1:56">
       <c r="A204">
         <v>51000201</v>
       </c>
@@ -53191,7 +53179,7 @@
         <v>0.3885246</v>
       </c>
     </row>
-    <row r="205" spans="1:56" hidden="1">
+    <row r="205" spans="1:56">
       <c r="A205">
         <v>51000202</v>
       </c>
@@ -53353,7 +53341,7 @@
         <v>0.3180328</v>
       </c>
     </row>
-    <row r="206" spans="1:56" hidden="1">
+    <row r="206" spans="1:56">
       <c r="A206">
         <v>51000203</v>
       </c>
@@ -53517,7 +53505,7 @@
         <v>0.54754100000000006</v>
       </c>
     </row>
-    <row r="207" spans="1:56" hidden="1">
+    <row r="207" spans="1:56">
       <c r="A207">
         <v>51000204</v>
       </c>
@@ -53677,7 +53665,7 @@
         <v>0.20491799999999999</v>
       </c>
     </row>
-    <row r="208" spans="1:56" hidden="1">
+    <row r="208" spans="1:56">
       <c r="A208">
         <v>51000205</v>
       </c>
@@ -53839,7 +53827,7 @@
         <v>0.53278689999999995</v>
       </c>
     </row>
-    <row r="209" spans="1:56" hidden="1">
+    <row r="209" spans="1:56">
       <c r="A209">
         <v>51000206</v>
       </c>
@@ -53999,7 +53987,7 @@
         <v>0.1622951</v>
       </c>
     </row>
-    <row r="210" spans="1:56" hidden="1">
+    <row r="210" spans="1:56">
       <c r="A210">
         <v>51000207</v>
       </c>
@@ -54153,7 +54141,7 @@
         <v>0.37704919999999997</v>
       </c>
     </row>
-    <row r="211" spans="1:56" hidden="1">
+    <row r="211" spans="1:56">
       <c r="A211">
         <v>51000208</v>
       </c>
@@ -54323,7 +54311,7 @@
         <v>0.6426229</v>
       </c>
     </row>
-    <row r="212" spans="1:56" hidden="1">
+    <row r="212" spans="1:56">
       <c r="A212">
         <v>51000209</v>
       </c>
@@ -54483,7 +54471,7 @@
         <v>0.67704920000000002</v>
       </c>
     </row>
-    <row r="213" spans="1:56" hidden="1">
+    <row r="213" spans="1:56">
       <c r="A213">
         <v>51000210</v>
       </c>
@@ -54649,7 +54637,7 @@
         <v>0.79016390000000003</v>
       </c>
     </row>
-    <row r="214" spans="1:56" hidden="1">
+    <row r="214" spans="1:56">
       <c r="A214">
         <v>51000211</v>
       </c>
@@ -54803,7 +54791,7 @@
         <v>0.3803279</v>
       </c>
     </row>
-    <row r="215" spans="1:56" hidden="1">
+    <row r="215" spans="1:56">
       <c r="A215">
         <v>51000212</v>
       </c>
@@ -54969,7 +54957,7 @@
         <v>0.75901640000000004</v>
       </c>
     </row>
-    <row r="216" spans="1:56" hidden="1">
+    <row r="216" spans="1:56">
       <c r="A216">
         <v>51000213</v>
       </c>
@@ -55123,7 +55111,7 @@
         <v>0.75737699999999997</v>
       </c>
     </row>
-    <row r="217" spans="1:56" hidden="1">
+    <row r="217" spans="1:56">
       <c r="A217">
         <v>51000214</v>
       </c>
@@ -55285,7 +55273,7 @@
         <v>0.37377050000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:56" hidden="1">
+    <row r="218" spans="1:56">
       <c r="A218">
         <v>51000215</v>
       </c>
@@ -55451,7 +55439,7 @@
         <v>0.24098359999999999</v>
       </c>
     </row>
-    <row r="219" spans="1:56" hidden="1">
+    <row r="219" spans="1:56">
       <c r="A219">
         <v>51000216</v>
       </c>
@@ -55617,7 +55605,7 @@
         <v>0.48032789999999997</v>
       </c>
     </row>
-    <row r="220" spans="1:56" hidden="1">
+    <row r="220" spans="1:56">
       <c r="A220">
         <v>51000217</v>
       </c>
@@ -55779,7 +55767,7 @@
         <v>0.404918</v>
       </c>
     </row>
-    <row r="221" spans="1:56" hidden="1">
+    <row r="221" spans="1:56">
       <c r="A221">
         <v>51000218</v>
       </c>
@@ -55945,7 +55933,7 @@
         <v>0.69672129999999999</v>
       </c>
     </row>
-    <row r="222" spans="1:56" hidden="1">
+    <row r="222" spans="1:56">
       <c r="A222">
         <v>51000219</v>
       </c>
@@ -56105,7 +56093,7 @@
         <v>0.41639340000000002</v>
       </c>
     </row>
-    <row r="223" spans="1:56" hidden="1">
+    <row r="223" spans="1:56">
       <c r="A223">
         <v>51000220</v>
       </c>
@@ -56265,7 +56253,7 @@
         <v>0.49508200000000002</v>
       </c>
     </row>
-    <row r="224" spans="1:56" hidden="1">
+    <row r="224" spans="1:56">
       <c r="A224">
         <v>51000221</v>
       </c>
@@ -56429,7 +56417,7 @@
         <v>0.83934430000000004</v>
       </c>
     </row>
-    <row r="225" spans="1:56" hidden="1">
+    <row r="225" spans="1:56">
       <c r="A225">
         <v>51000222</v>
       </c>
@@ -56595,7 +56583,7 @@
         <v>0.69016390000000005</v>
       </c>
     </row>
-    <row r="226" spans="1:56" hidden="1">
+    <row r="226" spans="1:56">
       <c r="A226">
         <v>51000223</v>
       </c>
@@ -56757,7 +56745,7 @@
         <v>0.82786890000000002</v>
       </c>
     </row>
-    <row r="227" spans="1:56" hidden="1">
+    <row r="227" spans="1:56">
       <c r="A227">
         <v>51000224</v>
       </c>
@@ -56917,7 +56905,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="228" spans="1:56" hidden="1">
+    <row r="228" spans="1:56">
       <c r="A228">
         <v>51000225</v>
       </c>
@@ -57083,7 +57071,7 @@
         <v>0.52295080000000005</v>
       </c>
     </row>
-    <row r="229" spans="1:56" hidden="1">
+    <row r="229" spans="1:56">
       <c r="A229">
         <v>51000226</v>
       </c>
@@ -57249,7 +57237,7 @@
         <v>0.47540979999999999</v>
       </c>
     </row>
-    <row r="230" spans="1:56" hidden="1">
+    <row r="230" spans="1:56">
       <c r="A230">
         <v>51000227</v>
       </c>
@@ -57411,7 +57399,7 @@
         <v>5.2459020000000002E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:56" hidden="1">
+    <row r="231" spans="1:56">
       <c r="A231">
         <v>51000228</v>
       </c>
@@ -57729,7 +57717,7 @@
         <v>3.9344259999999999E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:56" hidden="1">
+    <row r="233" spans="1:56">
       <c r="A233">
         <v>51000230</v>
       </c>
@@ -57891,7 +57879,7 @@
         <v>0.54426229999999998</v>
       </c>
     </row>
-    <row r="234" spans="1:56" hidden="1">
+    <row r="234" spans="1:56">
       <c r="A234">
         <v>51000231</v>
       </c>
@@ -58051,7 +58039,7 @@
         <v>0.8573771</v>
       </c>
     </row>
-    <row r="235" spans="1:56" hidden="1">
+    <row r="235" spans="1:56">
       <c r="A235">
         <v>51000232</v>
       </c>
@@ -58213,7 +58201,7 @@
         <v>0.595082</v>
       </c>
     </row>
-    <row r="236" spans="1:56" hidden="1">
+    <row r="236" spans="1:56">
       <c r="A236">
         <v>51000233</v>
       </c>
@@ -58375,7 +58363,7 @@
         <v>0.47704920000000001</v>
       </c>
     </row>
-    <row r="237" spans="1:56" hidden="1">
+    <row r="237" spans="1:56">
       <c r="A237">
         <v>51000234</v>
       </c>
@@ -58539,7 +58527,7 @@
         <v>0.70327870000000003</v>
       </c>
     </row>
-    <row r="238" spans="1:56" hidden="1">
+    <row r="238" spans="1:56">
       <c r="A238">
         <v>51000235</v>
       </c>
@@ -58693,7 +58681,7 @@
         <v>9.3442629999999999E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:56" hidden="1">
+    <row r="239" spans="1:56">
       <c r="A239">
         <v>51000236</v>
       </c>
@@ -58857,7 +58845,7 @@
         <v>0.77377050000000003</v>
       </c>
     </row>
-    <row r="240" spans="1:56" hidden="1">
+    <row r="240" spans="1:56">
       <c r="A240">
         <v>51000237</v>
       </c>
@@ -59023,7 +59011,7 @@
         <v>0.63934429999999998</v>
       </c>
     </row>
-    <row r="241" spans="1:56" hidden="1">
+    <row r="241" spans="1:56">
       <c r="A241">
         <v>51000238</v>
       </c>
@@ -59197,7 +59185,7 @@
         <v>0.89016399999999996</v>
       </c>
     </row>
-    <row r="242" spans="1:56" hidden="1">
+    <row r="242" spans="1:56">
       <c r="A242">
         <v>51000239</v>
       </c>
@@ -59351,7 +59339,7 @@
         <v>0.51311479999999998</v>
       </c>
     </row>
-    <row r="243" spans="1:56" hidden="1">
+    <row r="243" spans="1:56">
       <c r="A243">
         <v>51000240</v>
       </c>
@@ -59513,7 +59501,7 @@
         <v>0.54590170000000005</v>
       </c>
     </row>
-    <row r="244" spans="1:56" hidden="1">
+    <row r="244" spans="1:56">
       <c r="A244">
         <v>51000241</v>
       </c>
@@ -59679,7 +59667,7 @@
         <v>0.62131150000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:56" hidden="1">
+    <row r="245" spans="1:56">
       <c r="A245">
         <v>51000242</v>
       </c>
@@ -59849,7 +59837,7 @@
         <v>0.84590169999999998</v>
       </c>
     </row>
-    <row r="246" spans="1:56" hidden="1">
+    <row r="246" spans="1:56">
       <c r="A246">
         <v>51000243</v>
       </c>
@@ -60011,7 +59999,7 @@
         <v>0.85245899999999997</v>
       </c>
     </row>
-    <row r="247" spans="1:56" hidden="1">
+    <row r="247" spans="1:56">
       <c r="A247">
         <v>51000244</v>
       </c>
@@ -60175,7 +60163,7 @@
         <v>0.90983610000000004</v>
       </c>
     </row>
-    <row r="248" spans="1:56" hidden="1">
+    <row r="248" spans="1:56">
       <c r="A248">
         <v>51000245</v>
       </c>
@@ -60335,7 +60323,7 @@
         <v>5.0819669999999997E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:56" hidden="1">
+    <row r="249" spans="1:56">
       <c r="A249">
         <v>51000246</v>
       </c>
@@ -60489,7 +60477,7 @@
         <v>0.59836069999999997</v>
       </c>
     </row>
-    <row r="250" spans="1:56" hidden="1">
+    <row r="250" spans="1:56">
       <c r="A250">
         <v>51000247</v>
       </c>
@@ -60653,7 +60641,7 @@
         <v>0.94262299999999999</v>
       </c>
     </row>
-    <row r="251" spans="1:56" hidden="1">
+    <row r="251" spans="1:56">
       <c r="A251">
         <v>51000248</v>
       </c>
@@ -60813,7 +60801,7 @@
         <v>0.35573769999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:56" hidden="1">
+    <row r="252" spans="1:56">
       <c r="A252">
         <v>51000249</v>
       </c>
@@ -60973,7 +60961,7 @@
         <v>0.90163930000000003</v>
       </c>
     </row>
-    <row r="253" spans="1:56" hidden="1">
+    <row r="253" spans="1:56">
       <c r="A253">
         <v>51000250</v>
       </c>
@@ -61133,7 +61121,7 @@
         <v>0.64918039999999999</v>
       </c>
     </row>
-    <row r="254" spans="1:56" hidden="1">
+    <row r="254" spans="1:56">
       <c r="A254">
         <v>51000251</v>
       </c>
@@ -61295,7 +61283,7 @@
         <v>0.49836069999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:56" hidden="1">
+    <row r="255" spans="1:56">
       <c r="A255">
         <v>51000252</v>
       </c>
@@ -61461,7 +61449,7 @@
         <v>0.82786890000000002</v>
       </c>
     </row>
-    <row r="256" spans="1:56" hidden="1">
+    <row r="256" spans="1:56">
       <c r="A256">
         <v>51000253</v>
       </c>
@@ -61621,7 +61609,7 @@
         <v>0.63278690000000004</v>
       </c>
     </row>
-    <row r="257" spans="1:56" hidden="1">
+    <row r="257" spans="1:56">
       <c r="A257">
         <v>51000254</v>
       </c>
@@ -61787,7 +61775,7 @@
         <v>0.49344260000000001</v>
       </c>
     </row>
-    <row r="258" spans="1:56" hidden="1">
+    <row r="258" spans="1:56">
       <c r="A258">
         <v>51000255</v>
       </c>
@@ -61953,7 +61941,7 @@
         <v>0.2147541</v>
       </c>
     </row>
-    <row r="259" spans="1:56" hidden="1">
+    <row r="259" spans="1:56">
       <c r="A259">
         <v>51000256</v>
       </c>
@@ -62119,7 +62107,7 @@
         <v>0.25245899999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:56" hidden="1">
+    <row r="260" spans="1:56">
       <c r="A260">
         <v>51000257</v>
       </c>
@@ -62285,7 +62273,7 @@
         <v>0.28032790000000002</v>
       </c>
     </row>
-    <row r="261" spans="1:56" hidden="1">
+    <row r="261" spans="1:56">
       <c r="A261">
         <v>51000258</v>
       </c>
@@ -62447,7 +62435,7 @@
         <v>0.50327869999999997</v>
       </c>
     </row>
-    <row r="262" spans="1:56" hidden="1">
+    <row r="262" spans="1:56">
       <c r="A262">
         <v>51000259</v>
       </c>
@@ -62763,7 +62751,7 @@
         <v>0.1065574</v>
       </c>
     </row>
-    <row r="264" spans="1:56" hidden="1">
+    <row r="264" spans="1:56">
       <c r="A264">
         <v>51000261</v>
       </c>
@@ -62923,7 +62911,7 @@
         <v>0.4360656</v>
       </c>
     </row>
-    <row r="265" spans="1:56" hidden="1">
+    <row r="265" spans="1:56">
       <c r="A265">
         <v>51000262</v>
       </c>
@@ -63083,7 +63071,7 @@
         <v>0.57704920000000004</v>
       </c>
     </row>
-    <row r="266" spans="1:56" hidden="1">
+    <row r="266" spans="1:56">
       <c r="A266">
         <v>51000263</v>
       </c>
@@ -63253,7 +63241,7 @@
         <v>0.64590159999999996</v>
       </c>
     </row>
-    <row r="267" spans="1:56" hidden="1">
+    <row r="267" spans="1:56">
       <c r="A267">
         <v>51000264</v>
       </c>
@@ -63423,7 +63411,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="268" spans="1:56" hidden="1">
+    <row r="268" spans="1:56">
       <c r="A268">
         <v>51000265</v>
       </c>
@@ -63589,7 +63577,7 @@
         <v>0.5557377</v>
       </c>
     </row>
-    <row r="269" spans="1:56" hidden="1">
+    <row r="269" spans="1:56">
       <c r="A269">
         <v>51000266</v>
       </c>
@@ -63749,7 +63737,7 @@
         <v>0.4606557</v>
       </c>
     </row>
-    <row r="270" spans="1:56" hidden="1">
+    <row r="270" spans="1:56">
       <c r="A270">
         <v>51000267</v>
       </c>
@@ -63911,7 +63899,7 @@
         <v>0.58688530000000005</v>
       </c>
     </row>
-    <row r="271" spans="1:56" hidden="1">
+    <row r="271" spans="1:56">
       <c r="A271">
         <v>51000268</v>
       </c>
@@ -64077,7 +64065,7 @@
         <v>0.81147539999999996</v>
       </c>
     </row>
-    <row r="272" spans="1:56" hidden="1">
+    <row r="272" spans="1:56">
       <c r="A272">
         <v>51000269</v>
       </c>
@@ -64243,7 +64231,7 @@
         <v>0.77213109999999996</v>
       </c>
     </row>
-    <row r="273" spans="1:56" hidden="1">
+    <row r="273" spans="1:56">
       <c r="A273">
         <v>51000270</v>
       </c>
@@ -64413,7 +64401,7 @@
         <v>0.83442620000000001</v>
       </c>
     </row>
-    <row r="274" spans="1:56" hidden="1">
+    <row r="274" spans="1:56">
       <c r="A274">
         <v>51000271</v>
       </c>
@@ -64575,7 +64563,7 @@
         <v>0.12950819999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:56" hidden="1">
+    <row r="275" spans="1:56">
       <c r="A275">
         <v>51000272</v>
       </c>
@@ -64737,7 +64725,7 @@
         <v>0.40655740000000001</v>
       </c>
     </row>
-    <row r="276" spans="1:56" hidden="1">
+    <row r="276" spans="1:56">
       <c r="A276">
         <v>51000273</v>
       </c>
@@ -64891,7 +64879,7 @@
         <v>0.67049179999999997</v>
       </c>
     </row>
-    <row r="277" spans="1:56" hidden="1">
+    <row r="277" spans="1:56">
       <c r="A277">
         <v>51000274</v>
       </c>
@@ -65053,7 +65041,7 @@
         <v>0.48196719999999998</v>
       </c>
     </row>
-    <row r="278" spans="1:56" hidden="1">
+    <row r="278" spans="1:56">
       <c r="A278">
         <v>51000275</v>
       </c>
@@ -65217,7 +65205,7 @@
         <v>0.52295080000000005</v>
       </c>
     </row>
-    <row r="279" spans="1:56" hidden="1">
+    <row r="279" spans="1:56">
       <c r="A279">
         <v>51000276</v>
       </c>
@@ -65377,7 +65365,7 @@
         <v>0.10983610000000001</v>
       </c>
     </row>
-    <row r="280" spans="1:56" hidden="1">
+    <row r="280" spans="1:56">
       <c r="A280">
         <v>51000277</v>
       </c>
@@ -65537,7 +65525,7 @@
         <v>0.50655740000000005</v>
       </c>
     </row>
-    <row r="281" spans="1:56" hidden="1">
+    <row r="281" spans="1:56">
       <c r="A281">
         <v>51000278</v>
       </c>
@@ -65697,7 +65685,7 @@
         <v>5.5737700000000001E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:56" hidden="1">
+    <row r="282" spans="1:56">
       <c r="A282">
         <v>51000279</v>
       </c>
@@ -65857,7 +65845,7 @@
         <v>0.14590159999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:56" hidden="1">
+    <row r="283" spans="1:56">
       <c r="A283">
         <v>51000280</v>
       </c>
@@ -66017,7 +66005,7 @@
         <v>0.1245902</v>
       </c>
     </row>
-    <row r="284" spans="1:56" hidden="1">
+    <row r="284" spans="1:56">
       <c r="A284">
         <v>51000281</v>
       </c>
@@ -66183,7 +66171,7 @@
         <v>0.90163930000000003</v>
       </c>
     </row>
-    <row r="285" spans="1:56" hidden="1">
+    <row r="285" spans="1:56">
       <c r="A285">
         <v>51000282</v>
       </c>
@@ -66501,7 +66489,7 @@
         <v>0.2262295</v>
       </c>
     </row>
-    <row r="287" spans="1:56" hidden="1">
+    <row r="287" spans="1:56">
       <c r="A287">
         <v>51000284</v>
       </c>
@@ -66661,7 +66649,7 @@
         <v>0.74754100000000001</v>
       </c>
     </row>
-    <row r="288" spans="1:56" hidden="1">
+    <row r="288" spans="1:56">
       <c r="A288">
         <v>51000285</v>
       </c>
@@ -66821,7 +66809,7 @@
         <v>0.49672129999999998</v>
       </c>
     </row>
-    <row r="289" spans="1:56" hidden="1">
+    <row r="289" spans="1:56">
       <c r="A289">
         <v>51000286</v>
       </c>
@@ -66983,7 +66971,7 @@
         <v>8.6885240000000002E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:56" hidden="1">
+    <row r="290" spans="1:56">
       <c r="A290">
         <v>51000287</v>
       </c>
@@ -67149,7 +67137,7 @@
         <v>0.51967220000000003</v>
       </c>
     </row>
-    <row r="291" spans="1:56" hidden="1">
+    <row r="291" spans="1:56">
       <c r="A291">
         <v>51000288</v>
       </c>
@@ -67313,7 +67301,7 @@
         <v>0.72786890000000004</v>
       </c>
     </row>
-    <row r="292" spans="1:56" hidden="1">
+    <row r="292" spans="1:56">
       <c r="A292">
         <v>51000289</v>
       </c>
@@ -67475,7 +67463,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="293" spans="1:56" hidden="1">
+    <row r="293" spans="1:56">
       <c r="A293">
         <v>51000290</v>
       </c>
@@ -67637,7 +67625,7 @@
         <v>8.1967209999999999E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:56" hidden="1">
+    <row r="294" spans="1:56">
       <c r="A294">
         <v>51000291</v>
       </c>
@@ -67803,7 +67791,7 @@
         <v>0.33442620000000001</v>
       </c>
     </row>
-    <row r="295" spans="1:56" hidden="1">
+    <row r="295" spans="1:56">
       <c r="A295">
         <v>51000292</v>
       </c>
@@ -67963,7 +67951,7 @@
         <v>0.34426230000000002</v>
       </c>
     </row>
-    <row r="296" spans="1:56" hidden="1">
+    <row r="296" spans="1:56">
       <c r="A296">
         <v>51000293</v>
       </c>
@@ -68125,7 +68113,7 @@
         <v>0.1065574</v>
       </c>
     </row>
-    <row r="297" spans="1:56" hidden="1">
+    <row r="297" spans="1:56">
       <c r="A297">
         <v>51000294</v>
       </c>
@@ -68287,7 +68275,7 @@
         <v>0.50983610000000001</v>
       </c>
     </row>
-    <row r="298" spans="1:56" hidden="1">
+    <row r="298" spans="1:56">
       <c r="A298">
         <v>51000295</v>
       </c>
@@ -68449,7 +68437,7 @@
         <v>0.2377049</v>
       </c>
     </row>
-    <row r="299" spans="1:56" hidden="1">
+    <row r="299" spans="1:56">
       <c r="A299">
         <v>51000296</v>
       </c>
@@ -68609,7 +68597,7 @@
         <v>0.80983609999999995</v>
       </c>
     </row>
-    <row r="300" spans="1:56" hidden="1">
+    <row r="300" spans="1:56">
       <c r="A300">
         <v>51000297</v>
       </c>
@@ -68769,7 +68757,7 @@
         <v>0.81967210000000001</v>
       </c>
     </row>
-    <row r="301" spans="1:56" hidden="1">
+    <row r="301" spans="1:56">
       <c r="A301">
         <v>51000298</v>
       </c>
@@ -68938,24 +68926,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H301">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="137" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D301">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -68984,11 +68972,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AX1" sqref="AX1:AX3"/>
+      <selection pane="bottomRight" activeCell="AV8" sqref="AV8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -70610,25 +70598,25 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K9:K10 K4 J5:K6">
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="12" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="21" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="20" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -70646,13 +70634,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="16" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="15" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -70670,13 +70658,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -70694,19 +70682,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some weapon card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -8725,11 +8725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1078600864"/>
-        <c:axId val="1078600320"/>
+        <c:axId val="-1192022976"/>
+        <c:axId val="-1192016448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1078600864"/>
+        <c:axId val="-1192022976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8772,7 +8772,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078600320"/>
+        <c:crossAx val="-1192016448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8780,7 +8780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078600320"/>
+        <c:axId val="-1192016448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8831,7 +8831,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078600864"/>
+        <c:crossAx val="-1192022976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9506,7 +9506,6 @@
     <sheetNames>
       <sheetName val="Skill"/>
       <sheetName val="~标准"/>
-      <sheetName val="道具"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -9611,7 +9610,7 @@
             <v>55100010</v>
           </cell>
           <cell r="X13">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="14">
@@ -10666,7 +10665,6 @@
           <cell r="A145">
             <v>55900028</v>
           </cell>
-          <cell r="X145"/>
         </row>
         <row r="146">
           <cell r="A146">
@@ -10780,9 +10778,16 @@
             <v>15</v>
           </cell>
         </row>
+        <row r="160">
+          <cell r="A160">
+            <v>55990101</v>
+          </cell>
+          <cell r="X160">
+            <v>5</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -20284,7 +20289,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -33319,7 +33324,7 @@
         <v>5</v>
       </c>
       <c r="L82" s="4">
-        <v>-8</v>
+        <v>-15</v>
       </c>
       <c r="M82" s="4">
         <v>0</v>
@@ -33382,7 +33387,7 @@
 IF(ISBLANK($AB82),0, LOOKUP($AB82,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC82/100)+
 IF(ISBLANK($AD82),0, LOOKUP($AD82,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE82/100)+
 IF(ISBLANK($AF82),0, LOOKUP($AF82,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG82/100)</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="AI82" s="20">
         <v>0</v>
@@ -33483,7 +33488,7 @@
         <v>-5</v>
       </c>
       <c r="L83" s="4">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="M83" s="4">
         <v>0</v>
@@ -33542,7 +33547,7 @@
 IF(ISBLANK($AB83),0, LOOKUP($AB83,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC83/100)+
 IF(ISBLANK($AD83),0, LOOKUP($AD83,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE83/100)+
 IF(ISBLANK($AF83),0, LOOKUP($AF83,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG83/100)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AI83" s="20">
         <v>0</v>
@@ -40311,7 +40316,7 @@
         <v>-10</v>
       </c>
       <c r="L125" s="4">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="M125" s="4">
         <v>0</v>
@@ -40374,7 +40379,7 @@
 IF(ISBLANK($AB125),0, LOOKUP($AB125,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC125/100)+
 IF(ISBLANK($AD125),0, LOOKUP($AD125,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE125/100)+
 IF(ISBLANK($AF125),0, LOOKUP($AF125,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG125/100)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AI125" s="20">
         <v>0</v>
@@ -47649,7 +47654,7 @@
         <v>4</v>
       </c>
       <c r="L171" s="4">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="M171" s="4">
         <v>0</v>
@@ -47708,7 +47713,7 @@
 IF(ISBLANK($AB171),0, LOOKUP($AB171,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC171/100)+
 IF(ISBLANK($AD171),0, LOOKUP($AD171,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE171/100)+
 IF(ISBLANK($AF171),0, LOOKUP($AF171,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG171/100)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AI171" s="20">
         <v>0</v>
@@ -51749,7 +51754,7 @@
         <v>-10</v>
       </c>
       <c r="L196" s="4">
-        <v>-4</v>
+        <v>-11</v>
       </c>
       <c r="M196" s="4">
         <v>0</v>
@@ -51774,7 +51779,7 @@
       </c>
       <c r="T196" s="14">
         <f t="shared" ref="T196:T259" si="13">SUM(J196:K196)+SUM(M196:S196)*5+4.4*SUM(AO196:AU196)+2.5*SUM(AI196:AM196)+IF(ISNUMBER(AH196),AH196,0)+L196</f>
-        <v>6.4</v>
+        <v>6.3999999999999986</v>
       </c>
       <c r="U196" s="4">
         <v>10</v>
@@ -51812,7 +51817,7 @@
 IF(ISBLANK($AB196),0, LOOKUP($AB196,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC196/100)+
 IF(ISBLANK($AD196),0, LOOKUP($AD196,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE196/100)+
 IF(ISBLANK($AF196),0, LOOKUP($AF196,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG196/100)</f>
-        <v>10.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="AI196" s="20">
         <v>0</v>
@@ -55803,7 +55808,7 @@
         <v>-8</v>
       </c>
       <c r="L221" s="4">
-        <v>-14</v>
+        <v>-20</v>
       </c>
       <c r="M221" s="4">
         <v>0</v>
@@ -55828,7 +55833,7 @@
       </c>
       <c r="T221" s="14">
         <f t="shared" si="13"/>
-        <v>6.5</v>
+        <v>5.3999999999999986</v>
       </c>
       <c r="U221" s="4">
         <v>10</v>
@@ -55866,7 +55871,7 @@
 IF(ISBLANK($AB221),0, LOOKUP($AB221,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC221/100)+
 IF(ISBLANK($AD221),0, LOOKUP($AD221,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE221/100)+
 IF(ISBLANK($AF221),0, LOOKUP($AF221,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG221/100)</f>
-        <v>8.5</v>
+        <v>13.4</v>
       </c>
       <c r="AI221" s="20">
         <v>0</v>
@@ -59861,7 +59866,7 @@
       </c>
       <c r="H246" s="4">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I246" s="4">
         <v>6</v>
@@ -59898,7 +59903,7 @@
       </c>
       <c r="T246" s="14">
         <f t="shared" si="13"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="U246" s="4">
         <v>10</v>
@@ -59932,7 +59937,7 @@
 IF(ISBLANK($AB246),0, LOOKUP($AB246,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC246/100)+
 IF(ISBLANK($AD246),0, LOOKUP($AD246,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE246/100)+
 IF(ISBLANK($AF246),0, LOOKUP($AF246,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AG246/100)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AI246" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
add some spell card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -8725,11 +8725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1192022976"/>
-        <c:axId val="-1192016448"/>
+        <c:axId val="1925403232"/>
+        <c:axId val="1925396160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1192022976"/>
+        <c:axId val="1925403232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8772,7 +8772,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1192016448"/>
+        <c:crossAx val="1925396160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8780,7 +8780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1192016448"/>
+        <c:axId val="1925396160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8831,7 +8831,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1192022976"/>
+        <c:crossAx val="1925403232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10271,23 +10271,23 @@
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55600001</v>
+            <v>55520004</v>
           </cell>
           <cell r="X96">
-            <v>8</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55600002</v>
+            <v>55600001</v>
           </cell>
           <cell r="X97">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55600003</v>
+            <v>55600002</v>
           </cell>
           <cell r="X98">
             <v>10</v>
@@ -10295,23 +10295,23 @@
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55600004</v>
+            <v>55600003</v>
           </cell>
           <cell r="X99">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55600005</v>
+            <v>55600004</v>
           </cell>
           <cell r="X100">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55600006</v>
+            <v>55600005</v>
           </cell>
           <cell r="X101">
             <v>15</v>
@@ -10319,79 +10319,79 @@
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55600007</v>
+            <v>55600006</v>
           </cell>
           <cell r="X102">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55600008</v>
+            <v>55600007</v>
           </cell>
           <cell r="X103">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55600009</v>
+            <v>55600008</v>
           </cell>
           <cell r="X104">
-            <v>13</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55600010</v>
+            <v>55600009</v>
           </cell>
           <cell r="X105">
-            <v>30</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55600011</v>
+            <v>55600010</v>
           </cell>
           <cell r="X106">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55600012</v>
+            <v>55600011</v>
           </cell>
           <cell r="X107">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55600013</v>
+            <v>55600012</v>
           </cell>
           <cell r="X108">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55610001</v>
+            <v>55600013</v>
           </cell>
           <cell r="X109">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55610002</v>
+            <v>55610001</v>
           </cell>
           <cell r="X110">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55610003</v>
+            <v>55610002</v>
           </cell>
           <cell r="X111">
             <v>5</v>
@@ -10399,23 +10399,23 @@
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55610004</v>
+            <v>55610003</v>
           </cell>
           <cell r="X112">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55700001</v>
+            <v>55610004</v>
           </cell>
           <cell r="X113">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55700002</v>
+            <v>55700001</v>
           </cell>
           <cell r="X114">
             <v>20</v>
@@ -10423,7 +10423,7 @@
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55700003</v>
+            <v>55700002</v>
           </cell>
           <cell r="X115">
             <v>20</v>
@@ -10431,215 +10431,215 @@
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55700004</v>
+            <v>55700003</v>
           </cell>
           <cell r="X116">
-            <v>9</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55700005</v>
+            <v>55700004</v>
           </cell>
           <cell r="X117">
-            <v>40</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55900001</v>
+            <v>55700005</v>
           </cell>
           <cell r="X118">
-            <v>35</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55900002</v>
+            <v>55900001</v>
           </cell>
           <cell r="X119">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55900003</v>
+            <v>55900002</v>
           </cell>
           <cell r="X120">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55900004</v>
+            <v>55900003</v>
           </cell>
           <cell r="X121">
-            <v>-30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55900005</v>
+            <v>55900004</v>
           </cell>
           <cell r="X122">
-            <v>20</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55900006</v>
+            <v>55900005</v>
           </cell>
           <cell r="X123">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55900007</v>
+            <v>55900006</v>
           </cell>
           <cell r="X124">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55900008</v>
+            <v>55900007</v>
           </cell>
           <cell r="X125">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55900009</v>
+            <v>55900008</v>
           </cell>
           <cell r="X126">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55900010</v>
+            <v>55900009</v>
           </cell>
           <cell r="X127">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55900011</v>
+            <v>55900010</v>
           </cell>
           <cell r="X128">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55900012</v>
+            <v>55900011</v>
           </cell>
           <cell r="X129">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55900013</v>
+            <v>55900012</v>
           </cell>
           <cell r="X130">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55900014</v>
+            <v>55900013</v>
           </cell>
           <cell r="X131">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55900015</v>
+            <v>55900014</v>
           </cell>
           <cell r="X132">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900016</v>
+            <v>55900015</v>
           </cell>
           <cell r="X133">
-            <v>45</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900017</v>
+            <v>55900016</v>
           </cell>
           <cell r="X134">
-            <v>10</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900018</v>
+            <v>55900017</v>
           </cell>
           <cell r="X135">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900019</v>
+            <v>55900018</v>
           </cell>
           <cell r="X136">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900020</v>
+            <v>55900019</v>
           </cell>
           <cell r="X137">
-            <v>20</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900021</v>
+            <v>55900020</v>
           </cell>
           <cell r="X138">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900022</v>
+            <v>55900021</v>
           </cell>
           <cell r="X139">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900023</v>
+            <v>55900022</v>
           </cell>
           <cell r="X140">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900024</v>
+            <v>55900023</v>
           </cell>
           <cell r="X141">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900025</v>
+            <v>55900024</v>
           </cell>
           <cell r="X142">
             <v>10</v>
@@ -10647,52 +10647,52 @@
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900026</v>
+            <v>55900025</v>
           </cell>
           <cell r="X143">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900027</v>
+            <v>55900026</v>
           </cell>
           <cell r="X144">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900028</v>
+            <v>55900027</v>
+          </cell>
+          <cell r="X145">
+            <v>35</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900029</v>
-          </cell>
-          <cell r="X146">
-            <v>15</v>
+            <v>55900028</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900030</v>
+            <v>55900029</v>
           </cell>
           <cell r="X147">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55990001</v>
+            <v>55900030</v>
           </cell>
           <cell r="X148">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X149">
             <v>15</v>
@@ -10700,7 +10700,7 @@
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X150">
             <v>15</v>
@@ -10708,7 +10708,7 @@
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X151">
             <v>15</v>
@@ -10716,7 +10716,7 @@
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X152">
             <v>15</v>
@@ -10724,7 +10724,7 @@
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X153">
             <v>15</v>
@@ -10732,7 +10732,7 @@
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X154">
             <v>15</v>
@@ -10740,7 +10740,7 @@
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X155">
             <v>15</v>
@@ -10748,7 +10748,7 @@
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X156">
             <v>15</v>
@@ -10756,7 +10756,7 @@
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X157">
             <v>15</v>
@@ -10764,7 +10764,7 @@
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X158">
             <v>15</v>
@@ -10772,7 +10772,7 @@
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X159">
             <v>15</v>
@@ -10780,14 +10780,46 @@
         </row>
         <row r="160">
           <cell r="A160">
+            <v>55990016</v>
+          </cell>
+          <cell r="X160">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="A161">
             <v>55990101</v>
           </cell>
-          <cell r="X160">
-            <v>5</v>
+          <cell r="X161">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="A162">
+            <v>55990102</v>
+          </cell>
+          <cell r="X162">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="A163">
+            <v>55990103</v>
+          </cell>
+          <cell r="X163">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="A164">
+            <v>55990104</v>
+          </cell>
+          <cell r="X164">
+            <v>50</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19719,7 +19751,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -20285,7 +20317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -68977,11 +69009,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AV8" sqref="AV8"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
close #46 finish initial deck， all basic cards will give to player fro free
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -8737,11 +8737,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1078651840"/>
-        <c:axId val="1078637696"/>
+        <c:axId val="-791279376"/>
+        <c:axId val="-791273936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1078651840"/>
+        <c:axId val="-791279376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8784,7 +8784,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078637696"/>
+        <c:crossAx val="-791273936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8792,7 +8792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078637696"/>
+        <c:axId val="-791273936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8843,7 +8843,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078651840"/>
+        <c:crossAx val="-791279376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20330,11 +20330,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -69022,7 +69022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
fix some attr related show bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -8737,11 +8737,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-791279376"/>
-        <c:axId val="-791273936"/>
+        <c:axId val="833487232"/>
+        <c:axId val="833489408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-791279376"/>
+        <c:axId val="833487232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8784,7 +8784,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-791273936"/>
+        <c:crossAx val="833489408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8792,7 +8792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-791273936"/>
+        <c:axId val="833489408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8843,7 +8843,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-791279376"/>
+        <c:crossAx val="833487232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20334,7 +20334,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
fix the card big demon and angel
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -429,32 +429,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B285" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>real:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-给一个复活技能吧</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -660,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="1122">
   <si>
     <t>arrow</t>
   </si>
@@ -3590,10 +3564,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000289;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>55510009;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4156,9 +4126,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55200010;100|55000288;40</t>
-  </si>
-  <si>
     <t>职业id</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4579,6 +4546,18 @@
   </si>
   <si>
     <t>魔法，治疗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55200010;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900038;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群疗</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8784,11 +8763,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1860187296"/>
-        <c:axId val="-1860188928"/>
+        <c:axId val="2097681904"/>
+        <c:axId val="2097682448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1860187296"/>
+        <c:axId val="2097681904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8831,7 +8810,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1860188928"/>
+        <c:crossAx val="2097682448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8839,7 +8818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1860188928"/>
+        <c:axId val="2097682448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8890,7 +8869,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1860187296"/>
+        <c:crossAx val="2097681904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9260,11 +9239,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1860176960"/>
-        <c:axId val="-1860185120"/>
+        <c:axId val="237683312"/>
+        <c:axId val="237676240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1860176960"/>
+        <c:axId val="237683312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9307,7 +9286,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1860185120"/>
+        <c:crossAx val="237676240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9315,7 +9294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1860185120"/>
+        <c:axId val="237676240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9366,7 +9345,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1860176960"/>
+        <c:crossAx val="237683312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11957,15 +11936,15 @@
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55990001</v>
+            <v>55900038</v>
           </cell>
           <cell r="X168">
-            <v>15</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X169">
             <v>15</v>
@@ -11973,7 +11952,7 @@
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X170">
             <v>15</v>
@@ -11981,7 +11960,7 @@
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X171">
             <v>15</v>
@@ -11989,7 +11968,7 @@
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X172">
             <v>15</v>
@@ -11997,7 +11976,7 @@
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X173">
             <v>15</v>
@@ -12005,7 +11984,7 @@
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X174">
             <v>15</v>
@@ -12013,7 +11992,7 @@
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X175">
             <v>15</v>
@@ -12021,7 +12000,7 @@
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X176">
             <v>15</v>
@@ -12029,7 +12008,7 @@
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X177">
             <v>15</v>
@@ -12037,7 +12016,7 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X178">
             <v>15</v>
@@ -12045,7 +12024,7 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X179">
             <v>15</v>
@@ -12053,38 +12032,46 @@
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X180">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X181">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X182">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
+            <v>55990103</v>
+          </cell>
+          <cell r="X183">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="A184">
             <v>55990104</v>
           </cell>
-          <cell r="X183">
+          <cell r="X184">
             <v>50</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39980,10 +39967,10 @@
   <dimension ref="A1:BB301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B268" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B274" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D273" sqref="D273"/>
+      <selection pane="bottomRight" activeCell="I284" sqref="H284:I284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40159,7 +40146,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -40323,7 +40310,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -40388,7 +40375,7 @@
         <v>714</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>724</v>
@@ -40487,7 +40474,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -41290,7 +41277,7 @@
         <v>325</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
@@ -41355,7 +41342,7 @@
         <v>11</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="Z9" s="37">
         <v>55100011</v>
@@ -41516,7 +41503,7 @@
         <v>12</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Z10" s="37">
         <v>55900008</v>
@@ -42138,7 +42125,7 @@
         <v>6</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="Z14" s="37">
         <v>55110014</v>
@@ -43770,7 +43757,7 @@
         <v>329</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E25" s="4">
         <v>3</v>
@@ -43835,7 +43822,7 @@
         <v>31</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Z25" s="18">
         <v>55600010</v>
@@ -44302,7 +44289,7 @@
         <v>6</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="Z28" s="37">
         <v>55900007</v>
@@ -44459,7 +44446,7 @@
         <v>9</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z29" s="37">
         <v>55100001</v>
@@ -44616,7 +44603,7 @@
         <v>12</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Z30" s="18">
         <v>55500012</v>
@@ -45232,7 +45219,7 @@
         <v>16</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="Z34" s="37">
         <v>55900006</v>
@@ -45479,13 +45466,13 @@
         <v>51000033</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>1033</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>1035</v>
       </c>
       <c r="E36" s="4">
         <v>2</v>
@@ -45547,10 +45534,10 @@
         <v>0</v>
       </c>
       <c r="X36" s="4" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="Z36" s="37">
         <v>55300008</v>
@@ -45644,7 +45631,7 @@
         <v>494</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="E37" s="4">
         <v>2</v>
@@ -45709,7 +45696,7 @@
         <v>38</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="Z37" s="37">
         <v>55610003</v>
@@ -46256,13 +46243,13 @@
         <v>51000038</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="E41" s="4">
         <v>4</v>
@@ -46324,10 +46311,10 @@
         <v>0</v>
       </c>
       <c r="X41" s="4" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="Z41" s="37">
         <v>55100011</v>
@@ -46419,13 +46406,13 @@
         <v>51000039</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>409</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="E42" s="4">
         <v>3</v>
@@ -46490,7 +46477,7 @@
         <v>50</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="Z42" s="18">
         <v>55100011</v>
@@ -46647,7 +46634,7 @@
         <v>4</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="Z43" s="37">
         <v>55900004</v>
@@ -46741,7 +46728,7 @@
         <v>497</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E44" s="4">
         <v>3</v>
@@ -46806,7 +46793,7 @@
         <v>16</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="Z44" s="18">
         <v>55900026</v>
@@ -46963,7 +46950,7 @@
         <v>4</v>
       </c>
       <c r="Y45" s="4" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="Z45" s="37">
         <v>55110013</v>
@@ -47120,7 +47107,7 @@
         <v>2</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z46" s="37">
         <v>55510003</v>
@@ -47438,7 +47425,7 @@
         <v>16</v>
       </c>
       <c r="Y48" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="Z48" s="37">
         <v>55500009</v>
@@ -47597,7 +47584,7 @@
         <v>19</v>
       </c>
       <c r="Y49" s="4" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="Z49" s="37">
         <v>55100015</v>
@@ -47842,7 +47829,7 @@
         <v>335</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E51" s="4">
         <v>3</v>
@@ -47907,7 +47894,7 @@
         <v>9</v>
       </c>
       <c r="Y51" s="4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="Z51" s="37">
         <v>55900017</v>
@@ -48221,7 +48208,7 @@
         <v>16</v>
       </c>
       <c r="Y53" s="4" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="Z53" s="37">
         <v>55110006</v>
@@ -48315,7 +48302,7 @@
         <v>504</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E54" s="4">
         <v>3</v>
@@ -48380,7 +48367,7 @@
         <v>61</v>
       </c>
       <c r="Y54" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Z54" s="37">
         <v>55100011</v>
@@ -48700,7 +48687,7 @@
         <v>4</v>
       </c>
       <c r="Y56" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="Z56" s="37">
         <v>55510003</v>
@@ -49269,7 +49256,7 @@
         <v>507</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E60" s="4">
         <v>3</v>
@@ -49334,7 +49321,7 @@
         <v>9</v>
       </c>
       <c r="Y60" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="Z60" s="37">
         <v>55900018</v>
@@ -49491,7 +49478,7 @@
         <v>24</v>
       </c>
       <c r="Y61" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="Z61" s="37">
         <v>55510007</v>
@@ -49648,7 +49635,7 @@
         <v>62</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="Z62" s="37">
         <v>55510002</v>
@@ -49805,7 +49792,7 @@
         <v>38</v>
       </c>
       <c r="Y63" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="Z63" s="37">
         <v>55510009</v>
@@ -49962,7 +49949,7 @@
         <v>24</v>
       </c>
       <c r="Y64" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="Z64" s="37">
         <v>55110010</v>
@@ -50368,7 +50355,7 @@
         <v>340</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="E67" s="4">
         <v>6</v>
@@ -50433,7 +50420,7 @@
         <v>75</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="Z67" s="37">
         <v>55510010</v>
@@ -50527,7 +50514,7 @@
         <v>512</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E68" s="4">
         <v>7</v>
@@ -50592,7 +50579,7 @@
         <v>75</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="Z68" s="37">
         <v>55300010</v>
@@ -50688,7 +50675,7 @@
         <v>341</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E69" s="4">
         <v>6</v>
@@ -50753,7 +50740,7 @@
         <v>40</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Z69" s="18">
         <v>55200008</v>
@@ -51373,7 +51360,7 @@
         <v>728</v>
       </c>
       <c r="Y73" s="4" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="Z73" s="37">
         <v>55510007</v>
@@ -51530,7 +51517,7 @@
         <v>6</v>
       </c>
       <c r="Y74" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Z74" s="37">
         <v>55500012</v>
@@ -51624,7 +51611,7 @@
         <v>342</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E75" s="4">
         <v>2</v>
@@ -51689,7 +51676,7 @@
         <v>86</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="Z75" s="37">
         <v>55500008</v>
@@ -51787,7 +51774,7 @@
         <v>518</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E76" s="4">
         <v>4</v>
@@ -51852,7 +51839,7 @@
         <v>12</v>
       </c>
       <c r="Y76" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="Z76" s="37">
         <v>55100001</v>
@@ -52013,7 +52000,7 @@
         <v>89</v>
       </c>
       <c r="Y77" s="4" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="Z77" s="37">
         <v>55110007</v>
@@ -52576,7 +52563,7 @@
         <v>344</v>
       </c>
       <c r="D81" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E81" s="4">
         <v>3</v>
@@ -52641,7 +52628,7 @@
         <v>2</v>
       </c>
       <c r="Y81" s="4" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="Z81" s="37">
         <v>55600014</v>
@@ -52798,7 +52785,7 @@
         <v>2</v>
       </c>
       <c r="Y82" s="4" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="Z82" s="37">
         <v>55100010</v>
@@ -52959,7 +52946,7 @@
         <v>38</v>
       </c>
       <c r="Y83" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Z83" s="37">
         <v>55100010</v>
@@ -53530,7 +53517,7 @@
         <v>523</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="E87" s="4">
         <v>3</v>
@@ -53595,7 +53582,7 @@
         <v>83</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="Z87" s="37">
         <v>55100011</v>
@@ -53756,7 +53743,7 @@
         <v>0</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="Z88" s="37">
         <v>55200003</v>
@@ -54070,7 +54057,7 @@
         <v>103</v>
       </c>
       <c r="Y90" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="Z90" s="37">
         <v>55100002</v>
@@ -54168,7 +54155,7 @@
         <v>524</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E91" s="4">
         <v>3</v>
@@ -54233,7 +54220,7 @@
         <v>101</v>
       </c>
       <c r="Y91" s="4" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Z91" s="37">
         <v>55600009</v>
@@ -54700,7 +54687,7 @@
         <v>75</v>
       </c>
       <c r="Y94" s="4" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="Z94" s="37">
         <v>55500008</v>
@@ -55012,7 +54999,7 @@
         <v>2</v>
       </c>
       <c r="Y96" s="4" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="Z96" s="37">
         <v>55500008</v>
@@ -55175,7 +55162,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="Z97" s="37">
         <v>55110007</v>
@@ -55340,7 +55327,7 @@
         <v>91</v>
       </c>
       <c r="Y98" s="4" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="Z98" s="37">
         <v>55510002</v>
@@ -55497,7 +55484,7 @@
         <v>727</v>
       </c>
       <c r="Y99" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z99" s="37">
         <v>55510010</v>
@@ -55654,7 +55641,7 @@
         <v>4</v>
       </c>
       <c r="Y100" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="Z100" s="37">
         <v>55900016</v>
@@ -55962,7 +55949,7 @@
         <v>16</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="Z102" s="37">
         <v>55900003</v>
@@ -56219,7 +56206,7 @@
         <v>350</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="E104" s="4">
         <v>3</v>
@@ -56284,7 +56271,7 @@
         <v>4</v>
       </c>
       <c r="Y104" s="4" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="Z104" s="37">
         <v>55100015</v>
@@ -56382,7 +56369,7 @@
         <v>536</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E105" s="4">
         <v>2</v>
@@ -56447,7 +56434,7 @@
         <v>103</v>
       </c>
       <c r="Y105" s="4" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="Z105" s="37">
         <v>55900035</v>
@@ -56541,7 +56528,7 @@
         <v>537</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="E106" s="4">
         <v>2</v>
@@ -56606,7 +56593,7 @@
         <v>9</v>
       </c>
       <c r="Y106" s="4" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="Z106" s="37">
         <v>55300009</v>
@@ -56922,7 +56909,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="Z108" s="37">
         <v>55900027</v>
@@ -57230,7 +57217,7 @@
         <v>126</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="Z110" s="37">
         <v>55510009</v>
@@ -57842,7 +57829,7 @@
         <v>86</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Z114" s="37"/>
       <c r="AA114" s="18"/>
@@ -58007,7 +57994,7 @@
         <v>91</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="Z115" s="37"/>
       <c r="AA115" s="18"/>
@@ -58172,7 +58159,7 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="Z116" s="37"/>
       <c r="AA116" s="18"/>
@@ -58337,7 +58324,7 @@
         <v>75</v>
       </c>
       <c r="Y117" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Z117" s="37"/>
       <c r="AA117" s="18"/>
@@ -58602,7 +58589,7 @@
         <v>672</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E119" s="8">
         <v>2</v>
@@ -58667,7 +58654,7 @@
         <v>6</v>
       </c>
       <c r="Y119" s="8" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="Z119" s="37">
         <v>55100014</v>
@@ -58826,7 +58813,7 @@
         <v>49</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="Z120" s="37"/>
       <c r="AA120" s="18"/>
@@ -58991,7 +58978,7 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="Z121" s="37"/>
       <c r="AA121" s="18"/>
@@ -59305,7 +59292,7 @@
         <v>4</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="Z123" s="37">
         <v>55100005</v>
@@ -59621,7 +59608,7 @@
         <v>2</v>
       </c>
       <c r="Y125" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="Z125" s="37">
         <v>55100010</v>
@@ -59719,7 +59706,7 @@
         <v>355</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E126" s="4">
         <v>1</v>
@@ -59784,7 +59771,7 @@
         <v>24</v>
       </c>
       <c r="Y126" s="4" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="Z126" s="37">
         <v>55600012</v>
@@ -59941,7 +59928,7 @@
         <v>4</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Z127" s="37">
         <v>55110005</v>
@@ -60035,7 +60022,7 @@
         <v>550</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E128" s="4">
         <v>2</v>
@@ -60100,7 +60087,7 @@
         <v>4</v>
       </c>
       <c r="Y128" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="Z128" s="37">
         <v>55900019</v>
@@ -60345,7 +60332,7 @@
         <v>552</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E130" s="4">
         <v>1</v>
@@ -60410,7 +60397,7 @@
         <v>103</v>
       </c>
       <c r="Y130" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="Z130" s="37">
         <v>55900024</v>
@@ -60718,7 +60705,7 @@
         <v>4</v>
       </c>
       <c r="Y132" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="Z132" s="37">
         <v>55100007</v>
@@ -60875,7 +60862,7 @@
         <v>103</v>
       </c>
       <c r="Y133" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="Z133" s="37">
         <v>55900027</v>
@@ -61036,7 +61023,7 @@
         <v>2</v>
       </c>
       <c r="Y134" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="Z134" s="37">
         <v>55900008</v>
@@ -61197,7 +61184,7 @@
         <v>75</v>
       </c>
       <c r="Y135" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="Z135" s="37">
         <v>55900016</v>
@@ -61354,7 +61341,7 @@
         <v>103</v>
       </c>
       <c r="Y136" s="4" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="Z136" s="37">
         <v>55110005</v>
@@ -61511,7 +61498,7 @@
         <v>2</v>
       </c>
       <c r="Y137" s="4" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="Z137" s="37">
         <v>55510010</v>
@@ -61672,7 +61659,7 @@
         <v>6</v>
       </c>
       <c r="Y138" s="4" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="Z138" s="37">
         <v>55100006</v>
@@ -62441,7 +62428,7 @@
         <v>4</v>
       </c>
       <c r="Y143" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="Z143" s="18">
         <v>55110015</v>
@@ -62598,7 +62585,7 @@
         <v>16</v>
       </c>
       <c r="Y144" s="4" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="Z144" s="37">
         <v>55510004</v>
@@ -62908,7 +62895,7 @@
         <v>103</v>
       </c>
       <c r="Y146" s="4" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="Z146" s="37">
         <v>55110007</v>
@@ -63006,7 +62993,7 @@
         <v>360</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="E147" s="4">
         <v>3</v>
@@ -63071,7 +63058,7 @@
         <v>19</v>
       </c>
       <c r="Y147" s="4" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="Z147" s="18">
         <v>55510006</v>
@@ -63165,7 +63152,7 @@
         <v>470</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E148" s="4">
         <v>2</v>
@@ -63230,7 +63217,7 @@
         <v>731</v>
       </c>
       <c r="Y148" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="Z148" s="37">
         <v>55100012</v>
@@ -63328,7 +63315,7 @@
         <v>361</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="E149" s="4">
         <v>3</v>
@@ -63393,7 +63380,7 @@
         <v>162</v>
       </c>
       <c r="Y149" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="Z149" s="37">
         <v>55100011</v>
@@ -63554,7 +63541,7 @@
         <v>4</v>
       </c>
       <c r="Y150" s="4" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z150" s="37">
         <v>55500005</v>
@@ -64260,7 +64247,7 @@
         <v>568</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="E155" s="4">
         <v>3</v>
@@ -64325,7 +64312,7 @@
         <v>735</v>
       </c>
       <c r="Y155" s="4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="Z155" s="37">
         <v>55100013</v>
@@ -64482,7 +64469,7 @@
         <v>4</v>
       </c>
       <c r="Y156" s="4" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="Z156" s="37">
         <v>55110004</v>
@@ -65400,7 +65387,7 @@
         <v>103</v>
       </c>
       <c r="Y162" s="4" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="Z162" s="37">
         <v>55110010</v>
@@ -65494,7 +65481,7 @@
         <v>575</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E163" s="4">
         <v>3</v>
@@ -65559,7 +65546,7 @@
         <v>103</v>
       </c>
       <c r="Y163" s="4" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Z163" s="37">
         <v>55900010</v>
@@ -65716,7 +65703,7 @@
         <v>16</v>
       </c>
       <c r="Y164" s="4" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="Z164" s="37">
         <v>55110005</v>
@@ -66895,7 +66882,7 @@
         <v>579</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E172" s="4">
         <v>4</v>
@@ -66960,7 +66947,7 @@
         <v>4</v>
       </c>
       <c r="Y172" s="4" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="Z172" s="37">
         <v>55510018</v>
@@ -67058,7 +67045,7 @@
         <v>580</v>
       </c>
       <c r="D173" s="19" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E173" s="4">
         <v>2</v>
@@ -67123,7 +67110,7 @@
         <v>729</v>
       </c>
       <c r="Y173" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z173" s="37">
         <v>55200004</v>
@@ -67376,7 +67363,7 @@
         <v>582</v>
       </c>
       <c r="D175" s="19" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E175" s="4">
         <v>2</v>
@@ -67441,7 +67428,7 @@
         <v>2</v>
       </c>
       <c r="Y175" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Z175" s="37">
         <v>55700003</v>
@@ -67602,7 +67589,7 @@
         <v>12</v>
       </c>
       <c r="Y176" s="4" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="Z176" s="37">
         <v>55610003</v>
@@ -67855,7 +67842,7 @@
         <v>584</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E178" s="4">
         <v>4</v>
@@ -67920,7 +67907,7 @@
         <v>4</v>
       </c>
       <c r="Y178" s="4" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="Z178" s="37">
         <v>55510004</v>
@@ -68077,7 +68064,7 @@
         <v>2</v>
       </c>
       <c r="Y179" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="Z179" s="37">
         <v>55110005</v>
@@ -68234,7 +68221,7 @@
         <v>62</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="Z180" s="18">
         <v>55900023</v>
@@ -68332,7 +68319,7 @@
         <v>586</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E181" s="4">
         <v>5</v>
@@ -68397,7 +68384,7 @@
         <v>654</v>
       </c>
       <c r="Y181" s="4" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="Z181" s="37">
         <v>55200012</v>
@@ -68558,7 +68545,7 @@
         <v>4</v>
       </c>
       <c r="Y182" s="4" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="Z182" s="37">
         <v>55610003</v>
@@ -68715,7 +68702,7 @@
         <v>16</v>
       </c>
       <c r="Y183" s="4" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="Z183" s="37">
         <v>55900031</v>
@@ -68813,7 +68800,7 @@
         <v>589</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="E184" s="4">
         <v>3</v>
@@ -68878,7 +68865,7 @@
         <v>75</v>
       </c>
       <c r="Y184" s="4" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="Z184" s="37">
         <v>55510010</v>
@@ -68972,7 +68959,7 @@
         <v>367</v>
       </c>
       <c r="D185" s="19" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E185" s="4">
         <v>6</v>
@@ -69037,7 +69024,7 @@
         <v>12</v>
       </c>
       <c r="Y185" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="Z185" s="37">
         <v>55600011</v>
@@ -69135,7 +69122,7 @@
         <v>590</v>
       </c>
       <c r="D186" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E186" s="4">
         <v>4</v>
@@ -69200,7 +69187,7 @@
         <v>75</v>
       </c>
       <c r="Y186" s="4" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="Z186" s="37">
         <v>55600016</v>
@@ -69665,7 +69652,7 @@
         <v>4</v>
       </c>
       <c r="Y189" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="Z189" s="37">
         <v>55510012</v>
@@ -69975,7 +69962,7 @@
         <v>24</v>
       </c>
       <c r="Y191" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="Z191" s="37">
         <v>55900004</v>
@@ -70136,7 +70123,7 @@
         <v>730</v>
       </c>
       <c r="Y192" s="4" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="Z192" s="37">
         <v>55110001</v>
@@ -70234,7 +70221,7 @@
         <v>596</v>
       </c>
       <c r="D193" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E193" s="4">
         <v>5</v>
@@ -70299,7 +70286,7 @@
         <v>2</v>
       </c>
       <c r="Y193" s="4" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="Z193" s="37">
         <v>55100011</v>
@@ -70397,7 +70384,7 @@
         <v>597</v>
       </c>
       <c r="D194" s="19" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E194" s="4">
         <v>5</v>
@@ -70462,7 +70449,7 @@
         <v>16</v>
       </c>
       <c r="Y194" s="4" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Z194" s="37">
         <v>55900014</v>
@@ -70560,7 +70547,7 @@
         <v>598</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E195" s="4">
         <v>5</v>
@@ -70625,7 +70612,7 @@
         <v>204</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="Z195" s="18">
         <v>55100011</v>
@@ -70723,7 +70710,7 @@
         <v>599</v>
       </c>
       <c r="D196" s="19" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E196" s="4">
         <v>5</v>
@@ -70788,7 +70775,7 @@
         <v>4</v>
       </c>
       <c r="Y196" s="4" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="Z196" s="18">
         <v>55520003</v>
@@ -70886,7 +70873,7 @@
         <v>600</v>
       </c>
       <c r="D197" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E197" s="4">
         <v>5</v>
@@ -70951,7 +70938,7 @@
         <v>4</v>
       </c>
       <c r="Y197" s="4" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="Z197" s="18">
         <v>55600008</v>
@@ -71112,7 +71099,7 @@
         <v>22</v>
       </c>
       <c r="Y198" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="Z198" s="37">
         <v>55100004</v>
@@ -71210,7 +71197,7 @@
         <v>602</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E199" s="4">
         <v>5</v>
@@ -71275,7 +71262,7 @@
         <v>2</v>
       </c>
       <c r="Y199" s="4" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="Z199" s="37">
         <v>55100010</v>
@@ -71436,7 +71423,7 @@
         <v>4</v>
       </c>
       <c r="Y200" s="4" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="Z200" s="37">
         <v>55110008</v>
@@ -71909,7 +71896,7 @@
         <v>16</v>
       </c>
       <c r="Y203" s="4" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="Z203" s="37">
         <v>55110011</v>
@@ -72003,7 +71990,7 @@
         <v>673</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E204" s="8">
         <v>3</v>
@@ -72068,7 +72055,7 @@
         <v>6</v>
       </c>
       <c r="Y204" s="8" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="Z204" s="37">
         <v>55100014</v>
@@ -72162,7 +72149,7 @@
         <v>604</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E205" s="4">
         <v>2</v>
@@ -72227,7 +72214,7 @@
         <v>734</v>
       </c>
       <c r="Y205" s="4" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="Z205" s="37">
         <v>55510013</v>
@@ -72545,7 +72532,7 @@
         <v>168</v>
       </c>
       <c r="Y207" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z207" s="37">
         <v>55900029</v>
@@ -72861,7 +72848,7 @@
         <v>2</v>
       </c>
       <c r="Y209" s="4" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="Z209" s="37">
         <v>55510003</v>
@@ -73328,7 +73315,7 @@
         <v>128</v>
       </c>
       <c r="Y212" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Z212" s="18">
         <v>55510013</v>
@@ -73422,7 +73409,7 @@
         <v>609</v>
       </c>
       <c r="D213" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E213" s="4">
         <v>4</v>
@@ -73487,7 +73474,7 @@
         <v>812</v>
       </c>
       <c r="Y213" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="Z213" s="18">
         <v>55900005</v>
@@ -73736,7 +73723,7 @@
         <v>611</v>
       </c>
       <c r="D215" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E215" s="4">
         <v>4</v>
@@ -73801,7 +73788,7 @@
         <v>185</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="Z215" s="37">
         <v>55100001</v>
@@ -73962,7 +73949,7 @@
         <v>6</v>
       </c>
       <c r="Y216" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="Z216" s="37">
         <v>55900031</v>
@@ -74215,7 +74202,7 @@
         <v>613</v>
       </c>
       <c r="D218" s="19" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E218" s="4">
         <v>2</v>
@@ -74280,7 +74267,7 @@
         <v>4</v>
       </c>
       <c r="Y218" s="4" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="Z218" s="37">
         <v>55900034</v>
@@ -74374,7 +74361,7 @@
         <v>614</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E219" s="4">
         <v>3</v>
@@ -74439,7 +74426,7 @@
         <v>733</v>
       </c>
       <c r="Y219" s="4" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="Z219" s="37">
         <v>55510019</v>
@@ -74596,7 +74583,7 @@
         <v>62</v>
       </c>
       <c r="Y220" s="4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="Z220" s="37">
         <v>55100001</v>
@@ -74690,7 +74677,7 @@
         <v>615</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E221" s="4">
         <v>4</v>
@@ -74755,7 +74742,7 @@
         <v>231</v>
       </c>
       <c r="Y221" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Z221" s="37">
         <v>55200009</v>
@@ -74916,7 +74903,7 @@
         <v>6</v>
       </c>
       <c r="Y222" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="Z222" s="37">
         <v>55900005</v>
@@ -75073,7 +75060,7 @@
         <v>9</v>
       </c>
       <c r="Y223" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Z223" s="37">
         <v>55100008</v>
@@ -75230,7 +75217,7 @@
         <v>103</v>
       </c>
       <c r="Y224" s="7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="Z224" s="37">
         <v>55900016</v>
@@ -75391,7 +75378,7 @@
         <v>16</v>
       </c>
       <c r="Y225" s="4" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="Z225" s="37">
         <v>55610002</v>
@@ -75711,7 +75698,7 @@
         <v>168</v>
       </c>
       <c r="Y227" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="Z227" s="37">
         <v>55110012</v>
@@ -75805,7 +75792,7 @@
         <v>429</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E228" s="4">
         <v>3</v>
@@ -75870,7 +75857,7 @@
         <v>239</v>
       </c>
       <c r="Y228" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="Z228" s="37">
         <v>55510001</v>
@@ -75964,7 +75951,7 @@
         <v>375</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E229" s="4">
         <v>2</v>
@@ -76029,7 +76016,7 @@
         <v>24</v>
       </c>
       <c r="Y229" s="4" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="Z229" s="37">
         <v>55510007</v>
@@ -76594,7 +76581,7 @@
         <v>376</v>
       </c>
       <c r="D233" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E233" s="4">
         <v>3</v>
@@ -76659,7 +76646,7 @@
         <v>245</v>
       </c>
       <c r="Y233" s="4" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="Z233" s="37">
         <v>55100009</v>
@@ -76820,7 +76807,7 @@
         <v>22</v>
       </c>
       <c r="Y234" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Z234" s="37">
         <v>55110009</v>
@@ -76914,7 +76901,7 @@
         <v>623</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E235" s="4">
         <v>3</v>
@@ -76979,7 +76966,7 @@
         <v>6</v>
       </c>
       <c r="Y235" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="Z235" s="18">
         <v>55600013</v>
@@ -77073,7 +77060,7 @@
         <v>624</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E236" s="4">
         <v>2</v>
@@ -77138,7 +77125,7 @@
         <v>12</v>
       </c>
       <c r="Y236" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="Z236" s="37">
         <v>55600013</v>
@@ -77295,7 +77282,7 @@
         <v>2</v>
       </c>
       <c r="Y237" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="Z237" s="37">
         <v>55100001</v>
@@ -77607,7 +77594,7 @@
         <v>4</v>
       </c>
       <c r="Y239" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="Z239" s="37">
         <v>55110001</v>
@@ -77856,7 +77843,7 @@
         <v>435</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E241" s="4">
         <v>5</v>
@@ -77921,7 +77908,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="Z241" s="37">
         <v>55100010</v>
@@ -78237,7 +78224,7 @@
         <v>66</v>
       </c>
       <c r="Y243" s="4" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="Z243" s="37">
         <v>55900033</v>
@@ -78331,7 +78318,7 @@
         <v>378</v>
       </c>
       <c r="D244" s="19" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E244" s="4">
         <v>3</v>
@@ -78396,7 +78383,7 @@
         <v>2</v>
       </c>
       <c r="Y244" s="4" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="Z244" s="37">
         <v>55510014</v>
@@ -78490,7 +78477,7 @@
         <v>379</v>
       </c>
       <c r="D245" s="19" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E245" s="4">
         <v>6</v>
@@ -78555,7 +78542,7 @@
         <v>66</v>
       </c>
       <c r="Y245" s="4" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="Z245" s="37">
         <v>55510014</v>
@@ -78867,7 +78854,7 @@
         <v>2</v>
       </c>
       <c r="Y247" s="4" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="Z247" s="37">
         <v>55510010</v>
@@ -79028,7 +79015,7 @@
         <v>19</v>
       </c>
       <c r="Y248" s="4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="Z248" s="37">
         <v>55900025</v>
@@ -79336,7 +79323,7 @@
         <v>2</v>
       </c>
       <c r="Y250" s="4" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="Z250" s="37">
         <v>55510009</v>
@@ -79497,7 +79484,7 @@
         <v>4</v>
       </c>
       <c r="Y251" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="Z251" s="18">
         <v>55900030</v>
@@ -79654,7 +79641,7 @@
         <v>131</v>
       </c>
       <c r="Y252" s="4" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="Z252" s="18">
         <v>55110007</v>
@@ -79811,7 +79798,7 @@
         <v>19</v>
       </c>
       <c r="Y253" s="4" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="Z253" s="37">
         <v>55900015</v>
@@ -79905,7 +79892,7 @@
         <v>380</v>
       </c>
       <c r="D254" s="19" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E254" s="4">
         <v>3</v>
@@ -79970,7 +79957,7 @@
         <v>204</v>
       </c>
       <c r="Y254" s="4" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Z254" s="18">
         <v>55100013</v>
@@ -80064,7 +80051,7 @@
         <v>381</v>
       </c>
       <c r="D255" s="19" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="E255" s="4">
         <v>4</v>
@@ -80129,7 +80116,7 @@
         <v>0</v>
       </c>
       <c r="Y255" s="4" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="Z255" s="37">
         <v>55510018</v>
@@ -80290,7 +80277,7 @@
         <v>4</v>
       </c>
       <c r="Y256" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="Z256" s="37">
         <v>55110005</v>
@@ -80384,7 +80371,7 @@
         <v>630</v>
       </c>
       <c r="D257" s="19" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E257" s="4">
         <v>3</v>
@@ -80449,7 +80436,7 @@
         <v>2</v>
       </c>
       <c r="Y257" s="4" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="Z257" s="37">
         <v>55200013</v>
@@ -80540,7 +80527,7 @@
         <v>259</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D258" s="19"/>
       <c r="E258" s="4">
@@ -80606,7 +80593,7 @@
         <v>245</v>
       </c>
       <c r="Y258" s="4" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="Z258" s="37">
         <v>55410001</v>
@@ -80704,7 +80691,7 @@
         <v>631</v>
       </c>
       <c r="D259" s="19" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E259" s="4">
         <v>2</v>
@@ -80769,7 +80756,7 @@
         <v>4</v>
       </c>
       <c r="Y259" s="7" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="Z259" s="37">
         <v>55100012</v>
@@ -80867,7 +80854,7 @@
         <v>383</v>
       </c>
       <c r="D260" s="19" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="E260" s="4">
         <v>3</v>
@@ -80916,7 +80903,7 @@
         <v>0</v>
       </c>
       <c r="T260" s="12">
-        <f t="shared" ref="T260:T323" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AM260:AS260)+2.5*SUM(AG260:AK260)+IF(ISNUMBER(AF260),AF260,0)+L260</f>
+        <f t="shared" ref="T260:T301" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AM260:AS260)+2.5*SUM(AG260:AK260)+IF(ISNUMBER(AF260),AF260,0)+L260</f>
         <v>7</v>
       </c>
       <c r="U260" s="4">
@@ -80932,7 +80919,7 @@
         <v>6</v>
       </c>
       <c r="Y260" s="4" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="Z260" s="37">
         <v>55900010</v>
@@ -81030,7 +81017,7 @@
         <v>384</v>
       </c>
       <c r="D261" s="19" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E261" s="4">
         <v>3</v>
@@ -81095,7 +81082,7 @@
         <v>16</v>
       </c>
       <c r="Y261" s="4" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Z261" s="37">
         <v>55900014</v>
@@ -81562,7 +81549,7 @@
         <v>4</v>
       </c>
       <c r="Y264" s="4" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Z264" s="37">
         <v>55100005</v>
@@ -81719,7 +81706,7 @@
         <v>2</v>
       </c>
       <c r="Y265" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Z265" s="37">
         <v>55110007</v>
@@ -81876,7 +81863,7 @@
         <v>24</v>
       </c>
       <c r="Y266" s="4" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="Z266" s="37">
         <v>55900031</v>
@@ -81970,7 +81957,7 @@
         <v>388</v>
       </c>
       <c r="D267" s="19" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="E267" s="4">
         <v>5</v>
@@ -82035,7 +82022,7 @@
         <v>91</v>
       </c>
       <c r="Y267" s="4" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="Z267" s="37">
         <v>55510001</v>
@@ -82196,7 +82183,7 @@
         <v>16</v>
       </c>
       <c r="Y268" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="Z268" s="37">
         <v>55900031</v>
@@ -82510,7 +82497,7 @@
         <v>16</v>
       </c>
       <c r="Y270" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Z270" s="37">
         <v>55100008</v>
@@ -82604,7 +82591,7 @@
         <v>390</v>
       </c>
       <c r="D271" s="19" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E271" s="4">
         <v>5</v>
@@ -82669,7 +82656,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="Z271" s="18">
         <v>55100012</v>
@@ -82767,7 +82754,7 @@
         <v>632</v>
       </c>
       <c r="D272" s="19" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="E272" s="4">
         <v>5</v>
@@ -82832,7 +82819,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="Z272" s="18">
         <v>55100012</v>
@@ -82930,7 +82917,7 @@
         <v>391</v>
       </c>
       <c r="D273" s="19" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="E273" s="4">
         <v>5</v>
@@ -82995,7 +82982,7 @@
         <v>736</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="Z273" s="18">
         <v>55100012</v>
@@ -83156,7 +83143,7 @@
         <v>0</v>
       </c>
       <c r="Y274" s="4" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Z274" s="37">
         <v>55200003</v>
@@ -83315,7 +83302,7 @@
         <v>271</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="Z275" s="37">
         <v>55700005</v>
@@ -83560,7 +83547,7 @@
         <v>460</v>
       </c>
       <c r="D277" s="19" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E277" s="4">
         <v>3</v>
@@ -83625,7 +83612,7 @@
         <v>75</v>
       </c>
       <c r="Y277" s="4" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="Z277" s="18">
         <v>55310003</v>
@@ -83782,7 +83769,7 @@
         <v>4</v>
       </c>
       <c r="Y278" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="Z278" s="18">
         <v>55110016</v>
@@ -83943,7 +83930,7 @@
         <v>4</v>
       </c>
       <c r="Y279" s="7" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="Z279" s="37">
         <v>55900022</v>
@@ -84100,7 +84087,7 @@
         <v>16</v>
       </c>
       <c r="Y280" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="Z280" s="37">
         <v>55110019</v>
@@ -84194,7 +84181,7 @@
         <v>393</v>
       </c>
       <c r="D281" s="19" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E281" s="4">
         <v>1</v>
@@ -84259,7 +84246,7 @@
         <v>9</v>
       </c>
       <c r="Y281" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z281" s="37">
         <v>55900009</v>
@@ -84353,7 +84340,7 @@
         <v>394</v>
       </c>
       <c r="D282" s="19" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E282" s="4">
         <v>1</v>
@@ -84418,7 +84405,7 @@
         <v>6</v>
       </c>
       <c r="Y282" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z282" s="37">
         <v>55900009</v>
@@ -84512,7 +84499,7 @@
         <v>395</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E283" s="4">
         <v>1</v>
@@ -84577,7 +84564,7 @@
         <v>16</v>
       </c>
       <c r="Y283" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z283" s="37">
         <v>55900009</v>
@@ -84671,7 +84658,7 @@
         <v>633</v>
       </c>
       <c r="D284" s="19" t="s">
-        <v>737</v>
+        <v>809</v>
       </c>
       <c r="E284" s="4">
         <v>6</v>
@@ -84684,19 +84671,19 @@
       </c>
       <c r="H284" s="4">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I284" s="4">
         <v>6</v>
       </c>
       <c r="J284" s="4">
-        <v>30</v>
+        <v>-15</v>
       </c>
       <c r="K284" s="4">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="L284" s="4">
-        <v>0</v>
+        <v>-18</v>
       </c>
       <c r="M284" s="4">
         <v>0</v>
@@ -84714,14 +84701,14 @@
         <v>0</v>
       </c>
       <c r="R284" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S284" s="4">
         <v>0</v>
       </c>
       <c r="T284" s="12">
         <f t="shared" si="17"/>
-        <v>21.32</v>
+        <v>9.07</v>
       </c>
       <c r="U284" s="4">
         <v>10</v>
@@ -84736,7 +84723,7 @@
         <v>6</v>
       </c>
       <c r="Y284" s="4" t="s">
-        <v>1013</v>
+        <v>1119</v>
       </c>
       <c r="Z284" s="37">
         <v>55200010</v>
@@ -84744,22 +84731,18 @@
       <c r="AA284" s="18">
         <v>100</v>
       </c>
-      <c r="AB284" s="18">
-        <v>55000288</v>
-      </c>
-      <c r="AC284" s="18">
-        <v>40</v>
-      </c>
+      <c r="AB284" s="18"/>
+      <c r="AC284" s="18"/>
       <c r="AD284" s="18"/>
       <c r="AE284" s="18"/>
-      <c r="AF284" s="18" t="e">
+      <c r="AF284" s="18">
         <f>IF(ISBLANK($Z284),0, LOOKUP($Z284,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA284/100)+
 IF(ISBLANK($AB284),0, LOOKUP($AB284,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC284/100)+
 IF(ISBLANK($AD284),0, LOOKUP($AD284,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE284/100)</f>
-        <v>#N/A</v>
+        <v>25</v>
       </c>
       <c r="AG284" s="18">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AH284" s="18">
         <v>0</v>
@@ -84775,7 +84758,7 @@
       </c>
       <c r="AL284" s="4" t="str">
         <f t="shared" si="18"/>
-        <v>0;0;0;0;0</v>
+        <v>0.3;0;0;0;0</v>
       </c>
       <c r="AM284" s="18">
         <v>0</v>
@@ -84787,20 +84770,20 @@
         <v>0</v>
       </c>
       <c r="AP284" s="18">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AQ284" s="18">
         <v>0</v>
       </c>
       <c r="AR284" s="18">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AS284" s="18">
         <v>0</v>
       </c>
       <c r="AT284" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>0;0;0;0;0;0.3;0</v>
+        <v>0;0;0;0.3;0;0;0</v>
       </c>
       <c r="AU284" s="50" t="s">
         <v>797</v>
@@ -84834,7 +84817,7 @@
         <v>636</v>
       </c>
       <c r="D285" s="19" t="s">
-        <v>737</v>
+        <v>1121</v>
       </c>
       <c r="E285" s="4">
         <v>6</v>
@@ -84847,22 +84830,22 @@
       </c>
       <c r="H285" s="4">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I285" s="4">
         <v>6</v>
       </c>
       <c r="J285" s="4">
-        <v>17</v>
+        <v>-15</v>
       </c>
       <c r="K285" s="4">
-        <v>9</v>
+        <v>-5</v>
       </c>
       <c r="L285" s="4">
-        <v>0</v>
+        <v>-17</v>
       </c>
       <c r="M285" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N285" s="4">
         <v>0</v>
@@ -84877,14 +84860,14 @@
         <v>0</v>
       </c>
       <c r="R285" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S285" s="4">
         <v>0</v>
       </c>
       <c r="T285" s="12">
         <f t="shared" si="17"/>
-        <v>42.32</v>
+        <v>9.32</v>
       </c>
       <c r="U285" s="4">
         <v>10</v>
@@ -84899,10 +84882,10 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>868</v>
+        <v>1120</v>
       </c>
       <c r="Z285" s="37">
-        <v>55000289</v>
+        <v>55900038</v>
       </c>
       <c r="AA285" s="18">
         <v>100</v>
@@ -84911,11 +84894,11 @@
       <c r="AC285" s="18"/>
       <c r="AD285" s="18"/>
       <c r="AE285" s="18"/>
-      <c r="AF285" s="18" t="e">
+      <c r="AF285" s="18">
         <f>IF(ISBLANK($Z285),0, LOOKUP($Z285,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA285/100)+
 IF(ISBLANK($AB285),0, LOOKUP($AB285,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC285/100)+
 IF(ISBLANK($AD285),0, LOOKUP($AD285,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE285/100)</f>
-        <v>#N/A</v>
+        <v>40</v>
       </c>
       <c r="AG285" s="18">
         <v>0</v>
@@ -85209,7 +85192,7 @@
         <v>16</v>
       </c>
       <c r="Y287" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="Z287" s="37">
         <v>55110017</v>
@@ -85366,7 +85349,7 @@
         <v>0</v>
       </c>
       <c r="Y288" s="8" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Z288" s="37">
         <v>55200003</v>
@@ -85454,13 +85437,13 @@
         <v>51000286</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C289" s="53" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D289" s="19" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E289" s="4">
         <v>2</v>
@@ -85525,7 +85508,7 @@
         <v>97</v>
       </c>
       <c r="Y289" s="4" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="Z289" s="37">
         <v>55510011</v>
@@ -85619,7 +85602,7 @@
         <v>674</v>
       </c>
       <c r="D290" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E290" s="8">
         <v>4</v>
@@ -85684,7 +85667,7 @@
         <v>75</v>
       </c>
       <c r="Y290" s="8" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="Z290" s="37">
         <v>55100014</v>
@@ -85845,7 +85828,7 @@
         <v>75</v>
       </c>
       <c r="Y291" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="Z291" s="37">
         <v>55510010</v>
@@ -85937,10 +85920,10 @@
         <v>51000289</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D292" s="19" t="s">
         <v>815</v>
@@ -86005,10 +85988,10 @@
         <v>0</v>
       </c>
       <c r="X292" s="4" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="Y292" s="4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="Z292" s="37">
         <v>55900032</v>
@@ -86096,10 +86079,10 @@
         <v>51000290</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D293" s="19" t="s">
         <v>815</v>
@@ -86164,10 +86147,10 @@
         <v>0</v>
       </c>
       <c r="X293" s="4" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="Y293" s="4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="Z293" s="37">
         <v>55900032</v>
@@ -86261,7 +86244,7 @@
         <v>635</v>
       </c>
       <c r="D294" s="19" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E294" s="4">
         <v>3</v>
@@ -86326,7 +86309,7 @@
         <v>204</v>
       </c>
       <c r="Y294" s="4" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="Z294" s="37">
         <v>55200005</v>
@@ -86487,7 +86470,7 @@
         <v>675</v>
       </c>
       <c r="Y295" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Z295" s="37">
         <v>55900028</v>
@@ -86581,7 +86564,7 @@
         <v>663</v>
       </c>
       <c r="D296" s="19" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E296" s="8">
         <v>2</v>
@@ -86646,7 +86629,7 @@
         <v>75</v>
       </c>
       <c r="Y296" s="8" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="Z296" s="37">
         <v>55100012</v>
@@ -86740,7 +86723,7 @@
         <v>396</v>
       </c>
       <c r="D297" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E297" s="4">
         <v>3</v>
@@ -86805,7 +86788,7 @@
         <v>44</v>
       </c>
       <c r="Y297" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="Z297" s="37">
         <v>55900011</v>
@@ -86899,7 +86882,7 @@
         <v>397</v>
       </c>
       <c r="D298" s="19" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E298" s="4">
         <v>2</v>
@@ -86964,7 +86947,7 @@
         <v>2</v>
       </c>
       <c r="Y298" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="Z298" s="37">
         <v>55900012</v>
@@ -87372,7 +87355,7 @@
         <v>638</v>
       </c>
       <c r="D301" s="8" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E301" s="4">
         <v>5</v>
@@ -87437,7 +87420,7 @@
         <v>107</v>
       </c>
       <c r="Y301" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="Z301" s="18">
         <v>55200007</v>
@@ -87751,7 +87734,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -87915,7 +87898,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -88079,7 +88062,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -88407,10 +88390,10 @@
         <v>51013003</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="4">
@@ -88558,10 +88541,10 @@
         <v>51013004</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="4">
@@ -90157,7 +90140,7 @@
         <v>666</v>
       </c>
       <c r="B1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -90218,7 +90201,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -90226,7 +90209,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="24" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
@@ -90234,7 +90217,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="B11" s="22"/>
     </row>

</xml_diff>

<commit_message>
#53 fix two monster card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -3893,16 +3893,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000109;100|55900020;100|55000331;20</t>
-  </si>
-  <si>
     <t>55900020;100|55000142;100|55000325;20</t>
   </si>
   <si>
     <t>55900020;100|55000147;100|55000330;20</t>
-  </si>
-  <si>
-    <t>55900020;100|55000149;100|55000327;20</t>
   </si>
   <si>
     <t>55110013;80</t>
@@ -4580,6 +4574,14 @@
   </si>
   <si>
     <t>召唤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900020;100|55900040;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900041;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5626,310 +5628,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="148">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="141">
     <dxf>
       <font>
         <b/>
@@ -7274,6 +6973,202 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8612,6 +8507,51 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -8909,11 +8849,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2100549840"/>
-        <c:axId val="2100545488"/>
+        <c:axId val="-1789746656"/>
+        <c:axId val="-1789751552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2100549840"/>
+        <c:axId val="-1789746656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8956,7 +8896,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100545488"/>
+        <c:crossAx val="-1789751552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8964,7 +8904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100545488"/>
+        <c:axId val="-1789751552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9015,7 +8955,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100549840"/>
+        <c:crossAx val="-1789746656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9385,11 +9325,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2100551472"/>
-        <c:axId val="2100554192"/>
+        <c:axId val="-1789746112"/>
+        <c:axId val="-1617347488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2100551472"/>
+        <c:axId val="-1789746112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9432,7 +9372,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100554192"/>
+        <c:crossAx val="-1617347488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9440,7 +9380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100554192"/>
+        <c:axId val="-1617347488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9491,7 +9431,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100551472"/>
+        <c:crossAx val="-1789746112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12106,23 +12046,23 @@
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55990001</v>
+            <v>55900040</v>
           </cell>
           <cell r="X171">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55990002</v>
+            <v>55900041</v>
           </cell>
           <cell r="X172">
-            <v>15</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55990003</v>
+            <v>55990001</v>
           </cell>
           <cell r="X173">
             <v>15</v>
@@ -12130,7 +12070,7 @@
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55990004</v>
+            <v>55990002</v>
           </cell>
           <cell r="X174">
             <v>15</v>
@@ -12138,7 +12078,7 @@
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55990005</v>
+            <v>55990003</v>
           </cell>
           <cell r="X175">
             <v>15</v>
@@ -12146,7 +12086,7 @@
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55990006</v>
+            <v>55990004</v>
           </cell>
           <cell r="X176">
             <v>15</v>
@@ -12154,7 +12094,7 @@
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55990011</v>
+            <v>55990005</v>
           </cell>
           <cell r="X177">
             <v>15</v>
@@ -12162,7 +12102,7 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55990012</v>
+            <v>55990006</v>
           </cell>
           <cell r="X178">
             <v>15</v>
@@ -12170,7 +12110,7 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55990013</v>
+            <v>55990011</v>
           </cell>
           <cell r="X179">
             <v>15</v>
@@ -12178,7 +12118,7 @@
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55990014</v>
+            <v>55990012</v>
           </cell>
           <cell r="X180">
             <v>15</v>
@@ -12186,7 +12126,7 @@
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55990015</v>
+            <v>55990013</v>
           </cell>
           <cell r="X181">
             <v>15</v>
@@ -12194,7 +12134,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990016</v>
+            <v>55990014</v>
           </cell>
           <cell r="X182">
             <v>15</v>
@@ -12202,33 +12142,49 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990101</v>
+            <v>55990015</v>
           </cell>
           <cell r="X183">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990102</v>
+            <v>55990016</v>
           </cell>
           <cell r="X184">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990103</v>
+            <v>55990101</v>
           </cell>
           <cell r="X185">
-            <v>35</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
+            <v>55990102</v>
+          </cell>
+          <cell r="X186">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="A187">
+            <v>55990103</v>
+          </cell>
+          <cell r="X187">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="A188">
             <v>55990104</v>
           </cell>
-          <cell r="X186">
+          <cell r="X188">
             <v>50</v>
           </cell>
         </row>
@@ -39666,163 +39622,163 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BB301" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BB301" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
   <autoFilter ref="A3:BB301"/>
   <sortState ref="A4:BD301">
     <sortCondition ref="A3:A301"/>
   </sortState>
   <tableColumns count="54">
-    <tableColumn id="1" name="Id" dataDxfId="144"/>
-    <tableColumn id="2" name="Name" dataDxfId="143"/>
-    <tableColumn id="22" name="Ename" dataDxfId="142"/>
-    <tableColumn id="23" name="Remark" dataDxfId="141"/>
-    <tableColumn id="3" name="Star" dataDxfId="140"/>
-    <tableColumn id="4" name="Type" dataDxfId="139"/>
-    <tableColumn id="5" name="Attr" dataDxfId="138"/>
-    <tableColumn id="58" name="Quality" dataDxfId="137">
+    <tableColumn id="1" name="Id" dataDxfId="131"/>
+    <tableColumn id="2" name="Name" dataDxfId="130"/>
+    <tableColumn id="22" name="Ename" dataDxfId="129"/>
+    <tableColumn id="23" name="Remark" dataDxfId="128"/>
+    <tableColumn id="3" name="Star" dataDxfId="127"/>
+    <tableColumn id="4" name="Type" dataDxfId="126"/>
+    <tableColumn id="5" name="Attr" dataDxfId="125"/>
+    <tableColumn id="58" name="Quality" dataDxfId="124">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="136"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="135"/>
-    <tableColumn id="24" name="VitP" dataDxfId="134"/>
-    <tableColumn id="25" name="Modify" dataDxfId="133"/>
-    <tableColumn id="9" name="Def" dataDxfId="132"/>
-    <tableColumn id="10" name="Mag" dataDxfId="131"/>
-    <tableColumn id="32" name="Spd" dataDxfId="130"/>
-    <tableColumn id="35" name="Hit" dataDxfId="129"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="128"/>
-    <tableColumn id="34" name="Crt" dataDxfId="127"/>
-    <tableColumn id="33" name="Luk" dataDxfId="126"/>
-    <tableColumn id="7" name="Sum" dataDxfId="125">
+    <tableColumn id="12" name="Cost" dataDxfId="123"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="122"/>
+    <tableColumn id="24" name="VitP" dataDxfId="121"/>
+    <tableColumn id="25" name="Modify" dataDxfId="120"/>
+    <tableColumn id="9" name="Def" dataDxfId="119"/>
+    <tableColumn id="10" name="Mag" dataDxfId="118"/>
+    <tableColumn id="32" name="Spd" dataDxfId="117"/>
+    <tableColumn id="35" name="Hit" dataDxfId="116"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="115"/>
+    <tableColumn id="34" name="Crt" dataDxfId="114"/>
+    <tableColumn id="33" name="Luk" dataDxfId="113"/>
+    <tableColumn id="7" name="Sum" dataDxfId="112">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AM4:AS4)+2.5*SUM(AG4:AK4)+IF(ISNUMBER(AF4),AF4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="124"/>
-    <tableColumn id="14" name="Mov" dataDxfId="123"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="122"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="121"/>
-    <tableColumn id="18" name="Skills" dataDxfId="120"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="119"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="118"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="117"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="116"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="115"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="114"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="113">
+    <tableColumn id="13" name="Range" dataDxfId="111"/>
+    <tableColumn id="14" name="Mov" dataDxfId="110"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="109"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="108"/>
+    <tableColumn id="18" name="Skills" dataDxfId="107"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="106"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="105"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="104"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="103"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="102"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="101"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="100">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="112"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="111"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="110"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="109"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="108"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="107">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="99"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="98"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="97"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="96"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="95"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="94">
       <calculatedColumnFormula>CONCATENATE(AG4,";",AH4,";",AI4,";",AJ4,";",AK4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="106"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="105"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="104"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="103"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="102"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="101"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="100"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="99">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="93"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="92"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="91"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="90"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="89"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="88"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="87"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="86">
       <calculatedColumnFormula>CONCATENATE(AM4,";",AN4,";",AO4,";",AP4,";",AQ4,";",AR4,";",AS4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="98"/>
-    <tableColumn id="29" name="JobId" dataDxfId="97"/>
-    <tableColumn id="20" name="Res" dataDxfId="96"/>
-    <tableColumn id="21" name="Icon" dataDxfId="95"/>
-    <tableColumn id="17" name="Cover" dataDxfId="94"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="93"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="92"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="91"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="85"/>
+    <tableColumn id="29" name="JobId" dataDxfId="84"/>
+    <tableColumn id="20" name="Res" dataDxfId="83"/>
+    <tableColumn id="21" name="Icon" dataDxfId="82"/>
+    <tableColumn id="17" name="Cover" dataDxfId="81"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="80"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="79"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BB13" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BB13" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
   <autoFilter ref="A3:BB13"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="54">
-    <tableColumn id="1" name="Id" dataDxfId="87"/>
-    <tableColumn id="2" name="Name" dataDxfId="86"/>
-    <tableColumn id="22" name="Ename" dataDxfId="85"/>
-    <tableColumn id="23" name="Remark" dataDxfId="84"/>
-    <tableColumn id="3" name="Star" dataDxfId="83"/>
-    <tableColumn id="4" name="Type" dataDxfId="82"/>
-    <tableColumn id="5" name="Attr" dataDxfId="81"/>
-    <tableColumn id="58" name="Quality" dataDxfId="80">
+    <tableColumn id="1" name="Id" dataDxfId="54"/>
+    <tableColumn id="2" name="Name" dataDxfId="53"/>
+    <tableColumn id="22" name="Ename" dataDxfId="52"/>
+    <tableColumn id="23" name="Remark" dataDxfId="51"/>
+    <tableColumn id="3" name="Star" dataDxfId="50"/>
+    <tableColumn id="4" name="Type" dataDxfId="49"/>
+    <tableColumn id="5" name="Attr" dataDxfId="48"/>
+    <tableColumn id="58" name="Quality" dataDxfId="47">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="79"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="78"/>
-    <tableColumn id="24" name="VitP" dataDxfId="77"/>
-    <tableColumn id="25" name="Modify" dataDxfId="76"/>
-    <tableColumn id="9" name="Def" dataDxfId="75"/>
-    <tableColumn id="10" name="Mag" dataDxfId="74"/>
-    <tableColumn id="32" name="Spd" dataDxfId="73"/>
-    <tableColumn id="35" name="Hit" dataDxfId="72"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="71"/>
-    <tableColumn id="34" name="Crt" dataDxfId="70"/>
-    <tableColumn id="33" name="Luk" dataDxfId="69"/>
-    <tableColumn id="7" name="Sum" dataDxfId="68">
+    <tableColumn id="12" name="Cost" dataDxfId="46"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="45"/>
+    <tableColumn id="24" name="VitP" dataDxfId="44"/>
+    <tableColumn id="25" name="Modify" dataDxfId="43"/>
+    <tableColumn id="9" name="Def" dataDxfId="42"/>
+    <tableColumn id="10" name="Mag" dataDxfId="41"/>
+    <tableColumn id="32" name="Spd" dataDxfId="40"/>
+    <tableColumn id="35" name="Hit" dataDxfId="39"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="38"/>
+    <tableColumn id="34" name="Crt" dataDxfId="37"/>
+    <tableColumn id="33" name="Luk" dataDxfId="36"/>
+    <tableColumn id="7" name="Sum" dataDxfId="35">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AM4:AS4)+2.5*SUM(AG4:AK4)+IF(ISNUMBER(AF4),AF4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="67"/>
-    <tableColumn id="14" name="Mov" dataDxfId="66"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="65"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="64"/>
-    <tableColumn id="18" name="Skills" dataDxfId="63"/>
-    <tableColumn id="42" name="~Skill1" dataDxfId="62"/>
-    <tableColumn id="43" name="~SkillRate1" dataDxfId="61"/>
-    <tableColumn id="44" name="~Skill2" dataDxfId="60"/>
-    <tableColumn id="45" name="~SkillRate2" dataDxfId="59"/>
-    <tableColumn id="46" name="~Skill3" dataDxfId="58"/>
-    <tableColumn id="47" name="~SkillRate3" dataDxfId="57"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="56">
+    <tableColumn id="13" name="Range" dataDxfId="34"/>
+    <tableColumn id="14" name="Mov" dataDxfId="33"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="32"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="31"/>
+    <tableColumn id="18" name="Skills" dataDxfId="30"/>
+    <tableColumn id="42" name="~Skill1" dataDxfId="29"/>
+    <tableColumn id="43" name="~SkillRate1" dataDxfId="28"/>
+    <tableColumn id="44" name="~Skill2" dataDxfId="27"/>
+    <tableColumn id="45" name="~SkillRate2" dataDxfId="26"/>
+    <tableColumn id="46" name="~Skill3" dataDxfId="25"/>
+    <tableColumn id="47" name="~SkillRate3" dataDxfId="24"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="23">
       <calculatedColumnFormula>IF(ISBLANK($Z4),0, LOOKUP($Z4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA4/100)+
 IF(ISBLANK($AB4),0, LOOKUP($AB4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC4/100)+
 IF(ISBLANK($AD4),0, LOOKUP($AD4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="55"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="54"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="53"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="52"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="51"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="50">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="22"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="21"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="20"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="19"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="18"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="17">
       <calculatedColumnFormula>CONCATENATE(AG4,";",AH4,";",AI4,";",AJ4,";",AK4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="49"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="48"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="47"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="46"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="45"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="44"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="43"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="42">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="16"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="15"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="14"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="13"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="12"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE(AM4,";",AN4,";",AO4,";",AP4,";",AQ4,";",AR4,";",AS4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="41"/>
-    <tableColumn id="29" name="JobId" dataDxfId="40"/>
-    <tableColumn id="20" name="Res" dataDxfId="39"/>
-    <tableColumn id="21" name="Icon" dataDxfId="38"/>
-    <tableColumn id="17" name="Cover" dataDxfId="37"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="36"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="35"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="34"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
+    <tableColumn id="29" name="JobId" dataDxfId="7"/>
+    <tableColumn id="20" name="Res" dataDxfId="6"/>
+    <tableColumn id="21" name="Icon" dataDxfId="5"/>
+    <tableColumn id="17" name="Cover" dataDxfId="4"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -40132,7 +40088,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E115" sqref="E115"/>
+      <selection pane="bottomRight" activeCell="V115" sqref="V115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40308,7 +40264,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -40472,7 +40428,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -40636,7 +40592,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -42287,7 +42243,7 @@
         <v>6</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="Z14" s="37">
         <v>55110014</v>
@@ -45628,13 +45584,13 @@
         <v>51000033</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>1029</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>1031</v>
       </c>
       <c r="E36" s="4">
         <v>2</v>
@@ -45696,10 +45652,10 @@
         <v>0</v>
       </c>
       <c r="X36" s="4" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="Z36" s="37">
         <v>55300008</v>
@@ -45793,7 +45749,7 @@
         <v>494</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="E37" s="4">
         <v>2</v>
@@ -45858,7 +45814,7 @@
         <v>38</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="Z37" s="37">
         <v>55610003</v>
@@ -46405,13 +46361,13 @@
         <v>51000038</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="E41" s="4">
         <v>4</v>
@@ -46473,10 +46429,10 @@
         <v>0</v>
       </c>
       <c r="X41" s="4" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="Z41" s="37">
         <v>55100011</v>
@@ -46568,13 +46524,13 @@
         <v>51000039</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>409</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="E42" s="4">
         <v>3</v>
@@ -46639,7 +46595,7 @@
         <v>50</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="Z42" s="18">
         <v>55100011</v>
@@ -46890,7 +46846,7 @@
         <v>497</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="E44" s="4">
         <v>3</v>
@@ -46955,7 +46911,7 @@
         <v>16</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="Z44" s="18">
         <v>55900026</v>
@@ -47112,7 +47068,7 @@
         <v>4</v>
       </c>
       <c r="Y45" s="4" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="Z45" s="37">
         <v>55110013</v>
@@ -47746,7 +47702,7 @@
         <v>19</v>
       </c>
       <c r="Y49" s="4" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="Z49" s="37">
         <v>55100015</v>
@@ -49954,7 +49910,7 @@
         <v>38</v>
       </c>
       <c r="Y63" s="4" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="Z63" s="37">
         <v>55510009</v>
@@ -50517,7 +50473,7 @@
         <v>340</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E67" s="4">
         <v>6</v>
@@ -50582,7 +50538,7 @@
         <v>75</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="Z67" s="37">
         <v>55510010</v>
@@ -50676,7 +50632,7 @@
         <v>512</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="E68" s="4">
         <v>7</v>
@@ -50741,7 +50697,7 @@
         <v>75</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="Z68" s="37">
         <v>55300010</v>
@@ -50837,7 +50793,7 @@
         <v>341</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="E69" s="4">
         <v>6</v>
@@ -50902,7 +50858,7 @@
         <v>40</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="Z69" s="18">
         <v>55200008</v>
@@ -51838,7 +51794,7 @@
         <v>86</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="Z75" s="37">
         <v>55500008</v>
@@ -51936,7 +51892,7 @@
         <v>518</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E76" s="4">
         <v>4</v>
@@ -52001,7 +51957,7 @@
         <v>12</v>
       </c>
       <c r="Y76" s="4" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="Z76" s="37">
         <v>55100001</v>
@@ -52790,7 +52746,7 @@
         <v>2</v>
       </c>
       <c r="Y81" s="4" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="Z81" s="37">
         <v>55600014</v>
@@ -52947,7 +52903,7 @@
         <v>2</v>
       </c>
       <c r="Y82" s="4" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="Z82" s="37">
         <v>55100010</v>
@@ -53679,7 +53635,7 @@
         <v>523</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E87" s="4">
         <v>3</v>
@@ -53744,7 +53700,7 @@
         <v>83</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="Z87" s="37">
         <v>55100011</v>
@@ -54219,7 +54175,7 @@
         <v>103</v>
       </c>
       <c r="Y90" s="4" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="Z90" s="37">
         <v>55100002</v>
@@ -54849,7 +54805,7 @@
         <v>75</v>
       </c>
       <c r="Y94" s="4" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="Z94" s="37">
         <v>55500008</v>
@@ -55161,7 +55117,7 @@
         <v>2</v>
       </c>
       <c r="Y96" s="4" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="Z96" s="37">
         <v>55500008</v>
@@ -55324,7 +55280,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="Z97" s="37">
         <v>55110007</v>
@@ -55489,7 +55445,7 @@
         <v>91</v>
       </c>
       <c r="Y98" s="4" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="Z98" s="37">
         <v>55510002</v>
@@ -56368,7 +56324,7 @@
         <v>350</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E104" s="4">
         <v>3</v>
@@ -56433,7 +56389,7 @@
         <v>4</v>
       </c>
       <c r="Y104" s="4" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="Z104" s="37">
         <v>55100015</v>
@@ -56531,7 +56487,7 @@
         <v>536</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E105" s="4">
         <v>2</v>
@@ -56596,7 +56552,7 @@
         <v>103</v>
       </c>
       <c r="Y105" s="4" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="Z105" s="37">
         <v>55900035</v>
@@ -56690,7 +56646,7 @@
         <v>537</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E106" s="4">
         <v>2</v>
@@ -56755,7 +56711,7 @@
         <v>9</v>
       </c>
       <c r="Y106" s="4" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="Z106" s="37">
         <v>55300009</v>
@@ -57071,7 +57027,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="Z108" s="37">
         <v>55900027</v>
@@ -57926,7 +57882,7 @@
         <v>542</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="E114" s="4">
         <v>7</v>
@@ -57991,7 +57947,7 @@
         <v>86</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="Z114" s="37">
         <v>55900039</v>
@@ -58091,7 +58047,7 @@
         <v>354</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>737</v>
+        <v>809</v>
       </c>
       <c r="E115" s="4">
         <v>7</v>
@@ -58104,22 +58060,22 @@
       </c>
       <c r="H115" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I115" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J115" s="4">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K115" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L115" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M115" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N115" s="4">
         <v>0</v>
@@ -58141,13 +58097,13 @@
       </c>
       <c r="T115" s="12">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="U115" s="4">
         <v>10</v>
       </c>
       <c r="V115" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="W115" s="4">
         <v>0</v>
@@ -58156,23 +58112,23 @@
         <v>91</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>952</v>
-      </c>
-      <c r="Z115" s="37"/>
-      <c r="AA115" s="18"/>
-      <c r="AB115" s="18">
-        <v>55900020</v>
-      </c>
-      <c r="AC115" s="18">
+        <v>1126</v>
+      </c>
+      <c r="Z115" s="37">
+        <v>55900041</v>
+      </c>
+      <c r="AA115" s="18">
         <v>100</v>
       </c>
+      <c r="AB115" s="18"/>
+      <c r="AC115" s="18"/>
       <c r="AD115" s="18"/>
       <c r="AE115" s="18"/>
       <c r="AF115" s="18">
         <f>IF(ISBLANK($Z115),0, LOOKUP($Z115,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA115/100)+
 IF(ISBLANK($AB115),0, LOOKUP($AB115,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC115/100)+
 IF(ISBLANK($AD115),0, LOOKUP($AD115,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE115/100)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AG115" s="18">
         <v>0</v>
@@ -58317,7 +58273,7 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Z116" s="37"/>
       <c r="AA116" s="18"/>
@@ -58413,7 +58369,7 @@
         <v>533</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="E117" s="4">
         <v>7</v>
@@ -58429,7 +58385,7 @@
         <v>4</v>
       </c>
       <c r="I117" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J117" s="4">
         <v>0</v>
@@ -58478,7 +58434,7 @@
         <v>75</v>
       </c>
       <c r="Y117" s="4" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="Z117" s="37">
         <v>55400007</v>
@@ -58963,7 +58919,7 @@
         <v>49</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Z120" s="37"/>
       <c r="AA120" s="18"/>
@@ -59059,7 +59015,7 @@
         <v>545</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>737</v>
+        <v>1019</v>
       </c>
       <c r="E121" s="4">
         <v>7</v>
@@ -59072,16 +59028,16 @@
       </c>
       <c r="H121" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I121" s="4">
         <v>7</v>
       </c>
       <c r="J121" s="4">
-        <v>8</v>
+        <v>-40</v>
       </c>
       <c r="K121" s="4">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L121" s="7">
         <v>1</v>
@@ -59109,7 +59065,7 @@
       </c>
       <c r="T121" s="12">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="U121" s="4">
         <v>10</v>
@@ -59124,10 +59080,14 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>955</v>
-      </c>
-      <c r="Z121" s="37"/>
-      <c r="AA121" s="18"/>
+        <v>1125</v>
+      </c>
+      <c r="Z121" s="37">
+        <v>55900040</v>
+      </c>
+      <c r="AA121" s="18">
+        <v>100</v>
+      </c>
       <c r="AB121" s="18">
         <v>55900020</v>
       </c>
@@ -59140,7 +59100,7 @@
         <f>IF(ISBLANK($Z121),0, LOOKUP($Z121,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA121/100)+
 IF(ISBLANK($AB121),0, LOOKUP($AB121,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC121/100)+
 IF(ISBLANK($AD121),0, LOOKUP($AD121,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE121/100)</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="AG121" s="18">
         <v>0</v>
@@ -59434,7 +59394,7 @@
         <v>4</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="Z123" s="37">
         <v>55100005</v>
@@ -59750,7 +59710,7 @@
         <v>2</v>
       </c>
       <c r="Y125" s="4" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="Z125" s="37">
         <v>55100010</v>
@@ -59848,7 +59808,7 @@
         <v>355</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E126" s="4">
         <v>1</v>
@@ -59913,7 +59873,7 @@
         <v>24</v>
       </c>
       <c r="Y126" s="4" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="Z126" s="37">
         <v>55600012</v>
@@ -60474,7 +60434,7 @@
         <v>552</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="E130" s="4">
         <v>1</v>
@@ -60539,7 +60499,7 @@
         <v>103</v>
       </c>
       <c r="Y130" s="4" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="Z130" s="37">
         <v>55900024</v>
@@ -61004,7 +60964,7 @@
         <v>103</v>
       </c>
       <c r="Y133" s="4" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="Z133" s="37">
         <v>55900027</v>
@@ -61483,7 +61443,7 @@
         <v>103</v>
       </c>
       <c r="Y136" s="4" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="Z136" s="37">
         <v>55110005</v>
@@ -61640,7 +61600,7 @@
         <v>2</v>
       </c>
       <c r="Y137" s="4" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="Z137" s="37">
         <v>55510010</v>
@@ -61801,7 +61761,7 @@
         <v>6</v>
       </c>
       <c r="Y138" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="Z138" s="37">
         <v>55100006</v>
@@ -62570,7 +62530,7 @@
         <v>4</v>
       </c>
       <c r="Y143" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="Z143" s="18">
         <v>55110015</v>
@@ -63037,7 +62997,7 @@
         <v>103</v>
       </c>
       <c r="Y146" s="4" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="Z146" s="37">
         <v>55110007</v>
@@ -63135,7 +63095,7 @@
         <v>360</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E147" s="4">
         <v>3</v>
@@ -63200,7 +63160,7 @@
         <v>19</v>
       </c>
       <c r="Y147" s="4" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="Z147" s="18">
         <v>55510006</v>
@@ -63457,7 +63417,7 @@
         <v>361</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="E149" s="4">
         <v>3</v>
@@ -64389,7 +64349,7 @@
         <v>568</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E155" s="4">
         <v>3</v>
@@ -64454,7 +64414,7 @@
         <v>735</v>
       </c>
       <c r="Y155" s="4" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="Z155" s="37">
         <v>55100013</v>
@@ -64611,7 +64571,7 @@
         <v>4</v>
       </c>
       <c r="Y156" s="4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="Z156" s="37">
         <v>55110004</v>
@@ -67024,7 +66984,7 @@
         <v>579</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E172" s="4">
         <v>4</v>
@@ -67089,7 +67049,7 @@
         <v>4</v>
       </c>
       <c r="Y172" s="4" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="Z172" s="37">
         <v>55510018</v>
@@ -67187,7 +67147,7 @@
         <v>580</v>
       </c>
       <c r="D173" s="19" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E173" s="4">
         <v>2</v>
@@ -67252,7 +67212,7 @@
         <v>729</v>
       </c>
       <c r="Y173" s="4" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="Z173" s="37">
         <v>55200004</v>
@@ -67731,7 +67691,7 @@
         <v>12</v>
       </c>
       <c r="Y176" s="4" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="Z176" s="37">
         <v>55610003</v>
@@ -67984,7 +67944,7 @@
         <v>584</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E178" s="4">
         <v>4</v>
@@ -68049,7 +68009,7 @@
         <v>4</v>
       </c>
       <c r="Y178" s="4" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="Z178" s="37">
         <v>55510004</v>
@@ -68363,7 +68323,7 @@
         <v>62</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="Z180" s="18">
         <v>55900023</v>
@@ -68461,7 +68421,7 @@
         <v>586</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E181" s="4">
         <v>5</v>
@@ -68526,7 +68486,7 @@
         <v>654</v>
       </c>
       <c r="Y181" s="4" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="Z181" s="37">
         <v>55200012</v>
@@ -68687,7 +68647,7 @@
         <v>4</v>
       </c>
       <c r="Y182" s="4" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="Z182" s="37">
         <v>55610003</v>
@@ -68844,7 +68804,7 @@
         <v>16</v>
       </c>
       <c r="Y183" s="4" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="Z183" s="37">
         <v>55900031</v>
@@ -68942,7 +68902,7 @@
         <v>589</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E184" s="4">
         <v>3</v>
@@ -69007,7 +68967,7 @@
         <v>75</v>
       </c>
       <c r="Y184" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="Z184" s="37">
         <v>55510010</v>
@@ -69101,7 +69061,7 @@
         <v>367</v>
       </c>
       <c r="D185" s="19" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="E185" s="4">
         <v>6</v>
@@ -69166,7 +69126,7 @@
         <v>12</v>
       </c>
       <c r="Y185" s="4" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="Z185" s="37">
         <v>55600011</v>
@@ -69329,7 +69289,7 @@
         <v>75</v>
       </c>
       <c r="Y186" s="4" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="Z186" s="37">
         <v>55600016</v>
@@ -70265,7 +70225,7 @@
         <v>730</v>
       </c>
       <c r="Y192" s="4" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="Z192" s="37">
         <v>55110001</v>
@@ -70689,7 +70649,7 @@
         <v>598</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E195" s="4">
         <v>5</v>
@@ -70754,7 +70714,7 @@
         <v>204</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="Z195" s="18">
         <v>55100011</v>
@@ -70852,7 +70812,7 @@
         <v>599</v>
       </c>
       <c r="D196" s="19" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E196" s="4">
         <v>5</v>
@@ -70917,7 +70877,7 @@
         <v>4</v>
       </c>
       <c r="Y196" s="4" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="Z196" s="18">
         <v>55520003</v>
@@ -71339,7 +71299,7 @@
         <v>602</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E199" s="4">
         <v>5</v>
@@ -71404,7 +71364,7 @@
         <v>2</v>
       </c>
       <c r="Y199" s="4" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="Z199" s="37">
         <v>55100010</v>
@@ -71565,7 +71525,7 @@
         <v>4</v>
       </c>
       <c r="Y200" s="4" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="Z200" s="37">
         <v>55110008</v>
@@ -72291,7 +72251,7 @@
         <v>604</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="E205" s="4">
         <v>2</v>
@@ -72356,7 +72316,7 @@
         <v>734</v>
       </c>
       <c r="Y205" s="4" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="Z205" s="37">
         <v>55510013</v>
@@ -72674,7 +72634,7 @@
         <v>168</v>
       </c>
       <c r="Y207" s="4" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="Z207" s="37">
         <v>55900029</v>
@@ -72990,7 +72950,7 @@
         <v>2</v>
       </c>
       <c r="Y209" s="4" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="Z209" s="37">
         <v>55510003</v>
@@ -73930,7 +73890,7 @@
         <v>185</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="Z215" s="37">
         <v>55100001</v>
@@ -74091,7 +74051,7 @@
         <v>6</v>
       </c>
       <c r="Y216" s="4" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="Z216" s="37">
         <v>55900031</v>
@@ -74344,7 +74304,7 @@
         <v>613</v>
       </c>
       <c r="D218" s="19" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E218" s="4">
         <v>2</v>
@@ -74409,7 +74369,7 @@
         <v>4</v>
       </c>
       <c r="Y218" s="4" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="Z218" s="37">
         <v>55900034</v>
@@ -74503,7 +74463,7 @@
         <v>614</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="E219" s="4">
         <v>3</v>
@@ -74568,7 +74528,7 @@
         <v>733</v>
       </c>
       <c r="Y219" s="4" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="Z219" s="37">
         <v>55510019</v>
@@ -74725,7 +74685,7 @@
         <v>62</v>
       </c>
       <c r="Y220" s="4" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="Z220" s="37">
         <v>55100001</v>
@@ -74819,7 +74779,7 @@
         <v>615</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="E221" s="4">
         <v>4</v>
@@ -74884,7 +74844,7 @@
         <v>231</v>
       </c>
       <c r="Y221" s="4" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="Z221" s="37">
         <v>55200009</v>
@@ -75359,7 +75319,7 @@
         <v>103</v>
       </c>
       <c r="Y224" s="7" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="Z224" s="37">
         <v>55900016</v>
@@ -75520,7 +75480,7 @@
         <v>16</v>
       </c>
       <c r="Y225" s="4" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="Z225" s="37">
         <v>55610002</v>
@@ -75934,7 +75894,7 @@
         <v>429</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E228" s="4">
         <v>3</v>
@@ -75999,7 +75959,7 @@
         <v>239</v>
       </c>
       <c r="Y228" s="4" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Z228" s="37">
         <v>55510001</v>
@@ -76093,7 +76053,7 @@
         <v>375</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E229" s="4">
         <v>2</v>
@@ -76158,7 +76118,7 @@
         <v>24</v>
       </c>
       <c r="Y229" s="4" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="Z229" s="37">
         <v>55510007</v>
@@ -76788,7 +76748,7 @@
         <v>245</v>
       </c>
       <c r="Y233" s="4" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="Z233" s="37">
         <v>55100009</v>
@@ -77043,7 +77003,7 @@
         <v>623</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E235" s="4">
         <v>3</v>
@@ -77108,7 +77068,7 @@
         <v>6</v>
       </c>
       <c r="Y235" s="4" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="Z235" s="18">
         <v>55600013</v>
@@ -77202,7 +77162,7 @@
         <v>624</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E236" s="4">
         <v>2</v>
@@ -77267,7 +77227,7 @@
         <v>12</v>
       </c>
       <c r="Y236" s="4" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="Z236" s="37">
         <v>55600013</v>
@@ -77985,7 +77945,7 @@
         <v>435</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E241" s="4">
         <v>5</v>
@@ -78050,7 +78010,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="Z241" s="37">
         <v>55100010</v>
@@ -78366,7 +78326,7 @@
         <v>66</v>
       </c>
       <c r="Y243" s="4" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="Z243" s="37">
         <v>55900033</v>
@@ -78460,7 +78420,7 @@
         <v>378</v>
       </c>
       <c r="D244" s="19" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="E244" s="4">
         <v>3</v>
@@ -78525,7 +78485,7 @@
         <v>2</v>
       </c>
       <c r="Y244" s="4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="Z244" s="37">
         <v>55510014</v>
@@ -78619,7 +78579,7 @@
         <v>379</v>
       </c>
       <c r="D245" s="19" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="E245" s="4">
         <v>6</v>
@@ -78684,7 +78644,7 @@
         <v>66</v>
       </c>
       <c r="Y245" s="4" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="Z245" s="37">
         <v>55510014</v>
@@ -78996,7 +78956,7 @@
         <v>2</v>
       </c>
       <c r="Y247" s="4" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="Z247" s="37">
         <v>55510010</v>
@@ -79157,7 +79117,7 @@
         <v>19</v>
       </c>
       <c r="Y248" s="4" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="Z248" s="37">
         <v>55900025</v>
@@ -79465,7 +79425,7 @@
         <v>2</v>
       </c>
       <c r="Y250" s="4" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="Z250" s="37">
         <v>55510009</v>
@@ -79626,7 +79586,7 @@
         <v>4</v>
       </c>
       <c r="Y251" s="4" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="Z251" s="18">
         <v>55900030</v>
@@ -79783,7 +79743,7 @@
         <v>131</v>
       </c>
       <c r="Y252" s="4" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="Z252" s="18">
         <v>55110007</v>
@@ -80193,7 +80153,7 @@
         <v>381</v>
       </c>
       <c r="D255" s="19" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E255" s="4">
         <v>4</v>
@@ -80258,7 +80218,7 @@
         <v>0</v>
       </c>
       <c r="Y255" s="4" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="Z255" s="37">
         <v>55510018</v>
@@ -80513,7 +80473,7 @@
         <v>630</v>
       </c>
       <c r="D257" s="19" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E257" s="4">
         <v>3</v>
@@ -80578,7 +80538,7 @@
         <v>2</v>
       </c>
       <c r="Y257" s="4" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="Z257" s="37">
         <v>55200013</v>
@@ -80669,7 +80629,7 @@
         <v>259</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D258" s="19"/>
       <c r="E258" s="4">
@@ -80735,7 +80695,7 @@
         <v>245</v>
       </c>
       <c r="Y258" s="4" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="Z258" s="37">
         <v>55410001</v>
@@ -80833,7 +80793,7 @@
         <v>631</v>
       </c>
       <c r="D259" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E259" s="4">
         <v>2</v>
@@ -80898,7 +80858,7 @@
         <v>4</v>
       </c>
       <c r="Y259" s="7" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="Z259" s="37">
         <v>55100012</v>
@@ -80996,7 +80956,7 @@
         <v>383</v>
       </c>
       <c r="D260" s="19" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E260" s="4">
         <v>3</v>
@@ -81061,7 +81021,7 @@
         <v>6</v>
       </c>
       <c r="Y260" s="4" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="Z260" s="37">
         <v>55900010</v>
@@ -82005,7 +81965,7 @@
         <v>24</v>
       </c>
       <c r="Y266" s="4" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="Z266" s="37">
         <v>55900031</v>
@@ -82099,7 +82059,7 @@
         <v>388</v>
       </c>
       <c r="D267" s="19" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="E267" s="4">
         <v>5</v>
@@ -82164,7 +82124,7 @@
         <v>91</v>
       </c>
       <c r="Y267" s="4" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="Z267" s="37">
         <v>55510001</v>
@@ -82325,7 +82285,7 @@
         <v>16</v>
       </c>
       <c r="Y268" s="4" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="Z268" s="37">
         <v>55900031</v>
@@ -82733,7 +82693,7 @@
         <v>390</v>
       </c>
       <c r="D271" s="19" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E271" s="4">
         <v>5</v>
@@ -82798,7 +82758,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="Z271" s="18">
         <v>55100012</v>
@@ -82896,7 +82856,7 @@
         <v>632</v>
       </c>
       <c r="D272" s="19" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E272" s="4">
         <v>5</v>
@@ -82961,7 +82921,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="Z272" s="18">
         <v>55100012</v>
@@ -83059,7 +83019,7 @@
         <v>391</v>
       </c>
       <c r="D273" s="19" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E273" s="4">
         <v>5</v>
@@ -83124,7 +83084,7 @@
         <v>736</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="Z273" s="18">
         <v>55100012</v>
@@ -83285,7 +83245,7 @@
         <v>0</v>
       </c>
       <c r="Y274" s="4" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="Z274" s="37">
         <v>55200003</v>
@@ -83444,7 +83404,7 @@
         <v>271</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="Z275" s="37">
         <v>55700005</v>
@@ -83689,7 +83649,7 @@
         <v>460</v>
       </c>
       <c r="D277" s="19" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="E277" s="4">
         <v>3</v>
@@ -83754,7 +83714,7 @@
         <v>75</v>
       </c>
       <c r="Y277" s="4" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="Z277" s="18">
         <v>55310003</v>
@@ -83911,7 +83871,7 @@
         <v>4</v>
       </c>
       <c r="Y278" s="4" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="Z278" s="18">
         <v>55110016</v>
@@ -84072,7 +84032,7 @@
         <v>4</v>
       </c>
       <c r="Y279" s="7" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="Z279" s="37">
         <v>55900022</v>
@@ -84229,7 +84189,7 @@
         <v>16</v>
       </c>
       <c r="Y280" s="4" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="Z280" s="37">
         <v>55110019</v>
@@ -84323,7 +84283,7 @@
         <v>393</v>
       </c>
       <c r="D281" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E281" s="4">
         <v>1</v>
@@ -84482,7 +84442,7 @@
         <v>394</v>
       </c>
       <c r="D282" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E282" s="4">
         <v>1</v>
@@ -84641,7 +84601,7 @@
         <v>395</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E283" s="4">
         <v>1</v>
@@ -84865,7 +84825,7 @@
         <v>6</v>
       </c>
       <c r="Y284" s="4" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="Z284" s="37">
         <v>55200010</v>
@@ -84959,7 +84919,7 @@
         <v>636</v>
       </c>
       <c r="D285" s="19" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E285" s="4">
         <v>6</v>
@@ -85024,7 +84984,7 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="Z285" s="37">
         <v>55900038</v>
@@ -85334,7 +85294,7 @@
         <v>16</v>
       </c>
       <c r="Y287" s="4" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="Z287" s="37">
         <v>55110017</v>
@@ -85579,13 +85539,13 @@
         <v>51000286</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C289" s="53" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D289" s="19" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E289" s="4">
         <v>2</v>
@@ -85650,7 +85610,7 @@
         <v>97</v>
       </c>
       <c r="Y289" s="4" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="Z289" s="37">
         <v>55510011</v>
@@ -86062,10 +86022,10 @@
         <v>51000289</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="D292" s="19" t="s">
         <v>815</v>
@@ -86130,10 +86090,10 @@
         <v>0</v>
       </c>
       <c r="X292" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="Y292" s="4" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="Z292" s="37">
         <v>55900032</v>
@@ -86221,10 +86181,10 @@
         <v>51000290</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D293" s="19" t="s">
         <v>815</v>
@@ -86289,10 +86249,10 @@
         <v>0</v>
       </c>
       <c r="X293" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="Y293" s="4" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="Z293" s="37">
         <v>55900032</v>
@@ -86386,7 +86346,7 @@
         <v>635</v>
       </c>
       <c r="D294" s="19" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="E294" s="4">
         <v>3</v>
@@ -86451,7 +86411,7 @@
         <v>204</v>
       </c>
       <c r="Y294" s="4" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="Z294" s="37">
         <v>55200005</v>
@@ -86612,7 +86572,7 @@
         <v>675</v>
       </c>
       <c r="Y295" s="4" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="Z295" s="37">
         <v>55900028</v>
@@ -87497,7 +87457,7 @@
         <v>638</v>
       </c>
       <c r="D301" s="8" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E301" s="4">
         <v>5</v>
@@ -87562,7 +87522,7 @@
         <v>107</v>
       </c>
       <c r="Y301" s="4" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="Z301" s="18">
         <v>55200007</v>
@@ -87652,24 +87612,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H301">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="140" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D301">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -87876,7 +87836,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -88040,7 +88000,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -88204,7 +88164,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -88381,10 +88341,10 @@
         <v>51013001</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8">
@@ -88450,7 +88410,7 @@
         <v>9</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="Z5" s="18">
         <v>55510010</v>
@@ -88689,10 +88649,10 @@
         <v>51013003</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="4">
@@ -88840,10 +88800,10 @@
         <v>51013004</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="4">
@@ -89744,25 +89704,25 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K12:K13 K4 J6:K9">
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="32" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="31" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="24" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89780,13 +89740,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89804,13 +89764,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="21" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="20" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89828,19 +89788,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="69" priority="10" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="14" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89857,31 +89817,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="7" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -90480,7 +90440,7 @@
         <v>666</v>
       </c>
       <c r="B1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -90541,7 +90501,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -90549,7 +90509,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="24" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
@@ -90557,7 +90517,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="B11" s="22"/>
     </row>

</xml_diff>

<commit_message>
#53 fix 3 bigboss
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="1129">
   <si>
     <t>arrow</t>
   </si>
@@ -3557,9 +3557,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55000099;100|55000140;100|55000329;20</t>
-  </si>
-  <si>
     <t>55100004;100|55500005;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3893,12 +3890,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55900020;100|55000142;100|55000325;20</t>
-  </si>
-  <si>
-    <t>55900020;100|55000147;100|55000330;20</t>
-  </si>
-  <si>
     <t>55110013;80</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4582,6 +4573,26 @@
   </si>
   <si>
     <t>55900041;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900020;100|55900042;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900020;100|55900043;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>治疗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55900020;100|55900044;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8849,11 +8860,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1789746656"/>
-        <c:axId val="-1789751552"/>
+        <c:axId val="1327023040"/>
+        <c:axId val="1327021408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1789746656"/>
+        <c:axId val="1327023040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8896,7 +8907,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1789751552"/>
+        <c:crossAx val="1327021408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8904,7 +8915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1789751552"/>
+        <c:axId val="1327021408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8955,7 +8966,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1789746656"/>
+        <c:crossAx val="1327023040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9325,11 +9336,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1789746112"/>
-        <c:axId val="-1617347488"/>
+        <c:axId val="1327013248"/>
+        <c:axId val="1327013792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1789746112"/>
+        <c:axId val="1327013248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9372,7 +9383,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1617347488"/>
+        <c:crossAx val="1327013792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9380,7 +9391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1617347488"/>
+        <c:axId val="1327013792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9431,7 +9442,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1789746112"/>
+        <c:crossAx val="1327013248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12062,31 +12073,31 @@
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55990001</v>
+            <v>55900042</v>
           </cell>
           <cell r="X173">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55990002</v>
+            <v>55900043</v>
           </cell>
           <cell r="X174">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55990003</v>
+            <v>55900044</v>
           </cell>
           <cell r="X175">
-            <v>15</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55990004</v>
+            <v>55990001</v>
           </cell>
           <cell r="X176">
             <v>15</v>
@@ -12094,7 +12105,7 @@
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55990005</v>
+            <v>55990002</v>
           </cell>
           <cell r="X177">
             <v>15</v>
@@ -12102,7 +12113,7 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55990006</v>
+            <v>55990003</v>
           </cell>
           <cell r="X178">
             <v>15</v>
@@ -12110,7 +12121,7 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55990011</v>
+            <v>55990004</v>
           </cell>
           <cell r="X179">
             <v>15</v>
@@ -12118,7 +12129,7 @@
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55990012</v>
+            <v>55990005</v>
           </cell>
           <cell r="X180">
             <v>15</v>
@@ -12126,7 +12137,7 @@
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55990013</v>
+            <v>55990006</v>
           </cell>
           <cell r="X181">
             <v>15</v>
@@ -12134,7 +12145,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990014</v>
+            <v>55990011</v>
           </cell>
           <cell r="X182">
             <v>15</v>
@@ -12142,7 +12153,7 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990015</v>
+            <v>55990012</v>
           </cell>
           <cell r="X183">
             <v>15</v>
@@ -12150,7 +12161,7 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990016</v>
+            <v>55990013</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -12158,33 +12169,57 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990101</v>
+            <v>55990014</v>
           </cell>
           <cell r="X185">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990102</v>
+            <v>55990015</v>
           </cell>
           <cell r="X186">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990103</v>
+            <v>55990016</v>
           </cell>
           <cell r="X187">
-            <v>35</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="188">
           <cell r="A188">
+            <v>55990101</v>
+          </cell>
+          <cell r="X188">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="A189">
+            <v>55990102</v>
+          </cell>
+          <cell r="X189">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="A190">
+            <v>55990103</v>
+          </cell>
+          <cell r="X190">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="A191">
             <v>55990104</v>
           </cell>
-          <cell r="X188">
+          <cell r="X191">
             <v>50</v>
           </cell>
         </row>
@@ -40088,7 +40123,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V115" sqref="V115"/>
+      <selection pane="bottomRight" activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40264,7 +40299,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -40428,7 +40463,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -40493,7 +40528,7 @@
         <v>714</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>724</v>
@@ -40592,7 +40627,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -41395,7 +41430,7 @@
         <v>325</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
@@ -41460,7 +41495,7 @@
         <v>11</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="Z9" s="37">
         <v>55100011</v>
@@ -41621,7 +41656,7 @@
         <v>12</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="Z10" s="37">
         <v>55900008</v>
@@ -41929,7 +41964,7 @@
         <v>16</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="Z12" s="37">
         <v>55100004</v>
@@ -42243,7 +42278,7 @@
         <v>6</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="Z14" s="37">
         <v>55110014</v>
@@ -43875,7 +43910,7 @@
         <v>329</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E25" s="4">
         <v>3</v>
@@ -43940,7 +43975,7 @@
         <v>31</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Z25" s="18">
         <v>55600010</v>
@@ -44407,7 +44442,7 @@
         <v>6</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="Z28" s="37">
         <v>55900007</v>
@@ -44564,7 +44599,7 @@
         <v>9</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Z29" s="37">
         <v>55100001</v>
@@ -44721,7 +44756,7 @@
         <v>12</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z30" s="18">
         <v>55500012</v>
@@ -45337,7 +45372,7 @@
         <v>16</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Z34" s="37">
         <v>55900006</v>
@@ -45584,13 +45619,13 @@
         <v>51000033</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="E36" s="4">
         <v>2</v>
@@ -45652,10 +45687,10 @@
         <v>0</v>
       </c>
       <c r="X36" s="4" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="Z36" s="37">
         <v>55300008</v>
@@ -45749,7 +45784,7 @@
         <v>494</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="E37" s="4">
         <v>2</v>
@@ -45814,7 +45849,7 @@
         <v>38</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="Z37" s="37">
         <v>55610003</v>
@@ -46361,13 +46396,13 @@
         <v>51000038</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="E41" s="4">
         <v>4</v>
@@ -46429,10 +46464,10 @@
         <v>0</v>
       </c>
       <c r="X41" s="4" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="Z41" s="37">
         <v>55100011</v>
@@ -46524,13 +46559,13 @@
         <v>51000039</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>409</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="E42" s="4">
         <v>3</v>
@@ -46595,7 +46630,7 @@
         <v>50</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="Z42" s="18">
         <v>55100011</v>
@@ -46752,7 +46787,7 @@
         <v>4</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="Z43" s="37">
         <v>55900004</v>
@@ -46846,7 +46881,7 @@
         <v>497</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="E44" s="4">
         <v>3</v>
@@ -46911,7 +46946,7 @@
         <v>16</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="Z44" s="18">
         <v>55900026</v>
@@ -47068,7 +47103,7 @@
         <v>4</v>
       </c>
       <c r="Y45" s="4" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="Z45" s="37">
         <v>55110013</v>
@@ -47225,7 +47260,7 @@
         <v>2</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Z46" s="37">
         <v>55510003</v>
@@ -47543,7 +47578,7 @@
         <v>16</v>
       </c>
       <c r="Y48" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="Z48" s="37">
         <v>55500009</v>
@@ -47702,7 +47737,7 @@
         <v>19</v>
       </c>
       <c r="Y49" s="4" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="Z49" s="37">
         <v>55100015</v>
@@ -47947,7 +47982,7 @@
         <v>335</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E51" s="4">
         <v>3</v>
@@ -48012,7 +48047,7 @@
         <v>9</v>
       </c>
       <c r="Y51" s="4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="Z51" s="37">
         <v>55900017</v>
@@ -48326,7 +48361,7 @@
         <v>16</v>
       </c>
       <c r="Y53" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="Z53" s="37">
         <v>55110006</v>
@@ -48420,7 +48455,7 @@
         <v>504</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E54" s="4">
         <v>3</v>
@@ -48485,7 +48520,7 @@
         <v>61</v>
       </c>
       <c r="Y54" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="Z54" s="37">
         <v>55100011</v>
@@ -48805,7 +48840,7 @@
         <v>4</v>
       </c>
       <c r="Y56" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="Z56" s="37">
         <v>55510003</v>
@@ -49374,7 +49409,7 @@
         <v>507</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E60" s="4">
         <v>3</v>
@@ -49439,7 +49474,7 @@
         <v>9</v>
       </c>
       <c r="Y60" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="Z60" s="37">
         <v>55900018</v>
@@ -49596,7 +49631,7 @@
         <v>24</v>
       </c>
       <c r="Y61" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="Z61" s="37">
         <v>55510007</v>
@@ -49753,7 +49788,7 @@
         <v>62</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="Z62" s="37">
         <v>55510002</v>
@@ -49910,7 +49945,7 @@
         <v>38</v>
       </c>
       <c r="Y63" s="4" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="Z63" s="37">
         <v>55510009</v>
@@ -50067,7 +50102,7 @@
         <v>24</v>
       </c>
       <c r="Y64" s="4" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="Z64" s="37">
         <v>55110010</v>
@@ -50473,7 +50508,7 @@
         <v>340</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="E67" s="4">
         <v>6</v>
@@ -50538,7 +50573,7 @@
         <v>75</v>
       </c>
       <c r="Y67" s="4" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="Z67" s="37">
         <v>55510010</v>
@@ -50632,7 +50667,7 @@
         <v>512</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="E68" s="4">
         <v>7</v>
@@ -50697,7 +50732,7 @@
         <v>75</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="Z68" s="37">
         <v>55300010</v>
@@ -50793,7 +50828,7 @@
         <v>341</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E69" s="4">
         <v>6</v>
@@ -50858,7 +50893,7 @@
         <v>40</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="Z69" s="18">
         <v>55200008</v>
@@ -51478,7 +51513,7 @@
         <v>728</v>
       </c>
       <c r="Y73" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Z73" s="37">
         <v>55510007</v>
@@ -51635,7 +51670,7 @@
         <v>6</v>
       </c>
       <c r="Y74" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z74" s="37">
         <v>55500012</v>
@@ -51729,7 +51764,7 @@
         <v>342</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E75" s="4">
         <v>2</v>
@@ -51794,7 +51829,7 @@
         <v>86</v>
       </c>
       <c r="Y75" s="4" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="Z75" s="37">
         <v>55500008</v>
@@ -51892,7 +51927,7 @@
         <v>518</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E76" s="4">
         <v>4</v>
@@ -51957,7 +51992,7 @@
         <v>12</v>
       </c>
       <c r="Y76" s="4" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="Z76" s="37">
         <v>55100001</v>
@@ -52118,7 +52153,7 @@
         <v>89</v>
       </c>
       <c r="Y77" s="4" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="Z77" s="37">
         <v>55110007</v>
@@ -52681,7 +52716,7 @@
         <v>344</v>
       </c>
       <c r="D81" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E81" s="4">
         <v>3</v>
@@ -52746,7 +52781,7 @@
         <v>2</v>
       </c>
       <c r="Y81" s="4" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="Z81" s="37">
         <v>55600014</v>
@@ -52903,7 +52938,7 @@
         <v>2</v>
       </c>
       <c r="Y82" s="4" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="Z82" s="37">
         <v>55100010</v>
@@ -53064,7 +53099,7 @@
         <v>38</v>
       </c>
       <c r="Y83" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="Z83" s="37">
         <v>55100010</v>
@@ -53635,7 +53670,7 @@
         <v>523</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="E87" s="4">
         <v>3</v>
@@ -53700,7 +53735,7 @@
         <v>83</v>
       </c>
       <c r="Y87" s="4" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="Z87" s="37">
         <v>55100011</v>
@@ -53861,7 +53896,7 @@
         <v>0</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Z88" s="37">
         <v>55200003</v>
@@ -54175,7 +54210,7 @@
         <v>103</v>
       </c>
       <c r="Y90" s="4" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="Z90" s="37">
         <v>55100002</v>
@@ -54273,7 +54308,7 @@
         <v>524</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E91" s="4">
         <v>3</v>
@@ -54338,7 +54373,7 @@
         <v>101</v>
       </c>
       <c r="Y91" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="Z91" s="37">
         <v>55600009</v>
@@ -54805,7 +54840,7 @@
         <v>75</v>
       </c>
       <c r="Y94" s="4" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="Z94" s="37">
         <v>55500008</v>
@@ -55117,7 +55152,7 @@
         <v>2</v>
       </c>
       <c r="Y96" s="4" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="Z96" s="37">
         <v>55500008</v>
@@ -55280,7 +55315,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="Z97" s="37">
         <v>55110007</v>
@@ -55445,7 +55480,7 @@
         <v>91</v>
       </c>
       <c r="Y98" s="4" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="Z98" s="37">
         <v>55510002</v>
@@ -55602,7 +55637,7 @@
         <v>727</v>
       </c>
       <c r="Y99" s="4" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="Z99" s="37">
         <v>55510010</v>
@@ -55759,7 +55794,7 @@
         <v>4</v>
       </c>
       <c r="Y100" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Z100" s="37">
         <v>55900016</v>
@@ -56067,7 +56102,7 @@
         <v>16</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Z102" s="37">
         <v>55900003</v>
@@ -56324,7 +56359,7 @@
         <v>350</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="E104" s="4">
         <v>3</v>
@@ -56389,7 +56424,7 @@
         <v>4</v>
       </c>
       <c r="Y104" s="4" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="Z104" s="37">
         <v>55100015</v>
@@ -56487,7 +56522,7 @@
         <v>536</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="E105" s="4">
         <v>2</v>
@@ -56552,7 +56587,7 @@
         <v>103</v>
       </c>
       <c r="Y105" s="4" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="Z105" s="37">
         <v>55900035</v>
@@ -56646,7 +56681,7 @@
         <v>537</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E106" s="4">
         <v>2</v>
@@ -56711,7 +56746,7 @@
         <v>9</v>
       </c>
       <c r="Y106" s="4" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="Z106" s="37">
         <v>55300009</v>
@@ -57027,7 +57062,7 @@
         <v>2</v>
       </c>
       <c r="Y108" s="4" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="Z108" s="37">
         <v>55900027</v>
@@ -57335,7 +57370,7 @@
         <v>126</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="Z110" s="37">
         <v>55510009</v>
@@ -57882,7 +57917,7 @@
         <v>542</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="E114" s="4">
         <v>7</v>
@@ -57947,7 +57982,7 @@
         <v>86</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="Z114" s="37">
         <v>55900039</v>
@@ -58063,7 +58098,7 @@
         <v>4</v>
       </c>
       <c r="I115" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J115" s="4">
         <v>0</v>
@@ -58112,7 +58147,7 @@
         <v>91</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="Z115" s="37">
         <v>55900041</v>
@@ -58208,7 +58243,7 @@
         <v>415</v>
       </c>
       <c r="D116" s="19" t="s">
-        <v>737</v>
+        <v>804</v>
       </c>
       <c r="E116" s="4">
         <v>7</v>
@@ -58221,19 +58256,19 @@
       </c>
       <c r="H116" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I116" s="4">
         <v>7</v>
       </c>
       <c r="J116" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K116" s="4">
-        <v>-8</v>
+        <v>20</v>
       </c>
       <c r="L116" s="7">
-        <v>1</v>
+        <v>-70</v>
       </c>
       <c r="M116" s="4">
         <v>0</v>
@@ -58258,7 +58293,7 @@
       </c>
       <c r="T116" s="12">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="U116" s="4">
         <v>10</v>
@@ -58273,10 +58308,14 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>952</v>
-      </c>
-      <c r="Z116" s="37"/>
-      <c r="AA116" s="18"/>
+        <v>1128</v>
+      </c>
+      <c r="Z116" s="37">
+        <v>55900044</v>
+      </c>
+      <c r="AA116" s="18">
+        <v>100</v>
+      </c>
       <c r="AB116" s="18">
         <v>55900020</v>
       </c>
@@ -58289,7 +58328,7 @@
         <f>IF(ISBLANK($Z116),0, LOOKUP($Z116,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA116/100)+
 IF(ISBLANK($AB116),0, LOOKUP($AB116,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC116/100)+
 IF(ISBLANK($AD116),0, LOOKUP($AD116,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE116/100)</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="AG116" s="18">
         <v>0</v>
@@ -58369,7 +58408,7 @@
         <v>533</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="E117" s="4">
         <v>7</v>
@@ -58434,7 +58473,7 @@
         <v>75</v>
       </c>
       <c r="Y117" s="4" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="Z117" s="37">
         <v>55400007</v>
@@ -58534,7 +58573,7 @@
         <v>543</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>737</v>
+        <v>1124</v>
       </c>
       <c r="E118" s="4">
         <v>7</v>
@@ -58547,19 +58586,19 @@
       </c>
       <c r="H118" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I118" s="4">
         <v>7</v>
       </c>
       <c r="J118" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K118" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L118" s="7">
-        <v>1</v>
+        <v>-45</v>
       </c>
       <c r="M118" s="4">
         <v>0</v>
@@ -58584,13 +58623,13 @@
       </c>
       <c r="T118" s="12">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="U118" s="4">
         <v>10</v>
       </c>
       <c r="V118" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="W118" s="4">
         <v>0</v>
@@ -58599,23 +58638,27 @@
         <v>40</v>
       </c>
       <c r="Y118" s="4" t="s">
-        <v>866</v>
-      </c>
-      <c r="Z118" s="37"/>
-      <c r="AA118" s="18"/>
+        <v>1125</v>
+      </c>
+      <c r="Z118" s="37">
+        <v>55900042</v>
+      </c>
+      <c r="AA118" s="18">
+        <v>100</v>
+      </c>
       <c r="AB118" s="18">
-        <v>55000099</v>
+        <v>55900020</v>
       </c>
       <c r="AC118" s="18">
         <v>100</v>
       </c>
       <c r="AD118" s="18"/>
       <c r="AE118" s="18"/>
-      <c r="AF118" s="18" t="e">
+      <c r="AF118" s="18">
         <f>IF(ISBLANK($Z118),0, LOOKUP($Z118,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA118/100)+
 IF(ISBLANK($AB118),0, LOOKUP($AB118,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC118/100)+
 IF(ISBLANK($AD118),0, LOOKUP($AD118,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE118/100)</f>
-        <v>#N/A</v>
+        <v>45</v>
       </c>
       <c r="AG118" s="18">
         <v>0</v>
@@ -58695,7 +58738,7 @@
         <v>672</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E119" s="8">
         <v>2</v>
@@ -58760,7 +58803,7 @@
         <v>6</v>
       </c>
       <c r="Y119" s="8" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z119" s="37">
         <v>55100014</v>
@@ -58854,7 +58897,7 @@
         <v>544</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>737</v>
+        <v>1127</v>
       </c>
       <c r="E120" s="4">
         <v>7</v>
@@ -58867,19 +58910,19 @@
       </c>
       <c r="H120" s="4">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I120" s="4">
         <v>7</v>
       </c>
       <c r="J120" s="4">
-        <v>14</v>
+        <v>-25</v>
       </c>
       <c r="K120" s="4">
         <v>0</v>
       </c>
       <c r="L120" s="7">
-        <v>1</v>
+        <v>-13</v>
       </c>
       <c r="M120" s="4">
         <v>0</v>
@@ -58904,7 +58947,7 @@
       </c>
       <c r="T120" s="12">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="U120" s="4">
         <v>10</v>
@@ -58919,10 +58962,14 @@
         <v>49</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>953</v>
-      </c>
-      <c r="Z120" s="37"/>
-      <c r="AA120" s="18"/>
+        <v>1126</v>
+      </c>
+      <c r="Z120" s="37">
+        <v>55900043</v>
+      </c>
+      <c r="AA120" s="18">
+        <v>100</v>
+      </c>
       <c r="AB120" s="18">
         <v>55900020</v>
       </c>
@@ -58935,7 +58982,7 @@
         <f>IF(ISBLANK($Z120),0, LOOKUP($Z120,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA120/100)+
 IF(ISBLANK($AB120),0, LOOKUP($AB120,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC120/100)+
 IF(ISBLANK($AD120),0, LOOKUP($AD120,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE120/100)</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="AG120" s="18">
         <v>0</v>
@@ -59015,7 +59062,7 @@
         <v>545</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="E121" s="4">
         <v>7</v>
@@ -59080,7 +59127,7 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="Z121" s="37">
         <v>55900040</v>
@@ -59394,7 +59441,7 @@
         <v>4</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="Z123" s="37">
         <v>55100005</v>
@@ -59710,7 +59757,7 @@
         <v>2</v>
       </c>
       <c r="Y125" s="4" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="Z125" s="37">
         <v>55100010</v>
@@ -59808,7 +59855,7 @@
         <v>355</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="E126" s="4">
         <v>1</v>
@@ -59873,7 +59920,7 @@
         <v>24</v>
       </c>
       <c r="Y126" s="4" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="Z126" s="37">
         <v>55600012</v>
@@ -60030,7 +60077,7 @@
         <v>4</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="Z127" s="37">
         <v>55110005</v>
@@ -60124,7 +60171,7 @@
         <v>550</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E128" s="4">
         <v>2</v>
@@ -60189,7 +60236,7 @@
         <v>4</v>
       </c>
       <c r="Y128" s="4" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="Z128" s="37">
         <v>55900019</v>
@@ -60434,7 +60481,7 @@
         <v>552</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="E130" s="4">
         <v>1</v>
@@ -60499,7 +60546,7 @@
         <v>103</v>
       </c>
       <c r="Y130" s="4" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="Z130" s="37">
         <v>55900024</v>
@@ -60807,7 +60854,7 @@
         <v>4</v>
       </c>
       <c r="Y132" s="4" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Z132" s="37">
         <v>55100007</v>
@@ -60964,7 +61011,7 @@
         <v>103</v>
       </c>
       <c r="Y133" s="4" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="Z133" s="37">
         <v>55900027</v>
@@ -61125,7 +61172,7 @@
         <v>2</v>
       </c>
       <c r="Y134" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Z134" s="37">
         <v>55900008</v>
@@ -61286,7 +61333,7 @@
         <v>75</v>
       </c>
       <c r="Y135" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Z135" s="37">
         <v>55900016</v>
@@ -61443,7 +61490,7 @@
         <v>103</v>
       </c>
       <c r="Y136" s="4" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="Z136" s="37">
         <v>55110005</v>
@@ -61600,7 +61647,7 @@
         <v>2</v>
       </c>
       <c r="Y137" s="4" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="Z137" s="37">
         <v>55510010</v>
@@ -61761,7 +61808,7 @@
         <v>6</v>
       </c>
       <c r="Y138" s="4" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="Z138" s="37">
         <v>55100006</v>
@@ -62530,7 +62577,7 @@
         <v>4</v>
       </c>
       <c r="Y143" s="4" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="Z143" s="18">
         <v>55110015</v>
@@ -62687,7 +62734,7 @@
         <v>16</v>
       </c>
       <c r="Y144" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Z144" s="37">
         <v>55510004</v>
@@ -62997,7 +63044,7 @@
         <v>103</v>
       </c>
       <c r="Y146" s="4" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="Z146" s="37">
         <v>55110007</v>
@@ -63095,7 +63142,7 @@
         <v>360</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="E147" s="4">
         <v>3</v>
@@ -63160,7 +63207,7 @@
         <v>19</v>
       </c>
       <c r="Y147" s="4" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="Z147" s="18">
         <v>55510006</v>
@@ -63254,7 +63301,7 @@
         <v>470</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E148" s="4">
         <v>2</v>
@@ -63319,7 +63366,7 @@
         <v>731</v>
       </c>
       <c r="Y148" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="Z148" s="37">
         <v>55100012</v>
@@ -63417,7 +63464,7 @@
         <v>361</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="E149" s="4">
         <v>3</v>
@@ -63482,7 +63529,7 @@
         <v>162</v>
       </c>
       <c r="Y149" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="Z149" s="37">
         <v>55100011</v>
@@ -63643,7 +63690,7 @@
         <v>4</v>
       </c>
       <c r="Y150" s="4" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="Z150" s="37">
         <v>55500005</v>
@@ -64349,7 +64396,7 @@
         <v>568</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="E155" s="4">
         <v>3</v>
@@ -64414,7 +64461,7 @@
         <v>735</v>
       </c>
       <c r="Y155" s="4" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="Z155" s="37">
         <v>55100013</v>
@@ -64571,7 +64618,7 @@
         <v>4</v>
       </c>
       <c r="Y156" s="4" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="Z156" s="37">
         <v>55110004</v>
@@ -65489,7 +65536,7 @@
         <v>103</v>
       </c>
       <c r="Y162" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="Z162" s="37">
         <v>55110010</v>
@@ -65583,7 +65630,7 @@
         <v>575</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E163" s="4">
         <v>3</v>
@@ -65648,7 +65695,7 @@
         <v>103</v>
       </c>
       <c r="Y163" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="Z163" s="37">
         <v>55900010</v>
@@ -65805,7 +65852,7 @@
         <v>16</v>
       </c>
       <c r="Y164" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="Z164" s="37">
         <v>55110005</v>
@@ -66984,7 +67031,7 @@
         <v>579</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="E172" s="4">
         <v>4</v>
@@ -67049,7 +67096,7 @@
         <v>4</v>
       </c>
       <c r="Y172" s="4" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="Z172" s="37">
         <v>55510018</v>
@@ -67147,7 +67194,7 @@
         <v>580</v>
       </c>
       <c r="D173" s="19" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="E173" s="4">
         <v>2</v>
@@ -67212,7 +67259,7 @@
         <v>729</v>
       </c>
       <c r="Y173" s="4" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="Z173" s="37">
         <v>55200004</v>
@@ -67465,7 +67512,7 @@
         <v>582</v>
       </c>
       <c r="D175" s="19" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E175" s="4">
         <v>2</v>
@@ -67530,7 +67577,7 @@
         <v>2</v>
       </c>
       <c r="Y175" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Z175" s="37">
         <v>55700003</v>
@@ -67691,7 +67738,7 @@
         <v>12</v>
       </c>
       <c r="Y176" s="4" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="Z176" s="37">
         <v>55610003</v>
@@ -67944,7 +67991,7 @@
         <v>584</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="E178" s="4">
         <v>4</v>
@@ -68009,7 +68056,7 @@
         <v>4</v>
       </c>
       <c r="Y178" s="4" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="Z178" s="37">
         <v>55510004</v>
@@ -68166,7 +68213,7 @@
         <v>2</v>
       </c>
       <c r="Y179" s="4" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="Z179" s="37">
         <v>55110005</v>
@@ -68323,7 +68370,7 @@
         <v>62</v>
       </c>
       <c r="Y180" s="4" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="Z180" s="18">
         <v>55900023</v>
@@ -68421,7 +68468,7 @@
         <v>586</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="E181" s="4">
         <v>5</v>
@@ -68486,7 +68533,7 @@
         <v>654</v>
       </c>
       <c r="Y181" s="4" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="Z181" s="37">
         <v>55200012</v>
@@ -68647,7 +68694,7 @@
         <v>4</v>
       </c>
       <c r="Y182" s="4" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="Z182" s="37">
         <v>55610003</v>
@@ -68804,7 +68851,7 @@
         <v>16</v>
       </c>
       <c r="Y183" s="4" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="Z183" s="37">
         <v>55900031</v>
@@ -68902,7 +68949,7 @@
         <v>589</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="E184" s="4">
         <v>3</v>
@@ -68967,7 +69014,7 @@
         <v>75</v>
       </c>
       <c r="Y184" s="4" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Z184" s="37">
         <v>55510010</v>
@@ -69061,7 +69108,7 @@
         <v>367</v>
       </c>
       <c r="D185" s="19" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="E185" s="4">
         <v>6</v>
@@ -69126,7 +69173,7 @@
         <v>12</v>
       </c>
       <c r="Y185" s="4" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="Z185" s="37">
         <v>55600011</v>
@@ -69224,7 +69271,7 @@
         <v>590</v>
       </c>
       <c r="D186" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E186" s="4">
         <v>4</v>
@@ -69289,7 +69336,7 @@
         <v>75</v>
       </c>
       <c r="Y186" s="4" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="Z186" s="37">
         <v>55600016</v>
@@ -69754,7 +69801,7 @@
         <v>4</v>
       </c>
       <c r="Y189" s="4" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z189" s="37">
         <v>55510012</v>
@@ -70064,7 +70111,7 @@
         <v>24</v>
       </c>
       <c r="Y191" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="Z191" s="37">
         <v>55900004</v>
@@ -70225,7 +70272,7 @@
         <v>730</v>
       </c>
       <c r="Y192" s="4" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="Z192" s="37">
         <v>55110001</v>
@@ -70323,7 +70370,7 @@
         <v>596</v>
       </c>
       <c r="D193" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E193" s="4">
         <v>5</v>
@@ -70388,7 +70435,7 @@
         <v>2</v>
       </c>
       <c r="Y193" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="Z193" s="37">
         <v>55100011</v>
@@ -70486,7 +70533,7 @@
         <v>597</v>
       </c>
       <c r="D194" s="19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E194" s="4">
         <v>5</v>
@@ -70551,7 +70598,7 @@
         <v>16</v>
       </c>
       <c r="Y194" s="4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Z194" s="37">
         <v>55900014</v>
@@ -70649,7 +70696,7 @@
         <v>598</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="E195" s="4">
         <v>5</v>
@@ -70714,7 +70761,7 @@
         <v>204</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="Z195" s="18">
         <v>55100011</v>
@@ -70812,7 +70859,7 @@
         <v>599</v>
       </c>
       <c r="D196" s="19" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="E196" s="4">
         <v>5</v>
@@ -70877,7 +70924,7 @@
         <v>4</v>
       </c>
       <c r="Y196" s="4" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="Z196" s="18">
         <v>55520003</v>
@@ -70975,7 +71022,7 @@
         <v>600</v>
       </c>
       <c r="D197" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E197" s="4">
         <v>5</v>
@@ -71040,7 +71087,7 @@
         <v>4</v>
       </c>
       <c r="Y197" s="4" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="Z197" s="18">
         <v>55600008</v>
@@ -71201,7 +71248,7 @@
         <v>22</v>
       </c>
       <c r="Y198" s="4" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="Z198" s="37">
         <v>55100004</v>
@@ -71299,7 +71346,7 @@
         <v>602</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="E199" s="4">
         <v>5</v>
@@ -71364,7 +71411,7 @@
         <v>2</v>
       </c>
       <c r="Y199" s="4" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="Z199" s="37">
         <v>55100010</v>
@@ -71525,7 +71572,7 @@
         <v>4</v>
       </c>
       <c r="Y200" s="4" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="Z200" s="37">
         <v>55110008</v>
@@ -71998,7 +72045,7 @@
         <v>16</v>
       </c>
       <c r="Y203" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="Z203" s="37">
         <v>55110011</v>
@@ -72092,7 +72139,7 @@
         <v>673</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E204" s="8">
         <v>3</v>
@@ -72157,7 +72204,7 @@
         <v>6</v>
       </c>
       <c r="Y204" s="8" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z204" s="37">
         <v>55100014</v>
@@ -72251,7 +72298,7 @@
         <v>604</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="E205" s="4">
         <v>2</v>
@@ -72316,7 +72363,7 @@
         <v>734</v>
       </c>
       <c r="Y205" s="4" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="Z205" s="37">
         <v>55510013</v>
@@ -72634,7 +72681,7 @@
         <v>168</v>
       </c>
       <c r="Y207" s="4" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="Z207" s="37">
         <v>55900029</v>
@@ -72950,7 +72997,7 @@
         <v>2</v>
       </c>
       <c r="Y209" s="4" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="Z209" s="37">
         <v>55510003</v>
@@ -73417,7 +73464,7 @@
         <v>128</v>
       </c>
       <c r="Y212" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="Z212" s="18">
         <v>55510013</v>
@@ -73511,7 +73558,7 @@
         <v>609</v>
       </c>
       <c r="D213" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E213" s="4">
         <v>4</v>
@@ -73576,7 +73623,7 @@
         <v>812</v>
       </c>
       <c r="Y213" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="Z213" s="18">
         <v>55900005</v>
@@ -73825,7 +73872,7 @@
         <v>611</v>
       </c>
       <c r="D215" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E215" s="4">
         <v>4</v>
@@ -73890,7 +73937,7 @@
         <v>185</v>
       </c>
       <c r="Y215" s="4" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="Z215" s="37">
         <v>55100001</v>
@@ -74051,7 +74098,7 @@
         <v>6</v>
       </c>
       <c r="Y216" s="4" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="Z216" s="37">
         <v>55900031</v>
@@ -74304,7 +74351,7 @@
         <v>613</v>
       </c>
       <c r="D218" s="19" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="E218" s="4">
         <v>2</v>
@@ -74369,7 +74416,7 @@
         <v>4</v>
       </c>
       <c r="Y218" s="4" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="Z218" s="37">
         <v>55900034</v>
@@ -74463,7 +74510,7 @@
         <v>614</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="E219" s="4">
         <v>3</v>
@@ -74528,7 +74575,7 @@
         <v>733</v>
       </c>
       <c r="Y219" s="4" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="Z219" s="37">
         <v>55510019</v>
@@ -74685,7 +74732,7 @@
         <v>62</v>
       </c>
       <c r="Y220" s="4" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="Z220" s="37">
         <v>55100001</v>
@@ -74779,7 +74826,7 @@
         <v>615</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E221" s="4">
         <v>4</v>
@@ -74844,7 +74891,7 @@
         <v>231</v>
       </c>
       <c r="Y221" s="4" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="Z221" s="37">
         <v>55200009</v>
@@ -75005,7 +75052,7 @@
         <v>6</v>
       </c>
       <c r="Y222" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="Z222" s="37">
         <v>55900005</v>
@@ -75162,7 +75209,7 @@
         <v>9</v>
       </c>
       <c r="Y223" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="Z223" s="37">
         <v>55100008</v>
@@ -75319,7 +75366,7 @@
         <v>103</v>
       </c>
       <c r="Y224" s="7" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="Z224" s="37">
         <v>55900016</v>
@@ -75480,7 +75527,7 @@
         <v>16</v>
       </c>
       <c r="Y225" s="4" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="Z225" s="37">
         <v>55610002</v>
@@ -75800,7 +75847,7 @@
         <v>168</v>
       </c>
       <c r="Y227" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="Z227" s="37">
         <v>55110012</v>
@@ -75894,7 +75941,7 @@
         <v>429</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="E228" s="4">
         <v>3</v>
@@ -75959,7 +76006,7 @@
         <v>239</v>
       </c>
       <c r="Y228" s="4" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="Z228" s="37">
         <v>55510001</v>
@@ -76053,7 +76100,7 @@
         <v>375</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="E229" s="4">
         <v>2</v>
@@ -76118,7 +76165,7 @@
         <v>24</v>
       </c>
       <c r="Y229" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="Z229" s="37">
         <v>55510007</v>
@@ -76683,7 +76730,7 @@
         <v>376</v>
       </c>
       <c r="D233" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E233" s="4">
         <v>3</v>
@@ -76748,7 +76795,7 @@
         <v>245</v>
       </c>
       <c r="Y233" s="4" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="Z233" s="37">
         <v>55100009</v>
@@ -76909,7 +76956,7 @@
         <v>22</v>
       </c>
       <c r="Y234" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="Z234" s="37">
         <v>55110009</v>
@@ -77003,7 +77050,7 @@
         <v>623</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E235" s="4">
         <v>3</v>
@@ -77068,7 +77115,7 @@
         <v>6</v>
       </c>
       <c r="Y235" s="4" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="Z235" s="18">
         <v>55600013</v>
@@ -77162,7 +77209,7 @@
         <v>624</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E236" s="4">
         <v>2</v>
@@ -77227,7 +77274,7 @@
         <v>12</v>
       </c>
       <c r="Y236" s="4" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="Z236" s="37">
         <v>55600013</v>
@@ -77384,7 +77431,7 @@
         <v>2</v>
       </c>
       <c r="Y237" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="Z237" s="37">
         <v>55100001</v>
@@ -77696,7 +77743,7 @@
         <v>4</v>
       </c>
       <c r="Y239" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="Z239" s="37">
         <v>55110001</v>
@@ -77945,7 +77992,7 @@
         <v>435</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="E241" s="4">
         <v>5</v>
@@ -78010,7 +78057,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="Z241" s="37">
         <v>55100010</v>
@@ -78326,7 +78373,7 @@
         <v>66</v>
       </c>
       <c r="Y243" s="4" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="Z243" s="37">
         <v>55900033</v>
@@ -78420,7 +78467,7 @@
         <v>378</v>
       </c>
       <c r="D244" s="19" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="E244" s="4">
         <v>3</v>
@@ -78485,7 +78532,7 @@
         <v>2</v>
       </c>
       <c r="Y244" s="4" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="Z244" s="37">
         <v>55510014</v>
@@ -78579,7 +78626,7 @@
         <v>379</v>
       </c>
       <c r="D245" s="19" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="E245" s="4">
         <v>6</v>
@@ -78644,7 +78691,7 @@
         <v>66</v>
       </c>
       <c r="Y245" s="4" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="Z245" s="37">
         <v>55510014</v>
@@ -78956,7 +79003,7 @@
         <v>2</v>
       </c>
       <c r="Y247" s="4" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="Z247" s="37">
         <v>55510010</v>
@@ -79117,7 +79164,7 @@
         <v>19</v>
       </c>
       <c r="Y248" s="4" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="Z248" s="37">
         <v>55900025</v>
@@ -79425,7 +79472,7 @@
         <v>2</v>
       </c>
       <c r="Y250" s="4" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="Z250" s="37">
         <v>55510009</v>
@@ -79586,7 +79633,7 @@
         <v>4</v>
       </c>
       <c r="Y251" s="4" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="Z251" s="18">
         <v>55900030</v>
@@ -79743,7 +79790,7 @@
         <v>131</v>
       </c>
       <c r="Y252" s="4" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="Z252" s="18">
         <v>55110007</v>
@@ -79900,7 +79947,7 @@
         <v>19</v>
       </c>
       <c r="Y253" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="Z253" s="37">
         <v>55900015</v>
@@ -79994,7 +80041,7 @@
         <v>380</v>
       </c>
       <c r="D254" s="19" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E254" s="4">
         <v>3</v>
@@ -80059,7 +80106,7 @@
         <v>204</v>
       </c>
       <c r="Y254" s="4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Z254" s="18">
         <v>55100013</v>
@@ -80153,7 +80200,7 @@
         <v>381</v>
       </c>
       <c r="D255" s="19" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="E255" s="4">
         <v>4</v>
@@ -80218,7 +80265,7 @@
         <v>0</v>
       </c>
       <c r="Y255" s="4" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="Z255" s="37">
         <v>55510018</v>
@@ -80379,7 +80426,7 @@
         <v>4</v>
       </c>
       <c r="Y256" s="4" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="Z256" s="37">
         <v>55110005</v>
@@ -80473,7 +80520,7 @@
         <v>630</v>
       </c>
       <c r="D257" s="19" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="E257" s="4">
         <v>3</v>
@@ -80538,7 +80585,7 @@
         <v>2</v>
       </c>
       <c r="Y257" s="4" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="Z257" s="37">
         <v>55200013</v>
@@ -80629,7 +80676,7 @@
         <v>259</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="D258" s="19"/>
       <c r="E258" s="4">
@@ -80695,7 +80742,7 @@
         <v>245</v>
       </c>
       <c r="Y258" s="4" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="Z258" s="37">
         <v>55410001</v>
@@ -80793,7 +80840,7 @@
         <v>631</v>
       </c>
       <c r="D259" s="19" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="E259" s="4">
         <v>2</v>
@@ -80858,7 +80905,7 @@
         <v>4</v>
       </c>
       <c r="Y259" s="7" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="Z259" s="37">
         <v>55100012</v>
@@ -80956,7 +81003,7 @@
         <v>383</v>
       </c>
       <c r="D260" s="19" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="E260" s="4">
         <v>3</v>
@@ -81021,7 +81068,7 @@
         <v>6</v>
       </c>
       <c r="Y260" s="4" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="Z260" s="37">
         <v>55900010</v>
@@ -81119,7 +81166,7 @@
         <v>384</v>
       </c>
       <c r="D261" s="19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E261" s="4">
         <v>3</v>
@@ -81184,7 +81231,7 @@
         <v>16</v>
       </c>
       <c r="Y261" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="Z261" s="37">
         <v>55900014</v>
@@ -81651,7 +81698,7 @@
         <v>4</v>
       </c>
       <c r="Y264" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Z264" s="37">
         <v>55100005</v>
@@ -81808,7 +81855,7 @@
         <v>2</v>
       </c>
       <c r="Y265" s="4" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="Z265" s="37">
         <v>55110007</v>
@@ -81965,7 +82012,7 @@
         <v>24</v>
       </c>
       <c r="Y266" s="4" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="Z266" s="37">
         <v>55900031</v>
@@ -82059,7 +82106,7 @@
         <v>388</v>
       </c>
       <c r="D267" s="19" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="E267" s="4">
         <v>5</v>
@@ -82124,7 +82171,7 @@
         <v>91</v>
       </c>
       <c r="Y267" s="4" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="Z267" s="37">
         <v>55510001</v>
@@ -82285,7 +82332,7 @@
         <v>16</v>
       </c>
       <c r="Y268" s="4" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="Z268" s="37">
         <v>55900031</v>
@@ -82599,7 +82646,7 @@
         <v>16</v>
       </c>
       <c r="Y270" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="Z270" s="37">
         <v>55100008</v>
@@ -82693,7 +82740,7 @@
         <v>390</v>
       </c>
       <c r="D271" s="19" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="E271" s="4">
         <v>5</v>
@@ -82758,7 +82805,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="Z271" s="18">
         <v>55100012</v>
@@ -82856,7 +82903,7 @@
         <v>632</v>
       </c>
       <c r="D272" s="19" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="E272" s="4">
         <v>5</v>
@@ -82921,7 +82968,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="Z272" s="18">
         <v>55100012</v>
@@ -83019,7 +83066,7 @@
         <v>391</v>
       </c>
       <c r="D273" s="19" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="E273" s="4">
         <v>5</v>
@@ -83084,7 +83131,7 @@
         <v>736</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="Z273" s="18">
         <v>55100012</v>
@@ -83245,7 +83292,7 @@
         <v>0</v>
       </c>
       <c r="Y274" s="4" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="Z274" s="37">
         <v>55200003</v>
@@ -83404,7 +83451,7 @@
         <v>271</v>
       </c>
       <c r="Y275" s="4" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="Z275" s="37">
         <v>55700005</v>
@@ -83649,7 +83696,7 @@
         <v>460</v>
       </c>
       <c r="D277" s="19" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="E277" s="4">
         <v>3</v>
@@ -83714,7 +83761,7 @@
         <v>75</v>
       </c>
       <c r="Y277" s="4" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="Z277" s="18">
         <v>55310003</v>
@@ -83871,7 +83918,7 @@
         <v>4</v>
       </c>
       <c r="Y278" s="4" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="Z278" s="18">
         <v>55110016</v>
@@ -84032,7 +84079,7 @@
         <v>4</v>
       </c>
       <c r="Y279" s="7" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="Z279" s="37">
         <v>55900022</v>
@@ -84189,7 +84236,7 @@
         <v>16</v>
       </c>
       <c r="Y280" s="4" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="Z280" s="37">
         <v>55110019</v>
@@ -84283,7 +84330,7 @@
         <v>393</v>
       </c>
       <c r="D281" s="19" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="E281" s="4">
         <v>1</v>
@@ -84348,7 +84395,7 @@
         <v>9</v>
       </c>
       <c r="Y281" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z281" s="37">
         <v>55900009</v>
@@ -84442,7 +84489,7 @@
         <v>394</v>
       </c>
       <c r="D282" s="19" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="E282" s="4">
         <v>1</v>
@@ -84507,7 +84554,7 @@
         <v>6</v>
       </c>
       <c r="Y282" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z282" s="37">
         <v>55900009</v>
@@ -84601,7 +84648,7 @@
         <v>395</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="E283" s="4">
         <v>1</v>
@@ -84666,7 +84713,7 @@
         <v>16</v>
       </c>
       <c r="Y283" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z283" s="37">
         <v>55900009</v>
@@ -84825,7 +84872,7 @@
         <v>6</v>
       </c>
       <c r="Y284" s="4" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="Z284" s="37">
         <v>55200010</v>
@@ -84919,7 +84966,7 @@
         <v>636</v>
       </c>
       <c r="D285" s="19" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="E285" s="4">
         <v>6</v>
@@ -84984,7 +85031,7 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="Z285" s="37">
         <v>55900038</v>
@@ -85294,7 +85341,7 @@
         <v>16</v>
       </c>
       <c r="Y287" s="4" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="Z287" s="37">
         <v>55110017</v>
@@ -85451,7 +85498,7 @@
         <v>0</v>
       </c>
       <c r="Y288" s="8" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="Z288" s="37">
         <v>55200003</v>
@@ -85539,13 +85586,13 @@
         <v>51000286</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C289" s="53" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="D289" s="19" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="E289" s="4">
         <v>2</v>
@@ -85610,7 +85657,7 @@
         <v>97</v>
       </c>
       <c r="Y289" s="4" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="Z289" s="37">
         <v>55510011</v>
@@ -85704,7 +85751,7 @@
         <v>674</v>
       </c>
       <c r="D290" s="19" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E290" s="8">
         <v>4</v>
@@ -85769,7 +85816,7 @@
         <v>75</v>
       </c>
       <c r="Y290" s="8" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="Z290" s="37">
         <v>55100014</v>
@@ -85930,7 +85977,7 @@
         <v>75</v>
       </c>
       <c r="Y291" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="Z291" s="37">
         <v>55510010</v>
@@ -86022,10 +86069,10 @@
         <v>51000289</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="D292" s="19" t="s">
         <v>815</v>
@@ -86090,10 +86137,10 @@
         <v>0</v>
       </c>
       <c r="X292" s="4" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="Y292" s="4" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="Z292" s="37">
         <v>55900032</v>
@@ -86181,10 +86228,10 @@
         <v>51000290</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="D293" s="19" t="s">
         <v>815</v>
@@ -86249,10 +86296,10 @@
         <v>0</v>
       </c>
       <c r="X293" s="4" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="Y293" s="4" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="Z293" s="37">
         <v>55900032</v>
@@ -86346,7 +86393,7 @@
         <v>635</v>
       </c>
       <c r="D294" s="19" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="E294" s="4">
         <v>3</v>
@@ -86411,7 +86458,7 @@
         <v>204</v>
       </c>
       <c r="Y294" s="4" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="Z294" s="37">
         <v>55200005</v>
@@ -86572,7 +86619,7 @@
         <v>675</v>
       </c>
       <c r="Y295" s="4" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="Z295" s="37">
         <v>55900028</v>
@@ -86666,7 +86713,7 @@
         <v>663</v>
       </c>
       <c r="D296" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E296" s="8">
         <v>2</v>
@@ -86731,7 +86778,7 @@
         <v>75</v>
       </c>
       <c r="Y296" s="8" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Z296" s="37">
         <v>55100012</v>
@@ -86825,7 +86872,7 @@
         <v>396</v>
       </c>
       <c r="D297" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E297" s="4">
         <v>3</v>
@@ -86890,7 +86937,7 @@
         <v>44</v>
       </c>
       <c r="Y297" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Z297" s="37">
         <v>55900011</v>
@@ -86984,7 +87031,7 @@
         <v>397</v>
       </c>
       <c r="D298" s="19" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E298" s="4">
         <v>2</v>
@@ -87049,7 +87096,7 @@
         <v>2</v>
       </c>
       <c r="Y298" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="Z298" s="37">
         <v>55900012</v>
@@ -87457,7 +87504,7 @@
         <v>638</v>
       </c>
       <c r="D301" s="8" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E301" s="4">
         <v>5</v>
@@ -87522,7 +87569,7 @@
         <v>107</v>
       </c>
       <c r="Y301" s="4" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="Z301" s="18">
         <v>55200007</v>
@@ -87836,7 +87883,7 @@
         <v>794</v>
       </c>
       <c r="AV1" s="48" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="AW1" s="14" t="s">
         <v>317</v>
@@ -88000,7 +88047,7 @@
         <v>795</v>
       </c>
       <c r="AV2" s="49" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>286</v>
@@ -88164,7 +88211,7 @@
         <v>796</v>
       </c>
       <c r="AV3" s="11" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>300</v>
@@ -88341,10 +88388,10 @@
         <v>51013001</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8">
@@ -88410,7 +88457,7 @@
         <v>9</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="Z5" s="18">
         <v>55510010</v>
@@ -88649,10 +88696,10 @@
         <v>51013003</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="4">
@@ -88800,10 +88847,10 @@
         <v>51013004</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="4">
@@ -90440,7 +90487,7 @@
         <v>666</v>
       </c>
       <c r="B1" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -90501,7 +90548,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -90509,7 +90556,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="24" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
@@ -90517,7 +90564,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B11" s="22"/>
     </row>

</xml_diff>

<commit_message>
fix the chao warrior
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -4444,10 +4444,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>55100010;100|55110006;100|55110007;100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>魔法</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4589,6 +4585,10 @@
   </si>
   <si>
     <t>55900045;100|55100008;100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55100010;100|55110020;100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8856,11 +8856,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="229272160"/>
-        <c:axId val="229276080"/>
+        <c:axId val="341837728"/>
+        <c:axId val="341829568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="229272160"/>
+        <c:axId val="341837728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8903,7 +8903,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229276080"/>
+        <c:crossAx val="341829568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8911,7 +8911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229276080"/>
+        <c:axId val="341829568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8962,7 +8962,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229272160"/>
+        <c:crossAx val="341837728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9332,11 +9332,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="229280560"/>
-        <c:axId val="229281120"/>
+        <c:axId val="341828480"/>
+        <c:axId val="341837184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="229280560"/>
+        <c:axId val="341828480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9379,7 +9379,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229281120"/>
+        <c:crossAx val="341837184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9387,7 +9387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229281120"/>
+        <c:axId val="341837184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9438,7 +9438,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229280560"/>
+        <c:crossAx val="341828480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10992,7 +10992,7 @@
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55200001</v>
+            <v>55110020</v>
           </cell>
           <cell r="X38">
             <v>40</v>
@@ -11000,39 +11000,39 @@
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55200002</v>
+            <v>55200001</v>
           </cell>
           <cell r="X39">
-            <v>15</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55200003</v>
+            <v>55200002</v>
           </cell>
           <cell r="X40">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55200004</v>
+            <v>55200003</v>
           </cell>
           <cell r="X41">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55200005</v>
+            <v>55200004</v>
           </cell>
           <cell r="X42">
-            <v>20</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55200006</v>
+            <v>55200005</v>
           </cell>
           <cell r="X43">
             <v>20</v>
@@ -11040,7 +11040,7 @@
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55200007</v>
+            <v>55200006</v>
           </cell>
           <cell r="X44">
             <v>20</v>
@@ -11048,15 +11048,15 @@
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55200008</v>
+            <v>55200007</v>
           </cell>
           <cell r="X45">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55200009</v>
+            <v>55200008</v>
           </cell>
           <cell r="X46">
             <v>25</v>
@@ -11064,7 +11064,7 @@
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55200010</v>
+            <v>55200009</v>
           </cell>
           <cell r="X47">
             <v>25</v>
@@ -11072,55 +11072,55 @@
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55200011</v>
+            <v>55200010</v>
           </cell>
           <cell r="X48">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55200012</v>
+            <v>55200011</v>
           </cell>
           <cell r="X49">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55200013</v>
+            <v>55200012</v>
           </cell>
           <cell r="X50">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55200014</v>
+            <v>55200013</v>
           </cell>
           <cell r="X51">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55300001</v>
+            <v>55200014</v>
           </cell>
           <cell r="X52">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55300002</v>
+            <v>55300001</v>
           </cell>
           <cell r="X53">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55300003</v>
+            <v>55300002</v>
           </cell>
           <cell r="X54">
             <v>30</v>
@@ -11128,7 +11128,7 @@
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55300004</v>
+            <v>55300003</v>
           </cell>
           <cell r="X55">
             <v>30</v>
@@ -11136,7 +11136,7 @@
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55300005</v>
+            <v>55300004</v>
           </cell>
           <cell r="X56">
             <v>30</v>
@@ -11144,15 +11144,15 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55300006</v>
+            <v>55300005</v>
           </cell>
           <cell r="X57">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55300007</v>
+            <v>55300006</v>
           </cell>
           <cell r="X58">
             <v>25</v>
@@ -11160,15 +11160,15 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55300008</v>
+            <v>55300007</v>
           </cell>
           <cell r="X59">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55300009</v>
+            <v>55300008</v>
           </cell>
           <cell r="X60">
             <v>30</v>
@@ -11176,47 +11176,47 @@
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55300010</v>
+            <v>55300009</v>
           </cell>
           <cell r="X61">
-            <v>35</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55310001</v>
+            <v>55300010</v>
           </cell>
           <cell r="X62">
-            <v>100</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55310002</v>
+            <v>55310001</v>
           </cell>
           <cell r="X63">
-            <v>15</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55310003</v>
+            <v>55310002</v>
           </cell>
           <cell r="X64">
-            <v>13</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55400001</v>
+            <v>55310003</v>
           </cell>
           <cell r="X65">
-            <v>80</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55400002</v>
+            <v>55400001</v>
           </cell>
           <cell r="X66">
             <v>80</v>
@@ -11224,7 +11224,7 @@
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55400003</v>
+            <v>55400002</v>
           </cell>
           <cell r="X67">
             <v>80</v>
@@ -11232,7 +11232,7 @@
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55400004</v>
+            <v>55400003</v>
           </cell>
           <cell r="X68">
             <v>80</v>
@@ -11240,47 +11240,47 @@
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55400005</v>
+            <v>55400004</v>
           </cell>
           <cell r="X69">
-            <v>55</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55400006</v>
+            <v>55400005</v>
           </cell>
           <cell r="X70">
-            <v>30</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55400007</v>
+            <v>55400006</v>
           </cell>
           <cell r="X71">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55410001</v>
+            <v>55400007</v>
           </cell>
           <cell r="X72">
-            <v>50</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55500001</v>
+            <v>55410001</v>
           </cell>
           <cell r="X73">
-            <v>5</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55500002</v>
+            <v>55500001</v>
           </cell>
           <cell r="X74">
             <v>5</v>
@@ -11288,7 +11288,7 @@
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55500003</v>
+            <v>55500002</v>
           </cell>
           <cell r="X75">
             <v>5</v>
@@ -11296,7 +11296,7 @@
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55500004</v>
+            <v>55500003</v>
           </cell>
           <cell r="X76">
             <v>5</v>
@@ -11304,7 +11304,7 @@
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55500005</v>
+            <v>55500004</v>
           </cell>
           <cell r="X77">
             <v>5</v>
@@ -11312,7 +11312,7 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55500006</v>
+            <v>55500005</v>
           </cell>
           <cell r="X78">
             <v>5</v>
@@ -11320,7 +11320,7 @@
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55500007</v>
+            <v>55500006</v>
           </cell>
           <cell r="X79">
             <v>5</v>
@@ -11328,7 +11328,7 @@
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55500008</v>
+            <v>55500007</v>
           </cell>
           <cell r="X80">
             <v>5</v>
@@ -11336,7 +11336,7 @@
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55500009</v>
+            <v>55500008</v>
           </cell>
           <cell r="X81">
             <v>5</v>
@@ -11344,7 +11344,7 @@
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55500010</v>
+            <v>55500009</v>
           </cell>
           <cell r="X82">
             <v>5</v>
@@ -11352,7 +11352,7 @@
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55500011</v>
+            <v>55500010</v>
           </cell>
           <cell r="X83">
             <v>5</v>
@@ -11360,7 +11360,7 @@
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55500012</v>
+            <v>55500011</v>
           </cell>
           <cell r="X84">
             <v>5</v>
@@ -11368,7 +11368,7 @@
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500013</v>
+            <v>55500012</v>
           </cell>
           <cell r="X85">
             <v>5</v>
@@ -11376,7 +11376,7 @@
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500014</v>
+            <v>55500013</v>
           </cell>
           <cell r="X86">
             <v>5</v>
@@ -11384,7 +11384,7 @@
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500015</v>
+            <v>55500014</v>
           </cell>
           <cell r="X87">
             <v>5</v>
@@ -11392,7 +11392,7 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500016</v>
+            <v>55500015</v>
           </cell>
           <cell r="X88">
             <v>5</v>
@@ -11400,23 +11400,23 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55510001</v>
+            <v>55500016</v>
           </cell>
           <cell r="X89">
-            <v>12</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55510002</v>
+            <v>55510001</v>
           </cell>
           <cell r="X90">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55510003</v>
+            <v>55510002</v>
           </cell>
           <cell r="X91">
             <v>15</v>
@@ -11424,87 +11424,87 @@
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55510004</v>
+            <v>55510003</v>
           </cell>
           <cell r="X92">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55510006</v>
+            <v>55510004</v>
           </cell>
           <cell r="X93">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55510007</v>
+            <v>55510006</v>
           </cell>
           <cell r="X94">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55510009</v>
+            <v>55510007</v>
           </cell>
           <cell r="X95">
-            <v>50</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55510010</v>
+            <v>55510009</v>
           </cell>
           <cell r="X96">
-            <v>5</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55510011</v>
+            <v>55510010</v>
           </cell>
           <cell r="X97">
-            <v>15</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55510012</v>
+            <v>55510011</v>
           </cell>
           <cell r="X98">
-            <v>62</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55510013</v>
+            <v>55510012</v>
           </cell>
           <cell r="X99">
-            <v>12</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55510014</v>
+            <v>55510013</v>
           </cell>
           <cell r="X100">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510018</v>
+            <v>55510014</v>
           </cell>
           <cell r="X101">
-            <v>37</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510019</v>
+            <v>55510018</v>
           </cell>
           <cell r="X102">
             <v>37</v>
@@ -11512,55 +11512,55 @@
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55520001</v>
+            <v>55510019</v>
           </cell>
           <cell r="X103">
-            <v>-25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55520002</v>
+            <v>55520001</v>
           </cell>
           <cell r="X104">
-            <v>62</v>
+            <v>-25</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55520003</v>
+            <v>55520002</v>
           </cell>
           <cell r="X105">
-            <v>27</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55520004</v>
+            <v>55520003</v>
           </cell>
           <cell r="X106">
-            <v>150</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55600001</v>
+            <v>55520004</v>
           </cell>
           <cell r="X107">
-            <v>8</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55600002</v>
+            <v>55600001</v>
           </cell>
           <cell r="X108">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55600003</v>
+            <v>55600002</v>
           </cell>
           <cell r="X109">
             <v>10</v>
@@ -11568,23 +11568,23 @@
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55600004</v>
+            <v>55600003</v>
           </cell>
           <cell r="X110">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55600005</v>
+            <v>55600004</v>
           </cell>
           <cell r="X111">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55600006</v>
+            <v>55600005</v>
           </cell>
           <cell r="X112">
             <v>15</v>
@@ -11592,103 +11592,103 @@
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55600007</v>
+            <v>55600006</v>
           </cell>
           <cell r="X113">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55600008</v>
+            <v>55600007</v>
           </cell>
           <cell r="X114">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55600009</v>
+            <v>55600008</v>
           </cell>
           <cell r="X115">
-            <v>13</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55600010</v>
+            <v>55600009</v>
           </cell>
           <cell r="X116">
-            <v>30</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55600011</v>
+            <v>55600010</v>
           </cell>
           <cell r="X117">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55600012</v>
+            <v>55600011</v>
           </cell>
           <cell r="X118">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55600013</v>
+            <v>55600012</v>
           </cell>
           <cell r="X119">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55600014</v>
+            <v>55600013</v>
           </cell>
           <cell r="X120">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55600015</v>
+            <v>55600014</v>
           </cell>
           <cell r="X121">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55600016</v>
+            <v>55600015</v>
           </cell>
           <cell r="X122">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55610001</v>
+            <v>55600016</v>
           </cell>
           <cell r="X123">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55610002</v>
+            <v>55610001</v>
           </cell>
           <cell r="X124">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55610003</v>
+            <v>55610002</v>
           </cell>
           <cell r="X125">
             <v>5</v>
@@ -11696,23 +11696,23 @@
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55610004</v>
+            <v>55610003</v>
           </cell>
           <cell r="X126">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55700001</v>
+            <v>55610004</v>
           </cell>
           <cell r="X127">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55700002</v>
+            <v>55700001</v>
           </cell>
           <cell r="X128">
             <v>20</v>
@@ -11720,7 +11720,7 @@
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55700003</v>
+            <v>55700002</v>
           </cell>
           <cell r="X129">
             <v>20</v>
@@ -11728,7 +11728,7 @@
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55700004</v>
+            <v>55700003</v>
           </cell>
           <cell r="X130">
             <v>20</v>
@@ -11736,207 +11736,207 @@
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55700005</v>
+            <v>55700004</v>
           </cell>
           <cell r="X131">
-            <v>40</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55900001</v>
+            <v>55700005</v>
           </cell>
           <cell r="X132">
-            <v>35</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900002</v>
+            <v>55900001</v>
           </cell>
           <cell r="X133">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900003</v>
+            <v>55900002</v>
           </cell>
           <cell r="X134">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900004</v>
+            <v>55900003</v>
           </cell>
           <cell r="X135">
-            <v>-30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900005</v>
+            <v>55900004</v>
           </cell>
           <cell r="X136">
-            <v>20</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900006</v>
+            <v>55900005</v>
           </cell>
           <cell r="X137">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900007</v>
+            <v>55900006</v>
           </cell>
           <cell r="X138">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900008</v>
+            <v>55900007</v>
           </cell>
           <cell r="X139">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900009</v>
+            <v>55900008</v>
           </cell>
           <cell r="X140">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900010</v>
+            <v>55900009</v>
           </cell>
           <cell r="X141">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900011</v>
+            <v>55900010</v>
           </cell>
           <cell r="X142">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900012</v>
+            <v>55900011</v>
           </cell>
           <cell r="X143">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900013</v>
+            <v>55900012</v>
           </cell>
           <cell r="X144">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900014</v>
+            <v>55900013</v>
           </cell>
           <cell r="X145">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900015</v>
+            <v>55900014</v>
           </cell>
           <cell r="X146">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900016</v>
+            <v>55900015</v>
           </cell>
           <cell r="X147">
-            <v>45</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900017</v>
+            <v>55900016</v>
           </cell>
           <cell r="X148">
-            <v>10</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900018</v>
+            <v>55900017</v>
           </cell>
           <cell r="X149">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900019</v>
+            <v>55900018</v>
           </cell>
           <cell r="X150">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900020</v>
+            <v>55900019</v>
           </cell>
           <cell r="X151">
-            <v>20</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900021</v>
+            <v>55900020</v>
           </cell>
           <cell r="X152">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900022</v>
+            <v>55900021</v>
           </cell>
           <cell r="X153">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900023</v>
+            <v>55900022</v>
           </cell>
           <cell r="X154">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900024</v>
+            <v>55900023</v>
           </cell>
           <cell r="X155">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900025</v>
+            <v>55900024</v>
           </cell>
           <cell r="X156">
             <v>10</v>
@@ -11944,60 +11944,60 @@
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900026</v>
+            <v>55900025</v>
           </cell>
           <cell r="X157">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900027</v>
+            <v>55900026</v>
           </cell>
           <cell r="X158">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900028</v>
+            <v>55900027</v>
+          </cell>
+          <cell r="X159">
+            <v>35</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900029</v>
-          </cell>
-          <cell r="X160">
-            <v>15</v>
+            <v>55900028</v>
           </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900030</v>
+            <v>55900029</v>
           </cell>
           <cell r="X161">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900031</v>
+            <v>55900030</v>
           </cell>
           <cell r="X162">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900032</v>
+            <v>55900031</v>
           </cell>
           <cell r="X163">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900033</v>
+            <v>55900032</v>
           </cell>
           <cell r="X164">
             <v>20</v>
@@ -12005,15 +12005,15 @@
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900034</v>
+            <v>55900033</v>
           </cell>
           <cell r="X165">
-            <v>14</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900035</v>
+            <v>55900034</v>
           </cell>
           <cell r="X166">
             <v>14</v>
@@ -12021,31 +12021,31 @@
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900036</v>
+            <v>55900035</v>
           </cell>
           <cell r="X167">
-            <v>50</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900037</v>
+            <v>55900036</v>
           </cell>
           <cell r="X168">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900038</v>
+            <v>55900037</v>
           </cell>
           <cell r="X169">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900039</v>
+            <v>55900038</v>
           </cell>
           <cell r="X170">
             <v>40</v>
@@ -12053,63 +12053,63 @@
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900040</v>
+            <v>55900039</v>
           </cell>
           <cell r="X171">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900041</v>
+            <v>55900040</v>
           </cell>
           <cell r="X172">
-            <v>0</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900042</v>
+            <v>55900041</v>
           </cell>
           <cell r="X173">
-            <v>25</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900043</v>
+            <v>55900042</v>
           </cell>
           <cell r="X174">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900044</v>
+            <v>55900043</v>
           </cell>
           <cell r="X175">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900045</v>
+            <v>55900044</v>
           </cell>
           <cell r="X176">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55990001</v>
+            <v>55900045</v>
           </cell>
           <cell r="X177">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X178">
             <v>15</v>
@@ -12117,7 +12117,7 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X179">
             <v>15</v>
@@ -12125,7 +12125,7 @@
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X180">
             <v>15</v>
@@ -12133,7 +12133,7 @@
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X181">
             <v>15</v>
@@ -12141,7 +12141,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X182">
             <v>15</v>
@@ -12149,7 +12149,7 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X183">
             <v>15</v>
@@ -12157,7 +12157,7 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -12165,7 +12165,7 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -12173,7 +12173,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -12181,7 +12181,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -12189,7 +12189,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -12197,33 +12197,41 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X189">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X190">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X191">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="192">
           <cell r="A192">
+            <v>55990103</v>
+          </cell>
+          <cell r="X192">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="A193">
             <v>55990104</v>
           </cell>
-          <cell r="X192">
+          <cell r="X193">
             <v>50</v>
           </cell>
         </row>
@@ -40124,43 +40132,43 @@
   <dimension ref="A1:BB301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B163" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B229" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C171" sqref="C171"/>
+      <selection pane="bottomRight" activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="5" max="9" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="7.25" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="5" max="9" width="3.375" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4.109375" customWidth="1"/>
-    <col min="12" max="19" width="4.77734375" customWidth="1"/>
-    <col min="20" max="20" width="4.109375" customWidth="1"/>
-    <col min="21" max="23" width="4.77734375" customWidth="1"/>
-    <col min="24" max="24" width="6.44140625" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="5.44140625" customWidth="1"/>
-    <col min="28" max="30" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="4.6640625" customWidth="1"/>
-    <col min="38" max="38" width="10.109375" customWidth="1"/>
-    <col min="39" max="44" width="3.77734375" customWidth="1"/>
-    <col min="45" max="45" width="4.33203125" customWidth="1"/>
-    <col min="46" max="46" width="15.77734375" customWidth="1"/>
-    <col min="47" max="47" width="6.33203125" customWidth="1"/>
-    <col min="48" max="48" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.125" customWidth="1"/>
+    <col min="12" max="19" width="4.75" customWidth="1"/>
+    <col min="20" max="20" width="4.125" customWidth="1"/>
+    <col min="21" max="23" width="4.75" customWidth="1"/>
+    <col min="24" max="24" width="6.5" customWidth="1"/>
+    <col min="25" max="25" width="17.375" customWidth="1"/>
+    <col min="26" max="26" width="8.875" customWidth="1"/>
+    <col min="27" max="27" width="5.5" customWidth="1"/>
+    <col min="28" max="30" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="4.625" customWidth="1"/>
+    <col min="38" max="38" width="10.125" customWidth="1"/>
+    <col min="39" max="44" width="3.75" customWidth="1"/>
+    <col min="45" max="45" width="4.375" customWidth="1"/>
+    <col min="46" max="46" width="15.75" customWidth="1"/>
+    <col min="47" max="47" width="6.375" customWidth="1"/>
+    <col min="48" max="48" width="9.625" customWidth="1"/>
     <col min="49" max="49" width="6" customWidth="1"/>
-    <col min="50" max="50" width="4.6640625" customWidth="1"/>
-    <col min="51" max="51" width="5.77734375" customWidth="1"/>
-    <col min="52" max="52" width="4.6640625" customWidth="1"/>
-    <col min="53" max="54" width="4.109375" customWidth="1"/>
+    <col min="50" max="50" width="4.625" customWidth="1"/>
+    <col min="51" max="51" width="5.75" customWidth="1"/>
+    <col min="52" max="52" width="4.625" customWidth="1"/>
+    <col min="53" max="54" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="73.2">
+    <row r="1" spans="1:54" ht="69">
       <c r="A1" s="13" t="s">
         <v>302</v>
       </c>
@@ -50671,7 +50679,7 @@
         <v>512</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E68" s="4">
         <v>7</v>
@@ -50736,7 +50744,7 @@
         <v>75</v>
       </c>
       <c r="Y68" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="Z68" s="37">
         <v>55300010</v>
@@ -55317,7 +55325,7 @@
         <v>22</v>
       </c>
       <c r="Y97" s="4" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="Z97" s="37">
         <v>55900045</v>
@@ -57915,7 +57923,7 @@
         <v>542</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E114" s="4">
         <v>7</v>
@@ -57980,7 +57988,7 @@
         <v>86</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="Z114" s="37">
         <v>55900039</v>
@@ -58145,7 +58153,7 @@
         <v>91</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="Z115" s="37">
         <v>55900041</v>
@@ -58306,7 +58314,7 @@
         <v>31</v>
       </c>
       <c r="Y116" s="4" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="Z116" s="37">
         <v>55900044</v>
@@ -58406,7 +58414,7 @@
         <v>533</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E117" s="4">
         <v>7</v>
@@ -58471,7 +58479,7 @@
         <v>75</v>
       </c>
       <c r="Y117" s="4" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="Z117" s="37">
         <v>55400007</v>
@@ -58571,7 +58579,7 @@
         <v>543</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E118" s="4">
         <v>7</v>
@@ -58636,7 +58644,7 @@
         <v>40</v>
       </c>
       <c r="Y118" s="4" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="Z118" s="37">
         <v>55900042</v>
@@ -58895,7 +58903,7 @@
         <v>544</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E120" s="4">
         <v>7</v>
@@ -58960,7 +58968,7 @@
         <v>49</v>
       </c>
       <c r="Y120" s="4" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="Z120" s="37">
         <v>55900043</v>
@@ -59125,7 +59133,7 @@
         <v>22</v>
       </c>
       <c r="Y121" s="4" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="Z121" s="37">
         <v>55900040</v>
@@ -70270,7 +70278,7 @@
         <v>730</v>
       </c>
       <c r="Y192" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="Z192" s="37">
         <v>55110001</v>
@@ -70694,7 +70702,7 @@
         <v>598</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E195" s="4">
         <v>5</v>
@@ -70759,7 +70767,7 @@
         <v>204</v>
       </c>
       <c r="Y195" s="4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="Z195" s="18">
         <v>55100011</v>
@@ -71344,7 +71352,7 @@
         <v>602</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E199" s="4">
         <v>5</v>
@@ -71409,7 +71417,7 @@
         <v>2</v>
       </c>
       <c r="Y199" s="4" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="Z199" s="37">
         <v>55100010</v>
@@ -71570,7 +71578,7 @@
         <v>4</v>
       </c>
       <c r="Y200" s="4" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="Z200" s="37">
         <v>55110008</v>
@@ -77990,7 +77998,7 @@
         <v>435</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E241" s="4">
         <v>5</v>
@@ -78015,7 +78023,7 @@
         <v>-12</v>
       </c>
       <c r="L241" s="4">
-        <v>-22</v>
+        <v>-37</v>
       </c>
       <c r="M241" s="4">
         <v>0</v>
@@ -78040,7 +78048,7 @@
       </c>
       <c r="T241" s="12">
         <f t="shared" si="13"/>
-        <v>7.1999999999999993</v>
+        <v>7.2000000000000028</v>
       </c>
       <c r="U241" s="4">
         <v>10</v>
@@ -78055,7 +78063,7 @@
         <v>16</v>
       </c>
       <c r="Y241" s="4" t="s">
-        <v>1090</v>
+        <v>1127</v>
       </c>
       <c r="Z241" s="37">
         <v>55100010</v>
@@ -78064,22 +78072,18 @@
         <v>100</v>
       </c>
       <c r="AB241" s="18">
-        <v>55110006</v>
+        <v>55110020</v>
       </c>
       <c r="AC241" s="18">
         <v>100</v>
       </c>
-      <c r="AD241" s="18">
-        <v>55110007</v>
-      </c>
-      <c r="AE241" s="18">
-        <v>100</v>
-      </c>
+      <c r="AD241" s="18"/>
+      <c r="AE241" s="18"/>
       <c r="AF241" s="18">
         <f>IF(ISBLANK($Z241),0, LOOKUP($Z241,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AA241/100)+
 IF(ISBLANK($AB241),0, LOOKUP($AB241,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AC241/100)+
 IF(ISBLANK($AD241),0, LOOKUP($AD241,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AE241/100)</f>
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="AG241" s="18">
         <v>0</v>
@@ -82104,7 +82108,7 @@
         <v>388</v>
       </c>
       <c r="D267" s="19" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E267" s="4">
         <v>5</v>
@@ -82169,7 +82173,7 @@
         <v>91</v>
       </c>
       <c r="Y267" s="4" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="Z267" s="37">
         <v>55510001</v>
@@ -82738,7 +82742,7 @@
         <v>390</v>
       </c>
       <c r="D271" s="19" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E271" s="4">
         <v>5</v>
@@ -82803,7 +82807,7 @@
         <v>40</v>
       </c>
       <c r="Y271" s="4" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="Z271" s="18">
         <v>55100012</v>
@@ -82901,7 +82905,7 @@
         <v>632</v>
       </c>
       <c r="D272" s="19" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E272" s="4">
         <v>5</v>
@@ -82966,7 +82970,7 @@
         <v>31</v>
       </c>
       <c r="Y272" s="4" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="Z272" s="18">
         <v>55100012</v>
@@ -83064,7 +83068,7 @@
         <v>391</v>
       </c>
       <c r="D273" s="19" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E273" s="4">
         <v>5</v>
@@ -83129,7 +83133,7 @@
         <v>736</v>
       </c>
       <c r="Y273" s="4" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="Z273" s="18">
         <v>55100012</v>
@@ -84870,7 +84874,7 @@
         <v>6</v>
       </c>
       <c r="Y284" s="4" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="Z284" s="37">
         <v>55200010</v>
@@ -84964,7 +84968,7 @@
         <v>636</v>
       </c>
       <c r="D285" s="19" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E285" s="4">
         <v>6</v>
@@ -85029,7 +85033,7 @@
         <v>16</v>
       </c>
       <c r="Y285" s="4" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="Z285" s="37">
         <v>55900038</v>
@@ -87710,35 +87714,35 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="5" max="9" width="3.33203125" customWidth="1"/>
-    <col min="10" max="11" width="4.109375" customWidth="1"/>
-    <col min="12" max="19" width="4.77734375" customWidth="1"/>
-    <col min="20" max="20" width="4.109375" customWidth="1"/>
-    <col min="21" max="23" width="4.77734375" customWidth="1"/>
-    <col min="24" max="24" width="6.44140625" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="5.44140625" customWidth="1"/>
-    <col min="29" max="29" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="4.6640625" customWidth="1"/>
-    <col min="38" max="38" width="10.109375" customWidth="1"/>
-    <col min="39" max="45" width="3.77734375" customWidth="1"/>
-    <col min="46" max="46" width="14.77734375" customWidth="1"/>
-    <col min="47" max="47" width="5.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="7.25" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="5" max="9" width="3.375" customWidth="1"/>
+    <col min="10" max="11" width="4.125" customWidth="1"/>
+    <col min="12" max="19" width="4.75" customWidth="1"/>
+    <col min="20" max="20" width="4.125" customWidth="1"/>
+    <col min="21" max="23" width="4.75" customWidth="1"/>
+    <col min="24" max="24" width="6.5" customWidth="1"/>
+    <col min="25" max="25" width="17.375" customWidth="1"/>
+    <col min="26" max="26" width="8.875" customWidth="1"/>
+    <col min="27" max="27" width="5.5" customWidth="1"/>
+    <col min="29" max="29" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="4.625" customWidth="1"/>
+    <col min="38" max="38" width="10.125" customWidth="1"/>
+    <col min="39" max="45" width="3.75" customWidth="1"/>
+    <col min="46" max="46" width="14.75" customWidth="1"/>
+    <col min="47" max="47" width="5.875" customWidth="1"/>
     <col min="48" max="48" width="9" customWidth="1"/>
     <col min="49" max="49" width="6" customWidth="1"/>
-    <col min="50" max="50" width="5.6640625" customWidth="1"/>
-    <col min="51" max="51" width="5.77734375" customWidth="1"/>
-    <col min="52" max="52" width="4.6640625" customWidth="1"/>
-    <col min="53" max="54" width="4.109375" customWidth="1"/>
+    <col min="50" max="50" width="5.625" customWidth="1"/>
+    <col min="51" max="51" width="5.75" customWidth="1"/>
+    <col min="52" max="52" width="4.625" customWidth="1"/>
+    <col min="53" max="54" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="73.2">
+    <row r="1" spans="1:54" ht="69">
       <c r="A1" s="13" t="s">
         <v>302</v>
       </c>
@@ -88386,10 +88390,10 @@
         <v>51013001</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>1115</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>1116</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8">
@@ -88455,7 +88459,7 @@
         <v>9</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="Z5" s="18">
         <v>55510010</v>
@@ -89922,10 +89926,10 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="9" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="2" max="9" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -90381,10 +90385,10 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.75" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -90474,10 +90478,10 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -90485,7 +90489,7 @@
         <v>666</v>
       </c>
       <c r="B1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -90546,7 +90550,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -90554,7 +90558,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="24" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
@@ -90562,7 +90566,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B11" s="22"/>
     </row>

</xml_diff>

<commit_message>
new spell card VERTEX #62
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4758,296 +4758,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="139">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="137">
     <dxf>
       <font>
         <b/>
@@ -6329,6 +6040,226 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7604,6 +7535,51 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7901,11 +7877,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1711664848"/>
-        <c:axId val="-1711674096"/>
+        <c:axId val="-1711673008"/>
+        <c:axId val="-1711662128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1711664848"/>
+        <c:axId val="-1711673008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7948,7 +7924,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711674096"/>
+        <c:crossAx val="-1711662128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7956,7 +7932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1711674096"/>
+        <c:axId val="-1711662128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8007,7 +7983,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711664848"/>
+        <c:crossAx val="-1711673008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8377,11 +8353,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1711666480"/>
-        <c:axId val="-1711667024"/>
+        <c:axId val="-1711671376"/>
+        <c:axId val="-1711674096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1711666480"/>
+        <c:axId val="-1711671376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8424,7 +8400,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711667024"/>
+        <c:crossAx val="-1711674096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8432,7 +8408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1711667024"/>
+        <c:axId val="-1711674096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8483,7 +8459,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711666480"/>
+        <c:crossAx val="-1711671376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -38181,7 +38157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -38279,7 +38255,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="56">
     <pivotField dataField="1" showAll="0"/>
@@ -38723,155 +38699,155 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AY301" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137" tableBorderDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AY301" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129" tableBorderDxfId="128">
   <autoFilter ref="A3:AY301"/>
   <sortState ref="A4:BD301">
     <sortCondition ref="A3:A301"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="Id" dataDxfId="135"/>
-    <tableColumn id="2" name="Name" dataDxfId="134"/>
-    <tableColumn id="22" name="Ename" dataDxfId="133"/>
-    <tableColumn id="23" name="Remark" dataDxfId="132"/>
-    <tableColumn id="3" name="Star" dataDxfId="131"/>
-    <tableColumn id="4" name="Type" dataDxfId="130"/>
-    <tableColumn id="5" name="Attr" dataDxfId="129"/>
-    <tableColumn id="58" name="Quality" dataDxfId="128">
+    <tableColumn id="1" name="Id" dataDxfId="127"/>
+    <tableColumn id="2" name="Name" dataDxfId="126"/>
+    <tableColumn id="22" name="Ename" dataDxfId="125"/>
+    <tableColumn id="23" name="Remark" dataDxfId="124"/>
+    <tableColumn id="3" name="Star" dataDxfId="123"/>
+    <tableColumn id="4" name="Type" dataDxfId="122"/>
+    <tableColumn id="5" name="Attr" dataDxfId="121"/>
+    <tableColumn id="58" name="Quality" dataDxfId="120">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="127"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="126"/>
-    <tableColumn id="24" name="VitP" dataDxfId="125"/>
-    <tableColumn id="25" name="Modify" dataDxfId="124"/>
-    <tableColumn id="9" name="Def" dataDxfId="123"/>
-    <tableColumn id="10" name="Mag" dataDxfId="122"/>
-    <tableColumn id="32" name="Spd" dataDxfId="121"/>
-    <tableColumn id="35" name="Hit" dataDxfId="120"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="119"/>
-    <tableColumn id="34" name="Crt" dataDxfId="118"/>
-    <tableColumn id="33" name="Luk" dataDxfId="117"/>
-    <tableColumn id="7" name="Sum" dataDxfId="116">
+    <tableColumn id="12" name="Cost" dataDxfId="119"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="118"/>
+    <tableColumn id="24" name="VitP" dataDxfId="117"/>
+    <tableColumn id="25" name="Modify" dataDxfId="116"/>
+    <tableColumn id="9" name="Def" dataDxfId="115"/>
+    <tableColumn id="10" name="Mag" dataDxfId="114"/>
+    <tableColumn id="32" name="Spd" dataDxfId="113"/>
+    <tableColumn id="35" name="Hit" dataDxfId="112"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="111"/>
+    <tableColumn id="34" name="Crt" dataDxfId="110"/>
+    <tableColumn id="33" name="Luk" dataDxfId="109"/>
+    <tableColumn id="7" name="Sum" dataDxfId="108">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="115"/>
-    <tableColumn id="14" name="Mov" dataDxfId="114"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="113"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="112"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="111"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="110"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="109"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="108"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="107">
+    <tableColumn id="13" name="Range" dataDxfId="107"/>
+    <tableColumn id="14" name="Mov" dataDxfId="106"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="105"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="104"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="103"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="102"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="101"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="100"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="99">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="106"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="105"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="104"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="103"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="102"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="101">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="98"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="97"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="96"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="95"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="94"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="93">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="100"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="99"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="98"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="97"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="96"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="95"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="94"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="93">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="92"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="91"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="90"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="89"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="88"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="87"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="86"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="85">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="92"/>
-    <tableColumn id="29" name="JobId" dataDxfId="91"/>
-    <tableColumn id="20" name="Res" dataDxfId="90"/>
-    <tableColumn id="21" name="Icon" dataDxfId="89"/>
-    <tableColumn id="17" name="Cover" dataDxfId="88"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="87"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="86"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="85"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="84"/>
+    <tableColumn id="29" name="JobId" dataDxfId="83"/>
+    <tableColumn id="20" name="Res" dataDxfId="82"/>
+    <tableColumn id="21" name="Icon" dataDxfId="81"/>
+    <tableColumn id="17" name="Cover" dataDxfId="80"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="79"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="78"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:AY14" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:AY14" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="A3:AY14"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="Id" dataDxfId="81"/>
-    <tableColumn id="2" name="Name" dataDxfId="80"/>
-    <tableColumn id="22" name="Ename" dataDxfId="79"/>
-    <tableColumn id="23" name="Remark" dataDxfId="78"/>
-    <tableColumn id="3" name="Star" dataDxfId="77"/>
-    <tableColumn id="4" name="Type" dataDxfId="76"/>
-    <tableColumn id="5" name="Attr" dataDxfId="75"/>
-    <tableColumn id="58" name="Quality" dataDxfId="74">
+    <tableColumn id="1" name="Id" dataDxfId="51"/>
+    <tableColumn id="2" name="Name" dataDxfId="50"/>
+    <tableColumn id="22" name="Ename" dataDxfId="49"/>
+    <tableColumn id="23" name="Remark" dataDxfId="48"/>
+    <tableColumn id="3" name="Star" dataDxfId="47"/>
+    <tableColumn id="4" name="Type" dataDxfId="46"/>
+    <tableColumn id="5" name="Attr" dataDxfId="45"/>
+    <tableColumn id="58" name="Quality" dataDxfId="44">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="73"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="72"/>
-    <tableColumn id="24" name="VitP" dataDxfId="71"/>
-    <tableColumn id="25" name="Modify" dataDxfId="70"/>
-    <tableColumn id="9" name="Def" dataDxfId="69"/>
-    <tableColumn id="10" name="Mag" dataDxfId="68"/>
-    <tableColumn id="32" name="Spd" dataDxfId="67"/>
-    <tableColumn id="35" name="Hit" dataDxfId="66"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="65"/>
-    <tableColumn id="34" name="Crt" dataDxfId="64"/>
-    <tableColumn id="33" name="Luk" dataDxfId="63"/>
-    <tableColumn id="7" name="Sum" dataDxfId="62">
+    <tableColumn id="12" name="Cost" dataDxfId="43"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="42"/>
+    <tableColumn id="24" name="VitP" dataDxfId="41"/>
+    <tableColumn id="25" name="Modify" dataDxfId="40"/>
+    <tableColumn id="9" name="Def" dataDxfId="39"/>
+    <tableColumn id="10" name="Mag" dataDxfId="38"/>
+    <tableColumn id="32" name="Spd" dataDxfId="37"/>
+    <tableColumn id="35" name="Hit" dataDxfId="36"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="35"/>
+    <tableColumn id="34" name="Crt" dataDxfId="34"/>
+    <tableColumn id="33" name="Luk" dataDxfId="33"/>
+    <tableColumn id="7" name="Sum" dataDxfId="32">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="61"/>
-    <tableColumn id="14" name="Mov" dataDxfId="60"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="59"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="58"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="57"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="56"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="55"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="54"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="53">
+    <tableColumn id="13" name="Range" dataDxfId="31"/>
+    <tableColumn id="14" name="Mov" dataDxfId="30"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="29"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="28"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="27"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="26"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="25"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="24"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="23">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="52"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="51"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="50"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="49"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="48"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="47">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="22"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="21"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="20"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="19"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="18"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="17">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="46"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="45"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="44"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="43"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="42"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="41"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="40"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="39">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="16"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="15"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="14"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="13"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="12"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="38"/>
-    <tableColumn id="29" name="JobId" dataDxfId="37"/>
-    <tableColumn id="20" name="Res" dataDxfId="36"/>
-    <tableColumn id="21" name="Icon" dataDxfId="35"/>
-    <tableColumn id="17" name="Cover" dataDxfId="34"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="33"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="32"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="31"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
+    <tableColumn id="29" name="JobId" dataDxfId="7"/>
+    <tableColumn id="20" name="Res" dataDxfId="6"/>
+    <tableColumn id="21" name="Icon" dataDxfId="5"/>
+    <tableColumn id="17" name="Cover" dataDxfId="4"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39178,7 +39154,7 @@
   <dimension ref="A1:AY301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B212" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B224" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A232" sqref="A232"/>
@@ -85021,24 +84997,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H301">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="136" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D301">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -85071,7 +85047,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AU13" sqref="AU13"/>
+      <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -87190,37 +87166,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 J6:K9 K12 K14">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="35" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="22" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="21" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="32" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="31" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="27" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -87238,13 +87214,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="17" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -87262,19 +87238,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="13" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -87291,31 +87267,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="5" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -87344,13 +87320,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
adjust the monster TYPe info
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
-    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -7877,11 +7877,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1711673008"/>
-        <c:axId val="-1711662128"/>
+        <c:axId val="208151648"/>
+        <c:axId val="208151088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1711673008"/>
+        <c:axId val="208151648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7924,7 +7924,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711662128"/>
+        <c:crossAx val="208151088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7932,7 +7932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1711662128"/>
+        <c:axId val="208151088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7983,7 +7983,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711673008"/>
+        <c:crossAx val="208151648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8353,11 +8353,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1711671376"/>
-        <c:axId val="-1711674096"/>
+        <c:axId val="267701488"/>
+        <c:axId val="267702048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1711671376"/>
+        <c:axId val="267701488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8400,7 +8400,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711674096"/>
+        <c:crossAx val="267702048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8408,7 +8408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1711674096"/>
+        <c:axId val="267702048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8459,7 +8459,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1711671376"/>
+        <c:crossAx val="267701488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -38157,7 +38157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -38255,7 +38255,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="56">
     <pivotField dataField="1" showAll="0"/>
@@ -39153,43 +39153,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B224" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A232" sqref="A232"/>
+      <selection pane="bottomRight" activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="8.875" customWidth="1"/>
-    <col min="26" max="26" width="5.5" customWidth="1"/>
-    <col min="27" max="28" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="4.625" customWidth="1"/>
-    <col min="35" max="35" width="10.125" customWidth="1"/>
-    <col min="36" max="41" width="3.75" customWidth="1"/>
-    <col min="42" max="42" width="4.375" customWidth="1"/>
-    <col min="43" max="43" width="15.75" customWidth="1"/>
-    <col min="44" max="44" width="6.375" customWidth="1"/>
-    <col min="45" max="45" width="9.625" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" customWidth="1"/>
+    <col min="27" max="28" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="4.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" customWidth="1"/>
+    <col min="36" max="41" width="3.77734375" customWidth="1"/>
+    <col min="42" max="42" width="4.33203125" customWidth="1"/>
+    <col min="43" max="43" width="15.77734375" customWidth="1"/>
+    <col min="44" max="44" width="6.33203125" customWidth="1"/>
+    <col min="45" max="45" width="9.6640625" customWidth="1"/>
     <col min="46" max="46" width="6" customWidth="1"/>
-    <col min="47" max="47" width="4.625" customWidth="1"/>
-    <col min="48" max="48" width="5.75" customWidth="1"/>
-    <col min="49" max="49" width="4.625" customWidth="1"/>
-    <col min="50" max="51" width="4.125" customWidth="1"/>
+    <col min="47" max="47" width="4.6640625" customWidth="1"/>
+    <col min="48" max="48" width="5.77734375" customWidth="1"/>
+    <col min="49" max="49" width="4.6640625" customWidth="1"/>
+    <col min="50" max="51" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="69">
+    <row r="1" spans="1:51" ht="73.2">
       <c r="A1" s="13" t="s">
         <v>301</v>
       </c>
@@ -58197,7 +58197,7 @@
         <v>1</v>
       </c>
       <c r="F126" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G126" s="4">
         <v>2</v>
@@ -65751,7 +65751,7 @@
         <v>4</v>
       </c>
       <c r="F176" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G176" s="4">
         <v>1</v>
@@ -66208,7 +66208,7 @@
         <v>2</v>
       </c>
       <c r="F179" s="4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G179" s="4">
         <v>0</v>
@@ -66979,7 +66979,7 @@
         <v>3</v>
       </c>
       <c r="F184" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G184" s="4">
         <v>3</v>
@@ -68038,7 +68038,7 @@
         <v>5</v>
       </c>
       <c r="F191" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G191" s="4">
         <v>2</v>
@@ -77514,7 +77514,7 @@
         <v>3</v>
       </c>
       <c r="F253" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G253" s="4">
         <v>3</v>
@@ -82861,7 +82861,7 @@
         <v>3</v>
       </c>
       <c r="F288" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G288" s="8">
         <v>0</v>
@@ -84246,7 +84246,7 @@
         <v>3</v>
       </c>
       <c r="F297" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G297" s="4">
         <v>0</v>
@@ -85043,41 +85043,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
-    <col min="10" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="8.875" customWidth="1"/>
-    <col min="26" max="26" width="5.5" customWidth="1"/>
-    <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="4.625" customWidth="1"/>
-    <col min="35" max="35" width="10.125" customWidth="1"/>
-    <col min="36" max="42" width="3.75" customWidth="1"/>
-    <col min="43" max="43" width="14.75" customWidth="1"/>
-    <col min="44" max="44" width="5.875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
+    <col min="10" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" customWidth="1"/>
+    <col min="28" max="28" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="4.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" customWidth="1"/>
+    <col min="36" max="42" width="3.77734375" customWidth="1"/>
+    <col min="43" max="43" width="14.77734375" customWidth="1"/>
+    <col min="44" max="44" width="5.88671875" customWidth="1"/>
     <col min="45" max="45" width="9" customWidth="1"/>
     <col min="46" max="46" width="6" customWidth="1"/>
-    <col min="47" max="47" width="5.625" customWidth="1"/>
-    <col min="48" max="48" width="5.75" customWidth="1"/>
-    <col min="49" max="49" width="4.625" customWidth="1"/>
-    <col min="50" max="51" width="4.125" customWidth="1"/>
+    <col min="47" max="47" width="5.6640625" customWidth="1"/>
+    <col min="48" max="48" width="5.77734375" customWidth="1"/>
+    <col min="49" max="49" width="4.6640625" customWidth="1"/>
+    <col min="50" max="51" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="69">
+    <row r="1" spans="1:51" ht="73.2">
       <c r="A1" s="13" t="s">
         <v>301</v>
       </c>
@@ -87363,10 +87363,10 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.25" customWidth="1"/>
-    <col min="2" max="9" width="7.125" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -87822,10 +87822,10 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -87915,10 +87915,10 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
#58 adjust some job's monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -3719,6 +3719,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
   <fonts count="35">
     <font>
       <sz val="11"/>
@@ -4550,7 +4553,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4713,6 +4716,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4759,6 +4768,34 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="137">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6409,34 +6446,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -10991,7 +11000,6 @@
           <cell r="A160">
             <v>55900028</v>
           </cell>
-          <cell r="X160"/>
         </row>
         <row r="161">
           <cell r="A161">
@@ -38760,94 +38768,94 @@
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="50" name="IsBuilding" dataDxfId="84"/>
-    <tableColumn id="29" name="JobId" dataDxfId="83"/>
-    <tableColumn id="20" name="Res" dataDxfId="82"/>
-    <tableColumn id="21" name="Icon" dataDxfId="81"/>
-    <tableColumn id="17" name="Cover" dataDxfId="80"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="79"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="78"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="77"/>
+    <tableColumn id="29" name="JobId" dataDxfId="0"/>
+    <tableColumn id="20" name="Res" dataDxfId="83"/>
+    <tableColumn id="21" name="Icon" dataDxfId="82"/>
+    <tableColumn id="17" name="Cover" dataDxfId="81"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="80"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="79"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:AY14" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:AY14" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A3:AY14"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="51">
-    <tableColumn id="1" name="Id" dataDxfId="51"/>
-    <tableColumn id="2" name="Name" dataDxfId="50"/>
-    <tableColumn id="22" name="Ename" dataDxfId="49"/>
-    <tableColumn id="23" name="Remark" dataDxfId="48"/>
-    <tableColumn id="3" name="Star" dataDxfId="47"/>
-    <tableColumn id="4" name="Type" dataDxfId="46"/>
-    <tableColumn id="5" name="Attr" dataDxfId="45"/>
-    <tableColumn id="58" name="Quality" dataDxfId="44">
+    <tableColumn id="1" name="Id" dataDxfId="52"/>
+    <tableColumn id="2" name="Name" dataDxfId="51"/>
+    <tableColumn id="22" name="Ename" dataDxfId="50"/>
+    <tableColumn id="23" name="Remark" dataDxfId="49"/>
+    <tableColumn id="3" name="Star" dataDxfId="48"/>
+    <tableColumn id="4" name="Type" dataDxfId="47"/>
+    <tableColumn id="5" name="Attr" dataDxfId="46"/>
+    <tableColumn id="58" name="Quality" dataDxfId="45">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="43"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="42"/>
-    <tableColumn id="24" name="VitP" dataDxfId="41"/>
-    <tableColumn id="25" name="Modify" dataDxfId="40"/>
-    <tableColumn id="9" name="Def" dataDxfId="39"/>
-    <tableColumn id="10" name="Mag" dataDxfId="38"/>
-    <tableColumn id="32" name="Spd" dataDxfId="37"/>
-    <tableColumn id="35" name="Hit" dataDxfId="36"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="35"/>
-    <tableColumn id="34" name="Crt" dataDxfId="34"/>
-    <tableColumn id="33" name="Luk" dataDxfId="33"/>
-    <tableColumn id="7" name="Sum" dataDxfId="32">
+    <tableColumn id="12" name="Cost" dataDxfId="44"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="43"/>
+    <tableColumn id="24" name="VitP" dataDxfId="42"/>
+    <tableColumn id="25" name="Modify" dataDxfId="41"/>
+    <tableColumn id="9" name="Def" dataDxfId="40"/>
+    <tableColumn id="10" name="Mag" dataDxfId="39"/>
+    <tableColumn id="32" name="Spd" dataDxfId="38"/>
+    <tableColumn id="35" name="Hit" dataDxfId="37"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="36"/>
+    <tableColumn id="34" name="Crt" dataDxfId="35"/>
+    <tableColumn id="33" name="Luk" dataDxfId="34"/>
+    <tableColumn id="7" name="Sum" dataDxfId="33">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="31"/>
-    <tableColumn id="14" name="Mov" dataDxfId="30"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="29"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="28"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="27"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="26"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="25"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="24"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="23">
+    <tableColumn id="13" name="Range" dataDxfId="32"/>
+    <tableColumn id="14" name="Mov" dataDxfId="31"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="30"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="29"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="28"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="27"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="26"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="25"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="24">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="22"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="21"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="20"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="19"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="18"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="17">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="23"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="22"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="21"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="20"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="19"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="18">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="16"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="15"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="14"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="13"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="12"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="11"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="10"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="9">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="17"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="16"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="15"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="14"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="13"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="12"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="11"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="10">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="8"/>
-    <tableColumn id="29" name="JobId" dataDxfId="7"/>
-    <tableColumn id="20" name="Res" dataDxfId="6"/>
-    <tableColumn id="21" name="Icon" dataDxfId="5"/>
-    <tableColumn id="17" name="Cover" dataDxfId="4"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="9"/>
+    <tableColumn id="29" name="JobId" dataDxfId="8"/>
+    <tableColumn id="20" name="Res" dataDxfId="7"/>
+    <tableColumn id="21" name="Icon" dataDxfId="6"/>
+    <tableColumn id="17" name="Cover" dataDxfId="5"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="4"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="3"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39154,10 +39162,10 @@
   <dimension ref="A1:AY301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="U207" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F126" sqref="F126"/>
+      <selection pane="bottomRight" activeCell="AG213" sqref="AG213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -39181,7 +39189,7 @@
     <col min="42" max="42" width="4.33203125" customWidth="1"/>
     <col min="43" max="43" width="15.77734375" customWidth="1"/>
     <col min="44" max="44" width="6.33203125" customWidth="1"/>
-    <col min="45" max="45" width="9.6640625" customWidth="1"/>
+    <col min="45" max="45" width="10.44140625" customWidth="1"/>
     <col min="46" max="46" width="6" customWidth="1"/>
     <col min="47" max="47" width="4.6640625" customWidth="1"/>
     <col min="48" max="48" width="5.77734375" customWidth="1"/>
@@ -39789,7 +39797,7 @@
       <c r="AR4" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS4" s="12"/>
+      <c r="AS4" s="54"/>
       <c r="AT4" s="4">
         <v>6</v>
       </c>
@@ -39940,7 +39948,7 @@
       <c r="AR5" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS5" s="50"/>
+      <c r="AS5" s="54"/>
       <c r="AT5" s="4">
         <v>6</v>
       </c>
@@ -40087,7 +40095,7 @@
       <c r="AR6" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS6" s="50"/>
+      <c r="AS6" s="54"/>
       <c r="AT6" s="4">
         <v>6</v>
       </c>
@@ -40234,7 +40242,7 @@
       <c r="AR7" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS7" s="50"/>
+      <c r="AS7" s="54"/>
       <c r="AT7" s="4">
         <v>6</v>
       </c>
@@ -40383,7 +40391,7 @@
       <c r="AR8" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS8" s="50"/>
+      <c r="AS8" s="54"/>
       <c r="AT8" s="4">
         <v>6</v>
       </c>
@@ -40540,7 +40548,7 @@
       <c r="AR9" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS9" s="50"/>
+      <c r="AS9" s="54"/>
       <c r="AT9" s="4">
         <v>6</v>
       </c>
@@ -40691,7 +40699,7 @@
       <c r="AR10" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS10" s="50"/>
+      <c r="AS10" s="54"/>
       <c r="AT10" s="4">
         <v>6</v>
       </c>
@@ -40838,7 +40846,7 @@
       <c r="AR11" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS11" s="50"/>
+      <c r="AS11" s="54"/>
       <c r="AT11" s="4">
         <v>6</v>
       </c>
@@ -40993,7 +41001,7 @@
       <c r="AR12" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS12" s="50"/>
+      <c r="AS12" s="54"/>
       <c r="AT12" s="4">
         <v>6</v>
       </c>
@@ -41142,7 +41150,7 @@
       <c r="AR13" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS13" s="50"/>
+      <c r="AS13" s="54"/>
       <c r="AT13" s="4">
         <v>6</v>
       </c>
@@ -41297,7 +41305,9 @@
       <c r="AR14" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS14" s="50"/>
+      <c r="AS14" s="54">
+        <v>11000005</v>
+      </c>
       <c r="AT14" s="4">
         <v>6</v>
       </c>
@@ -41446,7 +41456,7 @@
       <c r="AR15" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS15" s="50"/>
+      <c r="AS15" s="54"/>
       <c r="AT15" s="4">
         <v>4</v>
       </c>
@@ -41595,7 +41605,7 @@
       <c r="AR16" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS16" s="50"/>
+      <c r="AS16" s="54"/>
       <c r="AT16" s="4">
         <v>6</v>
       </c>
@@ -41744,7 +41754,7 @@
       <c r="AR17" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS17" s="50"/>
+      <c r="AS17" s="54"/>
       <c r="AT17" s="4">
         <v>6</v>
       </c>
@@ -41893,7 +41903,7 @@
       <c r="AR18" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS18" s="50"/>
+      <c r="AS18" s="54"/>
       <c r="AT18" s="4">
         <v>6</v>
       </c>
@@ -42042,7 +42052,7 @@
       <c r="AR19" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS19" s="50"/>
+      <c r="AS19" s="54"/>
       <c r="AT19" s="4">
         <v>6</v>
       </c>
@@ -42191,7 +42201,7 @@
       <c r="AR20" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS20" s="50"/>
+      <c r="AS20" s="54"/>
       <c r="AT20" s="4">
         <v>6</v>
       </c>
@@ -42340,7 +42350,7 @@
       <c r="AR21" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS21" s="50"/>
+      <c r="AS21" s="54"/>
       <c r="AT21" s="4">
         <v>6</v>
       </c>
@@ -42489,7 +42499,7 @@
       <c r="AR22" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS22" s="50"/>
+      <c r="AS22" s="54"/>
       <c r="AT22" s="4">
         <v>6</v>
       </c>
@@ -42638,7 +42648,7 @@
       <c r="AR23" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS23" s="50"/>
+      <c r="AS23" s="54"/>
       <c r="AT23" s="4">
         <v>6</v>
       </c>
@@ -42789,7 +42799,7 @@
       <c r="AR24" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS24" s="50"/>
+      <c r="AS24" s="54"/>
       <c r="AT24" s="4">
         <v>6</v>
       </c>
@@ -42942,7 +42952,7 @@
       <c r="AR25" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS25" s="50"/>
+      <c r="AS25" s="54"/>
       <c r="AT25" s="4">
         <v>6</v>
       </c>
@@ -43091,7 +43101,7 @@
       <c r="AR26" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS26" s="50"/>
+      <c r="AS26" s="54"/>
       <c r="AT26" s="4">
         <v>6</v>
       </c>
@@ -43242,7 +43252,7 @@
       <c r="AR27" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS27" s="50"/>
+      <c r="AS27" s="54"/>
       <c r="AT27" s="4">
         <v>6</v>
       </c>
@@ -43393,7 +43403,7 @@
       <c r="AR28" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS28" s="50"/>
+      <c r="AS28" s="54"/>
       <c r="AT28" s="4">
         <v>6</v>
       </c>
@@ -43544,7 +43554,7 @@
       <c r="AR29" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS29" s="50"/>
+      <c r="AS29" s="54"/>
       <c r="AT29" s="4">
         <v>6</v>
       </c>
@@ -43695,7 +43705,7 @@
       <c r="AR30" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS30" s="50"/>
+      <c r="AS30" s="54"/>
       <c r="AT30" s="4">
         <v>6</v>
       </c>
@@ -43846,7 +43856,7 @@
       <c r="AR31" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS31" s="50"/>
+      <c r="AS31" s="54"/>
       <c r="AT31" s="4">
         <v>6</v>
       </c>
@@ -43993,7 +44003,7 @@
       <c r="AR32" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS32" s="50"/>
+      <c r="AS32" s="54"/>
       <c r="AT32" s="4">
         <v>6</v>
       </c>
@@ -44140,7 +44150,7 @@
       <c r="AR33" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS33" s="50"/>
+      <c r="AS33" s="54"/>
       <c r="AT33" s="4">
         <v>6</v>
       </c>
@@ -44291,7 +44301,7 @@
       <c r="AR34" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS34" s="50"/>
+      <c r="AS34" s="54"/>
       <c r="AT34" s="4">
         <v>6</v>
       </c>
@@ -44444,7 +44454,7 @@
       <c r="AR35" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS35" s="50"/>
+      <c r="AS35" s="54"/>
       <c r="AT35" s="4">
         <v>6</v>
       </c>
@@ -44597,7 +44607,9 @@
       <c r="AR36" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS36" s="50"/>
+      <c r="AS36" s="54">
+        <v>11000006</v>
+      </c>
       <c r="AT36" s="4">
         <v>6</v>
       </c>
@@ -44754,7 +44766,7 @@
       <c r="AR37" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS37" s="50"/>
+      <c r="AS37" s="54"/>
       <c r="AT37" s="4">
         <v>6</v>
       </c>
@@ -44903,7 +44915,7 @@
       <c r="AR38" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS38" s="50"/>
+      <c r="AS38" s="54"/>
       <c r="AT38" s="4">
         <v>6</v>
       </c>
@@ -45050,7 +45062,7 @@
       <c r="AR39" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS39" s="50"/>
+      <c r="AS39" s="54"/>
       <c r="AT39" s="4">
         <v>6</v>
       </c>
@@ -45197,7 +45209,7 @@
       <c r="AR40" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS40" s="50"/>
+      <c r="AS40" s="54"/>
       <c r="AT40" s="4">
         <v>6</v>
       </c>
@@ -45354,7 +45366,7 @@
       <c r="AR41" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS41" s="50"/>
+      <c r="AS41" s="54"/>
       <c r="AT41" s="4">
         <v>6</v>
       </c>
@@ -45507,7 +45519,7 @@
       <c r="AR42" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS42" s="50"/>
+      <c r="AS42" s="54"/>
       <c r="AT42" s="4">
         <v>6</v>
       </c>
@@ -45658,7 +45670,7 @@
       <c r="AR43" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS43" s="50"/>
+      <c r="AS43" s="54"/>
       <c r="AT43" s="4">
         <v>6</v>
       </c>
@@ -45811,7 +45823,7 @@
       <c r="AR44" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS44" s="50"/>
+      <c r="AS44" s="54"/>
       <c r="AT44" s="4">
         <v>6</v>
       </c>
@@ -45962,7 +45974,7 @@
       <c r="AR45" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS45" s="50"/>
+      <c r="AS45" s="54"/>
       <c r="AT45" s="4">
         <v>6</v>
       </c>
@@ -46117,7 +46129,9 @@
       <c r="AR46" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS46" s="50"/>
+      <c r="AS46" s="54">
+        <v>11000009</v>
+      </c>
       <c r="AT46" s="4">
         <v>6</v>
       </c>
@@ -46268,7 +46282,7 @@
       <c r="AR47" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS47" s="50"/>
+      <c r="AS47" s="54"/>
       <c r="AT47" s="4">
         <v>6</v>
       </c>
@@ -46419,7 +46433,7 @@
       <c r="AR48" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS48" s="50"/>
+      <c r="AS48" s="54"/>
       <c r="AT48" s="4">
         <v>6</v>
       </c>
@@ -46572,7 +46586,7 @@
       <c r="AR49" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS49" s="50"/>
+      <c r="AS49" s="54"/>
       <c r="AT49" s="4">
         <v>6</v>
       </c>
@@ -46719,7 +46733,7 @@
       <c r="AR50" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS50" s="50"/>
+      <c r="AS50" s="54"/>
       <c r="AT50" s="4">
         <v>4</v>
       </c>
@@ -46872,7 +46886,7 @@
       <c r="AR51" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS51" s="50"/>
+      <c r="AS51" s="54"/>
       <c r="AT51" s="4">
         <v>6</v>
       </c>
@@ -47023,7 +47037,7 @@
       <c r="AR52" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS52" s="50"/>
+      <c r="AS52" s="54"/>
       <c r="AT52" s="4">
         <v>6</v>
       </c>
@@ -47174,7 +47188,7 @@
       <c r="AR53" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS53" s="50"/>
+      <c r="AS53" s="54"/>
       <c r="AT53" s="4">
         <v>6</v>
       </c>
@@ -47331,7 +47345,7 @@
       <c r="AR54" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS54" s="50"/>
+      <c r="AS54" s="54"/>
       <c r="AT54" s="4">
         <v>6</v>
       </c>
@@ -47484,7 +47498,7 @@
       <c r="AR55" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS55" s="50"/>
+      <c r="AS55" s="54"/>
       <c r="AT55" s="4">
         <v>6</v>
       </c>
@@ -47635,7 +47649,7 @@
       <c r="AR56" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS56" s="50"/>
+      <c r="AS56" s="54"/>
       <c r="AT56" s="4">
         <v>6</v>
       </c>
@@ -47790,7 +47804,7 @@
       <c r="AR57" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS57" s="50"/>
+      <c r="AS57" s="54"/>
       <c r="AT57" s="4">
         <v>6</v>
       </c>
@@ -47941,7 +47955,7 @@
       <c r="AR58" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS58" s="50"/>
+      <c r="AS58" s="54"/>
       <c r="AT58" s="4">
         <v>6</v>
       </c>
@@ -48092,7 +48106,7 @@
       <c r="AR59" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS59" s="50"/>
+      <c r="AS59" s="54"/>
       <c r="AT59" s="4">
         <v>6</v>
       </c>
@@ -48245,7 +48259,7 @@
       <c r="AR60" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS60" s="50"/>
+      <c r="AS60" s="54"/>
       <c r="AT60" s="4">
         <v>6</v>
       </c>
@@ -48396,7 +48410,7 @@
       <c r="AR61" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS61" s="50"/>
+      <c r="AS61" s="54"/>
       <c r="AT61" s="4">
         <v>6</v>
       </c>
@@ -48547,7 +48561,7 @@
       <c r="AR62" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS62" s="50"/>
+      <c r="AS62" s="54"/>
       <c r="AT62" s="4">
         <v>6</v>
       </c>
@@ -48698,7 +48712,7 @@
       <c r="AR63" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS63" s="50"/>
+      <c r="AS63" s="54"/>
       <c r="AT63" s="4">
         <v>6</v>
       </c>
@@ -48849,7 +48863,7 @@
       <c r="AR64" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS64" s="50"/>
+      <c r="AS64" s="54"/>
       <c r="AT64" s="4">
         <v>6</v>
       </c>
@@ -48998,7 +49012,7 @@
       <c r="AR65" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS65" s="50"/>
+      <c r="AS65" s="54"/>
       <c r="AT65" s="4">
         <v>6</v>
       </c>
@@ -49151,7 +49165,7 @@
       <c r="AR66" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS66" s="50"/>
+      <c r="AS66" s="54"/>
       <c r="AT66" s="4">
         <v>6</v>
       </c>
@@ -49304,7 +49318,7 @@
       <c r="AR67" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS67" s="50"/>
+      <c r="AS67" s="54"/>
       <c r="AT67" s="4">
         <v>5</v>
       </c>
@@ -49457,7 +49471,7 @@
       <c r="AR68" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS68" s="50"/>
+      <c r="AS68" s="54"/>
       <c r="AT68" s="4">
         <v>5</v>
       </c>
@@ -49612,7 +49626,7 @@
       <c r="AR69" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS69" s="50"/>
+      <c r="AS69" s="54"/>
       <c r="AT69" s="4">
         <v>5</v>
       </c>
@@ -49767,7 +49781,7 @@
       <c r="AR70" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS70" s="50"/>
+      <c r="AS70" s="54"/>
       <c r="AT70" s="4">
         <v>5</v>
       </c>
@@ -49914,7 +49928,7 @@
       <c r="AR71" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS71" s="50"/>
+      <c r="AS71" s="54"/>
       <c r="AT71" s="4">
         <v>6</v>
       </c>
@@ -50061,7 +50075,9 @@
       <c r="AR72" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS72" s="50"/>
+      <c r="AS72" s="54">
+        <v>11000004</v>
+      </c>
       <c r="AT72" s="4">
         <v>6</v>
       </c>
@@ -50212,7 +50228,7 @@
       <c r="AR73" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS73" s="50"/>
+      <c r="AS73" s="54"/>
       <c r="AT73" s="4">
         <v>6</v>
       </c>
@@ -50363,7 +50379,7 @@
       <c r="AR74" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS74" s="50"/>
+      <c r="AS74" s="54"/>
       <c r="AT74" s="4">
         <v>6</v>
       </c>
@@ -50520,7 +50536,7 @@
       <c r="AR75" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS75" s="50"/>
+      <c r="AS75" s="54"/>
       <c r="AT75" s="4">
         <v>6</v>
       </c>
@@ -50677,7 +50693,7 @@
       <c r="AR76" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS76" s="50"/>
+      <c r="AS76" s="54"/>
       <c r="AT76" s="4">
         <v>6</v>
       </c>
@@ -50828,7 +50844,7 @@
       <c r="AR77" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS77" s="50"/>
+      <c r="AS77" s="54"/>
       <c r="AT77" s="4">
         <v>6</v>
       </c>
@@ -50985,7 +51001,7 @@
       <c r="AR78" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS78" s="50"/>
+      <c r="AS78" s="54"/>
       <c r="AT78" s="4">
         <v>6</v>
       </c>
@@ -51134,7 +51150,7 @@
       <c r="AR79" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS79" s="50"/>
+      <c r="AS79" s="54"/>
       <c r="AT79" s="4">
         <v>6</v>
       </c>
@@ -51283,7 +51299,7 @@
       <c r="AR80" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS80" s="50"/>
+      <c r="AS80" s="54"/>
       <c r="AT80" s="4">
         <v>6</v>
       </c>
@@ -51436,7 +51452,7 @@
       <c r="AR81" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS81" s="50"/>
+      <c r="AS81" s="54"/>
       <c r="AT81" s="4">
         <v>6</v>
       </c>
@@ -51591,7 +51607,7 @@
       <c r="AR82" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS82" s="50"/>
+      <c r="AS82" s="54"/>
       <c r="AT82" s="4">
         <v>6</v>
       </c>
@@ -51742,7 +51758,7 @@
       <c r="AR83" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS83" s="50"/>
+      <c r="AS83" s="54"/>
       <c r="AT83" s="4">
         <v>6</v>
       </c>
@@ -51895,7 +51911,7 @@
       <c r="AR84" s="51" t="s">
         <v>784</v>
       </c>
-      <c r="AS84" s="51"/>
+      <c r="AS84" s="55"/>
       <c r="AT84" s="8">
         <v>6</v>
       </c>
@@ -52048,7 +52064,7 @@
       <c r="AR85" s="51" t="s">
         <v>784</v>
       </c>
-      <c r="AS85" s="51"/>
+      <c r="AS85" s="55"/>
       <c r="AT85" s="8">
         <v>6</v>
       </c>
@@ -52201,7 +52217,7 @@
       <c r="AR86" s="51" t="s">
         <v>784</v>
       </c>
-      <c r="AS86" s="51"/>
+      <c r="AS86" s="55"/>
       <c r="AT86" s="8">
         <v>6</v>
       </c>
@@ -52358,7 +52374,7 @@
       <c r="AR87" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS87" s="50"/>
+      <c r="AS87" s="54"/>
       <c r="AT87" s="4">
         <v>6</v>
       </c>
@@ -52509,7 +52525,7 @@
       <c r="AR88" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS88" s="50"/>
+      <c r="AS88" s="54"/>
       <c r="AT88" s="4">
         <v>6</v>
       </c>
@@ -52660,7 +52676,7 @@
       <c r="AR89" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS89" s="50"/>
+      <c r="AS89" s="54"/>
       <c r="AT89" s="4">
         <v>6</v>
       </c>
@@ -52815,7 +52831,7 @@
       <c r="AR90" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS90" s="50"/>
+      <c r="AS90" s="54"/>
       <c r="AT90" s="4">
         <v>6</v>
       </c>
@@ -52968,7 +52984,7 @@
       <c r="AR91" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS91" s="50"/>
+      <c r="AS91" s="54"/>
       <c r="AT91" s="4">
         <v>6</v>
       </c>
@@ -53119,7 +53135,7 @@
       <c r="AR92" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS92" s="50"/>
+      <c r="AS92" s="54"/>
       <c r="AT92" s="4">
         <v>6</v>
       </c>
@@ -53266,7 +53282,7 @@
       <c r="AR93" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS93" s="50"/>
+      <c r="AS93" s="54"/>
       <c r="AT93" s="4">
         <v>6</v>
       </c>
@@ -53423,7 +53439,7 @@
       <c r="AR94" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS94" s="50"/>
+      <c r="AS94" s="54"/>
       <c r="AT94" s="4">
         <v>5</v>
       </c>
@@ -53570,7 +53586,9 @@
       <c r="AR95" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS95" s="50"/>
+      <c r="AS95" s="54">
+        <v>11000002</v>
+      </c>
       <c r="AT95" s="4">
         <v>6</v>
       </c>
@@ -53725,7 +53743,7 @@
       <c r="AR96" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS96" s="50"/>
+      <c r="AS96" s="54"/>
       <c r="AT96" s="4">
         <v>6</v>
       </c>
@@ -53880,7 +53898,7 @@
       <c r="AR97" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS97" s="50"/>
+      <c r="AS97" s="54"/>
       <c r="AT97" s="4">
         <v>3</v>
       </c>
@@ -54031,7 +54049,7 @@
       <c r="AR98" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS98" s="50"/>
+      <c r="AS98" s="54"/>
       <c r="AT98" s="4">
         <v>6</v>
       </c>
@@ -54182,7 +54200,7 @@
       <c r="AR99" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS99" s="50"/>
+      <c r="AS99" s="54"/>
       <c r="AT99" s="4">
         <v>6</v>
       </c>
@@ -54333,7 +54351,9 @@
       <c r="AR100" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS100" s="50"/>
+      <c r="AS100" s="54">
+        <v>11000004</v>
+      </c>
       <c r="AT100" s="4">
         <v>6</v>
       </c>
@@ -54480,7 +54500,7 @@
       <c r="AR101" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS101" s="50"/>
+      <c r="AS101" s="54"/>
       <c r="AT101" s="4">
         <v>6</v>
       </c>
@@ -54635,7 +54655,9 @@
       <c r="AR102" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS102" s="50"/>
+      <c r="AS102" s="54">
+        <v>11000001</v>
+      </c>
       <c r="AT102" s="4">
         <v>4</v>
       </c>
@@ -54788,7 +54810,9 @@
       <c r="AR103" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS103" s="50"/>
+      <c r="AS103" s="54">
+        <v>11000010</v>
+      </c>
       <c r="AT103" s="4">
         <v>6</v>
       </c>
@@ -54945,7 +54969,7 @@
       <c r="AR104" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS104" s="50"/>
+      <c r="AS104" s="54"/>
       <c r="AT104" s="4">
         <v>6</v>
       </c>
@@ -55098,7 +55122,9 @@
       <c r="AR105" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS105" s="50"/>
+      <c r="AS105" s="54">
+        <v>11000003</v>
+      </c>
       <c r="AT105" s="4">
         <v>6</v>
       </c>
@@ -55251,7 +55277,7 @@
       <c r="AR106" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS106" s="50"/>
+      <c r="AS106" s="54"/>
       <c r="AT106" s="4">
         <v>6</v>
       </c>
@@ -55404,7 +55430,7 @@
       <c r="AR107" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS107" s="50"/>
+      <c r="AS107" s="54"/>
       <c r="AT107" s="4">
         <v>6</v>
       </c>
@@ -55555,7 +55581,7 @@
       <c r="AR108" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS108" s="50"/>
+      <c r="AS108" s="54"/>
       <c r="AT108" s="4">
         <v>4</v>
       </c>
@@ -55702,7 +55728,7 @@
       <c r="AR109" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS109" s="50"/>
+      <c r="AS109" s="54"/>
       <c r="AT109" s="4">
         <v>6</v>
       </c>
@@ -55853,7 +55879,7 @@
       <c r="AR110" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS110" s="50"/>
+      <c r="AS110" s="54"/>
       <c r="AT110" s="4">
         <v>6</v>
       </c>
@@ -56000,7 +56026,7 @@
       <c r="AR111" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS111" s="50"/>
+      <c r="AS111" s="54"/>
       <c r="AT111" s="4">
         <v>6</v>
       </c>
@@ -56147,7 +56173,7 @@
       <c r="AR112" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS112" s="50"/>
+      <c r="AS112" s="54"/>
       <c r="AT112" s="4">
         <v>6</v>
       </c>
@@ -56294,7 +56320,7 @@
       <c r="AR113" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS113" s="50"/>
+      <c r="AS113" s="54"/>
       <c r="AT113" s="4">
         <v>6</v>
       </c>
@@ -56451,7 +56477,7 @@
       <c r="AR114" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS114" s="50"/>
+      <c r="AS114" s="54"/>
       <c r="AT114" s="4">
         <v>3</v>
       </c>
@@ -56606,7 +56632,7 @@
       <c r="AR115" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS115" s="50"/>
+      <c r="AS115" s="54"/>
       <c r="AT115" s="4">
         <v>6</v>
       </c>
@@ -56765,7 +56791,7 @@
       <c r="AR116" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS116" s="50"/>
+      <c r="AS116" s="54"/>
       <c r="AT116" s="4">
         <v>6</v>
       </c>
@@ -56924,7 +56950,7 @@
       <c r="AR117" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS117" s="50"/>
+      <c r="AS117" s="54"/>
       <c r="AT117" s="4">
         <v>5</v>
       </c>
@@ -57083,7 +57109,7 @@
       <c r="AR118" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS118" s="50"/>
+      <c r="AS118" s="54"/>
       <c r="AT118" s="4">
         <v>5</v>
       </c>
@@ -57238,7 +57264,7 @@
       <c r="AR119" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS119" s="50"/>
+      <c r="AS119" s="54"/>
       <c r="AT119" s="8">
         <v>6</v>
       </c>
@@ -57395,7 +57421,7 @@
       <c r="AR120" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS120" s="50"/>
+      <c r="AS120" s="54"/>
       <c r="AT120" s="4">
         <v>5</v>
       </c>
@@ -57554,7 +57580,7 @@
       <c r="AR121" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS121" s="50"/>
+      <c r="AS121" s="54"/>
       <c r="AT121" s="4">
         <v>6</v>
       </c>
@@ -57703,7 +57729,7 @@
       <c r="AR122" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS122" s="50"/>
+      <c r="AS122" s="54"/>
       <c r="AT122" s="4">
         <v>6</v>
       </c>
@@ -57854,7 +57880,7 @@
       <c r="AR123" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS123" s="50"/>
+      <c r="AS123" s="54"/>
       <c r="AT123" s="4">
         <v>6</v>
       </c>
@@ -58007,7 +58033,7 @@
       <c r="AR124" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS124" s="50"/>
+      <c r="AS124" s="54"/>
       <c r="AT124" s="4">
         <v>6</v>
       </c>
@@ -58162,7 +58188,7 @@
       <c r="AR125" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS125" s="50"/>
+      <c r="AS125" s="54"/>
       <c r="AT125" s="4">
         <v>6</v>
       </c>
@@ -58315,7 +58341,7 @@
       <c r="AR126" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS126" s="50"/>
+      <c r="AS126" s="54"/>
       <c r="AT126" s="4">
         <v>6</v>
       </c>
@@ -58466,7 +58492,7 @@
       <c r="AR127" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS127" s="50"/>
+      <c r="AS127" s="54"/>
       <c r="AT127" s="4">
         <v>6</v>
       </c>
@@ -58619,7 +58645,7 @@
       <c r="AR128" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS128" s="50"/>
+      <c r="AS128" s="54"/>
       <c r="AT128" s="4">
         <v>6</v>
       </c>
@@ -58766,7 +58792,7 @@
       <c r="AR129" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS129" s="50"/>
+      <c r="AS129" s="54"/>
       <c r="AT129" s="4">
         <v>3</v>
       </c>
@@ -58919,7 +58945,7 @@
       <c r="AR130" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS130" s="50"/>
+      <c r="AS130" s="54"/>
       <c r="AT130" s="4">
         <v>6</v>
       </c>
@@ -59066,7 +59092,7 @@
       <c r="AR131" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS131" s="50"/>
+      <c r="AS131" s="54"/>
       <c r="AT131" s="4">
         <v>6</v>
       </c>
@@ -59217,7 +59243,7 @@
       <c r="AR132" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS132" s="50"/>
+      <c r="AS132" s="54"/>
       <c r="AT132" s="4">
         <v>6</v>
       </c>
@@ -59372,7 +59398,7 @@
       <c r="AR133" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS133" s="50"/>
+      <c r="AS133" s="54"/>
       <c r="AT133" s="4">
         <v>6</v>
       </c>
@@ -59527,7 +59553,7 @@
       <c r="AR134" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS134" s="50"/>
+      <c r="AS134" s="54"/>
       <c r="AT134" s="4">
         <v>6</v>
       </c>
@@ -59678,7 +59704,7 @@
       <c r="AR135" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS135" s="50"/>
+      <c r="AS135" s="54"/>
       <c r="AT135" s="4">
         <v>6</v>
       </c>
@@ -59829,7 +59855,7 @@
       <c r="AR136" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS136" s="50"/>
+      <c r="AS136" s="54"/>
       <c r="AT136" s="4">
         <v>6</v>
       </c>
@@ -59984,7 +60010,7 @@
       <c r="AR137" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS137" s="50"/>
+      <c r="AS137" s="54"/>
       <c r="AT137" s="4">
         <v>5</v>
       </c>
@@ -60135,7 +60161,7 @@
       <c r="AR138" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS138" s="50"/>
+      <c r="AS138" s="54"/>
       <c r="AT138" s="4">
         <v>6</v>
       </c>
@@ -60282,7 +60308,7 @@
       <c r="AR139" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS139" s="50"/>
+      <c r="AS139" s="54"/>
       <c r="AT139" s="4">
         <v>6</v>
       </c>
@@ -60431,7 +60457,7 @@
       <c r="AR140" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS140" s="50"/>
+      <c r="AS140" s="54"/>
       <c r="AT140" s="4">
         <v>6</v>
       </c>
@@ -60582,7 +60608,7 @@
       <c r="AR141" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS141" s="50"/>
+      <c r="AS141" s="54"/>
       <c r="AT141" s="4">
         <v>6</v>
       </c>
@@ -60729,7 +60755,7 @@
       <c r="AR142" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS142" s="50"/>
+      <c r="AS142" s="54"/>
       <c r="AT142" s="4">
         <v>6</v>
       </c>
@@ -60880,7 +60906,7 @@
       <c r="AR143" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS143" s="50"/>
+      <c r="AS143" s="54"/>
       <c r="AT143" s="4">
         <v>6</v>
       </c>
@@ -61031,7 +61057,7 @@
       <c r="AR144" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS144" s="50"/>
+      <c r="AS144" s="54"/>
       <c r="AT144" s="4">
         <v>6</v>
       </c>
@@ -61180,7 +61206,7 @@
       <c r="AR145" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS145" s="50"/>
+      <c r="AS145" s="54"/>
       <c r="AT145" s="4">
         <v>6</v>
       </c>
@@ -61335,7 +61361,7 @@
       <c r="AR146" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS146" s="50"/>
+      <c r="AS146" s="54"/>
       <c r="AT146" s="4">
         <v>6</v>
       </c>
@@ -61488,7 +61514,7 @@
       <c r="AR147" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS147" s="50"/>
+      <c r="AS147" s="54"/>
       <c r="AT147" s="4">
         <v>6</v>
       </c>
@@ -61645,7 +61671,7 @@
       <c r="AR148" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS148" s="50"/>
+      <c r="AS148" s="54"/>
       <c r="AT148" s="4">
         <v>6</v>
       </c>
@@ -61802,7 +61828,7 @@
       <c r="AR149" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS149" s="50"/>
+      <c r="AS149" s="54"/>
       <c r="AT149" s="4">
         <v>6</v>
       </c>
@@ -61953,7 +61979,7 @@
       <c r="AR150" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS150" s="50"/>
+      <c r="AS150" s="54"/>
       <c r="AT150" s="4">
         <v>6</v>
       </c>
@@ -62100,7 +62126,7 @@
       <c r="AR151" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS151" s="50"/>
+      <c r="AS151" s="54"/>
       <c r="AT151" s="4">
         <v>6</v>
       </c>
@@ -62249,7 +62275,7 @@
       <c r="AR152" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS152" s="50"/>
+      <c r="AS152" s="54"/>
       <c r="AT152" s="4">
         <v>6</v>
       </c>
@@ -62400,7 +62426,7 @@
       <c r="AR153" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS153" s="50"/>
+      <c r="AS153" s="54"/>
       <c r="AT153" s="4">
         <v>6</v>
       </c>
@@ -62547,7 +62573,7 @@
       <c r="AR154" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS154" s="50"/>
+      <c r="AS154" s="54"/>
       <c r="AT154" s="4">
         <v>6</v>
       </c>
@@ -62700,7 +62726,7 @@
       <c r="AR155" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS155" s="50"/>
+      <c r="AS155" s="54"/>
       <c r="AT155" s="4">
         <v>6</v>
       </c>
@@ -62851,7 +62877,7 @@
       <c r="AR156" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS156" s="50"/>
+      <c r="AS156" s="54"/>
       <c r="AT156" s="4">
         <v>6</v>
       </c>
@@ -63000,7 +63026,7 @@
       <c r="AR157" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS157" s="50"/>
+      <c r="AS157" s="54"/>
       <c r="AT157" s="4">
         <v>6</v>
       </c>
@@ -63147,7 +63173,7 @@
       <c r="AR158" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS158" s="50"/>
+      <c r="AS158" s="54"/>
       <c r="AT158" s="4">
         <v>6</v>
       </c>
@@ -63296,7 +63322,7 @@
       <c r="AR159" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS159" s="50"/>
+      <c r="AS159" s="54"/>
       <c r="AT159" s="8">
         <v>6</v>
       </c>
@@ -63443,7 +63469,7 @@
       <c r="AR160" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS160" s="50"/>
+      <c r="AS160" s="54"/>
       <c r="AT160" s="4">
         <v>6</v>
       </c>
@@ -63592,7 +63618,7 @@
       <c r="AR161" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS161" s="50"/>
+      <c r="AS161" s="54"/>
       <c r="AT161" s="4">
         <v>6</v>
       </c>
@@ -63743,7 +63769,7 @@
       <c r="AR162" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS162" s="50"/>
+      <c r="AS162" s="54"/>
       <c r="AT162" s="4">
         <v>6</v>
       </c>
@@ -63896,7 +63922,7 @@
       <c r="AR163" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS163" s="50"/>
+      <c r="AS163" s="54"/>
       <c r="AT163" s="4">
         <v>6</v>
       </c>
@@ -64047,7 +64073,7 @@
       <c r="AR164" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS164" s="50"/>
+      <c r="AS164" s="54"/>
       <c r="AT164" s="4">
         <v>6</v>
       </c>
@@ -64196,7 +64222,7 @@
       <c r="AR165" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS165" s="50"/>
+      <c r="AS165" s="54"/>
       <c r="AT165" s="8">
         <v>6</v>
       </c>
@@ -64345,7 +64371,7 @@
       <c r="AR166" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS166" s="50"/>
+      <c r="AS166" s="54"/>
       <c r="AT166" s="8">
         <v>6</v>
       </c>
@@ -64492,7 +64518,7 @@
       <c r="AR167" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS167" s="50"/>
+      <c r="AS167" s="54"/>
       <c r="AT167" s="4">
         <v>6</v>
       </c>
@@ -64641,7 +64667,7 @@
       <c r="AR168" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS168" s="50"/>
+      <c r="AS168" s="54"/>
       <c r="AT168" s="8">
         <v>6</v>
       </c>
@@ -64794,7 +64820,7 @@
       <c r="AR169" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS169" s="50"/>
+      <c r="AS169" s="54"/>
       <c r="AT169" s="4">
         <v>6</v>
       </c>
@@ -64947,7 +64973,7 @@
       <c r="AR170" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS170" s="50"/>
+      <c r="AS170" s="54"/>
       <c r="AT170" s="4">
         <v>6</v>
       </c>
@@ -65098,7 +65124,7 @@
       <c r="AR171" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS171" s="50"/>
+      <c r="AS171" s="54"/>
       <c r="AT171" s="4">
         <v>6</v>
       </c>
@@ -65255,7 +65281,7 @@
       <c r="AR172" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS172" s="50"/>
+      <c r="AS172" s="54"/>
       <c r="AT172" s="4">
         <v>6</v>
       </c>
@@ -65408,7 +65434,9 @@
       <c r="AR173" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS173" s="50"/>
+      <c r="AS173" s="54">
+        <v>11000007</v>
+      </c>
       <c r="AT173" s="4">
         <v>6</v>
       </c>
@@ -65561,7 +65589,9 @@
       <c r="AR174" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS174" s="50"/>
+      <c r="AS174" s="54">
+        <v>11000009</v>
+      </c>
       <c r="AT174" s="4">
         <v>6</v>
       </c>
@@ -65718,7 +65748,7 @@
       <c r="AR175" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS175" s="50"/>
+      <c r="AS175" s="54"/>
       <c r="AT175" s="4">
         <v>6</v>
       </c>
@@ -65869,7 +65899,7 @@
       <c r="AR176" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS176" s="50"/>
+      <c r="AS176" s="54"/>
       <c r="AT176" s="4">
         <v>6</v>
       </c>
@@ -66022,7 +66052,7 @@
       <c r="AR177" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS177" s="50"/>
+      <c r="AS177" s="54"/>
       <c r="AT177" s="4">
         <v>6</v>
       </c>
@@ -66175,7 +66205,7 @@
       <c r="AR178" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS178" s="50"/>
+      <c r="AS178" s="54"/>
       <c r="AT178" s="4">
         <v>6</v>
       </c>
@@ -66326,7 +66356,7 @@
       <c r="AR179" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS179" s="50"/>
+      <c r="AS179" s="54"/>
       <c r="AT179" s="4">
         <v>6</v>
       </c>
@@ -66481,7 +66511,7 @@
       <c r="AR180" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS180" s="50"/>
+      <c r="AS180" s="54"/>
       <c r="AT180" s="4">
         <v>5</v>
       </c>
@@ -66638,7 +66668,7 @@
       <c r="AR181" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS181" s="50"/>
+      <c r="AS181" s="54"/>
       <c r="AT181" s="4">
         <v>6</v>
       </c>
@@ -66789,7 +66819,7 @@
       <c r="AR182" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS182" s="50"/>
+      <c r="AS182" s="54"/>
       <c r="AT182" s="4">
         <v>6</v>
       </c>
@@ -66944,7 +66974,7 @@
       <c r="AR183" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS183" s="50"/>
+      <c r="AS183" s="54"/>
       <c r="AT183" s="4">
         <v>5</v>
       </c>
@@ -67097,7 +67127,7 @@
       <c r="AR184" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS184" s="50"/>
+      <c r="AS184" s="54"/>
       <c r="AT184" s="4">
         <v>6</v>
       </c>
@@ -67254,7 +67284,7 @@
       <c r="AR185" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS185" s="50"/>
+      <c r="AS185" s="54"/>
       <c r="AT185" s="4">
         <v>3</v>
       </c>
@@ -67407,7 +67437,7 @@
       <c r="AR186" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS186" s="50"/>
+      <c r="AS186" s="54"/>
       <c r="AT186" s="4">
         <v>6</v>
       </c>
@@ -67558,7 +67588,7 @@
       <c r="AR187" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS187" s="50"/>
+      <c r="AS187" s="54"/>
       <c r="AT187" s="4">
         <v>6</v>
       </c>
@@ -67705,7 +67735,7 @@
       <c r="AR188" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS188" s="50"/>
+      <c r="AS188" s="54"/>
       <c r="AT188" s="4">
         <v>3</v>
       </c>
@@ -67856,7 +67886,7 @@
       <c r="AR189" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS189" s="50"/>
+      <c r="AS189" s="54"/>
       <c r="AT189" s="4">
         <v>6</v>
       </c>
@@ -68005,7 +68035,7 @@
       <c r="AR190" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS190" s="50"/>
+      <c r="AS190" s="54"/>
       <c r="AT190" s="4">
         <v>6</v>
       </c>
@@ -68160,7 +68190,7 @@
       <c r="AR191" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS191" s="50"/>
+      <c r="AS191" s="54"/>
       <c r="AT191" s="4">
         <v>6</v>
       </c>
@@ -68315,7 +68345,7 @@
       <c r="AR192" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS192" s="50"/>
+      <c r="AS192" s="54"/>
       <c r="AT192" s="4">
         <v>6</v>
       </c>
@@ -68472,7 +68502,7 @@
       <c r="AR193" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS193" s="50"/>
+      <c r="AS193" s="54"/>
       <c r="AT193" s="4">
         <v>6</v>
       </c>
@@ -68629,7 +68659,7 @@
       <c r="AR194" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS194" s="50"/>
+      <c r="AS194" s="54"/>
       <c r="AT194" s="4">
         <v>4</v>
       </c>
@@ -68786,7 +68816,7 @@
       <c r="AR195" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS195" s="50"/>
+      <c r="AS195" s="54"/>
       <c r="AT195" s="4">
         <v>5</v>
       </c>
@@ -68943,7 +68973,7 @@
       <c r="AR196" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS196" s="50"/>
+      <c r="AS196" s="54"/>
       <c r="AT196" s="4">
         <v>5</v>
       </c>
@@ -69100,7 +69130,7 @@
       <c r="AR197" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS197" s="50"/>
+      <c r="AS197" s="54"/>
       <c r="AT197" s="4">
         <v>5</v>
       </c>
@@ -69255,7 +69285,7 @@
       <c r="AR198" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS198" s="50"/>
+      <c r="AS198" s="54"/>
       <c r="AT198" s="4">
         <v>3</v>
       </c>
@@ -69412,7 +69442,7 @@
       <c r="AR199" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS199" s="50"/>
+      <c r="AS199" s="54"/>
       <c r="AT199" s="4">
         <v>6</v>
       </c>
@@ -69563,7 +69593,7 @@
       <c r="AR200" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS200" s="50"/>
+      <c r="AS200" s="54"/>
       <c r="AT200" s="4">
         <v>6</v>
       </c>
@@ -69716,7 +69746,7 @@
       <c r="AR201" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS201" s="50"/>
+      <c r="AS201" s="54"/>
       <c r="AT201" s="4">
         <v>3</v>
       </c>
@@ -69867,7 +69897,7 @@
       <c r="AR202" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS202" s="50"/>
+      <c r="AS202" s="54"/>
       <c r="AT202" s="4">
         <v>6</v>
       </c>
@@ -70018,7 +70048,7 @@
       <c r="AR203" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS203" s="50"/>
+      <c r="AS203" s="54"/>
       <c r="AT203" s="4">
         <v>6</v>
       </c>
@@ -70171,7 +70201,7 @@
       <c r="AR204" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS204" s="50"/>
+      <c r="AS204" s="54"/>
       <c r="AT204" s="8">
         <v>6</v>
       </c>
@@ -70324,7 +70354,7 @@
       <c r="AR205" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS205" s="50"/>
+      <c r="AS205" s="54"/>
       <c r="AT205" s="4">
         <v>6</v>
       </c>
@@ -70479,7 +70509,7 @@
       <c r="AR206" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS206" s="50"/>
+      <c r="AS206" s="54"/>
       <c r="AT206" s="4">
         <v>6</v>
       </c>
@@ -70630,7 +70660,7 @@
       <c r="AR207" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS207" s="50"/>
+      <c r="AS207" s="54"/>
       <c r="AT207" s="4">
         <v>6</v>
       </c>
@@ -70783,7 +70813,7 @@
       <c r="AR208" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS208" s="50"/>
+      <c r="AS208" s="54"/>
       <c r="AT208" s="4">
         <v>6</v>
       </c>
@@ -70934,7 +70964,7 @@
       <c r="AR209" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS209" s="50"/>
+      <c r="AS209" s="54"/>
       <c r="AT209" s="4">
         <v>6</v>
       </c>
@@ -71081,7 +71111,7 @@
       <c r="AR210" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS210" s="50"/>
+      <c r="AS210" s="54"/>
       <c r="AT210" s="4">
         <v>6</v>
       </c>
@@ -71234,7 +71264,7 @@
       <c r="AR211" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS211" s="50"/>
+      <c r="AS211" s="54"/>
       <c r="AT211" s="4">
         <v>6</v>
       </c>
@@ -71385,7 +71415,7 @@
       <c r="AR212" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS212" s="50"/>
+      <c r="AS212" s="54"/>
       <c r="AT212" s="4">
         <v>6</v>
       </c>
@@ -71542,7 +71572,7 @@
       <c r="AR213" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS213" s="50"/>
+      <c r="AS213" s="54"/>
       <c r="AT213" s="4">
         <v>6</v>
       </c>
@@ -71689,7 +71719,7 @@
       <c r="AR214" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS214" s="50"/>
+      <c r="AS214" s="54"/>
       <c r="AT214" s="4">
         <v>6</v>
       </c>
@@ -71846,7 +71876,7 @@
       <c r="AR215" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS215" s="50"/>
+      <c r="AS215" s="54"/>
       <c r="AT215" s="4">
         <v>6</v>
       </c>
@@ -71997,7 +72027,9 @@
       <c r="AR216" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS216" s="50"/>
+      <c r="AS216" s="54">
+        <v>11000001</v>
+      </c>
       <c r="AT216" s="4">
         <v>6</v>
       </c>
@@ -72150,7 +72182,7 @@
       <c r="AR217" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS217" s="50"/>
+      <c r="AS217" s="54"/>
       <c r="AT217" s="4">
         <v>6</v>
       </c>
@@ -72303,7 +72335,9 @@
       <c r="AR218" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS218" s="50"/>
+      <c r="AS218" s="54">
+        <v>11000008</v>
+      </c>
       <c r="AT218" s="4">
         <v>6</v>
       </c>
@@ -72456,7 +72490,7 @@
       <c r="AR219" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS219" s="50"/>
+      <c r="AS219" s="54"/>
       <c r="AT219" s="4">
         <v>6</v>
       </c>
@@ -72607,7 +72641,7 @@
       <c r="AR220" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS220" s="50"/>
+      <c r="AS220" s="54"/>
       <c r="AT220" s="4">
         <v>6</v>
       </c>
@@ -72764,7 +72798,7 @@
       <c r="AR221" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS221" s="50"/>
+      <c r="AS221" s="54"/>
       <c r="AT221" s="4">
         <v>6</v>
       </c>
@@ -72915,7 +72949,7 @@
       <c r="AR222" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS222" s="50"/>
+      <c r="AS222" s="54"/>
       <c r="AT222" s="4">
         <v>6</v>
       </c>
@@ -73066,7 +73100,7 @@
       <c r="AR223" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS223" s="50"/>
+      <c r="AS223" s="54"/>
       <c r="AT223" s="4">
         <v>6</v>
       </c>
@@ -73221,7 +73255,7 @@
       <c r="AR224" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS224" s="50"/>
+      <c r="AS224" s="54"/>
       <c r="AT224" s="4">
         <v>6</v>
       </c>
@@ -73376,7 +73410,7 @@
       <c r="AR225" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS225" s="50"/>
+      <c r="AS225" s="54"/>
       <c r="AT225" s="4">
         <v>6</v>
       </c>
@@ -73529,7 +73563,7 @@
       <c r="AR226" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS226" s="50"/>
+      <c r="AS226" s="54"/>
       <c r="AT226" s="4">
         <v>6</v>
       </c>
@@ -73680,7 +73714,7 @@
       <c r="AR227" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS227" s="50"/>
+      <c r="AS227" s="54"/>
       <c r="AT227" s="4">
         <v>6</v>
       </c>
@@ -73833,7 +73867,7 @@
       <c r="AR228" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS228" s="50"/>
+      <c r="AS228" s="54"/>
       <c r="AT228" s="4">
         <v>6</v>
       </c>
@@ -73986,7 +74020,7 @@
       <c r="AR229" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS229" s="50"/>
+      <c r="AS229" s="54"/>
       <c r="AT229" s="4">
         <v>6</v>
       </c>
@@ -74139,7 +74173,7 @@
       <c r="AR230" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS230" s="50"/>
+      <c r="AS230" s="54"/>
       <c r="AT230" s="4">
         <v>6</v>
       </c>
@@ -74292,7 +74326,7 @@
       <c r="AR231" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS231" s="50"/>
+      <c r="AS231" s="54"/>
       <c r="AT231" s="4">
         <v>6</v>
       </c>
@@ -74441,7 +74475,7 @@
       <c r="AR232" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS232" s="50"/>
+      <c r="AS232" s="54"/>
       <c r="AT232" s="4">
         <v>6</v>
       </c>
@@ -74598,7 +74632,7 @@
       <c r="AR233" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS233" s="50"/>
+      <c r="AS233" s="54"/>
       <c r="AT233" s="4">
         <v>6</v>
       </c>
@@ -74749,7 +74783,7 @@
       <c r="AR234" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS234" s="50"/>
+      <c r="AS234" s="54"/>
       <c r="AT234" s="4">
         <v>6</v>
       </c>
@@ -74902,7 +74936,7 @@
       <c r="AR235" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS235" s="50"/>
+      <c r="AS235" s="54"/>
       <c r="AT235" s="4">
         <v>6</v>
       </c>
@@ -75055,7 +75089,7 @@
       <c r="AR236" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS236" s="50"/>
+      <c r="AS236" s="54"/>
       <c r="AT236" s="4">
         <v>6</v>
       </c>
@@ -75210,7 +75244,7 @@
       <c r="AR237" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS237" s="50"/>
+      <c r="AS237" s="54"/>
       <c r="AT237" s="4">
         <v>6</v>
       </c>
@@ -75357,7 +75391,7 @@
       <c r="AR238" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS238" s="50"/>
+      <c r="AS238" s="54"/>
       <c r="AT238" s="4">
         <v>6</v>
       </c>
@@ -75512,7 +75546,7 @@
       <c r="AR239" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS239" s="50"/>
+      <c r="AS239" s="54"/>
       <c r="AT239" s="4">
         <v>6</v>
       </c>
@@ -75659,7 +75693,7 @@
       <c r="AR240" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS240" s="50"/>
+      <c r="AS240" s="54"/>
       <c r="AT240" s="4">
         <v>6</v>
       </c>
@@ -75816,7 +75850,7 @@
       <c r="AR241" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS241" s="50"/>
+      <c r="AS241" s="54"/>
       <c r="AT241" s="4">
         <v>3</v>
       </c>
@@ -75963,7 +75997,7 @@
       <c r="AR242" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS242" s="50"/>
+      <c r="AS242" s="54"/>
       <c r="AT242" s="4">
         <v>6</v>
       </c>
@@ -76114,7 +76148,7 @@
       <c r="AR243" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS243" s="50"/>
+      <c r="AS243" s="54"/>
       <c r="AT243" s="4">
         <v>6</v>
       </c>
@@ -76267,7 +76301,7 @@
       <c r="AR244" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS244" s="50"/>
+      <c r="AS244" s="54"/>
       <c r="AT244" s="4">
         <v>6</v>
       </c>
@@ -76424,7 +76458,7 @@
       <c r="AR245" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS245" s="50"/>
+      <c r="AS245" s="54"/>
       <c r="AT245" s="4">
         <v>4</v>
       </c>
@@ -76571,7 +76605,7 @@
       <c r="AR246" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS246" s="50"/>
+      <c r="AS246" s="54"/>
       <c r="AT246" s="4">
         <v>4</v>
       </c>
@@ -76726,7 +76760,7 @@
       <c r="AR247" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS247" s="50"/>
+      <c r="AS247" s="54"/>
       <c r="AT247" s="4">
         <v>6</v>
       </c>
@@ -76877,7 +76911,7 @@
       <c r="AR248" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS248" s="50"/>
+      <c r="AS248" s="54"/>
       <c r="AT248" s="4">
         <v>6</v>
       </c>
@@ -77024,7 +77058,7 @@
       <c r="AR249" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS249" s="50"/>
+      <c r="AS249" s="54"/>
       <c r="AT249" s="4">
         <v>6</v>
       </c>
@@ -77179,7 +77213,7 @@
       <c r="AR250" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS250" s="50"/>
+      <c r="AS250" s="54"/>
       <c r="AT250" s="4">
         <v>3</v>
       </c>
@@ -77330,7 +77364,7 @@
       <c r="AR251" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS251" s="50"/>
+      <c r="AS251" s="54"/>
       <c r="AT251" s="4">
         <v>6</v>
       </c>
@@ -77481,7 +77515,7 @@
       <c r="AR252" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS252" s="50"/>
+      <c r="AS252" s="54"/>
       <c r="AT252" s="4">
         <v>6</v>
       </c>
@@ -77632,7 +77666,7 @@
       <c r="AR253" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS253" s="50"/>
+      <c r="AS253" s="54"/>
       <c r="AT253" s="4">
         <v>6</v>
       </c>
@@ -77785,7 +77819,7 @@
       <c r="AR254" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS254" s="50"/>
+      <c r="AS254" s="54"/>
       <c r="AT254" s="4">
         <v>6</v>
       </c>
@@ -77942,7 +77976,7 @@
       <c r="AR255" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS255" s="50"/>
+      <c r="AS255" s="54"/>
       <c r="AT255" s="4">
         <v>6</v>
       </c>
@@ -78093,7 +78127,7 @@
       <c r="AR256" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS256" s="50"/>
+      <c r="AS256" s="54"/>
       <c r="AT256" s="4">
         <v>6</v>
       </c>
@@ -78246,7 +78280,7 @@
       <c r="AR257" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS257" s="50"/>
+      <c r="AS257" s="54"/>
       <c r="AT257" s="4">
         <v>6</v>
       </c>
@@ -78401,7 +78435,7 @@
       <c r="AR258" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS258" s="50"/>
+      <c r="AS258" s="54"/>
       <c r="AT258" s="4">
         <v>6</v>
       </c>
@@ -78558,7 +78592,7 @@
       <c r="AR259" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS259" s="50"/>
+      <c r="AS259" s="54"/>
       <c r="AT259" s="4">
         <v>6</v>
       </c>
@@ -78715,7 +78749,7 @@
       <c r="AR260" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS260" s="50"/>
+      <c r="AS260" s="54"/>
       <c r="AT260" s="4">
         <v>6</v>
       </c>
@@ -78868,7 +78902,7 @@
       <c r="AR261" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS261" s="50"/>
+      <c r="AS261" s="54"/>
       <c r="AT261" s="4">
         <v>6</v>
       </c>
@@ -79019,7 +79053,7 @@
       <c r="AR262" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS262" s="50"/>
+      <c r="AS262" s="54"/>
       <c r="AT262" s="4">
         <v>6</v>
       </c>
@@ -79168,7 +79202,7 @@
       <c r="AR263" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS263" s="50"/>
+      <c r="AS263" s="54"/>
       <c r="AT263" s="4">
         <v>6</v>
       </c>
@@ -79319,7 +79353,7 @@
       <c r="AR264" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS264" s="50"/>
+      <c r="AS264" s="54"/>
       <c r="AT264" s="4">
         <v>6</v>
       </c>
@@ -79470,7 +79504,7 @@
       <c r="AR265" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS265" s="50"/>
+      <c r="AS265" s="54"/>
       <c r="AT265" s="4">
         <v>6</v>
       </c>
@@ -79621,7 +79655,7 @@
       <c r="AR266" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS266" s="50"/>
+      <c r="AS266" s="54"/>
       <c r="AT266" s="4">
         <v>6</v>
       </c>
@@ -79778,7 +79812,7 @@
       <c r="AR267" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS267" s="50"/>
+      <c r="AS267" s="54"/>
       <c r="AT267" s="4">
         <v>6</v>
       </c>
@@ -79929,7 +79963,7 @@
       <c r="AR268" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS268" s="50"/>
+      <c r="AS268" s="54"/>
       <c r="AT268" s="4">
         <v>6</v>
       </c>
@@ -80080,7 +80114,7 @@
       <c r="AR269" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS269" s="50"/>
+      <c r="AS269" s="54"/>
       <c r="AT269" s="4">
         <v>6</v>
       </c>
@@ -80231,7 +80265,7 @@
       <c r="AR270" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS270" s="50"/>
+      <c r="AS270" s="54"/>
       <c r="AT270" s="4">
         <v>6</v>
       </c>
@@ -80388,7 +80422,7 @@
       <c r="AR271" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS271" s="50"/>
+      <c r="AS271" s="54"/>
       <c r="AT271" s="4">
         <v>5</v>
       </c>
@@ -80545,7 +80579,7 @@
       <c r="AR272" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS272" s="50"/>
+      <c r="AS272" s="54"/>
       <c r="AT272" s="4">
         <v>6</v>
       </c>
@@ -80702,7 +80736,7 @@
       <c r="AR273" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS273" s="50"/>
+      <c r="AS273" s="54"/>
       <c r="AT273" s="4">
         <v>3</v>
       </c>
@@ -80853,7 +80887,7 @@
       <c r="AR274" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS274" s="50"/>
+      <c r="AS274" s="54"/>
       <c r="AT274" s="4">
         <v>6</v>
       </c>
@@ -81006,7 +81040,7 @@
       <c r="AR275" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS275" s="50"/>
+      <c r="AS275" s="54"/>
       <c r="AT275" s="4">
         <v>6</v>
       </c>
@@ -81153,7 +81187,7 @@
       <c r="AR276" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS276" s="50"/>
+      <c r="AS276" s="54"/>
       <c r="AT276" s="4">
         <v>6</v>
       </c>
@@ -81306,7 +81340,7 @@
       <c r="AR277" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS277" s="50"/>
+      <c r="AS277" s="54"/>
       <c r="AT277" s="4">
         <v>6</v>
       </c>
@@ -81461,7 +81495,7 @@
       <c r="AR278" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS278" s="50"/>
+      <c r="AS278" s="54"/>
       <c r="AT278" s="4">
         <v>6</v>
       </c>
@@ -81612,7 +81646,7 @@
       <c r="AR279" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS279" s="50"/>
+      <c r="AS279" s="54"/>
       <c r="AT279" s="4">
         <v>6</v>
       </c>
@@ -81763,7 +81797,7 @@
       <c r="AR280" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS280" s="50"/>
+      <c r="AS280" s="54"/>
       <c r="AT280" s="4">
         <v>6</v>
       </c>
@@ -81916,7 +81950,7 @@
       <c r="AR281" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS281" s="50"/>
+      <c r="AS281" s="54"/>
       <c r="AT281" s="4">
         <v>6</v>
       </c>
@@ -82069,7 +82103,7 @@
       <c r="AR282" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS282" s="50"/>
+      <c r="AS282" s="54"/>
       <c r="AT282" s="4">
         <v>6</v>
       </c>
@@ -82222,7 +82256,7 @@
       <c r="AR283" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS283" s="50"/>
+      <c r="AS283" s="54"/>
       <c r="AT283" s="4">
         <v>6</v>
       </c>
@@ -82375,7 +82409,7 @@
       <c r="AR284" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS284" s="50"/>
+      <c r="AS284" s="54"/>
       <c r="AT284" s="4">
         <v>6</v>
       </c>
@@ -82528,7 +82562,9 @@
       <c r="AR285" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS285" s="50"/>
+      <c r="AS285" s="54">
+        <v>11000007</v>
+      </c>
       <c r="AT285" s="4">
         <v>5</v>
       </c>
@@ -82677,7 +82713,7 @@
       <c r="AR286" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS286" s="50"/>
+      <c r="AS286" s="54"/>
       <c r="AT286" s="4">
         <v>6</v>
       </c>
@@ -82828,7 +82864,7 @@
       <c r="AR287" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS287" s="50"/>
+      <c r="AS287" s="54"/>
       <c r="AT287" s="4">
         <v>6</v>
       </c>
@@ -82979,7 +83015,7 @@
       <c r="AR288" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS288" s="50"/>
+      <c r="AS288" s="54"/>
       <c r="AT288" s="8">
         <v>6</v>
       </c>
@@ -83132,7 +83168,7 @@
       <c r="AR289" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS289" s="50"/>
+      <c r="AS289" s="54"/>
       <c r="AT289" s="4">
         <v>6</v>
       </c>
@@ -83289,7 +83325,7 @@
       <c r="AR290" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS290" s="50"/>
+      <c r="AS290" s="54"/>
       <c r="AT290" s="8">
         <v>6</v>
       </c>
@@ -83444,7 +83480,7 @@
       <c r="AR291" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS291" s="50"/>
+      <c r="AS291" s="54"/>
       <c r="AT291" s="4">
         <v>6</v>
       </c>
@@ -83597,7 +83633,7 @@
       <c r="AR292" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS292" s="50"/>
+      <c r="AS292" s="54"/>
       <c r="AT292" s="4">
         <v>6</v>
       </c>
@@ -83750,7 +83786,7 @@
       <c r="AR293" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS293" s="50"/>
+      <c r="AS293" s="54"/>
       <c r="AT293" s="4">
         <v>6</v>
       </c>
@@ -83907,7 +83943,7 @@
       <c r="AR294" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS294" s="50"/>
+      <c r="AS294" s="54"/>
       <c r="AT294" s="4">
         <v>6</v>
       </c>
@@ -84058,7 +84094,7 @@
       <c r="AR295" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS295" s="50"/>
+      <c r="AS295" s="54"/>
       <c r="AT295" s="4">
         <v>6</v>
       </c>
@@ -84211,7 +84247,7 @@
       <c r="AR296" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS296" s="50"/>
+      <c r="AS296" s="54"/>
       <c r="AT296" s="8">
         <v>6</v>
       </c>
@@ -84364,7 +84400,7 @@
       <c r="AR297" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS297" s="50"/>
+      <c r="AS297" s="54"/>
       <c r="AT297" s="4">
         <v>6</v>
       </c>
@@ -84517,7 +84553,7 @@
       <c r="AR298" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS298" s="50"/>
+      <c r="AS298" s="54"/>
       <c r="AT298" s="4">
         <v>6</v>
       </c>
@@ -84668,7 +84704,7 @@
       <c r="AR299" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS299" s="50"/>
+      <c r="AS299" s="54"/>
       <c r="AT299" s="4">
         <v>6</v>
       </c>
@@ -84819,7 +84855,7 @@
       <c r="AR300" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS300" s="50"/>
+      <c r="AS300" s="54"/>
       <c r="AT300" s="4">
         <v>6</v>
       </c>
@@ -84976,7 +85012,9 @@
       <c r="AR301" s="50" t="s">
         <v>784</v>
       </c>
-      <c r="AS301" s="50"/>
+      <c r="AS301" s="54">
+        <v>11000002</v>
+      </c>
       <c r="AT301" s="4">
         <v>3</v>
       </c>
@@ -87166,37 +87204,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 J6:K9 K12 K14">
-    <cfRule type="cellIs" dxfId="76" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="35" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="75" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="74" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="32" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="73" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="31" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="72" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="27" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="71" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -87214,13 +87252,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="70" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="69" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -87238,19 +87276,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="68" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="69" priority="13" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -87267,31 +87305,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="63" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="61" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="5" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -87320,13 +87358,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix the item and drop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -39366,10 +39366,10 @@
   <dimension ref="A1:AZ303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AB73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AB283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AT86" sqref="AT86"/>
+      <selection pane="bottomRight" activeCell="AI291" sqref="AI291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -57317,9 +57317,11 @@
       </c>
       <c r="AS117" s="54"/>
       <c r="AT117" s="4">
-        <v>22011003</v>
-      </c>
-      <c r="AU117" s="4"/>
+        <v>22011178</v>
+      </c>
+      <c r="AU117" s="4">
+        <v>22011179</v>
+      </c>
       <c r="AV117" s="4">
         <v>114</v>
       </c>
@@ -57634,12 +57636,8 @@
         <v>782</v>
       </c>
       <c r="AS119" s="54"/>
-      <c r="AT119" s="8">
-        <v>22011178</v>
-      </c>
-      <c r="AU119" s="8">
-        <v>22011179</v>
-      </c>
+      <c r="AT119" s="8"/>
+      <c r="AU119" s="8"/>
       <c r="AV119" s="8">
         <v>116</v>
       </c>
@@ -83708,9 +83706,7 @@
         <v>782</v>
       </c>
       <c r="AS289" s="54"/>
-      <c r="AT289" s="4">
-        <v>22011070</v>
-      </c>
+      <c r="AT289" s="8"/>
       <c r="AU289" s="4"/>
       <c r="AV289" s="4">
         <v>286</v>
@@ -83866,9 +83862,7 @@
         <v>782</v>
       </c>
       <c r="AS290" s="54"/>
-      <c r="AT290" s="8">
-        <v>22011018</v>
-      </c>
+      <c r="AT290" s="8"/>
       <c r="AU290" s="8"/>
       <c r="AV290" s="8">
         <v>287</v>
@@ -84331,7 +84325,7 @@
       </c>
       <c r="AS293" s="54"/>
       <c r="AT293" s="4">
-        <v>22011098</v>
+        <v>22011097</v>
       </c>
       <c r="AU293" s="4"/>
       <c r="AV293" s="4">
@@ -84490,9 +84484,7 @@
       <c r="AS294" s="54">
         <v>11000007</v>
       </c>
-      <c r="AT294" s="4">
-        <v>22011097</v>
-      </c>
+      <c r="AT294" s="8"/>
       <c r="AU294" s="4"/>
       <c r="AV294" s="4">
         <v>291</v>
@@ -85098,7 +85090,9 @@
         <v>782</v>
       </c>
       <c r="AS298" s="54"/>
-      <c r="AT298" s="4"/>
+      <c r="AT298" s="4">
+        <v>22011070</v>
+      </c>
       <c r="AU298" s="4"/>
       <c r="AV298" s="4">
         <v>295</v>
@@ -85556,7 +85550,9 @@
       <c r="AS301" s="54">
         <v>11000002</v>
       </c>
-      <c r="AT301" s="4"/>
+      <c r="AT301" s="4">
+        <v>22011098</v>
+      </c>
       <c r="AU301" s="4"/>
       <c r="AV301" s="4">
         <v>298</v>

</xml_diff>

<commit_message>
turn 2 skill to spike skill #28
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -3495,10 +3495,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>魔法，光环</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>状态</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3892,6 +3888,10 @@
   </si>
   <si>
     <t>克洛玛古斯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8190,11 +8190,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="295799712"/>
-        <c:axId val="295800272"/>
+        <c:axId val="331921248"/>
+        <c:axId val="410598672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="295799712"/>
+        <c:axId val="331921248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8237,7 +8237,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295800272"/>
+        <c:crossAx val="410598672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8245,7 +8245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295800272"/>
+        <c:axId val="410598672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8296,7 +8296,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295799712"/>
+        <c:crossAx val="331921248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8666,11 +8666,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="493217952"/>
-        <c:axId val="493218512"/>
+        <c:axId val="410600912"/>
+        <c:axId val="410601472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="493217952"/>
+        <c:axId val="410600912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8713,7 +8713,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493218512"/>
+        <c:crossAx val="410601472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8721,7 +8721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="493218512"/>
+        <c:axId val="410601472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8772,7 +8772,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493217952"/>
+        <c:crossAx val="410600912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10534,15 +10534,15 @@
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55310001</v>
+            <v>55300012</v>
           </cell>
           <cell r="X64">
-            <v>100</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55310002</v>
+            <v>55300013</v>
           </cell>
           <cell r="X65">
             <v>15</v>
@@ -10550,31 +10550,31 @@
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55310003</v>
+            <v>55310001</v>
           </cell>
           <cell r="X66">
-            <v>13</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55400001</v>
+            <v>55310002</v>
           </cell>
           <cell r="X67">
-            <v>80</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55400002</v>
+            <v>55310003</v>
           </cell>
           <cell r="X68">
-            <v>80</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55400003</v>
+            <v>55400001</v>
           </cell>
           <cell r="X69">
             <v>80</v>
@@ -10582,7 +10582,7 @@
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55400004</v>
+            <v>55400002</v>
           </cell>
           <cell r="X70">
             <v>80</v>
@@ -10590,47 +10590,47 @@
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55400005</v>
+            <v>55400003</v>
           </cell>
           <cell r="X71">
-            <v>55</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55400006</v>
+            <v>55400005</v>
           </cell>
           <cell r="X72">
-            <v>30</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55400007</v>
+            <v>55400006</v>
           </cell>
           <cell r="X73">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55410001</v>
+            <v>55400007</v>
           </cell>
           <cell r="X74">
-            <v>50</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55500001</v>
+            <v>55410001</v>
           </cell>
           <cell r="X75">
-            <v>5</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55500002</v>
+            <v>55500001</v>
           </cell>
           <cell r="X76">
             <v>5</v>
@@ -10638,7 +10638,7 @@
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55500003</v>
+            <v>55500002</v>
           </cell>
           <cell r="X77">
             <v>5</v>
@@ -10646,7 +10646,7 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55500004</v>
+            <v>55500003</v>
           </cell>
           <cell r="X78">
             <v>5</v>
@@ -10654,7 +10654,7 @@
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55500005</v>
+            <v>55500004</v>
           </cell>
           <cell r="X79">
             <v>5</v>
@@ -10662,7 +10662,7 @@
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55500006</v>
+            <v>55500005</v>
           </cell>
           <cell r="X80">
             <v>5</v>
@@ -10670,7 +10670,7 @@
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55500007</v>
+            <v>55500006</v>
           </cell>
           <cell r="X81">
             <v>5</v>
@@ -10678,7 +10678,7 @@
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55500008</v>
+            <v>55500007</v>
           </cell>
           <cell r="X82">
             <v>5</v>
@@ -10686,7 +10686,7 @@
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55500009</v>
+            <v>55500008</v>
           </cell>
           <cell r="X83">
             <v>5</v>
@@ -10694,7 +10694,7 @@
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55500010</v>
+            <v>55500009</v>
           </cell>
           <cell r="X84">
             <v>5</v>
@@ -10702,7 +10702,7 @@
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500011</v>
+            <v>55500010</v>
           </cell>
           <cell r="X85">
             <v>5</v>
@@ -10710,7 +10710,7 @@
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500012</v>
+            <v>55500011</v>
           </cell>
           <cell r="X86">
             <v>5</v>
@@ -10718,7 +10718,7 @@
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500013</v>
+            <v>55500012</v>
           </cell>
           <cell r="X87">
             <v>5</v>
@@ -10726,7 +10726,7 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500014</v>
+            <v>55500013</v>
           </cell>
           <cell r="X88">
             <v>5</v>
@@ -10734,7 +10734,7 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55500015</v>
+            <v>55500014</v>
           </cell>
           <cell r="X89">
             <v>5</v>
@@ -10742,7 +10742,7 @@
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55500016</v>
+            <v>55500015</v>
           </cell>
           <cell r="X90">
             <v>5</v>
@@ -10750,23 +10750,23 @@
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55510001</v>
+            <v>55500016</v>
           </cell>
           <cell r="X91">
-            <v>12</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55510002</v>
+            <v>55510001</v>
           </cell>
           <cell r="X92">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55510003</v>
+            <v>55510002</v>
           </cell>
           <cell r="X93">
             <v>15</v>
@@ -10774,87 +10774,87 @@
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55510004</v>
+            <v>55510003</v>
           </cell>
           <cell r="X94">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55510006</v>
+            <v>55510004</v>
           </cell>
           <cell r="X95">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55510007</v>
+            <v>55510006</v>
           </cell>
           <cell r="X96">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55510009</v>
+            <v>55510007</v>
           </cell>
           <cell r="X97">
-            <v>50</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55510010</v>
+            <v>55510009</v>
           </cell>
           <cell r="X98">
-            <v>5</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55510011</v>
+            <v>55510010</v>
           </cell>
           <cell r="X99">
-            <v>15</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55510012</v>
+            <v>55510011</v>
           </cell>
           <cell r="X100">
-            <v>62</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510013</v>
+            <v>55510012</v>
           </cell>
           <cell r="X101">
-            <v>12</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510014</v>
+            <v>55510013</v>
           </cell>
           <cell r="X102">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55510018</v>
+            <v>55510014</v>
           </cell>
           <cell r="X103">
-            <v>37</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55510019</v>
+            <v>55510018</v>
           </cell>
           <cell r="X104">
             <v>37</v>
@@ -10862,47 +10862,47 @@
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55520001</v>
+            <v>55510019</v>
           </cell>
           <cell r="X105">
-            <v>-25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55520002</v>
+            <v>55520001</v>
           </cell>
           <cell r="X106">
-            <v>62</v>
+            <v>-25</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55520003</v>
+            <v>55520002</v>
           </cell>
           <cell r="X107">
-            <v>27</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55600001</v>
+            <v>55520003</v>
           </cell>
           <cell r="X108">
-            <v>8</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55600002</v>
+            <v>55600001</v>
           </cell>
           <cell r="X109">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55600003</v>
+            <v>55600002</v>
           </cell>
           <cell r="X110">
             <v>10</v>
@@ -11602,7 +11602,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39494,10 +39494,10 @@
   <dimension ref="A1:BA304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C287" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I301" sqref="I301"/>
+      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -39668,10 +39668,10 @@
         <v>826</v>
       </c>
       <c r="AT1" s="56" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AU1" s="56" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AV1" s="16" t="s">
         <v>313</v>
@@ -39680,7 +39680,7 @@
         <v>312</v>
       </c>
       <c r="AX1" s="14" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AY1" s="16" t="s">
         <v>651</v>
@@ -39829,10 +39829,10 @@
         <v>827</v>
       </c>
       <c r="AT2" s="57" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AU2" s="57" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>285</v>
@@ -39841,7 +39841,7 @@
         <v>286</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>285</v>
@@ -39927,16 +39927,16 @@
         <v>296</v>
       </c>
       <c r="Y3" s="40" t="s">
+        <v>876</v>
+      </c>
+      <c r="Z3" s="40" t="s">
         <v>877</v>
       </c>
-      <c r="Z3" s="40" t="s">
+      <c r="AA3" s="40" t="s">
         <v>878</v>
       </c>
-      <c r="AA3" s="40" t="s">
+      <c r="AB3" s="40" t="s">
         <v>879</v>
-      </c>
-      <c r="AB3" s="40" t="s">
-        <v>880</v>
       </c>
       <c r="AC3" s="40" t="s">
         <v>752</v>
@@ -39990,10 +39990,10 @@
         <v>828</v>
       </c>
       <c r="AT3" s="58" t="s">
+        <v>923</v>
+      </c>
+      <c r="AU3" s="58" t="s">
         <v>924</v>
-      </c>
-      <c r="AU3" s="58" t="s">
-        <v>925</v>
       </c>
       <c r="AV3" s="6" t="s">
         <v>298</v>
@@ -40002,7 +40002,7 @@
         <v>297</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="AY3" s="17" t="s">
         <v>652</v>
@@ -40159,7 +40159,7 @@
       </c>
       <c r="AW4" s="4"/>
       <c r="AX4" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY4" s="18">
         <v>0</v>
@@ -40316,7 +40316,7 @@
       </c>
       <c r="AW5" s="4"/>
       <c r="AX5" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY5" s="18">
         <v>0</v>
@@ -40467,7 +40467,7 @@
       </c>
       <c r="AW6" s="4"/>
       <c r="AX6" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY6" s="18">
         <v>0</v>
@@ -40620,7 +40620,7 @@
       </c>
       <c r="AW7" s="4"/>
       <c r="AX7" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY7" s="18">
         <v>0</v>
@@ -40643,7 +40643,7 @@
         <v>319</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E8" s="4">
         <v>3</v>
@@ -40773,7 +40773,7 @@
       </c>
       <c r="AW8" s="4"/>
       <c r="AX8" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY8" s="18">
         <v>0</v>
@@ -40936,7 +40936,7 @@
       </c>
       <c r="AW9" s="4"/>
       <c r="AX9" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY9" s="18">
         <v>0</v>
@@ -41091,7 +41091,7 @@
       </c>
       <c r="AW10" s="4"/>
       <c r="AX10" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY10" s="18">
         <v>0</v>
@@ -41244,7 +41244,7 @@
       </c>
       <c r="AW11" s="4"/>
       <c r="AX11" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY11" s="18">
         <v>0</v>
@@ -41403,7 +41403,7 @@
       </c>
       <c r="AW12" s="4"/>
       <c r="AX12" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY12" s="18">
         <v>0</v>
@@ -41556,7 +41556,7 @@
       </c>
       <c r="AW13" s="4"/>
       <c r="AX13" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY13" s="18">
         <v>0</v>
@@ -41717,7 +41717,7 @@
       </c>
       <c r="AW14" s="4"/>
       <c r="AX14" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY14" s="18">
         <v>0</v>
@@ -41872,7 +41872,7 @@
       </c>
       <c r="AW15" s="4"/>
       <c r="AX15" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY15" s="18">
         <v>0</v>
@@ -42023,7 +42023,7 @@
       </c>
       <c r="AW16" s="4"/>
       <c r="AX16" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY16" s="18">
         <v>0</v>
@@ -42176,7 +42176,7 @@
       </c>
       <c r="AW17" s="4"/>
       <c r="AX17" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY17" s="18">
         <v>0</v>
@@ -42329,7 +42329,7 @@
       </c>
       <c r="AW18" s="4"/>
       <c r="AX18" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY18" s="18">
         <v>0</v>
@@ -42482,7 +42482,7 @@
       </c>
       <c r="AW19" s="4"/>
       <c r="AX19" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY19" s="18">
         <v>0</v>
@@ -42635,7 +42635,7 @@
       </c>
       <c r="AW20" s="4"/>
       <c r="AX20" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY20" s="18">
         <v>0</v>
@@ -42788,7 +42788,7 @@
       </c>
       <c r="AW21" s="4"/>
       <c r="AX21" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY21" s="18">
         <v>0</v>
@@ -42941,7 +42941,7 @@
       </c>
       <c r="AW22" s="4"/>
       <c r="AX22" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY22" s="18">
         <v>0</v>
@@ -43096,7 +43096,7 @@
       </c>
       <c r="AW23" s="4"/>
       <c r="AX23" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY23" s="18">
         <v>0</v>
@@ -43251,7 +43251,7 @@
       </c>
       <c r="AW24" s="4"/>
       <c r="AX24" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY24" s="18">
         <v>0</v>
@@ -43408,7 +43408,7 @@
       </c>
       <c r="AW25" s="4"/>
       <c r="AX25" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY25" s="18">
         <v>0</v>
@@ -43561,7 +43561,7 @@
       </c>
       <c r="AW26" s="4"/>
       <c r="AX26" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY26" s="18">
         <v>0</v>
@@ -43718,7 +43718,7 @@
       </c>
       <c r="AW27" s="4"/>
       <c r="AX27" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY27" s="18">
         <v>0</v>
@@ -43873,7 +43873,7 @@
       </c>
       <c r="AW28" s="4"/>
       <c r="AX28" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY28" s="18">
         <v>0</v>
@@ -44032,7 +44032,7 @@
       </c>
       <c r="AW29" s="4"/>
       <c r="AX29" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY29" s="18">
         <v>0</v>
@@ -44187,7 +44187,7 @@
       </c>
       <c r="AW30" s="4"/>
       <c r="AX30" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY30" s="18">
         <v>0</v>
@@ -44210,7 +44210,7 @@
         <v>484</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E31" s="4">
         <v>3</v>
@@ -44344,7 +44344,7 @@
       </c>
       <c r="AW31" s="4"/>
       <c r="AX31" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY31" s="18">
         <v>0</v>
@@ -44495,7 +44495,7 @@
       </c>
       <c r="AW32" s="4"/>
       <c r="AX32" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY32" s="18">
         <v>0</v>
@@ -44648,7 +44648,7 @@
       </c>
       <c r="AW33" s="4"/>
       <c r="AX33" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY33" s="18">
         <v>0</v>
@@ -44803,7 +44803,7 @@
       </c>
       <c r="AW34" s="4"/>
       <c r="AX34" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY34" s="18">
         <v>0</v>
@@ -44826,7 +44826,7 @@
         <v>488</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E35" s="4">
         <v>3</v>
@@ -44960,7 +44960,7 @@
       </c>
       <c r="AW35" s="4"/>
       <c r="AX35" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY35" s="18">
         <v>0</v>
@@ -45119,7 +45119,7 @@
       </c>
       <c r="AW36" s="4"/>
       <c r="AX36" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY36" s="18">
         <v>0</v>
@@ -45142,7 +45142,7 @@
         <v>489</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E37" s="4">
         <v>2</v>
@@ -45280,7 +45280,7 @@
       </c>
       <c r="AW37" s="4"/>
       <c r="AX37" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY37" s="18">
         <v>0</v>
@@ -45433,7 +45433,7 @@
       </c>
       <c r="AW38" s="4"/>
       <c r="AX38" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY38" s="18">
         <v>0</v>
@@ -45584,7 +45584,7 @@
       </c>
       <c r="AW39" s="4"/>
       <c r="AX39" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY39" s="18">
         <v>0</v>
@@ -45735,7 +45735,7 @@
       </c>
       <c r="AW40" s="4"/>
       <c r="AX40" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY40" s="18">
         <v>0</v>
@@ -45896,7 +45896,7 @@
       </c>
       <c r="AW41" s="4"/>
       <c r="AX41" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY41" s="18">
         <v>0</v>
@@ -46053,7 +46053,7 @@
       </c>
       <c r="AW42" s="4"/>
       <c r="AX42" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY42" s="18">
         <v>0</v>
@@ -46208,7 +46208,7 @@
       </c>
       <c r="AW43" s="4"/>
       <c r="AX43" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY43" s="18">
         <v>0</v>
@@ -46231,7 +46231,7 @@
         <v>492</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E44" s="4">
         <v>3</v>
@@ -46365,7 +46365,7 @@
       </c>
       <c r="AW44" s="4"/>
       <c r="AX44" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY44" s="18">
         <v>0</v>
@@ -46520,7 +46520,7 @@
       </c>
       <c r="AW45" s="4"/>
       <c r="AX45" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY45" s="18">
         <v>0</v>
@@ -46681,7 +46681,7 @@
       </c>
       <c r="AW46" s="4"/>
       <c r="AX46" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY46" s="18">
         <v>0</v>
@@ -46836,7 +46836,7 @@
       </c>
       <c r="AW47" s="4"/>
       <c r="AX47" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY47" s="18">
         <v>0</v>
@@ -46993,7 +46993,7 @@
       </c>
       <c r="AW48" s="4"/>
       <c r="AX48" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY48" s="18">
         <v>0</v>
@@ -47016,7 +47016,7 @@
         <v>496</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E49" s="4">
         <v>2</v>
@@ -47150,7 +47150,7 @@
       </c>
       <c r="AW49" s="4"/>
       <c r="AX49" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY49" s="18">
         <v>0</v>
@@ -47301,7 +47301,7 @@
       </c>
       <c r="AW50" s="4"/>
       <c r="AX50" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY50" s="18">
         <v>0</v>
@@ -47458,7 +47458,7 @@
       </c>
       <c r="AW51" s="4"/>
       <c r="AX51" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY51" s="18">
         <v>0</v>
@@ -47613,7 +47613,7 @@
       </c>
       <c r="AW52" s="4"/>
       <c r="AX52" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY52" s="18">
         <v>0</v>
@@ -47768,7 +47768,7 @@
       </c>
       <c r="AW53" s="4"/>
       <c r="AX53" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY53" s="18">
         <v>0</v>
@@ -47929,7 +47929,7 @@
       </c>
       <c r="AW54" s="4"/>
       <c r="AX54" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY54" s="18">
         <v>0</v>
@@ -48086,7 +48086,7 @@
       </c>
       <c r="AW55" s="4"/>
       <c r="AX55" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY55" s="18">
         <v>0</v>
@@ -48241,7 +48241,7 @@
       </c>
       <c r="AW56" s="4"/>
       <c r="AX56" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY56" s="18">
         <v>0</v>
@@ -48400,7 +48400,7 @@
       </c>
       <c r="AW57" s="4"/>
       <c r="AX57" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY57" s="18">
         <v>0</v>
@@ -48555,7 +48555,7 @@
       </c>
       <c r="AW58" s="4"/>
       <c r="AX58" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY58" s="18">
         <v>0</v>
@@ -48578,7 +48578,7 @@
         <v>332</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E59" s="4">
         <v>2</v>
@@ -48712,7 +48712,7 @@
       </c>
       <c r="AW59" s="4"/>
       <c r="AX59" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY59" s="18">
         <v>0</v>
@@ -48871,7 +48871,7 @@
       </c>
       <c r="AW60" s="4"/>
       <c r="AX60" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY60" s="18">
         <v>0</v>
@@ -48894,7 +48894,7 @@
         <v>503</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E61" s="4">
         <v>1</v>
@@ -49028,7 +49028,7 @@
       </c>
       <c r="AW61" s="4"/>
       <c r="AX61" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY61" s="18">
         <v>0</v>
@@ -49051,7 +49051,7 @@
         <v>504</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E62" s="4">
         <v>1</v>
@@ -49185,7 +49185,7 @@
       </c>
       <c r="AW62" s="4"/>
       <c r="AX62" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY62" s="18">
         <v>0</v>
@@ -49208,7 +49208,7 @@
         <v>505</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E63" s="4">
         <v>4</v>
@@ -49342,7 +49342,7 @@
       </c>
       <c r="AW63" s="4"/>
       <c r="AX63" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY63" s="18">
         <v>0</v>
@@ -49497,7 +49497,7 @@
       </c>
       <c r="AW64" s="4"/>
       <c r="AX64" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY64" s="18">
         <v>0</v>
@@ -49650,7 +49650,7 @@
       </c>
       <c r="AW65" s="4"/>
       <c r="AX65" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY65" s="18">
         <v>0</v>
@@ -49807,7 +49807,7 @@
       </c>
       <c r="AW66" s="4"/>
       <c r="AX66" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY66" s="18">
         <v>0</v>
@@ -49964,7 +49964,7 @@
       </c>
       <c r="AW67" s="4"/>
       <c r="AX67" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY67" s="18">
         <v>0</v>
@@ -50123,7 +50123,7 @@
         <v>77</v>
       </c>
       <c r="AX68" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY68" s="18">
         <v>0</v>
@@ -50146,7 +50146,7 @@
         <v>336</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E69" s="4">
         <v>6</v>
@@ -50280,7 +50280,7 @@
       </c>
       <c r="AW69" s="4"/>
       <c r="AX69" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY69" s="18">
         <v>0</v>
@@ -50303,7 +50303,7 @@
         <v>508</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E70" s="4">
         <v>5</v>
@@ -50441,7 +50441,7 @@
       </c>
       <c r="AW70" s="4"/>
       <c r="AX70" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY70" s="18">
         <v>0</v>
@@ -50592,7 +50592,7 @@
       </c>
       <c r="AW71" s="4"/>
       <c r="AX71" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY71" s="18">
         <v>0</v>
@@ -50745,7 +50745,7 @@
       </c>
       <c r="AW72" s="4"/>
       <c r="AX72" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY72" s="18">
         <v>0</v>
@@ -50902,7 +50902,7 @@
       </c>
       <c r="AW73" s="4"/>
       <c r="AX73" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY73" s="18">
         <v>0</v>
@@ -51057,7 +51057,7 @@
       </c>
       <c r="AW74" s="4"/>
       <c r="AX74" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY74" s="18">
         <v>0</v>
@@ -51218,7 +51218,7 @@
       </c>
       <c r="AW75" s="4"/>
       <c r="AX75" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY75" s="18">
         <v>0</v>
@@ -51241,7 +51241,7 @@
         <v>513</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E76" s="4">
         <v>4</v>
@@ -51379,7 +51379,7 @@
       </c>
       <c r="AW76" s="4"/>
       <c r="AX76" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY76" s="18">
         <v>0</v>
@@ -51536,7 +51536,7 @@
       </c>
       <c r="AW77" s="4"/>
       <c r="AX77" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY77" s="18">
         <v>0</v>
@@ -51559,7 +51559,7 @@
         <v>338</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>919</v>
+        <v>949</v>
       </c>
       <c r="E78" s="4">
         <v>6</v>
@@ -51572,16 +51572,16 @@
       </c>
       <c r="H78" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I78" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J78" s="4">
         <v>-100</v>
       </c>
       <c r="K78" s="4">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="L78" s="4">
         <v>0</v>
@@ -51609,7 +51609,7 @@
       </c>
       <c r="T78" s="12">
         <f t="shared" si="5"/>
-        <v>1.6800000000000068</v>
+        <v>5.68</v>
       </c>
       <c r="U78" s="4">
         <v>0</v>
@@ -51624,7 +51624,7 @@
         <v>800</v>
       </c>
       <c r="Y78" s="37">
-        <v>55400004</v>
+        <v>55300012</v>
       </c>
       <c r="Z78" s="18">
         <v>100</v>
@@ -51638,7 +51638,7 @@
       <c r="AC78" s="18">
         <f>IF(ISBLANK($Y78),0, LOOKUP($Y78,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z78/100)+
 IF(ISBLANK($AA78),0, LOOKUP($AA78,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB78/100)</f>
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="AD78" s="18">
         <v>0</v>
@@ -51687,7 +51687,9 @@
       <c r="AR78" s="50" t="s">
         <v>781</v>
       </c>
-      <c r="AS78" s="54"/>
+      <c r="AS78" s="54">
+        <v>11000009</v>
+      </c>
       <c r="AT78" s="4">
         <v>22011052</v>
       </c>
@@ -51697,7 +51699,7 @@
       </c>
       <c r="AW78" s="4"/>
       <c r="AX78" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY78" s="18">
         <v>0</v>
@@ -51850,7 +51852,7 @@
       </c>
       <c r="AW79" s="4"/>
       <c r="AX79" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY79" s="18">
         <v>0</v>
@@ -52003,7 +52005,7 @@
       </c>
       <c r="AW80" s="4"/>
       <c r="AX80" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY80" s="18">
         <v>0</v>
@@ -52162,7 +52164,7 @@
       </c>
       <c r="AW81" s="4"/>
       <c r="AX81" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY81" s="18">
         <v>0</v>
@@ -52321,7 +52323,7 @@
       </c>
       <c r="AW82" s="4"/>
       <c r="AX82" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY82" s="18">
         <v>0</v>
@@ -52476,7 +52478,7 @@
       </c>
       <c r="AW83" s="4"/>
       <c r="AX83" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY83" s="18">
         <v>0</v>
@@ -52633,7 +52635,7 @@
       </c>
       <c r="AW84" s="8"/>
       <c r="AX84" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY84" s="18">
         <v>0</v>
@@ -52790,7 +52792,7 @@
       </c>
       <c r="AW85" s="8"/>
       <c r="AX85" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY85" s="18">
         <v>0</v>
@@ -52947,7 +52949,7 @@
       </c>
       <c r="AW86" s="8"/>
       <c r="AX86" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY86" s="18">
         <v>0</v>
@@ -53110,7 +53112,7 @@
       </c>
       <c r="AW87" s="4"/>
       <c r="AX87" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY87" s="18">
         <v>0</v>
@@ -53133,7 +53135,7 @@
         <v>341</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E88" s="4">
         <v>2</v>
@@ -53267,7 +53269,7 @@
       </c>
       <c r="AW88" s="4"/>
       <c r="AX88" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY88" s="18">
         <v>0</v>
@@ -53422,7 +53424,7 @@
       </c>
       <c r="AW89" s="4"/>
       <c r="AX89" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY89" s="18">
         <v>0</v>
@@ -53581,7 +53583,7 @@
       </c>
       <c r="AW90" s="4"/>
       <c r="AX90" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY90" s="18">
         <v>0</v>
@@ -53738,7 +53740,7 @@
       </c>
       <c r="AW91" s="4"/>
       <c r="AX91" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY91" s="18">
         <v>0</v>
@@ -53895,7 +53897,7 @@
       </c>
       <c r="AW92" s="4"/>
       <c r="AX92" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY92" s="18">
         <v>0</v>
@@ -54046,7 +54048,7 @@
       </c>
       <c r="AW93" s="4"/>
       <c r="AX93" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY93" s="18">
         <v>0</v>
@@ -54207,7 +54209,7 @@
       </c>
       <c r="AW94" s="4"/>
       <c r="AX94" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY94" s="18">
         <v>0</v>
@@ -54360,7 +54362,7 @@
       </c>
       <c r="AW95" s="4"/>
       <c r="AX95" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY95" s="18">
         <v>0</v>
@@ -54521,7 +54523,7 @@
       </c>
       <c r="AW96" s="4"/>
       <c r="AX96" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY96" s="18">
         <v>0</v>
@@ -54544,7 +54546,7 @@
         <v>525</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E97" s="4">
         <v>6</v>
@@ -54682,7 +54684,7 @@
       </c>
       <c r="AW97" s="4"/>
       <c r="AX97" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY97" s="18">
         <v>0</v>
@@ -54839,7 +54841,7 @@
       </c>
       <c r="AW98" s="4"/>
       <c r="AX98" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY98" s="18">
         <v>0</v>
@@ -54996,7 +54998,7 @@
       </c>
       <c r="AW99" s="4"/>
       <c r="AX99" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY99" s="18">
         <v>0</v>
@@ -55019,7 +55021,7 @@
         <v>412</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E100" s="4">
         <v>2</v>
@@ -55157,7 +55159,7 @@
       </c>
       <c r="AW100" s="4"/>
       <c r="AX100" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY100" s="18">
         <v>0</v>
@@ -55308,7 +55310,7 @@
       </c>
       <c r="AW101" s="4"/>
       <c r="AX101" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY101" s="18">
         <v>0</v>
@@ -55469,7 +55471,7 @@
       </c>
       <c r="AW102" s="4"/>
       <c r="AX102" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY102" s="18">
         <v>0</v>
@@ -55492,7 +55494,7 @@
         <v>344</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E103" s="4">
         <v>4</v>
@@ -55628,7 +55630,7 @@
       </c>
       <c r="AW103" s="4"/>
       <c r="AX103" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY103" s="18">
         <v>0</v>
@@ -55651,7 +55653,7 @@
         <v>345</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E104" s="4">
         <v>3</v>
@@ -55789,7 +55791,7 @@
       </c>
       <c r="AW104" s="4"/>
       <c r="AX104" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY104" s="18">
         <v>0</v>
@@ -55812,7 +55814,7 @@
         <v>531</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E105" s="4">
         <v>2</v>
@@ -55948,7 +55950,7 @@
       </c>
       <c r="AW105" s="4"/>
       <c r="AX105" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY105" s="18">
         <v>0</v>
@@ -55971,7 +55973,7 @@
         <v>532</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E106" s="4">
         <v>2</v>
@@ -56105,7 +56107,7 @@
       </c>
       <c r="AW106" s="4"/>
       <c r="AX106" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY106" s="18">
         <v>0</v>
@@ -56262,7 +56264,7 @@
       </c>
       <c r="AW107" s="4"/>
       <c r="AX107" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY107" s="18">
         <v>0</v>
@@ -56417,7 +56419,7 @@
       </c>
       <c r="AW108" s="4"/>
       <c r="AX108" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY108" s="18">
         <v>0</v>
@@ -56570,7 +56572,7 @@
       </c>
       <c r="AW109" s="4"/>
       <c r="AX109" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY109" s="18">
         <v>0</v>
@@ -56727,7 +56729,7 @@
       </c>
       <c r="AW110" s="4"/>
       <c r="AX110" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY110" s="18">
         <v>0</v>
@@ -56880,7 +56882,7 @@
       </c>
       <c r="AW111" s="4"/>
       <c r="AX111" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY111" s="18">
         <v>0</v>
@@ -57031,7 +57033,7 @@
       </c>
       <c r="AW112" s="4"/>
       <c r="AX112" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY112" s="18">
         <v>0</v>
@@ -57182,7 +57184,7 @@
       </c>
       <c r="AW113" s="4"/>
       <c r="AX113" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY113" s="18">
         <v>0</v>
@@ -57205,7 +57207,7 @@
         <v>537</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E114" s="4">
         <v>7</v>
@@ -57347,7 +57349,7 @@
         <v>77</v>
       </c>
       <c r="AX114" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY114" s="18">
         <v>0</v>
@@ -57370,7 +57372,7 @@
         <v>349</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E115" s="4">
         <v>7</v>
@@ -57508,7 +57510,7 @@
         <v>77</v>
       </c>
       <c r="AX115" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY115" s="18">
         <v>0</v>
@@ -57673,7 +57675,7 @@
         <v>77</v>
       </c>
       <c r="AX116" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY116" s="18">
         <v>0</v>
@@ -57696,7 +57698,7 @@
         <v>528</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E117" s="4">
         <v>7</v>
@@ -57838,7 +57840,7 @@
         <v>77</v>
       </c>
       <c r="AX117" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY117" s="18">
         <v>0</v>
@@ -57861,7 +57863,7 @@
         <v>538</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E118" s="4">
         <v>7</v>
@@ -58003,7 +58005,7 @@
         <v>77</v>
       </c>
       <c r="AX118" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY118" s="18">
         <v>0</v>
@@ -58026,7 +58028,7 @@
         <v>665</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E119" s="8">
         <v>2</v>
@@ -58160,7 +58162,7 @@
       </c>
       <c r="AW119" s="8"/>
       <c r="AX119" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY119" s="18">
         <v>0</v>
@@ -58183,7 +58185,7 @@
         <v>539</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E120" s="4">
         <v>7</v>
@@ -58325,7 +58327,7 @@
         <v>77</v>
       </c>
       <c r="AX120" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY120" s="18">
         <v>0</v>
@@ -58348,7 +58350,7 @@
         <v>540</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E121" s="4">
         <v>7</v>
@@ -58490,7 +58492,7 @@
         <v>77</v>
       </c>
       <c r="AX121" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY121" s="18">
         <v>0</v>
@@ -58641,7 +58643,7 @@
       </c>
       <c r="AW122" s="4"/>
       <c r="AX122" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY122" s="18">
         <v>0</v>
@@ -58796,7 +58798,7 @@
       </c>
       <c r="AW123" s="4"/>
       <c r="AX123" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY123" s="18">
         <v>0</v>
@@ -58953,7 +58955,7 @@
       </c>
       <c r="AW124" s="4"/>
       <c r="AX124" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY124" s="18">
         <v>0</v>
@@ -59112,7 +59114,7 @@
       </c>
       <c r="AW125" s="4"/>
       <c r="AX125" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY125" s="18">
         <v>0</v>
@@ -59271,7 +59273,7 @@
       </c>
       <c r="AW126" s="4"/>
       <c r="AX126" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY126" s="18">
         <v>0</v>
@@ -59426,7 +59428,7 @@
       </c>
       <c r="AW127" s="4"/>
       <c r="AX127" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY127" s="18">
         <v>0</v>
@@ -59583,7 +59585,7 @@
       </c>
       <c r="AW128" s="4"/>
       <c r="AX128" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY128" s="18">
         <v>0</v>
@@ -59734,7 +59736,7 @@
       </c>
       <c r="AW129" s="4"/>
       <c r="AX129" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY129" s="18">
         <v>0</v>
@@ -59891,7 +59893,7 @@
       </c>
       <c r="AW130" s="4"/>
       <c r="AX130" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY130" s="18">
         <v>0</v>
@@ -60042,7 +60044,7 @@
       </c>
       <c r="AW131" s="4"/>
       <c r="AX131" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY131" s="18">
         <v>0</v>
@@ -60197,7 +60199,7 @@
       </c>
       <c r="AW132" s="4"/>
       <c r="AX132" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY132" s="18">
         <v>0</v>
@@ -60356,7 +60358,7 @@
       </c>
       <c r="AW133" s="4"/>
       <c r="AX133" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY133" s="18">
         <v>0</v>
@@ -60517,7 +60519,7 @@
       </c>
       <c r="AW134" s="4"/>
       <c r="AX134" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY134" s="18">
         <v>0</v>
@@ -60540,7 +60542,7 @@
         <v>551</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E135" s="4">
         <v>3</v>
@@ -60674,7 +60676,7 @@
       </c>
       <c r="AW135" s="4"/>
       <c r="AX135" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY135" s="18">
         <v>0</v>
@@ -60829,7 +60831,7 @@
       </c>
       <c r="AW136" s="4"/>
       <c r="AX136" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY136" s="18">
         <v>0</v>
@@ -60988,7 +60990,7 @@
       </c>
       <c r="AW137" s="4"/>
       <c r="AX137" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY137" s="18">
         <v>0</v>
@@ -61143,7 +61145,7 @@
       </c>
       <c r="AW138" s="4"/>
       <c r="AX138" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY138" s="18">
         <v>0</v>
@@ -61294,7 +61296,7 @@
       </c>
       <c r="AW139" s="4"/>
       <c r="AX139" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY139" s="18">
         <v>0</v>
@@ -61447,7 +61449,7 @@
       </c>
       <c r="AW140" s="4"/>
       <c r="AX140" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY140" s="18">
         <v>0</v>
@@ -61602,7 +61604,7 @@
       </c>
       <c r="AW141" s="4"/>
       <c r="AX141" s="59" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AY141" s="18">
         <v>0</v>
@@ -61753,7 +61755,7 @@
       </c>
       <c r="AW142" s="4"/>
       <c r="AX142" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY142" s="18">
         <v>0</v>
@@ -61910,7 +61912,7 @@
       </c>
       <c r="AW143" s="4"/>
       <c r="AX143" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY143" s="18">
         <v>0</v>
@@ -62065,7 +62067,7 @@
       </c>
       <c r="AW144" s="4"/>
       <c r="AX144" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY144" s="18">
         <v>0</v>
@@ -62218,7 +62220,7 @@
       </c>
       <c r="AW145" s="4"/>
       <c r="AX145" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY145" s="18">
         <v>0</v>
@@ -62377,7 +62379,7 @@
       </c>
       <c r="AW146" s="4"/>
       <c r="AX146" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY146" s="18">
         <v>0</v>
@@ -62534,7 +62536,7 @@
       </c>
       <c r="AW147" s="4"/>
       <c r="AX147" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY147" s="18">
         <v>0</v>
@@ -62695,7 +62697,7 @@
       </c>
       <c r="AW148" s="4"/>
       <c r="AX148" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY148" s="18">
         <v>0</v>
@@ -62718,7 +62720,7 @@
         <v>356</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>844</v>
+        <v>949</v>
       </c>
       <c r="E149" s="4">
         <v>3</v>
@@ -62731,7 +62733,7 @@
       </c>
       <c r="H149" s="4">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I149" s="4">
         <v>3</v>
@@ -62743,7 +62745,7 @@
         <v>0</v>
       </c>
       <c r="L149" s="4">
-        <v>-16</v>
+        <v>-10</v>
       </c>
       <c r="M149" s="4">
         <v>0</v>
@@ -62768,7 +62770,7 @@
       </c>
       <c r="T149" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U149" s="4">
         <v>30</v>
@@ -62783,21 +62785,17 @@
         <v>162</v>
       </c>
       <c r="Y149" s="37">
-        <v>55100011</v>
+        <v>55300013</v>
       </c>
       <c r="Z149" s="18">
         <v>100</v>
       </c>
-      <c r="AA149" s="18">
-        <v>55600003</v>
-      </c>
-      <c r="AB149" s="18">
-        <v>100</v>
-      </c>
+      <c r="AA149" s="18"/>
+      <c r="AB149" s="18"/>
       <c r="AC149" s="18">
         <f>IF(ISBLANK($Y149),0, LOOKUP($Y149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z149/100)+
 IF(ISBLANK($AA149),0, LOOKUP($AA149,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB149/100)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AD149" s="18">
         <v>0</v>
@@ -62846,7 +62844,9 @@
       <c r="AR149" s="50" t="s">
         <v>781</v>
       </c>
-      <c r="AS149" s="54"/>
+      <c r="AS149" s="54">
+        <v>11000005</v>
+      </c>
       <c r="AT149" s="4">
         <v>22011013</v>
       </c>
@@ -62856,7 +62856,7 @@
       </c>
       <c r="AW149" s="4"/>
       <c r="AX149" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY149" s="18">
         <v>0</v>
@@ -63011,7 +63011,7 @@
       </c>
       <c r="AW150" s="4"/>
       <c r="AX150" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY150" s="18">
         <v>0</v>
@@ -63162,7 +63162,7 @@
       </c>
       <c r="AW151" s="4"/>
       <c r="AX151" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY151" s="18">
         <v>0</v>
@@ -63315,7 +63315,7 @@
       </c>
       <c r="AW152" s="4"/>
       <c r="AX152" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY152" s="18">
         <v>0</v>
@@ -63338,7 +63338,7 @@
         <v>358</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E153" s="4">
         <v>2</v>
@@ -63472,7 +63472,7 @@
       </c>
       <c r="AW153" s="4"/>
       <c r="AX153" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY153" s="18">
         <v>0</v>
@@ -63623,7 +63623,7 @@
       </c>
       <c r="AW154" s="4"/>
       <c r="AX154" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY154" s="18">
         <v>0</v>
@@ -63780,7 +63780,7 @@
       </c>
       <c r="AW155" s="4"/>
       <c r="AX155" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY155" s="18">
         <v>0</v>
@@ -63935,7 +63935,7 @@
       </c>
       <c r="AW156" s="4"/>
       <c r="AX156" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY156" s="18">
         <v>0</v>
@@ -64088,7 +64088,7 @@
       </c>
       <c r="AW157" s="4"/>
       <c r="AX157" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY157" s="18">
         <v>0</v>
@@ -64239,7 +64239,7 @@
       </c>
       <c r="AW158" s="4"/>
       <c r="AX158" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY158" s="18">
         <v>0</v>
@@ -64392,7 +64392,7 @@
       </c>
       <c r="AW159" s="8"/>
       <c r="AX159" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY159" s="18">
         <v>0</v>
@@ -64545,7 +64545,7 @@
       </c>
       <c r="AW160" s="4"/>
       <c r="AX160" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY160" s="18">
         <v>0</v>
@@ -64698,7 +64698,7 @@
       </c>
       <c r="AW161" s="4"/>
       <c r="AX161" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY161" s="18">
         <v>0</v>
@@ -64853,7 +64853,7 @@
       </c>
       <c r="AW162" s="4"/>
       <c r="AX162" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY162" s="18">
         <v>0</v>
@@ -65010,7 +65010,7 @@
       </c>
       <c r="AW163" s="4"/>
       <c r="AX163" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY163" s="18">
         <v>0</v>
@@ -65167,7 +65167,7 @@
       </c>
       <c r="AW164" s="4"/>
       <c r="AX164" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY164" s="18">
         <v>0</v>
@@ -65318,7 +65318,7 @@
       </c>
       <c r="AW165" s="8"/>
       <c r="AX165" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY165" s="18">
         <v>0</v>
@@ -65471,7 +65471,7 @@
       </c>
       <c r="AW166" s="8"/>
       <c r="AX166" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY166" s="18">
         <v>0</v>
@@ -65622,7 +65622,7 @@
       </c>
       <c r="AW167" s="4"/>
       <c r="AX167" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY167" s="18">
         <v>0</v>
@@ -65775,7 +65775,7 @@
       </c>
       <c r="AW168" s="8"/>
       <c r="AX168" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY168" s="18">
         <v>0</v>
@@ -65932,7 +65932,7 @@
       </c>
       <c r="AW169" s="4"/>
       <c r="AX169" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY169" s="18">
         <v>0</v>
@@ -66089,7 +66089,7 @@
       </c>
       <c r="AW170" s="4"/>
       <c r="AX170" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY170" s="18">
         <v>0</v>
@@ -66244,7 +66244,7 @@
       </c>
       <c r="AW171" s="4"/>
       <c r="AX171" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY171" s="18">
         <v>0</v>
@@ -66267,7 +66267,7 @@
         <v>574</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E172" s="4">
         <v>4</v>
@@ -66407,7 +66407,7 @@
       </c>
       <c r="AW172" s="4"/>
       <c r="AX172" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY172" s="18">
         <v>0</v>
@@ -66566,7 +66566,7 @@
       </c>
       <c r="AW173" s="4"/>
       <c r="AX173" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY173" s="18">
         <v>0</v>
@@ -66725,7 +66725,7 @@
       </c>
       <c r="AW174" s="4"/>
       <c r="AX174" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY174" s="18">
         <v>0</v>
@@ -66888,7 +66888,7 @@
       </c>
       <c r="AW175" s="4"/>
       <c r="AX175" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY175" s="18">
         <v>0</v>
@@ -67043,7 +67043,7 @@
       </c>
       <c r="AW176" s="4"/>
       <c r="AX176" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY176" s="18">
         <v>0</v>
@@ -67200,7 +67200,7 @@
       </c>
       <c r="AW177" s="4"/>
       <c r="AX177" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY177" s="18">
         <v>0</v>
@@ -67223,7 +67223,7 @@
         <v>579</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E178" s="4">
         <v>4</v>
@@ -67357,7 +67357,7 @@
       </c>
       <c r="AW178" s="4"/>
       <c r="AX178" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY178" s="18">
         <v>0</v>
@@ -67512,7 +67512,7 @@
       </c>
       <c r="AW179" s="4"/>
       <c r="AX179" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY179" s="18">
         <v>0</v>
@@ -67671,7 +67671,7 @@
       </c>
       <c r="AW180" s="4"/>
       <c r="AX180" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY180" s="18">
         <v>0</v>
@@ -67694,7 +67694,7 @@
         <v>581</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E181" s="4">
         <v>5</v>
@@ -67832,7 +67832,7 @@
       </c>
       <c r="AW181" s="4"/>
       <c r="AX181" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY181" s="18">
         <v>0</v>
@@ -67987,7 +67987,7 @@
       </c>
       <c r="AW182" s="4"/>
       <c r="AX182" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY182" s="18">
         <v>0</v>
@@ -68146,7 +68146,7 @@
       </c>
       <c r="AW183" s="4"/>
       <c r="AX183" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY183" s="18">
         <v>0</v>
@@ -68303,7 +68303,7 @@
       </c>
       <c r="AW184" s="4"/>
       <c r="AX184" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY184" s="18">
         <v>0</v>
@@ -68326,7 +68326,7 @@
         <v>362</v>
       </c>
       <c r="D185" s="19" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E185" s="4">
         <v>6</v>
@@ -68464,7 +68464,7 @@
       </c>
       <c r="AW185" s="4"/>
       <c r="AX185" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY185" s="18">
         <v>0</v>
@@ -68621,7 +68621,7 @@
       </c>
       <c r="AW186" s="4"/>
       <c r="AX186" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY186" s="18">
         <v>0</v>
@@ -68644,7 +68644,7 @@
         <v>586</v>
       </c>
       <c r="D187" s="19" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E187" s="4">
         <v>2</v>
@@ -68778,7 +68778,7 @@
       </c>
       <c r="AW187" s="4"/>
       <c r="AX187" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY187" s="18">
         <v>0</v>
@@ -68929,7 +68929,7 @@
       </c>
       <c r="AW188" s="4"/>
       <c r="AX188" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY188" s="18">
         <v>0</v>
@@ -69084,7 +69084,7 @@
       </c>
       <c r="AW189" s="4"/>
       <c r="AX189" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY189" s="18">
         <v>0</v>
@@ -69237,7 +69237,7 @@
       </c>
       <c r="AW190" s="4"/>
       <c r="AX190" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY190" s="18">
         <v>0</v>
@@ -69396,7 +69396,7 @@
       </c>
       <c r="AW191" s="4"/>
       <c r="AX191" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY191" s="18">
         <v>0</v>
@@ -69555,7 +69555,7 @@
       </c>
       <c r="AW192" s="4"/>
       <c r="AX192" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY192" s="18">
         <v>0</v>
@@ -69716,7 +69716,7 @@
       </c>
       <c r="AW193" s="4"/>
       <c r="AX193" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY193" s="18">
         <v>0</v>
@@ -69877,7 +69877,7 @@
       </c>
       <c r="AW194" s="4"/>
       <c r="AX194" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY194" s="18">
         <v>0</v>
@@ -69900,7 +69900,7 @@
         <v>593</v>
       </c>
       <c r="D195" s="19" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E195" s="4">
         <v>5</v>
@@ -70038,7 +70038,7 @@
       </c>
       <c r="AW195" s="4"/>
       <c r="AX195" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY195" s="18">
         <v>0</v>
@@ -70199,7 +70199,7 @@
       </c>
       <c r="AW196" s="4"/>
       <c r="AX196" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY196" s="18">
         <v>0</v>
@@ -70360,7 +70360,7 @@
       </c>
       <c r="AW197" s="4"/>
       <c r="AX197" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY197" s="18">
         <v>0</v>
@@ -70519,7 +70519,7 @@
       </c>
       <c r="AW198" s="4"/>
       <c r="AX198" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY198" s="18">
         <v>0</v>
@@ -70542,7 +70542,7 @@
         <v>597</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E199" s="4">
         <v>5</v>
@@ -70680,7 +70680,7 @@
       </c>
       <c r="AW199" s="4"/>
       <c r="AX199" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY199" s="18">
         <v>0</v>
@@ -70835,7 +70835,7 @@
       </c>
       <c r="AW200" s="4"/>
       <c r="AX200" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY200" s="18">
         <v>0</v>
@@ -70992,7 +70992,7 @@
       </c>
       <c r="AW201" s="4"/>
       <c r="AX201" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY201" s="18">
         <v>0</v>
@@ -71149,7 +71149,7 @@
       </c>
       <c r="AW202" s="4"/>
       <c r="AX202" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY202" s="18">
         <v>0</v>
@@ -71304,7 +71304,7 @@
       </c>
       <c r="AW203" s="4"/>
       <c r="AX203" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY203" s="18">
         <v>0</v>
@@ -71327,7 +71327,7 @@
         <v>666</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E204" s="8">
         <v>3</v>
@@ -71461,7 +71461,7 @@
       </c>
       <c r="AW204" s="8"/>
       <c r="AX204" s="59" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AY204" s="18">
         <v>0</v>
@@ -71484,7 +71484,7 @@
         <v>599</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E205" s="4">
         <v>2</v>
@@ -71618,7 +71618,7 @@
       </c>
       <c r="AW205" s="4"/>
       <c r="AX205" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY205" s="18">
         <v>0</v>
@@ -71641,7 +71641,7 @@
         <v>600</v>
       </c>
       <c r="D206" s="19" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E206" s="4">
         <v>3</v>
@@ -71779,7 +71779,7 @@
       </c>
       <c r="AW206" s="4"/>
       <c r="AX206" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY206" s="18">
         <v>0</v>
@@ -71934,7 +71934,7 @@
       </c>
       <c r="AW207" s="4"/>
       <c r="AX207" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY207" s="18">
         <v>0</v>
@@ -72091,7 +72091,7 @@
       </c>
       <c r="AW208" s="4"/>
       <c r="AX208" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY208" s="18">
         <v>0</v>
@@ -72246,7 +72246,7 @@
       </c>
       <c r="AW209" s="4"/>
       <c r="AX209" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY209" s="18">
         <v>0</v>
@@ -72397,7 +72397,7 @@
       </c>
       <c r="AW210" s="4"/>
       <c r="AX210" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY210" s="18">
         <v>0</v>
@@ -72554,7 +72554,7 @@
       </c>
       <c r="AW211" s="4"/>
       <c r="AX211" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY211" s="18">
         <v>0</v>
@@ -72577,7 +72577,7 @@
         <v>603</v>
       </c>
       <c r="D212" s="19" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E212" s="4">
         <v>3</v>
@@ -72711,7 +72711,7 @@
       </c>
       <c r="AW212" s="4"/>
       <c r="AX212" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY212" s="18">
         <v>0</v>
@@ -72734,7 +72734,7 @@
         <v>604</v>
       </c>
       <c r="D213" s="19" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E213" s="4">
         <v>4</v>
@@ -72872,7 +72872,7 @@
       </c>
       <c r="AW213" s="4"/>
       <c r="AX213" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY213" s="18">
         <v>0</v>
@@ -73023,7 +73023,7 @@
       </c>
       <c r="AW214" s="4"/>
       <c r="AX214" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY214" s="18">
         <v>0</v>
@@ -73046,7 +73046,7 @@
         <v>606</v>
       </c>
       <c r="D215" s="19" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E215" s="4">
         <v>4</v>
@@ -73184,7 +73184,7 @@
       </c>
       <c r="AW215" s="4"/>
       <c r="AX215" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY215" s="18">
         <v>0</v>
@@ -73341,7 +73341,7 @@
       </c>
       <c r="AW216" s="4"/>
       <c r="AX216" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY216" s="18">
         <v>0</v>
@@ -73500,7 +73500,7 @@
       </c>
       <c r="AW217" s="4"/>
       <c r="AX217" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY217" s="18">
         <v>0</v>
@@ -73523,7 +73523,7 @@
         <v>608</v>
       </c>
       <c r="D218" s="19" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E218" s="4">
         <v>2</v>
@@ -73659,7 +73659,7 @@
       </c>
       <c r="AW218" s="4"/>
       <c r="AX218" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY218" s="18">
         <v>0</v>
@@ -73682,7 +73682,7 @@
         <v>609</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E219" s="4">
         <v>3</v>
@@ -73816,7 +73816,7 @@
       </c>
       <c r="AW219" s="4"/>
       <c r="AX219" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY219" s="18">
         <v>0</v>
@@ -73971,7 +73971,7 @@
       </c>
       <c r="AW220" s="4"/>
       <c r="AX220" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY220" s="18">
         <v>0</v>
@@ -74132,7 +74132,7 @@
       </c>
       <c r="AW221" s="4"/>
       <c r="AX221" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY221" s="18">
         <v>0</v>
@@ -74287,7 +74287,7 @@
       </c>
       <c r="AW222" s="4"/>
       <c r="AX222" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY222" s="18">
         <v>0</v>
@@ -74444,7 +74444,7 @@
       </c>
       <c r="AW223" s="4"/>
       <c r="AX223" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY223" s="18">
         <v>0</v>
@@ -74603,7 +74603,7 @@
       </c>
       <c r="AW224" s="4"/>
       <c r="AX224" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY224" s="18">
         <v>0</v>
@@ -74762,7 +74762,7 @@
       </c>
       <c r="AW225" s="4"/>
       <c r="AX225" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY225" s="18">
         <v>0</v>
@@ -74919,7 +74919,7 @@
       </c>
       <c r="AW226" s="4"/>
       <c r="AX226" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY226" s="18">
         <v>0</v>
@@ -75074,7 +75074,7 @@
       </c>
       <c r="AW227" s="4"/>
       <c r="AX227" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY227" s="18">
         <v>0</v>
@@ -75097,7 +75097,7 @@
         <v>424</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E228" s="4">
         <v>3</v>
@@ -75233,7 +75233,7 @@
       </c>
       <c r="AW228" s="4"/>
       <c r="AX228" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY228" s="18">
         <v>0</v>
@@ -75256,7 +75256,7 @@
         <v>370</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E229" s="4">
         <v>2</v>
@@ -75390,7 +75390,7 @@
       </c>
       <c r="AW229" s="4"/>
       <c r="AX229" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY229" s="18">
         <v>0</v>
@@ -75547,7 +75547,7 @@
       </c>
       <c r="AW230" s="4"/>
       <c r="AX230" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY230" s="18">
         <v>0</v>
@@ -75704,7 +75704,7 @@
       </c>
       <c r="AW231" s="4"/>
       <c r="AX231" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY231" s="18">
         <v>0</v>
@@ -75727,7 +75727,7 @@
         <v>616</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E232" s="4">
         <v>1</v>
@@ -75859,7 +75859,7 @@
       </c>
       <c r="AW232" s="4"/>
       <c r="AX232" s="59" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AY232" s="18">
         <v>0</v>
@@ -76020,7 +76020,7 @@
       </c>
       <c r="AW233" s="4"/>
       <c r="AX233" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY233" s="18">
         <v>0</v>
@@ -76175,7 +76175,7 @@
       </c>
       <c r="AW234" s="4"/>
       <c r="AX234" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY234" s="18">
         <v>0</v>
@@ -76198,7 +76198,7 @@
         <v>618</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E235" s="4">
         <v>3</v>
@@ -76332,7 +76332,7 @@
       </c>
       <c r="AW235" s="4"/>
       <c r="AX235" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY235" s="18">
         <v>0</v>
@@ -76355,7 +76355,7 @@
         <v>619</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E236" s="4">
         <v>2</v>
@@ -76489,7 +76489,7 @@
       </c>
       <c r="AW236" s="4"/>
       <c r="AX236" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY236" s="18">
         <v>0</v>
@@ -76648,7 +76648,7 @@
       </c>
       <c r="AW237" s="4"/>
       <c r="AX237" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY237" s="18">
         <v>0</v>
@@ -76665,7 +76665,7 @@
         <v>51000235</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>621</v>
@@ -76799,7 +76799,7 @@
       </c>
       <c r="AW238" s="4"/>
       <c r="AX238" s="59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AY238" s="18">
         <v>0</v>
@@ -76958,7 +76958,7 @@
       </c>
       <c r="AW239" s="4"/>
       <c r="AX239" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY239" s="18">
         <v>0</v>
@@ -77109,7 +77109,7 @@
       </c>
       <c r="AW240" s="4"/>
       <c r="AX240" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY240" s="18">
         <v>0</v>
@@ -77132,7 +77132,7 @@
         <v>430</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E241" s="4">
         <v>5</v>
@@ -77272,7 +77272,7 @@
       </c>
       <c r="AW241" s="4"/>
       <c r="AX241" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY241" s="18">
         <v>0</v>
@@ -77423,7 +77423,7 @@
       </c>
       <c r="AW242" s="4"/>
       <c r="AX242" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY242" s="18">
         <v>0</v>
@@ -77578,7 +77578,7 @@
       </c>
       <c r="AW243" s="4"/>
       <c r="AX243" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY243" s="18">
         <v>0</v>
@@ -77601,7 +77601,7 @@
         <v>373</v>
       </c>
       <c r="D244" s="59" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E244" s="4">
         <v>3</v>
@@ -77735,7 +77735,7 @@
       </c>
       <c r="AW244" s="4"/>
       <c r="AX244" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY244" s="18">
         <v>0</v>
@@ -77758,7 +77758,7 @@
         <v>374</v>
       </c>
       <c r="D245" s="19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E245" s="4">
         <v>6</v>
@@ -77896,7 +77896,7 @@
       </c>
       <c r="AW245" s="4"/>
       <c r="AX245" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY245" s="18">
         <v>0</v>
@@ -78049,7 +78049,7 @@
       </c>
       <c r="AW246" s="4"/>
       <c r="AX246" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY246" s="18">
         <v>0</v>
@@ -78072,7 +78072,7 @@
         <v>436</v>
       </c>
       <c r="D247" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E247" s="4">
         <v>5</v>
@@ -78210,7 +78210,7 @@
       </c>
       <c r="AW247" s="4"/>
       <c r="AX247" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY247" s="18">
         <v>0</v>
@@ -78233,7 +78233,7 @@
         <v>438</v>
       </c>
       <c r="D248" s="19" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E248" s="4">
         <v>2</v>
@@ -78367,7 +78367,7 @@
       </c>
       <c r="AW248" s="4"/>
       <c r="AX248" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY248" s="18">
         <v>0</v>
@@ -78518,7 +78518,7 @@
       </c>
       <c r="AW249" s="4"/>
       <c r="AX249" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY249" s="18">
         <v>0</v>
@@ -78541,7 +78541,7 @@
         <v>440</v>
       </c>
       <c r="D250" s="19" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E250" s="4">
         <v>6</v>
@@ -78679,7 +78679,7 @@
       </c>
       <c r="AW250" s="4"/>
       <c r="AX250" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY250" s="18">
         <v>0</v>
@@ -78702,7 +78702,7 @@
         <v>441</v>
       </c>
       <c r="D251" s="19" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E251" s="4">
         <v>2</v>
@@ -78836,7 +78836,7 @@
       </c>
       <c r="AW251" s="4"/>
       <c r="AX251" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY251" s="18">
         <v>0</v>
@@ -78993,7 +78993,7 @@
       </c>
       <c r="AW252" s="4"/>
       <c r="AX252" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY252" s="18">
         <v>0</v>
@@ -79148,7 +79148,7 @@
       </c>
       <c r="AW253" s="4"/>
       <c r="AX253" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY253" s="18">
         <v>0</v>
@@ -79305,7 +79305,7 @@
       </c>
       <c r="AW254" s="4"/>
       <c r="AX254" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY254" s="18">
         <v>0</v>
@@ -79466,7 +79466,7 @@
       </c>
       <c r="AW255" s="4"/>
       <c r="AX255" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY255" s="18">
         <v>0</v>
@@ -79621,7 +79621,7 @@
       </c>
       <c r="AW256" s="4"/>
       <c r="AX256" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY256" s="18">
         <v>0</v>
@@ -79644,7 +79644,7 @@
         <v>625</v>
       </c>
       <c r="D257" s="19" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E257" s="4">
         <v>3</v>
@@ -79778,7 +79778,7 @@
       </c>
       <c r="AW257" s="4"/>
       <c r="AX257" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY257" s="18">
         <v>0</v>
@@ -79798,10 +79798,10 @@
         <v>258</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D258" s="19" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E258" s="4">
         <v>3</v>
@@ -79939,7 +79939,7 @@
       </c>
       <c r="AW258" s="4"/>
       <c r="AX258" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY258" s="18">
         <v>0</v>
@@ -79962,7 +79962,7 @@
         <v>626</v>
       </c>
       <c r="D259" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E259" s="4">
         <v>2</v>
@@ -80100,7 +80100,7 @@
       </c>
       <c r="AW259" s="4"/>
       <c r="AX259" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY259" s="18">
         <v>0</v>
@@ -80123,7 +80123,7 @@
         <v>378</v>
       </c>
       <c r="D260" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E260" s="4">
         <v>3</v>
@@ -80172,7 +80172,7 @@
         <v>0</v>
       </c>
       <c r="T260" s="12">
-        <f t="shared" ref="T260:T323" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AJ260:AP260)+2.5*SUM(AD260:AH260)+IF(ISNUMBER(AC260),AC260,0)+L260</f>
+        <f t="shared" ref="T260:T303" si="17">SUM(J260:K260)+SUM(M260:S260)*5+4.4*SUM(AJ260:AP260)+2.5*SUM(AD260:AH260)+IF(ISNUMBER(AC260),AC260,0)+L260</f>
         <v>7</v>
       </c>
       <c r="U260" s="4">
@@ -80220,7 +80220,7 @@
         <v>0</v>
       </c>
       <c r="AI260" s="4" t="str">
-        <f t="shared" ref="AI260:AI323" si="18">CONCATENATE(AD260,";",AE260,";",AF260,";",AG260,";",AH260)</f>
+        <f t="shared" ref="AI260:AI303" si="18">CONCATENATE(AD260,";",AE260,";",AF260,";",AG260,";",AH260)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ260" s="18">
@@ -80245,7 +80245,7 @@
         <v>0</v>
       </c>
       <c r="AQ260" s="4" t="str">
-        <f t="shared" ref="AQ260:AQ323" si="19">CONCATENATE(AJ260,";",AK260,";",AL260,";",AM260,";",AN260,";",AO260,";",AP260)</f>
+        <f t="shared" ref="AQ260:AQ303" si="19">CONCATENATE(AJ260,";",AK260,";",AL260,";",AM260,";",AN260,";",AO260,";",AP260)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR260" s="50" t="s">
@@ -80261,7 +80261,7 @@
       </c>
       <c r="AW260" s="4"/>
       <c r="AX260" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY260" s="18">
         <v>0</v>
@@ -80418,7 +80418,7 @@
       </c>
       <c r="AW261" s="4"/>
       <c r="AX261" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY261" s="18">
         <v>0</v>
@@ -80573,7 +80573,7 @@
       </c>
       <c r="AW262" s="4"/>
       <c r="AX262" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY262" s="18">
         <v>0</v>
@@ -80726,7 +80726,7 @@
       </c>
       <c r="AW263" s="4"/>
       <c r="AX263" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY263" s="18">
         <v>0</v>
@@ -80881,7 +80881,7 @@
       </c>
       <c r="AW264" s="4"/>
       <c r="AX264" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY264" s="18">
         <v>0</v>
@@ -81036,7 +81036,7 @@
       </c>
       <c r="AW265" s="4"/>
       <c r="AX265" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY265" s="18">
         <v>0</v>
@@ -81191,7 +81191,7 @@
       </c>
       <c r="AW266" s="4"/>
       <c r="AX266" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY266" s="18">
         <v>0</v>
@@ -81214,7 +81214,7 @@
         <v>383</v>
       </c>
       <c r="D267" s="19" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E267" s="4">
         <v>5</v>
@@ -81354,7 +81354,7 @@
       </c>
       <c r="AW267" s="4"/>
       <c r="AX267" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY267" s="18">
         <v>0</v>
@@ -81509,7 +81509,7 @@
       </c>
       <c r="AW268" s="4"/>
       <c r="AX268" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY268" s="18">
         <v>0</v>
@@ -81532,7 +81532,7 @@
         <v>449</v>
       </c>
       <c r="D269" s="19" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E269" s="4">
         <v>4</v>
@@ -81666,7 +81666,7 @@
       </c>
       <c r="AW269" s="4"/>
       <c r="AX269" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY269" s="18">
         <v>0</v>
@@ -81821,7 +81821,7 @@
       </c>
       <c r="AW270" s="4"/>
       <c r="AX270" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY270" s="18">
         <v>0</v>
@@ -81844,7 +81844,7 @@
         <v>385</v>
       </c>
       <c r="D271" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E271" s="4">
         <v>5</v>
@@ -81982,7 +81982,7 @@
       </c>
       <c r="AW271" s="4"/>
       <c r="AX271" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY271" s="18">
         <v>0</v>
@@ -82005,7 +82005,7 @@
         <v>627</v>
       </c>
       <c r="D272" s="19" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E272" s="4">
         <v>5</v>
@@ -82143,7 +82143,7 @@
       </c>
       <c r="AW272" s="4"/>
       <c r="AX272" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY272" s="18">
         <v>0</v>
@@ -82166,7 +82166,7 @@
         <v>386</v>
       </c>
       <c r="D273" s="19" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E273" s="4">
         <v>5</v>
@@ -82304,7 +82304,7 @@
       </c>
       <c r="AW273" s="4"/>
       <c r="AX273" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY273" s="18">
         <v>0</v>
@@ -82327,7 +82327,7 @@
         <v>387</v>
       </c>
       <c r="D274" s="19" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E274" s="4">
         <v>1</v>
@@ -82461,7 +82461,7 @@
       </c>
       <c r="AW274" s="4"/>
       <c r="AX274" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY274" s="18">
         <v>0</v>
@@ -82618,7 +82618,7 @@
       </c>
       <c r="AW275" s="4"/>
       <c r="AX275" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY275" s="18">
         <v>0</v>
@@ -82769,7 +82769,7 @@
       </c>
       <c r="AW276" s="4"/>
       <c r="AX276" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY276" s="18">
         <v>0</v>
@@ -82926,7 +82926,7 @@
       </c>
       <c r="AW277" s="4"/>
       <c r="AX277" s="59" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AY277" s="18">
         <v>0</v>
@@ -83085,7 +83085,7 @@
       </c>
       <c r="AW278" s="4"/>
       <c r="AX278" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY278" s="18">
         <v>0</v>
@@ -83108,7 +83108,7 @@
         <v>458</v>
       </c>
       <c r="D279" s="19" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E279" s="4">
         <v>2</v>
@@ -83242,7 +83242,7 @@
       </c>
       <c r="AW279" s="4"/>
       <c r="AX279" s="59" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AY279" s="18">
         <v>0</v>
@@ -83397,7 +83397,7 @@
       </c>
       <c r="AW280" s="4"/>
       <c r="AX280" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY280" s="18">
         <v>0</v>
@@ -83420,7 +83420,7 @@
         <v>388</v>
       </c>
       <c r="D281" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E281" s="4">
         <v>1</v>
@@ -83554,7 +83554,7 @@
       </c>
       <c r="AW281" s="4"/>
       <c r="AX281" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY281" s="18">
         <v>0</v>
@@ -83577,7 +83577,7 @@
         <v>389</v>
       </c>
       <c r="D282" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E282" s="4">
         <v>1</v>
@@ -83711,7 +83711,7 @@
       </c>
       <c r="AW282" s="4"/>
       <c r="AX282" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY282" s="18">
         <v>0</v>
@@ -83734,7 +83734,7 @@
         <v>390</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E283" s="4">
         <v>1</v>
@@ -83868,7 +83868,7 @@
       </c>
       <c r="AW283" s="4"/>
       <c r="AX283" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY283" s="18">
         <v>0</v>
@@ -83891,7 +83891,7 @@
         <v>628</v>
       </c>
       <c r="D284" s="19" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E284" s="4">
         <v>6</v>
@@ -84025,7 +84025,7 @@
       </c>
       <c r="AW284" s="4"/>
       <c r="AX284" s="59" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AY284" s="18">
         <v>0</v>
@@ -84048,7 +84048,7 @@
         <v>631</v>
       </c>
       <c r="D285" s="19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E285" s="4">
         <v>6</v>
@@ -84184,7 +84184,7 @@
       </c>
       <c r="AW285" s="4"/>
       <c r="AX285" s="59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AY285" s="18">
         <v>0</v>
@@ -84337,7 +84337,7 @@
       </c>
       <c r="AW286" s="4"/>
       <c r="AX286" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY286" s="18">
         <v>0</v>
@@ -84492,7 +84492,7 @@
       </c>
       <c r="AW287" s="4"/>
       <c r="AX287" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY287" s="18">
         <v>0</v>
@@ -84515,7 +84515,7 @@
         <v>671</v>
       </c>
       <c r="D288" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E288" s="8">
         <v>3</v>
@@ -84649,7 +84649,7 @@
       </c>
       <c r="AW288" s="8"/>
       <c r="AX288" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY288" s="18">
         <v>0</v>
@@ -84666,13 +84666,13 @@
         <v>51000286</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C289" s="53" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D289" s="19" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E289" s="4">
         <v>2</v>
@@ -84806,7 +84806,7 @@
       </c>
       <c r="AW289" s="4"/>
       <c r="AX289" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AY289" s="18">
         <v>0</v>
@@ -84829,7 +84829,7 @@
         <v>667</v>
       </c>
       <c r="D290" s="19" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E290" s="8">
         <v>4</v>
@@ -84967,7 +84967,7 @@
       </c>
       <c r="AW290" s="8"/>
       <c r="AX290" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY290" s="18">
         <v>0</v>
@@ -85126,7 +85126,7 @@
       </c>
       <c r="AW291" s="4"/>
       <c r="AX291" s="59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="AY291" s="18">
         <v>0</v>
@@ -85143,13 +85143,13 @@
         <v>51000289</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D292" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E292" s="4">
         <v>2</v>
@@ -85211,7 +85211,7 @@
         <v>0</v>
       </c>
       <c r="X292" s="4" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Y292" s="37">
         <v>55900032</v>
@@ -85283,7 +85283,7 @@
       </c>
       <c r="AW292" s="4"/>
       <c r="AX292" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY292" s="18">
         <v>0</v>
@@ -85300,13 +85300,13 @@
         <v>51000290</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D293" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E293" s="4">
         <v>4</v>
@@ -85368,7 +85368,7 @@
         <v>0</v>
       </c>
       <c r="X293" s="4" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Y293" s="37">
         <v>55900032</v>
@@ -85440,7 +85440,7 @@
       </c>
       <c r="AW293" s="4"/>
       <c r="AX293" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY293" s="21">
         <v>0</v>
@@ -85603,7 +85603,7 @@
       </c>
       <c r="AW294" s="4"/>
       <c r="AX294" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY294" s="21">
         <v>0</v>
@@ -85758,7 +85758,7 @@
       </c>
       <c r="AW295" s="4"/>
       <c r="AX295" s="59" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AY295" s="21">
         <v>0</v>
@@ -85915,7 +85915,7 @@
       </c>
       <c r="AW296" s="8"/>
       <c r="AX296" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY296" s="21">
         <v>0</v>
@@ -86072,7 +86072,7 @@
       </c>
       <c r="AW297" s="4"/>
       <c r="AX297" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY297" s="21">
         <v>0</v>
@@ -86229,7 +86229,7 @@
       </c>
       <c r="AW298" s="4"/>
       <c r="AX298" s="59" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AY298" s="21">
         <v>0</v>
@@ -86384,7 +86384,7 @@
       </c>
       <c r="AW299" s="4"/>
       <c r="AX299" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY299" s="21">
         <v>0</v>
@@ -86539,7 +86539,7 @@
       </c>
       <c r="AW300" s="4"/>
       <c r="AX300" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY300" s="21">
         <v>0</v>
@@ -86702,7 +86702,7 @@
       </c>
       <c r="AW301" s="4"/>
       <c r="AX301" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AY301" s="21">
         <v>0</v>
@@ -86719,13 +86719,13 @@
         <v>51000299</v>
       </c>
       <c r="B302" s="7" t="s">
+        <v>882</v>
+      </c>
+      <c r="C302" s="7" t="s">
         <v>883</v>
       </c>
-      <c r="C302" s="7" t="s">
+      <c r="D302" s="8" t="s">
         <v>884</v>
-      </c>
-      <c r="D302" s="8" t="s">
-        <v>885</v>
       </c>
       <c r="E302" s="4">
         <v>5</v>
@@ -86861,7 +86861,7 @@
       </c>
       <c r="AW302" s="4"/>
       <c r="AX302" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY302" s="21">
         <v>0</v>
@@ -86878,13 +86878,13 @@
         <v>51000300</v>
       </c>
       <c r="B303" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="C303" s="7" t="s">
         <v>910</v>
       </c>
-      <c r="C303" s="7" t="s">
+      <c r="D303" s="8" t="s">
         <v>911</v>
-      </c>
-      <c r="D303" s="8" t="s">
-        <v>912</v>
       </c>
       <c r="E303" s="4">
         <v>3</v>
@@ -87018,7 +87018,7 @@
       </c>
       <c r="AW303" s="4"/>
       <c r="AX303" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AY303" s="21">
         <v>0</v>
@@ -87035,13 +87035,13 @@
         <v>51000301</v>
       </c>
       <c r="B304" s="60" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C304" s="7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D304" s="8" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E304" s="4">
         <v>5</v>
@@ -87103,7 +87103,7 @@
         <v>0</v>
       </c>
       <c r="X304" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Y304" s="18">
         <v>55300011</v>
@@ -87173,7 +87173,7 @@
       </c>
       <c r="AW304" s="4"/>
       <c r="AX304" s="59" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AY304" s="21">
         <v>0</v>
@@ -87405,10 +87405,10 @@
         <v>826</v>
       </c>
       <c r="AT1" s="56" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AU1" s="56" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AV1" s="16" t="s">
         <v>313</v>
@@ -87417,7 +87417,7 @@
         <v>312</v>
       </c>
       <c r="AX1" s="14" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AY1" s="16" t="s">
         <v>651</v>
@@ -87566,10 +87566,10 @@
         <v>827</v>
       </c>
       <c r="AT2" s="57" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AU2" s="57" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>285</v>
@@ -87578,7 +87578,7 @@
         <v>286</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>285</v>
@@ -87664,16 +87664,16 @@
         <v>296</v>
       </c>
       <c r="Y3" s="40" t="s">
+        <v>876</v>
+      </c>
+      <c r="Z3" s="40" t="s">
         <v>877</v>
       </c>
-      <c r="Z3" s="40" t="s">
+      <c r="AA3" s="40" t="s">
         <v>878</v>
       </c>
-      <c r="AA3" s="40" t="s">
+      <c r="AB3" s="40" t="s">
         <v>879</v>
-      </c>
-      <c r="AB3" s="40" t="s">
-        <v>880</v>
       </c>
       <c r="AC3" s="40" t="s">
         <v>752</v>
@@ -87727,10 +87727,10 @@
         <v>828</v>
       </c>
       <c r="AT3" s="58" t="s">
+        <v>923</v>
+      </c>
+      <c r="AU3" s="58" t="s">
         <v>924</v>
-      </c>
-      <c r="AU3" s="58" t="s">
-        <v>925</v>
       </c>
       <c r="AV3" s="6" t="s">
         <v>298</v>
@@ -87739,7 +87739,7 @@
         <v>297</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="AY3" s="17" t="s">
         <v>652</v>
@@ -87888,7 +87888,7 @@
       </c>
       <c r="AW4" s="18"/>
       <c r="AX4" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY4" s="18">
         <v>1</v>
@@ -87905,10 +87905,10 @@
         <v>51013001</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>872</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>873</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8">
@@ -88041,7 +88041,7 @@
       </c>
       <c r="AW5" s="18"/>
       <c r="AX5" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY5" s="18">
         <v>1</v>
@@ -88190,7 +88190,7 @@
       </c>
       <c r="AW6" s="18"/>
       <c r="AX6" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY6" s="21">
         <v>1</v>
@@ -88339,7 +88339,7 @@
       </c>
       <c r="AW7" s="18"/>
       <c r="AX7" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY7" s="21">
         <v>1</v>
@@ -88488,7 +88488,7 @@
       </c>
       <c r="AW8" s="18"/>
       <c r="AX8" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY8" s="21">
         <v>1</v>
@@ -88637,7 +88637,7 @@
       </c>
       <c r="AW9" s="18"/>
       <c r="AX9" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY9" s="21">
         <v>1</v>
@@ -88786,7 +88786,7 @@
       </c>
       <c r="AW10" s="18"/>
       <c r="AX10" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY10" s="21">
         <v>1</v>
@@ -88935,7 +88935,7 @@
       </c>
       <c r="AW11" s="18"/>
       <c r="AX11" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY11" s="21">
         <v>1</v>
@@ -88952,7 +88952,7 @@
         <v>51019298</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>630</v>
@@ -89084,7 +89084,7 @@
       </c>
       <c r="AW12" s="18"/>
       <c r="AX12" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY12" s="21">
         <v>1</v>
@@ -89101,7 +89101,7 @@
         <v>51019299</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>630</v>
@@ -89233,7 +89233,7 @@
       </c>
       <c r="AW13" s="18"/>
       <c r="AX13" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY13" s="21">
         <v>1</v>
@@ -89382,7 +89382,7 @@
       </c>
       <c r="AW14" s="18"/>
       <c r="AX14" s="59" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AY14" s="21">
         <v>1</v>
@@ -90157,7 +90157,7 @@
         <v>659</v>
       </c>
       <c r="B1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -90218,7 +90218,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -90226,7 +90226,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="24" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
@@ -90234,7 +90234,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B11" s="22"/>
     </row>

</xml_diff>

<commit_message>
#58 new monster hulk
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="953">
   <si>
     <t>arrow</t>
   </si>
@@ -3892,6 +3892,18 @@
   </si>
   <si>
     <t>光环</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿巨人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hulk</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7930,7 +7942,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7993,7 +8004,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8030,9 +8040,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8106,7 +8114,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8195,11 +8202,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="32566240"/>
-        <c:axId val="32566800"/>
+        <c:axId val="215074144"/>
+        <c:axId val="215074704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32566240"/>
+        <c:axId val="215074144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8242,7 +8249,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32566800"/>
+        <c:crossAx val="215074704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8250,7 +8257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32566800"/>
+        <c:axId val="215074704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8301,7 +8308,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32566240"/>
+        <c:crossAx val="215074144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8315,7 +8322,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8412,7 +8418,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8460,7 +8465,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8497,9 +8501,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -8573,7 +8575,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8677,11 +8678,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="282225792"/>
-        <c:axId val="225106784"/>
+        <c:axId val="215076944"/>
+        <c:axId val="215077504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="282225792"/>
+        <c:axId val="215076944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8724,7 +8725,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225106784"/>
+        <c:crossAx val="215077504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8732,7 +8733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225106784"/>
+        <c:axId val="215077504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8783,7 +8784,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="282225792"/>
+        <c:crossAx val="215076944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8797,7 +8798,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11316,7 +11316,6 @@
           <cell r="A160">
             <v>55900028</v>
           </cell>
-          <cell r="X160"/>
         </row>
         <row r="161">
           <cell r="A161">
@@ -11480,7 +11479,7 @@
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55990001</v>
+            <v>55900049</v>
           </cell>
           <cell r="X181">
             <v>15</v>
@@ -11488,7 +11487,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X182">
             <v>15</v>
@@ -11496,7 +11495,7 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X183">
             <v>15</v>
@@ -11504,7 +11503,7 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -11512,7 +11511,7 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -11520,7 +11519,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11528,7 +11527,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11536,7 +11535,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11544,7 +11543,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11552,7 +11551,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11560,7 +11559,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11568,7 +11567,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11576,41 +11575,49 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X193">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X194">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X195">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X196">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
+            <v>55990104</v>
+          </cell>
+          <cell r="X197">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="A198">
             <v>55990105</v>
           </cell>
-          <cell r="X197">
+          <cell r="X198">
             <v>150</v>
           </cell>
         </row>
@@ -39048,8 +39055,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA304" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
-  <autoFilter ref="A3:BA304"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA305" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
+  <autoFilter ref="A3:BA305"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
@@ -39504,13 +39511,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA304"/>
+  <dimension ref="A1:BA305"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C281" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="G289" sqref="G289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -73343,7 +73350,7 @@
         <v>781</v>
       </c>
       <c r="AS216" s="54">
-        <v>11000001</v>
+        <v>11000005</v>
       </c>
       <c r="AT216" s="4">
         <v>22011014</v>
@@ -87198,9 +87205,168 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="305" spans="1:53">
+      <c r="A305">
+        <v>51000302</v>
+      </c>
+      <c r="B305" s="60" t="s">
+        <v>950</v>
+      </c>
+      <c r="C305" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="D305" s="8"/>
+      <c r="E305" s="4">
+        <v>6</v>
+      </c>
+      <c r="F305" s="4">
+        <v>9</v>
+      </c>
+      <c r="G305" s="4">
+        <v>0</v>
+      </c>
+      <c r="H305" s="4">
+        <f t="shared" ref="H305" si="20">IF(AND(T305&gt;=13,T305&lt;=16),5,IF(AND(T305&gt;=9,T305&lt;=12),4,IF(AND(T305&gt;=5,T305&lt;=8),3,IF(AND(T305&gt;=1,T305&lt;=4),2,IF(AND(T305&gt;=-3,T305&lt;=0),1,IF(AND(T305&gt;=-5,T305&lt;=-4),0,6))))))</f>
+        <v>4</v>
+      </c>
+      <c r="I305" s="4">
+        <v>6</v>
+      </c>
+      <c r="J305" s="4">
+        <v>-40</v>
+      </c>
+      <c r="K305" s="4">
+        <v>5</v>
+      </c>
+      <c r="L305" s="4">
+        <v>-5</v>
+      </c>
+      <c r="M305" s="4">
+        <v>0</v>
+      </c>
+      <c r="N305" s="4">
+        <v>0</v>
+      </c>
+      <c r="O305" s="4">
+        <v>0</v>
+      </c>
+      <c r="P305" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q305" s="4">
+        <v>0</v>
+      </c>
+      <c r="R305" s="4">
+        <v>0</v>
+      </c>
+      <c r="S305" s="4">
+        <v>0</v>
+      </c>
+      <c r="T305" s="12">
+        <f t="shared" ref="T305" si="21">SUM(J305:K305)+SUM(M305:S305)*5+4.4*SUM(AJ305:AP305)+2.5*SUM(AD305:AH305)+IF(ISNUMBER(AC305),AC305,0)+L305</f>
+        <v>10</v>
+      </c>
+      <c r="U305" s="4">
+        <v>10</v>
+      </c>
+      <c r="V305" s="4">
+        <v>15</v>
+      </c>
+      <c r="W305" s="4">
+        <v>0</v>
+      </c>
+      <c r="X305" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y305" s="18">
+        <v>55100005</v>
+      </c>
+      <c r="Z305" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA305" s="18">
+        <v>55900049</v>
+      </c>
+      <c r="AB305" s="18">
+        <v>100</v>
+      </c>
+      <c r="AC305" s="18">
+        <f>IF(ISBLANK($Y305),0, LOOKUP($Y305,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z305/100)+
+IF(ISBLANK($AA305),0, LOOKUP($AA305,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB305/100)</f>
+        <v>50</v>
+      </c>
+      <c r="AD305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI305" s="4" t="str">
+        <f t="shared" ref="AI305" si="22">CONCATENATE(AD305,";",AE305,";",AF305,";",AG305,";",AH305)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP305" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ305" s="4" t="str">
+        <f t="shared" ref="AQ305" si="23">CONCATENATE(AJ305,";",AK305,";",AL305,";",AM305,";",AN305,";",AO305,";",AP305)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR305" s="50" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS305" s="54">
+        <v>11000001</v>
+      </c>
+      <c r="AT305" s="4"/>
+      <c r="AU305" s="4"/>
+      <c r="AV305" s="4">
+        <v>302</v>
+      </c>
+      <c r="AW305" s="4"/>
+      <c r="AX305" s="59" t="s">
+        <v>932</v>
+      </c>
+      <c r="AY305" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ305" s="19">
+        <v>1</v>
+      </c>
+      <c r="BA305" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H304">
+  <conditionalFormatting sqref="H4:H305">
     <cfRule type="cellIs" dxfId="140" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -87217,12 +87383,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D304">
+  <conditionalFormatting sqref="D4:D305">
     <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T304">
+  <conditionalFormatting sqref="T4:T305">
     <cfRule type="colorScale" priority="167">
       <colorScale>
         <cfvo type="min"/>
@@ -87247,7 +87413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
taunt effect enhance, remove skill hide
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -4993,6 +4993,271 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="141">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6321,226 +6586,6 @@
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7857,51 +7902,6 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -39055,159 +39055,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA305" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA305" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139" tableBorderDxfId="138">
   <autoFilter ref="A3:BA305"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="131"/>
-    <tableColumn id="2" name="Name" dataDxfId="130"/>
-    <tableColumn id="22" name="Ename" dataDxfId="129"/>
-    <tableColumn id="23" name="Remark" dataDxfId="128"/>
-    <tableColumn id="3" name="Star" dataDxfId="127"/>
-    <tableColumn id="4" name="Type" dataDxfId="126"/>
-    <tableColumn id="5" name="Attr" dataDxfId="125"/>
-    <tableColumn id="58" name="Quality" dataDxfId="124">
+    <tableColumn id="1" name="Id" dataDxfId="137"/>
+    <tableColumn id="2" name="Name" dataDxfId="136"/>
+    <tableColumn id="22" name="Ename" dataDxfId="135"/>
+    <tableColumn id="23" name="Remark" dataDxfId="134"/>
+    <tableColumn id="3" name="Star" dataDxfId="133"/>
+    <tableColumn id="4" name="Type" dataDxfId="132"/>
+    <tableColumn id="5" name="Attr" dataDxfId="131"/>
+    <tableColumn id="58" name="Quality" dataDxfId="130">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="123"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="122"/>
-    <tableColumn id="24" name="VitP" dataDxfId="121"/>
-    <tableColumn id="25" name="Modify" dataDxfId="120"/>
-    <tableColumn id="9" name="Def" dataDxfId="119"/>
-    <tableColumn id="10" name="Mag" dataDxfId="118"/>
-    <tableColumn id="32" name="Spd" dataDxfId="117"/>
-    <tableColumn id="35" name="Hit" dataDxfId="116"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="115"/>
-    <tableColumn id="34" name="Crt" dataDxfId="114"/>
-    <tableColumn id="33" name="Luk" dataDxfId="113"/>
-    <tableColumn id="7" name="Sum" dataDxfId="112">
+    <tableColumn id="12" name="Cost" dataDxfId="129"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="128"/>
+    <tableColumn id="24" name="VitP" dataDxfId="127"/>
+    <tableColumn id="25" name="Modify" dataDxfId="126"/>
+    <tableColumn id="9" name="Def" dataDxfId="125"/>
+    <tableColumn id="10" name="Mag" dataDxfId="124"/>
+    <tableColumn id="32" name="Spd" dataDxfId="123"/>
+    <tableColumn id="35" name="Hit" dataDxfId="122"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="121"/>
+    <tableColumn id="34" name="Crt" dataDxfId="120"/>
+    <tableColumn id="33" name="Luk" dataDxfId="119"/>
+    <tableColumn id="7" name="Sum" dataDxfId="118">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="111"/>
-    <tableColumn id="14" name="Mov" dataDxfId="110"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="109"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="108"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="107"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="106"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="105"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="104"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="103">
+    <tableColumn id="13" name="Range" dataDxfId="117"/>
+    <tableColumn id="14" name="Mov" dataDxfId="116"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="115"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="114"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="113"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="112"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="111"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="110"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="109">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="102"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="101"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="100"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="99"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="98"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="97">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="108"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="107"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="106"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="105"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="104"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="103">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="96"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="95"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="94"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="93"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="92"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="91"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="90"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="89">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="102"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="101"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="100"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="99"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="98"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="97"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="96"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="95">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="88"/>
-    <tableColumn id="29" name="JobId" dataDxfId="87"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="86"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="85"/>
-    <tableColumn id="21" name="Icon" dataDxfId="84"/>
-    <tableColumn id="17" name="Cover" dataDxfId="83"/>
-    <tableColumn id="18" name="Sound" dataDxfId="82"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="81"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="80"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="79"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="94"/>
+    <tableColumn id="29" name="JobId" dataDxfId="93"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="92"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="91"/>
+    <tableColumn id="21" name="Icon" dataDxfId="90"/>
+    <tableColumn id="17" name="Cover" dataDxfId="89"/>
+    <tableColumn id="18" name="Sound" dataDxfId="88"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="87"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="86"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA14" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA14" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="A3:BA14"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" name="Name" dataDxfId="52"/>
-    <tableColumn id="22" name="Ename" dataDxfId="51"/>
-    <tableColumn id="23" name="Remark" dataDxfId="50"/>
-    <tableColumn id="3" name="Star" dataDxfId="49"/>
-    <tableColumn id="4" name="Type" dataDxfId="48"/>
-    <tableColumn id="5" name="Attr" dataDxfId="47"/>
-    <tableColumn id="58" name="Quality" dataDxfId="46">
+    <tableColumn id="1" name="Id" dataDxfId="81"/>
+    <tableColumn id="2" name="Name" dataDxfId="80"/>
+    <tableColumn id="22" name="Ename" dataDxfId="79"/>
+    <tableColumn id="23" name="Remark" dataDxfId="78"/>
+    <tableColumn id="3" name="Star" dataDxfId="77"/>
+    <tableColumn id="4" name="Type" dataDxfId="76"/>
+    <tableColumn id="5" name="Attr" dataDxfId="75"/>
+    <tableColumn id="58" name="Quality" dataDxfId="74">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="45"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="44"/>
-    <tableColumn id="24" name="VitP" dataDxfId="43"/>
-    <tableColumn id="25" name="Modify" dataDxfId="42"/>
-    <tableColumn id="9" name="Def" dataDxfId="41"/>
-    <tableColumn id="10" name="Mag" dataDxfId="40"/>
-    <tableColumn id="32" name="Spd" dataDxfId="39"/>
-    <tableColumn id="35" name="Hit" dataDxfId="38"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="37"/>
-    <tableColumn id="34" name="Crt" dataDxfId="36"/>
-    <tableColumn id="33" name="Luk" dataDxfId="35"/>
-    <tableColumn id="7" name="Sum" dataDxfId="34">
+    <tableColumn id="12" name="Cost" dataDxfId="73"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="72"/>
+    <tableColumn id="24" name="VitP" dataDxfId="71"/>
+    <tableColumn id="25" name="Modify" dataDxfId="70"/>
+    <tableColumn id="9" name="Def" dataDxfId="69"/>
+    <tableColumn id="10" name="Mag" dataDxfId="68"/>
+    <tableColumn id="32" name="Spd" dataDxfId="67"/>
+    <tableColumn id="35" name="Hit" dataDxfId="66"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="65"/>
+    <tableColumn id="34" name="Crt" dataDxfId="64"/>
+    <tableColumn id="33" name="Luk" dataDxfId="63"/>
+    <tableColumn id="7" name="Sum" dataDxfId="62">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="33"/>
-    <tableColumn id="14" name="Mov" dataDxfId="32"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="31"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="30"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="29"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="28"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="27"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="26"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
+    <tableColumn id="13" name="Range" dataDxfId="61"/>
+    <tableColumn id="14" name="Mov" dataDxfId="60"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="59"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="58"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="57"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="56"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="55"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="54"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="53">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="52"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="51"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="50"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="49"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="48"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="47">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="11">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="46"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="45"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="44"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="43"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="42"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="41"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="40"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="39">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
-    <tableColumn id="29" name="JobId" dataDxfId="9"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="8"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="7"/>
-    <tableColumn id="21" name="Icon" dataDxfId="6"/>
-    <tableColumn id="17" name="Cover" dataDxfId="5"/>
-    <tableColumn id="18" name="Sound" dataDxfId="4"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="38"/>
+    <tableColumn id="29" name="JobId" dataDxfId="37"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="36"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="35"/>
+    <tableColumn id="21" name="Icon" dataDxfId="34"/>
+    <tableColumn id="17" name="Cover" dataDxfId="33"/>
+    <tableColumn id="18" name="Sound" dataDxfId="32"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="31"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="30"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="28">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39514,10 +39514,10 @@
   <dimension ref="A1:BA305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C281" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C211" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G289" sqref="G289"/>
+      <selection pane="bottomRight" activeCell="Q233" sqref="Q233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -69477,7 +69477,7 @@
         <v>0</v>
       </c>
       <c r="Q192" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R192" s="4">
         <v>1</v>
@@ -69507,16 +69507,12 @@
       <c r="Z192" s="18">
         <v>100</v>
       </c>
-      <c r="AA192" s="18">
-        <v>55100009</v>
-      </c>
-      <c r="AB192" s="18">
-        <v>100</v>
-      </c>
+      <c r="AA192" s="18"/>
+      <c r="AB192" s="18"/>
       <c r="AC192" s="18">
         <f>IF(ISBLANK($Y192),0, LOOKUP($Y192,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z192/100)+
 IF(ISBLANK($AA192),0, LOOKUP($AA192,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB192/100)</f>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AD192" s="18">
         <v>0</v>
@@ -69960,7 +69956,7 @@
         <v>0</v>
       </c>
       <c r="Q195" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R195" s="4">
         <v>0</v>
@@ -69990,16 +69986,12 @@
       <c r="Z195" s="18">
         <v>100</v>
       </c>
-      <c r="AA195" s="18">
-        <v>55100009</v>
-      </c>
-      <c r="AB195" s="18">
-        <v>100</v>
-      </c>
+      <c r="AA195" s="18"/>
+      <c r="AB195" s="18"/>
       <c r="AC195" s="18">
         <f>IF(ISBLANK($Y195),0, LOOKUP($Y195,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z195/100)+
 IF(ISBLANK($AA195),0, LOOKUP($AA195,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB195/100)</f>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="AD195" s="18">
         <v>0</v>
@@ -75942,7 +75934,7 @@
         <v>0</v>
       </c>
       <c r="Q233" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R233" s="4">
         <v>0</v>
@@ -75966,22 +75958,18 @@
       <c r="X233" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="Y233" s="37">
-        <v>55100009</v>
+      <c r="Y233" s="18">
+        <v>55600005</v>
       </c>
       <c r="Z233" s="18">
         <v>100</v>
       </c>
-      <c r="AA233" s="18">
-        <v>55600005</v>
-      </c>
-      <c r="AB233" s="18">
-        <v>100</v>
-      </c>
+      <c r="AA233" s="18"/>
+      <c r="AB233" s="18"/>
       <c r="AC233" s="18">
         <f>IF(ISBLANK($Y233),0, LOOKUP($Y233,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z233/100)+
 IF(ISBLANK($AA233),0, LOOKUP($AA233,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB233/100)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AD233" s="18">
         <v>0</v>
@@ -87367,24 +87355,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H305">
-    <cfRule type="cellIs" dxfId="140" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D305">
-    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89576,37 +89564,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 J6:K9 K12 K14">
-    <cfRule type="cellIs" dxfId="78" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="35" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="77" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="76" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="32" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="75" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="31" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="74" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="73" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89624,13 +89612,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="72" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="71" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89648,19 +89636,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89677,31 +89665,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="64" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89730,13 +89718,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
#58 add new monster ballista
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="956">
   <si>
     <t>arrow</t>
   </si>
@@ -3904,6 +3904,18 @@
   </si>
   <si>
     <t>Hulk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩炮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ballista</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4992,7 +5004,52 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="147">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -10130,79 +10187,79 @@
         </row>
         <row r="12">
           <cell r="A12">
-            <v>55100009</v>
+            <v>55100010</v>
           </cell>
           <cell r="X12">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>55100010</v>
+            <v>55100011</v>
           </cell>
           <cell r="X13">
-            <v>12</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>55100011</v>
+            <v>55100012</v>
           </cell>
           <cell r="X14">
-            <v>6</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>55100012</v>
+            <v>55100013</v>
           </cell>
           <cell r="X15">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55100013</v>
+            <v>55100014</v>
           </cell>
           <cell r="X16">
-            <v>10</v>
+            <v>24</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55100014</v>
+            <v>55100015</v>
           </cell>
           <cell r="X17">
-            <v>24</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>55100015</v>
+            <v>55110001</v>
           </cell>
           <cell r="X18">
-            <v>16</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>55110001</v>
+            <v>55110002</v>
           </cell>
           <cell r="X19">
-            <v>5</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>55110002</v>
+            <v>55110003</v>
           </cell>
           <cell r="X20">
-            <v>8</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>55110003</v>
+            <v>55110004</v>
           </cell>
           <cell r="X21">
             <v>25</v>
@@ -10210,135 +10267,135 @@
         </row>
         <row r="22">
           <cell r="A22">
-            <v>55110004</v>
+            <v>55110005</v>
           </cell>
           <cell r="X22">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>55110005</v>
+            <v>55110006</v>
           </cell>
           <cell r="X23">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>55110006</v>
+            <v>55110007</v>
           </cell>
           <cell r="X24">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>55110007</v>
+            <v>55110008</v>
           </cell>
           <cell r="X25">
-            <v>10</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>55110008</v>
+            <v>55110009</v>
           </cell>
           <cell r="X26">
-            <v>50</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>55110009</v>
+            <v>55110010</v>
           </cell>
           <cell r="X27">
-            <v>12</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>55110010</v>
+            <v>55110011</v>
           </cell>
           <cell r="X28">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>55110011</v>
+            <v>55110012</v>
           </cell>
           <cell r="X29">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>55110012</v>
+            <v>55110013</v>
           </cell>
           <cell r="X30">
-            <v>30</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>55110013</v>
+            <v>55110014</v>
           </cell>
           <cell r="X31">
-            <v>200</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>55110014</v>
+            <v>55110015</v>
           </cell>
           <cell r="X32">
-            <v>50</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>55110015</v>
+            <v>55110016</v>
           </cell>
           <cell r="X33">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>55110016</v>
+            <v>55110017</v>
           </cell>
           <cell r="X34">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>55110017</v>
+            <v>55110018</v>
           </cell>
           <cell r="X35">
-            <v>8</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>55110018</v>
+            <v>55110019</v>
           </cell>
           <cell r="X36">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>55110019</v>
+            <v>55110020</v>
           </cell>
           <cell r="X37">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55110020</v>
+            <v>55200001</v>
           </cell>
           <cell r="X38">
             <v>40</v>
@@ -10346,39 +10403,39 @@
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55200001</v>
+            <v>55200002</v>
           </cell>
           <cell r="X39">
-            <v>40</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55200002</v>
+            <v>55200003</v>
           </cell>
           <cell r="X40">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55200003</v>
+            <v>55200004</v>
           </cell>
           <cell r="X41">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55200004</v>
+            <v>55200005</v>
           </cell>
           <cell r="X42">
-            <v>40</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55200005</v>
+            <v>55200006</v>
           </cell>
           <cell r="X43">
             <v>20</v>
@@ -10386,7 +10443,7 @@
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55200006</v>
+            <v>55200007</v>
           </cell>
           <cell r="X44">
             <v>20</v>
@@ -10394,15 +10451,15 @@
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55200007</v>
+            <v>55200008</v>
           </cell>
           <cell r="X45">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55200008</v>
+            <v>55200009</v>
           </cell>
           <cell r="X46">
             <v>25</v>
@@ -10410,7 +10467,7 @@
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55200009</v>
+            <v>55200010</v>
           </cell>
           <cell r="X47">
             <v>25</v>
@@ -10418,55 +10475,55 @@
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55200010</v>
+            <v>55200011</v>
           </cell>
           <cell r="X48">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55200011</v>
+            <v>55200012</v>
           </cell>
           <cell r="X49">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55200012</v>
+            <v>55200013</v>
           </cell>
           <cell r="X50">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55200013</v>
+            <v>55200014</v>
           </cell>
           <cell r="X51">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55200014</v>
+            <v>55300001</v>
           </cell>
           <cell r="X52">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55300001</v>
+            <v>55300002</v>
           </cell>
           <cell r="X53">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55300002</v>
+            <v>55300003</v>
           </cell>
           <cell r="X54">
             <v>30</v>
@@ -10474,7 +10531,7 @@
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55300003</v>
+            <v>55300004</v>
           </cell>
           <cell r="X55">
             <v>30</v>
@@ -10482,7 +10539,7 @@
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55300004</v>
+            <v>55300005</v>
           </cell>
           <cell r="X56">
             <v>30</v>
@@ -10490,15 +10547,15 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55300005</v>
+            <v>55300006</v>
           </cell>
           <cell r="X57">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55300006</v>
+            <v>55300007</v>
           </cell>
           <cell r="X58">
             <v>25</v>
@@ -10506,15 +10563,15 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55300007</v>
+            <v>55300008</v>
           </cell>
           <cell r="X59">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55300008</v>
+            <v>55300009</v>
           </cell>
           <cell r="X60">
             <v>30</v>
@@ -10522,71 +10579,71 @@
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55300009</v>
+            <v>55300010</v>
           </cell>
           <cell r="X61">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55300010</v>
+            <v>55300011</v>
           </cell>
           <cell r="X62">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55300011</v>
+            <v>55300012</v>
           </cell>
           <cell r="X63">
-            <v>25</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55300012</v>
+            <v>55300013</v>
           </cell>
           <cell r="X64">
-            <v>5</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55300013</v>
+            <v>55310001</v>
           </cell>
           <cell r="X65">
-            <v>15</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55310001</v>
+            <v>55310002</v>
           </cell>
           <cell r="X66">
-            <v>100</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55310002</v>
+            <v>55310003</v>
           </cell>
           <cell r="X67">
-            <v>15</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55310003</v>
+            <v>55400001</v>
           </cell>
           <cell r="X68">
-            <v>13</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55400001</v>
+            <v>55400002</v>
           </cell>
           <cell r="X69">
             <v>80</v>
@@ -10594,7 +10651,7 @@
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55400002</v>
+            <v>55400003</v>
           </cell>
           <cell r="X70">
             <v>80</v>
@@ -10602,47 +10659,47 @@
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55400003</v>
+            <v>55400005</v>
           </cell>
           <cell r="X71">
-            <v>80</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55400005</v>
+            <v>55400006</v>
           </cell>
           <cell r="X72">
-            <v>55</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55400006</v>
+            <v>55400007</v>
           </cell>
           <cell r="X73">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55400007</v>
+            <v>55410001</v>
           </cell>
           <cell r="X74">
-            <v>25</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55410001</v>
+            <v>55500001</v>
           </cell>
           <cell r="X75">
-            <v>50</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55500001</v>
+            <v>55500002</v>
           </cell>
           <cell r="X76">
             <v>5</v>
@@ -10650,7 +10707,7 @@
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55500002</v>
+            <v>55500003</v>
           </cell>
           <cell r="X77">
             <v>5</v>
@@ -10658,7 +10715,7 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55500003</v>
+            <v>55500004</v>
           </cell>
           <cell r="X78">
             <v>5</v>
@@ -10666,7 +10723,7 @@
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55500004</v>
+            <v>55500005</v>
           </cell>
           <cell r="X79">
             <v>5</v>
@@ -10674,7 +10731,7 @@
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55500005</v>
+            <v>55500006</v>
           </cell>
           <cell r="X80">
             <v>5</v>
@@ -10682,7 +10739,7 @@
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55500006</v>
+            <v>55500007</v>
           </cell>
           <cell r="X81">
             <v>5</v>
@@ -10690,7 +10747,7 @@
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55500007</v>
+            <v>55500008</v>
           </cell>
           <cell r="X82">
             <v>5</v>
@@ -10698,7 +10755,7 @@
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55500008</v>
+            <v>55500009</v>
           </cell>
           <cell r="X83">
             <v>5</v>
@@ -10706,7 +10763,7 @@
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55500009</v>
+            <v>55500010</v>
           </cell>
           <cell r="X84">
             <v>5</v>
@@ -10714,7 +10771,7 @@
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500010</v>
+            <v>55500011</v>
           </cell>
           <cell r="X85">
             <v>5</v>
@@ -10722,7 +10779,7 @@
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500011</v>
+            <v>55500012</v>
           </cell>
           <cell r="X86">
             <v>5</v>
@@ -10730,7 +10787,7 @@
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500012</v>
+            <v>55500013</v>
           </cell>
           <cell r="X87">
             <v>5</v>
@@ -10738,7 +10795,7 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500013</v>
+            <v>55500014</v>
           </cell>
           <cell r="X88">
             <v>5</v>
@@ -10746,7 +10803,7 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55500014</v>
+            <v>55500015</v>
           </cell>
           <cell r="X89">
             <v>5</v>
@@ -10754,7 +10811,7 @@
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55500015</v>
+            <v>55500016</v>
           </cell>
           <cell r="X90">
             <v>5</v>
@@ -10762,23 +10819,23 @@
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55500016</v>
+            <v>55510001</v>
           </cell>
           <cell r="X91">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55510001</v>
+            <v>55510002</v>
           </cell>
           <cell r="X92">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55510002</v>
+            <v>55510003</v>
           </cell>
           <cell r="X93">
             <v>15</v>
@@ -10786,87 +10843,87 @@
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55510003</v>
+            <v>55510004</v>
           </cell>
           <cell r="X94">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55510004</v>
+            <v>55510006</v>
           </cell>
           <cell r="X95">
-            <v>12</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55510006</v>
+            <v>55510007</v>
           </cell>
           <cell r="X96">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55510007</v>
+            <v>55510009</v>
           </cell>
           <cell r="X97">
-            <v>10</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55510009</v>
+            <v>55510010</v>
           </cell>
           <cell r="X98">
-            <v>50</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55510010</v>
+            <v>55510011</v>
           </cell>
           <cell r="X99">
-            <v>5</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55510011</v>
+            <v>55510012</v>
           </cell>
           <cell r="X100">
-            <v>15</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510012</v>
+            <v>55510013</v>
           </cell>
           <cell r="X101">
-            <v>62</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510013</v>
+            <v>55510014</v>
           </cell>
           <cell r="X102">
-            <v>12</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55510014</v>
+            <v>55510018</v>
           </cell>
           <cell r="X103">
-            <v>25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55510018</v>
+            <v>55510019</v>
           </cell>
           <cell r="X104">
             <v>37</v>
@@ -10874,63 +10931,63 @@
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55510019</v>
+            <v>55520001</v>
           </cell>
           <cell r="X105">
-            <v>37</v>
+            <v>-25</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55520001</v>
+            <v>55520002</v>
           </cell>
           <cell r="X106">
-            <v>-25</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55520002</v>
+            <v>55520003</v>
           </cell>
           <cell r="X107">
-            <v>62</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55520003</v>
+            <v>55600001</v>
           </cell>
           <cell r="X108">
-            <v>27</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55600001</v>
+            <v>55600002</v>
           </cell>
           <cell r="X109">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55600002</v>
+            <v>55600004</v>
           </cell>
           <cell r="X110">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55600004</v>
+            <v>55600005</v>
           </cell>
           <cell r="X111">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55600005</v>
+            <v>55600006</v>
           </cell>
           <cell r="X112">
             <v>15</v>
@@ -10938,103 +10995,103 @@
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55600006</v>
+            <v>55600007</v>
           </cell>
           <cell r="X113">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55600007</v>
+            <v>55600008</v>
           </cell>
           <cell r="X114">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55600008</v>
+            <v>55600009</v>
           </cell>
           <cell r="X115">
-            <v>30</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55600009</v>
+            <v>55600010</v>
           </cell>
           <cell r="X116">
-            <v>13</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55600010</v>
+            <v>55600011</v>
           </cell>
           <cell r="X117">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55600011</v>
+            <v>55600012</v>
           </cell>
           <cell r="X118">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55600012</v>
+            <v>55600013</v>
           </cell>
           <cell r="X119">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55600013</v>
+            <v>55600014</v>
           </cell>
           <cell r="X120">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55600014</v>
+            <v>55600015</v>
           </cell>
           <cell r="X121">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55600015</v>
+            <v>55600016</v>
           </cell>
           <cell r="X122">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55600016</v>
+            <v>55610001</v>
           </cell>
           <cell r="X123">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55610001</v>
+            <v>55610002</v>
           </cell>
           <cell r="X124">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55610002</v>
+            <v>55610003</v>
           </cell>
           <cell r="X125">
             <v>5</v>
@@ -11042,23 +11099,23 @@
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55610003</v>
+            <v>55610004</v>
           </cell>
           <cell r="X126">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55610004</v>
+            <v>55700001</v>
           </cell>
           <cell r="X127">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55700001</v>
+            <v>55700002</v>
           </cell>
           <cell r="X128">
             <v>20</v>
@@ -11066,7 +11123,7 @@
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55700002</v>
+            <v>55700003</v>
           </cell>
           <cell r="X129">
             <v>20</v>
@@ -11074,7 +11131,7 @@
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55700003</v>
+            <v>55700004</v>
           </cell>
           <cell r="X130">
             <v>20</v>
@@ -11082,207 +11139,207 @@
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55700004</v>
+            <v>55700005</v>
           </cell>
           <cell r="X131">
-            <v>20</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55700005</v>
+            <v>55900001</v>
           </cell>
           <cell r="X132">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900001</v>
+            <v>55900002</v>
           </cell>
           <cell r="X133">
-            <v>35</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900002</v>
+            <v>55900003</v>
           </cell>
           <cell r="X134">
-            <v>30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900003</v>
+            <v>55900004</v>
           </cell>
           <cell r="X135">
-            <v>80</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900004</v>
+            <v>55900005</v>
           </cell>
           <cell r="X136">
-            <v>-30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900005</v>
+            <v>55900006</v>
           </cell>
           <cell r="X137">
-            <v>20</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900006</v>
+            <v>55900007</v>
           </cell>
           <cell r="X138">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900007</v>
+            <v>55900008</v>
           </cell>
           <cell r="X139">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900008</v>
+            <v>55900009</v>
           </cell>
           <cell r="X140">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900009</v>
+            <v>55900010</v>
           </cell>
           <cell r="X141">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900010</v>
+            <v>55900011</v>
           </cell>
           <cell r="X142">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900011</v>
+            <v>55900012</v>
           </cell>
           <cell r="X143">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900012</v>
+            <v>55900013</v>
           </cell>
           <cell r="X144">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900013</v>
+            <v>55900014</v>
           </cell>
           <cell r="X145">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900014</v>
+            <v>55900015</v>
           </cell>
           <cell r="X146">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900015</v>
+            <v>55900016</v>
           </cell>
           <cell r="X147">
-            <v>30</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900016</v>
+            <v>55900017</v>
           </cell>
           <cell r="X148">
-            <v>45</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900017</v>
+            <v>55900018</v>
           </cell>
           <cell r="X149">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900018</v>
+            <v>55900019</v>
           </cell>
           <cell r="X150">
-            <v>30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900019</v>
+            <v>55900020</v>
           </cell>
           <cell r="X151">
-            <v>80</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900020</v>
+            <v>55900021</v>
           </cell>
           <cell r="X152">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900021</v>
+            <v>55900022</v>
           </cell>
           <cell r="X153">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900022</v>
+            <v>55900023</v>
           </cell>
           <cell r="X154">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900023</v>
+            <v>55900024</v>
           </cell>
           <cell r="X155">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900024</v>
+            <v>55900025</v>
           </cell>
           <cell r="X156">
             <v>10</v>
@@ -11290,60 +11347,60 @@
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900025</v>
+            <v>55900026</v>
           </cell>
           <cell r="X157">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900026</v>
+            <v>55900027</v>
           </cell>
           <cell r="X158">
-            <v>20</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900027</v>
-          </cell>
-          <cell r="X159">
-            <v>35</v>
+            <v>55900028</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900028</v>
+            <v>55900029</v>
+          </cell>
+          <cell r="X160">
+            <v>15</v>
           </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900029</v>
+            <v>55900030</v>
           </cell>
           <cell r="X161">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900030</v>
+            <v>55900031</v>
           </cell>
           <cell r="X162">
-            <v>25</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900031</v>
+            <v>55900032</v>
           </cell>
           <cell r="X163">
-            <v>5</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900032</v>
+            <v>55900033</v>
           </cell>
           <cell r="X164">
             <v>20</v>
@@ -11351,15 +11408,15 @@
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900033</v>
+            <v>55900034</v>
           </cell>
           <cell r="X165">
-            <v>20</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900034</v>
+            <v>55900035</v>
           </cell>
           <cell r="X166">
             <v>14</v>
@@ -11367,31 +11424,31 @@
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900035</v>
+            <v>55900036</v>
           </cell>
           <cell r="X167">
-            <v>14</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900036</v>
+            <v>55900037</v>
           </cell>
           <cell r="X168">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900037</v>
+            <v>55900038</v>
           </cell>
           <cell r="X169">
-            <v>35</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900038</v>
+            <v>55900039</v>
           </cell>
           <cell r="X170">
             <v>40</v>
@@ -11399,55 +11456,55 @@
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900039</v>
+            <v>55900040</v>
           </cell>
           <cell r="X171">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900040</v>
+            <v>55900041</v>
           </cell>
           <cell r="X172">
-            <v>30</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900041</v>
+            <v>55900042</v>
           </cell>
           <cell r="X173">
-            <v>0</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900042</v>
+            <v>55900043</v>
           </cell>
           <cell r="X174">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900043</v>
+            <v>55900044</v>
           </cell>
           <cell r="X175">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900044</v>
+            <v>55900045</v>
           </cell>
           <cell r="X176">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900045</v>
+            <v>55900046</v>
           </cell>
           <cell r="X177">
             <v>25</v>
@@ -11455,31 +11512,31 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900046</v>
+            <v>55900047</v>
           </cell>
           <cell r="X178">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900047</v>
+            <v>55900048</v>
           </cell>
           <cell r="X179">
-            <v>30</v>
+            <v>70</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900048</v>
+            <v>55900049</v>
           </cell>
           <cell r="X180">
-            <v>70</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55900049</v>
+            <v>55990001</v>
           </cell>
           <cell r="X181">
             <v>15</v>
@@ -11487,7 +11544,7 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990001</v>
+            <v>55990002</v>
           </cell>
           <cell r="X182">
             <v>15</v>
@@ -11495,7 +11552,7 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990002</v>
+            <v>55990003</v>
           </cell>
           <cell r="X183">
             <v>15</v>
@@ -11503,7 +11560,7 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990003</v>
+            <v>55990004</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -11511,7 +11568,7 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990004</v>
+            <v>55990005</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -11519,7 +11576,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990005</v>
+            <v>55990006</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11527,7 +11584,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990006</v>
+            <v>55990011</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11535,7 +11592,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990011</v>
+            <v>55990012</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11543,7 +11600,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990012</v>
+            <v>55990013</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11551,7 +11608,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990013</v>
+            <v>55990014</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11559,7 +11616,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990014</v>
+            <v>55990015</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11567,7 +11624,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990015</v>
+            <v>55990016</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11575,49 +11632,41 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990016</v>
+            <v>55990101</v>
           </cell>
           <cell r="X193">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990101</v>
+            <v>55990102</v>
           </cell>
           <cell r="X194">
-            <v>8</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990102</v>
+            <v>55990103</v>
           </cell>
           <cell r="X195">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990103</v>
+            <v>55990104</v>
           </cell>
           <cell r="X196">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990104</v>
+            <v>55990105</v>
           </cell>
           <cell r="X197">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="A198">
-            <v>55990105</v>
-          </cell>
-          <cell r="X198">
             <v>150</v>
           </cell>
         </row>
@@ -39055,159 +39104,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA305" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139" tableBorderDxfId="138">
-  <autoFilter ref="A3:BA305"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA306" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" tableBorderDxfId="144">
+  <autoFilter ref="A3:BA306"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="137"/>
-    <tableColumn id="2" name="Name" dataDxfId="136"/>
-    <tableColumn id="22" name="Ename" dataDxfId="135"/>
-    <tableColumn id="23" name="Remark" dataDxfId="134"/>
-    <tableColumn id="3" name="Star" dataDxfId="133"/>
-    <tableColumn id="4" name="Type" dataDxfId="132"/>
-    <tableColumn id="5" name="Attr" dataDxfId="131"/>
-    <tableColumn id="58" name="Quality" dataDxfId="130">
+    <tableColumn id="1" name="Id" dataDxfId="143"/>
+    <tableColumn id="2" name="Name" dataDxfId="142"/>
+    <tableColumn id="22" name="Ename" dataDxfId="141"/>
+    <tableColumn id="23" name="Remark" dataDxfId="140"/>
+    <tableColumn id="3" name="Star" dataDxfId="139"/>
+    <tableColumn id="4" name="Type" dataDxfId="138"/>
+    <tableColumn id="5" name="Attr" dataDxfId="137"/>
+    <tableColumn id="58" name="Quality" dataDxfId="136">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="129"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="128"/>
-    <tableColumn id="24" name="VitP" dataDxfId="127"/>
-    <tableColumn id="25" name="Modify" dataDxfId="126"/>
-    <tableColumn id="9" name="Def" dataDxfId="125"/>
-    <tableColumn id="10" name="Mag" dataDxfId="124"/>
-    <tableColumn id="32" name="Spd" dataDxfId="123"/>
-    <tableColumn id="35" name="Hit" dataDxfId="122"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="121"/>
-    <tableColumn id="34" name="Crt" dataDxfId="120"/>
-    <tableColumn id="33" name="Luk" dataDxfId="119"/>
-    <tableColumn id="7" name="Sum" dataDxfId="118">
+    <tableColumn id="12" name="Cost" dataDxfId="135"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="134"/>
+    <tableColumn id="24" name="VitP" dataDxfId="133"/>
+    <tableColumn id="25" name="Modify" dataDxfId="132"/>
+    <tableColumn id="9" name="Def" dataDxfId="131"/>
+    <tableColumn id="10" name="Mag" dataDxfId="130"/>
+    <tableColumn id="32" name="Spd" dataDxfId="129"/>
+    <tableColumn id="35" name="Hit" dataDxfId="128"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="127"/>
+    <tableColumn id="34" name="Crt" dataDxfId="126"/>
+    <tableColumn id="33" name="Luk" dataDxfId="125"/>
+    <tableColumn id="7" name="Sum" dataDxfId="124">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="117"/>
-    <tableColumn id="14" name="Mov" dataDxfId="116"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="115"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="114"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="113"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="112"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="111"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="110"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="109">
+    <tableColumn id="13" name="Range" dataDxfId="123"/>
+    <tableColumn id="14" name="Mov" dataDxfId="122"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="121"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="120"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="119"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="118"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="117"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="116"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="115">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="108"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="107"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="106"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="105"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="104"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="103">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="114"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="113"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="112"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="111"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="110"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="109">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="102"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="101"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="100"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="99"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="98"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="97"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="96"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="95">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="108"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="107"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="106"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="105"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="104"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="103"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="102"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="101">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="94"/>
-    <tableColumn id="29" name="JobId" dataDxfId="93"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="92"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="91"/>
-    <tableColumn id="21" name="Icon" dataDxfId="90"/>
-    <tableColumn id="17" name="Cover" dataDxfId="89"/>
-    <tableColumn id="18" name="Sound" dataDxfId="88"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="87"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="86"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="85"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="100"/>
+    <tableColumn id="29" name="JobId" dataDxfId="99"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="98"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="97"/>
+    <tableColumn id="21" name="Icon" dataDxfId="96"/>
+    <tableColumn id="17" name="Cover" dataDxfId="95"/>
+    <tableColumn id="18" name="Sound" dataDxfId="94"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="93"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="92"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA14" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA14" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A3:BA14"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="81"/>
-    <tableColumn id="2" name="Name" dataDxfId="80"/>
-    <tableColumn id="22" name="Ename" dataDxfId="79"/>
-    <tableColumn id="23" name="Remark" dataDxfId="78"/>
-    <tableColumn id="3" name="Star" dataDxfId="77"/>
-    <tableColumn id="4" name="Type" dataDxfId="76"/>
-    <tableColumn id="5" name="Attr" dataDxfId="75"/>
-    <tableColumn id="58" name="Quality" dataDxfId="74">
+    <tableColumn id="1" name="Id" dataDxfId="87"/>
+    <tableColumn id="2" name="Name" dataDxfId="86"/>
+    <tableColumn id="22" name="Ename" dataDxfId="85"/>
+    <tableColumn id="23" name="Remark" dataDxfId="84"/>
+    <tableColumn id="3" name="Star" dataDxfId="83"/>
+    <tableColumn id="4" name="Type" dataDxfId="82"/>
+    <tableColumn id="5" name="Attr" dataDxfId="81"/>
+    <tableColumn id="58" name="Quality" dataDxfId="80">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="73"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="72"/>
-    <tableColumn id="24" name="VitP" dataDxfId="71"/>
-    <tableColumn id="25" name="Modify" dataDxfId="70"/>
-    <tableColumn id="9" name="Def" dataDxfId="69"/>
-    <tableColumn id="10" name="Mag" dataDxfId="68"/>
-    <tableColumn id="32" name="Spd" dataDxfId="67"/>
-    <tableColumn id="35" name="Hit" dataDxfId="66"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="65"/>
-    <tableColumn id="34" name="Crt" dataDxfId="64"/>
-    <tableColumn id="33" name="Luk" dataDxfId="63"/>
-    <tableColumn id="7" name="Sum" dataDxfId="62">
+    <tableColumn id="12" name="Cost" dataDxfId="79"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="78"/>
+    <tableColumn id="24" name="VitP" dataDxfId="77"/>
+    <tableColumn id="25" name="Modify" dataDxfId="76"/>
+    <tableColumn id="9" name="Def" dataDxfId="75"/>
+    <tableColumn id="10" name="Mag" dataDxfId="74"/>
+    <tableColumn id="32" name="Spd" dataDxfId="73"/>
+    <tableColumn id="35" name="Hit" dataDxfId="72"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="71"/>
+    <tableColumn id="34" name="Crt" dataDxfId="70"/>
+    <tableColumn id="33" name="Luk" dataDxfId="69"/>
+    <tableColumn id="7" name="Sum" dataDxfId="68">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="61"/>
-    <tableColumn id="14" name="Mov" dataDxfId="60"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="59"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="58"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="57"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="56"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="55"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="54"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="53">
+    <tableColumn id="13" name="Range" dataDxfId="67"/>
+    <tableColumn id="14" name="Mov" dataDxfId="66"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="65"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="64"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="63"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="62"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="61"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="60"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="59">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="52"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="51"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="50"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="49"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="48"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="47">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="58"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="57"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="56"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="55"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="54"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="53">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="46"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="45"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="44"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="43"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="42"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="41"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="40"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="39">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="52"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="51"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="50"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="49"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="48"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="47"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="46"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="38"/>
-    <tableColumn id="29" name="JobId" dataDxfId="37"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="36"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="35"/>
-    <tableColumn id="21" name="Icon" dataDxfId="34"/>
-    <tableColumn id="17" name="Cover" dataDxfId="33"/>
-    <tableColumn id="18" name="Sound" dataDxfId="32"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="31"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="30"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="29"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="44"/>
+    <tableColumn id="29" name="JobId" dataDxfId="43"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="42"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="41"/>
+    <tableColumn id="21" name="Icon" dataDxfId="40"/>
+    <tableColumn id="17" name="Cover" dataDxfId="39"/>
+    <tableColumn id="18" name="Sound" dataDxfId="38"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="37"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="36"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39511,13 +39560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA305"/>
+  <dimension ref="A1:BA306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C211" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="Y300" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q233" sqref="Q233"/>
+      <selection pane="bottomRight" activeCell="AS305" sqref="AS305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -86716,7 +86765,7 @@
         <v>0</v>
       </c>
       <c r="AZ301" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA301" s="52">
         <v>0.75409839999999995</v>
@@ -87214,7 +87263,7 @@
         <v>0</v>
       </c>
       <c r="H305" s="4">
-        <f t="shared" ref="H305" si="20">IF(AND(T305&gt;=13,T305&lt;=16),5,IF(AND(T305&gt;=9,T305&lt;=12),4,IF(AND(T305&gt;=5,T305&lt;=8),3,IF(AND(T305&gt;=1,T305&lt;=4),2,IF(AND(T305&gt;=-3,T305&lt;=0),1,IF(AND(T305&gt;=-5,T305&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H305:H306" si="20">IF(AND(T305&gt;=13,T305&lt;=16),5,IF(AND(T305&gt;=9,T305&lt;=12),4,IF(AND(T305&gt;=5,T305&lt;=8),3,IF(AND(T305&gt;=1,T305&lt;=4),2,IF(AND(T305&gt;=-3,T305&lt;=0),1,IF(AND(T305&gt;=-5,T305&lt;=-4),0,6))))))</f>
         <v>4</v>
       </c>
       <c r="I305" s="4">
@@ -87251,7 +87300,7 @@
         <v>0</v>
       </c>
       <c r="T305" s="12">
-        <f t="shared" ref="T305" si="21">SUM(J305:K305)+SUM(M305:S305)*5+4.4*SUM(AJ305:AP305)+2.5*SUM(AD305:AH305)+IF(ISNUMBER(AC305),AC305,0)+L305</f>
+        <f t="shared" ref="T305:T306" si="21">SUM(J305:K305)+SUM(M305:S305)*5+4.4*SUM(AJ305:AP305)+2.5*SUM(AD305:AH305)+IF(ISNUMBER(AC305),AC305,0)+L305</f>
         <v>10</v>
       </c>
       <c r="U305" s="4">
@@ -87299,7 +87348,7 @@
         <v>0</v>
       </c>
       <c r="AI305" s="4" t="str">
-        <f t="shared" ref="AI305" si="22">CONCATENATE(AD305,";",AE305,";",AF305,";",AG305,";",AH305)</f>
+        <f t="shared" ref="AI305:AI306" si="22">CONCATENATE(AD305,";",AE305,";",AF305,";",AG305,";",AH305)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ305" s="18">
@@ -87324,7 +87373,7 @@
         <v>0</v>
       </c>
       <c r="AQ305" s="4" t="str">
-        <f t="shared" ref="AQ305" si="23">CONCATENATE(AJ305,";",AK305,";",AL305,";",AM305,";",AN305,";",AO305,";",AP305)</f>
+        <f t="shared" ref="AQ305:AQ306" si="23">CONCATENATE(AJ305,";",AK305,";",AL305,";",AM305,";",AN305,";",AO305,";",AP305)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR305" s="50" t="s">
@@ -87352,32 +87401,219 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="306" spans="1:53">
+      <c r="A306">
+        <v>51000303</v>
+      </c>
+      <c r="B306" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="C306" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="D306" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E306" s="8">
+        <v>4</v>
+      </c>
+      <c r="F306" s="8">
+        <v>2</v>
+      </c>
+      <c r="G306" s="8">
+        <v>4</v>
+      </c>
+      <c r="H306" s="21">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I306" s="8">
+        <v>4</v>
+      </c>
+      <c r="J306" s="8">
+        <v>-10</v>
+      </c>
+      <c r="K306" s="8">
+        <v>0</v>
+      </c>
+      <c r="L306" s="8">
+        <v>-1</v>
+      </c>
+      <c r="M306" s="8">
+        <v>0</v>
+      </c>
+      <c r="N306" s="8">
+        <v>0</v>
+      </c>
+      <c r="O306" s="8">
+        <v>3</v>
+      </c>
+      <c r="P306" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q306" s="8">
+        <v>0</v>
+      </c>
+      <c r="R306" s="8">
+        <v>0</v>
+      </c>
+      <c r="S306" s="8">
+        <v>0</v>
+      </c>
+      <c r="T306" s="21">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="U306" s="8">
+        <v>60</v>
+      </c>
+      <c r="V306" s="8">
+        <v>5</v>
+      </c>
+      <c r="W306" s="8">
+        <v>0</v>
+      </c>
+      <c r="X306" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y306" s="18"/>
+      <c r="Z306" s="18"/>
+      <c r="AA306" s="18"/>
+      <c r="AB306" s="18"/>
+      <c r="AC306" s="18">
+        <f>IF(ISBLANK($Y306),0, LOOKUP($Y306,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z306/100)+
+IF(ISBLANK($AA306),0, LOOKUP($AA306,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB306/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI306" s="8" t="str">
+        <f t="shared" si="22"/>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP306" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ306" s="8" t="str">
+        <f t="shared" si="23"/>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR306" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS306" s="55">
+        <v>11000004</v>
+      </c>
+      <c r="AT306" s="8"/>
+      <c r="AU306" s="8"/>
+      <c r="AV306" s="8">
+        <v>303</v>
+      </c>
+      <c r="AW306" s="8"/>
+      <c r="AX306" s="59" t="s">
+        <v>944</v>
+      </c>
+      <c r="AY306" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ306" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA306" s="8">
+        <v>0.24262300000000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H305">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H306">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D305">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+  <conditionalFormatting sqref="D4:D306">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T305">
-    <cfRule type="colorScale" priority="167">
+  <conditionalFormatting sqref="T4:T306">
+    <cfRule type="colorScale" priority="174">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H306">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D306">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"未完成"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T306">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -89564,37 +89800,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 J6:K9 K12 K14">
-    <cfRule type="cellIs" dxfId="21" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="35" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="20" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="18" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89612,13 +89848,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -89636,19 +89872,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89665,31 +89901,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89718,13 +89954,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
new monster shadow snake
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="6" r:id="rId7"/>
+    <pivotCache cacheId="7" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="962">
   <si>
     <t>arrow</t>
   </si>
@@ -3932,6 +3932,14 @@
   </si>
   <si>
     <t>Kathari</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗影蝮蛇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snake Shadow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8275,11 +8283,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="89250928"/>
-        <c:axId val="89251488"/>
+        <c:axId val="269065008"/>
+        <c:axId val="269065568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89250928"/>
+        <c:axId val="269065008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8322,7 +8330,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89251488"/>
+        <c:crossAx val="269065568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8330,7 +8338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89251488"/>
+        <c:axId val="269065568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8381,7 +8389,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89250928"/>
+        <c:crossAx val="269065008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8751,11 +8759,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="88892288"/>
-        <c:axId val="88892848"/>
+        <c:axId val="274121952"/>
+        <c:axId val="274122512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88892288"/>
+        <c:axId val="274121952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8798,7 +8806,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88892848"/>
+        <c:crossAx val="274122512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8806,7 +8814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88892848"/>
+        <c:axId val="274122512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8857,7 +8865,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88892288"/>
+        <c:crossAx val="274121952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11560,15 +11568,15 @@
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55990001</v>
+            <v>55900050</v>
           </cell>
           <cell r="X182">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X183">
             <v>15</v>
@@ -11576,7 +11584,7 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -11584,7 +11592,7 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -11592,7 +11600,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11600,7 +11608,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11608,7 +11616,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11616,7 +11624,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11624,7 +11632,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11632,7 +11640,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11640,7 +11648,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11648,7 +11656,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11656,41 +11664,49 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X194">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X195">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X196">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X197">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
+            <v>55990104</v>
+          </cell>
+          <cell r="X198">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="A199">
             <v>55990105</v>
           </cell>
-          <cell r="X198">
+          <cell r="X199">
             <v>150</v>
           </cell>
         </row>
@@ -38586,7 +38602,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -38684,7 +38700,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="56">
     <pivotField dataField="1" showAll="0"/>
@@ -39128,8 +39144,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA307" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
-  <autoFilter ref="A3:BA307"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA308" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
+  <autoFilter ref="A3:BA308"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
@@ -39584,13 +39600,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA307"/>
+  <dimension ref="A1:BA308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="S297" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AS307" sqref="AS307"/>
+      <selection pane="bottomRight" activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -87735,9 +87751,164 @@
         <v>0.24262300000000001</v>
       </c>
     </row>
+    <row r="308" spans="1:53">
+      <c r="A308">
+        <v>51000305</v>
+      </c>
+      <c r="B308" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="C308" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="D308" s="8"/>
+      <c r="E308" s="8">
+        <v>2</v>
+      </c>
+      <c r="F308" s="8">
+        <v>7</v>
+      </c>
+      <c r="G308" s="8">
+        <v>6</v>
+      </c>
+      <c r="H308" s="21">
+        <f t="shared" ref="H308" si="28">IF(AND(T308&gt;=13,T308&lt;=16),5,IF(AND(T308&gt;=9,T308&lt;=12),4,IF(AND(T308&gt;=5,T308&lt;=8),3,IF(AND(T308&gt;=1,T308&lt;=4),2,IF(AND(T308&gt;=-3,T308&lt;=0),1,IF(AND(T308&gt;=-5,T308&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I308" s="8">
+        <v>2</v>
+      </c>
+      <c r="J308" s="8">
+        <v>-20</v>
+      </c>
+      <c r="K308" s="8">
+        <v>10</v>
+      </c>
+      <c r="L308" s="8">
+        <v>-12</v>
+      </c>
+      <c r="M308" s="8">
+        <v>0</v>
+      </c>
+      <c r="N308" s="8">
+        <v>0</v>
+      </c>
+      <c r="O308" s="8">
+        <v>0</v>
+      </c>
+      <c r="P308" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q308" s="8">
+        <v>0</v>
+      </c>
+      <c r="R308" s="8">
+        <v>0</v>
+      </c>
+      <c r="S308" s="8">
+        <v>0</v>
+      </c>
+      <c r="T308" s="21">
+        <f t="shared" ref="T308" si="29">SUM(J308:K308)+SUM(M308:S308)*5+4.4*SUM(AJ308:AP308)+2.5*SUM(AD308:AH308)+IF(ISNUMBER(AC308),AC308,0)+L308</f>
+        <v>-2</v>
+      </c>
+      <c r="U308" s="8">
+        <v>60</v>
+      </c>
+      <c r="V308" s="8">
+        <v>15</v>
+      </c>
+      <c r="W308" s="8">
+        <v>0</v>
+      </c>
+      <c r="X308" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y308" s="18">
+        <v>55900050</v>
+      </c>
+      <c r="Z308" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA308" s="18"/>
+      <c r="AB308" s="18"/>
+      <c r="AC308" s="18">
+        <f>IF(ISBLANK($Y308),0, LOOKUP($Y308,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z308/100)+
+IF(ISBLANK($AA308),0, LOOKUP($AA308,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB308/100)</f>
+        <v>20</v>
+      </c>
+      <c r="AD308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI308" s="8" t="str">
+        <f t="shared" ref="AI308" si="30">CONCATENATE(AD308,";",AE308,";",AF308,";",AG308,";",AH308)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP308" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ308" s="8" t="str">
+        <f t="shared" ref="AQ308" si="31">CONCATENATE(AJ308,";",AK308,";",AL308,";",AM308,";",AN308,";",AO308,";",AP308)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR308" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS308" s="55">
+        <v>11000003</v>
+      </c>
+      <c r="AT308" s="8"/>
+      <c r="AU308" s="8"/>
+      <c r="AV308" s="8">
+        <v>305</v>
+      </c>
+      <c r="AW308" s="8"/>
+      <c r="AX308" s="59" t="s">
+        <v>935</v>
+      </c>
+      <c r="AY308" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ308" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA308" s="8">
+        <v>0.24262300000000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H307">
+  <conditionalFormatting sqref="H4:H308">
     <cfRule type="cellIs" dxfId="146" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -87754,12 +87925,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D307">
+  <conditionalFormatting sqref="D4:D308">
     <cfRule type="cellIs" dxfId="141" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T307">
+  <conditionalFormatting sqref="T4:T308">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -87771,7 +87942,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H307">
+  <conditionalFormatting sqref="H306:H308">
     <cfRule type="cellIs" dxfId="140" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -87788,12 +87959,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D307">
+  <conditionalFormatting sqref="D306:D308">
     <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T307">
+  <conditionalFormatting sqref="T306:T308">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
#58 new monster kid the thief
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId7"/>
-    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="969">
   <si>
     <t>arrow</t>
   </si>
@@ -3927,19 +3927,47 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Kathari</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗影蝮蛇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snake Shadow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪盗基德</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kid the Thief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bandattack</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kid Member</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>基德随从</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>连击，直伤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Kathari</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>暗影蝮蛇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Snake Shadow</t>
+    <t>连击，召唤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5028,7 +5056,357 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="148">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6107,34 +6485,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -6352,226 +6702,6 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7896,96 +8026,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -8283,11 +8323,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="269065008"/>
-        <c:axId val="269065568"/>
+        <c:axId val="214040640"/>
+        <c:axId val="214041200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="269065008"/>
+        <c:axId val="214040640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8330,7 +8370,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269065568"/>
+        <c:crossAx val="214041200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8338,7 +8378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="269065568"/>
+        <c:axId val="214041200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8389,7 +8429,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269065008"/>
+        <c:crossAx val="214040640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8759,11 +8799,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="274121952"/>
-        <c:axId val="274122512"/>
+        <c:axId val="214043440"/>
+        <c:axId val="214044000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="274121952"/>
+        <c:axId val="214043440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8806,7 +8846,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274122512"/>
+        <c:crossAx val="214044000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8814,7 +8854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274122512"/>
+        <c:axId val="214044000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8865,7 +8905,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274121952"/>
+        <c:crossAx val="214043440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11576,15 +11616,15 @@
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55990001</v>
+            <v>55900051</v>
           </cell>
           <cell r="X183">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X184">
             <v>15</v>
@@ -11592,7 +11632,7 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -11600,7 +11640,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11608,7 +11648,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11616,7 +11656,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11624,7 +11664,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11632,7 +11672,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11640,7 +11680,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11648,7 +11688,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11656,7 +11696,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11664,7 +11704,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -11672,41 +11712,49 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X195">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X196">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X197">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X198">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
+            <v>55990104</v>
+          </cell>
+          <cell r="X199">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="A200">
             <v>55990105</v>
           </cell>
-          <cell r="X199">
+          <cell r="X200">
             <v>150</v>
           </cell>
         </row>
@@ -38602,7 +38650,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -38700,7 +38748,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="56">
     <pivotField dataField="1" showAll="0"/>
@@ -39144,159 +39192,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA308" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
-  <autoFilter ref="A3:BA308"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA309" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+  <autoFilter ref="A3:BA309"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="131"/>
-    <tableColumn id="2" name="Name" dataDxfId="130"/>
-    <tableColumn id="22" name="Ename" dataDxfId="129"/>
-    <tableColumn id="23" name="Remark" dataDxfId="128"/>
-    <tableColumn id="3" name="Star" dataDxfId="127"/>
-    <tableColumn id="4" name="Type" dataDxfId="126"/>
-    <tableColumn id="5" name="Attr" dataDxfId="125"/>
-    <tableColumn id="58" name="Quality" dataDxfId="124">
+    <tableColumn id="1" name="Id" dataDxfId="144"/>
+    <tableColumn id="2" name="Name" dataDxfId="143"/>
+    <tableColumn id="22" name="Ename" dataDxfId="142"/>
+    <tableColumn id="23" name="Remark" dataDxfId="141"/>
+    <tableColumn id="3" name="Star" dataDxfId="140"/>
+    <tableColumn id="4" name="Type" dataDxfId="139"/>
+    <tableColumn id="5" name="Attr" dataDxfId="138"/>
+    <tableColumn id="58" name="Quality" dataDxfId="137">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="123"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="122"/>
-    <tableColumn id="24" name="VitP" dataDxfId="121"/>
-    <tableColumn id="25" name="Modify" dataDxfId="120"/>
-    <tableColumn id="9" name="Def" dataDxfId="119"/>
-    <tableColumn id="10" name="Mag" dataDxfId="118"/>
-    <tableColumn id="32" name="Spd" dataDxfId="117"/>
-    <tableColumn id="35" name="Hit" dataDxfId="116"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="115"/>
-    <tableColumn id="34" name="Crt" dataDxfId="114"/>
-    <tableColumn id="33" name="Luk" dataDxfId="113"/>
-    <tableColumn id="7" name="Sum" dataDxfId="112">
+    <tableColumn id="12" name="Cost" dataDxfId="136"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="135"/>
+    <tableColumn id="24" name="VitP" dataDxfId="134"/>
+    <tableColumn id="25" name="Modify" dataDxfId="133"/>
+    <tableColumn id="9" name="Def" dataDxfId="132"/>
+    <tableColumn id="10" name="Mag" dataDxfId="131"/>
+    <tableColumn id="32" name="Spd" dataDxfId="130"/>
+    <tableColumn id="35" name="Hit" dataDxfId="129"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="128"/>
+    <tableColumn id="34" name="Crt" dataDxfId="127"/>
+    <tableColumn id="33" name="Luk" dataDxfId="126"/>
+    <tableColumn id="7" name="Sum" dataDxfId="125">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="111"/>
-    <tableColumn id="14" name="Mov" dataDxfId="110"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="109"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="108"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="107"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="106"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="105"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="104"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="103">
+    <tableColumn id="13" name="Range" dataDxfId="124"/>
+    <tableColumn id="14" name="Mov" dataDxfId="123"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="122"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="121"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="120"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="119"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="118"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="117"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="116">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="102"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="101"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="100"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="99"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="98"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="97">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="115"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="114"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="113"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="112"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="111"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="110">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="96"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="95"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="94"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="93"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="92"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="91"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="90"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="89">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="109"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="108"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="107"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="106"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="105"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="104"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="103"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="102">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="88"/>
-    <tableColumn id="29" name="JobId" dataDxfId="87"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="86"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="85"/>
-    <tableColumn id="21" name="Icon" dataDxfId="84"/>
-    <tableColumn id="17" name="Cover" dataDxfId="83"/>
-    <tableColumn id="18" name="Sound" dataDxfId="82"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="81"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="80"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="79"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="101"/>
+    <tableColumn id="29" name="JobId" dataDxfId="100"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="99"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="98"/>
+    <tableColumn id="21" name="Icon" dataDxfId="97"/>
+    <tableColumn id="17" name="Cover" dataDxfId="96"/>
+    <tableColumn id="18" name="Sound" dataDxfId="95"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="94"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="93"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA14" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
-  <autoFilter ref="A3:BA14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+  <autoFilter ref="A3:BA15"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" name="Name" dataDxfId="52"/>
-    <tableColumn id="22" name="Ename" dataDxfId="51"/>
-    <tableColumn id="23" name="Remark" dataDxfId="50"/>
-    <tableColumn id="3" name="Star" dataDxfId="49"/>
-    <tableColumn id="4" name="Type" dataDxfId="48"/>
-    <tableColumn id="5" name="Attr" dataDxfId="47"/>
-    <tableColumn id="58" name="Quality" dataDxfId="46">
+    <tableColumn id="1" name="Id" dataDxfId="88"/>
+    <tableColumn id="2" name="Name" dataDxfId="87"/>
+    <tableColumn id="22" name="Ename" dataDxfId="86"/>
+    <tableColumn id="23" name="Remark" dataDxfId="85"/>
+    <tableColumn id="3" name="Star" dataDxfId="84"/>
+    <tableColumn id="4" name="Type" dataDxfId="83"/>
+    <tableColumn id="5" name="Attr" dataDxfId="82"/>
+    <tableColumn id="58" name="Quality" dataDxfId="0">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="45"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="44"/>
-    <tableColumn id="24" name="VitP" dataDxfId="43"/>
-    <tableColumn id="25" name="Modify" dataDxfId="42"/>
-    <tableColumn id="9" name="Def" dataDxfId="41"/>
-    <tableColumn id="10" name="Mag" dataDxfId="40"/>
-    <tableColumn id="32" name="Spd" dataDxfId="39"/>
-    <tableColumn id="35" name="Hit" dataDxfId="38"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="37"/>
-    <tableColumn id="34" name="Crt" dataDxfId="36"/>
-    <tableColumn id="33" name="Luk" dataDxfId="35"/>
-    <tableColumn id="7" name="Sum" dataDxfId="34">
+    <tableColumn id="12" name="Cost" dataDxfId="81"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="80"/>
+    <tableColumn id="24" name="VitP" dataDxfId="79"/>
+    <tableColumn id="25" name="Modify" dataDxfId="78"/>
+    <tableColumn id="9" name="Def" dataDxfId="77"/>
+    <tableColumn id="10" name="Mag" dataDxfId="76"/>
+    <tableColumn id="32" name="Spd" dataDxfId="75"/>
+    <tableColumn id="35" name="Hit" dataDxfId="74"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="73"/>
+    <tableColumn id="34" name="Crt" dataDxfId="72"/>
+    <tableColumn id="33" name="Luk" dataDxfId="71"/>
+    <tableColumn id="7" name="Sum" dataDxfId="70">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="33"/>
-    <tableColumn id="14" name="Mov" dataDxfId="32"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="31"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="30"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="29"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="28"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="27"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="26"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
+    <tableColumn id="13" name="Range" dataDxfId="69"/>
+    <tableColumn id="14" name="Mov" dataDxfId="68"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="67"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="66"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="65"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="64"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="63"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="62"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="61">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="60"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="59"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="58"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="57"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="56"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="55">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="11">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="54"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="53"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="52"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="51"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="50"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="49"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="48"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="47">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
-    <tableColumn id="29" name="JobId" dataDxfId="9"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="8"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="7"/>
-    <tableColumn id="21" name="Icon" dataDxfId="6"/>
-    <tableColumn id="17" name="Cover" dataDxfId="5"/>
-    <tableColumn id="18" name="Sound" dataDxfId="4"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="46"/>
+    <tableColumn id="29" name="JobId" dataDxfId="45"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="44"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="43"/>
+    <tableColumn id="21" name="Icon" dataDxfId="42"/>
+    <tableColumn id="17" name="Cover" dataDxfId="41"/>
+    <tableColumn id="18" name="Sound" dataDxfId="40"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="39"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="38"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39600,13 +39648,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA308"/>
+  <dimension ref="A1:BA309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C308" sqref="C308"/>
+      <selection pane="bottomRight" activeCell="U308" sqref="U308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -85308,7 +85356,7 @@
         <v>0</v>
       </c>
       <c r="X292" s="4" t="s">
-        <v>851</v>
+        <v>964</v>
       </c>
       <c r="Y292" s="37">
         <v>55900032</v>
@@ -87602,10 +87650,10 @@
         <v>956</v>
       </c>
       <c r="C307" s="8" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D307" s="8" t="s">
-        <v>958</v>
+        <v>967</v>
       </c>
       <c r="E307" s="8">
         <v>3</v>
@@ -87658,7 +87706,7 @@
         <v>3</v>
       </c>
       <c r="U307" s="8">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="V307" s="8">
         <v>15</v>
@@ -87756,10 +87804,10 @@
         <v>51000305</v>
       </c>
       <c r="B308" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="C308" s="8" t="s">
         <v>960</v>
-      </c>
-      <c r="C308" s="8" t="s">
-        <v>961</v>
       </c>
       <c r="D308" s="8"/>
       <c r="E308" s="8">
@@ -87813,7 +87861,7 @@
         <v>-2</v>
       </c>
       <c r="U308" s="8">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="V308" s="8">
         <v>15</v>
@@ -87906,31 +87954,188 @@
         <v>0.24262300000000001</v>
       </c>
     </row>
+    <row r="309" spans="1:53">
+      <c r="A309">
+        <v>51000306</v>
+      </c>
+      <c r="B309" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="C309" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="D309" s="8" t="s">
+        <v>968</v>
+      </c>
+      <c r="E309" s="8">
+        <v>2</v>
+      </c>
+      <c r="F309" s="8">
+        <v>8</v>
+      </c>
+      <c r="G309" s="8">
+        <v>0</v>
+      </c>
+      <c r="H309" s="21">
+        <f t="shared" ref="H309" si="32">IF(AND(T309&gt;=13,T309&lt;=16),5,IF(AND(T309&gt;=9,T309&lt;=12),4,IF(AND(T309&gt;=5,T309&lt;=8),3,IF(AND(T309&gt;=1,T309&lt;=4),2,IF(AND(T309&gt;=-3,T309&lt;=0),1,IF(AND(T309&gt;=-5,T309&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I309" s="8">
+        <v>2</v>
+      </c>
+      <c r="J309" s="8">
+        <v>0</v>
+      </c>
+      <c r="K309" s="8">
+        <v>0</v>
+      </c>
+      <c r="L309" s="8">
+        <v>-24</v>
+      </c>
+      <c r="M309" s="8">
+        <v>0</v>
+      </c>
+      <c r="N309" s="8">
+        <v>0</v>
+      </c>
+      <c r="O309" s="8">
+        <v>0</v>
+      </c>
+      <c r="P309" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q309" s="8">
+        <v>0</v>
+      </c>
+      <c r="R309" s="8">
+        <v>0</v>
+      </c>
+      <c r="S309" s="8">
+        <v>0</v>
+      </c>
+      <c r="T309" s="21">
+        <f t="shared" ref="T309" si="33">SUM(J309:K309)+SUM(M309:S309)*5+4.4*SUM(AJ309:AP309)+2.5*SUM(AD309:AH309)+IF(ISNUMBER(AC309),AC309,0)+L309</f>
+        <v>1</v>
+      </c>
+      <c r="U309" s="8">
+        <v>10</v>
+      </c>
+      <c r="V309" s="8">
+        <v>15</v>
+      </c>
+      <c r="W309" s="8">
+        <v>0</v>
+      </c>
+      <c r="X309" s="8" t="s">
+        <v>964</v>
+      </c>
+      <c r="Y309" s="18">
+        <v>55900051</v>
+      </c>
+      <c r="Z309" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA309" s="18"/>
+      <c r="AB309" s="18"/>
+      <c r="AC309" s="18">
+        <f>IF(ISBLANK($Y309),0, LOOKUP($Y309,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z309/100)+
+IF(ISBLANK($AA309),0, LOOKUP($AA309,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB309/100)</f>
+        <v>25</v>
+      </c>
+      <c r="AD309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI309" s="8" t="str">
+        <f t="shared" ref="AI309" si="34">CONCATENATE(AD309,";",AE309,";",AF309,";",AG309,";",AH309)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP309" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ309" s="8" t="str">
+        <f t="shared" ref="AQ309" si="35">CONCATENATE(AJ309,";",AK309,";",AL309,";",AM309,";",AN309,";",AO309,";",AP309)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR309" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS309" s="55">
+        <v>11000003</v>
+      </c>
+      <c r="AT309" s="8"/>
+      <c r="AU309" s="8"/>
+      <c r="AV309" s="8">
+        <v>306</v>
+      </c>
+      <c r="AW309" s="8"/>
+      <c r="AX309" s="59" t="s">
+        <v>929</v>
+      </c>
+      <c r="AY309" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ309" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA309" s="8">
+        <v>0.24262300000000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H308">
-    <cfRule type="cellIs" dxfId="146" priority="16" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H309">
+    <cfRule type="cellIs" dxfId="35" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D308">
-    <cfRule type="cellIs" dxfId="141" priority="8" operator="equal">
+  <conditionalFormatting sqref="D4:D309">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T308">
+  <conditionalFormatting sqref="T4:T309">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -87942,29 +88147,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H308">
-    <cfRule type="cellIs" dxfId="140" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H306:H309">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D308">
-    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
+  <conditionalFormatting sqref="D306:D309">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T308">
+  <conditionalFormatting sqref="T306:T309">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -87987,13 +88192,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -88527,7 +88732,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H14" si="0">IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H4:H15" si="0">IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I4" s="8">
@@ -88564,7 +88769,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="12">
-        <f t="shared" ref="T4:T14" si="1">SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</f>
+        <f t="shared" ref="T4:T15" si="1">SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</f>
         <v>-80</v>
       </c>
       <c r="U4" s="8">
@@ -88604,7 +88809,7 @@
         <v>0</v>
       </c>
       <c r="AI4" s="8" t="str">
-        <f t="shared" ref="AI4:AI14" si="2">CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</f>
+        <f t="shared" ref="AI4:AI15" si="2">CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ4" s="18">
@@ -88931,7 +89136,7 @@
         <v>0</v>
       </c>
       <c r="AQ6" s="8" t="str">
-        <f t="shared" ref="AQ6:AQ14" si="4">CONCATENATE(AJ6,";",AK6,";",AL6,";",AM6,";",AN6,";",AO6,";",AP6)</f>
+        <f t="shared" ref="AQ6:AQ15" si="4">CONCATENATE(AJ6,";",AK6,";",AL6,";",AM6,";",AN6,";",AO6,";",AP6)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR6" s="50" t="s">
@@ -89028,7 +89233,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>2</v>
+        <v>963</v>
       </c>
       <c r="Y7" s="47"/>
       <c r="Z7" s="47"/>
@@ -89176,8 +89381,8 @@
       <c r="W8" s="8">
         <v>0</v>
       </c>
-      <c r="X8" s="4" t="s">
-        <v>2</v>
+      <c r="X8" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="Y8" s="47"/>
       <c r="Z8" s="47"/>
@@ -89257,39 +89462,39 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9">
-        <v>51018001</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>696</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>695</v>
+        <v>51013005</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>965</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="8">
-        <v>35</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
+      <c r="F9" s="4">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" ref="H9" si="11">IF(AND(T9&gt;=13,T9&lt;=16),5,IF(AND(T9&gt;=9,T9&lt;=12),4,IF(AND(T9&gt;=5,T9&lt;=8),3,IF(AND(T9&gt;=1,T9&lt;=4),2,IF(AND(T9&gt;=-3,T9&lt;=0),1,IF(AND(T9&gt;=-5,T9&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
       </c>
       <c r="J9" s="4">
-        <v>-35</v>
+        <v>20</v>
       </c>
       <c r="K9" s="4">
-        <v>300</v>
+        <v>-20</v>
       </c>
       <c r="L9" s="4">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="M9" s="8">
         <v>0</v>
@@ -89313,20 +89518,20 @@
         <v>0</v>
       </c>
       <c r="T9" s="12">
-        <f t="shared" si="1"/>
-        <v>265</v>
+        <f t="shared" ref="T9" si="12">SUM(J9:K9)+SUM(M9:S9)*5+4.4*SUM(AJ9:AP9)+2.5*SUM(AD9:AH9)+IF(ISNUMBER(AC9),AC9,0)+L9</f>
+        <v>-3</v>
       </c>
       <c r="U9" s="8">
         <v>10</v>
       </c>
       <c r="V9" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W9" s="8">
         <v>0</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="Y9" s="47"/>
       <c r="Z9" s="47"/>
@@ -89353,7 +89558,7 @@
         <v>0</v>
       </c>
       <c r="AI9" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AI9" si="13">CONCATENATE(AD9,";",AE9,";",AF9,";",AG9,";",AH9)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ9" s="18">
@@ -89378,17 +89583,17 @@
         <v>0</v>
       </c>
       <c r="AQ9" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AQ9" si="14">CONCATENATE(AJ9,";",AK9,";",AL9,";",AM9,";",AN9,";",AO9,";",AP9)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR9" s="50" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="AS9" s="50"/>
       <c r="AT9" s="50"/>
       <c r="AU9" s="50"/>
-      <c r="AV9" s="8">
-        <v>10001</v>
+      <c r="AV9" s="4">
+        <v>10007</v>
       </c>
       <c r="AW9" s="18"/>
       <c r="AX9" s="59" t="s">
@@ -89405,18 +89610,18 @@
       </c>
     </row>
     <row r="10" spans="1:53">
-      <c r="A10" t="s">
-        <v>776</v>
+      <c r="A10">
+        <v>51018001</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>771</v>
+        <v>696</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>773</v>
+        <v>695</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10" s="8">
         <v>35</v>
@@ -89424,7 +89629,7 @@
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -89432,10 +89637,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="4">
-        <v>-40</v>
+        <v>-35</v>
       </c>
       <c r="K10" s="4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
@@ -89463,10 +89668,10 @@
       </c>
       <c r="T10" s="12">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>265</v>
       </c>
       <c r="U10" s="8">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="V10" s="8">
         <v>0</v>
@@ -89475,7 +89680,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="8" t="s">
-        <v>784</v>
+        <v>6</v>
       </c>
       <c r="Y10" s="47"/>
       <c r="Z10" s="47"/>
@@ -89531,13 +89736,13 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR10" s="50" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="AS10" s="50"/>
       <c r="AT10" s="50"/>
       <c r="AU10" s="50"/>
       <c r="AV10" s="8">
-        <v>10002</v>
+        <v>10001</v>
       </c>
       <c r="AW10" s="18"/>
       <c r="AX10" s="59" t="s">
@@ -89555,25 +89760,25 @@
     </row>
     <row r="11" spans="1:53">
       <c r="A11" t="s">
-        <v>799</v>
+        <v>776</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="8">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -89581,10 +89786,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>-45</v>
+        <v>-40</v>
       </c>
       <c r="K11" s="4">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
@@ -89596,7 +89801,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
         <v>0</v>
@@ -89612,10 +89817,10 @@
       </c>
       <c r="T11" s="12">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="U11" s="8">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="V11" s="8">
         <v>0</v>
@@ -89624,7 +89829,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="8" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
       <c r="Y11" s="47"/>
       <c r="Z11" s="47"/>
@@ -89651,7 +89856,7 @@
         <v>0</v>
       </c>
       <c r="AI11" s="19" t="str">
-        <f t="shared" ref="AI11" si="11">CONCATENATE(AD11,";",AE11,";",AF11,";",AG11,";",AH11)</f>
+        <f t="shared" si="2"/>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ11" s="18">
@@ -89686,7 +89891,7 @@
       <c r="AT11" s="50"/>
       <c r="AU11" s="50"/>
       <c r="AV11" s="8">
-        <v>10003</v>
+        <v>10002</v>
       </c>
       <c r="AW11" s="18"/>
       <c r="AX11" s="59" t="s">
@@ -89703,49 +89908,49 @@
       </c>
     </row>
     <row r="12" spans="1:53">
-      <c r="A12">
-        <v>51019298</v>
+      <c r="A12" t="s">
+        <v>799</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>880</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>630</v>
+        <v>772</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>774</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="31">
+      <c r="E12" s="8">
+        <v>3</v>
+      </c>
+      <c r="F12" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="31">
-        <v>8</v>
-      </c>
-      <c r="G12" s="31">
-        <v>0</v>
-      </c>
-      <c r="H12" s="31">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="31">
+        <v>6</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>-45</v>
+      </c>
+      <c r="K12" s="4">
+        <v>120</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
         <v>2</v>
-      </c>
-      <c r="J12" s="31">
-        <v>10</v>
-      </c>
-      <c r="K12" s="31">
-        <v>-10</v>
-      </c>
-      <c r="L12" s="31">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="8">
-        <v>0</v>
       </c>
       <c r="P12" s="8">
         <v>0</v>
@@ -89761,19 +89966,19 @@
       </c>
       <c r="T12" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="U12" s="8">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="V12" s="8">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W12" s="8">
         <v>0</v>
       </c>
       <c r="X12" s="8" t="s">
-        <v>6</v>
+        <v>777</v>
       </c>
       <c r="Y12" s="47"/>
       <c r="Z12" s="47"/>
@@ -89800,7 +90005,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AI12" si="15">CONCATENATE(AD12,";",AE12,";",AF12,";",AG12,";",AH12)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ12" s="18">
@@ -89829,13 +90034,13 @@
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR12" s="50" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="AS12" s="50"/>
       <c r="AT12" s="50"/>
       <c r="AU12" s="50"/>
-      <c r="AV12" s="31">
-        <v>280</v>
+      <c r="AV12" s="8">
+        <v>10003</v>
       </c>
       <c r="AW12" s="18"/>
       <c r="AX12" s="59" t="s">
@@ -89847,16 +90052,16 @@
       <c r="AZ12" s="32">
         <v>0</v>
       </c>
-      <c r="BA12" s="33">
+      <c r="BA12" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:53">
       <c r="A13">
-        <v>51019299</v>
+        <v>51019298</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>630</v>
@@ -89871,19 +90076,19 @@
       <c r="G13" s="31">
         <v>0</v>
       </c>
-      <c r="H13" s="31">
-        <f t="shared" ref="H13" si="12">IF(AND(T13&gt;=13,T13&lt;=16),5,IF(AND(T13&gt;=9,T13&lt;=12),4,IF(AND(T13&gt;=5,T13&lt;=8),3,IF(AND(T13&gt;=1,T13&lt;=4),2,IF(AND(T13&gt;=-3,T13&lt;=0),1,IF(AND(T13&gt;=-5,T13&lt;=-4),0,6))))))</f>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I13" s="31">
         <v>2</v>
       </c>
       <c r="J13" s="31">
+        <v>10</v>
+      </c>
+      <c r="K13" s="31">
         <v>-10</v>
       </c>
-      <c r="K13" s="31">
-        <v>10</v>
-      </c>
       <c r="L13" s="31">
         <v>0</v>
       </c>
@@ -89909,7 +90114,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="12">
-        <f t="shared" ref="T13" si="13">SUM(J13:K13)+SUM(M13:S13)*5+4.4*SUM(AJ13:AP13)+2.5*SUM(AD13:AH13)+IF(ISNUMBER(AC13),AC13,0)+L13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U13" s="8">
@@ -89949,7 +90154,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="19" t="str">
-        <f t="shared" ref="AI13" si="14">CONCATENATE(AD13,";",AE13,";",AF13,";",AG13,";",AH13)</f>
+        <f t="shared" si="2"/>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ13" s="18">
@@ -89974,7 +90179,7 @@
         <v>0</v>
       </c>
       <c r="AQ13" s="8" t="str">
-        <f t="shared" ref="AQ13" si="15">CONCATENATE(AJ13,";",AK13,";",AL13,";",AM13,";",AN13,";",AO13,";",AP13)</f>
+        <f t="shared" si="4"/>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR13" s="50" t="s">
@@ -89984,7 +90189,7 @@
       <c r="AT13" s="50"/>
       <c r="AU13" s="50"/>
       <c r="AV13" s="31">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AW13" s="18"/>
       <c r="AX13" s="59" t="s">
@@ -90001,39 +90206,39 @@
       </c>
     </row>
     <row r="14" spans="1:53">
-      <c r="A14" t="s">
-        <v>775</v>
+      <c r="A14">
+        <v>51019299</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>691</v>
+        <v>881</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>630</v>
       </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="8">
+      <c r="E14" s="31">
+        <v>2</v>
+      </c>
+      <c r="F14" s="31">
+        <v>8</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" ref="H14" si="16">IF(AND(T14&gt;=13,T14&lt;=16),5,IF(AND(T14&gt;=9,T14&lt;=12),4,IF(AND(T14&gt;=5,T14&lt;=8),3,IF(AND(T14&gt;=1,T14&lt;=4),2,IF(AND(T14&gt;=-3,T14&lt;=0),1,IF(AND(T14&gt;=-5,T14&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
-      <c r="F14" s="8">
-        <v>35</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>-35</v>
-      </c>
-      <c r="K14" s="4">
-        <v>300</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="I14" s="31">
+        <v>2</v>
+      </c>
+      <c r="J14" s="31">
+        <v>-10</v>
+      </c>
+      <c r="K14" s="31">
+        <v>10</v>
+      </c>
+      <c r="L14" s="31">
         <v>0</v>
       </c>
       <c r="M14" s="8">
@@ -90058,14 +90263,14 @@
         <v>0</v>
       </c>
       <c r="T14" s="12">
-        <f t="shared" si="1"/>
-        <v>265</v>
+        <f t="shared" ref="T14" si="17">SUM(J14:K14)+SUM(M14:S14)*5+4.4*SUM(AJ14:AP14)+2.5*SUM(AD14:AH14)+IF(ISNUMBER(AC14),AC14,0)+L14</f>
+        <v>0</v>
       </c>
       <c r="U14" s="8">
         <v>10</v>
       </c>
       <c r="V14" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="W14" s="8">
         <v>0</v>
@@ -90098,7 +90303,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AI14" si="18">CONCATENATE(AD14,";",AE14,";",AF14,";",AG14,";",AH14)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ14" s="18">
@@ -90123,7 +90328,7 @@
         <v>0</v>
       </c>
       <c r="AQ14" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AQ14" si="19">CONCATENATE(AJ14,";",AK14,";",AL14,";",AM14,";",AN14,";",AO14,";",AP14)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR14" s="50" t="s">
@@ -90132,8 +90337,8 @@
       <c r="AS14" s="50"/>
       <c r="AT14" s="50"/>
       <c r="AU14" s="50"/>
-      <c r="AV14" s="8">
-        <v>291</v>
+      <c r="AV14" s="31">
+        <v>278</v>
       </c>
       <c r="AW14" s="18"/>
       <c r="AX14" s="59" t="s">
@@ -90145,50 +90350,199 @@
       <c r="AZ14" s="32">
         <v>0</v>
       </c>
-      <c r="BA14" s="32">
+      <c r="BA14" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53">
+      <c r="A15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>35</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-35</v>
+      </c>
+      <c r="K15" s="4">
+        <v>300</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>0</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0</v>
+      </c>
+      <c r="S15" s="8">
+        <v>0</v>
+      </c>
+      <c r="T15" s="12">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="U15" s="8">
+        <v>10</v>
+      </c>
+      <c r="V15" s="8">
+        <v>10</v>
+      </c>
+      <c r="W15" s="8">
+        <v>0</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="18">
+        <f>IF(ISBLANK($Y15),0, LOOKUP($Y15,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z15/100)+
+IF(ISBLANK($AA15),0, LOOKUP($AA15,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB15/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR15" s="50" t="s">
+        <v>782</v>
+      </c>
+      <c r="AS15" s="50"/>
+      <c r="AT15" s="50"/>
+      <c r="AU15" s="50"/>
+      <c r="AV15" s="8">
+        <v>291</v>
+      </c>
+      <c r="AW15" s="18"/>
+      <c r="AX15" s="59" t="s">
+        <v>929</v>
+      </c>
+      <c r="AY15" s="21">
+        <v>1</v>
+      </c>
+      <c r="AZ15" s="32">
+        <v>0</v>
+      </c>
+      <c r="BA15" s="32">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="K4 J6:K9 K12 K14">
-    <cfRule type="cellIs" dxfId="78" priority="35" operator="between">
+  <conditionalFormatting sqref="K4 K13 K15 J6:K8 J10:K10">
+    <cfRule type="cellIs" dxfId="23" priority="37" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="77" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="36" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="76" priority="32" operator="between">
+  <conditionalFormatting sqref="J15">
+    <cfRule type="cellIs" dxfId="21" priority="34" operator="between">
+      <formula>-30</formula>
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="20" priority="33" operator="between">
+      <formula>-30</formula>
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="75" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="74" priority="27" operator="between">
-      <formula>-30</formula>
-      <formula>30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="73" priority="26" operator="between">
-      <formula>-30</formula>
-      <formula>30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T11">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="T12">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -90199,20 +90553,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="72" priority="24" operator="between">
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="17" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="71" priority="23" operator="between">
+  <conditionalFormatting sqref="J11">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T10">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="T11">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -90223,25 +90577,25 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H15">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -90253,36 +90607,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="64" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -90293,8 +90647,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T6:T9 T12 T14">
-    <cfRule type="colorScale" priority="174">
+  <conditionalFormatting sqref="T6:T8 T13 T15 T10">
+    <cfRule type="colorScale" priority="176">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -90305,20 +90659,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="between">
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="between">
+  <conditionalFormatting sqref="J14">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T13">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="T14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+      <formula>-30</formula>
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
#58 new cards for warrior
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="975">
   <si>
     <t>arrow</t>
   </si>
@@ -3980,6 +3980,18 @@
   </si>
   <si>
     <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>库卡隆精英</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korkron Elite</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5068,7 +5080,97 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="148">
+  <dxfs count="160">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -8335,11 +8437,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-588426352"/>
-        <c:axId val="-588423632"/>
+        <c:axId val="270815408"/>
+        <c:axId val="270815968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-588426352"/>
+        <c:axId val="270815408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8382,7 +8484,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588423632"/>
+        <c:crossAx val="270815968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8390,7 +8492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-588423632"/>
+        <c:axId val="270815968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8441,7 +8543,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588426352"/>
+        <c:crossAx val="270815408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8811,11 +8913,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-588435600"/>
-        <c:axId val="-588422544"/>
+        <c:axId val="270818208"/>
+        <c:axId val="270818768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-588435600"/>
+        <c:axId val="270818208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8858,7 +8960,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588422544"/>
+        <c:crossAx val="270818768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8866,7 +8968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-588422544"/>
+        <c:axId val="270818768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8917,7 +9019,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588435600"/>
+        <c:crossAx val="270818208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11449,6 +11551,7 @@
           <cell r="A160">
             <v>55900028</v>
           </cell>
+          <cell r="X160"/>
         </row>
         <row r="161">
           <cell r="A161">
@@ -39204,159 +39307,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA310" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
-  <autoFilter ref="A3:BA310"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA311" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+  <autoFilter ref="A3:BA311"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="132"/>
-    <tableColumn id="2" name="Name" dataDxfId="131"/>
-    <tableColumn id="22" name="Ename" dataDxfId="130"/>
-    <tableColumn id="23" name="Remark" dataDxfId="129"/>
-    <tableColumn id="3" name="Star" dataDxfId="128"/>
-    <tableColumn id="4" name="Type" dataDxfId="127"/>
-    <tableColumn id="5" name="Attr" dataDxfId="126"/>
-    <tableColumn id="58" name="Quality" dataDxfId="125">
+    <tableColumn id="1" name="Id" dataDxfId="144"/>
+    <tableColumn id="2" name="Name" dataDxfId="143"/>
+    <tableColumn id="22" name="Ename" dataDxfId="142"/>
+    <tableColumn id="23" name="Remark" dataDxfId="141"/>
+    <tableColumn id="3" name="Star" dataDxfId="140"/>
+    <tableColumn id="4" name="Type" dataDxfId="139"/>
+    <tableColumn id="5" name="Attr" dataDxfId="138"/>
+    <tableColumn id="58" name="Quality" dataDxfId="137">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="124"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="123"/>
-    <tableColumn id="24" name="VitP" dataDxfId="122"/>
-    <tableColumn id="25" name="Modify" dataDxfId="121"/>
-    <tableColumn id="9" name="Def" dataDxfId="120"/>
-    <tableColumn id="10" name="Mag" dataDxfId="119"/>
-    <tableColumn id="32" name="Spd" dataDxfId="118"/>
-    <tableColumn id="35" name="Hit" dataDxfId="117"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="116"/>
-    <tableColumn id="34" name="Crt" dataDxfId="115"/>
-    <tableColumn id="33" name="Luk" dataDxfId="114"/>
-    <tableColumn id="7" name="Sum" dataDxfId="113">
+    <tableColumn id="12" name="Cost" dataDxfId="136"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="135"/>
+    <tableColumn id="24" name="VitP" dataDxfId="134"/>
+    <tableColumn id="25" name="Modify" dataDxfId="133"/>
+    <tableColumn id="9" name="Def" dataDxfId="132"/>
+    <tableColumn id="10" name="Mag" dataDxfId="131"/>
+    <tableColumn id="32" name="Spd" dataDxfId="130"/>
+    <tableColumn id="35" name="Hit" dataDxfId="129"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="128"/>
+    <tableColumn id="34" name="Crt" dataDxfId="127"/>
+    <tableColumn id="33" name="Luk" dataDxfId="126"/>
+    <tableColumn id="7" name="Sum" dataDxfId="125">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="112"/>
-    <tableColumn id="14" name="Mov" dataDxfId="111"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="110"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="109"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="108"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="107"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="106"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="105"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="104">
+    <tableColumn id="13" name="Range" dataDxfId="124"/>
+    <tableColumn id="14" name="Mov" dataDxfId="123"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="122"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="121"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="120"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="119"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="118"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="117"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="116">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="103"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="102"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="101"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="100"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="99"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="98">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="115"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="114"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="113"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="112"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="111"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="110">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="97"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="96"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="95"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="94"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="93"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="92"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="91"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="90">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="109"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="108"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="107"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="106"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="105"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="104"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="103"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="102">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="89"/>
-    <tableColumn id="29" name="JobId" dataDxfId="88"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="87"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="86"/>
-    <tableColumn id="21" name="Icon" dataDxfId="85"/>
-    <tableColumn id="17" name="Cover" dataDxfId="84"/>
-    <tableColumn id="18" name="Sound" dataDxfId="83"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="82"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="81"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="80"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="101"/>
+    <tableColumn id="29" name="JobId" dataDxfId="100"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="99"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="98"/>
+    <tableColumn id="21" name="Icon" dataDxfId="97"/>
+    <tableColumn id="17" name="Cover" dataDxfId="96"/>
+    <tableColumn id="18" name="Sound" dataDxfId="95"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="94"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="93"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="A3:BA15"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" name="Name" dataDxfId="52"/>
-    <tableColumn id="22" name="Ename" dataDxfId="51"/>
-    <tableColumn id="23" name="Remark" dataDxfId="50"/>
-    <tableColumn id="3" name="Star" dataDxfId="49"/>
-    <tableColumn id="4" name="Type" dataDxfId="48"/>
-    <tableColumn id="5" name="Attr" dataDxfId="47"/>
-    <tableColumn id="58" name="Quality" dataDxfId="46">
+    <tableColumn id="1" name="Id" dataDxfId="65"/>
+    <tableColumn id="2" name="Name" dataDxfId="64"/>
+    <tableColumn id="22" name="Ename" dataDxfId="63"/>
+    <tableColumn id="23" name="Remark" dataDxfId="62"/>
+    <tableColumn id="3" name="Star" dataDxfId="61"/>
+    <tableColumn id="4" name="Type" dataDxfId="60"/>
+    <tableColumn id="5" name="Attr" dataDxfId="59"/>
+    <tableColumn id="58" name="Quality" dataDxfId="58">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="45"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="44"/>
-    <tableColumn id="24" name="VitP" dataDxfId="43"/>
-    <tableColumn id="25" name="Modify" dataDxfId="42"/>
-    <tableColumn id="9" name="Def" dataDxfId="41"/>
-    <tableColumn id="10" name="Mag" dataDxfId="40"/>
-    <tableColumn id="32" name="Spd" dataDxfId="39"/>
-    <tableColumn id="35" name="Hit" dataDxfId="38"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="37"/>
-    <tableColumn id="34" name="Crt" dataDxfId="36"/>
-    <tableColumn id="33" name="Luk" dataDxfId="35"/>
-    <tableColumn id="7" name="Sum" dataDxfId="34">
+    <tableColumn id="12" name="Cost" dataDxfId="57"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="56"/>
+    <tableColumn id="24" name="VitP" dataDxfId="55"/>
+    <tableColumn id="25" name="Modify" dataDxfId="54"/>
+    <tableColumn id="9" name="Def" dataDxfId="53"/>
+    <tableColumn id="10" name="Mag" dataDxfId="52"/>
+    <tableColumn id="32" name="Spd" dataDxfId="51"/>
+    <tableColumn id="35" name="Hit" dataDxfId="50"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="49"/>
+    <tableColumn id="34" name="Crt" dataDxfId="48"/>
+    <tableColumn id="33" name="Luk" dataDxfId="47"/>
+    <tableColumn id="7" name="Sum" dataDxfId="46">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="33"/>
-    <tableColumn id="14" name="Mov" dataDxfId="32"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="31"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="30"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="29"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="28"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="27"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="26"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
+    <tableColumn id="13" name="Range" dataDxfId="45"/>
+    <tableColumn id="14" name="Mov" dataDxfId="44"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="43"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="42"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="41"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="40"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="39"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="38"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="37">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="36"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="35"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="34"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="33"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="32"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="31">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="11">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="30"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="29"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="28"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="27"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="26"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="25"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="24"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="23">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
-    <tableColumn id="29" name="JobId" dataDxfId="9"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="8"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="7"/>
-    <tableColumn id="21" name="Icon" dataDxfId="6"/>
-    <tableColumn id="17" name="Cover" dataDxfId="5"/>
-    <tableColumn id="18" name="Sound" dataDxfId="4"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="22"/>
+    <tableColumn id="29" name="JobId" dataDxfId="21"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="20"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="19"/>
+    <tableColumn id="21" name="Icon" dataDxfId="18"/>
+    <tableColumn id="17" name="Cover" dataDxfId="17"/>
+    <tableColumn id="18" name="Sound" dataDxfId="16"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="15"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="14"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39660,47 +39763,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA310"/>
+  <dimension ref="A1:BA311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C292" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C300" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K305" sqref="K305"/>
+      <selection pane="bottomRight" activeCell="J311" sqref="J311"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="8.875" customWidth="1"/>
-    <col min="26" max="26" width="5.5" customWidth="1"/>
-    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.875" customWidth="1"/>
-    <col min="30" max="34" width="4.625" customWidth="1"/>
-    <col min="35" max="35" width="10.125" customWidth="1"/>
-    <col min="36" max="41" width="3.75" customWidth="1"/>
-    <col min="42" max="42" width="4.375" customWidth="1"/>
-    <col min="43" max="43" width="15.75" customWidth="1"/>
-    <col min="44" max="44" width="6.375" customWidth="1"/>
-    <col min="45" max="45" width="10.5" customWidth="1"/>
-    <col min="46" max="47" width="9.5" customWidth="1"/>
-    <col min="48" max="48" width="4.625" customWidth="1"/>
-    <col min="49" max="49" width="5.75" customWidth="1"/>
-    <col min="50" max="50" width="11.5" customWidth="1"/>
-    <col min="51" max="51" width="4.625" customWidth="1"/>
-    <col min="52" max="53" width="4.125" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" customWidth="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.88671875" customWidth="1"/>
+    <col min="30" max="34" width="4.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" customWidth="1"/>
+    <col min="36" max="41" width="3.77734375" customWidth="1"/>
+    <col min="42" max="42" width="4.33203125" customWidth="1"/>
+    <col min="43" max="43" width="15.77734375" customWidth="1"/>
+    <col min="44" max="44" width="6.33203125" customWidth="1"/>
+    <col min="45" max="45" width="10.44140625" customWidth="1"/>
+    <col min="46" max="47" width="9.44140625" customWidth="1"/>
+    <col min="48" max="48" width="4.6640625" customWidth="1"/>
+    <col min="49" max="49" width="5.77734375" customWidth="1"/>
+    <col min="50" max="50" width="11.44140625" customWidth="1"/>
+    <col min="51" max="51" width="4.6640625" customWidth="1"/>
+    <col min="52" max="53" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="69">
+    <row r="1" spans="1:53" ht="73.2">
       <c r="A1" s="13" t="s">
         <v>299</v>
       </c>
@@ -67830,7 +67933,9 @@
       <c r="AR180" s="50" t="s">
         <v>781</v>
       </c>
-      <c r="AS180" s="54"/>
+      <c r="AS180" s="54">
+        <v>11000004</v>
+      </c>
       <c r="AT180" s="4">
         <v>22011163</v>
       </c>
@@ -87024,7 +87129,7 @@
         <v>0</v>
       </c>
       <c r="AZ302" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA302" s="52">
         <v>0.75409839999999995</v>
@@ -87181,7 +87286,7 @@
         <v>0</v>
       </c>
       <c r="AZ303" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA303" s="52">
         <v>0.75409839999999995</v>
@@ -87336,7 +87441,7 @@
         <v>0</v>
       </c>
       <c r="AZ304" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA304" s="52">
         <v>0.75409839999999995</v>
@@ -87495,7 +87600,7 @@
         <v>0</v>
       </c>
       <c r="AZ305" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA305" s="52">
         <v>0.75409839999999995</v>
@@ -87650,8 +87755,8 @@
       <c r="AZ306" s="8">
         <v>1</v>
       </c>
-      <c r="BA306" s="8">
-        <v>0.24262300000000001</v>
+      <c r="BA306" s="52">
+        <v>0.75409839999999995</v>
       </c>
     </row>
     <row r="307" spans="1:53">
@@ -87807,8 +87912,8 @@
       <c r="AZ307" s="8">
         <v>1</v>
       </c>
-      <c r="BA307" s="8">
-        <v>0.24262300000000001</v>
+      <c r="BA307" s="52">
+        <v>0.75409839999999995</v>
       </c>
     </row>
     <row r="308" spans="1:53">
@@ -87962,8 +88067,8 @@
       <c r="AZ308" s="8">
         <v>1</v>
       </c>
-      <c r="BA308" s="8">
-        <v>0.24262300000000001</v>
+      <c r="BA308" s="52">
+        <v>0.75409839999999995</v>
       </c>
     </row>
     <row r="309" spans="1:53">
@@ -88119,8 +88224,8 @@
       <c r="AZ309" s="8">
         <v>1</v>
       </c>
-      <c r="BA309" s="8">
-        <v>0.24262300000000001</v>
+      <c r="BA309" s="52">
+        <v>0.75409839999999995</v>
       </c>
     </row>
     <row r="310" spans="1:53">
@@ -88280,35 +88385,190 @@
       <c r="AZ310" s="8">
         <v>1</v>
       </c>
-      <c r="BA310" s="8">
-        <v>0.24262300000000001</v>
+      <c r="BA310" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
+    <row r="311" spans="1:53">
+      <c r="A311">
+        <v>51000308</v>
+      </c>
+      <c r="B311" s="8" t="s">
+        <v>972</v>
+      </c>
+      <c r="C311" s="8" t="s">
+        <v>973</v>
+      </c>
+      <c r="D311" s="8"/>
+      <c r="E311" s="8">
+        <v>3</v>
+      </c>
+      <c r="F311" s="8">
+        <v>9</v>
+      </c>
+      <c r="G311" s="8">
+        <v>0</v>
+      </c>
+      <c r="H311" s="21">
+        <f t="shared" ref="H311" si="40">IF(AND(T311&gt;=13,T311&lt;=16),5,IF(AND(T311&gt;=9,T311&lt;=12),4,IF(AND(T311&gt;=5,T311&lt;=8),3,IF(AND(T311&gt;=1,T311&lt;=4),2,IF(AND(T311&gt;=-3,T311&lt;=0),1,IF(AND(T311&gt;=-5,T311&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I311" s="8">
+        <v>3</v>
+      </c>
+      <c r="J311" s="8">
+        <v>5</v>
+      </c>
+      <c r="K311" s="8">
+        <v>-10</v>
+      </c>
+      <c r="L311" s="8">
+        <v>-31</v>
+      </c>
+      <c r="M311" s="8">
+        <v>0</v>
+      </c>
+      <c r="N311" s="8">
+        <v>0</v>
+      </c>
+      <c r="O311" s="8">
+        <v>0</v>
+      </c>
+      <c r="P311" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q311" s="8">
+        <v>0</v>
+      </c>
+      <c r="R311" s="8">
+        <v>0</v>
+      </c>
+      <c r="S311" s="8">
+        <v>0</v>
+      </c>
+      <c r="T311" s="21">
+        <f t="shared" ref="T311" si="41">SUM(J311:K311)+SUM(M311:S311)*5+4.4*SUM(AJ311:AP311)+2.5*SUM(AD311:AH311)+IF(ISNUMBER(AC311),AC311,0)+L311</f>
+        <v>-1</v>
+      </c>
+      <c r="U311" s="8">
+        <v>10</v>
+      </c>
+      <c r="V311" s="8">
+        <v>15</v>
+      </c>
+      <c r="W311" s="8">
+        <v>0</v>
+      </c>
+      <c r="X311" s="8" t="s">
+        <v>974</v>
+      </c>
+      <c r="Y311" s="18">
+        <v>55100005</v>
+      </c>
+      <c r="Z311" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA311" s="18"/>
+      <c r="AB311" s="18"/>
+      <c r="AC311" s="18">
+        <f>IF(ISBLANK($Y311),0, LOOKUP($Y311,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z311/100)+
+IF(ISBLANK($AA311),0, LOOKUP($AA311,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB311/100)</f>
+        <v>35</v>
+      </c>
+      <c r="AD311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI311" s="8" t="str">
+        <f t="shared" ref="AI311" si="42">CONCATENATE(AD311,";",AE311,";",AF311,";",AG311,";",AH311)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP311" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ311" s="8" t="str">
+        <f t="shared" ref="AQ311" si="43">CONCATENATE(AJ311,";",AK311,";",AL311,";",AM311,";",AN311,";",AO311,";",AP311)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR311" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS311" s="55">
+        <v>11000001</v>
+      </c>
+      <c r="AT311" s="8"/>
+      <c r="AU311" s="8"/>
+      <c r="AV311" s="8">
+        <v>308</v>
+      </c>
+      <c r="AW311" s="8"/>
+      <c r="AX311" s="59" t="s">
+        <v>932</v>
+      </c>
+      <c r="AY311" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ311" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA311" s="52">
+        <v>0.75409839999999995</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H310">
-    <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H311">
+    <cfRule type="cellIs" dxfId="159" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D310">
-    <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
+  <conditionalFormatting sqref="D4:D311">
+    <cfRule type="cellIs" dxfId="154" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T310">
+  <conditionalFormatting sqref="T4:T311">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -88320,29 +88580,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H310">
-    <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H306:H311">
+    <cfRule type="cellIs" dxfId="153" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D310">
-    <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
+  <conditionalFormatting sqref="D306:D311">
+    <cfRule type="cellIs" dxfId="148" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T310">
+  <conditionalFormatting sqref="T306:T311">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -88374,34 +88634,34 @@
       <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="5" max="9" width="3.375" customWidth="1"/>
-    <col min="10" max="11" width="4.125" customWidth="1"/>
-    <col min="12" max="19" width="4.75" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
-    <col min="21" max="23" width="4.75" customWidth="1"/>
-    <col min="24" max="24" width="6.5" customWidth="1"/>
-    <col min="25" max="25" width="8.875" customWidth="1"/>
-    <col min="26" max="26" width="5.5" customWidth="1"/>
-    <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="4.625" customWidth="1"/>
-    <col min="35" max="35" width="10.125" customWidth="1"/>
-    <col min="36" max="42" width="3.75" customWidth="1"/>
-    <col min="43" max="43" width="14.75" customWidth="1"/>
-    <col min="44" max="44" width="5.875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="5" max="9" width="3.33203125" customWidth="1"/>
+    <col min="10" max="11" width="4.109375" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" customWidth="1"/>
+    <col min="20" max="20" width="4.109375" customWidth="1"/>
+    <col min="21" max="23" width="4.77734375" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="5.44140625" customWidth="1"/>
+    <col min="28" max="28" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="4.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" customWidth="1"/>
+    <col min="36" max="42" width="3.77734375" customWidth="1"/>
+    <col min="43" max="43" width="14.77734375" customWidth="1"/>
+    <col min="44" max="44" width="5.88671875" customWidth="1"/>
     <col min="45" max="47" width="9" customWidth="1"/>
-    <col min="48" max="48" width="7.375" customWidth="1"/>
-    <col min="49" max="49" width="5.75" customWidth="1"/>
-    <col min="50" max="50" width="11.125" customWidth="1"/>
-    <col min="51" max="51" width="4.625" customWidth="1"/>
-    <col min="52" max="53" width="4.125" customWidth="1"/>
+    <col min="48" max="48" width="7.33203125" customWidth="1"/>
+    <col min="49" max="49" width="5.77734375" customWidth="1"/>
+    <col min="50" max="50" width="11.109375" customWidth="1"/>
+    <col min="51" max="51" width="4.6640625" customWidth="1"/>
+    <col min="52" max="53" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="69">
+    <row r="1" spans="1:53" ht="73.2">
       <c r="A1" s="13" t="s">
         <v>299</v>
       </c>
@@ -90679,37 +90939,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 K13 K15 J6:K8 J10:K10">
-    <cfRule type="cellIs" dxfId="79" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="37" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="78" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="36" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="77" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="76" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="33" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="75" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="87" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="74" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -90727,13 +90987,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="73" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="72" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="84" priority="25" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -90751,19 +91011,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="71" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="83" priority="15" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -90780,31 +91040,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="66" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="65" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="64" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -90833,13 +91093,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="3" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -90857,7 +91117,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -90894,10 +91154,10 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.25" customWidth="1"/>
-    <col min="2" max="9" width="7.125" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -91353,10 +91613,10 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -91446,10 +91706,10 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
close #80 finish addskill function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="977">
   <si>
     <t>arrow</t>
   </si>
@@ -3992,6 +3992,14 @@
   </si>
   <si>
     <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>格斗技师</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sparring Partner</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5080,7 +5088,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="160">
+  <dxfs count="161">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -8437,11 +8452,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="270815408"/>
-        <c:axId val="270815968"/>
+        <c:axId val="667340544"/>
+        <c:axId val="311999760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="270815408"/>
+        <c:axId val="667340544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8484,7 +8499,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270815968"/>
+        <c:crossAx val="311999760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8492,7 +8507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270815968"/>
+        <c:axId val="311999760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8543,7 +8558,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270815408"/>
+        <c:crossAx val="667340544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8913,11 +8928,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="270818208"/>
-        <c:axId val="270818768"/>
+        <c:axId val="312002000"/>
+        <c:axId val="312002560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="270818208"/>
+        <c:axId val="312002000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8960,7 +8975,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270818768"/>
+        <c:crossAx val="312002560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8968,7 +8983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="270818768"/>
+        <c:axId val="312002560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9019,7 +9034,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="270818208"/>
+        <c:crossAx val="312002000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11551,7 +11566,6 @@
           <cell r="A160">
             <v>55900028</v>
           </cell>
-          <cell r="X160"/>
         </row>
         <row r="161">
           <cell r="A161">
@@ -11739,15 +11753,15 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990001</v>
+            <v>55900052</v>
           </cell>
           <cell r="X184">
-            <v>15</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X185">
             <v>15</v>
@@ -11755,7 +11769,7 @@
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11763,7 +11777,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11771,7 +11785,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11779,7 +11793,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11787,7 +11801,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11795,7 +11809,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11803,7 +11817,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11811,7 +11825,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11819,7 +11833,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -11827,7 +11841,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X195">
             <v>15</v>
@@ -11835,41 +11849,49 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X196">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X197">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X198">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X199">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
+            <v>55990104</v>
+          </cell>
+          <cell r="X200">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="A201">
             <v>55990105</v>
           </cell>
-          <cell r="X200">
+          <cell r="X201">
             <v>150</v>
           </cell>
         </row>
@@ -39307,159 +39329,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA311" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
-  <autoFilter ref="A3:BA311"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA312" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147" tableBorderDxfId="146">
+  <autoFilter ref="A3:BA312"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="144"/>
-    <tableColumn id="2" name="Name" dataDxfId="143"/>
-    <tableColumn id="22" name="Ename" dataDxfId="142"/>
-    <tableColumn id="23" name="Remark" dataDxfId="141"/>
-    <tableColumn id="3" name="Star" dataDxfId="140"/>
-    <tableColumn id="4" name="Type" dataDxfId="139"/>
-    <tableColumn id="5" name="Attr" dataDxfId="138"/>
-    <tableColumn id="58" name="Quality" dataDxfId="137">
+    <tableColumn id="1" name="Id" dataDxfId="145"/>
+    <tableColumn id="2" name="Name" dataDxfId="144"/>
+    <tableColumn id="22" name="Ename" dataDxfId="143"/>
+    <tableColumn id="23" name="Remark" dataDxfId="142"/>
+    <tableColumn id="3" name="Star" dataDxfId="141"/>
+    <tableColumn id="4" name="Type" dataDxfId="140"/>
+    <tableColumn id="5" name="Attr" dataDxfId="139"/>
+    <tableColumn id="58" name="Quality" dataDxfId="138">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="136"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="135"/>
-    <tableColumn id="24" name="VitP" dataDxfId="134"/>
-    <tableColumn id="25" name="Modify" dataDxfId="133"/>
-    <tableColumn id="9" name="Def" dataDxfId="132"/>
-    <tableColumn id="10" name="Mag" dataDxfId="131"/>
-    <tableColumn id="32" name="Spd" dataDxfId="130"/>
-    <tableColumn id="35" name="Hit" dataDxfId="129"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="128"/>
-    <tableColumn id="34" name="Crt" dataDxfId="127"/>
-    <tableColumn id="33" name="Luk" dataDxfId="126"/>
-    <tableColumn id="7" name="Sum" dataDxfId="125">
+    <tableColumn id="12" name="Cost" dataDxfId="137"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="136"/>
+    <tableColumn id="24" name="VitP" dataDxfId="135"/>
+    <tableColumn id="25" name="Modify" dataDxfId="134"/>
+    <tableColumn id="9" name="Def" dataDxfId="133"/>
+    <tableColumn id="10" name="Mag" dataDxfId="132"/>
+    <tableColumn id="32" name="Spd" dataDxfId="131"/>
+    <tableColumn id="35" name="Hit" dataDxfId="130"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="129"/>
+    <tableColumn id="34" name="Crt" dataDxfId="128"/>
+    <tableColumn id="33" name="Luk" dataDxfId="127"/>
+    <tableColumn id="7" name="Sum" dataDxfId="126">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="124"/>
-    <tableColumn id="14" name="Mov" dataDxfId="123"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="122"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="121"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="120"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="119"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="118"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="117"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="116">
+    <tableColumn id="13" name="Range" dataDxfId="125"/>
+    <tableColumn id="14" name="Mov" dataDxfId="124"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="123"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="122"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="121"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="120"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="119"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="118"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="117">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="115"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="114"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="113"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="112"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="111"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="110">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="116"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="115"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="114"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="113"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="112"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="111">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="109"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="108"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="107"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="106"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="105"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="104"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="103"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="102">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="110"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="109"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="108"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="107"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="106"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="105"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="104"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="103">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="101"/>
-    <tableColumn id="29" name="JobId" dataDxfId="100"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="99"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="98"/>
-    <tableColumn id="21" name="Icon" dataDxfId="97"/>
-    <tableColumn id="17" name="Cover" dataDxfId="96"/>
-    <tableColumn id="18" name="Sound" dataDxfId="95"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="94"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="93"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="92"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="102"/>
+    <tableColumn id="29" name="JobId" dataDxfId="101"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="100"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="99"/>
+    <tableColumn id="21" name="Icon" dataDxfId="98"/>
+    <tableColumn id="17" name="Cover" dataDxfId="97"/>
+    <tableColumn id="18" name="Sound" dataDxfId="96"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="95"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="94"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="A3:BA15"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="65"/>
-    <tableColumn id="2" name="Name" dataDxfId="64"/>
-    <tableColumn id="22" name="Ename" dataDxfId="63"/>
-    <tableColumn id="23" name="Remark" dataDxfId="62"/>
-    <tableColumn id="3" name="Star" dataDxfId="61"/>
-    <tableColumn id="4" name="Type" dataDxfId="60"/>
-    <tableColumn id="5" name="Attr" dataDxfId="59"/>
-    <tableColumn id="58" name="Quality" dataDxfId="58">
+    <tableColumn id="1" name="Id" dataDxfId="66"/>
+    <tableColumn id="2" name="Name" dataDxfId="65"/>
+    <tableColumn id="22" name="Ename" dataDxfId="64"/>
+    <tableColumn id="23" name="Remark" dataDxfId="63"/>
+    <tableColumn id="3" name="Star" dataDxfId="62"/>
+    <tableColumn id="4" name="Type" dataDxfId="61"/>
+    <tableColumn id="5" name="Attr" dataDxfId="60"/>
+    <tableColumn id="58" name="Quality" dataDxfId="59">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="57"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="56"/>
-    <tableColumn id="24" name="VitP" dataDxfId="55"/>
-    <tableColumn id="25" name="Modify" dataDxfId="54"/>
-    <tableColumn id="9" name="Def" dataDxfId="53"/>
-    <tableColumn id="10" name="Mag" dataDxfId="52"/>
-    <tableColumn id="32" name="Spd" dataDxfId="51"/>
-    <tableColumn id="35" name="Hit" dataDxfId="50"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="49"/>
-    <tableColumn id="34" name="Crt" dataDxfId="48"/>
-    <tableColumn id="33" name="Luk" dataDxfId="47"/>
-    <tableColumn id="7" name="Sum" dataDxfId="46">
+    <tableColumn id="12" name="Cost" dataDxfId="58"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="57"/>
+    <tableColumn id="24" name="VitP" dataDxfId="56"/>
+    <tableColumn id="25" name="Modify" dataDxfId="55"/>
+    <tableColumn id="9" name="Def" dataDxfId="54"/>
+    <tableColumn id="10" name="Mag" dataDxfId="53"/>
+    <tableColumn id="32" name="Spd" dataDxfId="52"/>
+    <tableColumn id="35" name="Hit" dataDxfId="51"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="50"/>
+    <tableColumn id="34" name="Crt" dataDxfId="49"/>
+    <tableColumn id="33" name="Luk" dataDxfId="48"/>
+    <tableColumn id="7" name="Sum" dataDxfId="47">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="45"/>
-    <tableColumn id="14" name="Mov" dataDxfId="44"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="43"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="42"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="41"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="40"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="39"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="38"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="37">
+    <tableColumn id="13" name="Range" dataDxfId="46"/>
+    <tableColumn id="14" name="Mov" dataDxfId="45"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="44"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="43"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="42"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="41"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="40"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="39"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="38">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="36"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="35"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="34"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="33"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="32"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="31">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="37"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="36"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="35"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="34"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="33"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="32">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="30"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="29"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="28"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="27"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="26"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="25"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="24"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="23">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="31"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="30"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="29"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="28"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="27"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="26"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="25"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="24">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="22"/>
-    <tableColumn id="29" name="JobId" dataDxfId="21"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="20"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="19"/>
-    <tableColumn id="21" name="Icon" dataDxfId="18"/>
-    <tableColumn id="17" name="Cover" dataDxfId="17"/>
-    <tableColumn id="18" name="Sound" dataDxfId="16"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="15"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="14"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="13"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="23"/>
+    <tableColumn id="29" name="JobId" dataDxfId="22"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="21"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="20"/>
+    <tableColumn id="21" name="Icon" dataDxfId="19"/>
+    <tableColumn id="17" name="Cover" dataDxfId="18"/>
+    <tableColumn id="18" name="Sound" dataDxfId="17"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="16"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="15"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39763,13 +39785,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA311"/>
+  <dimension ref="A1:BA312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C300" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J311" sqref="J311"/>
+      <selection pane="bottomRight" activeCell="E311" sqref="E311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -88544,31 +88566,192 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="312" spans="1:53">
+      <c r="A312">
+        <v>51000309</v>
+      </c>
+      <c r="B312" s="8" t="s">
+        <v>975</v>
+      </c>
+      <c r="C312" s="8" t="s">
+        <v>976</v>
+      </c>
+      <c r="D312" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="E312" s="8">
+        <v>2</v>
+      </c>
+      <c r="F312" s="8">
+        <v>9</v>
+      </c>
+      <c r="G312" s="8">
+        <v>0</v>
+      </c>
+      <c r="H312" s="21">
+        <f t="shared" ref="H312" si="44">IF(AND(T312&gt;=13,T312&lt;=16),5,IF(AND(T312&gt;=9,T312&lt;=12),4,IF(AND(T312&gt;=5,T312&lt;=8),3,IF(AND(T312&gt;=1,T312&lt;=4),2,IF(AND(T312&gt;=-3,T312&lt;=0),1,IF(AND(T312&gt;=-5,T312&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I312" s="8">
+        <v>2</v>
+      </c>
+      <c r="J312" s="8">
+        <v>15</v>
+      </c>
+      <c r="K312" s="8">
+        <v>-10</v>
+      </c>
+      <c r="L312" s="8">
+        <v>-33</v>
+      </c>
+      <c r="M312" s="8">
+        <v>2</v>
+      </c>
+      <c r="N312" s="8">
+        <v>0</v>
+      </c>
+      <c r="O312" s="8">
+        <v>0</v>
+      </c>
+      <c r="P312" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q312" s="8">
+        <v>0</v>
+      </c>
+      <c r="R312" s="8">
+        <v>0</v>
+      </c>
+      <c r="S312" s="8">
+        <v>0</v>
+      </c>
+      <c r="T312" s="21">
+        <f t="shared" ref="T312" si="45">SUM(J312:K312)+SUM(M312:S312)*5+4.4*SUM(AJ312:AP312)+2.5*SUM(AD312:AH312)+IF(ISNUMBER(AC312),AC312,0)+L312</f>
+        <v>2</v>
+      </c>
+      <c r="U312" s="8">
+        <v>10</v>
+      </c>
+      <c r="V312" s="8">
+        <v>15</v>
+      </c>
+      <c r="W312" s="8">
+        <v>0</v>
+      </c>
+      <c r="X312" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="Y312" s="18">
+        <v>55100008</v>
+      </c>
+      <c r="Z312" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA312" s="18">
+        <v>55900052</v>
+      </c>
+      <c r="AB312" s="18">
+        <v>100</v>
+      </c>
+      <c r="AC312" s="18">
+        <f>IF(ISBLANK($Y312),0, LOOKUP($Y312,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z312/100)+
+IF(ISBLANK($AA312),0, LOOKUP($AA312,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB312/100)</f>
+        <v>20</v>
+      </c>
+      <c r="AD312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI312" s="8" t="str">
+        <f t="shared" ref="AI312" si="46">CONCATENATE(AD312,";",AE312,";",AF312,";",AG312,";",AH312)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP312" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ312" s="8" t="str">
+        <f t="shared" ref="AQ312" si="47">CONCATENATE(AJ312,";",AK312,";",AL312,";",AM312,";",AN312,";",AO312,";",AP312)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR312" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS312" s="55">
+        <v>11000002</v>
+      </c>
+      <c r="AT312" s="8"/>
+      <c r="AU312" s="8"/>
+      <c r="AV312" s="8">
+        <v>309</v>
+      </c>
+      <c r="AW312" s="8"/>
+      <c r="AX312" s="59" t="s">
+        <v>929</v>
+      </c>
+      <c r="AY312" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ312" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA312" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H311">
-    <cfRule type="cellIs" dxfId="159" priority="16" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H312">
+    <cfRule type="cellIs" dxfId="160" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D311">
-    <cfRule type="cellIs" dxfId="154" priority="8" operator="equal">
+  <conditionalFormatting sqref="D4:D312">
+    <cfRule type="cellIs" dxfId="155" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T311">
+  <conditionalFormatting sqref="T4:T312">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -88580,29 +88763,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H311">
-    <cfRule type="cellIs" dxfId="153" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H306:H312">
+    <cfRule type="cellIs" dxfId="154" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D311">
-    <cfRule type="cellIs" dxfId="148" priority="1" operator="equal">
+  <conditionalFormatting sqref="D306:D312">
+    <cfRule type="cellIs" dxfId="149" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T311">
+  <conditionalFormatting sqref="T306:T312">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -90939,37 +91122,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 K13 K15 J6:K8 J10:K10">
-    <cfRule type="cellIs" dxfId="91" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="92" priority="37" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="90" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="36" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="89" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="88" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="33" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="87" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="86" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="87" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -90987,13 +91170,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="85" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="84" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="25" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -91011,19 +91194,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="83" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="84" priority="15" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -91040,31 +91223,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="78" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="77" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="76" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -91093,13 +91276,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="71" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="70" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="3" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -91117,7 +91300,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
add some new cards #58
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="979">
   <si>
     <t>arrow</t>
   </si>
@@ -4000,6 +4000,13 @@
   </si>
   <si>
     <t>Sparring Partner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Armorsmith</t>
+  </si>
+  <si>
+    <t>铸甲师</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5088,104 +5095,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="161">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="148">
     <dxf>
       <font>
         <b/>
@@ -11761,15 +11671,15 @@
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990001</v>
+            <v>55900053</v>
           </cell>
           <cell r="X185">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X186">
             <v>15</v>
@@ -11777,7 +11687,7 @@
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11785,7 +11695,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11793,7 +11703,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11801,7 +11711,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11809,7 +11719,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11817,7 +11727,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11825,7 +11735,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11833,7 +11743,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -11841,7 +11751,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X195">
             <v>15</v>
@@ -11849,7 +11759,7 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X196">
             <v>15</v>
@@ -11857,46 +11767,54 @@
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X197">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X198">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X199">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X200">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
+            <v>55990104</v>
+          </cell>
+          <cell r="X201">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="A202">
             <v>55990105</v>
           </cell>
-          <cell r="X201">
+          <cell r="X202">
             <v>150</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39329,159 +39247,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA312" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147" tableBorderDxfId="146">
-  <autoFilter ref="A3:BA312"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA313" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+  <autoFilter ref="A3:BA313"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="145"/>
-    <tableColumn id="2" name="Name" dataDxfId="144"/>
-    <tableColumn id="22" name="Ename" dataDxfId="143"/>
-    <tableColumn id="23" name="Remark" dataDxfId="142"/>
-    <tableColumn id="3" name="Star" dataDxfId="141"/>
-    <tableColumn id="4" name="Type" dataDxfId="140"/>
-    <tableColumn id="5" name="Attr" dataDxfId="139"/>
-    <tableColumn id="58" name="Quality" dataDxfId="138">
+    <tableColumn id="1" name="Id" dataDxfId="132"/>
+    <tableColumn id="2" name="Name" dataDxfId="131"/>
+    <tableColumn id="22" name="Ename" dataDxfId="130"/>
+    <tableColumn id="23" name="Remark" dataDxfId="129"/>
+    <tableColumn id="3" name="Star" dataDxfId="128"/>
+    <tableColumn id="4" name="Type" dataDxfId="127"/>
+    <tableColumn id="5" name="Attr" dataDxfId="126"/>
+    <tableColumn id="58" name="Quality" dataDxfId="125">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="137"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="136"/>
-    <tableColumn id="24" name="VitP" dataDxfId="135"/>
-    <tableColumn id="25" name="Modify" dataDxfId="134"/>
-    <tableColumn id="9" name="Def" dataDxfId="133"/>
-    <tableColumn id="10" name="Mag" dataDxfId="132"/>
-    <tableColumn id="32" name="Spd" dataDxfId="131"/>
-    <tableColumn id="35" name="Hit" dataDxfId="130"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="129"/>
-    <tableColumn id="34" name="Crt" dataDxfId="128"/>
-    <tableColumn id="33" name="Luk" dataDxfId="127"/>
-    <tableColumn id="7" name="Sum" dataDxfId="126">
+    <tableColumn id="12" name="Cost" dataDxfId="124"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="123"/>
+    <tableColumn id="24" name="VitP" dataDxfId="122"/>
+    <tableColumn id="25" name="Modify" dataDxfId="121"/>
+    <tableColumn id="9" name="Def" dataDxfId="120"/>
+    <tableColumn id="10" name="Mag" dataDxfId="119"/>
+    <tableColumn id="32" name="Spd" dataDxfId="118"/>
+    <tableColumn id="35" name="Hit" dataDxfId="117"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="116"/>
+    <tableColumn id="34" name="Crt" dataDxfId="115"/>
+    <tableColumn id="33" name="Luk" dataDxfId="114"/>
+    <tableColumn id="7" name="Sum" dataDxfId="113">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="125"/>
-    <tableColumn id="14" name="Mov" dataDxfId="124"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="123"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="122"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="121"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="120"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="119"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="118"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="117">
+    <tableColumn id="13" name="Range" dataDxfId="112"/>
+    <tableColumn id="14" name="Mov" dataDxfId="111"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="110"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="109"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="108"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="107"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="106"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="105"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="104">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="116"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="115"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="114"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="113"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="112"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="111">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="103"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="102"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="101"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="100"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="99"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="98">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="110"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="109"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="108"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="107"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="106"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="105"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="104"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="103">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="97"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="96"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="95"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="94"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="93"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="92"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="91"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="90">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="102"/>
-    <tableColumn id="29" name="JobId" dataDxfId="101"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="100"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="99"/>
-    <tableColumn id="21" name="Icon" dataDxfId="98"/>
-    <tableColumn id="17" name="Cover" dataDxfId="97"/>
-    <tableColumn id="18" name="Sound" dataDxfId="96"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="95"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="94"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="93"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="89"/>
+    <tableColumn id="29" name="JobId" dataDxfId="88"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="87"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="86"/>
+    <tableColumn id="21" name="Icon" dataDxfId="85"/>
+    <tableColumn id="17" name="Cover" dataDxfId="84"/>
+    <tableColumn id="18" name="Sound" dataDxfId="83"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="82"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="81"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A3:BA15"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="66"/>
-    <tableColumn id="2" name="Name" dataDxfId="65"/>
-    <tableColumn id="22" name="Ename" dataDxfId="64"/>
-    <tableColumn id="23" name="Remark" dataDxfId="63"/>
-    <tableColumn id="3" name="Star" dataDxfId="62"/>
-    <tableColumn id="4" name="Type" dataDxfId="61"/>
-    <tableColumn id="5" name="Attr" dataDxfId="60"/>
-    <tableColumn id="58" name="Quality" dataDxfId="59">
+    <tableColumn id="1" name="Id" dataDxfId="53"/>
+    <tableColumn id="2" name="Name" dataDxfId="52"/>
+    <tableColumn id="22" name="Ename" dataDxfId="51"/>
+    <tableColumn id="23" name="Remark" dataDxfId="50"/>
+    <tableColumn id="3" name="Star" dataDxfId="49"/>
+    <tableColumn id="4" name="Type" dataDxfId="48"/>
+    <tableColumn id="5" name="Attr" dataDxfId="47"/>
+    <tableColumn id="58" name="Quality" dataDxfId="46">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="58"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="57"/>
-    <tableColumn id="24" name="VitP" dataDxfId="56"/>
-    <tableColumn id="25" name="Modify" dataDxfId="55"/>
-    <tableColumn id="9" name="Def" dataDxfId="54"/>
-    <tableColumn id="10" name="Mag" dataDxfId="53"/>
-    <tableColumn id="32" name="Spd" dataDxfId="52"/>
-    <tableColumn id="35" name="Hit" dataDxfId="51"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="50"/>
-    <tableColumn id="34" name="Crt" dataDxfId="49"/>
-    <tableColumn id="33" name="Luk" dataDxfId="48"/>
-    <tableColumn id="7" name="Sum" dataDxfId="47">
+    <tableColumn id="12" name="Cost" dataDxfId="45"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="44"/>
+    <tableColumn id="24" name="VitP" dataDxfId="43"/>
+    <tableColumn id="25" name="Modify" dataDxfId="42"/>
+    <tableColumn id="9" name="Def" dataDxfId="41"/>
+    <tableColumn id="10" name="Mag" dataDxfId="40"/>
+    <tableColumn id="32" name="Spd" dataDxfId="39"/>
+    <tableColumn id="35" name="Hit" dataDxfId="38"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="37"/>
+    <tableColumn id="34" name="Crt" dataDxfId="36"/>
+    <tableColumn id="33" name="Luk" dataDxfId="35"/>
+    <tableColumn id="7" name="Sum" dataDxfId="34">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="46"/>
-    <tableColumn id="14" name="Mov" dataDxfId="45"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="44"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="43"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="42"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="41"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="40"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="39"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="38">
+    <tableColumn id="13" name="Range" dataDxfId="33"/>
+    <tableColumn id="14" name="Mov" dataDxfId="32"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="31"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="30"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="29"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="28"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="27"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="26"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="37"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="36"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="35"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="34"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="33"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="32">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="31"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="30"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="29"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="28"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="27"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="26"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="25"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="24">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="11">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="23"/>
-    <tableColumn id="29" name="JobId" dataDxfId="22"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="21"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="20"/>
-    <tableColumn id="21" name="Icon" dataDxfId="19"/>
-    <tableColumn id="17" name="Cover" dataDxfId="18"/>
-    <tableColumn id="18" name="Sound" dataDxfId="17"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="16"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="15"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="14"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
+    <tableColumn id="29" name="JobId" dataDxfId="9"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="8"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="7"/>
+    <tableColumn id="21" name="Icon" dataDxfId="6"/>
+    <tableColumn id="17" name="Cover" dataDxfId="5"/>
+    <tableColumn id="18" name="Sound" dataDxfId="4"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -39785,13 +39703,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA312"/>
+  <dimension ref="A1:BA313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C300" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E311" sqref="E311"/>
+      <selection pane="bottomRight" activeCell="L313" sqref="L313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -88583,7 +88501,7 @@
         <v>2</v>
       </c>
       <c r="F312" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G312" s="8">
         <v>0</v>
@@ -88727,31 +88645,188 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="313" spans="1:53">
+      <c r="A313">
+        <v>51000310</v>
+      </c>
+      <c r="B313" s="8" t="s">
+        <v>978</v>
+      </c>
+      <c r="C313" s="8" t="s">
+        <v>977</v>
+      </c>
+      <c r="D313" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="E313" s="8">
+        <v>2</v>
+      </c>
+      <c r="F313" s="8">
+        <v>8</v>
+      </c>
+      <c r="G313" s="8">
+        <v>0</v>
+      </c>
+      <c r="H313" s="21">
+        <f t="shared" ref="H313" si="48">IF(AND(T313&gt;=13,T313&lt;=16),5,IF(AND(T313&gt;=9,T313&lt;=12),4,IF(AND(T313&gt;=5,T313&lt;=8),3,IF(AND(T313&gt;=1,T313&lt;=4),2,IF(AND(T313&gt;=-3,T313&lt;=0),1,IF(AND(T313&gt;=-5,T313&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I313" s="8">
+        <v>2</v>
+      </c>
+      <c r="J313" s="8">
+        <v>-30</v>
+      </c>
+      <c r="K313" s="8">
+        <v>10</v>
+      </c>
+      <c r="L313" s="8">
+        <v>-7</v>
+      </c>
+      <c r="M313" s="8">
+        <v>0</v>
+      </c>
+      <c r="N313" s="8">
+        <v>0</v>
+      </c>
+      <c r="O313" s="8">
+        <v>0</v>
+      </c>
+      <c r="P313" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q313" s="8">
+        <v>0</v>
+      </c>
+      <c r="R313" s="8">
+        <v>0</v>
+      </c>
+      <c r="S313" s="8">
+        <v>0</v>
+      </c>
+      <c r="T313" s="21">
+        <f t="shared" ref="T313" si="49">SUM(J313:K313)+SUM(M313:S313)*5+4.4*SUM(AJ313:AP313)+2.5*SUM(AD313:AH313)+IF(ISNUMBER(AC313),AC313,0)+L313</f>
+        <v>3</v>
+      </c>
+      <c r="U313" s="8">
+        <v>10</v>
+      </c>
+      <c r="V313" s="8">
+        <v>10</v>
+      </c>
+      <c r="W313" s="8">
+        <v>0</v>
+      </c>
+      <c r="X313" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y313" s="18">
+        <v>55900053</v>
+      </c>
+      <c r="Z313" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA313" s="18"/>
+      <c r="AB313" s="18"/>
+      <c r="AC313" s="18">
+        <f>IF(ISBLANK($Y313),0, LOOKUP($Y313,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z313/100)+
+IF(ISBLANK($AA313),0, LOOKUP($AA313,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB313/100)</f>
+        <v>30</v>
+      </c>
+      <c r="AD313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI313" s="8" t="str">
+        <f t="shared" ref="AI313" si="50">CONCATENATE(AD313,";",AE313,";",AF313,";",AG313,";",AH313)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP313" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ313" s="8" t="str">
+        <f t="shared" ref="AQ313" si="51">CONCATENATE(AJ313,";",AK313,";",AL313,";",AM313,";",AN313,";",AO313,";",AP313)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR313" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS313" s="55">
+        <v>11000002</v>
+      </c>
+      <c r="AT313" s="8"/>
+      <c r="AU313" s="8"/>
+      <c r="AV313" s="8">
+        <v>310</v>
+      </c>
+      <c r="AW313" s="8"/>
+      <c r="AX313" s="59" t="s">
+        <v>929</v>
+      </c>
+      <c r="AY313" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ313" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA313" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H312">
-    <cfRule type="cellIs" dxfId="160" priority="16" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H4:H313">
+    <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D312">
-    <cfRule type="cellIs" dxfId="155" priority="8" operator="equal">
+  <conditionalFormatting sqref="D4:D313">
+    <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T312">
+  <conditionalFormatting sqref="T4:T313">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -88763,29 +88838,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H312">
-    <cfRule type="cellIs" dxfId="154" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H306:H313">
+    <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D312">
-    <cfRule type="cellIs" dxfId="149" priority="1" operator="equal">
+  <conditionalFormatting sqref="D306:D313">
+    <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T312">
+  <conditionalFormatting sqref="T306:T313">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -91122,37 +91197,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 K13 K15 J6:K8 J10:K10">
-    <cfRule type="cellIs" dxfId="92" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="37" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="91" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="90" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="89" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="33" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="88" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="87" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -91170,13 +91245,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="86" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="85" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="25" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -91194,19 +91269,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="84" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="15" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -91223,31 +91298,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="79" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="78" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="77" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -91276,13 +91351,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="71" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -91300,7 +91375,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="cellIs" dxfId="70" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
new cards for hunter
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="986">
   <si>
     <t>arrow</t>
   </si>
@@ -4019,6 +4019,21 @@
   </si>
   <si>
     <t>yellowsplash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SFX_CS2_125_Wolf</t>
+  </si>
+  <si>
+    <t>加兹瑞拉</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gahz'rilla</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成长</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8374,11 +8389,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="291593488"/>
-        <c:axId val="291226816"/>
+        <c:axId val="450572784"/>
+        <c:axId val="450573344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="291593488"/>
+        <c:axId val="450572784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8421,7 +8436,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291226816"/>
+        <c:crossAx val="450573344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8429,7 +8444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291226816"/>
+        <c:axId val="450573344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8480,7 +8495,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291593488"/>
+        <c:crossAx val="450572784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8850,11 +8865,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="291229056"/>
-        <c:axId val="291229616"/>
+        <c:axId val="452318368"/>
+        <c:axId val="452318928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="291229056"/>
+        <c:axId val="452318368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8897,7 +8912,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291229616"/>
+        <c:crossAx val="452318928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8905,7 +8920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291229616"/>
+        <c:axId val="452318928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8956,7 +8971,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291229056"/>
+        <c:crossAx val="452318368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11270,199 +11285,199 @@
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900001</v>
+            <v>55700006</v>
           </cell>
           <cell r="X133">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900002</v>
+            <v>55900001</v>
           </cell>
           <cell r="X134">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900003</v>
+            <v>55900002</v>
           </cell>
           <cell r="X135">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900004</v>
+            <v>55900003</v>
           </cell>
           <cell r="X136">
-            <v>-30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900005</v>
+            <v>55900004</v>
           </cell>
           <cell r="X137">
-            <v>20</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900006</v>
+            <v>55900005</v>
           </cell>
           <cell r="X138">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900007</v>
+            <v>55900006</v>
           </cell>
           <cell r="X139">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900008</v>
+            <v>55900007</v>
           </cell>
           <cell r="X140">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900009</v>
+            <v>55900008</v>
           </cell>
           <cell r="X141">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900010</v>
+            <v>55900009</v>
           </cell>
           <cell r="X142">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900011</v>
+            <v>55900010</v>
           </cell>
           <cell r="X143">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900012</v>
+            <v>55900011</v>
           </cell>
           <cell r="X144">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900013</v>
+            <v>55900012</v>
           </cell>
           <cell r="X145">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900014</v>
+            <v>55900013</v>
           </cell>
           <cell r="X146">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900015</v>
+            <v>55900014</v>
           </cell>
           <cell r="X147">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900016</v>
+            <v>55900015</v>
           </cell>
           <cell r="X148">
-            <v>45</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900017</v>
+            <v>55900016</v>
           </cell>
           <cell r="X149">
-            <v>10</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900018</v>
+            <v>55900017</v>
           </cell>
           <cell r="X150">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900019</v>
+            <v>55900018</v>
           </cell>
           <cell r="X151">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900020</v>
+            <v>55900019</v>
           </cell>
           <cell r="X152">
-            <v>20</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900021</v>
+            <v>55900020</v>
           </cell>
           <cell r="X153">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900022</v>
+            <v>55900021</v>
           </cell>
           <cell r="X154">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900023</v>
+            <v>55900022</v>
           </cell>
           <cell r="X155">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900024</v>
+            <v>55900023</v>
           </cell>
           <cell r="X156">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900025</v>
+            <v>55900024</v>
           </cell>
           <cell r="X157">
             <v>10</v>
@@ -11470,60 +11485,60 @@
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900026</v>
+            <v>55900025</v>
           </cell>
           <cell r="X158">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900027</v>
+            <v>55900026</v>
           </cell>
           <cell r="X159">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900028</v>
+            <v>55900027</v>
+          </cell>
+          <cell r="X160">
+            <v>35</v>
           </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900029</v>
-          </cell>
-          <cell r="X161">
-            <v>15</v>
+            <v>55900028</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900030</v>
+            <v>55900029</v>
           </cell>
           <cell r="X162">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900031</v>
+            <v>55900030</v>
           </cell>
           <cell r="X163">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900032</v>
+            <v>55900031</v>
           </cell>
           <cell r="X164">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900033</v>
+            <v>55900032</v>
           </cell>
           <cell r="X165">
             <v>20</v>
@@ -11531,15 +11546,15 @@
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900034</v>
+            <v>55900033</v>
           </cell>
           <cell r="X166">
-            <v>14</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900035</v>
+            <v>55900034</v>
           </cell>
           <cell r="X167">
             <v>14</v>
@@ -11547,31 +11562,31 @@
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900036</v>
+            <v>55900035</v>
           </cell>
           <cell r="X168">
-            <v>50</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900037</v>
+            <v>55900036</v>
           </cell>
           <cell r="X169">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900038</v>
+            <v>55900037</v>
           </cell>
           <cell r="X170">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900039</v>
+            <v>55900038</v>
           </cell>
           <cell r="X171">
             <v>40</v>
@@ -11579,55 +11594,55 @@
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900040</v>
+            <v>55900039</v>
           </cell>
           <cell r="X172">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900041</v>
+            <v>55900040</v>
           </cell>
           <cell r="X173">
-            <v>0</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900042</v>
+            <v>55900041</v>
           </cell>
           <cell r="X174">
-            <v>25</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900043</v>
+            <v>55900042</v>
           </cell>
           <cell r="X175">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900044</v>
+            <v>55900043</v>
           </cell>
           <cell r="X176">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900045</v>
+            <v>55900044</v>
           </cell>
           <cell r="X177">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900046</v>
+            <v>55900045</v>
           </cell>
           <cell r="X178">
             <v>25</v>
@@ -11635,71 +11650,71 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900047</v>
+            <v>55900046</v>
           </cell>
           <cell r="X179">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900048</v>
+            <v>55900047</v>
           </cell>
           <cell r="X180">
-            <v>70</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55900049</v>
+            <v>55900048</v>
           </cell>
           <cell r="X181">
-            <v>25</v>
+            <v>70</v>
           </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55900050</v>
+            <v>55900049</v>
           </cell>
           <cell r="X182">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55900051</v>
+            <v>55900050</v>
           </cell>
           <cell r="X183">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55900052</v>
+            <v>55900051</v>
           </cell>
           <cell r="X184">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55900053</v>
+            <v>55900052</v>
           </cell>
           <cell r="X185">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55900054</v>
+            <v>55900053</v>
           </cell>
           <cell r="X186">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990001</v>
+            <v>55900054</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -11707,7 +11722,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11715,7 +11730,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11723,7 +11738,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11731,7 +11746,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11739,7 +11754,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11747,7 +11762,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11755,7 +11770,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -11763,7 +11778,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X195">
             <v>15</v>
@@ -11771,7 +11786,7 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X196">
             <v>15</v>
@@ -11779,7 +11794,7 @@
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X197">
             <v>15</v>
@@ -11787,7 +11802,7 @@
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X198">
             <v>15</v>
@@ -11795,41 +11810,49 @@
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X199">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X200">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X201">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X202">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
+            <v>55990104</v>
+          </cell>
+          <cell r="X203">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="A204">
             <v>55990105</v>
           </cell>
-          <cell r="X203">
+          <cell r="X204">
             <v>150</v>
           </cell>
         </row>
@@ -39267,8 +39290,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA314" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
-  <autoFilter ref="A3:BA314"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA315" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+  <autoFilter ref="A3:BA315"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
@@ -39723,13 +39746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA314"/>
+  <dimension ref="A1:BA315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="S293" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C293" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AS313" sqref="AS313"/>
+      <selection pane="bottomRight" activeCell="P301" sqref="P301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -88979,9 +89002,166 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="315" spans="1:53">
+      <c r="A315">
+        <v>51000312</v>
+      </c>
+      <c r="B315" s="8" t="s">
+        <v>983</v>
+      </c>
+      <c r="C315" s="8" t="s">
+        <v>984</v>
+      </c>
+      <c r="D315" s="8" t="s">
+        <v>985</v>
+      </c>
+      <c r="E315" s="8">
+        <v>7</v>
+      </c>
+      <c r="F315" s="8">
+        <v>11</v>
+      </c>
+      <c r="G315" s="8">
+        <v>2</v>
+      </c>
+      <c r="H315" s="21">
+        <f t="shared" ref="H315" si="56">IF(AND(T315&gt;=13,T315&lt;=16),5,IF(AND(T315&gt;=9,T315&lt;=12),4,IF(AND(T315&gt;=5,T315&lt;=8),3,IF(AND(T315&gt;=1,T315&lt;=4),2,IF(AND(T315&gt;=-3,T315&lt;=0),1,IF(AND(T315&gt;=-5,T315&lt;=-4),0,6))))))</f>
+        <v>4</v>
+      </c>
+      <c r="I315" s="8">
+        <v>7</v>
+      </c>
+      <c r="J315" s="8">
+        <v>-60</v>
+      </c>
+      <c r="K315" s="8">
+        <v>0</v>
+      </c>
+      <c r="L315" s="8">
+        <v>20</v>
+      </c>
+      <c r="M315" s="8">
+        <v>0</v>
+      </c>
+      <c r="N315" s="8">
+        <v>0</v>
+      </c>
+      <c r="O315" s="8">
+        <v>0</v>
+      </c>
+      <c r="P315" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q315" s="8">
+        <v>0</v>
+      </c>
+      <c r="R315" s="8">
+        <v>0</v>
+      </c>
+      <c r="S315" s="8">
+        <v>0</v>
+      </c>
+      <c r="T315" s="21">
+        <f t="shared" ref="T315" si="57">SUM(J315:K315)+SUM(M315:S315)*5+4.4*SUM(AJ315:AP315)+2.5*SUM(AD315:AH315)+IF(ISNUMBER(AC315),AC315,0)+L315</f>
+        <v>10</v>
+      </c>
+      <c r="U315" s="8">
+        <v>10</v>
+      </c>
+      <c r="V315" s="8">
+        <v>15</v>
+      </c>
+      <c r="W315" s="8">
+        <v>0</v>
+      </c>
+      <c r="X315" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="Y315" s="18">
+        <v>55700006</v>
+      </c>
+      <c r="Z315" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA315" s="18"/>
+      <c r="AB315" s="18"/>
+      <c r="AC315" s="18">
+        <f>IF(ISBLANK($Y315),0, LOOKUP($Y315,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z315/100)+
+IF(ISBLANK($AA315),0, LOOKUP($AA315,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB315/100)</f>
+        <v>50</v>
+      </c>
+      <c r="AD315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI315" s="8" t="str">
+        <f t="shared" ref="AI315" si="58">CONCATENATE(AD315,";",AE315,";",AF315,";",AG315,";",AH315)</f>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP315" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ315" s="8" t="str">
+        <f t="shared" ref="AQ315" si="59">CONCATENATE(AJ315,";",AK315,";",AL315,";",AM315,";",AN315,";",AO315,";",AP315)</f>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR315" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS315" s="55">
+        <v>11000004</v>
+      </c>
+      <c r="AT315" s="8"/>
+      <c r="AU315" s="8"/>
+      <c r="AV315" s="8">
+        <v>312</v>
+      </c>
+      <c r="AW315" s="8"/>
+      <c r="AX315" s="59" t="s">
+        <v>982</v>
+      </c>
+      <c r="AY315" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ315" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA315" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H314">
+  <conditionalFormatting sqref="H4:H315">
     <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -88998,12 +89178,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D314">
+  <conditionalFormatting sqref="D4:D315">
     <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T314">
+  <conditionalFormatting sqref="T4:T315">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -89015,7 +89195,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H314">
+  <conditionalFormatting sqref="H306:H315">
     <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -89032,12 +89212,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D314">
+  <conditionalFormatting sqref="D306:D315">
     <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T314">
+  <conditionalFormatting sqref="T306:T315">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
balance the give card skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -11691,7 +11691,7 @@
             <v>55900048</v>
           </cell>
           <cell r="X181">
-            <v>70</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="182">
@@ -39811,10 +39811,10 @@
   <dimension ref="A1:BA315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C294" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="J303" sqref="J303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -39823,7 +39823,7 @@
     <col min="2" max="2" width="7.25" customWidth="1"/>
     <col min="3" max="3" width="12.875" customWidth="1"/>
     <col min="5" max="9" width="3.375" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.625" customWidth="1"/>
     <col min="11" max="11" width="4.125" customWidth="1"/>
     <col min="12" max="19" width="4.75" customWidth="1"/>
     <col min="20" max="20" width="4.125" customWidth="1"/>
@@ -87206,13 +87206,13 @@
       </c>
       <c r="H303" s="4">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I303" s="4">
         <v>3</v>
       </c>
       <c r="J303" s="4">
-        <v>-35</v>
+        <v>-27</v>
       </c>
       <c r="K303" s="4">
         <v>0</v>
@@ -87243,7 +87243,7 @@
       </c>
       <c r="T303" s="12">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U303" s="4">
         <v>10</v>
@@ -87261,14 +87261,14 @@
         <v>55900048</v>
       </c>
       <c r="Z303" s="18">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="AA303" s="18"/>
       <c r="AB303" s="18"/>
       <c r="AC303" s="18">
         <f>IF(ISBLANK($Y303),0, LOOKUP($Y303,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z303/100)+
 IF(ISBLANK($AA303),0, LOOKUP($AA303,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB303/100)</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AD303" s="18">
         <v>0</v>

</xml_diff>

<commit_message>
add 2 new cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId7"/>
-    <pivotCache cacheId="13" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="988">
   <si>
     <t>arrow</t>
   </si>
@@ -4034,6 +4034,14 @@
   </si>
   <si>
     <t>成长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>娜可露露</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nakoruru</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -11521,7 +11529,6 @@
           <cell r="A161">
             <v>55900028</v>
           </cell>
-          <cell r="X161"/>
         </row>
         <row r="162">
           <cell r="A162">
@@ -11733,7 +11740,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990001</v>
+            <v>55900055</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -11741,7 +11748,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -11749,7 +11756,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -11757,7 +11764,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -11765,7 +11772,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -11773,7 +11780,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -11781,7 +11788,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -11789,7 +11796,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="X195">
             <v>15</v>
@@ -11797,7 +11804,7 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="X196">
             <v>15</v>
@@ -11805,7 +11812,7 @@
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="X197">
             <v>15</v>
@@ -11813,7 +11820,7 @@
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="X198">
             <v>15</v>
@@ -11821,7 +11828,7 @@
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="X199">
             <v>15</v>
@@ -11829,41 +11836,49 @@
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="X200">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="X201">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="X202">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="X203">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="204">
           <cell r="A204">
+            <v>55990104</v>
+          </cell>
+          <cell r="X204">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="A205">
             <v>55990105</v>
           </cell>
-          <cell r="X204">
+          <cell r="X205">
             <v>150</v>
           </cell>
         </row>
@@ -46737,7 +46752,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField dataField="1" showAll="0"/>
@@ -46864,7 +46879,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField dataField="1" showAll="0"/>
@@ -46997,8 +47012,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA315" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
-  <autoFilter ref="A3:BA315"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA316" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+  <autoFilter ref="A3:BA316"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
@@ -47487,13 +47502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA315"/>
+  <dimension ref="A1:BA316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="S285" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G57" sqref="G57"/>
+      <selection pane="bottomRight" activeCell="AS314" sqref="AS314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -95478,8 +95493,8 @@
       <c r="AY306" s="21">
         <v>0</v>
       </c>
-      <c r="AZ306" s="8">
-        <v>1</v>
+      <c r="AZ306" s="19">
+        <v>0</v>
       </c>
       <c r="BA306" s="52">
         <v>0.75409839999999995</v>
@@ -95635,8 +95650,8 @@
       <c r="AY307" s="21">
         <v>0</v>
       </c>
-      <c r="AZ307" s="8">
-        <v>1</v>
+      <c r="AZ307" s="19">
+        <v>0</v>
       </c>
       <c r="BA307" s="52">
         <v>0.75409839999999995</v>
@@ -95790,8 +95805,8 @@
       <c r="AY308" s="21">
         <v>0</v>
       </c>
-      <c r="AZ308" s="8">
-        <v>1</v>
+      <c r="AZ308" s="19">
+        <v>0</v>
       </c>
       <c r="BA308" s="52">
         <v>0.75409839999999995</v>
@@ -96026,8 +96041,8 @@
       <c r="W310" s="8">
         <v>0</v>
       </c>
-      <c r="X310" s="8" t="s">
-        <v>668</v>
+      <c r="X310" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="Y310" s="18">
         <v>55100002</v>
@@ -96768,7 +96783,7 @@
         <v>2</v>
       </c>
       <c r="H315" s="21">
-        <f t="shared" ref="H315" si="56">IF(AND(T315&gt;=13,T315&lt;=16),5,IF(AND(T315&gt;=9,T315&lt;=12),4,IF(AND(T315&gt;=5,T315&lt;=8),3,IF(AND(T315&gt;=1,T315&lt;=4),2,IF(AND(T315&gt;=-3,T315&lt;=0),1,IF(AND(T315&gt;=-5,T315&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H315:H316" si="56">IF(AND(T315&gt;=13,T315&lt;=16),5,IF(AND(T315&gt;=9,T315&lt;=12),4,IF(AND(T315&gt;=5,T315&lt;=8),3,IF(AND(T315&gt;=1,T315&lt;=4),2,IF(AND(T315&gt;=-3,T315&lt;=0),1,IF(AND(T315&gt;=-5,T315&lt;=-4),0,6))))))</f>
         <v>4</v>
       </c>
       <c r="I315" s="8">
@@ -96805,7 +96820,7 @@
         <v>0</v>
       </c>
       <c r="T315" s="21">
-        <f t="shared" ref="T315" si="57">SUM(J315:K315)+SUM(M315:S315)*5+4.4*SUM(AJ315:AP315)+2.5*SUM(AD315:AH315)+IF(ISNUMBER(AC315),AC315,0)+L315</f>
+        <f t="shared" ref="T315:T316" si="57">SUM(J315:K315)+SUM(M315:S315)*5+4.4*SUM(AJ315:AP315)+2.5*SUM(AD315:AH315)+IF(ISNUMBER(AC315),AC315,0)+L315</f>
         <v>10</v>
       </c>
       <c r="U315" s="8">
@@ -96849,7 +96864,7 @@
         <v>0</v>
       </c>
       <c r="AI315" s="8" t="str">
-        <f t="shared" ref="AI315" si="58">CONCATENATE(AD315,";",AE315,";",AF315,";",AG315,";",AH315)</f>
+        <f t="shared" ref="AI315:AI316" si="58">CONCATENATE(AD315,";",AE315,";",AF315,";",AG315,";",AH315)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ315" s="18">
@@ -96874,7 +96889,7 @@
         <v>0</v>
       </c>
       <c r="AQ315" s="8" t="str">
-        <f t="shared" ref="AQ315" si="59">CONCATENATE(AJ315,";",AK315,";",AL315,";",AM315,";",AN315,";",AO315,";",AP315)</f>
+        <f t="shared" ref="AQ315:AQ316" si="59">CONCATENATE(AJ315,";",AK315,";",AL315,";",AM315,";",AN315,";",AO315,";",AP315)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR315" s="51" t="s">
@@ -96902,9 +96917,170 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="316" spans="1:53" x14ac:dyDescent="0.15">
+      <c r="A316">
+        <v>51000313</v>
+      </c>
+      <c r="B316" s="8" t="s">
+        <v>986</v>
+      </c>
+      <c r="C316" s="8" t="s">
+        <v>987</v>
+      </c>
+      <c r="D316" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="E316" s="8">
+        <v>4</v>
+      </c>
+      <c r="F316" s="8">
+        <v>8</v>
+      </c>
+      <c r="G316" s="8">
+        <v>1</v>
+      </c>
+      <c r="H316" s="21">
+        <f t="shared" si="56"/>
+        <v>4</v>
+      </c>
+      <c r="I316" s="8">
+        <v>4</v>
+      </c>
+      <c r="J316" s="8">
+        <v>10</v>
+      </c>
+      <c r="K316" s="8">
+        <v>-20</v>
+      </c>
+      <c r="L316" s="8">
+        <v>-11</v>
+      </c>
+      <c r="M316" s="8">
+        <v>0</v>
+      </c>
+      <c r="N316" s="8">
+        <v>0</v>
+      </c>
+      <c r="O316" s="8">
+        <v>0</v>
+      </c>
+      <c r="P316" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q316" s="8">
+        <v>0</v>
+      </c>
+      <c r="R316" s="8">
+        <v>1</v>
+      </c>
+      <c r="S316" s="8">
+        <v>0</v>
+      </c>
+      <c r="T316" s="21">
+        <f t="shared" si="57"/>
+        <v>9</v>
+      </c>
+      <c r="U316" s="8">
+        <v>10</v>
+      </c>
+      <c r="V316" s="8">
+        <v>20</v>
+      </c>
+      <c r="W316" s="8">
+        <v>0</v>
+      </c>
+      <c r="X316" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y316" s="18">
+        <v>55600015</v>
+      </c>
+      <c r="Z316" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA316" s="18">
+        <v>55900055</v>
+      </c>
+      <c r="AB316" s="18">
+        <v>100</v>
+      </c>
+      <c r="AC316" s="18">
+        <f>IF(ISBLANK($Y316),0, LOOKUP($Y316,[1]Skill!$A:$A,[1]Skill!$X:$X)*$Z316/100)+
+IF(ISBLANK($AA316),0, LOOKUP($AA316,[1]Skill!$A:$A,[1]Skill!$X:$X)*$AB316/100)</f>
+        <v>25</v>
+      </c>
+      <c r="AD316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI316" s="8" t="str">
+        <f t="shared" si="58"/>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP316" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ316" s="8" t="str">
+        <f t="shared" si="59"/>
+        <v>0;0;0;0;0;0;0</v>
+      </c>
+      <c r="AR316" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS316" s="55">
+        <v>11000005</v>
+      </c>
+      <c r="AT316" s="8"/>
+      <c r="AU316" s="8"/>
+      <c r="AV316" s="8">
+        <v>313</v>
+      </c>
+      <c r="AW316" s="8"/>
+      <c r="AX316" s="59" t="s">
+        <v>929</v>
+      </c>
+      <c r="AY316" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ316" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA316" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H315">
+  <conditionalFormatting sqref="H4:H316">
     <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -96921,12 +97097,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D315">
+  <conditionalFormatting sqref="D4:D316">
     <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T315">
+  <conditionalFormatting sqref="T4:T316">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -96938,7 +97114,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H315">
+  <conditionalFormatting sqref="H306:H316">
     <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -96955,12 +97131,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D315">
+  <conditionalFormatting sqref="D306:D316">
     <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T315">
+  <conditionalFormatting sqref="T306:T316">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
lock the tower attr modification
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -23,8 +23,8 @@
   </externalReferences>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId7"/>
-    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -5160,328 +5160,6 @@
   <dxfs count="148">
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -6808,6 +6486,238 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8124,6 +8034,96 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11564,6 +11564,7 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
+          <cell r="Y162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -46819,7 +46820,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField dataField="1" showAll="0"/>
@@ -46946,7 +46947,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField dataField="1" showAll="0"/>
@@ -47079,159 +47080,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA317" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA317" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
   <autoFilter ref="A3:BA317"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="144"/>
-    <tableColumn id="2" name="Name" dataDxfId="143"/>
-    <tableColumn id="22" name="Ename" dataDxfId="142"/>
-    <tableColumn id="23" name="Remark" dataDxfId="141"/>
-    <tableColumn id="3" name="Star" dataDxfId="140"/>
-    <tableColumn id="4" name="Type" dataDxfId="139"/>
-    <tableColumn id="5" name="Attr" dataDxfId="138"/>
-    <tableColumn id="58" name="Quality" dataDxfId="137">
+    <tableColumn id="1" name="Id" dataDxfId="132"/>
+    <tableColumn id="2" name="Name" dataDxfId="131"/>
+    <tableColumn id="22" name="Ename" dataDxfId="130"/>
+    <tableColumn id="23" name="Remark" dataDxfId="129"/>
+    <tableColumn id="3" name="Star" dataDxfId="128"/>
+    <tableColumn id="4" name="Type" dataDxfId="127"/>
+    <tableColumn id="5" name="Attr" dataDxfId="126"/>
+    <tableColumn id="58" name="Quality" dataDxfId="125">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="136"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="135"/>
-    <tableColumn id="24" name="VitP" dataDxfId="134"/>
-    <tableColumn id="25" name="Modify" dataDxfId="133"/>
-    <tableColumn id="9" name="Def" dataDxfId="132"/>
-    <tableColumn id="10" name="Mag" dataDxfId="131"/>
-    <tableColumn id="32" name="Spd" dataDxfId="130"/>
-    <tableColumn id="35" name="Hit" dataDxfId="129"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="128"/>
-    <tableColumn id="34" name="Crt" dataDxfId="127"/>
-    <tableColumn id="33" name="Luk" dataDxfId="126"/>
-    <tableColumn id="7" name="Sum" dataDxfId="125">
+    <tableColumn id="12" name="Cost" dataDxfId="124"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="123"/>
+    <tableColumn id="24" name="VitP" dataDxfId="122"/>
+    <tableColumn id="25" name="Modify" dataDxfId="121"/>
+    <tableColumn id="9" name="Def" dataDxfId="120"/>
+    <tableColumn id="10" name="Mag" dataDxfId="119"/>
+    <tableColumn id="32" name="Spd" dataDxfId="118"/>
+    <tableColumn id="35" name="Hit" dataDxfId="117"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="116"/>
+    <tableColumn id="34" name="Crt" dataDxfId="115"/>
+    <tableColumn id="33" name="Luk" dataDxfId="114"/>
+    <tableColumn id="7" name="Sum" dataDxfId="113">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="124"/>
-    <tableColumn id="14" name="Mov" dataDxfId="123"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="122"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="121"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="120"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="119"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="118"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="117"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="116">
+    <tableColumn id="13" name="Range" dataDxfId="112"/>
+    <tableColumn id="14" name="Mov" dataDxfId="111"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="110"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="109"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="108"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="107"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="106"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="105"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="104">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="115"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="114"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="113"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="112"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="111"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="110">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="103"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="102"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="101"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="100"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="99"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="98">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="109"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="108"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="107"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="106"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="105"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="104"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="103"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="102">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="97"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="96"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="95"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="94"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="93"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="92"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="91"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="90">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="101"/>
-    <tableColumn id="29" name="JobId" dataDxfId="100"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="99"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="98"/>
-    <tableColumn id="21" name="Icon" dataDxfId="97"/>
-    <tableColumn id="17" name="Cover" dataDxfId="96"/>
-    <tableColumn id="18" name="Sound" dataDxfId="95"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="94"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="93"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="92"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="89"/>
+    <tableColumn id="29" name="JobId" dataDxfId="88"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="87"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="86"/>
+    <tableColumn id="21" name="Icon" dataDxfId="85"/>
+    <tableColumn id="17" name="Cover" dataDxfId="84"/>
+    <tableColumn id="18" name="Sound" dataDxfId="83"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="82"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="81"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA16" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA16" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A3:BA16"/>
   <sortState ref="A4:AF312">
     <sortCondition ref="A3:A312"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="88"/>
-    <tableColumn id="2" name="Name" dataDxfId="87"/>
-    <tableColumn id="22" name="Ename" dataDxfId="86"/>
-    <tableColumn id="23" name="Remark" dataDxfId="85"/>
-    <tableColumn id="3" name="Star" dataDxfId="84"/>
-    <tableColumn id="4" name="Type" dataDxfId="83"/>
-    <tableColumn id="5" name="Attr" dataDxfId="82"/>
-    <tableColumn id="58" name="Quality" dataDxfId="81">
+    <tableColumn id="1" name="Id" dataDxfId="53"/>
+    <tableColumn id="2" name="Name" dataDxfId="52"/>
+    <tableColumn id="22" name="Ename" dataDxfId="51"/>
+    <tableColumn id="23" name="Remark" dataDxfId="50"/>
+    <tableColumn id="3" name="Star" dataDxfId="49"/>
+    <tableColumn id="4" name="Type" dataDxfId="48"/>
+    <tableColumn id="5" name="Attr" dataDxfId="47"/>
+    <tableColumn id="58" name="Quality" dataDxfId="46">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="80"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="79"/>
-    <tableColumn id="24" name="VitP" dataDxfId="78"/>
-    <tableColumn id="25" name="Modify" dataDxfId="77"/>
-    <tableColumn id="9" name="Def" dataDxfId="76"/>
-    <tableColumn id="10" name="Mag" dataDxfId="75"/>
-    <tableColumn id="32" name="Spd" dataDxfId="74"/>
-    <tableColumn id="35" name="Hit" dataDxfId="73"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="72"/>
-    <tableColumn id="34" name="Crt" dataDxfId="71"/>
-    <tableColumn id="33" name="Luk" dataDxfId="70"/>
-    <tableColumn id="7" name="Sum" dataDxfId="69">
+    <tableColumn id="12" name="Cost" dataDxfId="45"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="44"/>
+    <tableColumn id="24" name="VitP" dataDxfId="43"/>
+    <tableColumn id="25" name="Modify" dataDxfId="42"/>
+    <tableColumn id="9" name="Def" dataDxfId="41"/>
+    <tableColumn id="10" name="Mag" dataDxfId="40"/>
+    <tableColumn id="32" name="Spd" dataDxfId="39"/>
+    <tableColumn id="35" name="Hit" dataDxfId="38"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="37"/>
+    <tableColumn id="34" name="Crt" dataDxfId="36"/>
+    <tableColumn id="33" name="Luk" dataDxfId="35"/>
+    <tableColumn id="7" name="Sum" dataDxfId="34">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="68"/>
-    <tableColumn id="14" name="Mov" dataDxfId="67"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="66"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="65"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="64"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="63"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="62"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="61"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="60">
+    <tableColumn id="13" name="Range" dataDxfId="33"/>
+    <tableColumn id="14" name="Mov" dataDxfId="32"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="31"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="30"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="29"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="28"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="27"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="26"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="25">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="59"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="58"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="57"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="56"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="55"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="54">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="24"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="23"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="22"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="21"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="20"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="19">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="53"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="52"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="51"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="50"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="49"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="48"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="47"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="46">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="18"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="17"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="16"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="15"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="14"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="13"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="12"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="11">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="45"/>
-    <tableColumn id="29" name="JobId" dataDxfId="44"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="43"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="42"/>
-    <tableColumn id="21" name="Icon" dataDxfId="41"/>
-    <tableColumn id="17" name="Cover" dataDxfId="40"/>
-    <tableColumn id="18" name="Sound" dataDxfId="39"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="38"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="37"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="36"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="10"/>
+    <tableColumn id="29" name="JobId" dataDxfId="9"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="8"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="7"/>
+    <tableColumn id="21" name="Icon" dataDxfId="6"/>
+    <tableColumn id="17" name="Cover" dataDxfId="5"/>
+    <tableColumn id="18" name="Sound" dataDxfId="4"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="3"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="2"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -97303,24 +97304,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H317">
-    <cfRule type="cellIs" dxfId="34" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="30" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D317">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -97337,24 +97338,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H306:H317">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D306:D317">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -97387,7 +97388,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -99260,7 +99261,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="8">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="G13" s="8">
         <v>0</v>
@@ -99844,37 +99845,37 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="K4 K14 K16 J6:K8 J10:K11">
-    <cfRule type="cellIs" dxfId="22" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="37" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="21" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="20" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="34" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="19" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="33" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="18" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="29" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -99892,13 +99893,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="26" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="15" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="25" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -99916,19 +99917,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H16">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="15" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -99945,31 +99946,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -99998,13 +99999,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>
@@ -100022,7 +100023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="between">
       <formula>-30</formula>
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
optimise the card catalog
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -47572,11 +47572,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X44" sqref="X44"/>
+      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -97384,7 +97384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
new monster card the Ascended
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="995">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="998">
   <si>
     <t>arrow</t>
   </si>
@@ -4070,6 +4070,17 @@
   <si>
     <t>卫兵</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>升腾者</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Ascended</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterbolt</t>
   </si>
 </sst>
 </file>
@@ -11564,7 +11575,6 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
-          <cell r="Y162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -11784,7 +11794,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990001</v>
+            <v>55900056</v>
           </cell>
           <cell r="Y190">
             <v>10</v>
@@ -11792,7 +11802,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="Y191">
             <v>10</v>
@@ -11800,7 +11810,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="Y192">
             <v>10</v>
@@ -11808,7 +11818,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="Y193">
             <v>10</v>
@@ -11816,7 +11826,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="Y194">
             <v>10</v>
@@ -11824,7 +11834,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="Y195">
             <v>10</v>
@@ -11832,7 +11842,7 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="Y196">
             <v>10</v>
@@ -11840,7 +11850,7 @@
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="Y197">
             <v>10</v>
@@ -11848,7 +11858,7 @@
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="Y198">
             <v>10</v>
@@ -11856,7 +11866,7 @@
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="Y199">
             <v>10</v>
@@ -11864,7 +11874,7 @@
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="Y200">
             <v>10</v>
@@ -11872,7 +11882,7 @@
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="Y201">
             <v>10</v>
@@ -11880,73 +11890,81 @@
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="Y202">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="Y203">
-            <v>25</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="204">
           <cell r="A204">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="Y204">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="205">
           <cell r="A205">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="Y205">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="206">
           <cell r="A206">
-            <v>55990105</v>
+            <v>55990104</v>
           </cell>
           <cell r="Y206">
-            <v>150</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>55990106</v>
+            <v>55990105</v>
           </cell>
           <cell r="Y207">
-            <v>80</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>55990107</v>
+            <v>55990106</v>
           </cell>
           <cell r="Y208">
-            <v>50</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="209">
           <cell r="A209">
-            <v>55990108</v>
+            <v>55990107</v>
           </cell>
           <cell r="Y209">
-            <v>4</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="210">
           <cell r="A210">
+            <v>55990108</v>
+          </cell>
+          <cell r="Y210">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="A211">
             <v>55990109</v>
           </cell>
-          <cell r="Y210">
+          <cell r="Y211">
             <v>15</v>
           </cell>
         </row>
@@ -47080,8 +47098,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA317" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
-  <autoFilter ref="A3:BA317"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA318" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+  <autoFilter ref="A3:BA318"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
@@ -47570,13 +47588,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA317"/>
+  <dimension ref="A1:BA318"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AB304" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
+      <selection pane="bottomRight" activeCell="AS318" sqref="AS318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -97169,7 +97187,7 @@
         <v>0</v>
       </c>
       <c r="H317" s="21">
-        <f t="shared" ref="H317" si="60">IF(AND(T317&gt;=13,T317&lt;=16),5,IF(AND(T317&gt;=9,T317&lt;=12),4,IF(AND(T317&gt;=5,T317&lt;=8),3,IF(AND(T317&gt;=1,T317&lt;=4),2,IF(AND(T317&gt;=-3,T317&lt;=0),1,IF(AND(T317&gt;=-5,T317&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H317:H318" si="60">IF(AND(T317&gt;=13,T317&lt;=16),5,IF(AND(T317&gt;=9,T317&lt;=12),4,IF(AND(T317&gt;=5,T317&lt;=8),3,IF(AND(T317&gt;=1,T317&lt;=4),2,IF(AND(T317&gt;=-3,T317&lt;=0),1,IF(AND(T317&gt;=-5,T317&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
       <c r="I317" s="8">
@@ -97206,7 +97224,7 @@
         <v>0</v>
       </c>
       <c r="T317" s="21">
-        <f t="shared" ref="T317" si="61">SUM(J317:K317)+SUM(M317:S317)*5+4.4*SUM(AJ317:AP317)+2.5*SUM(AD317:AH317)+IF(ISNUMBER(AC317),AC317,0)+L317</f>
+        <f t="shared" ref="T317:T318" si="61">SUM(J317:K317)+SUM(M317:S317)*5+4.4*SUM(AJ317:AP317)+2.5*SUM(AD317:AH317)+IF(ISNUMBER(AC317),AC317,0)+L317</f>
         <v>1</v>
       </c>
       <c r="U317" s="8">
@@ -97250,7 +97268,7 @@
         <v>0</v>
       </c>
       <c r="AI317" s="8" t="str">
-        <f t="shared" ref="AI317" si="62">CONCATENATE(AD317,";",AE317,";",AF317,";",AG317,";",AH317)</f>
+        <f t="shared" ref="AI317:AI318" si="62">CONCATENATE(AD317,";",AE317,";",AF317,";",AG317,";",AH317)</f>
         <v>0;0;0;0;0</v>
       </c>
       <c r="AJ317" s="18">
@@ -97275,7 +97293,7 @@
         <v>0</v>
       </c>
       <c r="AQ317" s="8" t="str">
-        <f t="shared" ref="AQ317" si="63">CONCATENATE(AJ317,";",AK317,";",AL317,";",AM317,";",AN317,";",AO317,";",AP317)</f>
+        <f t="shared" ref="AQ317:AQ318" si="63">CONCATENATE(AJ317,";",AK317,";",AL317,";",AM317,";",AN317,";",AO317,";",AP317)</f>
         <v>0;0;0;0;0;0;0</v>
       </c>
       <c r="AR317" s="51" t="s">
@@ -97301,9 +97319,166 @@
         <v>0.75409839999999995</v>
       </c>
     </row>
+    <row r="318" spans="1:53" x14ac:dyDescent="0.15">
+      <c r="A318">
+        <v>51000315</v>
+      </c>
+      <c r="B318" s="8" t="s">
+        <v>995</v>
+      </c>
+      <c r="C318" s="8" t="s">
+        <v>996</v>
+      </c>
+      <c r="D318" s="8" t="s">
+        <v>809</v>
+      </c>
+      <c r="E318" s="8">
+        <v>4</v>
+      </c>
+      <c r="F318" s="8">
+        <v>13</v>
+      </c>
+      <c r="G318" s="8">
+        <v>1</v>
+      </c>
+      <c r="H318" s="21">
+        <f t="shared" si="60"/>
+        <v>3</v>
+      </c>
+      <c r="I318" s="8">
+        <v>4</v>
+      </c>
+      <c r="J318" s="8">
+        <v>0</v>
+      </c>
+      <c r="K318" s="8">
+        <v>10</v>
+      </c>
+      <c r="L318" s="8">
+        <v>-14</v>
+      </c>
+      <c r="M318" s="8">
+        <v>0</v>
+      </c>
+      <c r="N318" s="8">
+        <v>0</v>
+      </c>
+      <c r="O318" s="8">
+        <v>0</v>
+      </c>
+      <c r="P318" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q318" s="8">
+        <v>0</v>
+      </c>
+      <c r="R318" s="8">
+        <v>0</v>
+      </c>
+      <c r="S318" s="8">
+        <v>0</v>
+      </c>
+      <c r="T318" s="21">
+        <f t="shared" si="61"/>
+        <v>7.32</v>
+      </c>
+      <c r="U318" s="8">
+        <v>25</v>
+      </c>
+      <c r="V318" s="8">
+        <v>20</v>
+      </c>
+      <c r="W318" s="8">
+        <v>0</v>
+      </c>
+      <c r="X318" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="Y318" s="18">
+        <v>55900056</v>
+      </c>
+      <c r="Z318" s="18">
+        <v>100</v>
+      </c>
+      <c r="AA318" s="18"/>
+      <c r="AB318" s="18"/>
+      <c r="AC318" s="18">
+        <f>IF(ISBLANK($Y318),0, LOOKUP($Y318,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$Z318/100)+
+IF(ISBLANK($AA318),0, LOOKUP($AA318,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$AB318/100)</f>
+        <v>10</v>
+      </c>
+      <c r="AD318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI318" s="8" t="str">
+        <f t="shared" si="62"/>
+        <v>0;0;0;0;0</v>
+      </c>
+      <c r="AJ318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AK318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AL318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM318" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="AN318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP318" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ318" s="8" t="str">
+        <f t="shared" si="63"/>
+        <v>0;0;0;0.3;0;0;0</v>
+      </c>
+      <c r="AR318" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="AS318" s="55">
+        <v>11000010</v>
+      </c>
+      <c r="AT318" s="8"/>
+      <c r="AU318" s="8"/>
+      <c r="AV318" s="8">
+        <v>315</v>
+      </c>
+      <c r="AW318" s="8"/>
+      <c r="AX318" s="59" t="s">
+        <v>937</v>
+      </c>
+      <c r="AY318" s="21">
+        <v>0</v>
+      </c>
+      <c r="AZ318" s="8">
+        <v>1</v>
+      </c>
+      <c r="BA318" s="52">
+        <v>0.75409839999999995</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H317">
+  <conditionalFormatting sqref="H4:H318">
     <cfRule type="cellIs" dxfId="147" priority="16" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -97320,12 +97495,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D317">
+  <conditionalFormatting sqref="D4:D318">
     <cfRule type="cellIs" dxfId="142" priority="8" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T317">
+  <conditionalFormatting sqref="T4:T318">
     <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
@@ -97337,7 +97512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H306:H317">
+  <conditionalFormatting sqref="H306:H318">
     <cfRule type="cellIs" dxfId="141" priority="2" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -97354,12 +97529,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D306:D317">
+  <conditionalFormatting sqref="D306:D318">
     <cfRule type="cellIs" dxfId="136" priority="1" operator="equal">
       <formula>"未完成"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T306:T317">
+  <conditionalFormatting sqref="T306:T318">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
rearrange the format of card table
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="标准卡" sheetId="1" r:id="rId1"/>
@@ -5820,7 +5820,313 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="169">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9933FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9933FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -6038,96 +6344,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8782,6 +8998,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9933FF"/>
       <color rgb="FF9148C8"/>
     </mruColors>
   </colors>
@@ -47739,159 +47956,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA318" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" tableBorderDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:BA318" totalsRowShown="0" headerRowDxfId="168" dataDxfId="167" tableBorderDxfId="166">
   <autoFilter ref="A3:BA318"/>
   <sortState ref="A4:BA304">
     <sortCondition ref="A3:A304"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="143"/>
-    <tableColumn id="2" name="Name" dataDxfId="142"/>
-    <tableColumn id="22" name="Ename" dataDxfId="141"/>
-    <tableColumn id="23" name="Remark" dataDxfId="140"/>
-    <tableColumn id="3" name="Star" dataDxfId="139"/>
-    <tableColumn id="4" name="Type" dataDxfId="138"/>
-    <tableColumn id="5" name="Attr" dataDxfId="137"/>
-    <tableColumn id="58" name="Quality" dataDxfId="136">
+    <tableColumn id="1" name="Id" dataDxfId="165"/>
+    <tableColumn id="2" name="Name" dataDxfId="164"/>
+    <tableColumn id="22" name="Ename" dataDxfId="163"/>
+    <tableColumn id="23" name="Remark" dataDxfId="162"/>
+    <tableColumn id="3" name="Star" dataDxfId="161"/>
+    <tableColumn id="4" name="Type" dataDxfId="160"/>
+    <tableColumn id="5" name="Attr" dataDxfId="159"/>
+    <tableColumn id="58" name="Quality" dataDxfId="158">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="135"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="134"/>
-    <tableColumn id="24" name="VitP" dataDxfId="133"/>
-    <tableColumn id="25" name="Modify" dataDxfId="132"/>
-    <tableColumn id="9" name="Def" dataDxfId="131"/>
-    <tableColumn id="10" name="Mag" dataDxfId="130"/>
-    <tableColumn id="32" name="Spd" dataDxfId="129"/>
-    <tableColumn id="35" name="Hit" dataDxfId="128"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="127"/>
-    <tableColumn id="34" name="Crt" dataDxfId="126"/>
-    <tableColumn id="33" name="Luk" dataDxfId="125"/>
-    <tableColumn id="7" name="Sum" dataDxfId="124">
+    <tableColumn id="12" name="Cost" dataDxfId="157"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="156"/>
+    <tableColumn id="24" name="VitP" dataDxfId="155"/>
+    <tableColumn id="25" name="Modify" dataDxfId="154"/>
+    <tableColumn id="9" name="Def" dataDxfId="153"/>
+    <tableColumn id="10" name="Mag" dataDxfId="152"/>
+    <tableColumn id="32" name="Spd" dataDxfId="151"/>
+    <tableColumn id="35" name="Hit" dataDxfId="150"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="149"/>
+    <tableColumn id="34" name="Crt" dataDxfId="148"/>
+    <tableColumn id="33" name="Luk" dataDxfId="147"/>
+    <tableColumn id="7" name="Sum" dataDxfId="146">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="123"/>
-    <tableColumn id="14" name="Mov" dataDxfId="122"/>
-    <tableColumn id="51" name="LifeRound" dataDxfId="121"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="120"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="119"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="118"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="117"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="116"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="115">
+    <tableColumn id="13" name="Range" dataDxfId="145"/>
+    <tableColumn id="14" name="Mov" dataDxfId="144"/>
+    <tableColumn id="51" name="LifeRound" dataDxfId="143"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="142"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="141"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="140"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="139"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="138"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="137">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="114"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="113"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="112"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="111"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="110"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="109">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="136"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="135"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="134"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="133"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="132"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="131">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="108"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="107"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="106"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="105"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="104"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="103"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="102"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="101">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="130"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="129"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="128"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="127"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="126"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="125"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="124"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="123">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="IsBuilding" dataDxfId="100"/>
-    <tableColumn id="29" name="JobId" dataDxfId="99"/>
-    <tableColumn id="20" name="DropId1" dataDxfId="98"/>
-    <tableColumn id="39" name="DropId2" dataDxfId="97"/>
-    <tableColumn id="21" name="Icon" dataDxfId="96"/>
-    <tableColumn id="17" name="Cover" dataDxfId="95"/>
-    <tableColumn id="18" name="Sound" dataDxfId="94"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="93"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="92"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="91"/>
+    <tableColumn id="50" name="IsBuilding" dataDxfId="122"/>
+    <tableColumn id="29" name="JobId" dataDxfId="121"/>
+    <tableColumn id="20" name="DropId1" dataDxfId="120"/>
+    <tableColumn id="39" name="DropId2" dataDxfId="119"/>
+    <tableColumn id="21" name="Icon" dataDxfId="118"/>
+    <tableColumn id="17" name="Cover" dataDxfId="117"/>
+    <tableColumn id="18" name="Sound" dataDxfId="116"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="115"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="114"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_5" displayName="表1_5" ref="A3:BA15" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" tableBorderDxfId="110">
   <autoFilter ref="A3:BA15"/>
   <sortState ref="A4:AF311">
     <sortCondition ref="A3:A311"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" name="Id" dataDxfId="87"/>
-    <tableColumn id="2" name="Name" dataDxfId="86"/>
-    <tableColumn id="22" name="Ename" dataDxfId="85"/>
-    <tableColumn id="23" name="Remark" dataDxfId="84"/>
-    <tableColumn id="3" name="Star" dataDxfId="83"/>
-    <tableColumn id="4" name="Type" dataDxfId="82"/>
-    <tableColumn id="5" name="Attr" dataDxfId="81"/>
-    <tableColumn id="58" name="Quality" dataDxfId="80">
+    <tableColumn id="1" name="Id" dataDxfId="109"/>
+    <tableColumn id="2" name="Name" dataDxfId="108"/>
+    <tableColumn id="22" name="Ename" dataDxfId="107"/>
+    <tableColumn id="23" name="Remark" dataDxfId="106"/>
+    <tableColumn id="3" name="Star" dataDxfId="105"/>
+    <tableColumn id="4" name="Type" dataDxfId="104"/>
+    <tableColumn id="5" name="Attr" dataDxfId="103"/>
+    <tableColumn id="58" name="Quality" dataDxfId="102">
       <calculatedColumnFormula>IF(AND(T4&gt;=13,T4&lt;=16),5,IF(AND(T4&gt;=9,T4&lt;=12),4,IF(AND(T4&gt;=5,T4&lt;=8),3,IF(AND(T4&gt;=1,T4&lt;=4),2,IF(AND(T4&gt;=-3,T4&lt;=0),1,IF(AND(T4&gt;=-5,T4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Cost" dataDxfId="79"/>
-    <tableColumn id="6" name="AtkP" dataDxfId="78"/>
-    <tableColumn id="24" name="VitP" dataDxfId="77"/>
-    <tableColumn id="25" name="Modify" dataDxfId="76"/>
-    <tableColumn id="9" name="Def" dataDxfId="75"/>
-    <tableColumn id="10" name="Mag" dataDxfId="74"/>
-    <tableColumn id="32" name="Spd" dataDxfId="73"/>
-    <tableColumn id="35" name="Hit" dataDxfId="72"/>
-    <tableColumn id="36" name="Dhit" dataDxfId="71"/>
-    <tableColumn id="34" name="Crt" dataDxfId="70"/>
-    <tableColumn id="33" name="Luk" dataDxfId="69"/>
-    <tableColumn id="7" name="Sum" dataDxfId="68">
+    <tableColumn id="12" name="Cost" dataDxfId="101"/>
+    <tableColumn id="6" name="AtkP" dataDxfId="100"/>
+    <tableColumn id="24" name="VitP" dataDxfId="99"/>
+    <tableColumn id="25" name="Modify" dataDxfId="98"/>
+    <tableColumn id="9" name="Def" dataDxfId="97"/>
+    <tableColumn id="10" name="Mag" dataDxfId="96"/>
+    <tableColumn id="32" name="Spd" dataDxfId="95"/>
+    <tableColumn id="35" name="Hit" dataDxfId="94"/>
+    <tableColumn id="36" name="Dhit" dataDxfId="93"/>
+    <tableColumn id="34" name="Crt" dataDxfId="92"/>
+    <tableColumn id="33" name="Luk" dataDxfId="91"/>
+    <tableColumn id="7" name="Sum" dataDxfId="90">
       <calculatedColumnFormula>SUM(J4:K4)+SUM(M4:S4)*5+4.4*SUM(AJ4:AP4)+2.5*SUM(AD4:AH4)+IF(ISNUMBER(AC4),AC4,0)+L4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Range" dataDxfId="67"/>
-    <tableColumn id="14" name="Mov" dataDxfId="66"/>
-    <tableColumn id="60" name="LifeRound" dataDxfId="65"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="64"/>
-    <tableColumn id="42" name="Skill1" dataDxfId="63"/>
-    <tableColumn id="43" name="SkillRate1" dataDxfId="62"/>
-    <tableColumn id="44" name="Skill2" dataDxfId="61"/>
-    <tableColumn id="45" name="SkillRate2" dataDxfId="60"/>
-    <tableColumn id="54" name="~SkillMark" dataDxfId="59">
+    <tableColumn id="13" name="Range" dataDxfId="89"/>
+    <tableColumn id="14" name="Mov" dataDxfId="88"/>
+    <tableColumn id="60" name="LifeRound" dataDxfId="87"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="86"/>
+    <tableColumn id="42" name="Skill1" dataDxfId="85"/>
+    <tableColumn id="43" name="SkillRate1" dataDxfId="84"/>
+    <tableColumn id="44" name="Skill2" dataDxfId="83"/>
+    <tableColumn id="45" name="SkillRate2" dataDxfId="82"/>
+    <tableColumn id="54" name="~SkillMark" dataDxfId="81">
       <calculatedColumnFormula>IF(ISBLANK($Y4),0, LOOKUP($Y4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$Z4/100)+
 IF(ISBLANK($AA4),0, LOOKUP($AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*$AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="~AntiLife" dataDxfId="58"/>
-    <tableColumn id="57" name="~AntiMental" dataDxfId="57"/>
-    <tableColumn id="56" name="~AntiPhysical" dataDxfId="56"/>
-    <tableColumn id="55" name="~AntiElement" dataDxfId="55"/>
-    <tableColumn id="53" name="~AntiHelp" dataDxfId="54"/>
-    <tableColumn id="30" name="BuffImmune" dataDxfId="53">
+    <tableColumn id="52" name="~AntiLife" dataDxfId="80"/>
+    <tableColumn id="57" name="~AntiMental" dataDxfId="79"/>
+    <tableColumn id="56" name="~AntiPhysical" dataDxfId="78"/>
+    <tableColumn id="55" name="~AntiElement" dataDxfId="77"/>
+    <tableColumn id="53" name="~AntiHelp" dataDxfId="76"/>
+    <tableColumn id="30" name="BuffImmune" dataDxfId="75">
       <calculatedColumnFormula>CONCATENATE(AD4,";",AE4,";",AF4,";",AG4,";",AH4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="~AntiNull" dataDxfId="52"/>
-    <tableColumn id="11" name="~AntiWater" dataDxfId="51"/>
-    <tableColumn id="26" name="~AntiWind" dataDxfId="50"/>
-    <tableColumn id="27" name="~AntiFire" dataDxfId="49"/>
-    <tableColumn id="37" name="~AntiEarth" dataDxfId="48"/>
-    <tableColumn id="40" name="~AntiLight" dataDxfId="47"/>
-    <tableColumn id="41" name="~AntiDark" dataDxfId="46"/>
-    <tableColumn id="31" name="AttrDef" dataDxfId="45">
+    <tableColumn id="8" name="~AntiNull" dataDxfId="74"/>
+    <tableColumn id="11" name="~AntiWater" dataDxfId="73"/>
+    <tableColumn id="26" name="~AntiWind" dataDxfId="72"/>
+    <tableColumn id="27" name="~AntiFire" dataDxfId="71"/>
+    <tableColumn id="37" name="~AntiEarth" dataDxfId="70"/>
+    <tableColumn id="40" name="~AntiLight" dataDxfId="69"/>
+    <tableColumn id="41" name="~AntiDark" dataDxfId="68"/>
+    <tableColumn id="31" name="AttrDef" dataDxfId="67">
       <calculatedColumnFormula>CONCATENATE(AJ4,";",AK4,";",AL4,";",AM4,";",AN4,";",AO4,";",AP4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="IsBuilding" dataDxfId="44"/>
-    <tableColumn id="29" name="JobId" dataDxfId="43"/>
-    <tableColumn id="46" name="DropId1" dataDxfId="42"/>
-    <tableColumn id="38" name="DropId2" dataDxfId="41"/>
-    <tableColumn id="21" name="Icon" dataDxfId="40"/>
-    <tableColumn id="17" name="Cover" dataDxfId="39"/>
-    <tableColumn id="18" name="Sound" dataDxfId="38"/>
-    <tableColumn id="15" name="IsSpecial" dataDxfId="37"/>
-    <tableColumn id="28" name="IsNew" dataDxfId="36"/>
-    <tableColumn id="19" name="VsMark" dataDxfId="35"/>
+    <tableColumn id="59" name="IsBuilding" dataDxfId="66"/>
+    <tableColumn id="29" name="JobId" dataDxfId="65"/>
+    <tableColumn id="46" name="DropId1" dataDxfId="64"/>
+    <tableColumn id="38" name="DropId2" dataDxfId="63"/>
+    <tableColumn id="21" name="Icon" dataDxfId="62"/>
+    <tableColumn id="17" name="Cover" dataDxfId="61"/>
+    <tableColumn id="18" name="Sound" dataDxfId="60"/>
+    <tableColumn id="15" name="IsSpecial" dataDxfId="59"/>
+    <tableColumn id="28" name="IsNew" dataDxfId="58"/>
+    <tableColumn id="19" name="VsMark" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="56">
   <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
     <tableColumn id="1" name="星级"/>
@@ -48231,11 +48448,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml